<commit_message>
Put trend calc before paris path calc
</commit_message>
<xml_diff>
--- a/data/tests/reference_dataframes/df_trend.xlsx
+++ b/data/tests/reference_dataframes/df_trend.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T291"/>
+  <dimension ref="A1:S291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,15 +494,10 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>parisPath</t>
+          <t>trend</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>trend</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>trendEmission</t>
         </is>
@@ -568,15 +563,10 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>{2021: 140535.25077554, 2022: 104113.01437312477, 2023: 77130.25523518752, 2024: 57140.56315116006, 2025: 42331.55909151158, 2026: 31360.57463027921, 2027: 23232.917998962206, 2028: 17211.689680754313, 2029: 12750.97091462284, 2030: 9446.32759951271, 2031: 6998.142001483421, 2032: 5184.447708065165, 2033: 3840.8048924935515, 2034: 2845.3912649661515, 2035: 2107.9569718755943, 2036: 1561.6420314454656, 2037: 1156.9144280052456, 2038: 857.0792580984938, 2039: 634.951762101573, 2040: 470.3925995016457, 2041: 348.4819018905558, 2042: 258.1665529472984, 2043: 191.2580501285896, 2044: 141.69008851606503, 2045: 104.96855515463268, 2046: 77.76406724456157, 2047: 57.61011138534091, 2048: 42.67941546053193, 2049: 31.61827776844377, 2050: 23.42383273657904}</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
           <t>{2021: 140535.25077554, 2022: 142936.95388118387, 2023: 143719.28805910517, 2024: 144501.62223702623, 2025: 145283.9564149473, 2026: 146066.29059286858, 2027: 146848.62477078964, 2028: 147630.95894871093, 2029: 148413.293126632, 2030: 149195.6273045533, 2031: 149977.96148247435, 2032: 150760.2956603954, 2033: 151542.6298383167, 2034: 152324.96401623776, 2035: 153107.29819415906, 2036: 153889.63237208012, 2037: 154671.96655000118, 2038: 155454.30072792247, 2039: 156236.63490584353, 2040: 157018.96908376482, 2041: 157801.30326168588, 2042: 158583.63743960718, 2043: 159365.97161752824, 2044: 160148.3057954493, 2045: 160930.6399733706, 2046: 161712.97415129165, 2047: 162495.30832921294, 2048: 163277.642507134, 2049: 164059.97668505507, 2050: 164842.31086297636}</t>
         </is>
       </c>
-      <c r="T2" t="n">
+      <c r="S2" t="n">
         <v>4450645.808746605</v>
       </c>
     </row>
@@ -640,15 +630,10 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>{2021: 63674.7692719455, 2022: 49688.75098577729, 2023: 38774.72981459846, 2024: 30257.94857724359, 2025: 23611.85897311967, 2026: 18425.56783858743, 2027: 14378.433759107427, 2028: 11220.243477765704, 2029: 8755.742510591708, 2030: 6832.563577047149, 2031: 5331.806523309518, 2032: 4160.6873439869005, 2033: 3246.801829498384, 2034: 2533.6491902639937, 2035: 1977.1389066628542, 2036: 1542.864841455293, 2037: 1203.9780872132626, 2038: 939.5270379759384, 2039: 733.1620603917889, 2040: 572.1246808989646, 2041: 446.4587956431136, 2042: 348.3951363431914, 2043: 271.8709368302332, 2044: 212.15510373870097, 2045: 165.55571760318315, 2046: 129.19178067411775, 2047: 100.81509980678815, 2048: 78.6712923687477, 2049: 61.39132188363169, 2050: 47.906857624177974}</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
           <t>{2021: 63674.7692719455, 2022: 64183.36643868731, 2023: 62206.74147178279, 2024: 60230.11650487827, 2025: 58253.49153797375, 2026: 56276.86657106923, 2027: 54300.24160416471, 2028: 52323.61663726065, 2029: 50346.99167035613, 2030: 48370.36670345161, 2031: 46393.74173654709, 2032: 44417.11676964257, 2033: 42440.49180273805, 2034: 40463.86683583353, 2035: 38487.241868929006, 2036: 36510.616902024485, 2037: 34533.991935119964, 2038: 32557.366968215443, 2039: 30580.742001310922, 2040: 28604.1170344064, 2041: 26627.49206750188, 2042: 24650.86710059736, 2043: 22674.24213369284, 2044: 20697.617166788317, 2045: 18720.992199883796, 2046: 16744.367232979275, 2047: 14767.742266074754, 2048: 12791.117299170233, 2049: 10814.492332265712, 2050: 8837.867365361191}</t>
         </is>
       </c>
-      <c r="T3" t="n">
+      <c r="S3" t="n">
         <v>1086226.341111999</v>
       </c>
     </row>
@@ -712,15 +697,10 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>{2021: 52912.9774987249, 2022: 41003.86434721774, 2023: 31775.13288579443, 2024: 24623.510149194117, 2025: 19081.50169652097, 2026: 14786.831966207263, 2027: 11458.762684108577, 2028: 8879.741282702744, 2029: 6881.179706870716, 2030: 5332.433980986115, 2031: 4132.264142612613, 2032: 3202.2162871980286, 2033: 2481.4941146315828, 2034: 1922.984735781021, 2035: 1490.1789499491972, 2036: 1154.784674861072, 2037: 894.8775214811982, 2038: 693.467618583243, 2039: 537.3890018239978, 2040: 416.43896779403417, 2041: 322.71113347823683, 2042: 250.07860388876034, 2043: 193.79346305437895, 2044: 150.17640749192003, 2045: 116.37623380955219, 2046: 90.1834583865927, 2047: 69.88588563431183, 2048: 54.15668347908697, 2049: 41.96764967394256, 2050: 32.521999243821924}</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
           <t>{2021: 52912.9774987249, 2022: 50626.769764077384, 2023: 48593.747548584826, 2024: 46560.7253330918, 2025: 44527.70311759878, 2026: 42494.68090210622, 2027: 40461.6586866132, 2028: 38428.63647112064, 2029: 36395.61425562762, 2030: 34362.592040134594, 2031: 32329.569824642036, 2032: 30296.547609149013, 2033: 28263.52539365599, 2034: 26230.50317816343, 2035: 24197.48096267041, 2036: 22164.45874717785, 2037: 20131.436531684827, 2038: 18098.414316191804, 2039: 16065.392100699246, 2040: 14032.369885206223, 2041: 11999.3476697132, 2042: 9966.325454220641, 2043: 7933.303238727618, 2044: 5900.28102323506, 2045: 3867.258807742037, 2046: 1834.2365922490135, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T4" t="n">
+      <c r="S4" t="n">
         <v>682219.0682034459</v>
       </c>
     </row>
@@ -784,15 +764,10 @@
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>{2021: 16087.2823225698, 2022: 12387.680010703885, 2023: 9538.877541317348, 2024: 7345.215945974236, 2025: 5656.032070786311, 2026: 4355.3108609824785, 2027: 3353.717316025558, 2028: 2582.4608609619336, 2029: 1988.5707321044304, 2030: 1531.2578852054246, 2031: 1179.1135578679803, 2032: 907.9520803000286, 2033: 699.1497762198157, 2034: 538.3658677522862, 2035: 414.55753462123124, 2036: 319.2214807910311, 2037: 245.80991849906619, 2038: 189.28085880308095, 2039: 145.7518220908077, 2040: 112.23318499886634, 2041: 86.42284970641316, 2042: 66.54813325891737, 2043: 51.2440177023923, 2044: 39.45939910990995, 2045: 30.38489657774187, 2046: 23.39726303151443, 2047: 18.01657991381438, 2048: 13.87329583608352, 2049: 10.682845372218255, 2050: 8.226104783976284}</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
           <t>{2021: 16087.2823225698, 2022: 16081.702993880841, 2023: 15711.255263767787, 2024: 15340.807533654734, 2025: 14970.359803541796, 2026: 14599.912073428743, 2027: 14229.464343315689, 2028: 13859.016613202752, 2029: 13488.568883089698, 2030: 13118.121152976644, 2031: 12747.673422863707, 2032: 12377.225692750653, 2033: 12006.777962637716, 2034: 11636.330232524662, 2035: 11265.882502411609, 2036: 10895.434772298671, 2037: 10524.987042185618, 2038: 10154.539312072564, 2039: 9784.091581959627, 2040: 9413.643851846573, 2041: 9043.19612173352, 2042: 8672.748391620582, 2043: 8302.300661507528, 2044: 7931.852931394591, 2045: 7561.405201281537, 2046: 7190.957471168484, 2047: 6820.509741055546, 2048: 6450.062010942493, 2049: 6079.614280829439, 2050: 5709.166550716502}</t>
         </is>
       </c>
-      <c r="T5" t="n">
+      <c r="S5" t="n">
         <v>321156.666282587</v>
       </c>
     </row>
@@ -856,15 +831,10 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>{2021: 46192.2589353511, 2022: 35218.1311967816, 2023: 26851.182288565295, 2024: 20472.011597243687, 2025: 15608.37263453227, 2026: 11900.212890227966, 2027: 9073.019343441092, 2028: 6917.496415047685, 2029: 5274.0719313896025, 2030: 4021.084084259681, 2031: 3065.774874334395, 2032: 2337.423287638243, 2033: 1782.1098578804654, 2034: 1358.7250381011272, 2035: 1035.9258835808191, 2036: 789.8157509281353, 2037: 602.1752427479595, 2038: 459.1134356999649, 2039: 350.03954310431516, 2040: 266.8788848443781, 2041: 203.47512325072734, 2042: 155.13451281858065, 2043: 118.27842481659407, 2044: 90.1784233754278, 2045: 68.75428088502062, 2046: 52.41997989182395, 2047: 39.96630110137473, 2048: 30.471305540788308, 2049: 23.232083925027993, 2050: 17.712720670175162}</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
           <t>{2021: 46192.2589353511, 2022: 46160.89896231075, 2023: 45411.244647955056, 2024: 44661.590333599364, 2025: 43911.936019243905, 2026: 43162.28170488821, 2027: 42412.62739053252, 2028: 41662.97307617706, 2029: 40913.31876182137, 2030: 40163.66444746568, 2031: 39414.01013311022, 2032: 38664.35581875453, 2033: 37914.701504398836, 2034: 37165.04719004338, 2035: 36415.392875687685, 2036: 35665.73856133199, 2037: 34916.084246976534, 2038: 34166.42993262084, 2039: 33416.77561826515, 2040: 32667.12130390969, 2041: 31917.466989554, 2042: 31167.812675198307, 2043: 30418.158360842615, 2044: 29668.504046487156, 2045: 28918.849732131464, 2046: 28169.195417775773, 2047: 27419.541103420313, 2048: 26669.88678906462, 2049: 25920.23247470893, 2050: 25170.57816035347}</t>
         </is>
       </c>
-      <c r="T6" t="n">
+      <c r="S6" t="n">
         <v>1044817.258666128</v>
       </c>
     </row>
@@ -928,15 +898,10 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>{2021: 11742.698661745, 2022: 9128.03433787484, 2023: 7095.558974434283, 2024: 5515.640640260401, 2025: 4287.511636800633, 2026: 3332.841501949802, 2027: 2590.7410680307207, 2028: 2013.8789311325766, 2029: 1565.462638974771, 2030: 1216.8920564890318, 2031: 945.9352400232975, 2032: 735.3104768385007, 2033: 571.5840519221452, 2034: 444.3134413322032, 2035: 345.38128466774424, 2036: 268.477657216659, 2037: 208.6976209318546, 2038: 162.22838590798577, 2039: 126.10612941727737, 2040: 98.02696234447521, 2041: 76.19998639946064, 2042: 59.23307004937747, 2043: 46.04405792255222, 2044: 35.79175059148611, 2045: 27.822252603320045, 2046: 21.627266817932078, 2047: 16.811675053162674, 2048: 13.068337320312237, 2049: 10.158502337061146, 2050: 7.896579894037442}</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
           <t>{2021: 11742.698661745, 2022: 9449.445710867876, 2023: 8523.929245739244, 2024: 7598.4127806108445, 2025: 6672.896315482212, 2026: 5747.379850353813, 2027: 4821.8633852251805, 2028: 3896.346920096781, 2029: 2970.830454968149, 2030: 2045.3139898397494, 2031: 1119.7975247111171, 2032: 194.28105958271772, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T7" t="n">
+      <c r="S7" t="n">
         <v>58911.84656835019</v>
       </c>
     </row>
@@ -1000,15 +965,10 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>{2021: 36324.1026555328, 2022: 27558.22825538156, 2023: 20907.768920756316, 2024: 15862.22442142594, 2025: 12034.290437651332, 2026: 9130.128441640552, 2027: 6926.810167390518, 2028: 5255.205269209029, 2029: 3986.998597353844, 2030: 3024.8405154484253, 2031: 2294.874181789502, 2032: 1741.0661763313822, 2033: 1320.9052829211832, 2034: 1002.1392582133528, 2035: 760.2990962617973, 2036: 576.8207472553075, 2037: 437.620110427704, 2038: 332.01191524754694, 2039: 251.8895024239406, 2040: 191.10254336526907, 2041: 144.98493080989752, 2042: 109.99660073478151, 2043: 83.45179120077886, 2044: 63.31287883532089, 2045: 48.03396750073133, 2046: 36.44222275633025, 2047: 27.647843151864876, 2048: 20.975757600223208, 2049: 15.91380580707774, 2050: 12.073424001747915}</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
           <t>{2021: 36324.1026555328, 2022: 35461.88679012493, 2023: 34780.46276358259, 2024: 34099.03873704001, 2025: 33417.61471049767, 2026: 32736.190683955327, 2027: 32054.766657412983, 2028: 31373.342630870407, 2029: 30691.918604328064, 2030: 30010.49457778572, 2031: 29329.070551243378, 2032: 28647.646524701035, 2033: 27966.22249815846, 2034: 27284.798471616115, 2035: 26603.374445073772, 2036: 25921.95041853143, 2037: 25240.526391988853, 2038: 24559.10236544651, 2039: 23877.678338904167, 2040: 23196.254312361823, 2041: 22514.83028581948, 2042: 21833.406259276904, 2043: 21151.98223273456, 2044: 20470.558206192218, 2045: 19789.134179649875, 2046: 19107.7101531073, 2047: 18426.286126564955, 2048: 17744.862100022612, 2049: 17063.43807348027, 2050: 16382.014046937926}</t>
         </is>
       </c>
-      <c r="T8" t="n">
+      <c r="S8" t="n">
         <v>761707.6064417068</v>
       </c>
     </row>
@@ -1072,15 +1032,10 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>{2021: 62127.6159510355, 2022: 47223.67812609905, 2023: 35895.080498742944, 2024: 27284.126420028817, 2025: 20738.87407858535, 2026: 15763.777495609662, 2027: 11982.168366009979, 2028: 9107.7382176573, 2029: 6922.861781568985, 2030: 5262.120419073273, 2031: 3999.7781522300293, 2032: 3040.262098348969, 2033: 2310.9265751411353, 2034: 1756.5530414610173, 2035: 1335.1694600151934, 2036: 1014.8725628430308, 2037: 771.4124308983678, 2038: 586.3565144351716, 2039: 445.6940907993488, 2040: 338.7755020762551, 2041: 257.5058614781761, 2042: 195.732183375798, 2043: 148.7775361272851, 2044: 113.0869480651926, 2045: 85.95825791709828, 2046: 65.33753214281509, 2047: 49.663560080877744, 2048: 37.74965351485473, 2049: 28.693801615729804, 2050: 21.810379023449077}</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
           <t>{2021: 62127.6159510355, 2022: 59655.35764219379, 2023: 58164.495317440946, 2024: 56673.63299268857, 2025: 55182.77066793572, 2026: 53691.90834318288, 2027: 52201.0460184305, 2028: 50710.18369367765, 2029: 49219.32136892481, 2030: 47728.45904417243, 2031: 46237.596719419584, 2032: 44746.73439466674, 2033: 43255.87206991436, 2034: 41765.009745161515, 2035: 40274.14742040867, 2036: 38783.28509565629, 2037: 37292.422770903446, 2038: 35801.56044615107, 2039: 34310.69812139822, 2040: 32819.83579664538, 2041: 31328.973471892998, 2042: 29838.111147140153, 2043: 28347.248822387308, 2044: 26856.38649763493, 2045: 25365.524172882084, 2046: 23874.66184812924, 2047: 22383.79952337686, 2048: 20892.937198624015, 2049: 19402.07487387117, 2050: 17911.21254911879}</t>
         </is>
       </c>
-      <c r="T9" t="n">
+      <c r="S9" t="n">
         <v>1146823.469474989</v>
       </c>
     </row>
@@ -1144,15 +1099,10 @@
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>{2021: 83063.063221357, 2022: 59751.81117991578, 2023: 42982.75070551847, 2024: 30919.846975847817, 2025: 22242.33957383983, 2026: 16000.133186442981, 2027: 11509.772213216802, 2028: 8279.609604274066, 2029: 5955.976706512787, 2030: 4284.460285447618, 2031: 3082.0469659502123, 2032: 2217.0852026769358, 2033: 1594.8708278082854, 2034: 1147.2779459818212, 2035: 825.2998690465033, 2036: 593.6834018588977, 2037: 427.068990147741, 2038: 307.2141174483432, 2039: 220.99594242821124, 2040: 158.97448650921885, 2041: 114.35905602239508, 2042: 82.2647330493181, 2043: 59.17752855838785, 2044: 42.569637759346485, 2045: 30.622672205277844, 2046: 22.028565483529533, 2047: 15.846353773741344, 2048: 11.399150258345957, 2049: 8.200033172783924, 2050: 5.898733020518464}</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
           <t>{2021: 83063.063221357, 2022: 80611.78063574666, 2023: 81321.93432401074, 2024: 82032.08801227505, 2025: 82742.24170053913, 2026: 83452.39538880321, 2027: 84162.54907706729, 2028: 84872.70276533137, 2029: 85582.85645359545, 2030: 86293.01014185953, 2031: 87003.16383012361, 2032: 87713.31751838769, 2033: 88423.47120665177, 2034: 89133.62489491585, 2035: 89843.77858317993, 2036: 90553.932271444, 2037: 91264.08595970809, 2038: 91974.23964797216, 2039: 92684.39333623624, 2040: 93394.54702450056, 2041: 94104.70071276464, 2042: 94814.85440102872, 2043: 95525.0080892928, 2044: 96235.16177755687, 2045: 96945.31546582095, 2046: 97655.46915408503, 2047: 98365.62284234911, 2048: 99075.77653061319, 2049: 99785.93021887727, 2050: 100496.08390714135}</t>
         </is>
       </c>
-      <c r="T10" t="n">
+      <c r="S10" t="n">
         <v>2617347.525528986</v>
       </c>
     </row>
@@ -1216,15 +1166,10 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>{2021: 207670.893624396, 2022: 156019.5144898864, 2023: 117214.73566577987, 2024: 88061.38323221912, 2025: 66158.97884105139, 2026: 49704.085044274696, 2027: 37341.81079221191, 2028: 28054.250108401764, 2029: 21076.66801495623, 2030: 15834.532482464789, 2031: 11896.207633972794, 2032: 8937.41297555277, 2033: 6714.522237109237, 2034: 5044.503257929176, 2035: 3789.8471731346335, 2036: 2847.2459747429534, 2037: 2139.0861610877855, 2038: 1607.0580642300731, 2039: 1207.3546492833018, 2040: 907.06445622074, 2041: 681.4616800684274, 2042: 511.9702554949103, 2043: 384.634309129758, 2044: 288.96903711078363, 2045: 217.0973894597723, 2046: 163.10147613558703, 2047: 122.53528973243024, 2048: 92.05862255549842, 2049: 69.16203491517741, 2050: 51.9602286111169}</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
           <t>{2021: 207670.893624396, 2022: 207901.28197011352, 2023: 206561.02817861876, 2024: 205220.774387124, 2025: 203880.5205956297, 2026: 202540.26680413494, 2027: 201200.01301264018, 2028: 199859.75922114542, 2029: 198519.50542965112, 2030: 197179.25163815636, 2031: 195838.9978466616, 2032: 194498.74405516684, 2033: 193158.49026367208, 2034: 191818.23647217778, 2035: 190477.98268068302, 2036: 189137.72888918826, 2037: 187797.4750976935, 2038: 186457.2213061992, 2039: 185116.96751470445, 2040: 183776.7137232097, 2041: 182436.45993171493, 2042: 181096.20614022063, 2043: 179755.95234872587, 2044: 178415.6985572311, 2045: 177075.44476573635, 2046: 175735.19097424205, 2047: 174394.9371827473, 2048: 173054.68339125253, 2049: 171714.42959975777, 2050: 170374.175808263}</t>
         </is>
       </c>
-      <c r="T11" t="n">
+      <c r="S11" t="n">
         <v>5503642.496694528</v>
       </c>
     </row>
@@ -1288,15 +1233,10 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>{2021: 54901.5850984739, 2022: 42610.76770117101, 2023: 33071.49549191484, 2024: 25667.780072446014, 2025: 19921.53436207702, 2026: 15461.700630879528, 2027: 12000.28983982414, 2028: 9313.785053642883, 2029: 7228.708071498781, 2030: 5610.417255926851, 2031: 4354.413191716493, 2032: 3379.590746867228, 2033: 2623.001794601909, 2034: 2035.790404759069, 2035: 1580.0380238543034, 2036: 1226.3149246549624, 2037: 951.7798127180874, 2038: 738.7048739968316, 2039: 573.3310200269013, 2040: 444.9794093635523, 2041: 345.36187270705364, 2042: 268.04571314955916, 2043: 208.0383215862391, 2044: 161.46478427084904, 2045: 125.317664365142, 2046: 97.2627998907233, 2047: 75.48857769179958, 2048: 58.588950434629346, 2049: 45.47264259032856, 2050: 35.292682473547124}</t>
-        </is>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
           <t>{2021: 54901.5850984739, 2022: 55504.01357598929, 2023: 54073.623524431605, 2024: 52643.23347287392, 2025: 51212.84342131624, 2026: 49782.45336975856, 2027: 48352.063318200875, 2028: 46921.67326664319, 2029: 45491.28321508551, 2030: 44060.89316352783, 2031: 42630.503111970145, 2032: 41200.11306041246, 2033: 39769.72300885478, 2034: 38339.33295729663, 2035: 36908.94290573895, 2036: 35478.55285418127, 2037: 34048.162802623585, 2038: 32617.772751065902, 2039: 31187.38269950822, 2040: 29756.992647950538, 2041: 28326.602596392855, 2042: 26896.212544835173, 2043: 25465.82249327749, 2044: 24035.432441719808, 2045: 22605.042390162125, 2046: 21174.652338604443, 2047: 19744.26228704676, 2048: 18313.872235489078, 2049: 16883.482183931395, 2050: 15453.092132373713}</t>
         </is>
       </c>
-      <c r="T12" t="n">
+      <c r="S12" t="n">
         <v>1048602.279254312</v>
       </c>
     </row>
@@ -1360,15 +1300,10 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>{2021: 28585.8132476701, 2022: 23344.824012827707, 2023: 19064.729887799014, 2024: 15569.35813673377, 2025: 12714.835941368969, 2026: 10383.668459298704, 2027: 8479.902624762142, 2028: 6925.177629400589, 2029: 5655.499517023706, 2030: 4618.607131644624, 2031: 3771.8209987054574, 2032: 3080.286597403126, 2033: 2515.539715537351, 2034: 2054.334835524909, 2035: 1677.6883268367117, 2036: 1370.0970617503979, 2037: 1118.9002919013437, 2038: 913.7585198653527, 2039: 746.2279156328436, 2040: 609.4127605527489, 2041: 497.68161300903273, 2042: 406.4355129397289, 2043: 331.91868427653236, 2044: 271.06394363772466, 2045: 221.36645214952904, 2046: 180.78061390105813, 2047: 147.63587727542202, 2048: 120.56797345987935, 2049: 98.46276184686029, 2050: 80.41037094927736}</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
           <t>{2021: 28585.8132476701, 2022: 20333.569486629218, 2023: 16054.105502955616, 2024: 11774.64151928015, 2025: 7495.177535606548, 2026: 3215.713551931083, 2027: 0, 2028: 0, 2029: 0, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T13" t="n">
+      <c r="S13" t="n">
         <v>73166.11422023766</v>
       </c>
     </row>
@@ -1432,15 +1367,10 @@
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>{2021: 11516.2724727444, 2022: 8847.782595860463, 2023: 6797.6211095113085, 2024: 5222.512222451366, 2025: 4012.379253602548, 2026: 3082.651909464261, 2027: 2368.356078601377, 2028: 1819.573107760619, 2029: 1397.9512305602477, 2030: 1074.0253495118222, 2031: 825.1578640062421, 2032: 633.9566387709816, 2033: 487.0595523267786, 2034: 374.2006834610352, 2035: 287.49287604313184, 2036: 220.87654413425997, 2037: 169.69619706811235, 2038: 130.3750899048631, 2039: 100.16526216482426, 2040: 76.95549626749458, 2041: 59.123774827557945, 2042: 45.42392576755164, 2043: 34.89853342676472, 2044: 26.812029448344653, 2045: 20.599287492911262, 2046: 15.82612931382589, 2047: 12.158982156258135, 2048: 9.341566983598957, 2049: 7.176988385014742, 2050: 5.513974515097037}</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
           <t>{2021: 11516.2724727444, 2022: 11977.16764754086, 2023: 11846.832905431918, 2024: 11716.498163323035, 2025: 11586.16342121415, 2026: 11455.828679105209, 2027: 11325.493936996325, 2028: 11195.159194887383, 2029: 11064.8244527785, 2030: 10934.489710669615, 2031: 10804.154968560673, 2032: 10673.82022645179, 2033: 10543.485484342847, 2034: 10413.150742233964, 2035: 10282.816000125022, 2036: 10152.481258016138, 2037: 10022.146515907254, 2038: 9891.811773798312, 2039: 9761.477031689428, 2040: 9631.142289580486, 2041: 9500.807547471602, 2042: 9370.472805362719, 2043: 9240.138063253777, 2044: 9109.803321144893, 2045: 8979.46857903595, 2046: 8849.133836927067, 2047: 8718.799094818125, 2048: 8588.464352709241, 2049: 8458.129610600357, 2050: 8327.794868491415}</t>
         </is>
       </c>
-      <c r="T14" t="n">
+      <c r="S14" t="n">
         <v>296016.1952845945</v>
       </c>
     </row>
@@ -1504,15 +1434,10 @@
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>{2021: 50848.2087199788, 2022: 39646.026565104046, 2023: 30911.75602776654, 2024: 24101.70056136755, 2025: 18791.943409104217, 2026: 14651.95935829592, 2027: 11424.039992220736, 2028: 8907.251689171857, 2029: 6944.927775837737, 2030: 5414.9162384437805, 2031: 4221.9759248432565, 2032: 3291.8479114053484, 2033: 2566.6329852949275, 2034: 2001.187496657943, 2035: 1560.313227377894, 2036: 1216.566349528094, 2037: 948.5490841421049, 2038: 739.5777183676312, 2039: 576.644066870373, 2040: 449.6057298626107, 2041: 350.5547424122417, 2042: 273.3253143043017, 2043: 213.1100179260803, 2044: 166.16053238995397, 2045: 129.5543156196889, 2046: 101.01268005265929, 2047: 78.75894741610782, 2048: 61.40785290380918, 2049: 47.87931431247938, 2050: 37.331198383114156}</t>
-        </is>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
           <t>{2021: 50848.2087199788, 2022: 43566.39934455324, 2023: 40100.144019882195, 2024: 36633.88869521022, 2025: 33167.63337053824, 2026: 29701.378045867197, 2027: 26235.12272119522, 2028: 22768.867396523245, 2029: 19302.6120718522, 2030: 15836.356747180223, 2031: 12370.101422508247, 2032: 8903.846097837202, 2033: 5437.590773165226, 2034: 1971.3354484932497, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T15" t="n">
+      <c r="S15" t="n">
         <v>321419.3805147953</v>
       </c>
     </row>
@@ -1576,15 +1501,10 @@
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>{2021: 117644.889726228, 2022: 83770.93140060206, 2023: 59650.43585025235, 2024: 42475.04996822202, 2025: 30245.04086327351, 2026: 21536.46664348764, 2027: 15335.386636864183, 2028: 10919.808118720644, 2029: 7775.624584712797, 2030: 5536.7582493265945, 2031: 3942.537551485766, 2032: 2807.347123520492, 2033: 1999.016564590161, 2034: 1423.4318200360874, 2035: 1013.5774671315212, 2036: 721.7340988279324, 2037: 513.9223456546868, 2038: 365.9466523642566, 2039: 260.57818561286524, 2040: 185.54887817283682, 2041: 132.12305592743527, 2042: 94.08034195358296, 2043: 66.99141705414621, 2044: 47.70231342416625, 2045: 33.967197681132745, 2046: 24.186888129510365, 2047: 17.22266178332379, 2048: 12.263672669029999, 2049: 8.732544900738795, 2050: 6.21814871461754}</t>
-        </is>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
           <t>{2021: 117644.889726228, 2022: 119959.68802870438, 2023: 122938.58552350104, 2024: 125917.4830182977, 2025: 128896.38051309437, 2026: 131875.27800789196, 2027: 134854.17550268862, 2028: 137833.0729974853, 2029: 140811.97049228195, 2030: 143790.86798707955, 2031: 146769.7654818762, 2032: 149748.66297667287, 2033: 152727.56047146954, 2034: 155706.45796626713, 2035: 158685.3554610638, 2036: 161664.25295586046, 2037: 164643.15045065712, 2038: 167622.04794545472, 2039: 170600.94544025138, 2040: 173579.84293504804, 2041: 176558.7404298447, 2042: 179537.6379246423, 2043: 182516.53541943897, 2044: 185495.43291423563, 2045: 188474.3304090323, 2046: 191453.2279038299, 2047: 194432.12539862655, 2048: 197411.02289342321, 2049: 200389.92038821988, 2050: 203368.81788301654}</t>
         </is>
       </c>
-      <c r="T16" t="n">
+      <c r="S16" t="n">
         <v>4645401.371641561</v>
       </c>
     </row>
@@ -1648,15 +1568,10 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>{2021: 40428.9261016411, 2022: 30459.4578021449, 2023: 22948.38520489381, 2024: 17289.486468636518, 2025: 13026.029486615827, 2026: 9813.908845354277, 2027: 7393.872931416577, 2028: 5570.5996242072515, 2029: 4196.931765132822, 2030: 3162.0000411872325, 2031: 2382.2746758789963, 2032: 1794.8237056959379, 2033: 1352.2337147539422, 2034: 1018.7830779782554, 2035: 767.5588536584535, 2036: 578.284628557654, 2037: 435.6840000374363, 2038: 328.2476111496641, 2039: 247.30422557680072, 2040: 186.3208684868558, 2041: 140.3755473758183, 2042: 105.75999597409955, 2043: 79.68037850991385, 2044: 60.031798044300146, 2045: 45.22840935028006, 2046: 34.07542467488572, 2047: 25.67268191505875, 2048: 19.34199215417394, 2049: 14.572402748178968, 2050: 10.978958121917572}</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
           <t>{2021: 40428.9261016411, 2022: 42132.43465925561, 2023: 42216.868159533944, 2024: 42301.30165981231, 2025: 42385.73516009064, 2026: 42470.168660369, 2027: 42554.60216064734, 2028: 42639.0356609257, 2029: 42723.46916120403, 2030: 42807.902661482396, 2031: 42892.33616176073, 2032: 42976.76966203909, 2033: 43061.203162317426, 2034: 43145.63666259579, 2035: 43230.07016287412, 2036: 43314.503663152485, 2037: 43398.93716343082, 2038: 43483.37066370918, 2039: 43567.804163987515, 2040: 43652.23766426588, 2041: 43736.67116454421, 2042: 43821.104664822575, 2043: 43905.53816510091, 2044: 43989.97166537927, 2045: 44074.405165657605, 2046: 44158.83866593597, 2047: 44243.2721662143, 2048: 44327.705666492664, 2049: 44412.13916677103, 2050: 44496.57266704936}</t>
         </is>
       </c>
-      <c r="T17" t="n">
+      <c r="S17" t="n">
         <v>1254086.782948718</v>
       </c>
     </row>
@@ -1720,15 +1635,10 @@
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>{2021: 83466.9995600362, 2022: 63036.603584922676, 2023: 47606.9993227029, 2024: 35954.13229170117, 2025: 27153.562443341903, 2026: 20507.12689663917, 2027: 15487.55359199578, 2028: 11696.631979404769, 2029: 8833.622356751075, 2030: 6671.397721933236, 2031: 5038.425434861519, 2032: 3805.159266580679, 2033: 2873.7622956293235, 2034: 2170.3453530348092, 2035: 1639.1052797246975, 2036: 1237.897975206847, 2037: 934.8950405910406, 2038: 706.0587822479291, 2039: 533.2352642220301, 2040: 402.71412828357626, 2041: 304.14092990607645, 2042: 229.69570409259805, 2043: 173.4725954013739, 2044: 131.0113372566923, 2045: 98.94341207078533, 2046: 74.72482150936253, 2047: 56.43426715071616, 2048: 42.62073089648482, 2049: 32.18836345122136, 2050: 24.30954889498095}</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
           <t>{2021: 83466.9995600362, 2022: 76461.93214879185, 2023: 73881.20066807512, 2024: 71300.46918735933, 2025: 68719.7377066426, 2026: 66139.0062259268, 2027: 63558.274745210074, 2028: 60977.54326449428, 2029: 58396.81178377755, 2030: 55816.08030306175, 2031: 53235.34882234596, 2032: 50654.61734162923, 2033: 48073.88586091343, 2034: 45493.154380196705, 2035: 42912.42289948091, 2036: 40331.69141876418, 2037: 37750.959938048385, 2038: 35170.22845733166, 2039: 32589.49697661586, 2040: 30008.765495900065, 2041: 27428.034015183337, 2042: 24847.30253446754, 2043: 22266.571053750813, 2044: 19685.839573035017, 2045: 17105.10809231829, 2046: 14524.376611602493, 2047: 11943.645130885765, 2048: 9362.913650169969, 2049: 6782.182169454172, 2050: 4201.450688737445}</t>
         </is>
       </c>
-      <c r="T18" t="n">
+      <c r="S18" t="n">
         <v>1209251.82557982</v>
       </c>
     </row>
@@ -1792,15 +1702,10 @@
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>{2021: 44760.6499832772, 2022: 34827.74802822287, 2023: 27099.071018194656, 2024: 21085.476139716666, 2025: 16406.36698357861, 2026: 12765.605851928143, 2027: 9932.771400876987, 2028: 7728.575427321216, 2029: 6013.515838139551, 2030: 4679.047655757871, 2031: 3640.7132789104944, 2032: 2832.7972173833946, 2033: 2204.1670024662203, 2034: 1715.0370471093931, 2035: 1334.4506426539622, 2036: 1038.3207293865464, 2037: 807.9054425944589, 2038: 628.6219524475629, 2039: 489.12352642405205, 2040: 380.5814021766234, 2041: 296.1260210516884, 2042: 230.41225830370115, 2043: 179.28113371484076, 2044: 139.49659251077418, 2045: 108.54069761221132, 2046: 84.45427107644636, 2047: 65.7128990319982, 2048: 51.130452541362274, 2049: 39.784018291621614, 2050: 30.955488026390828}</t>
-        </is>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
           <t>{2021: 44760.6499832772, 2022: 44300.70058780536, 2023: 42809.55385685153, 2024: 41318.407125897706, 2025: 39827.26039494388, 2026: 38336.11366399005, 2027: 36844.96693303622, 2028: 35353.820202082396, 2029: 33862.67347112857, 2030: 32371.52674017474, 2031: 30880.380009220913, 2032: 29389.233278267086, 2033: 27898.086547313258, 2034: 26406.93981635943, 2035: 24915.793085405603, 2036: 23424.646354451776, 2037: 21933.499623498414, 2038: 20442.352892544586, 2039: 18951.20616159076, 2040: 17460.05943063693, 2041: 15968.912699683104, 2042: 14477.765968729276, 2043: 12986.619237775449, 2044: 11495.472506821621, 2045: 10004.325775867794, 2046: 8513.179044913966, 2047: 7022.032313960139, 2048: 5530.885583006311, 2049: 4039.7388520524837, 2050: 2548.592121098656}</t>
         </is>
       </c>
-      <c r="T19" t="n">
+      <c r="S19" t="n">
         <v>700420.7732101972</v>
       </c>
     </row>
@@ -1864,15 +1769,10 @@
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>{2021: 374800.097747541, 2022: 284017.243975418, 2023: 215223.5161094521, 2024: 163092.77999516373, 2025: 123588.98027213626, 2026: 93653.66170813583, 2027: 70969.17809361855, 2028: 53779.25590330878, 2029: 40753.020440765606, 2030: 30881.957125466255, 2031: 23401.830479910786, 2032: 17733.515644281342, 2033: 13438.161488091002, 2034: 10183.213966275569, 2035: 7716.66918684134, 2036: 5847.562816253523, 2037: 4431.185277235846, 2038: 3357.878073000666, 2039: 2544.543829178852, 2040: 1928.2127456242802, 2041: 1461.1673612192237, 2042: 1107.248182202591, 2043: 839.0541491208413, 2044: 635.8211975172953, 2045: 481.8146667124154, 2046: 365.11109407119284, 2047: 276.67507907855173, 2048: 209.6597463789925, 2049: 158.87664837071745, 2050: 120.39406625954868}</t>
-        </is>
-      </c>
-      <c r="S20" t="inlineStr">
-        <is>
           <t>{2021: 374800.097747541, 2022: 353125.6057465039, 2023: 343183.20415410027, 2024: 333240.80256170034, 2025: 323298.4009692967, 2026: 313355.99937689677, 2027: 303413.5977844931, 2028: 293471.1961920932, 2029: 283528.79459968954, 2030: 273586.3930072896, 2031: 263643.99141488597, 2032: 253701.58982248604, 2033: 243759.1882300824, 2034: 233816.78663768247, 2035: 223874.38504527882, 2036: 213931.9834528789, 2037: 203989.58186047524, 2038: 194047.18026807532, 2039: 184104.77867567167, 2040: 174162.37708327174, 2041: 164219.9754908681, 2042: 154277.57389846817, 2043: 144335.17230606452, 2044: 134392.7707136646, 2045: 124450.36912126094, 2046: 114507.96752886102, 2047: 104565.56593645737, 2048: 94623.16434405744, 2049: 84680.76275165752, 2050: 74738.36115925387}</t>
         </is>
       </c>
-      <c r="T20" t="n">
+      <c r="S20" t="n">
         <v>6354058.38842761</v>
       </c>
     </row>
@@ -1936,15 +1836,10 @@
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>{2021: 211464.938310871, 2022: 162301.40928173557, 2023: 124567.91969982698, 2024: 95607.09723355898, 2025: 73379.38261675807, 2026: 56319.39415609154, 2027: 43225.68608508324, 2028: 33176.13702213564, 2029: 25463.009784160367, 2030: 19543.10915811709, 2031: 14999.527502976778, 2032: 11512.284124919319, 2033: 8835.790710511865, 2034: 6781.555826178401, 2035: 5204.910452310838, 2036: 3994.8197008121087, 2037: 3066.063208620885, 2038: 2353.233513229023, 2039: 1806.1297471669127, 2040: 1386.222253449498, 2041: 1063.9391433383105, 2042: 816.5837028735142, 2043: 626.7359820096292, 2044: 481.0259986371748, 2045: 369.1921606654084, 2046: 283.3585957577362, 2047: 217.48049483250895, 2048: 166.9184077727123, 2049: 128.11151121775308, 2050: 98.32683839666716}</t>
-        </is>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
           <t>{2021: 211464.938310871, 2022: 205543.5100499764, 2023: 199704.62742255442, 2024: 193865.74479513243, 2025: 188026.86216771044, 2026: 182187.97954028845, 2027: 176349.09691286646, 2028: 170510.21428544447, 2029: 164671.33165802248, 2030: 158832.4490306005, 2031: 152993.5664031785, 2032: 147154.6837757565, 2033: 141315.80114833452, 2034: 135476.91852091253, 2035: 129638.03589349054, 2036: 123799.15326606855, 2037: 117960.27063864656, 2038: 112121.38801122457, 2039: 106282.50538380258, 2040: 100443.62275638059, 2041: 94604.7401289586, 2042: 88765.85750153661, 2043: 82926.97487411462, 2044: 77088.09224669263, 2045: 71249.20961927064, 2046: 65410.32699184865, 2047: 59571.44436442666, 2048: 53732.56173700467, 2049: 47893.67910958268, 2050: 42054.79648216069}</t>
         </is>
       </c>
-      <c r="T21" t="n">
+      <c r="S21" t="n">
         <v>3674880.515630343</v>
       </c>
     </row>
@@ -2008,15 +1903,10 @@
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>{2021: 87998.058069537, 2022: 68877.31409501539, 2023: 53911.23964570422, 2024: 42197.08329693545, 2025: 33028.24884885374, 2026: 25851.673546854654, 2027: 20234.4674170135, 2028: 15837.801406091035, 2029: 12396.469262535262, 2030: 9702.890334126865, 2031: 7594.5883333589, 2032: 5944.390791507528, 2033: 4652.758033894819, 2034: 3641.7789612520924, 2035: 2850.4714635925934, 2036: 2231.103988244843, 2037: 1746.316379567694, 2038: 1366.866319819312, 2039: 1069.86543682245, 2040: 837.3986806980508, 2041: 655.4436906734182, 2042: 513.0249683286753, 2043: 401.55183713527845, 2044: 314.30025410267064, 2045: 246.00721648727944, 2046: 192.55329823579993, 2047: 150.71416680738744, 2048: 117.96609190577766, 2049: 92.33371443646055, 2050: 72.27089313464224}</t>
-        </is>
-      </c>
-      <c r="S22" t="inlineStr">
-        <is>
           <t>{2021: 87998.058069537, 2022: 81621.35252710804, 2023: 76904.6633452028, 2024: 72187.97416329756, 2025: 67471.28498139232, 2026: 62754.595799487084, 2027: 58037.906617581844, 2028: 53321.217435676605, 2029: 48604.528253771365, 2030: 43887.839071866125, 2031: 39171.149889960885, 2032: 34454.460708055645, 2033: 29737.771526150405, 2034: 25021.082344245166, 2035: 20304.393162339926, 2036: 15587.703980434686, 2037: 10871.014798529446, 2038: 6154.325616624206, 2039: 1437.6364347189665, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T22" t="n">
+      <c r="S22" t="n">
         <v>791529.9296912116</v>
       </c>
     </row>
@@ -2080,15 +1970,10 @@
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>{2021: 42576.6794264777, 2022: 32270.217507671045, 2023: 24458.62270191016, 2024: 18537.96691429767, 2025: 14050.513861876461, 2026: 10649.330678787757, 2027: 8071.465927938973, 2028: 6117.620364221407, 2029: 4636.738760327383, 2030: 3514.3315621969864, 2031: 2663.623500794745, 2032: 2018.844843868595, 2033: 1530.1466225984032, 2034: 1159.7467203882343, 2035: 879.0088711676826, 2036: 666.2287394378931, 2037: 504.95592002771923, 2038: 382.72212841819334, 2039: 290.07725579870686, 2040: 219.85876458066951, 2041: 166.63794005442944, 2042: 126.30018693384882, 2043: 95.72692277829873, 2044: 72.55447491460913, 2045: 54.99134075714827, 2046: 41.679683600878676, 2047: 31.590355884231432, 2048: 23.94333398613794, 2049: 18.1474132318309, 2050: 13.754500822546127}</t>
-        </is>
-      </c>
-      <c r="S23" t="inlineStr">
-        <is>
           <t>{2021: 42576.6794264777, 2022: 37722.64099948527, 2023: 35989.90393816214, 2024: 34257.16687683854, 2025: 32524.429815514944, 2026: 30791.692754191812, 2027: 29058.955692868214, 2028: 27326.21863154508, 2029: 25593.481570221484, 2030: 23860.744508897886, 2031: 22128.007447574753, 2032: 20395.270386251155, 2033: 18662.533324927557, 2034: 16929.796263604425, 2035: 15197.059202280827, 2036: 13464.322140957695, 2037: 11731.585079634096, 2038: 9998.848018310498, 2039: 8266.110956987366, 2040: 6533.373895663768, 2041: 4800.63683434017, 2042: 3067.8997730170377, 2043: 1335.1627116934396, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T23" t="n">
+      <c r="S23" t="n">
         <v>450924.180536207</v>
       </c>
     </row>
@@ -2152,15 +2037,10 @@
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>{2021: 69760.3160810483, 2022: 53745.67477154209, 2023: 41407.460844821464, 2024: 31901.68922250238, 2025: 24578.12564414713, 2026: 18935.807943153748, 2027: 14588.778153853676, 2028: 11239.68138361416, 2029: 8659.425503142089, 2030: 6671.510293324322, 2031: 5139.954097160627, 2032: 3959.9921096357957, 2033: 3050.9100299242796, 2034: 2350.52286797325, 2035: 1810.9212329025374, 2036: 1395.1941316805637, 2037: 1074.9041038940893, 2038: 828.1419813432053, 2039: 638.0282099384596, 2040: 491.5582180932451, 2041: 378.7128500138141, 2042: 291.77301382921695, 2043: 224.79166364668956, 2044: 173.18699691200288, 2045: 133.42904008460016, 2046: 102.79818378595581, 2047: 79.19915022240203, 2048: 61.01766748147113, 2049: 47.01004662833182, 2050: 36.218108217083405}</t>
-        </is>
-      </c>
-      <c r="S24" t="inlineStr">
-        <is>
           <t>{2021: 69760.3160810483, 2022: 69760.62110681739, 2023: 68133.9635529453, 2024: 66507.3059990732, 2025: 64880.64844520064, 2026: 63253.99089132855, 2027: 61627.33333745645, 2028: 60000.67578358436, 2029: 58374.0182297118, 2030: 56747.36067583971, 2031: 55120.703121967614, 2032: 53494.045568095054, 2033: 51867.38801422296, 2034: 50240.73046035087, 2035: 48614.072906478774, 2036: 46987.415352606215, 2037: 45360.75779873412, 2038: 43734.10024486203, 2039: 42107.44269098947, 2040: 40480.785137117375, 2041: 38854.12758324528, 2042: 37227.47002937319, 2043: 35600.81247550063, 2044: 33974.154921628535, 2045: 32347.49736775644, 2046: 30720.839813884348, 2047: 29094.18226001179, 2048: 27467.524706139695, 2049: 25840.8671522676, 2050: 24214.209598395042}</t>
         </is>
       </c>
-      <c r="T24" t="n">
+      <c r="S24" t="n">
         <v>1385408.098466911</v>
       </c>
     </row>
@@ -2224,15 +2104,10 @@
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>{2021: 27906.4222363986, 2022: 22263.397908214833, 2023: 17761.463014524743, 2024: 14169.875133926758, 2025: 11304.5508214543, 2026: 9018.63058545027, 2027: 7194.9517430145415, 2028: 5740.04335733898, 2029: 4579.335473114203, 2030: 3653.33710389318, 2031: 2914.5870777634896, 2032: 2325.221459802714, 2033: 1855.0328718522496, 2034: 1479.9222418772847, 2035: 1180.6636287885322, 2036: 941.9188149884512, 2037: 751.4511605135218, 2038: 599.4984256090502, 2039: 478.27241634988815, 2040: 381.5598081158793, 2041: 304.40368750624174, 2042: 242.84949042446456, 2043: 193.74231463018268, 2044: 154.565218204301, 2045: 123.31021606790159, 2046: 98.37536260334063, 2047: 78.48264544447514, 2048: 62.6124821597764, 2049: 49.95146251768317, 2050: 39.85065791335839}</t>
-        </is>
-      </c>
-      <c r="S25" t="inlineStr">
-        <is>
           <t>{2021: 27906.4222363986, 2022: 25735.92634930974, 2023: 23730.355808773078, 2024: 21724.785268236417, 2025: 19719.214727699757, 2026: 17713.644187163096, 2027: 15708.073646626435, 2028: 13702.503106089775, 2029: 11696.932565553114, 2030: 9691.362025016919, 2031: 7685.791484480258, 2032: 5680.220943943597, 2033: 3674.6504034069367, 2034: 1669.079862870276, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T25" t="n">
+      <c r="S25" t="n">
         <v>192085.7514973687</v>
       </c>
     </row>
@@ -2296,15 +2171,10 @@
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>{2021: 51015.1708721754, 2022: 41816.640637619166, 2023: 34276.6946443674, 2024: 28096.27406287263, 2025: 23030.24327188939, 2026: 18877.6669808786, 2027: 15473.840481569434, 2028: 12683.756922483492, 2029: 10396.752497239835, 2030: 8522.117157358623, 2031: 6985.496756129122, 2032: 5725.943920843121, 2033: 4693.500681375777, 2034: 3847.216974285563, 2035: 3153.526429848606, 2036: 2584.915020448113, 2037: 2118.8297645753523, 2038: 1736.7842020865223, 2039: 1423.625160949094, 2040: 1166.9317330572817, 2041: 956.5226205388512, 2042: 784.0523123023166, 2043: 642.6800738703911, 2044: 526.7986215577814, 2045: 431.8117193270027, 2046: 353.95187708874886, 2047: 290.13091976731454, 2048: 237.81750021323322, 2049: 194.93669772608231, 2050: 159.78771993767464}</t>
-        </is>
-      </c>
-      <c r="S26" t="inlineStr">
-        <is>
           <t>{2021: 51015.1708721754, 2022: 50256.47665881179, 2023: 45880.55149605684, 2024: 41504.62633330189, 2025: 37128.701170546934, 2026: 32752.77600779198, 2027: 28376.85084503703, 2028: 24000.925682282075, 2029: 19625.000519527122, 2030: 15249.07535677217, 2031: 10873.150194017217, 2032: 6497.225031262264, 2033: 2121.2998685091734, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T26" t="n">
+      <c r="S26" t="n">
         <v>339774.2446000042</v>
       </c>
     </row>
@@ -2368,15 +2238,10 @@
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>{2021: 40976.4441285849, 2022: 31613.14525886387, 2023: 24389.401628455566, 2024: 18816.315394221197, 2025: 14516.70403433451, 2026: 11199.572902842814, 2027: 8640.420918510596, 2028: 6666.046490941197, 2029: 5142.825359837817, 2030: 3967.666999882657, 2031: 3061.0375271335847, 2032: 2361.5769021939614, 2033: 1821.9461262856462, 2034: 1405.6233714021284, 2035: 1084.4322089039215, 2036: 836.634648821447, 2037: 645.459928118569, 2038: 497.9694773503723, 2039: 384.18124746398047, 2040: 296.39413180164, 2041: 228.6667606666161, 2042: 176.41539363794573, 2043: 136.10369527124286, 2044: 105.00339842510719, 2045: 81.0096570768965, 2046: 62.49859183745425, 2047: 48.217386946311336, 2048: 37.19950058998025, 2049: 28.699250037849747, 2050: 22.1413443640926}</t>
-        </is>
-      </c>
-      <c r="S27" t="inlineStr">
-        <is>
           <t>{2021: 40976.4441285849, 2022: 38586.685532626696, 2023: 36992.708514933474, 2024: 35398.73149724072, 2025: 33804.75447954796, 2026: 32210.77746185474, 2027: 30616.800444161985, 2028: 29022.82342646923, 2029: 27428.846408776008, 2030: 25834.86939108325, 2031: 24240.89237339003, 2032: 22646.915355697274, 2033: 21052.93833800452, 2034: 19458.961320311297, 2035: 17864.98430261854, 2036: 16271.007284925785, 2037: 14677.030267232563, 2038: 13083.053249539807, 2039: 11489.076231846586, 2040: 9895.09921415383, 2041: 8301.122196461074, 2042: 6707.1451787678525, 2043: 5113.168161075097, 2044: 3519.1911433823407, 2045: 1925.214125689119, 2046: 331.2371079963632, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T27" t="n">
+      <c r="S27" t="n">
         <v>506962.2550720786</v>
       </c>
     </row>
@@ -2440,15 +2305,10 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>{2021: 12572.1630489804, 2022: 9670.000335579323, 2023: 7437.773923691499, 2024: 5720.835472611285, 2025: 4400.235721126103, 2026: 3384.4836989581013, 2027: 2603.208244848671, 2028: 2002.2827021250762, 2029: 1540.0750313244164, 2030: 1184.5635481900804, 2031: 911.1184657633031, 2032: 700.795546109163, 2033: 539.0236461018287, 2034: 414.5952306204456, 2035: 318.88991604785434, 2036: 245.27725127186434, 2037: 188.65736093847886, 2038: 145.10762678444198, 2039: 111.61092918012002, 2040: 85.84662149395285, 2041: 66.02975601101508, 2042: 50.78742299929999, 2043: 39.06363571114115, 2044: 30.046171765670703, 2045: 23.11030249329074, 2046: 17.77551181883415, 2047: 13.672206173555844, 2048: 10.516109103207736, 2049: 8.088566634144525, 2050: 6.221398955916072}</t>
-        </is>
-      </c>
-      <c r="S28" t="inlineStr">
-        <is>
           <t>{2021: 12572.1630489804, 2022: 11940.020779401646, 2023: 11503.75310466357, 2024: 11067.485429925495, 2025: 10631.217755187536, 2026: 10194.95008044946, 2027: 9758.682405711384, 2028: 9322.414730973309, 2029: 8886.147056235233, 2030: 8449.879381497158, 2031: 8013.611706759082, 2032: 7577.344032021123, 2033: 7141.076357283047, 2034: 6704.808682544972, 2035: 6268.541007806896, 2036: 5832.273333068821, 2037: 5396.005658330745, 2038: 4959.7379835926695, 2039: 4523.47030885471, 2040: 4087.2026341166347, 2041: 3650.934959378559, 2042: 3214.6672846404836, 2043: 2778.399609902408, 2044: 2342.1319351643324, 2045: 1905.8642604263732, 2046: 1469.5965856882976, 2047: 1033.328910950222, 2048: 597.0612362121465, 2049: 160.79356147407088, 2050: 0}</t>
         </is>
       </c>
-      <c r="T28" t="n">
+      <c r="S28" t="n">
         <v>175697.4822967506</v>
       </c>
     </row>
@@ -2512,15 +2372,10 @@
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>{2021: 32705.8422088023, 2022: 26252.13621871513, 2023: 21071.91282970519, 2024: 16913.88108774739, 2025: 13576.336223599561, 2026: 10897.375019961732, 2027: 8747.041938992317, 2028: 7021.025021377963, 2029: 5635.595747068558, 2030: 4523.547391965275, 2031: 3630.9348515637794, 2032: 2914.457781456506, 2033: 2339.360111689732, 2034: 1877.7440410991464, 2035: 1507.2167240367976, 2036: 1209.8040007020675, 2037: 971.0784764878947, 2038: 779.4596537545068, 2039: 625.6521656503514, 2040: 502.1948608853339, 2041: 403.0988657051701, 2042: 323.55706557079975, 2043: 259.7109135934841, 2044: 208.46325367851693, 2045: 167.32807848905122, 2046: 134.30993403766234, 2047: 107.80712086155674, 2048: 86.53399610187611, 2049: 69.45860738620027, 2050: 55.75263315414734}</t>
-        </is>
-      </c>
-      <c r="S29" t="inlineStr">
-        <is>
           <t>{2021: 32705.8422088023, 2022: 24712.003630937077, 2023: 20801.318899401464, 2024: 16890.63416786585, 2025: 12979.949436329305, 2026: 9069.264704793692, 2027: 5158.579973257147, 2028: 1247.8952417215332, 2029: 0, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T29" t="n">
+      <c r="S29" t="n">
         <v>107212.5671587072</v>
       </c>
     </row>
@@ -2584,15 +2439,10 @@
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>{2021: 52284.4338444058, 2022: 39689.69575772005, 2023: 30128.8898724286, 2024: 22871.175694723337, 2025: 17361.764070092464, 2026: 13179.508375474434, 2027: 10004.711521130337, 2028: 7594.687887395109, 2029: 5765.212118822729, 2030: 4376.436697311153, 2031: 3322.2018150969393, 2032: 2521.920380343775, 2033: 1914.4178345491969, 2034: 1453.2558893633443, 2035: 1103.1827231522643, 2036: 837.4382856929657, 2037: 635.7087249702856, 2038: 482.5735697872224, 2039: 366.3269687985931, 2040: 278.0828799396019, 2041: 211.09580976010335, 2042: 160.24517909175944, 2043: 121.64389928597824, 2044: 92.34123807883198, 2045: 70.09726176144058, 2046: 53.21161172061763, 2047: 40.393526804827665, 2048: 30.66317585528288, 2049: 23.27675813193988, 2050: 17.669646213097085}</t>
-        </is>
-      </c>
-      <c r="S30" t="inlineStr">
-        <is>
           <t>{2021: 52284.4338444058, 2022: 51536.55996318464, 2023: 50659.67092035944, 2024: 49782.781877534, 2025: 48905.89283470879, 2026: 48029.003791883355, 2027: 47152.11474905815, 2028: 46275.22570623271, 2029: 45398.33666340751, 2030: 44521.44762058207, 2031: 43644.55857775686, 2032: 42767.66953493166, 2033: 41890.78049210622, 2034: 41013.891449281015, 2035: 40137.00240645558, 2036: 39260.11336363037, 2037: 38383.22432080493, 2038: 37506.33527797973, 2039: 36629.44623515429, 2040: 35752.557192329085, 2041: 34875.66814950365, 2042: 33998.77910667844, 2043: 33121.890063853, 2044: 32245.001021027798, 2045: 31368.11197820236, 2046: 30491.222935377154, 2047: 29614.333892551716, 2048: 28737.44484972651, 2049: 27860.555806901306, 2050: 26983.666764075868}</t>
         </is>
       </c>
-      <c r="T30" t="n">
+      <c r="S30" t="n">
         <v>1151193.671085443</v>
       </c>
     </row>
@@ -2656,15 +2506,10 @@
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>{2021: 11311.794475375, 2022: 8576.873037012552, 2023: 6503.190210286616, 2024: 4930.874309164125, 2025: 3738.7067987518108, 2026: 2834.7768875500965, 2027: 2149.395615850664, 2028: 1629.7231481348504, 2029: 1235.6950577083062, 2030: 936.933538308182, 2031: 710.4054108905485, 2032: 538.6463683794059, 2033: 408.41455557694786, 2034: 309.6696812585311, 2035: 234.79895655357697, 2036: 178.0301829181082, 2037: 134.98674140241704, 2038: 102.35017487357547, 2039: 77.60434978885947, 2040: 58.84147353524948, 2041: 44.61501213810186, 2042: 33.82816895111488, 2043: 25.649326532579533, 2044: 19.447932654161754, 2045: 14.745887539791617, 2046: 11.18068450785439, 2047: 8.47746232479009, 2048: 6.427814631362588, 2049: 4.873722742988654, 2050: 3.695373114779692}</t>
-        </is>
-      </c>
-      <c r="S31" t="inlineStr">
-        <is>
           <t>{2021: 11311.794475375, 2022: 12117.62980881147, 2023: 12178.346947960541, 2024: 12239.064087109626, 2025: 12299.781226258696, 2026: 12360.498365407766, 2027: 12421.21550455685, 2028: 12481.93264370592, 2029: 12542.649782855005, 2030: 12603.366922004076, 2031: 12664.08406115316, 2032: 12724.80120030223, 2033: 12785.5183394513, 2034: 12846.235478600385, 2035: 12906.952617749455, 2036: 12967.66975689854, 2037: 13028.38689604761, 2038: 13089.104035196695, 2039: 13149.821174345765, 2040: 13210.53831349485, 2041: 13271.25545264392, 2042: 13331.97259179299, 2043: 13392.689730942075, 2044: 13453.406870091145, 2045: 13514.12400924023, 2046: 13574.8411483893, 2047: 13635.558287538384, 2048: 13696.275426687454, 2049: 13756.992565836525, 2050: 13817.70970498561}</t>
         </is>
       </c>
-      <c r="T31" t="n">
+      <c r="S31" t="n">
         <v>374809.4653352522</v>
       </c>
     </row>
@@ -2728,15 +2573,10 @@
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>{2021: 54733.137085012, 2022: 40245.042906722316, 2023: 29592.00887842851, 2024: 21758.878267085205, 2025: 15999.210644565594, 2026: 11764.15153884084, 2027: 8650.130591025103, 2028: 6360.404232701771, 2029: 4676.778180128771, 2030: 3438.8151044981123, 2031: 2528.5461203119885, 2032: 1859.2292078110818, 2033: 1367.0833287989656, 2034: 1005.2105571643773, 2035: 739.1270473047423, 2036: 543.4769742157524, 2037: 399.6163076155565, 2038: 293.8361713350071, 2039: 216.05648703375007, 2040: 158.86541598088013, 2041: 116.81306468171738, 2042: 85.89214962920138, 2043: 63.1561323044355, 2044: 46.438435466741375, 2045: 34.14598408597048, 2046: 25.107396868147895, 2047: 18.461362129952104, 2048: 13.574561053981984, 2049: 9.981317007444597, 2050: 7.339219942870852}</t>
-        </is>
-      </c>
-      <c r="S32" t="inlineStr">
-        <is>
           <t>{2021: 54733.137085012, 2022: 52015.440560412826, 2023: 51625.62927374488, 2024: 51235.81798707682, 2025: 50846.00670040888, 2026: 50456.19541374082, 2027: 50066.38412707287, 2028: 49676.57284040481, 2029: 49286.76155373675, 2030: 48896.95026706881, 2031: 48507.13898040075, 2032: 48117.327693732805, 2033: 47727.516407064744, 2034: 47337.7051203968, 2035: 46947.89383372874, 2036: 46558.082547060796, 2037: 46168.271260392736, 2038: 45778.45997372479, 2039: 45388.64868705673, 2040: 44998.83740038867, 2041: 44609.02611372073, 2042: 44219.21482705267, 2043: 43829.40354038472, 2044: 43439.59225371666, 2045: 43049.78096704872, 2046: 42659.96968038066, 2047: 42270.158393712714, 2048: 41880.347107044654, 2049: 41490.53582037659, 2050: 41100.72453370865}</t>
         </is>
       </c>
-      <c r="T32" t="n">
+      <c r="S32" t="n">
         <v>1357000.600140414</v>
       </c>
     </row>
@@ -2800,15 +2640,10 @@
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>{2021: 41621.0163834535, 2022: 31705.581838697413, 2023: 24152.315514571997, 2024: 18398.4746813087, 2025: 14015.379618344467, 2026: 10676.475590982696, 2027: 8133.003468250959, 2028: 6195.466364429149, 2029: 4719.511509199879, 2030: 3595.1755001614683, 2031: 2738.691674289941, 2032: 2086.249221070899, 2033: 1589.239071078487, 2034: 1210.6323633501213, 2035: 922.2216756828764, 2036: 702.5194806008711, 2037: 535.1572551775814, 2038: 407.6659732257506, 2039: 310.54712258539973, 2040: 236.56503529831414, 2041: 180.2078069820239, 2042: 137.27664215600927, 2043: 104.5730304209786, 2044: 79.66044710650152, 2045: 60.682824315806506, 2046: 46.226267874442954, 2047: 35.21371764898476, 2048: 26.824703089387427, 2049: 20.43421552380559, 2050: 15.566142994459993}</t>
-        </is>
-      </c>
-      <c r="S33" t="inlineStr">
-        <is>
           <t>{2021: 41621.0163834535, 2022: 38633.08863250399, 2023: 37241.57411222113, 2024: 35850.059591938276, 2025: 34458.54507165542, 2026: 33067.03055137256, 2027: 31675.516031089704, 2028: 30284.001510806847, 2029: 28892.48699052399, 2030: 27500.972470240667, 2031: 26109.45794995781, 2032: 24717.943429674953, 2033: 23326.428909392096, 2034: 21934.91438910924, 2035: 20543.399868826382, 2036: 19151.885348543525, 2037: 17760.370828260668, 2038: 16368.85630797781, 2039: 14977.341787694953, 2040: 13585.827267412096, 2041: 12194.31274712924, 2042: 10802.798226845916, 2043: 9411.28370656306, 2044: 8019.769186280202, 2045: 6628.254665997345, 2046: 5236.740145714488, 2047: 3845.2256254316308, 2048: 2453.7111051487736, 2049: 1062.1965848659165, 2050: 0}</t>
         </is>
       </c>
-      <c r="T33" t="n">
+      <c r="S33" t="n">
         <v>576544.5012349054</v>
       </c>
     </row>
@@ -2872,15 +2707,10 @@
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>{2021: 66296.8699431275, 2022: 50492.60320595059, 2023: 38455.85742887488, 2024: 29288.5071612958, 2025: 22306.52777210416, 2026: 16988.95674359252, 2027: 12939.021894595477, 2028: 9854.536103399278, 2029: 7505.3495236577855, 2030: 5716.176883540897, 2031: 4353.51852181337, 2032: 3315.699269969324, 2033: 2525.2819285803416, 2034: 1923.2892670852648, 2035: 1464.8034197769346, 2036: 1115.6143255777226, 2037: 849.6671339173755, 2038: 647.1181141256075, 2039: 492.85400942694827, 2040: 375.36435668538564, 2041: 285.88262969324086, 2042: 217.73212214931854, 2043: 165.8277631855946, 2044: 126.29669325630864, 2045: 96.1892895439102, 2046: 73.2590789545476, 2047: 55.795116844258004, 2048: 42.49432436348094, 2049: 32.36425883199069, 2050: 24.649062326173777}</t>
-        </is>
-      </c>
-      <c r="S34" t="inlineStr">
-        <is>
           <t>{2021: 66296.8699431275, 2022: 63955.68469541287, 2023: 62352.67324674642, 2024: 60749.66179808043, 2025: 59146.65034941444, 2026: 57543.638900748454, 2027: 55940.627452082, 2028: 54337.61600341601, 2029: 52734.604554750025, 2030: 51131.59310608357, 2031: 49528.581657417584, 2032: 47925.5702087516, 2033: 46322.55876008514, 2034: 44719.547311419155, 2035: 43116.53586275317, 2036: 41513.52441408718, 2037: 39910.51296542073, 2038: 38307.50151675474, 2039: 36704.49006808875, 2040: 35101.4786194223, 2041: 33498.46717075631, 2042: 31895.455722090323, 2043: 30292.44427342387, 2044: 28689.43282475788, 2045: 27086.421376091894, 2046: 25483.409927425906, 2047: 23880.398478759453, 2048: 22277.387030093465, 2049: 20674.375581427477, 2050: 19071.364132761024}</t>
         </is>
       </c>
-      <c r="T34" t="n">
+      <c r="S34" t="n">
         <v>1227504.960913705</v>
       </c>
     </row>
@@ -2944,15 +2774,10 @@
       </c>
       <c r="R35" t="inlineStr">
         <is>
-          <t>{2021: 24807.5654940032, 2022: 19232.90546609901, 2023: 14910.961446713474, 2024: 11560.227946696807, 2025: 8962.458300034385, 2026: 6948.449386139248, 2027: 5387.020754289443, 2028: 4176.470316533385, 2029: 3237.950084189944, 2030: 2510.3304831837077, 2031: 1946.2187405454997, 2032: 1508.8720036760667, 2033: 1169.8041314920756, 2034: 906.9302781958925, 2035: 703.1284189938344, 2036: 545.1241241832084, 2037: 422.62594248678164, 2038: 327.65507769531627, 2039: 254.02569777855427, 2040: 196.94202691980362, 2041: 152.6859774678873, 2042: 118.37497602691688, 2043: 91.77420992913554, 2044: 71.15106495313572, 2045: 55.16227323421664, 2046: 42.76642085920417, 2047: 33.156116415668016, 2048: 25.705402362020024, 2049: 19.92898391082669, 2050: 15.450619839540177}</t>
-        </is>
-      </c>
-      <c r="S35" t="inlineStr">
-        <is>
           <t>{2021: 24807.5654940032, 2022: 23793.173673806945, 2023: 22845.8119354886, 2024: 21898.450197170256, 2025: 20951.08845885168, 2026: 20003.726720533334, 2027: 19056.36498221499, 2028: 18109.00324389641, 2029: 17161.641505578067, 2030: 16214.27976725949, 2031: 15266.918028941145, 2032: 14319.5562906228, 2033: 13372.194552304223, 2034: 12424.832813985879, 2035: 11477.471075667534, 2036: 10530.109337348957, 2037: 9582.747599030612, 2038: 8635.385860712267, 2039: 7688.02412239369, 2040: 6740.6623840753455, 2041: 5793.300645757001, 2042: 4845.9389074384235, 2043: 3898.577169120079, 2044: 2951.2154308015015, 2045: 2003.853692483157, 2046: 1056.4919541648123, 2047: 109.13021584623493, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T35" t="n">
+      <c r="S35" t="n">
         <v>323133.7333124951</v>
       </c>
     </row>
@@ -3016,15 +2841,10 @@
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>{2021: 148655.679597746, 2022: 115118.394217758, 2023: 89147.24767418894, 2024: 69035.29033640095, 2025: 53460.66688731943, 2026: 41399.73758508178, 2027: 32059.799697713257, 2028: 24826.987237423207, 2029: 19225.92471253461, 2030: 14888.483146069133, 2031: 11529.584855092347, 2032: 8928.466763645523, 2033: 6914.170783375031, 2034: 5354.307619347363, 2035: 4146.35550390717, 2036: 3210.9219691932562, 2037: 2486.5257893426206, 2038: 1925.5561363328213, 2039: 1491.143365598967, 2040: 1154.7357642890843, 2041: 894.2229943079177, 2042: 692.4828937305109, 2043: 536.2561253309253, 2044: 415.27470867294676, 2045: 321.58715866784644, 2046: 249.03587543422185, 2047: 192.85243698846145, 2048: 149.34419543987374, 2049: 115.65157827338042, 2050: 89.56014338373635}</t>
-        </is>
-      </c>
-      <c r="S36" t="inlineStr">
-        <is>
           <t>{2021: 148655.679597746, 2022: 145603.3699548114, 2023: 140811.64000288025, 2024: 136019.91005094722, 2025: 131228.18009901606, 2026: 126436.45014708303, 2027: 121644.72019515187, 2028: 116852.9902432207, 2029: 112061.26029128768, 2030: 107269.53033935651, 2031: 102477.80038742349, 2032: 97686.07043549232, 2033: 92894.3404835593, 2034: 88102.61053162813, 2035: 83310.88057969697, 2036: 78519.15062776394, 2037: 73727.42067583278, 2038: 68935.69072389975, 2039: 64143.96077196859, 2040: 59352.23082003556, 2041: 54560.5008681044, 2042: 49768.770916173235, 2043: 44977.04096424021, 2044: 40185.311012309045, 2045: 35393.58106037602, 2046: 30601.851108444855, 2047: 25810.12115651183, 2048: 21018.391204580665, 2049: 16226.661252649501, 2050: 11434.931300716475}</t>
         </is>
       </c>
-      <c r="T36" t="n">
+      <c r="S36" t="n">
         <v>2345665.742353677</v>
       </c>
     </row>
@@ -3088,15 +2908,10 @@
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>{2021: 164615.166399523, 2022: 126530.92266126136, 2023: 97257.59017035805, 2024: 74756.7365099227, 2025: 57461.52710369421, 2026: 44167.61955158812, 2027: 33949.299908676, 2028: 26095.02110348137, 2029: 20057.854748784262, 2030: 15417.40608401553, 2031: 11850.540017189342, 2032: 9108.879790395255, 2033: 7001.511400790151, 2034: 5381.689408952817, 2035: 4136.61840087361, 2036: 3179.5985413018793, 2037: 2443.988278375869, 2038: 1878.5637957907047, 2039: 1443.9520705069604, 2040: 1109.8891539340805, 2041: 853.112758505907, 2042: 655.7424010729486, 2043: 504.0343052869004, 2044: 387.4243612893752, 2045: 297.7924997288495, 2046: 228.89725519485268, 2047: 175.94114520494657, 2048: 135.23660014916683, 2049: 103.94918140723468, 2050: 79.90020677328279}</t>
-        </is>
-      </c>
-      <c r="S37" t="inlineStr">
-        <is>
           <t>{2021: 164615.166399523, 2022: 157400.80845420994, 2023: 152032.29153708182, 2024: 146663.77461995557, 2025: 141295.25770282745, 2026: 135926.74078569934, 2027: 130558.22386857122, 2028: 125189.7069514431, 2029: 119821.19003431499, 2030: 114452.67311718687, 2031: 109084.15620005876, 2032: 103715.63928293064, 2033: 98347.12236580253, 2034: 92978.60544867627, 2035: 87610.08853154816, 2036: 82241.57161442004, 2037: 76873.05469729193, 2038: 71504.53778016381, 2039: 66136.0208630357, 2040: 60767.50394590758, 2041: 55398.98702877946, 2042: 50030.470111651346, 2043: 44661.95319452323, 2044: 39293.43627739698, 2045: 33924.91936026886, 2046: 28556.402443140745, 2047: 23187.88552601263, 2048: 17819.368608884513, 2049: 12450.851691756397, 2050: 7082.334774628282}</t>
         </is>
       </c>
-      <c r="T37" t="n">
+      <c r="S37" t="n">
         <v>2463771.992630616</v>
       </c>
     </row>
@@ -3160,15 +2975,10 @@
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>{2021: 206371.803466873, 2022: 148150.23043234012, 2023: 106354.11625250762, 2024: 76349.51367164907, 2025: 54809.803732066495, 2026: 39346.872569054365, 2027: 28246.34053669567, 2028: 20277.488441164613, 2029: 14556.807348102055, 2030: 10450.043691781175, 2031: 7501.879399013526, 2032: 5385.450642814599, 2033: 3866.108355461697, 2034: 2775.402618555817, 2035: 1992.4065718966638, 2036: 1430.309217551521, 2037: 1026.790659431207, 2038: 737.1126784038892, 2039: 529.1585930132406, 2040: 379.87247372555197, 2041: 272.7029253605247, 2042: 195.76802912525886, 2043: 140.53799084450884, 2044: 100.88944021586865, 2045: 72.42653097505163, 2046: 51.9935721504285, 2047: 37.32515569319505, 2048: 26.794990032431713, 2049: 19.235592658733697, 2050: 13.808851001059713}</t>
-        </is>
-      </c>
-      <c r="S38" t="inlineStr">
-        <is>
           <t>{2021: 206371.803466873, 2022: 194919.10329792276, 2023: 195533.51527403155, 2024: 196147.92725014058, 2025: 196762.3392262496, 2026: 197376.75120235863, 2027: 197991.16317846766, 2028: 198605.57515457645, 2029: 199219.98713068548, 2030: 199834.3991067945, 2031: 200448.81108290353, 2032: 201063.22305901255, 2033: 201677.63503512158, 2034: 202292.04701123037, 2035: 202906.4589873394, 2036: 203520.87096344843, 2037: 204135.28293955745, 2038: 204749.69491566648, 2039: 205364.1068917755, 2040: 205978.5188678843, 2041: 206592.93084399332, 2042: 207207.34282010235, 2043: 207821.75479621137, 2044: 208436.1667723204, 2045: 209050.57874842943, 2046: 209664.99072453822, 2047: 210279.40270064725, 2048: 210893.81467675627, 2049: 211508.2266528653, 2050: 212122.63862897432}</t>
         </is>
       </c>
-      <c r="T38" t="n">
+      <c r="S38" t="n">
         <v>5899229.840358955</v>
       </c>
     </row>
@@ -3232,15 +3042,10 @@
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>{2021: 14794.4064289437, 2022: 11708.292408619738, 2023: 9265.94194800218, 2024: 7333.065932017324, 2025: 5803.3879626136895, 2026: 4592.800904402112, 2027: 3634.742375206768, 2028: 2876.53490954962, 2029: 2276.4895642395927, 2030: 1801.6137120001727, 2031: 1425.796989476307, 2032: 1128.375656589977, 2033: 892.9964306156356, 2034: 706.7173245319634, 2035: 559.2960505444506, 2036: 442.6268626735393, 2037: 350.2948740108249, 2038: 277.22334342089454, 2039: 219.3945382571721, 2040: 173.62882513107252, 2041: 137.40984235924137, 2042: 108.74614144821822, 2043: 86.06169017324807, 2044: 68.10921672106363, 2045: 53.901630249399744, 2046: 42.65774712168256, 2047: 33.759338652242, 2048: 26.717138694309156, 2049: 21.143942047085897, 2050: 16.73331453662563}</t>
-        </is>
-      </c>
-      <c r="S39" t="inlineStr">
-        <is>
           <t>{2021: 14794.4064289437, 2022: 14172.733631623443, 2023: 13352.342267934931, 2024: 12531.95090424642, 2025: 11711.559540557675, 2026: 10891.168176869163, 2027: 10070.776813180419, 2028: 9250.385449491907, 2029: 8429.994085803395, 2030: 7609.6027221146505, 2031: 6789.211358426139, 2032: 5968.819994737394, 2033: 5148.428631048882, 2034: 4328.037267360371, 2035: 3507.645903671626, 2036: 2687.2545399831142, 2037: 1866.8631762943696, 2038: 1046.4718126058578, 2039: 226.08044891734608, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T39" t="n">
+      <c r="S39" t="n">
         <v>136986.529939339</v>
       </c>
     </row>
@@ -3304,15 +3109,10 @@
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>{2021: 31616.9086770801, 2022: 24935.535426243274, 2023: 19666.088590254178, 2024: 15510.1959444066, 2025: 12232.538114015366, 2026: 9647.524070435813, 2027: 7608.7823983968265, 2028: 6000.87329800651, 2029: 4732.752029590825, 2030: 3732.6136815848126, 2031: 2943.82735643952, 2032: 2321.7295556935815, 2033: 1831.0951958475898, 2034: 1444.1430562115977, 2035: 1138.962721071856, 2036: 898.2739448226337, 2037: 708.4481915157518, 2038: 558.7369453992575, 2039: 440.66309702358996, 2040: 347.54094333186345, 2041: 274.09762266872036, 2042: 216.174549198089, 2043: 170.49194103181802, 2044: 134.46310893037293, 2045: 106.0479900328375, 2046: 83.63763324725925, 2047: 65.96309551022114, 2048: 52.02359034272577, 2049: 41.02982025348373, 2050: 32.35928429665893}</t>
-        </is>
-      </c>
-      <c r="S40" t="inlineStr">
-        <is>
           <t>{2021: 31616.9086770801, 2022: 28079.02995773405, 2023: 25869.88128668256, 2024: 23660.732615631074, 2025: 21451.583944579586, 2026: 19242.4352735281, 2027: 17033.28660247568, 2028: 14824.137931424193, 2029: 12614.989260372706, 2030: 10405.840589321218, 2031: 8196.691918269731, 2032: 5987.543247218244, 2033: 3778.394576165825, 2034: 1569.2459051143378, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T40" t="n">
+      <c r="S40" t="n">
         <v>208522.2474470573</v>
       </c>
     </row>
@@ -3376,15 +3176,10 @@
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>{2021: 151025.992624885, 2022: 114577.87322500153, 2023: 86926.02382274538, 2024: 65947.58136934687, 2025: 50032.007645202204, 2026: 37957.44646024405, 2027: 28796.920403422097, 2028: 21847.165762048367, 2029: 16574.642189089718, 2030: 12574.5722208772, 2031: 9539.866063723484, 2032: 7237.545970962202, 2033: 5490.8602837707, 2034: 4165.714010916631, 2035: 3160.3742080339916, 2036: 2397.659827014556, 2037: 1819.0164416180546, 2038: 1380.0209594355947, 2039: 1046.9712119740284, 2040: 794.2986019217219, 2041: 602.605173665895, 2042: 457.1744107950605, 2043: 346.84143286445163, 2044: 263.1358551810828, 2045: 199.63150800654054, 2046: 151.4530924017934, 2047: 114.90189813781629, 2048: 87.17184962224498, 2049: 66.13408037392853, 2050: 50.17349758962933}</t>
-        </is>
-      </c>
-      <c r="S41" t="inlineStr">
-        <is>
           <t>{2021: 151025.992624885, 2022: 148443.25598497968, 2023: 145862.25237088464, 2024: 143281.2487567896, 2025: 140700.24514269456, 2026: 138119.24152859952, 2027: 135538.23791450355, 2028: 132957.2343004085, 2029: 130376.23068631347, 2030: 127795.22707221843, 2031: 125214.2234581234, 2032: 122633.21984402742, 2033: 120052.21622993238, 2034: 117471.21261583734, 2035: 114890.2090017423, 2036: 112309.20538764726, 2037: 109728.20177355129, 2038: 107147.19815945625, 2039: 104566.19454536121, 2040: 101985.19093126617, 2041: 99404.1873171702, 2042: 96823.18370307516, 2043: 94242.18008898012, 2044: 91661.17647488508, 2045: 89080.17286079004, 2046: 86499.16924669407, 2047: 83918.16563259903, 2048: 81337.162018504, 2049: 78756.15840440895, 2050: 76175.15479031391}</t>
         </is>
       </c>
-      <c r="T41" t="n">
+      <c r="S41" t="n">
         <v>3294392.375159043</v>
       </c>
     </row>
@@ -3448,15 +3243,10 @@
       </c>
       <c r="R42" t="inlineStr">
         <is>
-          <t>{2021: 78304.915550821, 2022: 60644.8273977097, 2023: 46967.61453897564, 2024: 36375.02009883049, 2025: 28171.370851554002, 2026: 21817.888581216273, 2027: 16897.305589092735, 2028: 13086.46045690219, 2029: 10135.074280754594, 2030: 7849.313495784554, 2031: 6079.059772862198, 2032: 4708.050932336688, 2033: 3646.2453750541213, 2034: 2823.9085613513057, 2035: 2187.033164973117, 2036: 1693.7921185392402, 2037: 1311.791602785737, 2038: 1015.9435684605871, 2039: 786.8180678276659, 2040: 609.3671844373499, 2041: 471.93675469897033, 2042: 365.5009756415509, 2043: 283.0696313961347, 2044: 219.22900774231022, 2045: 169.78634408302065, 2046: 131.4944720771745, 2047: 101.83855645304494, 2048: 78.87093211304885, 2049: 61.08319038525774, 2050: 47.30711363083201}</t>
-        </is>
-      </c>
-      <c r="S42" t="inlineStr">
-        <is>
           <t>{2021: 78304.915550821, 2022: 75655.85794758704, 2023: 72865.85504138656, 2024: 70075.85213518515, 2025: 67285.84922898468, 2026: 64495.8463227842, 2027: 61705.84341658279, 2028: 58915.84051038232, 2029: 56125.83760418184, 2030: 53335.834697980434, 2031: 50545.83179177996, 2032: 47755.82888557948, 2033: 44965.825979378074, 2034: 42175.8230731776, 2035: 39385.82016697712, 2036: 36595.817260775715, 2037: 33805.81435457524, 2038: 31015.811448374763, 2039: 28225.808542173356, 2040: 25435.80563597288, 2041: 22645.802729771473, 2042: 19855.799823570997, 2043: 17065.79691737052, 2044: 14275.794011169113, 2045: 11485.791104968637, 2046: 8695.788198768161, 2047: 5905.785292566754, 2048: 3115.782386366278, 2049: 325.77948016580194, 2050: 0}</t>
         </is>
       </c>
-      <c r="T42" t="n">
+      <c r="S42" t="n">
         <v>1102895.381763947</v>
       </c>
     </row>
@@ -3520,15 +3310,10 @@
       </c>
       <c r="R43" t="inlineStr">
         <is>
-          <t>{2021: 94224.9197475128, 2022: 73759.70500737232, 2023: 57739.4398143618, 2024: 45198.70178091262, 2025: 35381.753776068465, 2026: 27697.001262080455, 2027: 21681.341285873572, 2028: 16972.254703909268, 2029: 13285.959846130618, 2030: 10400.311102586596, 2031: 8141.411857577471, 2032: 6373.135032299017, 2033: 4988.9197169301315, 2034: 3905.349536112961, 2035: 3057.125763611743, 2036: 2393.132253109636, 2037: 1873.3550477516274, 2038: 1466.4710361812683, 2039: 1147.9603412815984, 2040: 898.6286893104854, 2041: 703.4507135937642, 2042: 550.6644872814682, 2043: 431.0627193820363, 2044: 337.4378997243348, 2045: 264.1479558557142, 2046: 206.77624724357682, 2047: 161.86540715647897, 2048: 126.70899285191744, 2049: 99.1883883752035, 2050: 77.64513131256669}</t>
-        </is>
-      </c>
-      <c r="S43" t="inlineStr">
-        <is>
           <t>{2021: 94224.9197475128, 2022: 83308.24585822597, 2023: 77226.67395072244, 2024: 71145.10204321891, 2025: 65063.53013571352, 2026: 58981.95822820999, 2027: 52900.38632070646, 2028: 46818.81441320293, 2029: 40737.242505699396, 2030: 34655.670598195866, 2031: 28574.098690692335, 2032: 22492.526783188805, 2033: 16410.954875685275, 2034: 10329.382968181744, 2035: 4247.811060678214, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T43" t="n">
+      <c r="S43" t="n">
         <v>660004.8583060782</v>
       </c>
     </row>
@@ -3592,15 +3377,10 @@
       </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>{2021: 39073.6294879557, 2022: 30282.629818240577, 2023: 23469.477515296257, 2024: 18189.18562050431, 2025: 14096.882784098254, 2026: 10925.288705866535, 2027: 8467.257274862142, 2028: 6562.247249375499, 2029: 5085.83683760069, 2030: 3941.5973455065596, 2031: 3054.7951360220504, 2032: 2367.510556019184, 2033: 1834.855033899664, 2034: 1422.0392753339245, 2035: 1102.1010724179164, 2036: 854.1443227997358, 2037: 661.9742439506215, 2038: 513.039644421708, 2039: 397.6131687201806, 2040: 308.1559751935096, 2041: 238.82535217109694, 2042: 185.09311332947908, 2043: 143.44984856321113, 2044: 111.1757141184293, 2045: 86.1627916204894, 2046: 66.77741374278447, 2047: 51.75346460240063, 2048: 40.10968601852072, 2049: 31.085588662786645, 2050: 24.09178227089021}</t>
-        </is>
-      </c>
-      <c r="S44" t="inlineStr">
-        <is>
           <t>{2021: 39073.6294879557, 2022: 38436.26228732243, 2023: 37194.481840590015, 2024: 35952.701393858064, 2025: 34710.92094712611, 2026: 33469.14050039416, 2027: 32227.36005366221, 2028: 30985.579606929794, 2029: 29743.799160197843, 2030: 28502.01871346589, 2031: 27260.23826673394, 2032: 26018.457820001524, 2033: 24776.677373269573, 2034: 23534.89692653762, 2035: 22293.11647980567, 2036: 21051.33603307372, 2037: 19809.555586341303, 2038: 18567.77513960935, 2039: 17325.9946928774, 2040: 16084.21424614545, 2041: 14842.433799413498, 2042: 13600.653352681082, 2043: 12358.87290594913, 2044: 11117.09245921718, 2045: 9875.312012485228, 2046: 8633.531565752812, 2047: 7391.751119020861, 2048: 6149.97067228891, 2049: 4908.1902255569585, 2050: 3666.4097788250074}</t>
         </is>
       </c>
-      <c r="T44" t="n">
+      <c r="S44" t="n">
         <v>628192.3548136981</v>
       </c>
     </row>
@@ -3664,15 +3444,10 @@
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>{2021: 73237.1079251592, 2022: 55940.59143369857, 2023: 42729.01891688384, 2024: 32637.64309255362, 2025: 24929.56247624039, 2026: 19041.91070091597, 2027: 14544.754384969081, 2028: 11109.698151714429, 2029: 8485.904248046836, 2030: 6481.775645354215, 2031: 4950.965069677413, 2032: 3781.688299985327, 2033: 2888.561360659675, 2034: 2206.365536347468, 2035: 1685.2849125109503, 2036: 1287.2686730952257, 2037: 983.2525197555141, 2038: 751.0363126300128, 2039: 573.6629518418512, 2040: 438.1801209631086, 2041: 334.69447136299647, 2042: 255.64918124249394, 2043: 195.2721346241612, 2044: 149.1544247290489, 2045: 113.92840283674998, 2046: 87.02176282407595, 2047: 66.4697039232693, 2048: 50.77145528043373, 2049: 38.78068532197392, 2050: 29.621793303639098}</t>
-        </is>
-      </c>
-      <c r="S45" t="inlineStr">
-        <is>
           <t>{2021: 73237.1079251592, 2022: 71380.21577896085, 2023: 69649.26468487224, 2024: 67918.31359078363, 2025: 66187.36249669502, 2026: 64456.411402606405, 2027: 62725.460308517795, 2028: 60994.509214429185, 2029: 59263.558120340575, 2030: 57532.607026251964, 2031: 55801.655932163354, 2032: 54070.704838074744, 2033: 52339.75374398613, 2034: 50608.80264989752, 2035: 48877.85155580891, 2036: 47146.90046172077, 2037: 45415.94936763216, 2038: 43684.99827354355, 2039: 41954.04717945494, 2040: 40223.09608536633, 2041: 38492.14499127772, 2042: 36761.19389718911, 2043: 35030.2428031005, 2044: 33299.291709011886, 2045: 31568.340614923276, 2046: 29837.389520834666, 2047: 28106.438426746055, 2048: 26375.487332657445, 2049: 24644.536238568835, 2050: 22913.585144480225}</t>
         </is>
       </c>
-      <c r="T45" t="n">
+      <c r="S45" t="n">
         <v>1392421.874780235</v>
       </c>
     </row>
@@ -3736,15 +3511,10 @@
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>{2021: 40493.1623118517, 2022: 31384.371252725443, 2023: 24324.5699445067, 2024: 18852.84552048549, 2025: 14611.96580371847, 2026: 11325.056709186874, 2027: 8777.525980361906, 2028: 6803.053116142851, 2029: 5272.730813284669, 2030: 4086.6490022533326, 2031: 3167.3720239122913, 2032: 2454.8830918267195, 2033: 1902.6659795690596, 2034: 1474.6681183565797, 2035: 1142.9468349404533, 2036: 885.8450598065524, 2037: 686.57740324777, 2038: 532.1342885327953, 2039: 412.4325963726999, 2040: 319.6573688565143, 2041: 247.75159471617673, 2042: 192.02076555901598, 2043: 148.82638575186974, 2044: 115.3484261531961, 2045: 89.40121302282023, 2046: 69.29073205850783, 2047: 53.704031375708354, 2048: 41.62350288878124, 2049: 32.26044578686952, 2050: 25.003574666659233}</t>
-        </is>
-      </c>
-      <c r="S46" t="inlineStr">
-        <is>
           <t>{2021: 40493.1623118517, 2022: 37062.474532493856, 2023: 35081.49371446064, 2024: 33100.51289642742, 2025: 31119.5320783942, 2026: 29138.551260360982, 2027: 27157.570442327764, 2028: 25176.589624294546, 2029: 23195.608806261327, 2030: 21214.627988227643, 2031: 19233.647170194425, 2032: 17252.666352161206, 2033: 15271.685534127988, 2034: 13290.70471609477, 2035: 11309.723898061551, 2036: 9328.743080028333, 2037: 7347.762261994649, 2038: 5366.78144396143, 2039: 3385.800625928212, 2040: 1404.8198078949936, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T46" t="n">
+      <c r="S46" t="n">
         <v>385685.8773896218</v>
       </c>
     </row>
@@ -3808,15 +3578,10 @@
       </c>
       <c r="R47" t="inlineStr">
         <is>
-          <t>{2021: 18740.6365816607, 2022: 14394.321289121646, 2023: 11056.000391001658, 2024: 8491.900534289636, 2025: 6522.464918051196, 2026: 5009.779428695035, 2027: 3847.9148971298387, 2028: 2955.50917286803, 2029: 2270.0695583009215, 2030: 1743.5966184208635, 2031: 1339.2229135234584, 2032: 1028.6312746640963, 2033: 790.071830859956, 2034: 606.8389259525891, 2035: 466.1012678435395, 2036: 358.00338869878, 2037: 274.9754938723586, 2038: 211.20337018364427, 2039: 162.221232695142, 2040: 124.59899818004565, 2041: 95.70208590786984, 2042: 73.50692526341743, 2043: 56.45925070936526, 2044: 43.36526088174407, 2045: 33.30801999166072, 2046: 25.583247355302234, 2047: 19.649998571108263, 2048: 15.092784683744666, 2049: 11.592476645001103, 2050: 8.903957591711544}</t>
-        </is>
-      </c>
-      <c r="S47" t="inlineStr">
-        <is>
           <t>{2021: 18740.6365816607, 2022: 17459.580516267102, 2023: 16743.24152156408, 2024: 16026.902526861057, 2025: 15310.563532158034, 2026: 14594.224537455011, 2027: 13877.885542751988, 2028: 13161.546548048966, 2029: 12445.207553345943, 2030: 11728.86855864292, 2031: 11012.529563939897, 2032: 10296.190569236875, 2033: 9579.851574533852, 2034: 8863.512579830829, 2035: 8147.173585127806, 2036: 7430.8345904247835, 2037: 6714.495595721761, 2038: 5998.156601018738, 2039: 5281.817606315715, 2040: 4565.4786116126925, 2041: 3849.1396169096697, 2042: 3132.800622206647, 2043: 2416.461627503624, 2044: 1700.1226328006014, 2045: 983.7836380975787, 2046: 267.4446433945559, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T47" t="n">
+      <c r="S47" t="n">
         <v>230958.1327866011</v>
       </c>
     </row>
@@ -3880,15 +3645,10 @@
       </c>
       <c r="R48" t="inlineStr">
         <is>
-          <t>{2021: 20970.6401639379, 2022: 15888.981164371064, 2023: 12038.722731787659, 2024: 9121.468740730155, 2025: 6911.1311757707235, 2026: 5236.408245903459, 2027: 3967.508446937832, 2028: 3006.0916829465355, 2029: 2277.6478808141865, 2030: 1725.722438343082, 2031: 1307.5409764990586, 2032: 990.6943128499912, 2033: 750.6267406939833, 2034: 568.7329547940864, 2035: 430.9161349218168, 2036: 326.4954382732885, 2037: 247.3782311089546, 2038: 187.43290733321695, 2039: 142.01368727513167, 2040: 107.60056844033554, 2041: 81.52652431489093, 2042: 61.77080905062338, 2043: 46.802349086181316, 2044: 35.46108450983083, 2045: 26.868064085797023, 2046: 20.35732628307987, 2047: 15.424287067070296, 2048: 11.686634493112741, 2049: 8.854699421874422, 2050: 6.709006078520719}</t>
-        </is>
-      </c>
-      <c r="S48" t="inlineStr">
-        <is>
           <t>{2021: 20970.6401639379, 2022: 21251.269496103225, 2023: 21070.1846784777, 2024: 20889.099860852235, 2025: 20708.01504322671, 2026: 20526.930225601245, 2027: 20345.84540797572, 2028: 20164.760590350255, 2029: 19983.67577272473, 2030: 19802.590955099266, 2031: 19621.50613747374, 2032: 19440.421319848276, 2033: 19259.33650222275, 2034: 19078.251684597286, 2035: 18897.166866971762, 2036: 18716.082049346296, 2037: 18534.997231720772, 2038: 18353.912414095306, 2039: 18172.827596469782, 2040: 17991.742778844316, 2041: 17810.657961218792, 2042: 17629.573143593327, 2043: 17448.488325967803, 2044: 17267.403508342337, 2045: 17086.318690716813, 2046: 16905.233873091347, 2047: 16724.149055465823, 2048: 16543.064237840357, 2049: 16361.979420214891, 2050: 16180.894602589367}</t>
         </is>
       </c>
-      <c r="T48" t="n">
+      <c r="S48" t="n">
         <v>545161.2522117165</v>
       </c>
     </row>
@@ -3952,15 +3712,10 @@
       </c>
       <c r="R49" t="inlineStr">
         <is>
-          <t>{2021: 23598.9801315176, 2022: 18486.96434666264, 2023: 14482.31444113671, 2024: 11345.15259720397, 2025: 8887.56337786997, 2026: 6962.337625597241, 2027: 5454.15465992711, 2028: 4272.674589212097, 2029: 3347.1269671591467, 2030: 2622.071655672221, 2031: 2054.077970431757, 2032: 1609.1231906213332, 2033: 1260.5546039964224, 2034: 987.493014156993, 2035: 773.5820803932671, 2036: 606.0085757836416, 2037: 474.73487717892874, 2038: 371.89771335934967, 2039: 291.3371564857336, 2040: 228.22764351653672, 2041: 178.78892583913182, 2042: 140.05963304964175, 2043: 109.71988739196709, 2044: 85.95234349242584, 2045: 67.33332969480288, 2046: 52.74757038112105, 2047: 41.321381160303304, 2048: 32.370335328396216, 2049: 25.358266830622195, 2050: 19.865154009972155}</t>
-        </is>
-      </c>
-      <c r="S49" t="inlineStr">
-        <is>
           <t>{2021: 23598.9801315176, 2022: 21641.651221164968, 2023: 20298.447318035644, 2024: 18955.243414906785, 2025: 17612.039511777926, 2026: 16268.835608648602, 2027: 14925.631705519743, 2028: 13582.427802390885, 2029: 12239.22389926156, 2030: 10896.019996132702, 2031: 9552.816093003843, 2032: 8209.612189874984, 2033: 6866.40828674566, 2034: 5523.204383616801, 2035: 4180.000480487943, 2036: 2836.7965773586184, 2037: 1493.5926742297597, 2038: 150.38877110090107, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T49" t="n">
+      <c r="S49" t="n">
         <v>197031.8300000161</v>
       </c>
     </row>
@@ -4024,15 +3779,10 @@
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t>{2021: 66254.0238426647, 2022: 51497.01162157579, 2023: 40026.88519342393, 2024: 31111.54390978842, 2025: 24181.950700718407, 2026: 18795.81230001235, 2027: 14609.349112881948, 2028: 11355.352889000938, 2029: 8826.131693987938, 2030: 6860.253612644196, 2031: 5332.243077888305, 2032: 4144.572175769558, 2033: 3221.4357577572964, 2034: 2503.913046086699, 2035: 1946.206913257812, 2036: 1512.7208012004387, 2037: 1175.786709417245, 2038: 913.8992370205742, 2039: 710.342963343023, 2040: 552.125557316324, 2041: 429.14851948023494, 2042: 333.5626277965678, 2043: 259.26694748314543, 2044: 201.51942830425114, 2045: 156.63423501644854, 2046: 121.74649256222853, 2047: 94.62943046677016, 2048: 73.55225536282485, 2049: 57.169680111917565, 2050: 44.43605852704961}</t>
-        </is>
-      </c>
-      <c r="S50" t="inlineStr">
-        <is>
           <t>{2021: 66254.0238426647, 2022: 62186.69878190849, 2023: 59187.361482637934, 2024: 56188.02418336831, 2025: 53188.686884097755, 2026: 50189.34958482813, 2027: 47190.01228555851, 2028: 44190.67498628795, 2029: 41191.33768701833, 2030: 38192.0003877487, 2031: 35192.66308847815, 2032: 32193.325789208524, 2033: 29193.9884899389, 2034: 26194.651190668344, 2035: 23195.31389139872, 2036: 20195.976592128165, 2037: 17196.63929285854, 2038: 14197.301993588917, 2039: 11197.964694318362, 2040: 8198.627395048738, 2041: 5199.2900957791135, 2042: 2199.952796508558, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T50" t="n">
+      <c r="S50" t="n">
         <v>709186.8534947095</v>
       </c>
     </row>
@@ -4096,15 +3846,10 @@
       </c>
       <c r="R51" t="inlineStr">
         <is>
-          <t>{2021: 17725.0476255144, 2022: 14098.57343432665, 2023: 11214.061427794479, 2024: 8919.709096252549, 2025: 7094.772119276516, 2026: 5643.209983788713, 2027: 4488.631683406352, 2028: 3570.275507584887, 2029: 2839.8113499005385, 2030: 2258.7972513300997, 2031: 1796.6563246516753, 2032: 1429.0675920603603, 2033: 1136.6860510026208, 2034: 904.124609446297, 2035: 719.1443131420414, 2036: 572.0102491638424, 2037: 454.9792290213876, 2038: 361.89228976840053, 2039: 287.85056776220324, 2040: 228.95748736191445, 2041: 182.1136967927998, 2042: 144.85395931653935, 2043: 115.21741581881524, 2044: 91.64439115507163, 2045: 72.89431350717942, 2046: 57.9804271130117, 2047: 46.117862511678084, 2048: 36.682331409882686, 2049: 29.177272414213306, 2050: 23.207718615830878}</t>
-        </is>
-      </c>
-      <c r="S51" t="inlineStr">
-        <is>
           <t>{2021: 17725.0476255144, 2022: 14814.346514039673, 2023: 13207.875206804369, 2024: 11601.403899569064, 2025: 9994.93259233376, 2026: 8388.46128509799, 2027: 6781.989977862686, 2028: 5175.518670627382, 2029: 3569.0473633920774, 2030: 1962.5760561563075, 2031: 356.1047489210032, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T51" t="n">
+      <c r="S51" t="n">
         <v>84714.78012756151</v>
       </c>
     </row>
@@ -4168,15 +3913,10 @@
       </c>
       <c r="R52" t="inlineStr">
         <is>
-          <t>{2021: 21233.9116098986, 2022: 17339.417337300933, 2023: 14159.209057691276, 2024: 11562.280164289188, 2025: 9441.651864367162, 2026: 7709.966257627718, 2027: 6295.887684452579, 2028: 5141.164099911114, 2029: 4198.227418746123, 2030: 3428.2339791131053, 2031: 2799.4644032542346, 2032: 2286.016938410675, 2033: 1866.7404510040221, 2034: 1524.3631194777622, 2035: 1244.780932868406, 2036: 1016.4766852687834, 2037: 830.0455320392044, 2038: 677.8075633638981, 2039: 553.491435372976, 2040: 451.97602622023874, 2041: 369.0794748073746, 2042: 301.3869117423285, 2043: 246.10978602097853, 2044: 200.97099248648306, 2045: 164.11106796687568, 2046: 134.0115919019503, 2047: 109.43263599819943, 2048: 89.36168619111928, 2049: 72.97193278841844, 2050: 59.58821058377304}</t>
-        </is>
-      </c>
-      <c r="S52" t="inlineStr">
-        <is>
           <t>{2021: 21233.9116098986, 2022: 21740.60284140939, 2023: 20222.985016007908, 2024: 18705.367190606426, 2025: 17187.74936520448, 2026: 15670.131539802998, 2027: 14152.513714401517, 2028: 12634.895889000036, 2029: 11117.278063598089, 2030: 9599.660238196608, 2031: 8082.042412795126, 2032: 6564.4245873931795, 2033: 5046.806761991698, 2034: 3529.188936590217, 2035: 2011.5711111887358, 2036: 493.9532857867889, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T52" t="n">
+      <c r="S52" t="n">
         <v>177376.1267589225</v>
       </c>
     </row>
@@ -4240,15 +3980,10 @@
       </c>
       <c r="R53" t="inlineStr">
         <is>
-          <t>{2021: 119802.94296870008, 2022: 108214.88677215017, 2023: 97747.69658345352, 2024: 88292.95554768197, 2025: 79752.73353566235, 2026: 72038.57280522706, 2027: 65070.57177536654, 2028: 58776.55742321841, 2029: 53091.33773176272, 2030: 47956.02644524105, 2031: 43317.433138264656, 2032: 39127.512281081305, 2033: 35342.86559454017, 2034: 31924.292540256833, 2035: 28836.384290054273, 2036: 26047.156969104733, 2037: 23527.72037398536, 2038: 21251.97873430223, 2039: 19196.36041843733, 2040: 17339.573783770134, 2041: 15662.386642523967, 2042: 14147.42705899288, 2043: 12779.003414850584, 2044: 11542.941878817364, 2045: 10426.439597231582, 2046: 9417.932084905955, 2047: 8506.973442732253, 2048: 7684.128161354696, 2049: 6940.873390238315, 2050: 6269.5106598567}</t>
-        </is>
-      </c>
-      <c r="S53" t="inlineStr">
-        <is>
           <t>{2021: 119802.94296870008, 2022: 224084.6072674282, 2023: 212057.23936547711, 2024: 200029.87146352604, 2025: 188002.50356157497, 2026: 175975.13565962762, 2027: 163947.76775767654, 2028: 151920.39985572547, 2029: 139893.0319537744, 2030: 127865.66405182332, 2031: 115838.29614987224, 2032: 103810.92824792117, 2033: 91783.5603459701, 2034: 79756.19244401902, 2035: 67728.82454206795, 2036: 55701.45664011687, 2037: 43674.088738165796, 2038: 31646.72083621472, 2039: 19619.352934263647, 2040: 7591.985032312572, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T53" t="n">
+      <c r="S53" t="n">
         <v>2260829.098331908</v>
       </c>
     </row>
@@ -4312,15 +4047,10 @@
       </c>
       <c r="R54" t="inlineStr">
         <is>
-          <t>{2021: 52270.3371590495, 2022: 40394.22669726283, 2023: 31216.43439002321, 2024: 24123.887389399013, 2025: 18642.806398234898, 2026: 14407.057402978808, 2027: 11133.694068312514, 2028: 8604.057035349038, 2029: 6649.1675640913, 2030: 5138.439821322074, 2031: 3970.95779928007, 2032: 3068.7341667856936, 2033: 2371.500746773285, 2034: 1832.6826262168706, 2035: 1416.2869706059012, 2036: 1094.4987170248185, 2037: 845.8225390977714, 2038: 653.6469678014049, 2039: 505.1347519914974, 2040: 390.3653351713184, 2041: 301.67216629352146, 2042: 233.13057722271012, 2043: 180.1620172784271, 2044: 139.22820788465143, 2045: 107.5947869789581, 2046: 83.14865472260074, 2047: 64.25681927815295, 2048: 49.65731360922327, 2049: 38.374896588184086, 2050: 29.65590727969418}</t>
-        </is>
-      </c>
-      <c r="S54" t="inlineStr">
-        <is>
           <t>{2021: 52270.3371590495, 2022: 58872.26422920241, 2023: 59186.91165715468, 2024: 59501.55908510694, 2025: 59816.20651305921, 2026: 60130.853941011475, 2027: 60445.50136896374, 2028: 60760.148796916124, 2029: 61074.79622486839, 2030: 61389.44365282066, 2031: 61704.09108077292, 2032: 62018.73850872519, 2033: 62333.385936677456, 2034: 62648.03336462972, 2035: 62962.68079258199, 2036: 63277.328220534255, 2037: 63591.97564848652, 2038: 63906.62307643879, 2039: 64221.270504391054, 2040: 64535.91793234332, 2041: 64850.565360295586, 2042: 65165.21278824797, 2043: 65479.860216200235, 2044: 65794.5076441525, 2045: 66109.15507210477, 2046: 66423.80250005703, 2047: 66738.4499280093, 2048: 67053.09735596157, 2049: 67367.74478391383, 2050: 67682.3922118661}</t>
         </is>
       </c>
-      <c r="T54" t="n">
+      <c r="S54" t="n">
         <v>1827336.490869086</v>
       </c>
     </row>
@@ -4384,15 +4114,10 @@
       </c>
       <c r="R55" t="inlineStr">
         <is>
-          <t>{2021: 22395.1016488455, 2022: 17106.997508584496, 2023: 13067.561306371772, 2024: 9981.94793739198, 2025: 7624.93339719169, 2026: 5824.475310457245, 2027: 4449.155274539267, 2028: 3398.5864136844625, 2029: 2596.085975551104, 2030: 1983.0781307533541, 2031: 1514.8184265497575, 2032: 1157.1278155051593, 2033: 883.8978704962051, 2034: 675.1850875926353, 2035: 515.7551768413632, 2036: 393.9710863388554, 2037: 300.9435946364891, 2038: 229.88247181884452, 2039: 175.60084943284673, 2040: 134.1366224121556, 2041: 102.4632484993868, 2042: 78.26883593943616, 2043: 59.78739469060489, 2044: 45.6699339013566, 2045: 34.885996845118235, 2046: 26.64844618576177, 2047: 20.35600952634996, 2048: 15.549391546072426, 2049: 11.877749277926533, 2050: 9.073083502416488}</t>
-        </is>
-      </c>
-      <c r="S55" t="inlineStr">
-        <is>
           <t>{2021: 22395.1016488455, 2022: 21510.56886509573, 2023: 20901.21498796367, 2024: 20291.86111083161, 2025: 19682.50723369955, 2026: 19073.15335656749, 2027: 18463.79947943543, 2028: 17854.44560230337, 2029: 17245.09172517131, 2030: 16635.73784803925, 2031: 16026.38397090719, 2032: 15417.03009377513, 2033: 14807.67621664307, 2034: 14198.32233951101, 2035: 13588.968462379184, 2036: 12979.614585247124, 2037: 12370.260708115064, 2038: 11760.906830983004, 2039: 11151.552953850944, 2040: 10542.199076718884, 2041: 9932.845199586824, 2042: 9323.491322454764, 2043: 8714.137445322704, 2044: 8104.783568190644, 2045: 7495.429691058584, 2046: 6886.075813926524, 2047: 6276.7219367944635, 2048: 5667.3680596624035, 2049: 5058.0141825303435, 2050: 4448.6603053982835}</t>
         </is>
       </c>
-      <c r="T55" t="n">
+      <c r="S55" t="n">
         <v>385382.0436438872</v>
       </c>
     </row>
@@ -4456,15 +4181,10 @@
       </c>
       <c r="R56" t="inlineStr">
         <is>
-          <t>{2021: 22545.4803600213, 2022: 17389.39936924739, 2023: 13412.498008221448, 2024: 10345.101576002862, 2025: 7979.209134064082, 2026: 6154.388909319112, 2027: 4746.899374456964, 2028: 3661.298303248251, 2029: 2823.9708087138542, 2030: 2178.1374987645345, 2031: 1680.0042510655248, 2032: 1295.7925223725047, 2033: 999.4488168536244, 2034: 770.8779918572135, 2035: 594.5806011363183, 2036: 458.6018734247478, 2037: 353.72105633239414, 2038: 272.8261547615231, 2039: 210.4316646957324, 2040: 162.3065997661534, 2041: 125.18758698098408, 2042: 96.55757656620936, 2043: 74.47516017507076, 2044: 57.44292349030928, 2045: 44.30590617538592, 2046: 34.17328371793724, 2047: 26.357960391190737, 2048: 20.329977116565946, 2049: 15.68057480267817, 2050: 12.094476286548748}</t>
-        </is>
-      </c>
-      <c r="S56" t="inlineStr">
-        <is>
           <t>{2021: 22545.4803600213, 2022: 21462.501178817358, 2023: 20647.559440587414, 2024: 19832.61770235747, 2025: 19017.675964127295, 2026: 18202.73422589735, 2027: 17387.792487667408, 2028: 16572.85074943723, 2029: 15757.909011207288, 2030: 14942.967272977345, 2031: 14128.025534747401, 2032: 13313.083796517225, 2033: 12498.142058287282, 2034: 11683.200320057338, 2035: 10868.258581827395, 2036: 10053.316843597218, 2037: 9238.375105367275, 2038: 8423.433367137332, 2039: 7608.491628907155, 2040: 6793.549890677212, 2041: 5978.608152447268, 2042: 5163.666414217325, 2043: 4348.724675987149, 2044: 3533.782937757205, 2045: 2718.841199527262, 2046: 1903.8994612973183, 2047: 1088.957723067142, 2048: 274.01598483719863, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T56" t="n">
+      <c r="S56" t="n">
         <v>304715.7218893475</v>
       </c>
     </row>
@@ -4528,15 +4248,10 @@
       </c>
       <c r="R57" t="inlineStr">
         <is>
-          <t>{2021: 379312.20194903, 2022: 287227.6995970893, 2023: 217498.27975985254, 2024: 164696.86511730307, 2025: 124713.89387270946, 2026: 94437.47040246111, 2027: 71511.16478744875, 2028: 54150.61063647866, 2029: 41004.62691412033, 2030: 31050.054812004968, 2031: 23512.124762108586, 2032: 17804.155714894958, 2033: 13481.893445507514, 2034: 10208.93401443107, 2035: 7730.541272430623, 2036: 5853.820612443604, 2037: 4432.705881136238, 2038: 3356.5909735757364, 2039: 2541.7213020689073, 2040: 1924.6751326715078, 2041: 1457.4274383697384, 2042: 1103.6120860379544, 2043: 835.691441222927, 2044: 632.8130996104677, 2045: 479.1869334602704, 2046: 362.856137681729, 2047: 274.7666254222229, 2048: 208.06234373837827, 2049: 157.55166339938543, 2050: 119.3033116608816}</t>
-        </is>
-      </c>
-      <c r="S57" t="inlineStr">
-        <is>
           <t>{2021: 379312.20194903, 2022: 429001.1505482327, 2023: 437020.7483017165, 2024: 445040.3460552003, 2025: 453059.943808686, 2026: 461079.5415621698, 2027: 469099.1393156536, 2028: 477118.7370691374, 2029: 485138.3348226212, 2030: 493157.93257610686, 2031: 501177.53032959066, 2032: 509197.12808307447, 2033: 517216.72583655827, 2034: 525236.3235900421, 2035: 533255.9213435277, 2036: 541275.5190970115, 2037: 549295.1168504953, 2038: 557314.7146039791, 2039: 565334.312357463, 2040: 573353.9101109467, 2041: 581373.5078644324, 2042: 589393.1056179162, 2043: 597412.7033714, 2044: 605432.3011248838, 2045: 613451.8988783676, 2046: 621471.4966318533, 2047: 629491.0943853371, 2048: 637510.6921388209, 2049: 645530.2898923047, 2050: 653549.8876457885}</t>
         </is>
       </c>
-      <c r="T57" t="n">
+      <c r="S57" t="n">
         <v>15559871.21096494</v>
       </c>
     </row>
@@ -4600,15 +4315,10 @@
       </c>
       <c r="R58" t="inlineStr">
         <is>
-          <t>{2021: 235613.396453782, 2022: 179897.29311146846, 2023: 137356.51943365598, 2024: 104875.47146825607, 2025: 80075.30010981033, 2026: 61139.688793837755, 2027: 46681.829986040444, 2028: 35642.85808182302, 2029: 27214.30013820958, 2030: 20778.86487981307, 2031: 15865.233480221868, 2032: 12113.54108310739, 2033: 9249.020996448544, 2034: 7061.88131165375, 2035: 5391.940150101698, 2036: 4116.8942522867765, 2037: 3143.361723737274, 2038: 2400.0429257487494, 2039: 1832.4986278028696, 2040: 1399.162983658628, 2041: 1068.2993291993375, 2042: 815.6758505599541, 2043: 622.790892965692, 2044: 475.5179353351401, 2045: 363.0709912096463, 2046: 277.21466397487046, 2047: 211.66100234740705, 2048: 161.60898298933512, 2049: 123.39289284844084, 2050: 94.2138594270566}</t>
-        </is>
-      </c>
-      <c r="S58" t="inlineStr">
-        <is>
           <t>{2021: 235613.396453782, 2022: 214052.3302645944, 2023: 204649.64151547477, 2024: 195246.95276635513, 2025: 185844.2640172355, 2026: 176441.57526811212, 2027: 167038.88651899248, 2028: 157636.19776987284, 2029: 148233.5090207532, 2030: 138830.82027162984, 2031: 129428.1315225102, 2032: 120025.44277339056, 2033: 110622.75402427092, 2034: 101220.06527514756, 2035: 91817.37652602792, 2036: 82414.68777690828, 2037: 73011.99902778864, 2038: 63609.310278665274, 2039: 54206.621529545635, 2040: 44803.932780425996, 2041: 35401.244031306356, 2042: 25998.55528218299, 2043: 16595.866533063352, 2044: 7193.177783943713, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T58" t="n">
+      <c r="S58" t="n">
         <v>2662130.040785089</v>
       </c>
     </row>
@@ -4672,15 +4382,10 @@
       </c>
       <c r="R59" t="inlineStr">
         <is>
-          <t>{2021: 2043704.69976698, 2022: 1563724.8916275904, 2023: 1196472.042646142, 2024: 915471.357205179, 2025: 700465.8495902339, 2026: 535956.0433873861, 2027: 410082.6337379612, 2028: 313771.56497871986, 2029: 240079.8933907191, 2030: 183695.2791257809, 2031: 140553.0263135439, 2032: 107543.06425245093, 2033: 82285.74632755751, 2034: 62960.30428135057, 2035: 48173.591321887376, 2036: 36859.651924135236, 2037: 28202.878437902928, 2038: 21579.21495895382, 2039: 16511.169924376052, 2040: 12633.394346836663, 2041: 9666.344265953989, 2042: 7396.128776059143, 2043: 5659.090900033391, 2044: 4330.009763824676, 2045: 3313.0735812542575, 2046: 2534.9727029505502, 2047: 1939.6148160016558, 2048: 1484.0813197216212, 2049: 1135.5333777491553, 2050: 868.8446076689879}</t>
-        </is>
-      </c>
-      <c r="S59" t="inlineStr">
-        <is>
           <t>{2021: 2043704.69976698, 2022: 2031081.8973403573, 2023: 1990184.2466693372, 2024: 1949286.595998302, 2025: 1908388.945327267, 2026: 1867491.294656232, 2027: 1826593.643985197, 2028: 1785695.993314162, 2029: 1744798.3426431417, 2030: 1703900.6919721067, 2031: 1663003.0413010716, 2032: 1622105.3906300366, 2033: 1581207.7399590015, 2034: 1540310.0892879814, 2035: 1499412.4386169463, 2036: 1458514.7879459113, 2037: 1417617.1372748762, 2038: 1376719.4866038412, 2039: 1335821.8359328061, 2040: 1294924.185261786, 2041: 1254026.534590751, 2042: 1213128.8839197159, 2043: 1172231.2332486808, 2044: 1131333.5825776458, 2045: 1090435.9319066107, 2046: 1049538.2812355906, 2047: 1008640.6305645555, 2048: 967742.9798935205, 2049: 926845.3292224854, 2050: 885947.6785514504}</t>
         </is>
       </c>
-      <c r="T59" t="n">
+      <c r="S59" t="n">
         <v>42875807.36103913</v>
       </c>
     </row>
@@ -4744,15 +4449,10 @@
       </c>
       <c r="R60" t="inlineStr">
         <is>
-          <t>{2021: 101111.400908884, 2022: 76989.406978137, 2023: 58622.16064226652, 2024: 44636.7604746403, 2025: 33987.83606474346, 2026: 25879.409439226, 2027: 19705.397885505394, 2028: 15004.310926721588, 2029: 11424.75517083236, 2030: 8699.168615667995, 2031: 6623.821121088372, 2032: 5043.586138237801, 2033: 3840.345424310731, 2034: 2924.1600269718633, 2035: 2226.547593664645, 2036: 1695.3635030664216, 2037: 1290.9031972673658, 2038: 982.9343746642039, 2039: 748.4372081049261, 2040: 569.8836757716002, 2041: 433.9273894910639, 2042: 330.40598872320413, 2043: 251.5815319060567, 2044: 191.56210648839627, 2045: 145.86142458173114, 2046: 111.06348521126118, 2047: 84.56723758624923, 2048: 64.39215966764914, 2049: 49.03021956269064, 2050: 37.33315426557142}</t>
-        </is>
-      </c>
-      <c r="S60" t="inlineStr">
-        <is>
           <t>{2021: 101111.400908884, 2022: 104697.62903068285, 2023: 104058.05439084605, 2024: 103418.47975100903, 2025: 102778.90511117224, 2026: 102139.33047133544, 2027: 101499.75583149865, 2028: 100860.18119166186, 2029: 100220.60655182484, 2030: 99581.03191198804, 2031: 98941.45727215125, 2032: 98301.88263231446, 2033: 97662.30799247767, 2034: 97022.73335264088, 2035: 96383.15871280385, 2036: 95743.58407296706, 2037: 95104.00943313027, 2038: 94464.43479329348, 2039: 93824.86015345668, 2040: 93185.28551361966, 2041: 92545.71087378287, 2042: 91906.13623394608, 2043: 91266.56159410928, 2044: 90626.98695427249, 2045: 89987.4123144357, 2046: 89347.83767459868, 2047: 88708.26303476188, 2048: 88068.68839492509, 2049: 87429.1137550883, 2050: 86789.53911525151}</t>
         </is>
       </c>
-      <c r="T60" t="n">
+      <c r="S60" t="n">
         <v>2783724.869012862</v>
       </c>
     </row>
@@ -4816,15 +4516,10 @@
       </c>
       <c r="R61" t="inlineStr">
         <is>
-          <t>{2021: 33448.1706049408, 2022: 25259.877720492274, 2023: 19076.12317547707, 2024: 14406.185153887654, 2025: 10879.473191643552, 2026: 8216.119372570283, 2027: 6204.768958498332, 2028: 4685.8079931110615, 2029: 3538.6968789918437, 2030: 2672.4047634466983, 2031: 2018.18563836054, 2032: 1524.122889839317, 2033: 1151.0093715755434, 2034: 869.2360585138896, 2035: 656.4423749100396, 2036: 495.7417347760055, 2037: 374.38147961182875, 2038: 282.7308706209138, 2039: 213.51682589892255, 2040: 161.2467532881375, 2041: 121.77267686750811, 2042: 91.96206763295763, 2043: 69.44925660565171, 2044: 52.44770335447641, 2045: 39.60822219852677, 2046: 29.911915401229308, 2047: 22.589316897024936, 2048: 17.059330070626142, 2049: 12.883113897830931, 2050: 9.72925800821866}</t>
-        </is>
-      </c>
-      <c r="S61" t="inlineStr">
-        <is>
           <t>{2021: 33448.1706049408, 2022: 33952.249976868276, 2023: 33746.792717992095, 2024: 33541.335459115915, 2025: 33335.87820023979, 2026: 33130.42094136361, 2027: 32924.96368248743, 2028: 32719.506423611252, 2029: 32514.049164735072, 2030: 32308.59190585895, 2031: 32103.13464698277, 2032: 31897.67738810659, 2033: 31692.22012923041, 2034: 31486.76287035423, 2035: 31281.30561147805, 2036: 31075.848352601926, 2037: 30870.391093725746, 2038: 30664.933834849566, 2039: 30459.476575973385, 2040: 30254.019317097205, 2041: 30048.562058221083, 2042: 29843.104799344903, 2043: 29637.647540468723, 2044: 29432.190281592542, 2045: 29226.733022716362, 2046: 29021.27576384024, 2047: 28815.81850496406, 2048: 28610.36124608788, 2049: 28404.9039872117, 2050: 28199.44672833552}</t>
         </is>
       </c>
-      <c r="T61" t="n">
+      <c r="S61" t="n">
         <v>903823.9641637581</v>
       </c>
     </row>
@@ -4888,15 +4583,10 @@
       </c>
       <c r="R62" t="inlineStr">
         <is>
-          <t>{2021: 79688.3208022694, 2022: 58610.11853218889, 2023: 43107.27042273683, 2024: 31705.050421940563, 2025: 23318.809388766065, 2026: 17150.79661041341, 2027: 12614.272858779657, 2028: 9277.696154307647, 2029: 6823.670844550142, 2030: 5018.754981876037, 2031: 3691.253892796184, 2032: 2714.887526943933, 2033: 1996.7779237131776, 2034: 1468.6140906605037, 2035: 1080.1538426846057, 2036: 794.4444570469753, 2037: 584.3075036089558, 2038: 429.75346576499817, 2039: 316.08021494899197, 2040: 232.47445393920987, 2041: 170.98308966619555, 2042: 125.75668619246659, 2043: 92.49303046859838, 2044: 68.02787942560751, 2045: 50.033957755510414, 2046: 36.79957320171669, 2047: 27.065789887056518, 2048: 19.906670607150335, 2049: 14.641196001122081, 2050: 10.76848181062861}</t>
-        </is>
-      </c>
-      <c r="S62" t="inlineStr">
-        <is>
           <t>{2021: 79688.3208022694, 2022: 72151.6844737134, 2023: 70678.12303419923, 2024: 69204.56159468507, 2025: 67731.00015517091, 2026: 66257.43871565675, 2027: 64783.87727614213, 2028: 63310.31583662797, 2029: 61836.75439711381, 2030: 60363.19295759965, 2031: 58889.63151808549, 2032: 57416.07007857133, 2033: 55942.50863905717, 2034: 54468.94719954301, 2035: 52995.38576002885, 2036: 51521.82432051469, 2037: 50048.262881000526, 2038: 48574.701441486366, 2039: 47101.140001972206, 2040: 45627.578562458046, 2041: 44154.017122943886, 2042: 42680.455683429725, 2043: 41206.894243915565, 2044: 39733.332804401405, 2045: 38259.771364887245, 2046: 36786.209925373085, 2047: 35312.648485858925, 2048: 33839.087046344765, 2049: 32365.525606830604, 2050: 30891.964167316444}</t>
         </is>
       </c>
-      <c r="T62" t="n">
+      <c r="S62" t="n">
         <v>1518531.083612405</v>
       </c>
     </row>
@@ -4960,15 +4650,10 @@
       </c>
       <c r="R63" t="inlineStr">
         <is>
-          <t>{2021: 45571.0255636995, 2022: 35082.5068531677, 2023: 27008.000629306942, 2024: 20791.90352746362, 2025: 16006.488530152537, 2026: 12322.473251546451, 2027: 9486.362155512115, 2028: 7303.003634780764, 2029: 5622.161711234167, 2030: 4328.178361671648, 2031: 3332.0151380580637, 2032: 2565.1264695016202, 2033: 1974.7430704569576, 2034: 1520.2409084630553, 2035: 1170.3458816188063, 2036: 900.9818608333987, 2037: 693.6140215471919, 2038: 533.9734702781428, 2039: 411.075408084845, 2040: 316.463271188548, 2041: 243.62683838943212, 2042: 187.55426549410703, 2043: 144.3872224323864, 2044: 111.15540319393295, 2045: 85.57214032558628, 2046: 65.87706030921498, 2047: 50.714953003066796, 2048: 39.04252020400946, 2049: 30.056586738595804, 2050: 23.138834318435165}</t>
-        </is>
-      </c>
-      <c r="S63" t="inlineStr">
-        <is>
           <t>{2021: 45571.0255636995, 2022: 41965.16419702163, 2023: 40026.22762812255, 2024: 38087.29105922347, 2025: 36148.35449032439, 2026: 34209.41792142531, 2027: 32270.48135252623, 2028: 30331.54478362715, 2029: 28392.60821472807, 2030: 26453.67164582899, 2031: 24514.73507692991, 2032: 22575.798508030828, 2033: 20636.861939131748, 2034: 18697.925370232668, 2035: 16758.988801333588, 2036: 14820.052232434507, 2037: 12881.115663535427, 2038: 10942.179094635881, 2039: 9003.242525736801, 2040: 7064.305956837721, 2041: 5125.369387938641, 2042: 3186.432819039561, 2043: 1247.4962501404807, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T63" t="n">
+      <c r="S63" t="n">
         <v>498124.7777006353</v>
       </c>
     </row>
@@ -5032,15 +4717,10 @@
       </c>
       <c r="R64" t="inlineStr">
         <is>
-          <t>{2021: 35566.2660676553, 2022: 26900.11592582608, 2023: 20345.577898067673, 2024: 15388.132197933193, 2025: 11638.62799707242, 2026: 8802.735764931338, 2027: 6657.842914705467, 2028: 5035.579104110429, 2029: 3808.5994576030575, 2030: 2880.588216083002, 2031: 2178.69811803693, 2032: 1647.8320167511529, 2033: 1246.3178505321243, 2034: 942.6374586515803, 2035: 712.9524607817584, 2036: 539.2329857778805, 2037: 407.8423582858434, 2038: 308.4666435459397, 2039: 233.30502152944402, 2040: 176.4574361919553, 2041: 133.46145137946965, 2042: 100.94195738477228, 2043: 76.34623073068578, 2044: 57.743549835921904, 2045: 43.673636743319115, 2046: 33.03202785085481, 2047: 24.98337544803978, 2048: 18.89587437973673, 2049: 14.291666445048177, 2050: 10.809329363215305}</t>
-        </is>
-      </c>
-      <c r="S64" t="inlineStr">
-        <is>
           <t>{2021: 35566.2660676553, 2022: 35436.592202680185, 2023: 35017.980652291095, 2024: 34599.369101902004, 2025: 34180.757551512914, 2026: 33762.14600112382, 2027: 33343.53445073473, 2028: 32924.92290034576, 2029: 32506.311349956668, 2030: 32087.699799567577, 2031: 31669.088249178487, 2032: 31250.476698789396, 2033: 30831.865148400306, 2034: 30413.253598011215, 2035: 29994.642047622125, 2036: 29576.030497233034, 2037: 29157.418946843944, 2038: 28738.807396454853, 2039: 28320.195846065762, 2040: 27901.584295676672, 2041: 27482.97274528758, 2042: 27064.361194898607, 2043: 26645.749644509517, 2044: 26227.138094120426, 2045: 25808.526543731336, 2046: 25389.914993342245, 2047: 24971.303442953154, 2048: 24552.691892564064, 2049: 24134.080342174973, 2050: 23715.468791785883}</t>
         </is>
       </c>
-      <c r="T64" t="n">
+      <c r="S64" t="n">
         <v>863630.283057693</v>
       </c>
     </row>
@@ -5104,15 +4784,10 @@
       </c>
       <c r="R65" t="inlineStr">
         <is>
-          <t>{2021: 323846.285250688, 2022: 245207.58787852738, 2023: 185664.50779777163, 2024: 140580.10909868518, 2025: 106443.43018819785, 2026: 80596.06656213442, 2027: 61025.14672632405, 2028: 46206.57920195595, 2029: 34986.363426892756, 2030: 26490.721602407753, 2031: 20058.052974915834, 2032: 15187.411471190817, 2033: 11499.494366861716, 2034: 8707.103968594573, 2035: 6592.782004258276, 2036: 4991.874992241246, 2037: 3779.711800279231, 2038: 2861.894842193525, 2039: 2166.948836461239, 2040: 1640.7546464012232, 2041: 1242.3347355461913, 2042: 940.6620292253076, 2043: 712.2436714588449, 2044: 539.2915114804417, 2045: 408.3368459549234, 2046: 309.1815395104021, 2047: 234.1038417693392, 2048: 177.257053632466, 2049: 134.21421376510736, 2050: 101.62334760418601}</t>
-        </is>
-      </c>
-      <c r="S65" t="inlineStr">
-        <is>
           <t>{2021: 323846.285250688, 2022: 304823.0623716749, 2023: 296324.7607831955, 2024: 287826.45919471607, 2025: 279328.1576062329, 2026: 270829.8560177535, 2027: 262331.55442927405, 2028: 253833.2528407909, 2029: 245334.95125231147, 2030: 236836.64966383204, 2031: 228338.34807534888, 2032: 219840.04648686945, 2033: 211341.74489839002, 2034: 202843.44330990687, 2035: 194345.14172142744, 2036: 185846.840132948, 2037: 177348.53854446858, 2038: 168850.23695598543, 2039: 160351.935367506, 2040: 151853.63377902657, 2041: 143355.3321905434, 2042: 134857.03060206398, 2043: 126358.72901358455, 2044: 117860.4274251014, 2045: 109362.12583662197, 2046: 100863.82424814254, 2047: 92365.52265965939, 2048: 83867.22107117996, 2049: 75368.91948270053, 2050: 66870.61789421737}</t>
         </is>
       </c>
-      <c r="T65" t="n">
+      <c r="S65" t="n">
         <v>5518046.197533709</v>
       </c>
     </row>
@@ -5176,15 +4851,10 @@
       </c>
       <c r="R66" t="inlineStr">
         <is>
-          <t>{2021: 60909.6622028492, 2022: 47177.43148311438, 2023: 36541.16540544266, 2024: 28302.871250331445, 2025: 21921.920445742675, 2026: 16979.570439301027, 2027: 13151.485200247376, 2028: 10186.45104071584, 2029: 7889.891006602739, 2030: 6111.09598890255, 2031: 4733.334611888539, 2032: 3666.192870933039, 2033: 2839.640817516061, 2034: 2199.436924454857, 2035: 1703.5685481120106, 2036: 1319.494897011324, 2037: 1022.0115798501157, 2038: 791.5965963290614, 2039: 613.1292283514571, 2040: 474.89776030136306, 2041: 367.83091118594325, 2042: 284.9025422609325, 2043: 220.67057476229942, 2044: 170.9198597509356, 2045: 132.38556381496545, 2046: 102.5389181347627, 2047: 79.4212709396565, 2048: 61.51555323979841, 2049: 47.64672291977854, 2050: 36.904653952220386}</t>
-        </is>
-      </c>
-      <c r="S66" t="inlineStr">
-        <is>
           <t>{2021: 60909.6622028492, 2022: 58515.67462476529, 2023: 56257.53343027085, 2024: 53999.39223577641, 2025: 51741.25104128197, 2026: 49483.10984678753, 2027: 47224.968652293086, 2028: 44966.82745779771, 2029: 42708.68626330327, 2030: 40450.54506880883, 2031: 38192.40387431439, 2032: 35934.26267981995, 2033: 33676.12148532551, 2034: 31417.980290831067, 2035: 29159.839096336626, 2036: 26901.697901841253, 2037: 24643.556707346812, 2038: 22385.41551285237, 2039: 20127.27431835793, 2040: 17869.13312386349, 2041: 15610.991929369047, 2042: 13352.850734874606, 2043: 11094.709540380165, 2044: 8836.568345884793, 2045: 6578.427151390351, 2046: 4320.28595689591, 2047: 2062.144762401469, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T66" t="n">
+      <c r="S66" t="n">
         <v>817966.4831345952</v>
       </c>
     </row>
@@ -5248,15 +4918,10 @@
       </c>
       <c r="R67" t="inlineStr">
         <is>
-          <t>{2021: 107898.699030336, 2022: 84250.37150280415, 2023: 65785.08510436123, 2024: 51366.86456087628, 2025: 40108.70808526907, 2026: 31318.019466864756, 2027: 24453.999895527668, 2028: 19094.378286697345, 2029: 14909.43337339995, 2030: 11641.709417201497, 2031: 9090.17765868669, 2032: 7097.86912774104, 2033: 5542.21799024971, 2034: 4327.521358684621, 2035: 3379.0516978614555, 2036: 2638.4596239846087, 2037: 2060.1842794541435, 2038: 1608.6504514706742, 2039: 1256.0800025628998, 2040: 980.7829733277362, 2041: 765.8232268699982, 2042: 597.9765460483761, 2043: 466.9170861863214, 2044: 364.58213422151147, 2045: 284.6760945913871, 2046: 222.28318731209708, 2047: 173.5650316284752, 2048: 135.5245107309747, 2049: 105.82139061389597, 2050: 82.62835003837701}</t>
-        </is>
-      </c>
-      <c r="S67" t="inlineStr">
-        <is>
           <t>{2021: 107898.699030336, 2022: 101667.53271860257, 2023: 96492.11420881748, 2024: 91316.6956990324, 2025: 86141.27718924917, 2026: 80965.85867946409, 2027: 75790.44016968086, 2028: 70615.02165989578, 2029: 65439.603150112554, 2030: 60264.18464032747, 2031: 55088.766130544245, 2032: 49913.34762075916, 2033: 44737.92911097407, 2034: 39562.51060119085, 2035: 34387.092091405764, 2036: 29211.67358162254, 2037: 24036.255071837455, 2038: 18860.83656205423, 2039: 13685.418052269146, 2040: 8509.99954248406, 2041: 3334.5810327008367, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T67" t="n">
+      <c r="S67" t="n">
         <v>1103970.487028193</v>
       </c>
     </row>
@@ -5320,15 +4985,10 @@
       </c>
       <c r="R68" t="inlineStr">
         <is>
-          <t>{2021: 26695.9585691294, 2022: 20491.742192972855, 2023: 15729.40327337937, 2024: 12073.845405952952, 2025: 9267.84953969406, 2026: 7113.975059516516, 2027: 5460.667108444844, 2028: 4191.59260747787, 2029: 3217.454614637143, 2030: 2469.709050154751, 2031: 1895.7416725221362, 2032: 1455.165938964284, 2033: 1116.9812536244065, 2034: 857.3916469185398, 2035: 658.1313999857657, 2036: 505.1797987581466, 2037: 387.7745828247082, 2038: 297.65467157340817, 2039: 228.47888292235976, 2040: 175.37974346414757, 2041: 134.6209943962401, 2042: 103.33469404314253, 2043: 79.31941849694222, 2044: 60.885361000500986, 2045: 46.73543067268247, 2046: 35.87398422657191, 2047: 27.536768694860147, 2048: 21.137145664254827, 2049: 16.22481315011081, 2050: 12.454120624299007}</t>
-        </is>
-      </c>
-      <c r="S68" t="inlineStr">
-        <is>
           <t>{2021: 26695.9585691294, 2022: 26749.33097979799, 2023: 26210.306528806454, 2024: 25671.282077814918, 2025: 25132.257626823615, 2026: 24593.23317583208, 2027: 24054.208724840544, 2028: 23515.18427384901, 2029: 22976.159822857706, 2030: 22437.13537186617, 2031: 21898.110920874635, 2032: 21359.086469883332, 2033: 20820.062018891796, 2034: 20281.03756790026, 2035: 19742.013116908725, 2036: 19202.988665917423, 2037: 18663.964214925887, 2038: 18124.93976393435, 2039: 17585.915312942816, 2040: 17046.890861951513, 2041: 16507.866410959978, 2042: 15968.841959968442, 2043: 15429.81750897714, 2044: 14890.793057985604, 2045: 14351.768606994068, 2046: 13812.744156002533, 2047: 13273.71970501123, 2048: 12734.695254019694, 2049: 12195.670803028159, 2050: 11656.646352036856}</t>
         </is>
       </c>
-      <c r="T68" t="n">
+      <c r="S68" t="n">
         <v>564406.3274201492</v>
       </c>
     </row>
@@ -5392,15 +5052,10 @@
       </c>
       <c r="R69" t="inlineStr">
         <is>
-          <t>{2021: 46040.8639867489, 2022: 35467.49506419384, 2023: 27322.31972212045, 2024: 21047.698847822197, 2025: 16214.056174372103, 2026: 12490.468413030145, 2027: 9622.009415725084, 2028: 7412.29729220714, 2029: 5710.049613781327, 2030: 4398.72623918133, 2031: 3388.55068449206, 2032: 2610.3638001142426, 2033: 2010.8889620956868, 2034: 1549.0846209640572, 2035: 1193.3344944150983, 2036: 919.2830374074058, 2037: 708.168000522933, 2038: 545.5359193605944, 2039: 420.2525941483448, 2040: 323.74081452861117, 2041: 249.3931422459045, 2042: 192.11954936806148, 2043: 147.99894222028544, 2044: 114.0107134873631, 2045: 87.82794386834456, 2046: 67.6580953508029, 2047: 52.120289567068255, 2048: 40.15076940120825, 2049: 30.930071511490233, 2050: 23.826923816735395}</t>
-        </is>
-      </c>
-      <c r="S69" t="inlineStr">
-        <is>
           <t>{2021: 46040.8639867489, 2022: 41119.0098768007, 2023: 38818.60167533811, 2024: 36518.19347387552, 2025: 34217.78527241293, 2026: 31917.377070950344, 2027: 29616.968869487755, 2028: 27316.560668025166, 2029: 25016.152466562577, 2030: 22715.744265099987, 2031: 20415.3360636374, 2032: 18114.92786217481, 2033: 15814.51966071222, 2034: 13514.11145924963, 2035: 11213.703257787041, 2036: 8913.295056324452, 2037: 6612.886854861863, 2038: 4312.478653399274, 2039: 2012.0704519366845, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T69" t="n">
+      <c r="S69" t="n">
         <v>411200.154952011</v>
       </c>
     </row>
@@ -5464,15 +5119,10 @@
       </c>
       <c r="R70" t="inlineStr">
         <is>
-          <t>{2021: 58791.6820261748, 2022: 43234.38174740309, 2023: 31793.81335352821, 2024: 23380.618079954536, 2025: 17193.70041341813, 2026: 12643.948628536411, 2027: 9298.140195365051, 2028: 6837.690790481391, 2029: 5028.319036267061, 2030: 3697.7384771015145, 2031: 2719.2526461463017, 2032: 1999.6911624127997, 2033: 1470.538146096453, 2034: 1081.4082093134673, 2035: 795.2488130109723, 2036: 584.8121635740615, 2037: 430.06070687395805, 2038: 316.25917365774126, 2039: 232.57150286922416, 2040: 171.02904343064446, 2041: 125.77178775530886, 2042: 92.49038805260687, 2043: 68.015824810924, 2044: 50.01765612745654, 2045: 36.782115506782546, 2046: 27.048928836383876, 2047: 19.89131242494319, 2048: 14.627725644147713, 2049: 10.756975354333266, 2050: 7.910492826342254}</t>
-        </is>
-      </c>
-      <c r="S70" t="inlineStr">
-        <is>
           <t>{2021: 58791.6820261748, 2022: 60816.67669059592, 2023: 61630.40092231287, 2024: 62444.12515403004, 2025: 63257.84938574722, 2026: 64071.5736174644, 2027: 64885.297849181574, 2028: 65699.02208089852, 2029: 66512.7463126157, 2030: 67326.47054433287, 2031: 68140.19477605005, 2032: 68953.91900776722, 2033: 69767.64323948417, 2034: 70581.36747120135, 2035: 71395.09170291852, 2036: 72208.8159346357, 2037: 73022.54016635264, 2038: 73836.26439806982, 2039: 74649.988629787, 2040: 75463.71286150417, 2041: 76277.43709322135, 2042: 77091.1613249383, 2043: 77904.88555665547, 2044: 78718.60978837265, 2045: 79532.33402008982, 2046: 80346.05825180677, 2047: 81159.78248352394, 2048: 81973.50671524112, 2049: 82787.2309469583, 2050: 83600.95517867547}</t>
         </is>
       </c>
-      <c r="T70" t="n">
+      <c r="S70" t="n">
         <v>2081651.025528183</v>
       </c>
     </row>
@@ -5536,15 +5186,10 @@
       </c>
       <c r="R71" t="inlineStr">
         <is>
-          <t>{2021: 433330.272411755, 2022: 326062.0738267072, 2023: 245347.4468710786, 2024: 184613.220972608, 2025: 138913.37282099333, 2026: 104526.23624050994, 2027: 78651.42023933162, 2028: 59181.753100055605, 2029: 44531.68028419705, 2030: 33508.14136210645, 2031: 25213.410551259953, 2032: 18971.988471592842, 2033: 14275.591389530011, 2034: 10741.75803058104, 2035: 8082.70301657542, 2036: 6081.880439697781, 2037: 4576.348977182951, 2038: 3443.502411567323, 2039: 2591.084927655404, 2040: 1949.678060270977, 2041: 1467.0474511005837, 2042: 1103.8890305210648, 2043: 830.628205509345, 2044: 625.0113885650292, 2045: 470.2937285839507, 2046: 353.87545761877345, 2047: 266.27580146976646, 2048: 200.36089229095222, 2049: 150.76280660142768, 2050: 113.44241680324106}</t>
-        </is>
-      </c>
-      <c r="S71" t="inlineStr">
-        <is>
           <t>{2021: 433330.272411755, 2022: 420009.65124240704, 2023: 413353.93418391794, 2024: 406698.2171254307, 2025: 400042.5000669416, 2026: 393386.7830084525, 2027: 386731.06594996527, 2028: 380075.34889147617, 2029: 373419.63183298707, 2030: 366763.91477449983, 2031: 360108.19771601073, 2032: 353452.48065752164, 2033: 346796.7635990344, 2034: 340141.0465405453, 2035: 333485.3294820562, 2036: 326829.61242356896, 2037: 320173.89536507986, 2038: 313518.17830659077, 2039: 306862.46124810353, 2040: 300206.74418961443, 2041: 293551.0271311272, 2042: 286895.3100726381, 2043: 280239.593014149, 2044: 273583.87595566176, 2045: 266928.15889717266, 2046: 260272.44183868356, 2047: 253616.72478019632, 2048: 246961.00772170722, 2049: 240305.29066321813, 2050: 233649.5736047309}</t>
         </is>
       </c>
-      <c r="T71" t="n">
+      <c r="S71" t="n">
         <v>9577899.109687002</v>
       </c>
     </row>
@@ -5608,15 +5253,10 @@
       </c>
       <c r="R72" t="inlineStr">
         <is>
-          <t>{2021: 21156.8159179098, 2022: 16434.109111243175, 2023: 12765.623302115904, 2024: 9916.03117567455, 2025: 7702.536096349624, 2026: 5983.146005138791, 2027: 4647.564863184949, 2028: 3610.1173427758067, 2029: 2804.2528963607083, 2030: 2178.276648675621, 2031: 1692.0332557464044, 2032: 1314.3310057941678, 2033: 1020.9409223637705, 2034: 793.0425154409091, 2035: 616.0164780550896, 2036: 478.5068818465787, 2037: 371.6927129895043, 2038: 288.7220187019045, 2039: 224.27236577451245, 2040: 174.20941525775248, 2041: 135.32171143618038, 2042: 105.11467224043712, 2043: 81.65056592138534, 2044: 63.42420875396873, 2045: 49.2664099834907, 2046: 38.26897016684524, 2047: 29.726421675978678, 2048: 23.090774112956517, 2049: 17.93636162964201, 2050: 13.9325371655157}</t>
-        </is>
-      </c>
-      <c r="S72" t="inlineStr">
-        <is>
           <t>{2021: 21156.8159179098, 2022: 20091.85724540893, 2023: 19202.850225555012, 2024: 18313.843205701327, 2025: 17424.836185847642, 2026: 16535.829165993724, 2027: 15646.822146140039, 2028: 14757.815126286354, 2029: 13868.808106432436, 2030: 12979.801086578751, 2031: 12090.794066724833, 2032: 11201.787046871148, 2033: 10312.780027017463, 2034: 9423.773007163545, 2035: 8534.76598730986, 2036: 7645.758967456175, 2037: 6756.751947602257, 2038: 5867.744927748572, 2039: 4978.737907894654, 2040: 4089.730888040969, 2041: 3200.723868187284, 2042: 2311.716848333366, 2043: 1422.7098284796812, 2044: 533.7028086259961, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T72" t="n">
+      <c r="S72" t="n">
         <v>247772.3485803549</v>
       </c>
     </row>
@@ -5680,15 +5320,10 @@
       </c>
       <c r="R73" t="inlineStr">
         <is>
-          <t>{2021: 18812.6023604529, 2022: 14558.273552675564, 2023: 11266.029269829865, 2024: 8718.301318451107, 2025: 6746.722918859785, 2026: 5221.002174762487, 2027: 4040.3117241817076, 2028: 3126.6255561946355, 2029: 2419.5626565495572, 2030: 1872.3967241201415, 2031: 1448.9682600306865, 2032: 1121.2949646464137, 2033: 867.7225253469488, 2034: 671.4935897637937, 2035: 519.6403549781971, 2036: 402.12758935919516, 2037: 311.18945358010603, 2038: 240.8162945840179, 2039: 186.35749724162224, 2040: 144.21414812544856, 2041: 111.60120106455123, 2042: 86.36342717370705, 2043: 66.83298640194793, 2044: 51.719208206257974, 2045: 40.023297498558286, 2046: 30.972329202524005, 2047: 23.968169445910245, 2048: 18.547947841812643, 2049: 14.353468666807352, 2050: 11.107539471541157}</t>
-        </is>
-      </c>
-      <c r="S73" t="inlineStr">
-        <is>
           <t>{2021: 18812.6023604529, 2022: 17747.910900079412, 2023: 16981.722424515523, 2024: 16215.533948951634, 2025: 15449.345473387511, 2026: 14683.156997823622, 2027: 13916.968522259733, 2028: 13150.780046695843, 2029: 12384.591571131954, 2030: 11618.403095567832, 2031: 10852.214620003942, 2032: 10086.026144440053, 2033: 9319.837668876164, 2034: 8553.649193312274, 2035: 7787.460717748385, 2036: 7021.272242184263, 2037: 6255.083766620373, 2038: 5488.895291056484, 2039: 4722.706815492595, 2040: 3956.5183399287052, 2041: 3190.329864364583, 2042: 2424.1413888006937, 2043: 1657.9529132368043, 2044: 891.7644376729149, 2045: 125.57596210902557, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T73" t="n">
+      <c r="S73" t="n">
         <v>223888.1435264868</v>
       </c>
     </row>
@@ -5752,15 +5387,10 @@
       </c>
       <c r="R74" t="inlineStr">
         <is>
-          <t>{2021: 88139.5693861936, 2022: 68359.02792815694, 2023: 53017.69377619086, 2024: 41119.30696703418, 2025: 31891.19112926197, 2026: 24734.076195848746, 2027: 19183.182051193868, 2028: 14878.035900568997, 2029: 11539.063314307847, 2030: 8949.432778725379, 2031: 6940.974746330919, 2032: 5383.2607742169275, 2033: 4175.133554338537, 2034: 3238.1377993153696, 2035: 2511.4253881673, 2036: 1947.8039142326807, 2037: 1510.6720295874525, 2038: 1171.6425684855947, 2039: 908.699096429556, 2040: 704.766171921522, 2041: 546.6004742785838, 2042: 423.93078780580566, 2043: 328.7909932512338, 2044: 255.00275128083635, 2045: 197.7742836498824, 2046: 153.38919708417936, 2047: 118.96514222132633, 2048: 92.26663502237028, 2049: 71.55988535291456, 2050: 55.5002053611332}</t>
-        </is>
-      </c>
-      <c r="S74" t="inlineStr">
-        <is>
           <t>{2021: 88139.5693861936, 2022: 79001.64650530554, 2023: 74226.95056099631, 2024: 69452.25461668707, 2025: 64677.55867237784, 2026: 59902.862728068605, 2027: 55128.16678375937, 2028: 50353.470839450136, 2029: 45578.7748951409, 2030: 40804.07895083167, 2031: 36029.38300652243, 2032: 31254.687062213197, 2033: 26479.991117903963, 2034: 21705.295173594728, 2035: 16930.599229285493, 2036: 12155.903284976259, 2037: 7381.207340667024, 2038: 2606.5113963577896, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T74" t="n">
+      <c r="S74" t="n">
         <v>737739.1268572351</v>
       </c>
     </row>
@@ -5824,15 +5454,10 @@
       </c>
       <c r="R75" t="inlineStr">
         <is>
-          <t>{2021: 104930.608832851, 2022: 81743.64272668763, 2023: 63680.39984283772, 2024: 49608.66911329545, 2025: 38646.42899960105, 2026: 30106.56204080518, 2027: 23453.786064585896, 2028: 18271.10249313116, 2029: 14233.658710589845, 2030: 11088.386175148133, 2031: 8638.13798470099, 2032: 6729.331632584237, 2033: 5242.322396505031, 2034: 4083.903960956147, 2035: 3181.4662092191097, 2036: 2478.443993093623, 2037: 1930.7716074751527, 2038: 1504.120734872448, 2039: 1171.7487331563366, 2040: 912.8223963815722, 2041: 711.1121213600862, 2042: 553.9746298401083, 2043: 431.56048292289756, 2044: 336.19671441343735, 2045: 261.9058863241284, 2046: 204.03142074396678, 2047: 158.94572372948795, 2048: 123.8228063097863, 2049: 96.46115040203759, 2050: 75.14571680442617}</t>
-        </is>
-      </c>
-      <c r="S75" t="inlineStr">
-        <is>
           <t>{2021: 104930.608832851, 2022: 97374.26597972587, 2023: 92160.02247765288, 2024: 86945.77897557989, 2025: 81731.5354735069, 2026: 76517.29197143577, 2027: 71303.04846936278, 2028: 66088.80496728979, 2029: 60874.5614652168, 2030: 55660.31796314567, 2031: 50446.07446107268, 2032: 45231.83095899969, 2033: 40017.5874569267, 2034: 34803.343954855576, 2035: 29589.100452782586, 2036: 24374.856950709596, 2037: 19160.613448636606, 2038: 13946.369946565479, 2039: 8732.12644449249, 2040: 3517.882942419499, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T75" t="n">
+      <c r="S75" t="n">
         <v>1010940.719176803</v>
       </c>
     </row>
@@ -5896,15 +5521,10 @@
       </c>
       <c r="R76" t="inlineStr">
         <is>
-          <t>{2021: 118289.914595419, 2022: 92353.8454460693, 2023: 72104.47989457563, 2024: 56294.95984445267, 2025: 43951.81143421506, 2026: 34315.00322029548, 2027: 26791.147112817926, 2028: 20916.960403959183, 2029: 16330.739057136907, 2030: 12750.085719998631, 2031: 9954.521059857885, 2032: 7771.907711626329, 2033: 6067.850890547935, 2034: 4737.4230106778705, 2035: 3698.702751094386, 2036: 2887.73073675675, 2037: 2254.571229207946, 2038: 1760.2373250634573, 2039: 1374.290330864848, 2040: 1072.9654954001878, 2041: 837.7086911430714, 2042: 654.0339407232296, 2043: 510.6314404286164, 2044: 398.67115713577914, 2045: 311.25911753214876, 2046: 243.01291054746636, 2047: 189.73026448502762, 2048: 148.1302914337439, 2049: 115.65146604208454, 2050: 90.29389916285936}</t>
-        </is>
-      </c>
-      <c r="S76" t="inlineStr">
-        <is>
           <t>{2021: 118289.914595419, 2022: 109252.78523007222, 2023: 103038.04982997291, 2024: 96823.3144298736, 2025: 90608.57902977243, 2026: 84393.84362967312, 2027: 78179.10822957382, 2028: 71964.37282947451, 2029: 65749.63742937334, 2030: 59534.90202927403, 2031: 53320.166629174724, 2032: 47105.43122907542, 2033: 40890.69582897425, 2034: 34675.96042887494, 2035: 28461.225028775632, 2036: 22246.489628676325, 2037: 16031.754228577018, 2038: 9817.018828475848, 2039: 3602.2834283765405, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T76" t="n">
+      <c r="S76" t="n">
         <v>1074840.57522375</v>
       </c>
     </row>
@@ -5968,15 +5588,10 @@
       </c>
       <c r="R77" t="inlineStr">
         <is>
-          <t>{2021: 40751.1227109742, 2022: 31299.69701909995, 2023: 24040.34461665594, 2024: 18464.65698805021, 2025: 14182.141026802694, 2026: 10892.87086320031, 2027: 8366.482565510667, 2028: 6426.040609319096, 2029: 4935.64620368006, 2030: 3790.9196235973764, 2031: 2911.68997928994, 2032: 2236.3804504650375, 2033: 1717.6957556593554, 2034: 1319.3098286996005, 2035: 1013.3217238085502, 2036: 778.3015737512051, 2037: 597.7897497616951, 2038: 459.1441119639606, 2039: 352.6546175059263, 2040: 270.86327801588544, 2041: 208.04183962309236, 2042: 159.79060487934484, 2043: 122.73030008754426, 2044: 94.26540797534554, 2045: 72.40239072519113, 2046: 55.61007261639686, 2047: 42.71240418204808, 2048: 32.806097621831185, 2049: 25.19736506954717, 2050: 19.353329181875317}</t>
-        </is>
-      </c>
-      <c r="S77" t="inlineStr">
-        <is>
           <t>{2021: 40751.1227109742, 2022: 37966.99699595617, 2023: 36410.12595556304, 2024: 34853.25491517037, 2025: 33296.38387477724, 2026: 31739.51283438457, 2027: 30182.64179399144, 2028: 28625.770753598772, 2029: 27068.89971320564, 2030: 25512.028672812972, 2031: 23955.15763241984, 2032: 22398.286592027172, 2033: 20841.41555163404, 2034: 19284.544511241373, 2035: 17727.67347084824, 2036: 16170.802430455573, 2037: 14613.93139006244, 2038: 13057.060349669773, 2039: 11500.18930927664, 2040: 9943.318268883973, 2041: 8386.44722849084, 2042: 6829.576188098174, 2043: 5272.705147705041, 2044: 3715.834107312374, 2045: 2158.963066919241, 2046: 602.092026526574, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T77" t="n">
+      <c r="S77" t="n">
         <v>502489.1741365186</v>
       </c>
     </row>
@@ -6040,15 +5655,10 @@
       </c>
       <c r="R78" t="inlineStr">
         <is>
-          <t>{2021: 43088.441163385, 2022: 32185.080144089352, 2023: 24040.77186161256, 2024: 17957.34884345913, 2025: 13413.312157443064, 2026: 10019.126130555944, 2027: 7483.825563866144, 2028: 5590.072860702536, 2029: 4175.5268507113415, 2030: 3118.926159903436, 2031: 2329.694129322336, 2032: 1740.1741682679005, 2033: 1299.8299209294596, 2034: 970.9130581022262, 2035: 725.2273172165075, 2036: 541.7113893442717, 2037: 404.6334471674281, 2038: 302.2425405616537, 2039: 225.76125123775054, 2040: 168.633252174632, 2041: 125.96126918629461, 2042: 94.0872641096404, 2043: 70.27885098985988, 2044: 52.49506342005379, 2045: 39.21139353677083, 2046: 29.289104211428686, 2047: 21.877611279065377, 2048: 16.341567561193163, 2049: 12.20639799065161, 2050: 9.117616859474948}</t>
-        </is>
-      </c>
-      <c r="S78" t="inlineStr">
-        <is>
           <t>{2021: 43088.441163385, 2022: 37479.95586147439, 2023: 35934.471928820945, 2024: 34388.98799616704, 2025: 32843.504063513596, 2026: 31298.020130859688, 2027: 29752.536198206246, 2028: 28207.05226555234, 2029: 26661.568332898896, 2030: 25116.08440024499, 2031: 23570.600467591546, 2032: 22025.11653493764, 2033: 20479.632602284197, 2034: 18934.14866963029, 2035: 17388.664736976847, 2036: 15843.18080432294, 2037: 14297.696871669497, 2038: 12752.21293901559, 2039: 11206.729006362148, 2040: 9661.24507370824, 2041: 8115.761141054798, 2042: 6570.27720840089, 2043: 5024.793275747448, 2044: 3479.3093430935405, 2045: 1933.8254104400985, 2046: 388.3414777861908, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T78" t="n">
+      <c r="S78" t="n">
         <v>494897.9373224525</v>
       </c>
     </row>
@@ -6112,15 +5722,10 @@
       </c>
       <c r="R79" t="inlineStr">
         <is>
-          <t>{2021: 31849.0491117575, 2022: 24677.26166727275, 2023: 19120.421500127002, 2024: 14814.873841021392, 2025: 11478.851913589984, 2026: 8894.037348416876, 2027: 6891.272833773733, 2028: 5339.491999992662, 2029: 4137.142078929006, 2030: 3205.5380139662234, 2031: 2483.713095403908, 2032: 1924.4291327708029, 2033: 1491.0850588621317, 2034: 1155.3216561218437, 2035: 895.1656521343594, 2036: 693.5917287753352, 2037: 537.4083389800934, 2038: 416.39441594161804, 2039: 322.6304786345785, 2040: 249.98035938736382, 2041: 193.68963634156208, 2042: 150.0744911242931, 2043: 116.28062973125986, 2044: 90.09648974588205, 2045: 69.80850966571283, 2046: 54.088988766298336, 2047: 41.90919874626248, 2048: 32.47206094280122, 2049: 25.159983331034972, 2050: 19.49444361825437}</t>
-        </is>
-      </c>
-      <c r="S79" t="inlineStr">
-        <is>
           <t>{2021: 31849.0491117575, 2022: 29535.626407840755, 2023: 28081.032003912143, 2024: 26626.437599983998, 2025: 25171.843196055386, 2026: 23717.24879212724, 2027: 22262.65438819863, 2028: 20808.059984270018, 2029: 19353.465580341872, 2030: 17898.87117641326, 2031: 16444.276772485115, 2032: 14989.682368556503, 2033: 13535.087964628357, 2034: 12080.493560699746, 2035: 10625.899156771135, 2036: 9171.304752842989, 2037: 7716.710348914377, 2038: 6262.115944986232, 2039: 4807.52154105762, 2040: 3352.9271371294744, 2041: 1898.332733200863, 2042: 443.7383292722516, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T79" t="n">
+      <c r="S79" t="n">
         <v>330707.8542955667</v>
       </c>
     </row>
@@ -6184,15 +5789,10 @@
       </c>
       <c r="R80" t="inlineStr">
         <is>
-          <t>{2021: 41363.3668840834, 2022: 34636.62780141969, 2023: 29003.828165538467, 2024: 24287.06550415403, 2025: 20337.36882719246, 2026: 17029.993629428656, 2027: 14260.482045769999, 2028: 11941.363725838995, 2029: 9999.393230545165, 2030: 8373.236698478284, 2031: 7011.534719384275, 2032: 5871.280233850974, 2033: 4916.460227902334, 2034: 4116.9183227167005, 2035: 3447.402336284533, 2036: 2886.7667358475974, 2037: 2417.3047919256237, 2038: 2024.1893411422052, 2039: 1695.0044952874043, 2040: 1419.3535064379475, 2041: 1188.530403216487, 2042: 995.245027375217, 2043: 833.3927864482889, 2044: 697.8618504990467, 2045: 584.3717035966596, 2046: 489.33795094295476, 2047: 409.7591118106603, 2048: 343.12182283902735, 2049: 287.32145769287547, 2050: 240.5956559909282}</t>
-        </is>
-      </c>
-      <c r="S80" t="inlineStr">
-        <is>
           <t>{2021: 41363.3668840834, 2022: 25946.91946527362, 2023: 17468.90219083801, 2024: 8990.8849164024, 2025: 512.8676419630647, 2026: 0, 2027: 0, 2028: 0, 2029: 0, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T80" t="n">
+      <c r="S80" t="n">
         <v>73601.25765651879</v>
       </c>
     </row>
@@ -6256,15 +5856,10 @@
       </c>
       <c r="R81" t="inlineStr">
         <is>
-          <t>{2021: 59782.1249581941, 2022: 46620.02709100488, 2023: 36355.799120320924, 2024: 28351.423457927427, 2025: 22109.353433010776, 2026: 17241.58612181089, 2027: 13445.544343778689, 2028: 10485.268665150594, 2029: 8176.750317383695, 2030: 6376.4933344103365, 2031: 4972.5949387664905, 2032: 3877.7897393242893, 2033: 3024.0253725832126, 2034: 2358.2324129880553, 2035: 1839.0256127106734, 2036: 1434.1314221530029, 2037: 1118.3818875556751, 2038: 872.1502277210077, 2039: 680.1308463393185, 2040: 530.3879462956603, 2041: 413.6136084546612, 2042: 322.5492175938719, 2043: 251.53427170620571, 2044: 196.15452895760913, 2045: 152.96762134872233, 2046: 119.2890794081174, 2047: 93.0254673542715, 2048: 72.54425651885585, 2049: 56.572348449823835, 2050: 44.116939957836955}</t>
-        </is>
-      </c>
-      <c r="S81" t="inlineStr">
-        <is>
           <t>{2021: 59782.1249581941, 2022: 55260.955024997704, 2023: 52187.259563962, 2024: 49113.56410292629, 2025: 46039.86864189152, 2026: 42966.17318085581, 2027: 39892.477719820105, 2028: 36818.78225878533, 2029: 33745.086797749624, 2030: 30671.391336713918, 2031: 27597.695875679143, 2032: 24524.000414643437, 2033: 21450.304953608662, 2034: 18376.609492572956, 2035: 15302.91403153725, 2036: 12229.218570502475, 2037: 9155.523109466769, 2038: 6081.827648431063, 2039: 3008.132187396288, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T81" t="n">
+      <c r="S81" t="n">
         <v>554312.8473906374</v>
       </c>
     </row>
@@ -6328,15 +5923,10 @@
       </c>
       <c r="R82" t="inlineStr">
         <is>
-          <t>{2021: 131690.249963079, 2022: 99790.41923281428, 2023: 75617.8059761654, 2024: 57300.616878947, 2025: 43420.470249332226, 2026: 32902.5643939593, 2027: 24932.45092653706, 2028: 18892.968394837506, 2029: 14316.452715381152, 2030: 10848.52385651319, 2031: 8220.644611139798, 2032: 6229.326562441858, 2033: 4720.373067698328, 2034: 3576.93912414143, 2035: 2710.4835389742416, 2036: 2053.912789699422, 2037: 1556.38567326896, 2038: 1179.376444854491, 2039: 893.6915975049919, 2040: 677.20927862822, 2041: 513.166296226246, 2042: 388.8600701337019, 2043: 294.6650145506066, 2044: 223.28718597992147, 2045: 169.1994806335225, 2046: 128.21364612131438, 2047: 97.15596637868603, 2048: 73.62150666899389, 2049: 55.787888754938756, 2050: 42.27417601933132}</t>
-        </is>
-      </c>
-      <c r="S82" t="inlineStr">
-        <is>
           <t>{2021: 131690.249963079, 2022: 131344.1780527183, 2023: 129670.07550462475, 2024: 127995.97295653075, 2025: 126321.87040843721, 2026: 124647.76786034368, 2027: 122973.66531224968, 2028: 121299.56276415614, 2029: 119625.46021606261, 2030: 117951.35766796861, 2031: 116277.25511987507, 2032: 114603.15257178154, 2033: 112929.05002368754, 2034: 111254.947475594, 2035: 109580.84492750047, 2036: 107906.74237940647, 2037: 106232.63983131293, 2038: 104558.53728321893, 2039: 102884.4347351254, 2040: 101210.33218703186, 2041: 99536.22963893786, 2042: 97862.12709084433, 2043: 96188.02454275079, 2044: 94513.92199465679, 2045: 92839.81944656326, 2046: 91165.71689846972, 2047: 89491.61435037572, 2048: 87817.51180228218, 2049: 86143.40925418865, 2050: 84469.30670609465}</t>
         </is>
       </c>
-      <c r="T82" t="n">
+      <c r="S82" t="n">
         <v>3152906.000631282</v>
       </c>
     </row>
@@ -6400,15 +5990,10 @@
       </c>
       <c r="R83" t="inlineStr">
         <is>
-          <t>{2021: 174606.772585002, 2022: 133687.6894897754, 2023: 102357.9902229392, 2024: 78370.40345648747, 2025: 60004.30571717274, 2026: 45942.30150415131, 2027: 35175.726846119986, 2028: 26932.298092228615, 2029: 20620.71620301628, 2030: 15788.253021305849, 2031: 12088.277197099078, 2032: 9255.390409357618, 2033: 7086.39041220746, 2034: 5425.695389732476, 2035: 4154.184112048387, 2036: 3180.6513999021495, 2037: 2435.266000454453, 2038: 1864.5616093457702, 2039: 1427.6017463378992, 2040: 1093.0433920400833, 2041: 836.8887611319217, 2042: 640.763947350444, 2043: 490.60096788586424, 2044: 375.62867056705664, 2045: 287.6001218668607, 2046: 220.2010564661281, 2047: 168.5969566148023, 2048: 129.0862734082565, 2049: 98.83491562959897, 2050: 75.6729611104038}</t>
-        </is>
-      </c>
-      <c r="S83" t="inlineStr">
-        <is>
           <t>{2021: 174606.772585002, 2022: 183584.46941203158, 2023: 182524.70803548768, 2024: 181464.94665894425, 2025: 180405.18528240034, 2026: 179345.4239058569, 2027: 178285.66252931347, 2028: 177225.90115276957, 2029: 176166.13977622613, 2030: 175106.37839968223, 2031: 174046.6170231388, 2032: 172986.8556465949, 2033: 171927.09427005146, 2034: 170867.33289350756, 2035: 169807.57151696412, 2036: 168747.81014042022, 2037: 167688.04876387678, 2038: 166628.28738733334, 2039: 165568.52601078944, 2040: 164508.764634246, 2041: 163449.0032577021, 2042: 162389.24188115867, 2043: 161329.48050461477, 2044: 160269.71912807133, 2045: 159209.95775152743, 2046: 158150.196374984, 2047: 157090.4349984401, 2048: 156030.67362189665, 2049: 154970.91224535322, 2050: 153911.15086880932}</t>
         </is>
       </c>
-      <c r="T83" t="n">
+      <c r="S83" t="n">
         <v>4904034.304930289</v>
       </c>
     </row>
@@ -6472,15 +6057,10 @@
       </c>
       <c r="R84" t="inlineStr">
         <is>
-          <t>{2021: 70300.7397701479, 2022: 52834.2095156673, 2023: 39707.31608617831, 2024: 29841.857486296514, 2025: 22427.515783229115, 2026: 16855.300124597383, 2027: 12667.526133353485, 2028: 9520.223143640198, 2029: 7154.881525451304, 2030: 5377.2195116500425, 2031: 4041.225500885719, 2032: 3037.165121049258, 2033: 2282.567990946419, 2034: 1715.4538609653262, 2035: 1289.2417491058752, 2036: 968.923924717071, 2037: 728.1904829255068, 2038: 547.2683312862987, 2039: 411.29708977469403, 2040: 309.1085056201349, 2041: 232.3091279324481, 2042: 174.59089588125252, 2043: 131.21301429654562, 2044: 98.61255957180884, 2045: 74.11183225564811, 2046: 55.69841918857896, 2047: 41.85990017633428, 2048: 31.45962252250011, 2049: 23.64333992888336, 2050: 17.769047374707846}</t>
-        </is>
-      </c>
-      <c r="S84" t="inlineStr">
-        <is>
           <t>{2021: 70300.7397701479, 2022: 67049.97637300054, 2023: 65749.27698854217, 2024: 64448.57760408381, 2025: 63147.87821962545, 2026: 61847.178835167084, 2027: 60546.47945070872, 2028: 59245.78006625036, 2029: 57945.080681791995, 2030: 56644.38129733363, 2031: 55343.68191287527, 2032: 54042.982528416906, 2033: 52742.28314395854, 2034: 51441.58375950018, 2035: 50140.88437504182, 2036: 48840.18499058299, 2037: 47539.485606124625, 2038: 46238.78622166626, 2039: 44938.0868372079, 2040: 43637.387452749535, 2041: 42336.68806829117, 2042: 41035.98868383281, 2043: 39735.289299374446, 2044: 38434.58991491608, 2045: 37133.89053045772, 2046: 35833.19114599936, 2047: 34532.491761540994, 2048: 33231.79237708263, 2049: 31931.092992624268, 2050: 30630.393608165905}</t>
         </is>
       </c>
-      <c r="T84" t="n">
+      <c r="S84" t="n">
         <v>1436200.537807904</v>
       </c>
     </row>
@@ -6544,15 +6124,10 @@
       </c>
       <c r="R85" t="inlineStr">
         <is>
-          <t>{2021: 241295.112733841, 2022: 175031.41883791765, 2023: 126964.84911489855, 2024: 92098.16739071536, 2025: 66806.46254344196, 2026: 48460.284976509196, 2027: 35152.276151089405, 2028: 25498.870243983056, 2029: 18496.451863454484, 2030: 13417.015274149971, 2031: 9732.477352721477, 2032: 7059.775478062679, 2033: 5121.042463738006, 2034: 3714.7181233877477, 2035: 2694.594085859812, 2036: 1954.6132563428346, 2037: 1417.8436009786103, 2038: 1028.4799155600297, 2039: 746.0420429871674, 2040: 541.1663577323218, 2041: 392.5529794120527, 2042: 284.7513328267554, 2043: 206.55383043597445, 2044: 149.83067662665036, 2045: 108.68465431512995, 2046: 78.83802135548962, 2047: 57.18777549981475, 2048: 41.483051075957604, 2049: 30.091107960233305, 2050: 21.827583911714772}</t>
-        </is>
-      </c>
-      <c r="S85" t="inlineStr">
-        <is>
           <t>{2021: 241295.112733841, 2022: 218378.61377188656, 2023: 215556.82212197874, 2024: 212735.03047206998, 2025: 209913.23882216215, 2026: 207091.4471722534, 2027: 204269.65552234557, 2028: 201447.8638724368, 2029: 198626.07222252898, 2030: 195804.28057262022, 2031: 192982.4889227124, 2032: 190160.69727280363, 2033: 187338.9056228958, 2034: 184517.11397298705, 2035: 181695.32232307922, 2036: 178873.53067317046, 2037: 176051.73902326263, 2038: 173229.94737335388, 2039: 170408.15572344605, 2040: 167586.3640735373, 2041: 164764.57242362946, 2042: 161942.7807737207, 2043: 159120.98912381288, 2044: 156299.19747390412, 2045: 153477.4058239963, 2046: 150655.61417408753, 2047: 147833.8225241797, 2048: 145012.03087427095, 2049: 142190.2392243622, 2050: 139368.44757445436}</t>
         </is>
       </c>
-      <c r="T85" t="n">
+      <c r="S85" t="n">
         <v>5238295.722101643</v>
       </c>
     </row>
@@ -6616,15 +6191,10 @@
       </c>
       <c r="R86" t="inlineStr">
         <is>
-          <t>{2021: 17959.3007233107, 2022: 13997.739096266967, 2023: 10910.040587094803, 2024: 8503.443648538896, 2025: 6627.707138817463, 2026: 5165.730936016683, 2027: 4026.2455091039205, 2028: 3138.114063695232, 2029: 2445.891551942026, 2030: 1906.36330051589, 2031: 1485.847167127374, 2032: 1158.0908022426765, 2033: 902.6327444107268, 2034: 703.5250342241401, 2035: 548.337601139429, 2036: 427.3822681447753, 2037: 333.107929759002, 2038: 259.6291450040699, 2039: 202.35871594024334, 2040: 157.72131405486923, 2041: 122.93027652211713, 2042: 95.81363797506135, 2043: 74.67853714918184, 2044: 58.205533456451136, 2045: 45.36623579251735, 2046: 35.359101236004186, 2047: 27.559395624889156, 2048: 21.480192104989992, 2049: 16.74197283377946, 2050: 13.048936108066528}</t>
-        </is>
-      </c>
-      <c r="S86" t="inlineStr">
-        <is>
           <t>{2021: 17959.3007233107, 2022: 15577.125830624718, 2023: 14405.391130300704, 2024: 13233.65642997669, 2025: 12061.921729652677, 2026: 10890.187029328663, 2027: 9718.452329005115, 2028: 8546.7176286811, 2029: 7374.982928357087, 2030: 6203.248228033073, 2031: 5031.513527709059, 2032: 3859.7788273850456, 2033: 2688.0441270614974, 2034: 1516.3094267374836, 2035: 344.57472641346976, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T86" t="n">
+      <c r="S86" t="n">
         <v>120431.5542609217</v>
       </c>
     </row>
@@ -6688,15 +6258,10 @@
       </c>
       <c r="R87" t="inlineStr">
         <is>
-          <t>{2021: 41796.3025070363, 2022: 31990.852720755596, 2023: 24485.770185742782, 2024: 18741.386696454687, 2025: 14344.640688924024, 2026: 10979.375209906962, 2027: 8403.60400891726, 2028: 6432.111025312946, 2029: 4923.13205120702, 2030: 3768.1608881187826, 2031: 2884.14698835204, 2032: 2207.523536653706, 2033: 1689.6365492330679, 2034: 1293.246310221367, 2035: 989.8495742533083, 2036: 757.6299827074248, 2037: 579.8893141215437, 2038: 443.8467646576931, 2039: 339.71991843914327, 2040: 260.02132306474095, 2041: 199.02008913395568, 2042: 152.32979900277522, 2043: 116.59309251242264, 2044: 89.24024918698069, 2045: 68.30440726242755, 2046: 52.280132496001734, 2047: 40.015166858829716, 2048: 30.62757308165662, 2049: 23.44231716392876, 2050: 17.942728682716268}</t>
-        </is>
-      </c>
-      <c r="S87" t="inlineStr">
-        <is>
           <t>{2021: 41796.3025070363, 2022: 41347.59122243873, 2023: 40453.91104177572, 2024: 39560.23086111271, 2025: 38666.5506804497, 2026: 37772.87049978669, 2027: 36879.19031912368, 2028: 35985.51013846067, 2029: 35091.82995779766, 2030: 34198.14977713465, 2031: 33304.46959647164, 2032: 32410.789415808627, 2033: 31517.109235145617, 2034: 30623.429054482607, 2035: 29729.748873819597, 2036: 28836.068693156587, 2037: 27942.388512493577, 2038: 27048.708331830567, 2039: 26155.028151167324, 2040: 25261.347970504314, 2041: 24367.667789841304, 2042: 23473.987609178293, 2043: 22580.307428515283, 2044: 21686.627247852273, 2045: 20792.947067189263, 2046: 19899.266886526253, 2047: 19005.586705863243, 2048: 18111.906525200233, 2049: 17218.226344537223, 2050: 16324.546163874213}</t>
         </is>
       </c>
-      <c r="T87" t="n">
+      <c r="S87" t="n">
         <v>848981.8702731193</v>
       </c>
     </row>
@@ -6760,15 +6325,10 @@
       </c>
       <c r="R88" t="inlineStr">
         <is>
-          <t>{2021: 43181.7418189813, 2022: 33390.6558271724, 2023: 25819.61379053478, 2024: 19965.239968418653, 2025: 15438.29470999557, 2026: 11937.795084341027, 2027: 9231.0034335235, 2028: 7137.953347975929, 2029: 5519.48424294247, 2030: 4267.988991092092, 2031: 3300.25944930905, 2032: 2551.95420032391, 2033: 1973.3206860188866, 2034: 1525.8873099586976, 2035: 1179.9055770252562, 2036: 912.3722057384349, 2037: 705.4997094790397, 2038: 545.5337601743008, 2039: 421.8387045257226, 2040: 326.1904315125878, 2041: 252.22957606508655, 2042: 195.03870406915394, 2043: 150.81536700977108, 2044: 116.61928864245984, 2045: 90.17687489758403, 2046: 69.73004947085396, 2047: 53.919364634557894, 2048: 41.69361566005506, 2049: 32.239949387204824, 2050: 24.929820070398687}</t>
-        </is>
-      </c>
-      <c r="S88" t="inlineStr">
-        <is>
           <t>{2021: 43181.7418189813, 2022: 41095.81622094149, 2023: 39451.54107758403, 2024: 37807.26593422657, 2025: 36162.990790868644, 2026: 34518.715647511184, 2027: 32874.44050415326, 2028: 31230.1653607958, 2029: 29585.89021743834, 2030: 27941.615074080415, 2031: 26297.339930722956, 2032: 24653.064787365496, 2033: 23008.78964400757, 2034: 21364.51450065011, 2035: 19720.239357292652, 2036: 18075.964213934727, 2037: 16431.689070577268, 2038: 14787.413927219808, 2039: 13143.138783861883, 2040: 11498.863640504424, 2041: 9854.588497146498, 2042: 8210.313353789039, 2043: 6566.0382104315795, 2044: 4921.763067073654, 2045: 3277.487923716195, 2046: 1633.2127803587355, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T88" t="n">
+      <c r="S88" t="n">
         <v>555703.7334257429</v>
       </c>
     </row>
@@ -6832,15 +6392,10 @@
       </c>
       <c r="R89" t="inlineStr">
         <is>
-          <t>{2021: 31891.2540988899, 2022: 24756.417048947445, 2023: 19217.8138621005, 2024: 14918.328807764388, 2025: 11580.741493988404, 2026: 8989.85236743033, 2027: 6978.607166919778, 2028: 5417.325668953652, 2029: 4205.340220698725, 2030: 3264.5049333432853, 2031: 2534.1570242923085, 2032: 1967.2054277440232, 2033: 1527.0944767229873, 2034: 1185.446882134823, 2035: 920.2340338358056, 2036: 714.3556491579747, 2037: 554.5371880637957, 2038: 430.47394292768786, 2039: 334.16661592475924, 2040: 259.4055436646107, 2041: 201.37031312273135, 2042: 156.31895307362666, 2043: 121.34666084142022, 2044: 94.19850765266543, 2045: 73.12404628575045, 2046: 56.76444646996771, 2047: 44.06488079790155, 2048: 34.20651200678179, 2049: 26.553696333290198, 2050: 20.612998741900242}</t>
-        </is>
-      </c>
-      <c r="S89" t="inlineStr">
-        <is>
           <t>{2021: 31891.2540988899, 2022: 26652.894434583373, 2023: 24420.339035529643, 2024: 22187.783636475913, 2025: 19955.228237422183, 2026: 17722.672838368453, 2027: 15490.117439314723, 2028: 13257.562040260993, 2029: 11025.006641207263, 2030: 8792.451242153533, 2031: 6559.895843099803, 2032: 4327.340444046073, 2033: 2094.7850449923426, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T89" t="n">
+      <c r="S89" t="n">
         <v>188431.7039268992</v>
       </c>
     </row>
@@ -6904,15 +6459,10 @@
       </c>
       <c r="R90" t="inlineStr">
         <is>
-          <t>{2021: 72857.259205152, 2022: 55651.618389137875, 2023: 42509.18389078272, 2024: 32470.407283125453, 2025: 24802.342755882848, 2026: 18945.13366637027, 2027: 14471.136584527067, 2028: 11053.698418595517, 2029: 8443.306993584993, 2030: 6449.373801260202, 2031: 4926.318853499444, 2032: 3762.9416737485453, 2033: 2874.302387060276, 2034: 2195.5201351899777, 2035: 1677.0360299337328, 2036: 1280.994785981563, 2037: 978.4808509908935, 2038: 747.4072386814877, 2039: 570.9029255583109, 2040: 436.08107273086665, 2041: 333.0981388966105, 2042: 254.43518894676393, 2043: 194.3489254812953, 2044: 148.45236223845225, 2045: 113.3945237906533, 2046: 86.61578591154594, 2047: 66.16099365543737, 2048: 50.53671262586019, 2049: 38.6021911389307, 2050: 29.486072269054276}</t>
-        </is>
-      </c>
-      <c r="S90" t="inlineStr">
-        <is>
           <t>{2021: 72857.259205152, 2022: 74932.9882925069, 2023: 74190.72850280395, 2024: 73448.46871310077, 2025: 72706.20892339782, 2026: 71963.94913369487, 2027: 71221.68934399169, 2028: 70479.42955428874, 2029: 69737.1697645858, 2030: 68994.90997488284, 2031: 68252.65018517966, 2032: 67510.39039547672, 2033: 66768.13060577377, 2034: 66025.87081607082, 2035: 65283.61102636764, 2036: 64541.35123666469, 2037: 63799.09144696174, 2038: 63056.831657258794, 2039: 62314.57186755561, 2040: 61572.312077852665, 2041: 60830.052288149716, 2042: 60087.79249844677, 2043: 59345.53270874359, 2044: 58603.27291904064, 2045: 57861.01312933769, 2046: 57118.75333963474, 2047: 56376.49354993156, 2048: 55634.23376022861, 2049: 54891.973970525665, 2050: 54149.714180822484}</t>
         </is>
       </c>
-      <c r="T90" t="n">
+      <c r="S90" t="n">
         <v>1881052.958375442</v>
       </c>
     </row>
@@ -6976,15 +6526,10 @@
       </c>
       <c r="R91" t="inlineStr">
         <is>
-          <t>{2021: 385811.84637716, 2022: 292368.3268474023, 2023: 221556.80118745522, 2024: 167895.80691494697, 2025: 127231.4902026905, 2026: 96416.05943975603, 2027: 73064.11724865569, 2028: 55368.00881870613, 2029: 41957.89282056541, 2030: 31795.703105495824, 2031: 24094.792850924998, 2032: 18259.040871111847, 2033: 13836.706362060884, 2034: 10485.46001410193, 2035: 7945.884579063572, 2036: 6021.393592545013, 2037: 4563.01377594577, 2038: 3457.85313639838, 2039: 2620.362089619563, 2040: 1985.7111363229205, 2041: 1504.772463522145, 2042: 1140.3170005721672, 2043: 864.1325471562027, 2044: 654.8398898551798, 2045: 496.23785466331964, 2046: 376.04918731403717, 2047: 284.97018103443895, 2048: 215.95048418754976, 2049: 163.64733829888428, 2050: 124.01199947785756}</t>
-        </is>
-      </c>
-      <c r="S91" t="inlineStr">
-        <is>
           <t>{2021: 385811.84637716, 2022: 370695.2034085393, 2023: 362253.81933544204, 2024: 353812.4352623485, 2025: 345371.05118925497, 2026: 336929.6671161577, 2027: 328488.2830430642, 2028: 320046.8989699669, 2029: 311605.5148968734, 2030: 303164.1308237761, 2031: 294722.7467506826, 2032: 286281.36267758533, 2033: 277839.9786044918, 2034: 269398.59453139454, 2035: 260957.210458301, 2036: 252515.82638520375, 2037: 244074.44231211022, 2038: 235633.05823901668, 2039: 227191.67416591942, 2040: 218750.2900928259, 2041: 210308.90601972863, 2042: 201867.5219466351, 2043: 193426.13787353784, 2044: 184984.7538004443, 2045: 176543.36972734705, 2046: 168101.9856542535, 2047: 159660.60158115625, 2048: 151219.21750806272, 2049: 142777.8334349692, 2050: 134336.44936187193}</t>
         </is>
       </c>
-      <c r="T91" t="n">
+      <c r="S91" t="n">
         <v>7448696.663678605</v>
       </c>
     </row>
@@ -7048,15 +6593,10 @@
       </c>
       <c r="R92" t="inlineStr">
         <is>
-          <t>{2021: 64815.2841043127, 2022: 48227.05310215367, 2023: 35884.262223934194, 2024: 26700.37235384317, 2025: 19866.92325970057, 2026: 14782.364626837134, 2027: 10999.101426239631, 2028: 8184.092006840978, 2029: 6089.530351693222, 2030: 4531.031649350506, 2031: 3371.4008505939096, 2032: 2508.5553522925916, 2033: 1866.538639096343, 2034: 1388.8338114826122, 2035: 1033.3883882795742, 2036: 768.9124157274499, 2037: 572.1240046485514, 2038: 425.69981964125304, 2039: 316.75010132447943, 2040: 235.68397744123732, 2041: 175.36517586025732, 2042: 130.48381667000078, 2043: 97.08898205843234, 2044: 72.24091598257003, 2045: 53.75223667356897, 2046: 39.995380846340446, 2047: 29.759328877013697, 2048: 22.1429984280621, 2049: 16.475921933974835, 2050: 12.259225165748731}</t>
-        </is>
-      </c>
-      <c r="S92" t="inlineStr">
-        <is>
           <t>{2021: 64815.2841043127, 2022: 60480.66651944583, 2023: 59324.284727805294, 2024: 58167.902936164755, 2025: 57011.52114452422, 2026: 55855.13935288321, 2027: 54698.75756124267, 2028: 53542.375769602135, 2029: 52385.99397796113, 2030: 51229.61218632059, 2031: 50073.23039468005, 2032: 48916.848603039514, 2033: 47760.46681139851, 2034: 46604.08501975797, 2035: 45447.70322811743, 2036: 44291.32143647643, 2037: 43134.93964483589, 2038: 41978.55785319535, 2039: 40822.17606155481, 2040: 39665.79426991381, 2041: 38509.41247827327, 2042: 37353.03068663273, 2043: 36196.648894991726, 2044: 35040.26710335119, 2045: 33883.88531171065, 2046: 32727.50352007011, 2047: 31571.121728429105, 2048: 30414.739936788566, 2049: 29258.358145148028, 2050: 28101.976353507023}</t>
         </is>
       </c>
-      <c r="T92" t="n">
+      <c r="S92" t="n">
         <v>1302804.975533225</v>
       </c>
     </row>
@@ -7120,15 +6660,10 @@
       </c>
       <c r="R93" t="inlineStr">
         <is>
-          <t>{2021: 116813.181802889, 2022: 90978.90497758235, 2023: 70858.1088467128, 2024: 55187.20620532601, 2025: 42982.06342675295, 2026: 33476.19681177336, 2027: 26072.637366289513, 2028: 20306.441112658325, 2029: 15815.49057998284, 2030: 12317.753805200447, 2031: 9593.572708871021, 2032: 7471.868554601069, 2033: 5819.398194127642, 2034: 4532.386389608293, 2035: 3530.008722454491, 2036: 2749.315814992048, 2037: 2141.2801057640545, 2038: 1667.7169157280625, 2039: 1298.8864481198268, 2040: 1011.6261274311131, 2041: 787.8959882772289, 2042: 613.6457644878532, 2043: 477.93253154804074, 2044: 372.233490281738, 2045: 289.91073455186466, 2046: 225.7943903564047, 2047: 175.85794743071062, 2048: 136.9653941611545, 2049: 106.67427586752545, 2050: 83.08230850248083}</t>
-        </is>
-      </c>
-      <c r="S93" t="inlineStr">
-        <is>
           <t>{2021: 116813.181802889, 2022: 107194.90756044537, 2023: 101110.43690934218, 2024: 95025.96625823714, 2025: 88941.49560713395, 2026: 82857.02495603077, 2027: 76772.55430492572, 2028: 70688.08365382254, 2029: 64603.61300271936, 2030: 58519.14235161431, 2031: 52434.67170051113, 2032: 46350.201049407944, 2033: 40265.7303983029, 2034: 34181.259747199714, 2035: 28096.78909609653, 2036: 22012.318444991484, 2037: 15927.8477938883, 2038: 9843.377142783254, 2039: 3758.9064916800708, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T93" t="n">
+      <c r="S93" t="n">
         <v>1056990.917370577</v>
       </c>
     </row>
@@ -7192,15 +6727,10 @@
       </c>
       <c r="R94" t="inlineStr">
         <is>
-          <t>{2021: 17780.8039766664, 2022: 13996.276282722954, 2023: 11017.260526542299, 2024: 8672.308766835287, 2025: 6826.464633938549, 2026: 5373.4963377485155, 2027: 4229.782829056789, 2028: 3329.5012514105424, 2029: 2620.838712330858, 2030: 2063.010354221103, 2031: 1623.9121093561582, 2032: 1278.2730506019257, 2033: 1006.2010021853872, 2034: 792.0377076886114, 2035: 623.4576680386265, 2036: 490.7587859301501, 2037: 386.30399193793113, 2038: 304.0817168547264, 2039: 239.35991461401917, 2040: 188.41372416810617, 2041: 148.3110967521041, 2042: 116.74405098105595, 2043: 91.89584419463901, 2044: 72.33641551136259, 2045: 56.94008314401838, 2046: 44.82075930260113, 2047: 35.28095418091677, 2048: 27.77163411070799, 2049: 21.860623644816577, 2050: 17.20773305003514}</t>
-        </is>
-      </c>
-      <c r="S94" t="inlineStr">
-        <is>
           <t>{2021: 17780.8039766664, 2022: 16518.201988180168, 2023: 15487.26094591245, 2024: 14456.3199036445, 2025: 13425.378861376783, 2026: 12394.437819109065, 2027: 11363.496776841348, 2028: 10332.555734573398, 2029: 9301.61469230568, 2030: 8270.673650037963, 2031: 7239.732607770013, 2032: 6208.791565502295, 2033: 5177.850523234578, 2034: 4146.909480966628, 2035: 3115.96843869891, 2036: 2085.0273964311928, 2037: 1054.0863541634753, 2038: 23.145311895757914, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T94" t="n">
+      <c r="S94" t="n">
         <v>149491.8540389774</v>
       </c>
     </row>
@@ -7264,15 +6794,10 @@
       </c>
       <c r="R95" t="inlineStr">
         <is>
-          <t>{2021: 161074.659994972, 2022: 88182.7920236098, 2023: 48277.021409338726, 2024: 26429.995497690106, 2025: 14469.506229164179, 2026: 7921.5530147978625, 2027: 4336.775641989402, 2028: 2374.2343116077095, 2029: 1299.8109728889476, 2030: 711.6014442982522, 2031: 389.5771201268524, 2032: 213.2799669567854, 2033: 116.76338767090786, 2034: 63.92390666090619, 2035: 34.996122708508565, 2036: 19.159163896626993, 2037: 10.488978001227824, 2038: 5.742351811584546, 2039: 3.1437385343117605, 2040: 1.7210878567521155, 2041: 0.9422359328963944, 2042: 0.5158415067296644, 2043: 0.28240534114122856, 2044: 0.1546071335180277, 2045: 0.08464204550121228, 2046: 0.046338585443044256, 2047: 0.025368769010096322, 2048: 0.01388852151904064, 2049: 0.007603484028258814, 2050: 0.004162643899044797}</t>
-        </is>
-      </c>
-      <c r="S95" t="inlineStr">
-        <is>
           <t>{2021: 161074.659994972, 2022: 123270.19169470947, 2023: 127277.5643997658, 2024: 131284.9371048212, 2025: 135292.30980987754, 2026: 139299.68251493294, 2027: 143307.05521998927, 2028: 147314.42792504467, 2029: 151321.800630101, 2030: 155329.1733351564, 2031: 159336.5460402118, 2032: 163343.91874526814, 2033: 167351.29145032354, 2034: 171358.66415537987, 2035: 175366.03686043527, 2036: 179373.4095654916, 2037: 183380.782270547, 2038: 187388.15497560333, 2039: 191395.52768065874, 2040: 195402.90038571414, 2041: 199410.27309077047, 2042: 203417.64579582587, 2043: 207425.0185008822, 2044: 211432.3912059376, 2045: 215439.76391099393, 2046: 219447.13661604933, 2047: 223454.50932110567, 2048: 227461.88202616107, 2049: 231469.25473121647, 2050: 235476.6274362728}</t>
         </is>
       </c>
-      <c r="T95" t="n">
+      <c r="S95" t="n">
         <v>5164627.893678596</v>
       </c>
     </row>
@@ -7336,15 +6861,10 @@
       </c>
       <c r="R96" t="inlineStr">
         <is>
-          <t>{2021: 81092.8269941256, 2022: 63210.34467837942, 2023: 49271.28357048113, 2024: 38406.04567234902, 2025: 29936.795579449026, 2026: 23335.173248803356, 2027: 18189.33189113521, 2028: 14178.244623182076, 2029: 11051.676982856214, 2030: 8614.575878715623, 2031: 6714.901067527387, 2032: 5234.140018208659, 2033: 4079.9144253515237, 2034: 3180.217124548438, 2035: 2478.9198754823733, 2036: 1932.2717627130833, 2037: 1506.1697644631583, 2038: 1174.0312119438938, 2039: 915.1354111199619, 2040: 713.3309678360774, 2041: 556.0281718868523, 2042: 433.4135792109354, 2043: 337.8377933747202, 2044: 263.33825266871196, 2045: 205.2672515584797, 2046: 160.00199035033054, 2047: 124.71856431893515, 2048: 97.21579245182326, 2049: 75.77789524475075, 2050: 59.06745460692609}</t>
-        </is>
-      </c>
-      <c r="S96" t="inlineStr">
-        <is>
           <t>{2021: 81092.8269941256, 2022: 77461.40557587333, 2023: 73946.3310853364, 2024: 70431.25659479853, 2025: 66916.18210426159, 2026: 63401.10761372466, 2027: 59886.03312318772, 2028: 56370.958632650785, 2029: 52855.88414211385, 2030: 49340.809651576914, 2031: 45825.73516103905, 2032: 42310.66067050211, 2033: 38795.586179965176, 2034: 35280.51168942824, 2035: 31765.437198891304, 2036: 28250.36270835437, 2037: 24735.288217817433, 2038: 21220.213727279566, 2039: 17705.13923674263, 2040: 14190.064746205695, 2041: 10674.99025566876, 2042: 7159.915765131824, 2043: 3644.841274594888, 2044: 129.76678405795246, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T96" t="n">
+      <c r="S96" t="n">
         <v>932844.8956362656</v>
       </c>
     </row>
@@ -7408,15 +6928,10 @@
       </c>
       <c r="R97" t="inlineStr">
         <is>
-          <t>{2021: 104241.611582051, 2022: 80528.98577922294, 2023: 62210.44985980346, 2024: 48058.96950409184, 2025: 37126.63314604307, 2026: 28681.157814744747, 2027: 22156.83847114392, 2028: 17116.655269194973, 2029: 13223.000564183556, 2030: 10215.064869307378, 2031: 7891.3669993177255, 2032: 6096.258214182371, 2033: 4709.496367004498, 2034: 3638.1916991689072, 2035: 2810.584786228566, 2036: 2171.239861380578, 2037: 1677.331549913461, 2038: 1295.7762881831823, 2039: 1001.0162803557904, 2040: 773.3075552279948, 2041: 597.3974516779588, 2042: 461.50294647787194, 2043: 356.52138958666325, 2044: 275.4207794400287, 2045: 212.76873692009914, 2046: 164.36862716972945, 2047: 126.97845552284875, 2048: 98.09370829823072, 2049: 75.77959243619023, 2050: 58.54143685073297}</t>
-        </is>
-      </c>
-      <c r="S97" t="inlineStr">
-        <is>
           <t>{2021: 104241.611582051, 2022: 103744.41315040365, 2023: 100983.2006800687, 2024: 98221.98820973467, 2025: 95460.77573939972, 2026: 92699.5632690657, 2027: 89938.35079873167, 2028: 87177.13832839672, 2029: 84415.92585806269, 2030: 81654.71338772774, 2031: 78893.50091739371, 2032: 76132.28844705876, 2033: 73371.07597672474, 2034: 70609.86350638978, 2035: 67848.65103605576, 2036: 65087.438565720804, 2037: 62326.22609538678, 2038: 59565.01362505276, 2039: 56803.8011547178, 2040: 54042.58868438378, 2041: 51281.376214048825, 2042: 48520.1637437148, 2043: 45758.95127337985, 2044: 42997.738803045824, 2045: 40236.52633271087, 2046: 37475.31386237685, 2047: 34714.10139204189, 2048: 31952.88892170787, 2049: 29191.676451373845, 2050: 26430.46398103889}</t>
         </is>
       </c>
-      <c r="T97" t="n">
+      <c r="S97" t="n">
         <v>1926441.292206421</v>
       </c>
     </row>
@@ -7480,15 +6995,10 @@
       </c>
       <c r="R98" t="inlineStr">
         <is>
-          <t>{2021: 196040.384620013, 2022: 149371.1322748057, 2023: 113811.93319072781, 2024: 86717.93498077065, 2025: 66073.9171763916, 2026: 50344.40144360849, 2027: 38359.444468063324, 2028: 29227.61891501726, 2029: 22269.710088025262, 2030: 16968.19671991407, 2031: 12928.758335319368, 2032: 9850.94614661779, 2033: 7505.836018178366, 2034: 5719.001352080938, 2035: 4357.539438097323, 2036: 3320.186302747494, 2037: 2529.784811257025, 2038: 1927.5458084899694, 2039: 1468.6754491110603, 2040: 1119.043482816817, 2041: 852.6446855176497, 2042: 649.664620637891, 2043: 495.00586408081017, 2044: 377.16507516416596, 2045: 287.3773913522122, 2046: 218.96450784701085, 2047: 166.8379529478064, 2048: 127.12061337019301, 2049: 96.85835901300875, 2050: 73.80031815432271}</t>
-        </is>
-      </c>
-      <c r="S98" t="inlineStr">
-        <is>
           <t>{2021: 196040.384620013, 2022: 188826.4148816131, 2023: 183957.67806071043, 2024: 179088.94123980775, 2025: 174220.20441890694, 2026: 169351.46759800427, 2027: 164482.7307771016, 2028: 159613.99395620078, 2029: 154745.2571352981, 2030: 149876.52031439543, 2031: 145007.78349349461, 2032: 140139.04667259194, 2033: 135270.30985169113, 2034: 130401.57303078845, 2035: 125532.83620988578, 2036: 120664.09938898496, 2037: 115795.36256808229, 2038: 110926.62574717961, 2039: 106057.8889262788, 2040: 101189.15210537612, 2041: 96320.41528447345, 2042: 91451.67846357264, 2043: 86582.94164266996, 2044: 81714.20482176915, 2045: 76845.46800086647, 2046: 71976.7311799638, 2047: 67107.99435906298, 2048: 62239.25753816031, 2049: 57370.520717257634, 2050: 52501.78389635682}</t>
         </is>
       </c>
-      <c r="T98" t="n">
+      <c r="S98" t="n">
         <v>3571028.182642373</v>
       </c>
     </row>
@@ -7552,15 +7062,10 @@
       </c>
       <c r="R99" t="inlineStr">
         <is>
-          <t>{2021: 70156.4487205661, 2022: 53769.46660472666, 2023: 41210.1181243127, 2024: 31584.35340830622, 2025: 24206.952700585643, 2026: 18552.748301451298, 2027: 14219.239975987415, 2028: 10897.942569452229, 2029: 8352.42618083965, 2030: 6401.485662250298, 2031: 4906.2413479333045, 2032: 3760.252765403948, 2033: 2881.941563205839, 2034: 2208.784273798968, 2035: 1692.8615175508944, 2036: 1297.4468134345045, 2037: 994.3921674861637, 2038: 762.1243295055087, 2039: 584.1090795119352, 2040: 447.6742226424542, 2041: 343.1075061972746, 2042: 262.96524314944736, 2043: 201.5424257867701, 2044: 154.46660899186253, 2045: 118.38665333267595, 2046: 90.73417082684551, 2047: 69.54069165635309, 2048: 53.29753666094203, 2049: 40.84842049259293, 2050: 31.307140278445168}</t>
-        </is>
-      </c>
-      <c r="S99" t="inlineStr">
-        <is>
           <t>{2021: 70156.4487205661, 2022: 64621.3902753545, 2023: 61861.08166215848, 2024: 59100.77304896247, 2025: 56340.46443576738, 2026: 53580.15582257137, 2027: 50819.84720937535, 2028: 48059.53859618027, 2029: 45299.22998298425, 2030: 42538.92136978824, 2031: 39778.61275659315, 2032: 37018.30414339714, 2033: 34257.99553020112, 2034: 31497.686917006038, 2035: 28737.378303810023, 2036: 25977.069690614007, 2037: 23216.761077418923, 2038: 20456.452464222908, 2039: 17696.143851026893, 2040: 14935.835237830877, 2041: 12175.526624635793, 2042: 9415.218011439778, 2043: 6654.909398243763, 2044: 3894.6007850486785, 2045: 1134.2921718526632, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T99" t="n">
+      <c r="S99" t="n">
         <v>824146.4137267671</v>
       </c>
     </row>
@@ -7624,15 +7129,10 @@
       </c>
       <c r="R100" t="inlineStr">
         <is>
-          <t>{2021: 35690.6495938968, 2022: 26653.205262849795, 2023: 19904.186638986903, 2024: 14864.127666920047, 2025: 11100.292380987426, 2026: 8289.520495550132, 2027: 6190.481087132686, 2028: 4622.952088811288, 2029: 3452.3465486175364, 2030: 2578.157087242516, 2031: 1925.3264041990526, 2032: 1437.802910089848, 2033: 1073.7281760402777, 2034: 801.8429980439648, 2035: 598.803503399929, 2036: 447.176862002565, 2037: 333.9445156467409, 2038: 249.3844136548745, 2039: 186.23628435262358, 2040: 139.07827318138135, 2041: 103.86142602851199, 2042: 77.56204883711611, 2043: 57.9220953326763, 2044: 43.25529273695737, 2045: 32.3023595574996, 2046: 24.122884552587163, 2047: 18.01458367465748, 2048: 13.453002449345583, 2049: 10.046486678273977, 2050: 7.502555281378574}</t>
-        </is>
-      </c>
-      <c r="S100" t="inlineStr">
-        <is>
           <t>{2021: 35690.6495938968, 2022: 34365.34639013617, 2023: 33919.957372837, 2024: 33474.56835553795, 2025: 33029.179338238784, 2026: 32583.790320939734, 2027: 32138.401303640567, 2028: 31693.012286341516, 2029: 31247.62326904235, 2030: 30802.2342517433, 2031: 30356.845234444132, 2032: 29911.456217144965, 2033: 29466.067199845915, 2034: 29020.678182546748, 2035: 28575.289165247697, 2036: 28129.90014794853, 2037: 27684.51113064948, 2038: 27239.122113350313, 2039: 26793.733096051263, 2040: 26348.344078752096, 2041: 25902.955061453045, 2042: 25457.56604415388, 2043: 25012.177026854828, 2044: 24566.78800955566, 2045: 24121.39899225661, 2046: 23676.009974957444, 2047: 23230.620957658393, 2048: 22785.231940359226, 2049: 22339.84292306006, 2050: 21894.45390576101}</t>
         </is>
       </c>
-      <c r="T100" t="n">
+      <c r="S100" t="n">
         <v>822665.2021345767</v>
       </c>
     </row>
@@ -7696,15 +7196,10 @@
       </c>
       <c r="R101" t="inlineStr">
         <is>
-          <t>{2021: 38712.3814730806, 2022: 30173.35826835228, 2023: 23517.838855339574, 2024: 18330.367455512376, 2025: 14287.127874329324, 2026: 11135.73000611363, 2027: 8679.454951324888, 2028: 6764.975283229709, 2029: 5272.783929332225, 2030: 4109.734212088789, 2031: 3203.2253777848405, 2032: 2496.6706583367645, 2033: 1945.9649700048117, 2034: 1516.7317530813264, 2035: 1182.1770927353664, 2036: 921.4171693505173, 2037: 718.1746332179798, 2038: 559.7625277173162, 2039: 436.2923346825817, 2040: 340.05670597319164, 2041: 265.0483496609419, 2042: 206.58503838923613, 2043: 161.01733189765713, 2044: 125.50076895012526, 2045: 97.8183082618939, 2046: 76.24193470098544, 2047: 59.42479184353031, 2048: 46.317107501224804, 2049: 36.100664061704684, 2050: 28.137723100726728}</t>
-        </is>
-      </c>
-      <c r="S101" t="inlineStr">
-        <is>
           <t>{2021: 38712.3814730806, 2022: 36430.448973326944, 2023: 34617.57751195319, 2024: 32804.70605057897, 2025: 30991.83458920475, 2026: 29178.96312783053, 2027: 27366.091666456312, 2028: 25553.220205082092, 2029: 23740.348743707873, 2030: 21927.477282333653, 2031: 20114.605820959434, 2032: 18301.734359585214, 2033: 16488.86289821146, 2034: 14675.991436837241, 2035: 12863.119975463022, 2036: 11050.248514088802, 2037: 9237.377052714583, 2038: 7424.505591340363, 2039: 5611.6341299661435, 2040: 3798.762668591924, 2041: 1985.8912072177045, 2042: 173.019745843485, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T101" t="n">
+      <c r="S101" t="n">
         <v>403692.612287834</v>
       </c>
     </row>
@@ -7768,15 +7263,10 @@
       </c>
       <c r="R102" t="inlineStr">
         <is>
-          <t>{2021: 685614.104946655, 2022: 512309.66025283316, 2023: 382811.8267910991, 2024: 286047.4945149701, 2025: 213742.531948844, 2026: 159714.2811593886, 2027: 119342.8905968295, 2028: 89176.28049675246, 2029: 66634.96219561766, 2030: 49791.47102881349, 2031: 37205.55254364984, 2032: 27801.00911815288, 2033: 20773.676377493706, 2034: 15522.66064885606, 2035: 11598.957702094269, 2036: 8667.05926376652, 2037: 6476.264351587211, 2038: 4839.2423168238765, 2039: 3616.0145617279404, 2040: 2701.9852395426974, 2041: 2018.9974653248896, 2042: 1508.6502714123776, 2043: 1127.304853285881, 2044: 842.3530995372315, 2045: 629.4293351365881, 2046: 470.3268595416104, 2047: 351.44112683955365, 2048: 262.6064472580436, 2049: 196.2267386337387, 2050: 146.62600007302055}</t>
-        </is>
-      </c>
-      <c r="S102" t="inlineStr">
-        <is>
           <t>{2021: 685614.104946655, 2022: 704453.9260673192, 2023: 706737.6150065442, 2024: 709021.3039457691, 2025: 711304.992884994, 2026: 713588.681824219, 2027: 715872.3707634439, 2028: 718156.0597026697, 2029: 720439.7486418947, 2030: 722723.4375811196, 2031: 725007.1265203445, 2032: 727290.8154595695, 2033: 729574.5043987944, 2034: 731858.1933380202, 2035: 734141.8822772452, 2036: 736425.5712164701, 2037: 738709.260155695, 2038: 740992.94909492, 2039: 743276.6380341449, 2040: 745560.3269733707, 2041: 747844.0159125957, 2042: 750127.7048518206, 2043: 752411.3937910455, 2044: 754695.0827302705, 2045: 756978.7716694954, 2046: 759262.4606087212, 2047: 761546.1495479462, 2048: 763829.8384871711, 2049: 766113.527426396, 2050: 768397.216365621}</t>
         </is>
       </c>
-      <c r="T102" t="n">
+      <c r="S102" t="n">
         <v>21314950.00956815</v>
       </c>
     </row>
@@ -7840,15 +7330,10 @@
       </c>
       <c r="R103" t="inlineStr">
         <is>
-          <t>{2021: 67082.1645574866, 2022: 51089.42431701824, 2023: 38909.43731858209, 2024: 29633.223170697656, 2025: 22568.507179747932, 2026: 17188.056573811537, 2027: 13090.333641989944, 2028: 9969.529371907023, 2029: 7592.741225364803, 2030: 5782.591852109331, 2031: 4403.991593493908, 2032: 3354.056874771508, 2033: 2554.432105597429, 2034: 1945.4420797653977, 2035: 1481.6384735489933, 2036: 1128.4080822212488, 2037: 859.3896707961892, 2038: 654.5066611162164, 2039: 498.4688366670986, 2040: 379.6312488317541, 2041: 289.1251658843564, 2042: 220.19620830714018, 2043: 167.7002761227464, 2044: 127.71964979713718, 2045: 97.27061470288662, 2046: 74.08078944552112, 2047: 56.41954028598091, 2048: 42.96882565516278, 2049: 32.72483201431808, 2050: 24.923060242784747}</t>
-        </is>
-      </c>
-      <c r="S103" t="inlineStr">
-        <is>
           <t>{2021: 67082.1645574866, 2022: 63796.74409774132, 2023: 61946.72401086707, 2024: 60096.70392399235, 2025: 58246.68383711809, 2026: 56396.66375024337, 2027: 54546.64366336912, 2028: 52696.623576494865, 2029: 50846.603489620145, 2030: 48996.58340274589, 2031: 47146.56331587117, 2032: 45296.54322899692, 2033: 43446.5231421222, 2034: 41596.503055247944, 2035: 39746.48296837369, 2036: 37896.46288149897, 2037: 36046.442794624716, 2038: 34196.422707749996, 2039: 32346.402620875742, 2040: 30496.382534001023, 2041: 28646.36244712677, 2042: 26796.342360252514, 2043: 24946.322273377795, 2044: 23096.30218650354, 2045: 21246.28209962882, 2046: 19396.262012754567, 2047: 17546.241925879847, 2048: 15696.221839005593, 2049: 13846.20175213134, 2050: 11996.18166525662}</t>
         </is>
       </c>
-      <c r="T103" t="n">
+      <c r="S103" t="n">
         <v>1126540.415009587</v>
       </c>
     </row>
@@ -7912,15 +7397,10 @@
       </c>
       <c r="R104" t="inlineStr">
         <is>
-          <t>{2021: 58815.7302393248, 2022: 45703.58324090827, 2023: 35514.60659519323, 2024: 27597.120229347634, 2025: 21444.72705650492, 2026: 16663.92415970081, 2027: 12948.934610759183, 2028: 10062.150184241329, 2029: 7818.934095636137, 2030: 6075.8117571777075, 2031: 4721.294239999021, 2032: 3668.747517451431, 2033: 2850.8514112030507, 2034: 2215.2938380464666, 2035: 1721.4249643462408, 2036: 1337.6572701017462, 2037: 1039.4452324766908, 2038: 807.7154107167819, 2039: 627.6465217459254, 2040: 487.7214808990312, 2041: 378.9907769561992, 2042: 294.5000674423829, 2043: 228.84538357404833, 2044: 177.82749606126745, 2045: 138.18333523511018, 2046: 107.37728731286926, 2047: 83.4390182510294, 2048: 64.83745250902052, 2049: 50.38284649049824, 2050: 39.15069334551586}</t>
-        </is>
-      </c>
-      <c r="S104" t="inlineStr">
-        <is>
           <t>{2021: 58815.7302393248, 2022: 57155.65197950788, 2023: 54992.5366402138, 2024: 52829.42130092066, 2025: 50666.30596162658, 2026: 48503.19062233344, 2027: 46340.07528304029, 2028: 44176.95994374622, 2029: 42013.84460445307, 2030: 39850.729265158996, 2031: 37687.61392586585, 2032: 35524.498586571775, 2033: 33361.38324727863, 2034: 31198.267907985486, 2035: 29035.15256869141, 2036: 26872.037229398265, 2037: 24708.92189010419, 2038: 22545.806550811045, 2039: 20382.6912115179, 2040: 18219.575872223824, 2041: 16056.46053293068, 2042: 13893.345193636604, 2043: 11730.229854343459, 2044: 9567.114515050314, 2045: 7403.999175756238, 2046: 5240.883836463094, 2047: 3077.768497169018, 2048: 914.6531578758731, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T104" t="n">
+      <c r="S104" t="n">
         <v>813356.984474337</v>
       </c>
     </row>
@@ -7984,15 +7464,10 @@
       </c>
       <c r="R105" t="inlineStr">
         <is>
-          <t>{2021: 82433.5722273519, 2022: 63093.72713886705, 2023: 48291.22767232148, 2024: 36961.561407954956, 2025: 28289.962536965057, 2026: 21652.81849187895, 2027: 16572.823241799615, 2028: 12684.652130019296, 2029: 9708.689781580702, 2030: 7430.921739816458, 2031: 5687.543751581953, 2032: 4353.181887629177, 2033: 3331.8763555026467, 2034: 2550.180611544268, 2035: 1951.8794989963503, 2036: 1493.9465704333743, 2037: 1143.4498679130884, 2038: 875.1836419766854, 2039: 669.8556960625689, 2040: 512.7000003496667, 2041: 392.41480202923464, 2042: 300.34986687462646, 2043: 229.88440309875293, 2044: 175.95093128551147, 2045: 134.67085980139163, 2046: 103.07555832266011, 2047: 78.89287065662822, 2048: 60.38371406109735, 2049: 46.21701420502216, 2050: 35.37398179691242}</t>
-        </is>
-      </c>
-      <c r="S105" t="inlineStr">
-        <is>
           <t>{2021: 82433.5722273519, 2022: 78519.97336343955, 2023: 76001.00901693944, 2024: 73482.04467044026, 2025: 70963.08032394014, 2026: 68444.11597744003, 2027: 65925.15163094085, 2028: 63406.18728444073, 2029: 60887.22293794155, 2030: 58368.25859144144, 2031: 55849.294244941324, 2032: 53330.32989844214, 2033: 50811.36555194203, 2034: 48292.401205441914, 2035: 45773.43685894273, 2036: 43254.47251244262, 2037: 40735.508165943436, 2038: 38216.54381944332, 2039: 35697.57947294321, 2040: 33178.61512644403, 2041: 30659.650779943913, 2042: 28140.68643344473, 2043: 25621.722086944617, 2044: 23102.757740444504, 2045: 20583.79339394532, 2046: 18064.829047445208, 2047: 15545.864700946026, 2048: 13026.900354445912, 2049: 10507.936007945798, 2050: 7988.971661446616}</t>
         </is>
       </c>
-      <c r="T105" t="n">
+      <c r="S105" t="n">
         <v>1291602.003143796</v>
       </c>
     </row>
@@ -8056,15 +7531,10 @@
       </c>
       <c r="R106" t="inlineStr">
         <is>
-          <t>{2021: 196241.92700692, 2022: 152642.72705132235, 2023: 118729.99046143123, 2024: 92351.66920355035, 2025: 71833.83719257129, 2026: 55874.46561940933, 2027: 43460.7982848703, 2028: 33805.083710761275, 2029: 26294.585690788073, 2030: 20452.700030738273, 2031: 15908.710008460457, 2032: 12374.261283494423, 2033: 9625.06339173677, 2034: 7486.656631254661, 2035: 5823.341128581966, 2036: 4529.565541748537, 2037: 3523.228940907293, 2038: 2740.4708146147964, 2039: 2131.6185838952274, 2040: 1658.0354598106442, 2041: 1289.6686146195732, 2042: 1003.142077386402, 2043: 780.2733322466281, 2044: 606.9194850259901, 2045: 472.07977779225814, 2046: 367.1974983483094, 2047: 285.6169849592484, 2048: 222.1612687018653, 2049: 172.80355129532782, 2050: 134.41167092158537}</t>
-        </is>
-      </c>
-      <c r="S106" t="inlineStr">
-        <is>
           <t>{2021: 196241.92700692, 2022: 189940.06575100496, 2023: 182382.14565159753, 2024: 174824.2255521901, 2025: 167266.30545278266, 2026: 159708.38535337523, 2027: 152150.46525396965, 2028: 144592.54515456222, 2029: 137034.6250551548, 2030: 129476.70495574735, 2031: 121918.78485633992, 2032: 114360.86475693434, 2033: 106802.94465752691, 2034: 99245.02455811948, 2035: 91687.10445871204, 2036: 84129.1843593046, 2037: 76571.26425989904, 2038: 69013.3441604916, 2039: 61455.424061084166, 2040: 53897.50396167673, 2041: 46339.58386227116, 2042: 38781.663762863725, 2043: 31223.74366345629, 2044: 23665.823564048856, 2045: 16107.903464641422, 2046: 8549.98336523585, 2047: 992.0632658284158, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T106" t="n">
+      <c r="S106" t="n">
         <v>2580238.640722279</v>
       </c>
     </row>
@@ -8128,15 +7598,10 @@
       </c>
       <c r="R107" t="inlineStr">
         <is>
-          <t>{2021: 80865.1948404024, 2022: 62416.445372792994, 2023: 48176.63100501677, 2024: 37185.51675173173, 2025: 28701.93758358343, 2026: 22153.819363383045, 2027: 17099.602107215305, 2028: 13198.46422095369, 2029: 10187.33983981358, 2030: 7863.179478646489, 2031: 6069.257773434473, 2032: 4684.605002394711, 2033: 3615.8497212819816, 2034: 2790.9224364085203, 2035: 2154.1957344639954, 2036: 1662.7331529695052, 2037: 1283.3938410298715, 2038: 990.5977686508636, 2039: 764.6007857327953, 2040: 590.1632126018401, 2041: 455.52218099634854, 2042: 351.5984272636501, 2043: 271.3840493647952, 2044: 209.46994223727523, 2045: 161.68104501199667, 2046: 124.7948036695432, 2047: 96.32386419672305, 2048: 74.34834256687209, 2049: 57.38636098684481, 2050: 44.2941202670446}</t>
-        </is>
-      </c>
-      <c r="S107" t="inlineStr">
-        <is>
           <t>{2021: 80865.1948404024, 2022: 75703.8092484381, 2023: 72419.05632735603, 2024: 69134.30340627395, 2025: 65849.55048519094, 2026: 62564.797564108856, 2027: 59280.04464302678, 2028: 55995.2917219447, 2029: 52710.53880086262, 2030: 49425.78587977961, 2031: 46141.03295869753, 2032: 42856.28003761545, 2033: 39571.52711653337, 2034: 36286.77419545129, 2035: 33002.02127436828, 2036: 29717.2683532862, 2037: 26432.51543220412, 2038: 23147.76251112204, 2039: 19863.00959003996, 2040: 16578.25666895788, 2041: 13293.50374787487, 2042: 10008.750826792791, 2043: 6723.997905710712, 2044: 3439.2449846286327, 2045: 154.49206354655325, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T107" t="n">
+      <c r="S107" t="n">
         <v>950732.2131640124</v>
       </c>
     </row>
@@ -8200,15 +7665,10 @@
       </c>
       <c r="R108" t="inlineStr">
         <is>
-          <t>{2021: 39702.8662282482, 2022: 31711.30103803911, 2023: 25328.3127657333, 2024: 20230.120069475313, 2025: 16158.113720826803, 2026: 12905.738478987827, 2027: 10308.015438296114, 2028: 8233.17336308557, 2029: 6575.964503777118, 2030: 5252.325834510327, 2031: 4195.114900030129, 2032: 3350.7039698148387, 2033: 2676.259735639729, 2034: 2137.5705634187166, 2035: 1707.311085223195, 2036: 1363.6561017494798, 2037: 1089.1734845120436, 2038: 869.9399194871529, 2039: 694.8346377128001, 2040: 554.9753068580831, 2041: 443.2674689852314, 2042: 354.0446694339466, 2043: 282.78102212542194, 2044: 225.8616309691885, 2045: 180.39922184536084, 2046: 144.08768369715398, 2047: 115.0850895078014, 2048: 91.92026332282741, 2049: 73.41815386749268, 2050: 58.64022928633435}</t>
-        </is>
-      </c>
-      <c r="S108" t="inlineStr">
-        <is>
           <t>{2021: 39702.8662282482, 2022: 32285.66622049734, 2023: 28305.32930536568, 2024: 24324.992390234023, 2025: 20344.655475102365, 2026: 16364.318559970707, 2027: 12383.981644839048, 2028: 8403.64472970739, 2029: 4423.3078145748, 2030: 442.9708994431421, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T108" t="n">
+      <c r="S108" t="n">
         <v>167130.3001538586</v>
       </c>
     </row>
@@ -8272,15 +7732,10 @@
       </c>
       <c r="R109" t="inlineStr">
         <is>
-          <t>{2021: 191950.953151967, 2022: 142414.7788601313, 2023: 105662.24811461565, 2024: 78394.32652982953, 2025: 58163.351071227495, 2026: 43153.31934827729, 2027: 32016.87895344821, 2028: 23754.38444599458, 2029: 17624.165716731655, 2030: 13075.953111603114, 2031: 9701.483322669921, 2032: 7197.8522603086685, 2033: 5340.32533356686, 2034: 3962.1644953175255, 2035: 2939.6612579536277, 2036: 2181.032191300017, 2037: 1618.1801241951084, 2038: 1200.5815066761213, 2039: 890.7512412375381, 2040: 660.8778907172177, 2041: 490.3272274221482, 2042: 363.7900334214149, 2043: 269.90789214895693, 2044: 200.25361761327602, 2045: 148.57480101053486, 2046: 110.2325728664219, 2047: 81.78520205380866, 2048: 60.679154092572254, 2049: 45.01987705511402, 2050: 33.401740026986985}</t>
-        </is>
-      </c>
-      <c r="S109" t="inlineStr">
-        <is>
           <t>{2021: 191950.953151967, 2022: 184945.44318343047, 2023: 183286.03948637284, 2024: 181626.63578931475, 2025: 179967.23209225712, 2026: 178307.82839519903, 2027: 176648.4246981414, 2028: 174989.02100108378, 2029: 173329.61730402568, 2030: 171670.21360696806, 2031: 170010.80990990996, 2032: 168351.40621285234, 2033: 166692.00251579424, 2034: 165032.59881873662, 2035: 163373.195121679, 2036: 161713.7914246209, 2037: 160054.38772756327, 2038: 158394.98403050518, 2039: 156735.58033344755, 2040: 155076.17663638946, 2041: 153416.77293933183, 2042: 151757.3692422742, 2043: 150097.9655452161, 2044: 148438.56184815848, 2045: 146779.1581511004, 2046: 145119.75445404276, 2047: 143460.35075698467, 2048: 141800.94705992704, 2049: 140141.54336286942, 2050: 138482.13966581132}</t>
         </is>
       </c>
-      <c r="T109" t="n">
+      <c r="S109" t="n">
         <v>4716434.358057086</v>
       </c>
     </row>
@@ -8344,15 +7799,10 @@
       </c>
       <c r="R110" t="inlineStr">
         <is>
-          <t>{2021: 170972.7920826, 2022: 131252.57988882053, 2023: 100760.12398012677, 2024: 77351.64210174332, 2025: 59381.393149300704, 2026: 45585.97279310177, 2027: 34995.48941650062, 2028: 26865.375563198035, 2029: 20624.040874575356, 2030: 15832.686239414761, 2031: 12154.453876435831, 2032: 9330.744435940185, 2033: 7163.036086518023, 2034: 5498.927371660396, 2035: 4221.422574669006, 2036: 3240.7062958797087, 2037: 2487.828951115569, 2038: 1909.8592482379443, 2039: 1466.1628350471601, 2040: 1125.545487635699, 2041: 864.0599901008497, 2042: 663.3225175655715, 2043: 509.2201552558558, 2044: 390.9186853334355, 2045: 300.1008836070894, 2046: 230.38177431948114, 2047: 176.8597323028292, 2048: 135.77187259115325, 2049: 104.22949954116527, 2050: 80.01501612425758}</t>
-        </is>
-      </c>
-      <c r="S110" t="inlineStr">
-        <is>
           <t>{2021: 170972.7920826, 2022: 165931.0548950415, 2023: 161119.87476525642, 2024: 156308.6946354732, 2025: 151497.5145056881, 2026: 146686.334375903, 2027: 141875.15424611978, 2028: 137063.9741163347, 2029: 132252.7939865496, 2030: 127441.61385676451, 2031: 122630.43372698128, 2032: 117819.25359719619, 2033: 113008.0734674111, 2034: 108196.89333762787, 2035: 103385.71320784278, 2036: 98574.53307805769, 2037: 93763.35294827446, 2038: 88952.17281848937, 2039: 84140.99268870428, 2040: 79329.81255892105, 2041: 74518.63242913596, 2042: 69707.45229935087, 2043: 64896.27216956578, 2044: 60085.092039782554, 2045: 55273.91190999746, 2046: 50462.73178021237, 2047: 45651.551650429145, 2048: 40840.371520644054, 2049: 36029.19139085896, 2050: 31218.011261075735}</t>
         </is>
       </c>
-      <c r="T110" t="n">
+      <c r="S110" t="n">
         <v>2928538.849674452</v>
       </c>
     </row>
@@ -8416,15 +7866,10 @@
       </c>
       <c r="R111" t="inlineStr">
         <is>
-          <t>{2021: 33670.3774418063, 2022: 25625.463605533765, 2023: 19502.733111129262, 2024: 14842.915806674442, 2025: 11296.475647216057, 2026: 8597.39175982947, 2027: 6543.204038172701, 2028: 4979.826473094062, 2029: 3789.989056959606, 2030: 2884.441281133422, 2031: 2195.257395012391, 2032: 1670.7412495715414, 2033: 1271.5485342911782, 2034: 967.7355338372577, 2035: 736.5130297392377, 2036: 560.5368657124192, 2037: 426.6069507744426, 2038: 324.6771115005281, 2039: 247.10152176602028, 2040: 188.06118416198737, 2041: 143.12744306729869, 2042: 108.92978819774737, 2043: 82.9030303519558, 2044: 63.09488483591338, 2045: 48.01952926879057, 2046: 36.546151042084745, 2047: 27.81412430169187, 2048: 21.168453821008324, 2049: 16.11064336635992, 2050: 12.261303157647122}</t>
-        </is>
-      </c>
-      <c r="S111" t="inlineStr">
-        <is>
           <t>{2021: 33670.3774418063, 2022: 32842.559767727274, 2023: 32134.673877174966, 2024: 31426.787986622658, 2025: 30718.90209607035, 2026: 30011.01620551804, 2027: 29303.130314965732, 2028: 28595.244424413657, 2029: 27887.35853386135, 2030: 27179.47264330904, 2031: 26471.58675275673, 2032: 25763.700862204423, 2033: 25055.814971652115, 2034: 24347.929081099806, 2035: 23640.043190547498, 2036: 22932.15729999519, 2037: 22224.27140944288, 2038: 21516.385518890573, 2039: 20808.499628338264, 2040: 20100.613737785956, 2041: 19392.727847233647, 2042: 18684.841956681572, 2043: 17976.956066129263, 2044: 17269.070175576955, 2045: 16561.184285024647, 2046: 15853.298394472338, 2047: 15145.41250392003, 2048: 14437.526613367721, 2049: 13729.640722815413, 2050: 13021.754832263105}</t>
         </is>
       </c>
-      <c r="T111" t="n">
+      <c r="S111" t="n">
         <v>675356.8730046328</v>
       </c>
     </row>
@@ -8488,15 +7933,10 @@
       </c>
       <c r="R112" t="inlineStr">
         <is>
-          <t>{2021: 94700.2499214517, 2022: 72183.87821549515, 2023: 55021.10373046796, 2024: 41939.03030093864, 2025: 31967.411471774376, 2026: 24366.6910959279, 2027: 18573.15333425138, 2028: 14157.114046365627, 2029: 10791.05279081471, 2030: 8225.321909025934, 2031: 6269.631130401881, 2032: 4778.9344837884155, 2033: 3642.672802487204, 2034: 2776.5739812907345, 2035: 2116.402842527267, 2036: 1613.1970630133485, 2037: 1229.6358291634474, 2038: 937.2718975437214, 2039: 714.421773577352, 2040: 544.5575311699778, 2041: 415.0810007778045, 2042: 316.3894122197434, 2043: 241.16319459858875, 2044: 183.8231122241312, 2045: 140.116474423097, 2046: 106.80173002848954, 2047: 81.40805414954178, 2048: 62.05209670898487, 2049: 47.29830170007677, 2050: 36.05243758648943}</t>
-        </is>
-      </c>
-      <c r="S112" t="inlineStr">
-        <is>
           <t>{2021: 94700.2499214517, 2022: 93773.6012194599, 2023: 92036.84119936451, 2024: 90300.08117926866, 2025: 88563.32115917327, 2026: 86826.56113907741, 2027: 85089.80111898202, 2028: 83353.04109888617, 2029: 81616.28107879078, 2030: 79879.52105869493, 2031: 78142.76103859907, 2032: 76406.00101850368, 2033: 74669.24099840783, 2034: 72932.48097831244, 2035: 71195.72095821658, 2036: 69458.96093812119, 2037: 67722.20091802534, 2038: 65985.44089792995, 2039: 64248.68087783409, 2040: 62511.92085773824, 2041: 60775.16083764285, 2042: 59038.40081754699, 2043: 57301.640797451604, 2044: 55564.88077735575, 2045: 53828.12075726036, 2046: 52091.360737164505, 2047: 50354.600717069115, 2048: 48617.84069697326, 2049: 46881.080676877405, 2050: 45144.320656782016}</t>
         </is>
       </c>
-      <c r="T112" t="n">
+      <c r="S112" t="n">
         <v>2039087.831837845</v>
       </c>
     </row>
@@ -8560,15 +8000,10 @@
       </c>
       <c r="R113" t="inlineStr">
         <is>
-          <t>{2021: 64984.7393355088, 2022: 49916.43536324418, 2023: 38342.08684763397, 2024: 29451.53461246596, 2025: 22622.47473582169, 2026: 17376.89970682447, 2027: 13347.639767408005, 2028: 10252.662463749075, 2029: 7875.331476373977, 2030: 6049.242924172852, 2031: 4646.577742846189, 2032: 3569.154849780777, 2033: 2741.5588518509626, 2034: 2105.8612625406327, 2035: 1617.5657342081768, 2036: 1242.493487594581, 2037: 954.390930808542, 2038: 733.0920104643677, 2039: 563.106666731832, 2040: 432.53658966625306, 2041: 332.2423839979313, 2042: 255.2038471700217, 2043: 196.02858258681823, 2044: 150.5745529196354, 2045: 115.66015367634806, 2046: 88.84151331716829, 2047: 68.24143179483457, 2048: 52.4179838853458, 2049: 40.263590055746, 2050: 30.927490224025686}</t>
-        </is>
-      </c>
-      <c r="S113" t="inlineStr">
-        <is>
           <t>{2021: 64984.7393355088, 2022: 62381.65052912757, 2023: 60354.77870488493, 2024: 58327.90688064229, 2025: 56301.03505639965, 2026: 54274.16323215701, 2027: 52247.29140791437, 2028: 50220.419583671726, 2029: 48193.547759429086, 2030: 46166.675935186446, 2031: 44139.804110943805, 2032: 42112.932286701165, 2033: 40086.060462458525, 2034: 38059.188638215885, 2035: 36032.316813973244, 2036: 34005.444989730604, 2037: 31978.573165487964, 2038: 29951.701341245323, 2039: 27924.829517002683, 2040: 25897.957692759577, 2041: 23871.085868516937, 2042: 21844.214044274297, 2043: 19817.342220031656, 2044: 17790.470395789016, 2045: 15763.598571546376, 2046: 13736.726747303735, 2047: 11709.854923061095, 2048: 9682.983098818455, 2049: 7656.111274575815, 2050: 5629.239450333174}</t>
         </is>
       </c>
-      <c r="T113" t="n">
+      <c r="S113" t="n">
         <v>1015835.65464477</v>
       </c>
     </row>
@@ -8632,15 +8067,10 @@
       </c>
       <c r="R114" t="inlineStr">
         <is>
-          <t>{2021: 270481.333456314, 2022: 205556.07336256202, 2023: 156215.21365746812, 2024: 118717.93705168617, 2025: 90221.35711257807, 2026: 68564.9825240097, 2027: 52106.917685262226, 2028: 39599.38106464075, 2029: 30094.10363081501, 2030: 22870.43506725196, 2031: 17380.70708408811, 2032: 13208.711502625938, 2033: 10038.145094760186, 2034: 7628.628797246859, 2035: 5797.48317809849, 2036: 4405.8784473121805, 2037: 3348.308963762586, 2038: 2544.5942394648428, 2039: 1933.7999908591403, 2040: 1469.6183566906468, 2041: 1116.8570299571581, 2042: 848.771124616058, 2043: 645.0354903614145, 2044: 490.2037448717402, 2045: 372.537193808728, 2046: 283.11485218701074, 2047: 215.15709266341446, 2048: 163.5116425922958, 2049: 124.26296029690165, 2050: 94.43537510201074}</t>
-        </is>
-      </c>
-      <c r="S114" t="inlineStr">
-        <is>
           <t>{2021: 270481.333456314, 2022: 246851.15575986728, 2023: 237177.1457912475, 2024: 227503.1358226277, 2025: 217829.12585401163, 2026: 208155.11588539183, 2027: 198481.10591677204, 2028: 188807.09594815224, 2029: 179133.08597953618, 2030: 169459.07601091638, 2031: 159785.0660422966, 2032: 150111.05607368052, 2033: 140437.04610506073, 2034: 130763.03613644093, 2035: 121089.02616782486, 2036: 111415.01619920507, 2037: 101741.00623058528, 2038: 92066.99626196921, 2039: 82392.98629334942, 2040: 72718.97632472962, 2041: 63044.96635611355, 2042: 53370.95638749376, 2043: 43696.946418873966, 2044: 34022.9364502579, 2045: 24348.926481638104, 2046: 14674.91651301831, 2047: 5000.906544402242, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T114" t="n">
+      <c r="S114" t="n">
         <v>3409317.47668362</v>
       </c>
     </row>
@@ -8704,15 +8134,10 @@
       </c>
       <c r="R115" t="inlineStr">
         <is>
-          <t>{2021: 77361.1891192005, 2022: 60932.56619343478, 2023: 47992.76827553089, 2024: 37800.8994309676, 2025: 29773.402309002773, 2026: 23450.645312622422, 2027: 18470.605403808117, 2028: 14548.139696588774, 2029: 11458.658988396028, 2030: 9025.268422679246, 2031: 7108.638993786232, 2032: 5599.029965357745, 2033: 4410.0054286589475, 2034: 3473.4852288933525, 2035: 2735.8468896509303, 2036: 2154.8553427985466, 2037: 1697.2446689002759, 2038: 1336.8133855190817, 2039: 1052.9242250387597, 2040: 829.3225035616966, 2041: 653.2054240546347, 2042: 514.489024694182, 2043: 405.23079996444, 2044: 319.1749354370182, 2045: 251.39411767359317, 2046: 198.0074103073024, 2047: 155.95804269179507, 2048: 122.83838792955903, 2049: 96.75210902045173, 2050: 76.20558001195343}</t>
-        </is>
-      </c>
-      <c r="S115" t="inlineStr">
-        <is>
           <t>{2021: 77361.1891192005, 2022: 72287.36137899384, 2023: 67866.15655204095, 2024: 63444.95172508806, 2025: 59023.74689813517, 2026: 54602.54207118228, 2027: 50181.33724422939, 2028: 45760.1324172765, 2029: 41338.92759032361, 2030: 36917.72276337072, 2031: 32496.517936417833, 2032: 28075.313109464943, 2033: 23654.108282512054, 2034: 19232.903455559164, 2035: 14811.698628606275, 2036: 10390.493801653385, 2037: 5969.288974700496, 2038: 1548.084147747606, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T115" t="n">
+      <c r="S115" t="n">
         <v>666281.8815369025</v>
       </c>
     </row>
@@ -8776,15 +8201,10 @@
       </c>
       <c r="R116" t="inlineStr">
         <is>
-          <t>{2021: 200544.976214399, 2022: 150743.3853249106, 2023: 113309.08730877965, 2024: 85170.8964812998, 2025: 64020.29863377262, 2026: 48122.055848705546, 2027: 36171.844063912526, 2028: 27189.243682721833, 2029: 20437.3039630556, 2030: 15362.082084826687, 2031: 11547.196558193647, 2032: 8679.66644217183, 2033: 6524.23375385487, 2034: 4904.062426653394, 2035: 3686.2303209635365, 2036: 2770.824022414369, 2037: 2082.7417428387257, 2038: 1565.5318173483715, 2039: 1176.761295324878, 2040: 884.5346551436708, 2041: 664.8770309310079, 2042: 499.7672659731245, 2043: 375.6594204924027, 2044: 282.3714352917956, 2045: 212.24977498031703, 2046: 159.54151641663645, 2047: 119.92236723398314, 2048: 90.14189212948136, 2049: 67.75684056360475, 2050: 50.930697533696964}</t>
-        </is>
-      </c>
-      <c r="S116" t="inlineStr">
-        <is>
           <t>{2021: 200544.976214399, 2022: 198429.64659976307, 2023: 196488.87809868297, 2024: 194548.10959760332, 2025: 192607.34109652322, 2026: 190666.5725954431, 2027: 188725.804094363, 2028: 186785.03559328336, 2029: 184844.26709220326, 2030: 182903.49859112315, 2031: 180962.7300900435, 2032: 179021.9615889634, 2033: 177081.1930878833, 2034: 175140.42458680365, 2035: 173199.65608572355, 2036: 171258.88758464344, 2037: 169318.1190835638, 2038: 167377.3505824837, 2039: 165436.58208140358, 2040: 163495.81358032394, 2041: 161555.04507924384, 2042: 159614.27657816373, 2043: 157673.50807708362, 2044: 155732.73957600398, 2045: 153791.97107492387, 2046: 151851.20257384377, 2047: 149910.43407276412, 2048: 147969.66557168402, 2049: 146028.8970706039, 2050: 144088.12856952427}</t>
         </is>
       </c>
-      <c r="T116" t="n">
+      <c r="S116" t="n">
         <v>4994736.1637771</v>
       </c>
     </row>
@@ -8848,15 +8268,10 @@
       </c>
       <c r="R117" t="inlineStr">
         <is>
-          <t>{2021: 31187.2362827871, 2022: 24139.662054804845, 2023: 18684.672115105062, 2024: 14462.380262672114, 2025: 11194.226025140602, 2026: 8664.596976845245, 2027: 6706.603976241653, 2028: 5191.070861615183, 2029: 4018.0122138971574, 2030: 3110.0369425516665, 2031: 2407.2425042866457, 2032: 1863.2629069961513, 2033: 1442.2097708915928, 2034: 1116.3046371209052, 2035: 864.0463183710493, 2036: 668.7923846810148, 2037: 517.6611997497574, 2038: 400.68207094518584, 2039: 310.1374452142297, 2040: 240.0537530843693, 2041: 185.8073098206052, 2042: 143.81927355510422, 2043: 111.31953563015392, 2044: 86.16396611240783, 2045: 66.69295747770892, 2046: 51.62193406140083, 2047: 39.95660377079981, 2048: 30.927360896585704, 2049: 23.938512329885924, 2050: 18.5289774476478}</t>
-        </is>
-      </c>
-      <c r="S117" t="inlineStr">
-        <is>
           <t>{2021: 31187.2362827871, 2022: 30404.135164321866, 2023: 29374.42756361491, 2024: 28344.719962908188, 2025: 27315.012362201232, 2026: 26285.304761494277, 2027: 25255.59716078732, 2028: 24225.8895600806, 2029: 23196.181959373644, 2030: 22166.47435866669, 2031: 21136.766757959733, 2032: 20107.059157252777, 2033: 19077.351556546055, 2034: 18047.6439558391, 2035: 17017.936355132144, 2036: 15988.228754425189, 2037: 14958.521153718233, 2038: 13928.81355301151, 2039: 12899.105952304322, 2040: 11869.3983515976, 2041: 10839.690750890877, 2042: 9809.983150183689, 2043: 8780.275549476966, 2044: 7750.567948770244, 2045: 6720.860348063055, 2046: 5691.152747356333, 2047: 4661.445146649145, 2048: 3631.737545942422, 2049: 2602.0299452356994, 2050: 1572.3223445285112}</t>
         </is>
       </c>
-      <c r="T117" t="n">
+      <c r="S117" t="n">
         <v>478466.0908474616</v>
       </c>
     </row>
@@ -8920,15 +8335,10 @@
       </c>
       <c r="R118" t="inlineStr">
         <is>
-          <t>{2021: 25252.8960235231, 2022: 19291.842824867144, 2023: 14737.921513346282, 2024: 11258.972639647296, 2025: 8601.2444010868, 2026: 6570.884184113677, 2027: 5019.799106694344, 2028: 3834.8542396305015, 2029: 2929.6206335429124, 2030: 2238.07125908059, 2031: 1709.7650471778081, 2032: 1306.167757031935, 2033: 997.8413187975357, 2034: 762.2966438569513, 2035: 582.3532883322878, 2036: 444.8863249817341, 2037: 339.86902129900676, 2038: 259.64149750722794, 2039: 198.35202093481573, 2040: 151.53018522330117, 2041: 115.76084239320035, 2042: 88.4350046285215, 2043: 67.55954675141521, 2044: 51.61182923469431, 2045: 39.42863806876335, 2046: 30.12134084394157, 2047: 23.011070599359375, 2048: 17.579209799194718, 2049: 13.429562776305884, 2050: 10.259457530963791}</t>
-        </is>
-      </c>
-      <c r="S118" t="inlineStr">
-        <is>
           <t>{2021: 25252.8960235231, 2022: 24736.205273374682, 2023: 24167.625875891652, 2024: 23599.04647840862, 2025: 23030.46708092559, 2026: 22461.887683442328, 2027: 21893.308285959298, 2028: 21324.728888476267, 2029: 20756.149490993237, 2030: 20187.570093510207, 2031: 19618.990696027176, 2032: 19050.411298543913, 2033: 18481.831901060883, 2034: 17913.252503577853, 2035: 17344.673106094822, 2036: 16776.093708611792, 2037: 16207.514311128762, 2038: 15638.934913645731, 2039: 15070.355516162468, 2040: 14501.776118679438, 2041: 13933.196721196407, 2042: 13364.617323713377, 2043: 12796.037926230347, 2044: 12227.458528747316, 2045: 11658.879131264053, 2046: 11090.299733781023, 2047: 10521.720336297993, 2048: 9953.140938814962, 2049: 9384.561541331932, 2050: 8815.982143848902}</t>
         </is>
       </c>
-      <c r="T118" t="n">
+      <c r="S118" t="n">
         <v>494725.1744895781</v>
       </c>
     </row>
@@ -8992,15 +8402,10 @@
       </c>
       <c r="R119" t="inlineStr">
         <is>
-          <t>{2021: 35064.8140512671, 2022: 26961.435351733697, 2023: 20730.724399761868, 2024: 15939.913010278475, 2025: 12256.244493712124, 2026: 9423.861284110262, 2027: 7246.033770598693, 2028: 5571.495995297205, 2029: 4283.939132545338, 2030: 3293.932995167545, 2031: 2532.7144576414235, 2032: 1947.4113569877306, 2033: 1497.3701365674115, 2034: 1151.3321609421187, 2035: 885.2625763315882, 2036: 680.6809152381871, 2037: 523.377493590049, 2038: 402.42644485007924, 2039: 309.4268391325281, 2040: 237.91917753122922, 2041: 182.93673294737147, 2042: 140.6605747746635, 2043: 108.15431639762971, 2044: 83.16016178788983, 2045: 63.94208515139374, 2046: 49.165251312720315, 2047: 37.80330170528163, 2048: 29.06706630523837, 2049: 22.34975003453417, 2050: 17.18478643013725}</t>
-        </is>
-      </c>
-      <c r="S119" t="inlineStr">
-        <is>
           <t>{2021: 35064.8140512671, 2022: 31325.386217971798, 2023: 29622.860235315282, 2024: 27920.334252658766, 2025: 26217.80827000225, 2026: 24515.282287345733, 2027: 22812.756304689217, 2028: 21110.2303220327, 2029: 19407.704339376185, 2030: 17705.17835671967, 2031: 16002.652374063153, 2032: 14300.126391406637, 2033: 12597.60040875012, 2034: 10895.074426093604, 2035: 9192.548443437088, 2036: 7490.022460780572, 2037: 5787.496478124056, 2038: 4084.97049546754, 2039: 2382.4445128110237, 2040: 679.9185301545076, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T119" t="n">
+      <c r="S119" t="n">
         <v>321582.8021328335</v>
       </c>
     </row>
@@ -9064,15 +8469,10 @@
       </c>
       <c r="R120" t="inlineStr">
         <is>
-          <t>{2021: 61848.1688683312, 2022: 48256.33578319339, 2023: 37651.46140668826, 2024: 29377.127853811584, 2025: 22921.17247767413, 2026: 17883.98615295946, 2027: 13953.778369355927, 2028: 10887.278099848276, 2029: 8494.675870999024, 2030: 6627.87498321905, 2031: 5171.324657972458, 2032: 4034.8677043340253, 2033: 3148.159991537013, 2034: 2456.3163054066413, 2035: 1916.5130769801908, 2036: 1495.3376998521421, 2037: 1166.7203649465143, 2038: 910.320397937887, 2039: 710.2672172348539, 2040: 554.1779806552948, 2041: 432.39111533093865, 2042: 337.368288065248, 2043: 263.2277994541215, 2044: 205.38051991436288, 2045: 160.2458328784754, 2046: 125.03000267807043, 2047: 97.5532485860859, 2048: 76.11482128975307, 2049: 59.38773033128257, 2050: 46.33660638149525}</t>
-        </is>
-      </c>
-      <c r="S120" t="inlineStr">
-        <is>
           <t>{2021: 61848.1688683312, 2022: 54995.39154841006, 2023: 51245.96082262695, 2024: 47496.53009684384, 2025: 43747.09937106073, 2026: 39997.66864527762, 2027: 36248.23791949451, 2028: 32498.80719371047, 2029: 28749.37646792736, 2030: 24999.94574214425, 2031: 21250.51501636114, 2032: 17501.08429057803, 2033: 13751.65356479492, 2034: 10002.22283901181, 2035: 6252.792113228701, 2036: 2503.3613874455914, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T120" t="n">
+      <c r="S120" t="n">
         <v>462164.7314530816</v>
       </c>
     </row>
@@ -9136,15 +8536,10 @@
       </c>
       <c r="R121" t="inlineStr">
         <is>
-          <t>{2021: 18018.7501951159, 2022: 13797.069929816791, 2023: 10564.502897645632, 2024: 8089.306065860101, 2025: 6194.032342188485, 2026: 4742.809376195569, 2027: 3631.5988577775006, 2028: 2780.7380009841286, 2029: 2129.2285114467227, 2030: 1630.3636129520796, 2031: 1248.3796342892754, 2032: 955.8921083170862, 2033: 731.9325769545147, 2034: 560.4453604606674, 2035: 429.13652425311676, 2036: 328.5925255883537, 2037: 251.60535580245144, 2038: 192.65579749608864, 2039: 147.51775132321055, 2040: 112.95526653382126, 2041: 86.49055536219454, 2042: 66.22636019030578, 2043: 50.70993897182485, 2044: 38.82891801900078, 2045: 29.731545828993656, 2046: 22.765630939007504, 2047: 17.43178625935033, 2048: 13.34762796628743, 2049: 10.220362369969653, 2050: 7.825795507435432}</t>
-        </is>
-      </c>
-      <c r="S121" t="inlineStr">
-        <is>
           <t>{2021: 18018.7501951159, 2022: 16499.39944294491, 2023: 15777.670823313296, 2024: 15055.94220368145, 2025: 14334.213584049838, 2026: 13612.484964418225, 2027: 12890.756344786612, 2028: 12169.027725155, 2029: 11447.299105523387, 2030: 10725.570485891774, 2031: 10003.841866260162, 2032: 9282.113246628549, 2033: 8560.384626996936, 2034: 7838.656007365091, 2035: 7116.927387733478, 2036: 6395.198768101865, 2037: 5673.470148470253, 2038: 4951.74152883864, 2039: 4230.012909207027, 2040: 3508.2842895754147, 2041: 2786.555669943802, 2042: 2064.8270503121894, 2043: 1343.0984306805767, 2044: 621.3698110487312, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T121" t="n">
+      <c r="S121" t="n">
         <v>205898.2215184852</v>
       </c>
     </row>
@@ -9208,15 +8603,10 @@
       </c>
       <c r="R122" t="inlineStr">
         <is>
-          <t>{2021: 28583.0430247821, 2022: 20269.70067986171, 2023: 14374.283567182169, 2024: 10193.54115450969, 2025: 7228.762448092719, 2026: 5126.285923497496, 2027: 3635.312068718228, 2028: 2577.9860964040613, 2029: 1828.182061848672, 2030: 1296.457593750115, 2031: 919.3845227278389, 2032: 651.9826832025307, 2033: 462.3543345440964, 2034: 327.87915412365084, 2035: 232.51591188140532, 2036: 164.888949474515, 2037: 116.93120457354594, 2038: 82.92190984656443, 2039: 58.80417599116535, 2040: 41.701054888851154, 2041: 29.572355186207123, 2042: 20.971272635431525, 2043: 14.87180419619482, 2044: 10.546358530301323, 2045: 7.47896333103406, 2046: 5.303716192299214, 2047: 3.7611369655649303, 2048: 2.6672149792401503, 2049: 1.8914588356168762, 2050: 1.3413303969417416}</t>
-        </is>
-      </c>
-      <c r="S122" t="inlineStr">
-        <is>
           <t>{2021: 28583.0430247821, 2022: 28038.377532879123, 2023: 28534.737740429933, 2024: 29031.097947980743, 2025: 29527.458155531553, 2026: 30023.818363082362, 2027: 30520.178570633172, 2028: 31016.53877818398, 2029: 31512.89898573479, 2030: 32009.2591932856, 2031: 32505.61940083641, 2032: 33001.97960838722, 2033: 33498.33981593803, 2034: 33994.70002348884, 2035: 34491.06023103965, 2036: 34987.42043859046, 2037: 35483.78064614127, 2038: 35980.14085369208, 2039: 36476.50106124277, 2040: 36972.86126879358, 2041: 37469.22147634439, 2042: 37965.5816838952, 2043: 38461.94189144601, 2044: 38958.30209899682, 2045: 39454.66230654763, 2046: 39951.02251409844, 2047: 40447.38272164925, 2048: 40943.74292920006, 2049: 41440.10313675087, 2050: 41936.46334430168}</t>
         </is>
       </c>
-      <c r="T122" t="n">
+      <c r="S122" t="n">
         <v>1007958.482559362</v>
       </c>
     </row>
@@ -9280,15 +8670,10 @@
       </c>
       <c r="R123" t="inlineStr">
         <is>
-          <t>{2021: 116793.301802271, 2022: 90287.42338769816, 2023: 69796.97205401685, 2024: 53956.765240605775, 2025: 41711.44434427217, 2026: 32245.16113089698, 2027: 24927.22159836425, 2028: 19270.065796587696, 2029: 14896.783997346362, 2030: 11516.00496885126, 2031: 8902.483278688265, 2032: 6882.0922482833785, 2033: 5320.222709911218, 2034: 4112.8146298991, 2035: 3179.424077191373, 2036: 2457.8636219430628, 2037: 1900.0590790668061, 2038: 1468.846551010075, 2039: 1135.496371762205, 2040: 877.7989841066021, 2041: 678.5852211071157, 2042: 524.5824051319147, 2043: 405.5300516639834, 2044: 313.49626139526816, 2045: 242.34925501956045, 2046: 187.34884156874494, 2047: 144.83060174588846, 2048: 111.96174487355624, 2049: 86.55237335218186, 2050: 66.90958006554635}</t>
-        </is>
-      </c>
-      <c r="S123" t="inlineStr">
-        <is>
           <t>{2021: 116793.301802271, 2022: 115358.56333628204, 2023: 111986.12599193677, 2024: 108613.68864759244, 2025: 105241.25130324718, 2026: 101868.81395890191, 2027: 98496.37661455758, 2028: 95123.93927021232, 2029: 91751.50192586705, 2030: 88379.06458152179, 2031: 85006.62723717745, 2032: 81634.18989283219, 2033: 78261.75254848693, 2034: 74889.31520414166, 2035: 71516.87785979733, 2036: 68144.44051545206, 2037: 64772.0031711068, 2038: 61399.565826761536, 2039: 58027.1284824172, 2040: 54654.69113807194, 2041: 51282.253793726675, 2042: 47909.81644938141, 2043: 44537.37910503708, 2044: 41164.941760691814, 2045: 37792.50441634655, 2046: 34420.067072001286, 2047: 31047.629727656953, 2048: 27675.19238331169, 2049: 24302.755038966425, 2050: 20930.317694622092}</t>
         </is>
       </c>
-      <c r="T123" t="n">
+      <c r="S123" t="n">
         <v>2024120.267001931</v>
       </c>
     </row>
@@ -9352,15 +8737,10 @@
       </c>
       <c r="R124" t="inlineStr">
         <is>
-          <t>{2021: 45044.8635477766, 2022: 33921.56764026027, 2023: 25545.03800310768, 2024: 19236.993216248913, 2025: 14486.64542824273, 2026: 10909.339801937502, 2027: 8215.407459487638, 2028: 6186.709823945383, 2029: 4658.975058078176, 2030: 3508.4963105562597, 2031: 2642.1146728062904, 2032: 1989.6757261094335, 2033: 1498.3488551101748, 2034: 1128.349339618215, 2035: 849.7168252070676, 2036: 639.8893123687016, 2037: 481.8762203324722, 2038: 362.88259115056746, 2039: 273.2730303007985, 2040: 205.79148989485589, 2041: 154.97371718873507, 2042: 116.70479197932275, 2043: 87.88592490396182, 2044: 66.183535956204, 2045: 49.84029509222004, 2046: 37.53282412295652, 2047: 28.26453743980106, 2048: 21.28494445472031, 2049: 16.028879347679077, 2050: 12.070737308664903}</t>
-        </is>
-      </c>
-      <c r="S124" t="inlineStr">
-        <is>
           <t>{2021: 45044.8635477766, 2022: 46440.72932252592, 2023: 46421.9214766393, 2024: 46403.113630752676, 2025: 46384.30578486605, 2026: 46365.497938979424, 2027: 46346.6900930928, 2028: 46327.88224720618, 2029: 46309.07440131955, 2030: 46290.26655543293, 2031: 46271.45870954631, 2032: 46252.650863659685, 2033: 46233.84301777306, 2034: 46215.03517188643, 2035: 46196.22732599981, 2036: 46177.41948011319, 2037: 46158.61163422657, 2038: 46139.80378833994, 2039: 46120.995942453315, 2040: 46102.18809656669, 2041: 46083.38025068007, 2042: 46064.57240479344, 2043: 46045.76455890682, 2044: 46026.9567130202, 2045: 46008.148867133576, 2046: 45989.341021246946, 2047: 45970.533175360324, 2048: 45951.7253294737, 2049: 45932.91748358708, 2050: 45914.10963770046}</t>
         </is>
       </c>
-      <c r="T124" t="n">
+      <c r="S124" t="n">
         <v>1338710.541878321</v>
       </c>
     </row>
@@ -9424,15 +8804,10 @@
       </c>
       <c r="R125" t="inlineStr">
         <is>
-          <t>{2021: 75179.0501123718, 2022: 57200.63033882929, 2023: 43521.59419770266, 2024: 33113.78126935992, 2025: 25194.9068081907, 2026: 19169.762701210362, 2027: 14585.479708988278, 2028: 11097.48835481812, 2029: 8443.619972912526, 2030: 6424.401266978017, 2031: 4888.061254717049, 2032: 3719.1236719099197, 2033: 2829.7274044208757, 2034: 2153.022563839186, 2035: 1638.145834527603, 2036: 1246.397422976833, 2037: 948.3322566646094, 2038: 721.5467975556834, 2039: 548.9951200162436, 2040: 417.7076841345001, 2041: 317.8165033230987, 2042: 241.8134346601995, 2043: 183.9858426820491, 2044: 139.98721929983523, 2045: 106.51048625064739, 2046: 81.03942444239041, 2047: 61.65954682151301, 2048: 46.91419935906705, 2049: 35.695074241680594, 2050: 27.158905886194944}</t>
-        </is>
-      </c>
-      <c r="S125" t="inlineStr">
-        <is>
           <t>{2021: 75179.0501123718, 2022: 71632.5786566753, 2023: 69641.13874990027, 2024: 67649.69884312479, 2025: 65658.25893634977, 2026: 63666.81902957475, 2027: 61675.37912279926, 2028: 59683.93921602424, 2029: 57692.49930924922, 2030: 55701.0594024742, 2031: 53709.61949569872, 2032: 51718.1795889237, 2033: 49726.73968214868, 2034: 47735.299775373656, 2035: 45743.85986859817, 2036: 43752.41996182315, 2037: 41760.98005504813, 2038: 39769.54014827311, 2039: 37778.100241497625, 2040: 35786.660334722605, 2041: 33795.220427947585, 2042: 31803.780521172564, 2043: 29812.34061439708, 2044: 27820.90070762206, 2045: 25829.46080084704, 2046: 23838.02089407202, 2047: 21846.580987296533, 2048: 19855.141080521513, 2049: 17863.701173746493, 2050: 15872.261266971007}</t>
         </is>
       </c>
-      <c r="T125" t="n">
+      <c r="S125" t="n">
         <v>1298473.573315574</v>
       </c>
     </row>
@@ -9496,15 +8871,10 @@
       </c>
       <c r="R126" t="inlineStr">
         <is>
-          <t>{2021: 534930.625645295, 2022: 402562.8391944822, 2023: 302949.2643178372, 2024: 227984.92015399318, 2025: 171570.39128205698, 2026: 129115.55354097641, 2027: 97166.10215562409, 2028: 73122.49492173597, 2029: 55028.44248105735, 2030: 41411.73636282633, 2031: 31164.46388927999, 2032: 23452.86372435389, 2033: 17649.48753257126, 2034: 13282.14813438396, 2035: 9995.500364424372, 2036: 7522.128689151354, 2037: 5660.7891504401305, 2038: 4260.035307818691, 2039: 3205.895916906016, 2040: 2412.6017479646907, 2041: 1815.6070393887694, 2042: 1366.3377821304211, 2043: 1028.239533321908, 2044: 773.8031925293963, 2045: 582.326745242181, 2046: 438.23085960125405, 2047: 329.7912862082006, 2048: 248.18492371309065, 2049: 186.77193405160662, 2050: 140.5554971973414}</t>
-        </is>
-      </c>
-      <c r="S126" t="inlineStr">
-        <is>
           <t>{2021: 534930.625645295, 2022: 515102.9410064779, 2023: 505999.5806408264, 2024: 496896.22027517855, 2025: 487792.8599095307, 2026: 478689.4995438792, 2027: 469586.13917823136, 2028: 460482.77881258354, 2029: 451379.418446932, 2030: 442276.05808128417, 2031: 433172.69771563634, 2032: 424069.3373499848, 2033: 414965.976984337, 2034: 405862.61661868915, 2035: 396759.2562530376, 2036: 387655.8958873898, 2037: 378552.53552174196, 2038: 369449.1751560904, 2039: 360345.8147904426, 2040: 351242.45442479476, 2041: 342139.0940591432, 2042: 333035.7336934954, 2043: 323932.37332784757, 2044: 314829.012962196, 2045: 305725.6525965482, 2046: 296622.2922309004, 2047: 287518.93186524883, 2048: 278415.571499601, 2049: 269312.2111339532, 2050: 260208.85076830164}</t>
         </is>
       </c>
-      <c r="T126" t="n">
+      <c r="S126" t="n">
         <v>11379381.8681728</v>
       </c>
     </row>
@@ -9568,15 +8938,10 @@
       </c>
       <c r="R127" t="inlineStr">
         <is>
-          <t>{2021: 138928.587827763, 2022: 107789.48907901214, 2023: 83629.82837138337, 2024: 64885.25229301638, 2025: 50342.037609262974, 2026: 39058.50191053687, 2027: 30304.0290767791, 2028: 23511.761418543625, 2029: 18241.8952807206, 2030: 14153.203475870796, 2031: 10980.940606599534, 2032: 8519.700632527476, 2033: 6610.116698406089, 2034: 5128.542028780743, 2035: 3979.0437205613516, 2036: 3087.191026472452, 2037: 2395.235916781396, 2038: 1858.37385760839, 2039: 1441.842688833344, 2040: 1118.6717520970703, 2041: 867.9355235018812, 2042: 673.398672617164, 2043: 522.464814497912, 2044: 405.360885740154, 2045: 314.5043324036108, 2046: 244.01213481669419, 2047: 189.3198783073962, 2048: 146.8862044473829, 2049: 113.96350583918306, 2050: 88.42001678796129}</t>
-        </is>
-      </c>
-      <c r="S127" t="inlineStr">
-        <is>
           <t>{2021: 138928.587827763, 2022: 130049.44578203, 2023: 123865.53436541744, 2024: 117681.62294880673, 2025: 111497.71153219417, 2026: 105313.80011558346, 2027: 99129.88869897276, 2028: 92945.9772823602, 2029: 86762.0658657495, 2030: 80578.15444913879, 2031: 74394.24303252622, 2032: 68210.33161591552, 2033: 62026.42019930482, 2034: 55842.50878269225, 2035: 49658.59736608155, 2036: 43474.685949468985, 2037: 37290.77453285828, 2038: 31106.86311624758, 2039: 24922.951699635014, 2040: 18739.04028302431, 2041: 12555.128866413608, 2042: 6371.217449801043, 2043: 187.3060331903398, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T127" t="n">
+      <c r="S127" t="n">
         <v>1502068.563881294</v>
       </c>
     </row>
@@ -9640,15 +9005,10 @@
       </c>
       <c r="R128" t="inlineStr">
         <is>
-          <t>{2021: 61431.3880270318, 2022: 48845.21435295444, 2023: 38837.71866161015, 2024: 30880.576752902434, 2025: 24553.70844257418, 2026: 19523.10033284188, 2027: 15523.172293816295, 2028: 12342.756732041502, 2029: 9813.95045180568, 2030: 7803.250567230985, 2031: 6204.506504695804, 2032: 4933.3160117236885, 2033: 3922.5693216873387, 2034: 3118.9062380917003, 2035: 2479.89909782471, 2036: 1971.8128939825467, 2037: 1567.8243087738113, 2038: 1246.6056341772949, 2039: 991.1988214916585, 2040: 788.12021764593, 2041: 626.6487247508247, 2042: 498.2598028061932, 2043: 396.17543495549836, 2044: 315.0062966713545, 2045: 250.46723796428128, 2046: 199.1510581101367, 2047: 158.34862981977346, 2048: 125.90587669352358, 2049: 100.11005339299278, 2050: 79.59932493654112}</t>
-        </is>
-      </c>
-      <c r="S128" t="inlineStr">
-        <is>
           <t>{2021: 61431.3880270318, 2022: 57085.317437249236, 2023: 52973.74767869618, 2024: 48862.17792014405, 2025: 44750.60816159099, 2026: 40639.038403037935, 2027: 36527.46864448488, 2028: 32415.89888593182, 2029: 28304.32912737876, 2030: 24192.759368826635, 2031: 20081.189610273577, 2032: 15969.61985172052, 2033: 11858.050093167461, 2034: 7746.480334614404, 2035: 3634.910576062277, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T128" t="n">
+      <c r="S128" t="n">
         <v>455757.2901066946</v>
       </c>
     </row>
@@ -9712,15 +9072,10 @@
       </c>
       <c r="R129" t="inlineStr">
         <is>
-          <t>{2021: 25568.9786086761, 2022: 20075.444968359403, 2023: 15762.205320977206, 2024: 12375.671720961394, 2025: 9716.739975539685, 2026: 7629.083728225816, 2027: 5989.963576137297, 2028: 4703.010862327437, 2029: 3692.561881224849, 2030: 2899.2093885845443, 2031: 2276.309876239265, 2032: 1787.2412641413878, 2033: 1403.2497814080375, 2034: 1101.7594482229504, 2035: 865.0447681028858, 2036: 679.1885942336386, 2037: 533.2638997964567, 2038: 418.69134617461344, 2039: 328.7348786002985, 2040: 258.1056938379715, 2041: 202.6512960086014, 2042: 159.11135923931366, 2043: 124.92604359119119, 2044: 98.08549459925736, 2045: 77.01167806341483, 2046: 60.465602812874536, 2047: 47.4744767996578, 2048: 37.27451381533825, 2049: 29.266028271002593, 2050: 22.978177931503378}</t>
-        </is>
-      </c>
-      <c r="S129" t="inlineStr">
-        <is>
           <t>{2021: 25568.9786086761, 2022: 21980.12846724037, 2023: 20109.771087557077, 2024: 18239.41370787332, 2025: 16369.056328190025, 2026: 14498.698948506732, 2027: 12628.341568823438, 2028: 10757.984189140145, 2029: 8887.626809456851, 2030: 7017.269429773092, 2031: 5146.912050089799, 2032: 3276.5546704065055, 2033: 1406.197290723212, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T129" t="n">
+      <c r="S129" t="n">
         <v>153102.4438521186</v>
       </c>
     </row>
@@ -9784,15 +9139,10 @@
       </c>
       <c r="R130" t="inlineStr">
         <is>
-          <t>{2021: 68352.2524712745, 2022: 52786.17529513155, 2023: 40765.010684312874, 2024: 31481.46435692621, 2025: 24312.08974116134, 2026: 18775.41974797751, 2027: 14499.633329171187, 2028: 11197.585433639051, 2029: 8647.523471603032, 2030: 6678.1952801429115, 2031: 5157.348499391316, 2032: 3982.8490225887276, 2033: 3075.8220699276358, 2034: 2375.3552675980627, 2035: 1834.4080115917134, 2036: 1416.6524051766685, 2037: 1094.0336197896622, 2038: 844.8858427489887, 2039: 652.4772862235344, 2040: 503.88654596513294, 2041: 389.13485046234507, 2042: 300.51592577117503, 2043: 232.07847237225363, 2044: 179.22649922936327, 2045: 138.41067505170867, 2046: 106.889969120878, 2047: 82.5475744150068, 2048: 63.74875114890586, 2049: 49.23104405968259, 2050: 38.01950086120247}</t>
-        </is>
-      </c>
-      <c r="S130" t="inlineStr">
-        <is>
           <t>{2021: 68352.2524712745, 2022: 64786.94272489473, 2023: 62183.237042020075, 2024: 59579.53135914635, 2025: 56975.82567627169, 2026: 54372.119993397035, 2027: 51768.41431052331, 2028: 49164.70862764865, 2029: 46561.002944773994, 2030: 43957.29726189934, 2031: 41353.59157902561, 2032: 38749.885896150954, 2033: 36146.1802132763, 2034: 33542.47453040257, 2035: 30938.768847527914, 2036: 28335.063164653257, 2037: 25731.35748177953, 2038: 23127.651798904873, 2039: 20523.946116030216, 2040: 17920.24043315649, 2041: 15316.534750281833, 2042: 12712.829067407176, 2043: 10109.123384532519, 2044: 7505.417701658793, 2045: 4901.712018784136, 2046: 2298.0063359094784, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T130" t="n">
+      <c r="S130" t="n">
         <v>872737.9894956941</v>
       </c>
     </row>
@@ -9856,15 +9206,10 @@
       </c>
       <c r="R131" t="inlineStr">
         <is>
-          <t>{2021: 45248.6761688049, 2022: 36998.286487657824, 2023: 30252.22656053139, 2024: 24736.205342239824, 2025: 20225.94447748001, 2026: 16538.059267624994, 2027: 13522.602350857127, 2028: 11056.966925821585, 2029: 9040.901627264313, 2030: 7392.4343612701, 2031: 6044.539365508266, 2032: 4942.411979008997, 2033: 4041.2403151249227, 2034: 3304.3832351397064, 2035: 2701.8805399437933, 2036: 2209.234804999342, 2037: 1806.4153286814128, 2038: 1477.0436950888743, 2039: 1207.7278367618203, 2040: 987.5175206659145, 2041: 807.4591178065855, 2042: 660.231553653176, 2043: 539.8486373197424, 2044: 441.415666372523, 2045: 360.93041095090086, 2046: 295.1203853268929, 2047: 241.30979045526277, 2048: 197.31071747234049, 2049: 161.3341885383113, 2050: 131.91741799309082}</t>
-        </is>
-      </c>
-      <c r="S131" t="inlineStr">
-        <is>
           <t>{2021: 45248.6761688049, 2022: 40527.30157988705, 2023: 35771.316687176004, 2024: 31015.33179446496, 2025: 26259.346901753917, 2026: 21503.362009042874, 2027: 16747.37711633183, 2028: 11991.392223620787, 2029: 7235.407330909744, 2030: 2479.422438200563, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T131" t="n">
+      <c r="S131" t="n">
         <v>216154.5961657902</v>
       </c>
     </row>
@@ -9928,15 +9273,10 @@
       </c>
       <c r="R132" t="inlineStr">
         <is>
-          <t>{2021: 3410027.6165376, 2022: 2535088.2363595497, 2023: 1884639.3897108515, 2024: 1401081.6579505962, 2025: 1041594.3882753968, 2026: 774343.78184191, 2027: 575663.9045166356, 2028: 427960.9893361222, 2029: 318155.4496583166, 2030: 236523.63806408725, 2031: 175836.78488975076, 2032: 130720.86652069396, 2033: 97180.71764469068, 2034: 72246.24601491635, 2035: 53709.420857862715, 2036: 39928.744370903754, 2037: 29683.89160732463, 2038: 22067.64662495831, 2039: 16405.56548333001, 2040: 12196.251979285864, 2041: 9066.957337946113, 2042: 6740.572063266642, 2043: 5011.086966290167, 2044: 3725.3503631491153, 2045: 2769.505981751031, 2046: 2058.910608469858, 2047: 1530.6386487706807, 2048: 1137.9098555675998, 2049: 845.9467820427873, 2050: 628.8951225328706}</t>
-        </is>
-      </c>
-      <c r="S132" t="inlineStr">
-        <is>
           <t>{2021: 3410027.6165376, 2022: 3553505.1782942116, 2023: 3587213.084647909, 2024: 3620920.991001621, 2025: 3654628.897355318, 2026: 3688336.8037090153, 2027: 3722044.7100627273, 2028: 3755752.6164164245, 2029: 3789460.5227701217, 2030: 3823168.429123834, 2031: 3856876.335477531, 2032: 3890584.241831228, 2033: 3924292.14818494, 2034: 3958000.0545386374, 2035: 3991707.9608923346, 2036: 4025415.8672460467, 2037: 4059123.773599744, 2038: 4092831.679953441, 2039: 4126539.586307153, 2040: 4160247.4926608503, 2041: 4193955.3990145624, 2042: 4227663.30536826, 2043: 4261371.211721957, 2044: 4295079.118075669, 2045: 4328787.024429366, 2046: 4362494.930783063, 2047: 4396202.837136775, 2048: 4429910.743490472, 2049: 4463618.64984417, 2050: 4497326.556197882}</t>
         </is>
       </c>
-      <c r="T132" t="n">
+      <c r="S132" t="n">
         <v>116193410.6803051</v>
       </c>
     </row>
@@ -10000,15 +9340,10 @@
       </c>
       <c r="R133" t="inlineStr">
         <is>
-          <t>{2021: 138840.37075476, 2022: 109354.37941489456, 2023: 86130.4261304469, 2024: 67838.62105116517, 2025: 53431.50745769696, 2026: 42084.08049816765, 2027: 33146.544345177885, 2028: 26107.102472505747, 2029: 20562.65028451062, 2030: 16195.691849310855, 2031: 12756.158902114827, 2032: 10047.091007287054, 2033: 7913.356872026188, 2034: 6232.770952171683, 2035: 4909.096653982743, 2036: 3866.535469227804, 2037: 3045.3864709849795, 2038: 2398.6276167564947, 2039: 1889.2230916117844, 2040: 1488.0024998234335, 2041: 1171.9904596295144, 2042: 923.0909475122435, 2043: 727.0510526582387, 2044: 572.6448023307496, 2045: 451.03032096229975, 2046: 355.2435115090043, 2047: 279.79926537975825, 2048: 220.3773647391952, 2049: 173.57509078330045, 2050: 136.7123714183906}</t>
-        </is>
-      </c>
-      <c r="S133" t="inlineStr">
-        <is>
           <t>{2021: 138840.37075476, 2022: 132437.60999295302, 2023: 125180.30450269766, 2024: 117922.99901244417, 2025: 110665.69352219068, 2026: 103408.38803193532, 2027: 96151.08254168183, 2028: 88893.77705142833, 2029: 81636.47156117484, 2030: 74379.16607091948, 2031: 67121.86058066599, 2032: 59864.5550904125, 2033: 52607.24960015714, 2034: 45349.94410990365, 2035: 38092.638619650155, 2036: 30835.333129396662, 2037: 23578.027639141306, 2038: 16320.722148887813, 2039: 9063.41665863432, 2040: 1806.111168378964, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T133" t="n">
+      <c r="S133" t="n">
         <v>1344735.536410034</v>
       </c>
     </row>
@@ -10072,15 +9407,10 @@
       </c>
       <c r="R134" t="inlineStr">
         <is>
-          <t>{2021: 53014.7113861568, 2022: 41597.52535509708, 2023: 32639.131109554146, 2024: 25610.006136005126, 2025: 20094.665268041797, 2026: 15767.101737119418, 2027: 12371.517209796253, 2028: 9707.2017815398, 2029: 7616.670197323462, 2030: 5976.353041833346, 2031: 4689.292664028139, 2032: 3679.4120988144455, 2033: 2887.0182270246296, 2034: 2265.2733695847883, 2035: 1777.4267550220925, 2036: 1394.6422148808629, 2037: 1094.2937041046303, 2038: 858.6278961484948, 2039: 673.714800038637, 2040: 528.624371310436, 2041: 414.78044704870376, 2042: 325.4538167194903, 2043: 255.36446467267163, 2044: 200.36947323240562, 2045: 157.21813861178236, 2046: 123.35982477672191, 2047: 96.7931976762576, 2048: 75.94792821206254, 2049: 59.591871517635155, 2050: 46.75823599899477}</t>
-        </is>
-      </c>
-      <c r="S134" t="inlineStr">
-        <is>
           <t>{2021: 53014.7113861568, 2022: 52620.389775073156, 2023: 50532.800064861774, 2024: 48445.210354651324, 2025: 46357.620644440874, 2026: 44270.03093422949, 2027: 42182.44122401904, 2028: 40094.85151380859, 2029: 38007.26180359721, 2030: 35919.67209338676, 2031: 33832.08238317631, 2032: 31744.49267296493, 2033: 29656.90296275448, 2034: 27569.31325254403, 2035: 25481.72354233265, 2036: 23394.1338321222, 2037: 21306.54412191175, 2038: 19218.954411700368, 2039: 17131.364701489918, 2040: 15043.774991279468, 2041: 12956.185281068087, 2042: 10868.595570857637, 2043: 8781.005860647187, 2044: 6693.416150435805, 2045: 4605.826440225355, 2046: 2518.2367300149053, 2047: 430.647019803524, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T134" t="n">
+      <c r="S134" t="n">
         <v>716170.8340264752</v>
       </c>
     </row>
@@ -10144,15 +9474,10 @@
       </c>
       <c r="R135" t="inlineStr">
         <is>
-          <t>{2021: 1743973.00699289, 2022: 1242547.7246381845, 2023: 885291.7114042373, 2024: 630753.5708612399, 2025: 449399.9684275151, 2026: 320188.9627781134, 2027: 228128.56939810832, 2028: 162537.2833719205, 2029: 115804.73482837282, 2030: 82508.67942700308, 2031: 58785.870809835316, 2032: 41883.819143270106, 2033: 29841.42757195765, 2034: 21261.45174312456, 2035: 15148.38152883847, 2036: 10792.93482475677, 2037: 7689.7615702170215, 2038: 5478.809421803319, 2039: 3903.5479066997486, 2040: 2781.203923476606, 2041: 1981.5551003449311, 2042: 1411.8204647125146, 2043: 1005.8953315171989, 2044: 716.6813651296171, 2045: 510.6218937802774, 2046: 363.80842462758966, 2047: 259.206609513227, 2048: 184.67979812209984, 2049: 131.5808570563444, 2050: 93.7488676061655}</t>
-        </is>
-      </c>
-      <c r="S135" t="inlineStr">
-        <is>
           <t>{2021: 1743973.00699289, 2022: 1406315.31029962, 2023: 1357047.6970992386, 2024: 1307780.0838988721, 2025: 1258512.4706985056, 2026: 1209244.8574981242, 2027: 1159977.2442977577, 2028: 1110709.6310973763, 2029: 1061442.0178970098, 2030: 1012174.4046966434, 2031: 962906.791496262, 2032: 913639.1782958955, 2033: 864371.5650955141, 2034: 815103.9518951476, 2035: 765836.3386947662, 2036: 716568.7254943997, 2037: 667301.1122940332, 2038: 618033.4990936518, 2039: 568765.8858932853, 2040: 519498.2726929039, 2041: 470230.6594925374, 2042: 420963.0462921709, 2043: 371695.4330917895, 2044: 322427.819891423, 2045: 273160.2066910416, 2046: 223892.5934906751, 2047: 174624.9802902937, 2048: 125357.3670899272, 2049: 76089.7538895607, 2050: 26822.1406891793}</t>
         </is>
       </c>
-      <c r="T135" t="n">
+      <c r="S135" t="n">
         <v>21639068.47248946</v>
       </c>
     </row>
@@ -10216,15 +9541,10 @@
       </c>
       <c r="R136" t="inlineStr">
         <is>
-          <t>{2021: 670375.543352161, 2022: 534800.4936889664, 2023: 426643.79822059674, 2024: 340360.43853385217, 2025: 271526.8066759949, 2026: 216613.9139473763, 2027: 172806.4653726493, 2028: 137858.5240920547, 2029: 109978.36582014602, 2030: 87736.62004674661, 2031: 69992.98852845017, 2032: 55837.784046542154, 2033: 44545.29221824778, 2034: 35536.565296988454, 2035: 28349.740460110952, 2036: 22616.360850826568, 2037: 18042.485392573464, 2038: 14393.618906612446, 2039: 11482.68992441961, 2040: 9160.45983680966, 2041: 7307.871672416022, 2042: 5829.946239805802, 2043: 4650.912698332742, 2044: 3710.3239099908556, 2045: 2959.9574126568414, 2046: 2361.343132644116, 2047: 1883.7910863996517, 2048: 1502.8179548074215, 2049: 1198.8918631141785, 2050: 956.431013379511}</t>
-        </is>
-      </c>
-      <c r="S136" t="inlineStr">
-        <is>
           <t>{2021: 670375.543352161, 2022: 539598.1808344126, 2023: 471780.83422094584, 2024: 403963.4876074791, 2025: 336146.14099398255, 2026: 268328.7943805158, 2027: 200511.44776704907, 2028: 132694.10115358233, 2029: 64876.754540115595, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T136" t="n">
+      <c r="S136" t="n">
         <v>2753087.513174163</v>
       </c>
     </row>
@@ -10288,15 +9608,10 @@
       </c>
       <c r="R137" t="inlineStr">
         <is>
-          <t>{2021: 38990.1000466931, 2022: 30229.628687543584, 2023: 23437.499506089716, 2024: 18171.45651293781, 2025: 14088.611787097612, 2026: 10923.119010643122, 2027: 8468.863414203926, 2028: 6566.041023498748, 2029: 5090.75334122874, 2030: 3946.9399427270473, 2031: 3060.123692367717, 2032: 2372.561312934532, 2033: 1839.4835469144882, 2034: 1426.1800952928531, 2035: 1105.7395254343555, 2036: 857.2969866451068, 2037: 664.6756368974643, 2038: 515.3333199197843, 2039: 399.5459076236827, 2040: 309.77413283441706, 2041: 240.1726848963153, 2042: 186.20960388948262, 2043: 144.3711910688224, 2044: 111.93322135522611, 2045: 86.78356083510718, 2046: 67.2846393593864, 2047: 52.16682341860372, 2048: 40.44574648088891, 2049: 31.358213922087455, 2050: 24.312509124983958}</t>
-        </is>
-      </c>
-      <c r="S137" t="inlineStr">
-        <is>
           <t>{2021: 38990.1000466931, 2022: 33720.49754332006, 2023: 31311.50034698751, 2024: 28902.503150655888, 2025: 26493.505954324268, 2026: 24084.508757992648, 2027: 21675.511561660096, 2028: 19266.514365328476, 2029: 16857.517168996856, 2030: 14448.519972665235, 2031: 12039.522776332684, 2032: 9630.525580001064, 2033: 7221.528383669443, 2034: 4812.531187337823, 2035: 2403.5339910052717, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T137" t="n">
+      <c r="S137" t="n">
         <v>272363.2707636239</v>
       </c>
     </row>
@@ -10360,15 +9675,10 @@
       </c>
       <c r="R138" t="inlineStr">
         <is>
-          <t>{2021: 9691.38713817754, 2022: 7438.206672061892, 2023: 5708.875077165709, 2024: 4381.601114835571, 2025: 3362.909166872116, 2026: 2581.056049657526, 2027: 1980.9783734569264, 2028: 1520.4146057288267, 2029: 1166.928727888915, 2030: 895.6258712863952, 2031: 687.3990520129471, 2032: 527.583527739789, 2033: 404.92400728117104, 2034: 310.78197678967473, 2035: 238.5273171275098, 2036: 183.07136599028755, 2037: 140.50853985681482, 2038: 107.8412763563556, 2039: 82.76892563269922, 2040: 63.525723005665725, 2041: 48.75643186793125, 2042: 37.42089874805844, 2043: 28.72079866109892, 2044: 22.043411658416677, 2045: 16.91847094073213, 2046: 12.985043486365532, 2047: 9.966110704299112, 2048: 7.649058909555149, 2049: 5.870705628084809, 2050: 4.505807182184591}</t>
-        </is>
-      </c>
-      <c r="S138" t="inlineStr">
-        <is>
           <t>{2021: 9691.38713817754, 2022: 9656.753873407608, 2023: 9448.37079324678, 2024: 9239.987713085953, 2025: 9031.604632925068, 2026: 8823.22155276424, 2027: 8614.838472603413, 2028: 8406.455392442585, 2029: 8198.072312281758, 2030: 7989.6892321208725, 2031: 7781.306151960045, 2032: 7572.923071799218, 2033: 7364.53999163839, 2034: 7156.156911477505, 2035: 6947.773831316677, 2036: 6739.39075115585, 2037: 6531.007670995023, 2038: 6322.624590834137, 2039: 6114.24151067331, 2040: 5905.858430512482, 2041: 5697.475350351655, 2042: 5489.092270190769, 2043: 5280.709190029942, 2044: 5072.326109869115, 2045: 4863.943029708287, 2046: 4655.559949547402, 2047: 4447.176869386574, 2048: 4238.793789225747, 2049: 4030.4107090649195, 2050: 3822.027628904092}</t>
         </is>
       </c>
-      <c r="T138" t="n">
+      <c r="S138" t="n">
         <v>198377.0115381561</v>
       </c>
     </row>
@@ -10432,15 +9742,10 @@
       </c>
       <c r="R139" t="inlineStr">
         <is>
-          <t>{2021: 84355.9376558259, 2022: 64639.76579531418, 2023: 49531.774978551286, 2024: 37954.91370273018, 2025: 29083.86535321026, 2026: 22286.21122705435, 2027: 17077.34528491966, 2028: 13085.926495497646, 2029: 10027.40586364931, 2030: 7683.74087909966, 2031: 5887.851224928934, 2032: 4511.707590399541, 2033: 3457.2044373479425, 2034: 2649.1660379434848, 2035: 2029.987182932354, 2036: 1555.5264954508464, 2037: 1191.9595839784297, 2038: 913.3676951135712, 2039: 699.8899607758639, 2040: 536.3075131904362, 2041: 410.9585289459818, 2042: 314.90685541352065, 2043: 241.3049507471513, 2044: 184.90572133979995, 2045: 141.6884555344972, 2046: 108.57218633520996, 2047: 83.19604869104896, 2048: 63.75097298338846, 2049: 48.850716112987634, 2050: 37.43303596909067}</t>
-        </is>
-      </c>
-      <c r="S139" t="inlineStr">
-        <is>
           <t>{2021: 84355.9376558259, 2022: 81691.34000113048, 2023: 79381.36288961861, 2024: 77071.38577810768, 2025: 74761.40866659582, 2026: 72451.43155508395, 2027: 70141.45444357302, 2028: 67831.47733206116, 2029: 65521.50022054929, 2030: 63211.52310903743, 2031: 60901.5459975265, 2032: 58591.56888601463, 2033: 56281.59177450277, 2034: 53971.61466299184, 2035: 51661.63755147997, 2036: 49351.66043996811, 2037: 47041.68332845718, 2038: 44731.70621694531, 2039: 42421.72910543345, 2040: 40111.75199392252, 2041: 37801.77488241065, 2042: 35491.79777089879, 2043: 33181.820659386925, 2044: 30871.843547875993, 2045: 28561.86643636413, 2046: 26251.889324852265, 2047: 23941.912213341333, 2048: 21631.93510182947, 2049: 19321.957990317605, 2050: 17011.980878806673}</t>
         </is>
       </c>
-      <c r="T139" t="n">
+      <c r="S139" t="n">
         <v>1464870.131147593</v>
       </c>
     </row>
@@ -10504,15 +9809,10 @@
       </c>
       <c r="R140" t="inlineStr">
         <is>
-          <t>{2021: 67266.4918853514, 2022: 51690.04126084496, 2023: 39720.524895244394, 2024: 30522.70920025067, 2025: 23454.770030861517, 2026: 18023.506157051143, 2027: 13849.923651599693, 2028: 10642.789670537919, 2029: 8178.310207379796, 2030: 6284.513733583162, 2031: 4829.251014709186, 2032: 3710.973728714041, 2033: 2851.648417789916, 2034: 2191.311308878941, 2035: 1683.8840379005283, 2036: 1293.9582986713065, 2037: 994.3250491214935, 2038: 764.0758626654999, 2039: 587.1439369085965, 2040: 451.18295118746215, 2041: 346.70553955480557, 2042: 266.4212617999501, 2043: 204.7278760824566, 2044: 157.32041415187678, 2045: 120.89078039841428, 2046: 92.8969127377756, 2047: 71.38539736255271, 2048: 54.855159406576874, 2049: 42.15271784841905, 2050: 32.39169553475747}</t>
-        </is>
-      </c>
-      <c r="S140" t="inlineStr">
-        <is>
           <t>{2021: 67266.4918853514, 2022: 64312.02968478203, 2023: 62129.723555357195, 2024: 59947.41742593236, 2025: 57765.11129650753, 2026: 55582.8051670827, 2027: 53400.499037657864, 2028: 51218.19290823396, 2029: 49035.88677880913, 2030: 46853.5806493843, 2031: 44671.274519959465, 2032: 42488.96839053463, 2033: 40306.6622611098, 2034: 38124.3561316859, 2035: 35942.050002261065, 2036: 33759.74387283623, 2037: 31577.4377434114, 2038: 29395.131613986567, 2039: 27212.825484561734, 2040: 25030.519355137832, 2041: 22848.213225713, 2042: 20665.907096288167, 2043: 18483.600966863334, 2044: 16301.294837438501, 2045: 14118.988708013669, 2046: 11936.682578589767, 2047: 9754.376449164934, 2048: 7572.070319740102, 2049: 5389.764190315269, 2050: 3207.458060890436}</t>
         </is>
       </c>
-      <c r="T140" t="n">
+      <c r="S140" t="n">
         <v>1011062.089224479</v>
       </c>
     </row>
@@ -10576,15 +9876,10 @@
       </c>
       <c r="R141" t="inlineStr">
         <is>
-          <t>{2021: 53982.9166032395, 2022: 41444.64702550412, 2023: 31818.561781183034, 2024: 24428.26628973195, 2025: 18754.467848856588, 2026: 14398.486577888661, 2027: 11054.241442861276, 2028: 8486.742909822553, 2029: 6515.580973123787, 2030: 5002.248314627025, 2031: 3840.407832302987, 2032: 2948.420668219829, 2033: 2263.60970406958, 2034: 1737.8554381969016, 2035: 1334.2147803311018, 2036: 1024.3251774157518, 2037: 786.4116666639153, 2038: 603.7568177572033, 2039: 463.52605186373574, 2040: 355.86579635575333, 2041: 273.21110540976326, 2042: 209.75409517750919, 2043: 161.03584214759135, 2044: 123.63306868568145, 2045: 94.91760013667889, 2046: 72.87169129977187, 2047: 55.94624585158681, 2048: 42.95196624448311, 2049: 32.975785527437495, 2050: 25.31670901774434}</t>
-        </is>
-      </c>
-      <c r="S141" t="inlineStr">
-        <is>
           <t>{2021: 53982.9166032395, 2022: 52366.64851130545, 2023: 50838.737074654084, 2024: 49310.825638002716, 2025: 47782.914201351814, 2026: 46255.002764700446, 2027: 44727.09132804908, 2028: 43199.17989139771, 2029: 41671.26845474634, 2030: 40143.357018094976, 2031: 38615.44558144361, 2032: 37087.534144792706, 2033: 35559.62270814134, 2034: 34031.71127148997, 2035: 32503.799834838603, 2036: 30975.888398187235, 2037: 29447.976961535867, 2038: 27920.065524884965, 2039: 26392.154088233598, 2040: 24864.24265158223, 2041: 23336.331214930862, 2042: 21808.419778279494, 2043: 20280.508341628127, 2044: 18752.59690497676, 2045: 17224.685468325857, 2046: 15696.77403167449, 2047: 14168.862595023122, 2048: 12640.951158371754, 2049: 11113.039721720386, 2050: 9585.128285069019}</t>
         </is>
       </c>
-      <c r="T141" t="n">
+      <c r="S141" t="n">
         <v>920499.6577065178</v>
       </c>
     </row>
@@ -10648,15 +9943,10 @@
       </c>
       <c r="R142" t="inlineStr">
         <is>
-          <t>{2021: 27478.4286960322, 2022: 21119.468288956636, 2023: 16232.075921890337, 2024: 12475.70654379523, 2025: 9588.622830244214, 2026: 7369.657779134571, 2027: 5664.197741749677, 2028: 4353.409211005413, 2029: 3345.9587081104337, 2030: 2571.6488236570967, 2031: 1976.5269834880025, 2032: 1519.126126599428, 2033: 1167.5753520169387, 2034: 897.3792095124326, 2035: 689.7108989788568, 2036: 530.1004515456544, 2037: 407.42648716287886, 2038: 313.14129606544407, 2039: 240.67524913358244, 2040: 184.9790374930496, 2041: 142.17184540178212, 2042: 109.27094171796462, 2043: 83.98384835047766, 2044: 64.54860434863849, 2045: 49.6109955091546, 2046: 38.13019507154181, 2047: 29.306240708786945, 2048: 22.524294535339553, 2049: 17.311802266150416, 2050: 13.305566451019278}</t>
-        </is>
-      </c>
-      <c r="S142" t="inlineStr">
-        <is>
           <t>{2021: 27478.4286960322, 2022: 25976.78196628089, 2023: 25007.89887116989, 2024: 24039.01577605889, 2025: 23070.132680947892, 2026: 22101.249585836893, 2027: 21132.366490725894, 2028: 20163.483395614894, 2029: 19194.600300503895, 2030: 18225.717205393128, 2031: 17256.83411028213, 2032: 16287.95101517113, 2033: 15319.06792006013, 2034: 14350.18482494913, 2035: 13381.301729838131, 2036: 12412.418634727132, 2037: 11443.535539616132, 2038: 10474.652444505133, 2039: 9505.769349394133, 2040: 8536.886254283134, 2041: 7568.0031591721345, 2042: 6599.120064061368, 2043: 5630.2369689503685, 2044: 4661.353873839369, 2045: 3692.4707787283696, 2046: 2723.58768361737, 2047: 1754.7045885063708, 2048: 785.8214933953714, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T142" t="n">
+      <c r="S142" t="n">
         <v>375034.3610536454</v>
       </c>
     </row>
@@ -10720,15 +10010,10 @@
       </c>
       <c r="R143" t="inlineStr">
         <is>
-          <t>{2021: 96057.566686439, 2022: 73822.91584743923, 2023: 56734.96729318542, 2024: 43602.40281501257, 2025: 33509.66118334169, 2026: 25753.108088706897, 2027: 19791.980963338465, 2028: 15210.688710032951, 2029: 11689.837993583931, 2030: 8983.96613863399, 2031: 6904.428241385504, 2032: 5306.245438241388, 2033: 4077.9974338914208, 2034: 3134.054627585528, 2035: 2408.6082857873084, 2036: 1851.0825635584617, 2037: 1422.6085151866585, 2038: 1093.3142731305682, 2039: 840.2424750523755, 2040: 645.7497484786136, 2041: 496.27667017690277, 2042: 381.40244567208094, 2043: 293.1184041208127, 2044: 225.26965888467922, 2045: 173.1260081270909, 2046: 133.0521599687122, 2047: 102.25429133295893, 2048: 78.58527135872426, 2049: 60.3949701672205, 2050: 46.41521697939032}</t>
-        </is>
-      </c>
-      <c r="S143" t="inlineStr">
-        <is>
           <t>{2021: 96057.566686439, 2022: 92344.25144417211, 2023: 89346.23527793027, 2024: 86348.21911168844, 2025: 83350.2029454466, 2026: 80352.18677920476, 2027: 77354.17061296292, 2028: 74356.15444672108, 2029: 71358.1382804783, 2030: 68360.12211423647, 2031: 65362.10594799463, 2032: 62364.08978175279, 2033: 59366.07361551095, 2034: 56368.05744926911, 2035: 53370.04128302727, 2036: 50372.02511678543, 2037: 47374.00895054359, 2038: 44375.99278430175, 2039: 41377.97661805991, 2040: 38379.96045181807, 2041: 35381.94428557623, 2042: 32383.928119334392, 2043: 29385.911953092553, 2044: 26387.895786850713, 2045: 23389.879620608874, 2046: 20391.863454367034, 2047: 17393.847288125195, 2048: 14395.831121883355, 2049: 11397.814955641516, 2050: 8399.798789399676}</t>
         </is>
       </c>
-      <c r="T143" t="n">
+      <c r="S143" t="n">
         <v>1504617.612335304</v>
       </c>
     </row>
@@ -10792,15 +10077,10 @@
       </c>
       <c r="R144" t="inlineStr">
         <is>
-          <t>{2021: 58397.5072941933, 2022: 45422.03238093691, 2023: 35329.60773858287, 2024: 27479.64187278377, 2025: 21373.87776971511, 2026: 16624.767274248403, 2027: 12930.87243693939, 2028: 10057.732491654275, 2029: 7822.982042936402, 2030: 6084.7758771559365, 2031: 4732.785691186557, 2032: 3681.197278406543, 2033: 2863.263685863265, 2034: 2227.068617830781, 2035: 1732.2311783629273, 2036: 1347.3427945903604, 2037: 1047.97363585741, 2038: 815.1219911233547, 2039: 634.00818272427, 2040: 493.13646317818484, 2041: 383.5653512718935, 2042: 298.34009383153517, 2043: 232.05123010267917, 2044: 180.4912397144081, 2045: 140.38748081287503, 2046: 109.1944672781372, 2047: 84.93230033844067, 2048: 66.06099943145526, 2049: 51.382755777162764, 2050: 39.965904451612275}</t>
-        </is>
-      </c>
-      <c r="S144" t="inlineStr">
-        <is>
           <t>{2021: 58397.5072941933, 2022: 54873.87793009728, 2023: 52213.979584635235, 2024: 49554.08123917319, 2025: 46894.18289371114, 2026: 44234.284548249096, 2027: 41574.38620278705, 2028: 38914.487857325, 2029: 36254.589511862956, 2030: 33594.69116640091, 2031: 30934.792820938863, 2032: 28274.894475476816, 2033: 25614.99613001477, 2034: 22955.097784552723, 2035: 20295.199439090677, 2036: 17635.30109362863, 2037: 14975.402748166583, 2038: 12315.504402704537, 2039: 9655.60605724249, 2040: 6995.707711780444, 2041: 4335.809366318397, 2042: 1675.9110208563507, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T144" t="n">
+      <c r="S144" t="n">
         <v>622971.5376321098</v>
       </c>
     </row>
@@ -10864,15 +10144,10 @@
       </c>
       <c r="R145" t="inlineStr">
         <is>
-          <t>{2021: 74871.3006511838, 2022: 57826.522411886945, 2023: 44662.06230116548, 2024: 34494.548968124574, 2025: 26641.714403844122, 2026: 20576.611888211195, 2027: 15892.256420892438, 2028: 12274.314912461194, 2029: 9480.013572660871, 2030: 7321.847123752334, 2031: 5654.996682515623, 2032: 4367.612016306887, 2033: 3373.3060859201682, 2034: 2605.358238511287, 2035: 2012.2370689427194, 2036: 1554.1425212760219, 2037: 1200.3351959455163, 2038: 927.0736518054949, 2039: 716.0212903654519, 2040: 553.015919779555, 2041: 427.11943296202224, 2042: 329.8838306255643, 2043: 254.78433737729785, 2044: 196.78157140860526, 2045: 151.98338816525052, 2046: 117.38370678129009, 2047: 90.66079381474337, 2048: 70.02146857087926, 2049: 54.08077576335207, 2050: 41.76905121899021}</t>
-        </is>
-      </c>
-      <c r="S145" t="inlineStr">
-        <is>
           <t>{2021: 74871.3006511838, 2022: 68251.4099735422, 2023: 64715.11517315172, 2024: 61178.82037276216, 2025: 57642.5255723726, 2026: 54106.23077198211, 2027: 50569.93597159255, 2028: 47033.641171202995, 2029: 43497.346370812505, 2030: 39961.05157042295, 2031: 36424.75677003339, 2032: 32888.4619696429, 2033: 29352.167169253342, 2034: 25815.872368863784, 2035: 22279.577568473294, 2036: 18743.282768083736, 2037: 15206.987967694178, 2038: 11670.693167303689, 2039: 8134.398366914131, 2040: 4598.103566524573, 2041: 1061.8087661340833, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T145" t="n">
+      <c r="S145" t="n">
         <v>730567.8377223548</v>
       </c>
     </row>
@@ -10936,15 +10211,10 @@
       </c>
       <c r="R146" t="inlineStr">
         <is>
-          <t>{2021: 15721.0330251436, 2022: 12026.94814183942, 2023: 9200.889113021469, 2024: 7038.889622847371, 2025: 5384.9107965564945, 2026: 4119.579342848216, 2027: 3151.5719764335167, 2028: 2411.0243051597467, 2029: 1844.4884786192877, 2030: 1411.0756745498177, 2031: 1079.5050131170829, 2032: 825.845909161955, 2033: 631.7909202757584, 2034: 483.3344362605678, 2035: 369.7618464876891, 2036: 282.8762299160429, 2037: 216.40675535240268, 2038: 165.55609418314955, 2039: 126.65418081125337, 2040: 96.89333150867691, 2041: 74.12560430864362, 2042: 56.707774710270506, 2043: 43.38273856360061, 2044: 33.18878257687751, 2045: 25.39017418922085, 2046: 19.42406124315356, 2047: 14.859849025295652, 2048: 11.368122777743563, 2049: 8.696872711819553, 2050: 6.653305602370029}</t>
-        </is>
-      </c>
-      <c r="S146" t="inlineStr">
-        <is>
           <t>{2021: 15721.0330251436, 2022: 15364.241592120961, 2023: 14986.400364014204, 2024: 14608.559135907446, 2025: 14230.717907800688, 2026: 13852.87667969393, 2027: 13475.035451587173, 2028: 13097.194223480416, 2029: 12719.352995373658, 2030: 12341.5117672669, 2031: 11963.670539160143, 2032: 11585.829311053385, 2033: 11207.988082946744, 2034: 10830.146854839986, 2035: 10452.305626733229, 2036: 10074.464398626471, 2037: 9696.623170519713, 2038: 9318.781942412956, 2039: 8940.940714306198, 2040: 8563.09948619944, 2041: 8185.258258092683, 2042: 7807.417029985925, 2043: 7429.575801879168, 2044: 7051.73457377241, 2045: 6673.893345665652, 2046: 6296.052117558895, 2047: 5918.210889452137, 2048: 5540.369661345379, 2049: 5162.528433238622, 2050: 4784.687205131864}</t>
         </is>
       </c>
-      <c r="T146" t="n">
+      <c r="S146" t="n">
         <v>297627.6404701723</v>
       </c>
     </row>
@@ -11008,15 +10278,10 @@
       </c>
       <c r="R147" t="inlineStr">
         <is>
-          <t>{2021: 77022.5277997303, 2022: 59690.7706122443, 2023: 46259.03872627825, 2024: 35849.74095543602, 2025: 27782.763368184394, 2026: 21531.032576554386, 2027: 16686.078258994337, 2028: 12931.344870494828, 2029: 10021.508802976881, 2030: 7766.449637987272, 2031: 6018.828218908044, 2032: 4664.459929223471, 2033: 3614.854194207041, 2034: 2801.432758272538, 2035: 2171.0489766639207, 2036: 1682.5153647378422, 2037: 1303.9125247781697, 2038: 1010.5036232690168, 2039: 783.1181564986733, 2040: 606.8994043325806, 2041: 470.33373434480586, 2042: 364.49833379883347, 2043: 282.4782184233586, 2044: 218.91442699343844, 2045: 169.6538820350426, 2046: 131.47803954657982, 2047: 101.89259848142716, 2048: 78.9645302067284, 2049: 61.1957799064855, 2050: 47.42538793758215}</t>
-        </is>
-      </c>
-      <c r="S147" t="inlineStr">
-        <is>
           <t>{2021: 77022.5277997303, 2022: 86960.87805970327, 2023: 87314.48518824019, 2024: 87668.09231677698, 2025: 88021.69944531389, 2026: 88375.30657385068, 2027: 88728.9137023876, 2028: 89082.52083092439, 2029: 89436.1279594613, 2030: 89789.7350879981, 2031: 90143.342216535, 2032: 90496.9493450718, 2033: 90850.55647360871, 2034: 91204.1636021455, 2035: 91557.77073068242, 2036: 91911.37785921921, 2037: 92264.98498775612, 2038: 92618.59211629292, 2039: 92972.19924482983, 2040: 93325.80637336662, 2041: 93679.41350190353, 2042: 94033.02063044033, 2043: 94386.62775897724, 2044: 94740.23488751403, 2045: 95093.84201605094, 2046: 95447.44914458774, 2047: 95801.05627312465, 2048: 96154.66340166144, 2049: 96508.27053019824, 2050: 96861.87765873515}</t>
         </is>
       </c>
-      <c r="T147" t="n">
+      <c r="S147" t="n">
         <v>2655510.282987855</v>
       </c>
     </row>
@@ -11080,15 +10345,10 @@
       </c>
       <c r="R148" t="inlineStr">
         <is>
-          <t>{2021: 6579.59905935159, 2022: 5127.918890913112, 2023: 3996.5280429070617, 2024: 3114.759951848308, 2025: 2427.5394676277724, 2026: 1891.9428649368745, 2027: 1474.5168315155915, 2028: 1149.1889774881347, 2029: 895.6393564004295, 2030: 698.0312833201168, 2031: 544.0221770197497, 2032: 423.99264354113575, 2033: 330.44564977444753, 2034: 257.53825949167145, 2035: 200.71668411211235, 2036: 156.43185350588413, 2037: 121.9177414151476, 2038: 95.01859972023982, 2039: 74.05431061958156, 2040: 57.71544663347963, 2041: 44.98148388976064, 2042: 35.05706030092642, 2043: 27.322297324712164, 2044: 21.294082409991653, 2045: 16.595893833326944, 2046: 12.93428318835773, 2047: 10.08054662658059, 2048: 7.856440036981107, 2049: 6.123045936013576, 2050: 4.7720966949477095}</t>
-        </is>
-      </c>
-      <c r="S148" t="inlineStr">
-        <is>
           <t>{2021: 6579.59905935159, 2022: 5916.860855815234, 2023: 5540.402715367847, 2024: 5163.944574920577, 2025: 4787.486434473307, 2026: 4411.02829402592, 2027: 4034.57015357865, 2028: 3658.11201313138, 2029: 3281.6538726839935, 2030: 2905.1957322367234, 2031: 2528.7375917894533, 2032: 2152.2794513420667, 2033: 1775.8213108947966, 2034: 1399.3631704475265, 2035: 1022.90503000014, 2036: 646.4468895528698, 2037: 269.9887491055997, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T148" t="n">
+      <c r="S148" t="n">
         <v>52784.59636904188</v>
       </c>
     </row>
@@ -11152,15 +10412,10 @@
       </c>
       <c r="R149" t="inlineStr">
         <is>
-          <t>{2021: 135435.135194512, 2022: 104874.71258178135, 2023: 81210.13297852808, 2024: 62885.37566429432, 2025: 48695.53006993605, 2026: 37707.569108765325, 2027: 29198.999703879384, 2028: 22610.356590421557, 2029: 17508.415710490855, 2030: 13557.708365432181, 2031: 10498.463091207728, 2032: 8129.524865608616, 2033: 6295.128531327343, 2034: 4874.656745756168, 2035: 3774.70901041885, 2036: 2922.9602937154114, 2037: 2263.405432062393, 2038: 1752.6766138097726, 2039: 1357.1918088915384, 2040: 1050.94664446878, 2041: 813.8045354269125, 2042: 630.1726404161769, 2043: 487.9765833705669, 2044: 377.8665252124445, 2045: 292.6023824542787, 2046: 226.577768882239, 2047: 175.4513579863801, 2048: 135.86142705493782, 2049: 105.20481330692849, 2050: 81.46574773184248}</t>
-        </is>
-      </c>
-      <c r="S149" t="inlineStr">
-        <is>
           <t>{2021: 135435.135194512, 2022: 124869.41999418102, 2023: 118563.19712628424, 2024: 112256.97425838746, 2025: 105950.75139049068, 2026: 99644.52852259576, 2027: 93338.30565469898, 2028: 87032.0827868022, 2029: 80725.85991890728, 2030: 74419.6370510105, 2031: 68113.41418311372, 2032: 61807.19131521694, 2033: 55500.968447322026, 2034: 49194.745579425246, 2035: 42888.522711528465, 2036: 36582.29984363355, 2037: 30276.076975736767, 2038: 23969.854107839987, 2039: 17663.631239943206, 2040: 11357.408372048289, 2041: 5051.185504151508, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T149" t="n">
+      <c r="S149" t="n">
         <v>1366923.622580574</v>
       </c>
     </row>
@@ -11224,15 +10479,10 @@
       </c>
       <c r="R150" t="inlineStr">
         <is>
-          <t>{2021: 49623.5862728977, 2022: 39075.26726087766, 2023: 30769.168981705243, 2024: 24228.670107462425, 2025: 19078.46310458626, 2026: 15023.018300990074, 2027: 11829.625774081818, 2028: 9315.041967671592, 2029: 7334.974792659309, 2030: 5775.803844541982, 2031: 4548.060626467571, 2032: 3581.2946593695983, 2033: 2820.030885821934, 2034: 2220.586394974131, 2035: 1748.5638055722936, 2036: 1376.8774721296438, 2037: 1084.1992538199877, 2038: 853.7346610556908, 2039: 672.2591524757593, 2040: 529.3592830453744, 2041: 416.83515875437206, 2042: 328.22990951287306, 2043: 258.45918041264275, 2044: 203.51938078621393, 2045: 160.257949783307, 2046: 126.19245582182235, 2047: 99.3681494607598, 2048: 78.2457957803559, 2049: 61.613349856322756, 2050: 48.51640708178067}</t>
-        </is>
-      </c>
-      <c r="S150" t="inlineStr">
-        <is>
           <t>{2021: 49623.5862728977, 2022: 45371.93333962001, 2023: 42297.75673761405, 2024: 39223.58013560809, 2025: 36149.40353360213, 2026: 33075.226931596175, 2027: 30001.050329591148, 2028: 26926.87372758519, 2029: 23852.69712557923, 2030: 20778.520523573272, 2031: 17704.343921567313, 2032: 14630.167319561355, 2033: 11555.990717555396, 2034: 8481.814115549438, 2035: 5407.6375135444105, 2036: 2333.460911538452, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T150" t="n">
+      <c r="S150" t="n">
         <v>382602.2500201345</v>
       </c>
     </row>
@@ -11296,15 +10546,10 @@
       </c>
       <c r="R151" t="inlineStr">
         <is>
-          <t>{2021: 41166.6984468059, 2022: 30906.585969776803, 2023: 23203.63527673954, 2024: 17420.516474464548, 2025: 13078.743507975594, 2026: 9819.084985117894, 2027: 7371.841942322122, 2028: 5534.533381159766, 2029: 4155.14331246269, 2030: 3119.5431950733805, 2031: 2342.0491218053558, 2032: 1758.332469193525, 2033: 1320.0974494663687, 2034: 991.085193852388, 2035: 744.0737514268257, 2036: 558.6257881730086, 2037: 419.39763445963223, 2038: 314.86977421074613, 2039: 236.39373846079465, 2040: 177.47654478282226, 2041: 133.24347824582057, 2042: 100.0347652517677, 2043: 75.10276968689202, 2044: 56.38465787815377, 2045: 42.331723014888105, 2046: 31.781247609618106, 2047: 23.86030210177415, 2048: 17.913520053744953, 2049: 13.448874173812852, 2050: 10.09696676032344}</t>
-        </is>
-      </c>
-      <c r="S151" t="inlineStr">
-        <is>
           <t>{2021: 41166.6984468059, 2022: 40643.47096043837, 2023: 40252.51989679551, 2024: 39861.56883315253, 2025: 39470.61776950967, 2026: 39079.66670586669, 2027: 38688.71564222383, 2028: 38297.764578580856, 2029: 37906.813514937996, 2030: 37515.86245129502, 2031: 37124.91138765216, 2032: 36733.96032400918, 2033: 36343.00926036632, 2034: 35952.058196723345, 2035: 35561.107133080484, 2036: 35170.15606943751, 2037: 34779.20500579465, 2038: 34388.25394215167, 2039: 33997.30287850881, 2040: 33606.35181486583, 2041: 33215.40075122297, 2042: 32824.449687579996, 2043: 32433.498623937136, 2044: 32042.54756029416, 2045: 31651.5964966513, 2046: 31260.64543300832, 2047: 30869.69436936546, 2048: 30478.743305722484, 2049: 30087.792242079508, 2050: 29696.841178436647}</t>
         </is>
       </c>
-      <c r="T151" t="n">
+      <c r="S151" t="n">
         <v>1025669.454647873</v>
       </c>
     </row>
@@ -11368,15 +10613,10 @@
       </c>
       <c r="R152" t="inlineStr">
         <is>
-          <t>{2021: 89603.7420854587, 2022: 68581.07140205991, 2023: 52490.70234330897, 2024: 40175.42706996998, 2025: 30749.53978893031, 2026: 23535.13742577659, 2027: 18013.365320335368, 2028: 13787.101570457646, 2029: 10552.39630873021, 2030: 8076.611845313819, 2031: 6181.691531609366, 2032: 4731.35405338848, 2033: 3621.2921761056587, 2034: 2771.671043162011, 2035: 2121.3865100949106, 2036: 1623.6705781933645, 2037: 1242.7278734665017, 2038: 951.1612689373084, 2039: 728.0015028574301, 2040: 557.1990843937612, 2041: 426.470025721977, 2042: 326.41238640438075, 2043: 249.83009255534708, 2044: 191.21540035214696, 2045: 146.35278303686178, 2046: 112.01575324575703, 2047: 85.73481634479066, 2048: 65.61986614104565, 2049: 50.224249796627525, 2050: 38.44072559081642}</t>
-        </is>
-      </c>
-      <c r="S152" t="inlineStr">
-        <is>
           <t>{2021: 89603.7420854587, 2022: 88055.60655205604, 2023: 85994.56744903699, 2024: 83933.5283460184, 2025: 81872.48924299935, 2026: 79811.45013998076, 2027: 77750.41103696171, 2028: 75689.37193394313, 2029: 73628.33283092408, 2030: 71567.29372790502, 2031: 69506.25462488644, 2032: 67445.21552186739, 2033: 65384.1764188488, 2034: 63323.13731582975, 2035: 61262.098212811165, 2036: 59201.05910979211, 2037: 57140.02000677306, 2038: 55078.98090375494, 2039: 53017.94180073589, 2040: 50956.90269771684, 2041: 48895.86359469779, 2042: 46834.82449167967, 2043: 44773.78538866062, 2044: 42712.746285641566, 2045: 40651.707182622515, 2046: 38590.668079604395, 2047: 36529.62897658534, 2048: 34468.58987356629, 2049: 32407.55077054724, 2050: 30346.51166752819}</t>
         </is>
       </c>
-      <c r="T152" t="n">
+      <c r="S152" t="n">
         <v>1746459.329392941</v>
       </c>
     </row>
@@ -11440,15 +10680,10 @@
       </c>
       <c r="R153" t="inlineStr">
         <is>
-          <t>{2021: 20293.7181386378, 2022: 15864.841990009261, 2023: 12402.518338359838, 2024: 9695.807952592302, 2025: 7579.806720607054, 2026: 5925.599001411628, 2027: 4632.403545339789, 2028: 3621.4334790060097, 2029: 2831.0962796104145, 2030: 2213.2413009623665, 2031: 1730.226234820831, 2032: 1352.6237841127165, 2033: 1057.4288289744168, 2034: 826.6568586768454, 2035: 646.2482800476054, 2036: 505.2118482788147, 2037: 394.95503434453127, 2038: 308.7605322114356, 2039: 241.37701247359456, 2040: 188.69918941187763, 2041: 147.51770982580612, 2042: 115.32362581988357, 2043: 90.15553920915029, 2044: 70.48010494213267, 2045: 55.09861331016109, 2046: 43.07395954071342, 2047: 33.6735514571082, 2048: 26.324676900500577, 2049: 20.57961171094307, 2050: 16.0883424998516}</t>
-        </is>
-      </c>
-      <c r="S153" t="inlineStr">
-        <is>
           <t>{2021: 20293.7181386378, 2022: 18587.19970992254, 2023: 17460.61202347465, 2024: 16334.02433702629, 2025: 15207.436650578398, 2026: 14080.848964130506, 2027: 12954.261277682614, 2028: 11827.673591234256, 2029: 10701.085904786363, 2030: 9574.49821833847, 2031: 8447.910531890579, 2032: 7321.322845442221, 2033: 6194.735158994328, 2034: 5068.147472546436, 2035: 3941.559786098078, 2036: 2814.9720996501856, 2037: 1688.3844132022932, 2038: 561.7967267544009, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T153" t="n">
+      <c r="S153" t="n">
         <v>172913.3287810715</v>
       </c>
     </row>
@@ -11512,15 +10747,10 @@
       </c>
       <c r="R154" t="inlineStr">
         <is>
-          <t>{2021: 15596.1794677321, 2022: 12102.950293388843, 2023: 9392.133894541641, 2024: 7288.4856133948815, 2025: 5656.012055741316, 2026: 4389.179600752529, 2027: 3406.0920269974836, 2028: 2643.1962124281126, 2029: 2051.1736506288717, 2030: 1591.752184439315, 2031: 1235.2318468455992, 2032: 958.564863536872, 2033: 743.8656961071017, 2034: 577.2548054841342, 2035: 447.96138899588163, 2036: 347.62708620991276, 2037: 269.7656406005678, 2038: 209.34358608837186, 2039: 162.45485132492917, 2040: 126.06824604535043, 2041: 97.83150537722443, 2042: 75.91922426628295, 2043: 58.91485151915062, 2044: 45.71911479692345, 2045: 35.478956560466266, 2046: 27.532386928544728, 2047: 21.365688381821432, 2048: 16.580205748736642, 2049: 12.866574563744726, 2050: 9.984721752745253}</t>
-        </is>
-      </c>
-      <c r="S154" t="inlineStr">
-        <is>
           <t>{2021: 15596.1794677321, 2022: 14238.2978310443, 2023: 13451.393019699259, 2024: 12664.488208354218, 2025: 11877.58339700941, 2026: 11090.67858566437, 2027: 10303.773774319561, 2028: 9516.86896297452, 2029: 8729.964151629712, 2030: 7943.059340284672, 2031: 7156.154528939864, 2032: 6369.249717594823, 2033: 5582.344906249782, 2034: 4795.440094904974, 2035: 4008.5352835599333, 2036: 3221.6304722151253, 2037: 2434.7256608700845, 2038: 1647.8208495252766, 2039: 860.9160381802358, 2040: 74.01122683519498, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T154" t="n">
+      <c r="S154" t="n">
         <v>143765.0257837214</v>
       </c>
     </row>
@@ -11584,15 +10814,10 @@
       </c>
       <c r="R155" t="inlineStr">
         <is>
-          <t>{2021: 39224.6787840837, 2022: 30599.94838897429, 2023: 23871.625477474612, 2024: 18622.727584146643, 2025: 14527.95843335361, 2026: 11333.547961090568, 2027: 8841.525116938896, 2028: 6897.448765544307, 2029: 5380.836319987744, 2030: 4197.696929208639, 2031: 3274.7064697050214, 2032: 2554.663341250219, 2033: 1992.943443176943, 2034: 1554.7346312012328, 2035: 1212.8792624456937, 2036: 946.1911221043649, 2037: 738.142424616814, 2038: 575.8395172926719, 2039: 449.22380643274033, 2040: 350.4483839780547, 2041: 273.391721618873, 2042: 213.27829394245913, 2043: 166.38261904074352, 2044: 129.79837472971315, 2045: 101.2582815417121, 2046: 78.99358988224283, 2047: 61.62446317947329, 2048: 48.07446360925448, 2049: 37.50384071641481, 2050: 29.257488547650695}</t>
-        </is>
-      </c>
-      <c r="S155" t="inlineStr">
-        <is>
           <t>{2021: 39224.6787840837, 2022: 36384.49622808257, 2023: 34387.81964153238, 2024: 32391.14305498218, 2025: 30394.466468431987, 2026: 28397.789881881792, 2027: 26401.113295332063, 2028: 24404.43670878187, 2029: 22407.760122231673, 2030: 20411.08353568148, 2031: 18414.40694913175, 2032: 16417.730362581555, 2033: 14421.05377603136, 2034: 12424.377189481165, 2035: 10427.70060293097, 2036: 8431.024016381241, 2037: 6434.347429831047, 2038: 4437.670843280852, 2039: 2440.994256730657, 2040: 444.3176701804623, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T155" t="n">
+      <c r="S155" t="n">
         <v>369486.0714255409</v>
       </c>
     </row>
@@ -11656,15 +10881,10 @@
       </c>
       <c r="R156" t="inlineStr">
         <is>
-          <t>{2021: 33896.0681128131, 2022: 26021.028297245048, 2023: 19975.58865507703, 2024: 15334.679996450734, 2025: 11771.98903391413, 2026: 9037.014521768258, 2027: 6937.453919755843, 2028: 5325.682145669335, 2029: 4088.371705926854, 2030: 3138.524370894938, 2031: 2409.354123163893, 2032: 1849.5912743706315, 2033: 1419.8775718928498, 2034: 1089.9988268220754, 2035: 836.7604827292531, 2036: 642.3567514275718, 2037: 493.1186458026049, 2038: 378.552880930703, 2039: 290.6040663453212, 2040: 223.08831244080565, 2041: 171.25842653745732, 2042: 131.470126512647, 2043: 100.92580268726815, 2044: 77.47781125843451, 2045: 59.47746837345551, 2046: 45.6591272605199, 2047: 35.051187604393164, 2048: 26.907780025412087, 2049: 20.656322235575793, 2050: 15.85725942076891}</t>
-        </is>
-      </c>
-      <c r="S156" t="inlineStr">
-        <is>
           <t>{2021: 33896.0681128131, 2022: 34698.09880006558, 2023: 34194.96985922323, 2024: 33691.84091838088, 2025: 33188.711977538536, 2026: 32685.583036696073, 2027: 32182.454095853725, 2028: 31679.32515501138, 2029: 31176.19621416903, 2030: 30673.067273326684, 2031: 30169.93833248422, 2032: 29666.809391641873, 2033: 29163.680450799526, 2034: 28660.55150995718, 2035: 28157.42256911483, 2036: 27654.293628272368, 2037: 27151.16468743002, 2038: 26648.035746587673, 2039: 26144.906805745326, 2040: 25641.77786490298, 2041: 25138.648924060515, 2042: 24635.519983218168, 2043: 24132.39104237582, 2044: 23629.262101533473, 2045: 23126.133160691126, 2046: 22623.004219848663, 2047: 22119.875279006315, 2048: 21616.746338163968, 2049: 21113.61739732162, 2050: 20610.488456479274}</t>
         </is>
       </c>
-      <c r="T156" t="n">
+      <c r="S156" t="n">
         <v>808617.3050480669</v>
       </c>
     </row>
@@ -11728,15 +10948,10 @@
       </c>
       <c r="R157" t="inlineStr">
         <is>
-          <t>{2021: 543303.129520453, 2022: 408309.290636402, 2023: 306857.19952902576, 2024: 230612.78070855033, 2025: 173312.7158422737, 2026: 130249.92535251552, 2027: 97886.89174875779, 2028: 73565.06002057352, 2029: 55286.44294601644, 2030: 41549.490651789194, 2031: 31225.741455437725, 2032: 23467.121116197246, 2033: 17636.275323299622, 2034: 13254.212382470105, 2035: 9960.955057644027, 2036: 7485.969199620823, 2037: 5625.939935816371, 2038: 4228.069781935076, 2039: 3177.5266506322, 2040: 2388.0106375294763, 2041: 1794.6646659342239, 2042: 1348.746614665381, 2043: 1013.6252555150043, 2044: 761.7710750456711, 2045: 572.4947830758224, 2046: 430.2477310908439, 2047: 323.3446235339796, 2048: 243.00359540131006, 2049: 182.62480053811083, 2050: 137.24824818540506}</t>
-        </is>
-      </c>
-      <c r="S157" t="inlineStr">
-        <is>
           <t>{2021: 543303.129520453, 2022: 522772.98167590424, 2023: 513875.21056812257, 2024: 504977.43946033716, 2025: 496079.66835255176, 2026: 487181.8972447701, 2027: 478284.1261369847, 2028: 469386.355029203, 2029: 460488.5839214176, 2030: 451590.8128136322, 2031: 442693.0417058505, 2032: 433795.2705980651, 2033: 424897.4994902797, 2034: 415999.728382498, 2035: 407101.9572747126, 2036: 398204.18616693094, 2037: 389306.41505914554, 2038: 380408.64395136014, 2039: 371510.87284357846, 2040: 362613.10173579305, 2041: 353715.33062800765, 2042: 344817.559520226, 2043: 335919.78841244057, 2044: 327022.0173046589, 2045: 318124.2461968735, 2046: 309226.4750890881, 2047: 300328.7039813064, 2048: 291430.932873521, 2049: 282533.1617657356, 2050: 273635.3906579539}</t>
         </is>
       </c>
-      <c r="T157" t="n">
+      <c r="S157" t="n">
         <v>11682755.2682722</v>
       </c>
     </row>
@@ -11800,15 +11015,10 @@
       </c>
       <c r="R158" t="inlineStr">
         <is>
-          <t>{2021: 152121.872219682, 2022: 116573.93263378636, 2023: 89332.85905186426, 2024: 68457.49753892508, 2025: 52460.304293755085, 2026: 40201.34573321992, 2027: 30807.06870688637, 2028: 23608.05254154863, 2029: 18091.307229108013, 2030: 13863.718605418948, 2031: 10624.035683888837, 2032: 8141.404007466325, 2033: 6238.915341117023, 2034: 4781.001483027846, 2035: 3663.773898336299, 2036: 2807.6207936311544, 2037: 2151.534111973869, 2038: 1648.762199470776, 2039: 1263.4783595923411, 2040: 968.2279019197335, 2041: 741.9717662266573, 2042: 568.5873137780567, 2043: 435.7194547084526, 2044: 333.9002447134059, 2045: 255.87421496768314, 2046: 196.08135939380315, 2047: 150.26093780718688, 2048: 115.14786260406166, 2049: 88.2400340086902, 2050: 67.62004457371629}</t>
-        </is>
-      </c>
-      <c r="S158" t="inlineStr">
-        <is>
           <t>{2021: 152121.872219682, 2022: 145684.03787789308, 2023: 141103.97323600948, 2024: 136523.90859412774, 2025: 131943.84395224415, 2026: 127363.77931036055, 2027: 122783.71466847695, 2028: 118203.65002659336, 2029: 113623.58538470976, 2030: 109043.52074282616, 2031: 104463.45610094257, 2032: 99883.39145905897, 2033: 95303.32681717537, 2034: 90723.26217529178, 2035: 86143.19753340818, 2036: 81563.13289152458, 2037: 76983.06824964099, 2038: 72403.00360775739, 2039: 67822.9389658738, 2040: 63242.87432399206, 2041: 58662.80968210846, 2042: 54082.745040224865, 2043: 49502.68039834127, 2044: 44922.61575645767, 2045: 40342.551114574075, 2046: 35762.48647269048, 2047: 31182.42183080688, 2048: 26602.357188923284, 2049: 22022.292547039688, 2050: 17442.22790515609}</t>
         </is>
       </c>
-      <c r="T158" t="n">
+      <c r="S158" t="n">
         <v>2432670.676011492</v>
       </c>
     </row>
@@ -11872,15 +11082,10 @@
       </c>
       <c r="R159" t="inlineStr">
         <is>
-          <t>{2021: 15373.6263462622, 2022: 12112.93453088141, 2023: 9543.823925777418, 2024: 7519.6126004004445, 2025: 5924.729343274755, 2026: 4668.115188432923, 2027: 3678.0244547734087, 2028: 2897.928466596495, 2029: 2283.2880805377044, 2030: 1799.0107481322675, 2031: 1417.4469264225536, 2032: 1116.8114427946848, 2033: 879.939682754178, 2034: 693.3075858785496, 2035: 546.2594971649044, 2036: 430.39978837780404, 2037: 339.1135143591606, 2038: 267.1887364407242, 2039: 210.5189497260221, 2040: 165.8686244941295, 2041: 130.688475443091, 2042: 102.96991167394569, 2043: 81.13035731874639, 2044: 63.92289525808085, 2045: 50.365075086775335, 2046: 39.68282065846895, 2047: 31.266234641744717, 2048: 24.634776773712215, 2049: 19.409827682939895, 2050: 15.293071828580185}</t>
-        </is>
-      </c>
-      <c r="S159" t="inlineStr">
-        <is>
           <t>{2021: 15373.6263462622, 2022: 13941.64697230095, 2023: 12952.635565133998, 2024: 11963.624157967279, 2025: 10974.61275080056, 2026: 9985.60134363384, 2027: 8996.589936466888, 2028: 8007.578529300168, 2029: 7018.567122133449, 2030: 6029.555714966729, 2031: 5040.544307799777, 2032: 4051.5329006330576, 2033: 3062.521493466338, 2034: 2073.5100862996187, 2035: 1084.4986791326664, 2036: 95.487271965947, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T159" t="n">
+      <c r="S159" t="n">
         <v>112965.3200051324</v>
       </c>
     </row>
@@ -11944,15 +11149,10 @@
       </c>
       <c r="R160" t="inlineStr">
         <is>
-          <t>{2021: 69235.9040374478, 2022: 50300.04439627163, 2023: 36543.098576403914, 2024: 26548.64562433184, 2025: 19287.652441751805, 2026: 14012.52410303236, 2027: 10180.13116583457, 2028: 7395.888834272858, 2029: 5373.130341630297, 2030: 3903.591618949284, 2031: 2835.9683385063054, 2032: 2060.337556307962, 2033: 1496.8399993382473, 2034: 1087.4577210706477, 2035: 790.0405491829304, 2036: 573.9662860076537, 2037: 416.9878341233594, 2038: 302.94262580532757, 2039: 220.08851822443538, 2040: 159.89481746076464, 2041: 116.16395465364515, 2042: 84.39338169347059, 2043: 61.311986966142115, 2044: 44.54330031933329, 2045: 32.36081069161865, 2046: 23.51020380419029, 2047: 17.080217432801188, 2048: 12.408817464175657, 2049: 9.015034584016885, 2050: 6.549443473211688}</t>
-        </is>
-      </c>
-      <c r="S160" t="inlineStr">
-        <is>
           <t>{2021: 69235.9040374478, 2022: 68306.6654896239, 2023: 68857.43067811907, 2024: 69408.19586661423, 2025: 69958.9610551094, 2026: 70509.72624360432, 2027: 71060.49143209949, 2028: 71611.25662059465, 2029: 72162.02180908981, 2030: 72712.78699758498, 2031: 73263.55218608014, 2032: 73814.3173745753, 2033: 74365.08256307046, 2034: 74915.84775156563, 2035: 75466.61294006079, 2036: 76017.37812855595, 2037: 76568.14331705112, 2038: 77118.90850554628, 2039: 77669.67369404144, 2040: 78220.4388825366, 2041: 78771.20407103177, 2042: 79321.96925952693, 2043: 79872.73444802209, 2044: 80423.49963651726, 2045: 80974.26482501242, 2046: 81525.03001350758, 2047: 82075.79520200274, 2048: 82626.5603904979, 2049: 83177.32557899307, 2050: 83728.09076748823}</t>
         </is>
       </c>
-      <c r="T160" t="n">
+      <c r="S160" t="n">
         <v>2197257.872363103</v>
       </c>
     </row>
@@ -12016,15 +11216,10 @@
       </c>
       <c r="R161" t="inlineStr">
         <is>
-          <t>{2021: 38141.8121612654, 2022: 29467.991661448905, 2023: 22766.682633948905, 2024: 17589.316710478037, 2025: 13589.334349491874, 2026: 10498.987032979565, 2027: 8111.414870206256, 2028: 6266.799929357646, 2029: 4841.668436766614, 2030: 3740.6257604883963, 2031: 2889.9709393098765, 2032: 2232.763330209525, 2033: 1725.0111483538997, 2034: 1332.726770313807, 2035: 1029.6516900809484, 2036: 795.4988422997765, 2037: 614.5946383582725, 2038: 474.82981673076154, 2039: 366.84888019660315, 2040: 283.42386294963933, 2041: 218.97050918145266, 2042: 169.1744773787957, 2043: 130.70254941350268, 2044: 100.97951350509274, 2045: 78.01578617617834, 2046: 60.27423465830243, 2047: 46.56728518302641, 2048: 35.977429852252975, 2049: 27.795811022403733, 2050: 21.474772199293128}</t>
-        </is>
-      </c>
-      <c r="S161" t="inlineStr">
-        <is>
           <t>{2021: 38141.8121612654, 2022: 37427.45519132633, 2023: 36281.55449908879, 2024: 35135.653806851245, 2025: 33989.75311461417, 2026: 32843.85242237663, 2027: 31697.951730139088, 2028: 30552.051037901547, 2029: 29406.150345664006, 2030: 28260.24965342693, 2031: 27114.34896118939, 2032: 25968.448268951848, 2033: 24822.547576714307, 2034: 23676.646884476766, 2035: 22530.746192239225, 2036: 21384.84550000215, 2037: 20238.94480776461, 2038: 19093.044115527067, 2039: 17947.143423289526, 2040: 16801.242731051985, 2041: 15655.34203881491, 2042: 14509.441346577369, 2043: 13363.540654339828, 2044: 12217.639962102287, 2045: 11071.739269864745, 2046: 9925.83857762767, 2047: 8779.937885390129, 2048: 7634.037193152588, 2049: 6488.136500915047, 2050: 5342.235808677506}</t>
         </is>
       </c>
-      <c r="T161" t="n">
+      <c r="S161" t="n">
         <v>636560.3076763516</v>
       </c>
     </row>
@@ -12088,15 +11283,10 @@
       </c>
       <c r="R162" t="inlineStr">
         <is>
-          <t>{2021: 213705.500467378, 2022: 162425.17962316176, 2023: 123449.97633621296, 2024: 93827.18056873453, 2025: 71312.6083515941, 2026: 54200.585364306, 2027: 41194.72729632324, 2028: 31309.72748010224, 2029: 23796.711356449836, 2030: 18086.502724818332, 2031: 13746.50370443722, 2032: 10447.921688962359, 2033: 7940.860451916566, 2034: 6035.388337895852, 2035: 4587.149290656238, 2036: 3486.4266285314106, 2037: 2649.8310532191067, 2038: 2013.9831864357907, 2039: 1530.7120317419992, 2040: 1163.4056033339286, 2041: 884.2372502478092, 2042: 672.0575459540636, 2043: 510.7920356750626, 2044: 388.22345687478975, 2045: 295.06617554955363, 2046: 224.26271883288058, 2047: 170.44911015179807, 2048: 129.54850143054702, 2049: 98.46231645301083, 2050: 74.83550681202126}</t>
-        </is>
-      </c>
-      <c r="S162" t="inlineStr">
-        <is>
           <t>{2021: 213705.500467378, 2022: 209602.0461340025, 2023: 205585.987681441, 2024: 201569.92922887858, 2025: 197553.87077631708, 2026: 193537.81232375465, 2027: 189521.75387119316, 2028: 185505.69541863073, 2029: 181489.63696606923, 2030: 177473.57851350773, 2031: 173457.5200609453, 2032: 169441.4616083838, 2033: 165425.40315582138, 2034: 161409.34470325988, 2035: 157393.28625069745, 2036: 153377.22779813595, 2037: 149361.16934557352, 2038: 145345.11089301202, 2039: 141329.0524404496, 2040: 137312.9939878881, 2041: 133296.93553532567, 2042: 129280.87708276417, 2043: 125264.81863020174, 2044: 121248.76017764024, 2045: 117232.70172507782, 2046: 113216.64327251632, 2047: 109200.58481995389, 2048: 105184.52636739239, 2049: 101168.4679148309, 2050: 97152.40946226846}</t>
         </is>
       </c>
-      <c r="T162" t="n">
+      <c r="S162" t="n">
         <v>4506216.151648488</v>
       </c>
     </row>
@@ -12160,15 +11350,10 @@
       </c>
       <c r="R163" t="inlineStr">
         <is>
-          <t>{2021: 186079.663676732, 2022: 147528.97233526394, 2023: 116964.9452726339, 2024: 92732.96089625177, 2025: 73521.1906143451, 2026: 58289.58136469198, 2027: 46213.55104943183, 2028: 36639.34875833754, 2029: 29048.66315075338, 2030: 23030.563026967528, 2031: 18259.25105697567, 2032: 14476.42633709274, 2033: 11477.300949493794, 2034: 9099.513513754786, 2035: 7214.339551726919, 2036: 5719.72282792237, 2037: 4534.750408362071, 2038: 3595.2723383293055, 2039: 2850.428804840147, 2040: 2259.8967774547027, 2041: 1791.7070709073764, 2042: 1420.513653528511, 2043: 1126.2215083177696, 2044: 892.8987642230321, 2045: 707.9142044995157, 2046: 561.2534600921501, 2047: 444.97686932008196, 2048: 352.78965442349676, 2049: 279.7011459459095, 2050: 221.75460664031436}</t>
-        </is>
-      </c>
-      <c r="S163" t="inlineStr">
-        <is>
           <t>{2021: 186079.663676732, 2022: 182518.53520077094, 2023: 172961.05546812713, 2024: 163403.5757354796, 2025: 153846.09600283578, 2026: 144288.61627018824, 2027: 134731.13653754443, 2028: 125173.65680489689, 2029: 115616.17707225308, 2030: 106058.69733960554, 2031: 96501.21760696173, 2032: 86943.73787431419, 2033: 77386.25814167038, 2034: 67828.77840902284, 2035: 58271.298676379025, 2036: 48713.81894373521, 2037: 39156.339211087674, 2038: 29598.85947844386, 2039: 20041.379745796323, 2040: 10483.90001315251, 2041: 926.4202805049717, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T163" t="n">
+      <c r="S163" t="n">
         <v>1927489.386651136</v>
       </c>
     </row>
@@ -12232,15 +11417,10 @@
       </c>
       <c r="R164" t="inlineStr">
         <is>
-          <t>{2021: 63097.8564675558, 2022: 48519.77731578855, 2023: 37309.80611019958, 2024: 28689.777838854912, 2025: 22061.31412239729, 2026: 16964.285451800893, 2027: 13044.870278058985, 2028: 10030.993704678673, 2029: 7713.440805351961, 2030: 5931.333505863724, 2031: 4560.962875785807, 2032: 3507.2015987182426, 2033: 2696.9004986545856, 2034: 2073.810727704241, 2035: 1594.6791275713342, 2036: 1226.2457156477526, 2037: 942.9348695587064, 2038: 725.0799386157471, 2039: 557.5580396438853, 2040: 428.7402685075215, 2041: 329.68445394009046, 2042: 253.51441689426645, 2043: 194.94264532387965, 2044: 149.90324980895164, 2045: 115.2697208245606, 2046: 88.63789514841255, 2047: 68.15906553897848, 2048: 52.411648622389066, 2049: 40.30250252984829, 2050: 30.991044030516694}</t>
-        </is>
-      </c>
-      <c r="S164" t="inlineStr">
-        <is>
           <t>{2021: 63097.8564675558, 2022: 60442.29463734198, 2023: 58393.62699066289, 2024: 56344.959343983326, 2025: 54296.29169730423, 2026: 52247.624050625134, 2027: 50198.95640394604, 2028: 48150.28875726648, 2029: 46101.62111058738, 2030: 44052.953463908285, 2031: 42004.28581722919, 2032: 39955.61817055009, 2033: 37906.95052387053, 2034: 35858.282877191436, 2035: 33809.61523051234, 2036: 31760.947583833244, 2037: 29712.279937153682, 2038: 27663.612290474586, 2039: 25614.94464379549, 2040: 23566.276997116394, 2041: 21517.6093504373, 2042: 19468.941703757737, 2043: 17420.27405707864, 2044: 15371.606410399545, 2045: 13322.938763720449, 2046: 11274.271117040887, 2047: 9225.603470361792, 2048: 7176.935823682696, 2049: 5128.2681770036, 2050: 3079.600530324504}</t>
         </is>
       </c>
-      <c r="T164" t="n">
+      <c r="S164" t="n">
         <v>951076.6078997755</v>
       </c>
     </row>
@@ -12304,15 +11484,10 @@
       </c>
       <c r="R165" t="inlineStr">
         <is>
-          <t>{2021: 14328.4594416561, 2022: 11461.193476149696, 2023: 9167.695692102521, 2024: 7333.149420947563, 2025: 5865.71394121076, 2026: 4691.926765030838, 2027: 3753.025972464783, 2028: 3002.008482948402, 2029: 2401.27699563335, 2030: 1920.7578001561012, 2031: 1536.3952320242129, 2032: 1228.947402319488, 2033: 983.0229137576598, 2034: 786.3103393593266, 2035: 628.9618900336255, 2036: 503.1004163534127, 2037: 402.42506413456215, 2038: 321.8958422207793, 2039: 257.481311363791, 2040: 205.9567630455647, 2041: 164.74278470748874, 2042: 131.77612966840832, 2043: 105.40642724485767, 2044: 84.31356219433027, 2045: 67.44158734631625, 2046: 53.94586096727227, 2047: 43.15076245991156, 2048: 34.5158695678495, 2049: 27.608903854980476, 2050: 22.084090061099612}</t>
-        </is>
-      </c>
-      <c r="S165" t="inlineStr">
-        <is>
           <t>{2021: 14328.4594416561, 2022: 12423.919117198791, 2023: 11159.893011445645, 2024: 9895.866905692033, 2025: 8631.840799938422, 2026: 7367.81469418481, 2027: 6103.788588431198, 2028: 4839.762482677586, 2029: 3575.7363769239746, 2030: 2311.710271170363, 2031: 1047.684165416751, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T165" t="n">
+      <c r="S165" t="n">
         <v>74522.24613390763</v>
       </c>
     </row>
@@ -12376,15 +11551,10 @@
       </c>
       <c r="R166" t="inlineStr">
         <is>
-          <t>{2021: 29250.7309323134, 2022: 22538.423786834337, 2023: 17366.4223287416, 2024: 13381.26513870894, 2025: 10310.601304223961, 2026: 7944.577598058249, 2027: 6121.496831199553, 2028: 4716.76725311928, 2029: 3634.3877867757974, 2030: 2800.3871880534034, 2031: 2157.7687531166657, 2032: 1662.615088295376, 2033: 1281.0867373228577, 2034: 987.1095481439281, 2035: 760.5927308818483, 2036: 586.0558266892158, 2037: 451.5707527182951, 2038: 347.9466211649903, 2039: 268.1016218418793, 2040: 206.57904190471382, 2041: 159.1743468804462, 2042: 122.64783722108285, 2043: 94.50324295225455, 2044: 72.81712528199117, 2045: 56.10742625003956, 2046: 43.23218292692189, 2047: 33.31148415715323, 2048: 25.667336267243122, 2049: 19.777328081440693, 2050: 15.238928651124686}</t>
-        </is>
-      </c>
-      <c r="S166" t="inlineStr">
-        <is>
           <t>{2021: 29250.7309323134, 2022: 27495.367590732872, 2023: 26371.912746458314, 2024: 25248.457902183756, 2025: 24125.003057909198, 2026: 23001.548213634174, 2027: 21878.093369359616, 2028: 20754.638525085058, 2029: 19631.1836808105, 2030: 18507.72883653594, 2031: 17384.273992261384, 2032: 16260.819147986826, 2033: 15137.364303712267, 2034: 14013.90945943771, 2035: 12890.454615162686, 2036: 11766.999770888127, 2037: 10643.54492661357, 2038: 9520.090082339011, 2039: 8396.635238064453, 2040: 7273.180393789895, 2041: 6149.725549515337, 2042: 5026.270705240779, 2043: 3902.8158609662205, 2044: 2779.3610166911967, 2045: 1655.9061724166386, 2046: 532.4513281420805, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T166" t="n">
+      <c r="S166" t="n">
         <v>364973.1019520943</v>
       </c>
     </row>
@@ -12448,15 +11618,10 @@
       </c>
       <c r="R167" t="inlineStr">
         <is>
-          <t>{2021: 18256.261785925, 2022: 14120.57551174975, 2023: 10921.767836214452, 2024: 8447.60276016451, 2025: 6533.923213137397, 2026: 5053.759482689543, 2027: 3908.904968078233, 2028: 3023.4003224338503, 2029: 2338.4936662164887, 2030: 1808.7424898243132, 2031: 1398.998612550866, 2032: 1082.0761545273115, 2033: 836.9477951530436, 2034: 647.3496425189554, 2035: 500.7021490423903, 2036: 387.27547771578037, 2037: 299.54394229549865, 2038: 231.6866895243466, 2039: 179.20149441645918, 2040: 138.60604451218452, 2041: 107.20689376990562, 2042: 82.92075653873427, 2043: 64.13628474035865, 2044: 49.60715738736493, 2045: 38.36938909101261, 2046: 29.67737110436594, 2047: 22.954401321770188, 2048: 17.754420975763928, 2049: 13.732419319761936, 2050: 10.621542692448012}</t>
-        </is>
-      </c>
-      <c r="S167" t="inlineStr">
-        <is>
           <t>{2021: 18256.261785925, 2022: 16993.85341228661, 2023: 16199.939025656553, 2024: 15406.024639026495, 2025: 14612.110252396436, 2026: 13818.195865766378, 2027: 13024.28147913632, 2028: 12230.367092506262, 2029: 11436.452705876203, 2030: 10642.538319246145, 2031: 9848.623932616087, 2032: 9054.709545985796, 2033: 8260.795159355737, 2034: 7466.880772725679, 2035: 6672.966386095621, 2036: 5879.051999465562, 2037: 5085.137612835504, 2038: 4291.223226205446, 2039: 3497.3088395753875, 2040: 2703.3944529453292, 2041: 1909.480066315271, 2042: 1115.5656796852127, 2043: 321.65129305492155, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T167" t="n">
+      <c r="S167" t="n">
         <v>199598.6826517215</v>
       </c>
     </row>
@@ -12520,15 +11685,10 @@
       </c>
       <c r="R168" t="inlineStr">
         <is>
-          <t>{2021: 38514.0563417962, 2022: 28916.967830584414, 2023: 21711.320695338007, 2024: 16301.205890516976, 2025: 12239.20539951696, 2026: 9189.390638805951, 2027: 6899.54106954584, 2028: 5180.285488063142, 2029: 3889.4409740217698, 2030: 2920.2543229051907, 2031: 2192.5735259657195, 2032: 1646.2191765486941, 2033: 1236.0076162294376, 2034: 928.0142335481942, 2035: 696.7678890970342, 2036: 523.144445123992, 2037: 392.78519396001633, 2038: 294.90938885462356, 2039: 221.4226731862525, 2040: 166.24767489214975, 2041: 124.82140608878653, 2042: 93.71790269000316, 2043: 70.36489621311779, 2044: 52.83108645164961, 2045: 39.666422404831735, 2046: 29.78218265184676, 2047: 22.360937783991353, 2048: 16.788948762575885, 2049: 12.605410527737083, 2050: 9.464343290330332}</t>
-        </is>
-      </c>
-      <c r="S168" t="inlineStr">
-        <is>
           <t>{2021: 38514.0563417962, 2022: 37113.541805813555, 2023: 36518.52005013684, 2024: 35923.49829445989, 2025: 35328.47653878294, 2026: 34733.45478310622, 2027: 34138.43302742927, 2028: 33543.411271752324, 2029: 32948.38951607561, 2030: 32353.367760398658, 2031: 31758.34600472171, 2032: 31163.324249044992, 2033: 30568.302493368043, 2034: 29973.280737691093, 2035: 29378.258982014377, 2036: 28783.237226337427, 2037: 28188.215470660478, 2038: 27593.19371498376, 2039: 26998.171959306812, 2040: 26403.150203629863, 2041: 25808.128447953146, 2042: 25213.106692276197, 2043: 24618.084936599247, 2044: 24023.06318092253, 2045: 23428.04142524558, 2046: 22833.01966956863, 2047: 22237.997913891915, 2048: 21642.976158214966, 2049: 21047.954402538016, 2050: 20452.9326468613}</t>
         </is>
       </c>
-      <c r="T168" t="n">
+      <c r="S168" t="n">
         <v>843744.4414112528</v>
       </c>
     </row>
@@ -12592,15 +11752,10 @@
       </c>
       <c r="R169" t="inlineStr">
         <is>
-          <t>{2021: 31969.8315052147, 2022: 24574.999289701438, 2023: 18890.640383585294, 2024: 14521.111064751489, 2025: 11162.282605203458, 2026: 8580.373251250248, 2027: 6595.676505847509, 2028: 5070.053166212784, 2029: 3897.3165353750564, 2030: 2995.8415975061134, 2031: 2302.883739589366, 2032: 1770.2115901187199, 2033: 1360.7500109186658, 2034: 1045.9995870273156, 2035: 804.0530055352772, 2036: 618.07025904058, 2037: 475.1065445693793, 2038: 365.21127718238154, 2039: 280.73550765771256, 2040: 215.79953901718028, 2041: 165.88368685021283, 2042: 127.51369946545042, 2043: 98.01894242950598, 2044: 75.34651661174648, 2045: 57.91837194741305, 2046: 44.52147172674881, 2047: 34.22336260617607, 2048: 26.30727383097991, 2049: 20.22222843448079, 2050: 15.54469404483676}</t>
-        </is>
-      </c>
-      <c r="S169" t="inlineStr">
-        <is>
           <t>{2021: 31969.8315052147, 2022: 32409.64653846342, 2023: 31825.880827790592, 2024: 31242.11511711753, 2025: 30658.3494064447, 2026: 30074.58369577187, 2027: 29490.81798509881, 2028: 28907.05227442598, 2029: 28323.286563752918, 2030: 27739.52085308009, 2031: 27155.75514240726, 2032: 26571.989431734197, 2033: 25988.223721061368, 2034: 25404.45801038854, 2035: 24820.692299715476, 2036: 24236.926589042647, 2037: 23653.160878369818, 2038: 23069.395167696755, 2039: 22485.629457023926, 2040: 21901.863746351097, 2041: 21318.098035678035, 2042: 20734.332325005205, 2043: 20150.566614332376, 2044: 19566.800903659314, 2045: 18983.035192986485, 2046: 18399.269482313655, 2047: 17815.503771640593, 2048: 17231.738060967764, 2049: 16647.972350294935, 2050: 16064.206639621872}</t>
         </is>
       </c>
-      <c r="T169" t="n">
+      <c r="S169" t="n">
         <v>710823.6835150337</v>
       </c>
     </row>
@@ -12664,15 +11819,10 @@
       </c>
       <c r="R170" t="inlineStr">
         <is>
-          <t>{2021: 72186.9558804449, 2022: 56429.29739913872, 2023: 44111.3711767287, 2024: 34482.319588845894, 2025: 26955.189387868937, 2026: 21071.15308944912, 2027: 16471.540456652056, 2028: 12875.975218982114, 2029: 10065.284317283555, 2030: 7868.137881967993, 2031: 6150.605564450418, 2032: 4807.992612349384, 2033: 3758.4580441994003, 2034: 2938.0259099659106, 2035: 2296.6855412828595, 2036: 1795.343076330782, 2037: 1403.4384349929164, 2038: 1097.0824834442233, 2039: 857.6008362534407, 2040: 670.3955312763796, 2041: 524.0551890302994, 2042: 409.65941498252823, 2043: 320.2350435540181, 2044: 250.3310783774313, 2045: 195.68641865716694, 2046: 152.97011739442223, 2047: 119.57833852873941, 2048: 93.47563621478393, 2049: 73.07088117517709, 2050: 57.120271034564965}</t>
-        </is>
-      </c>
-      <c r="S170" t="inlineStr">
-        <is>
           <t>{2021: 72186.9558804449, 2022: 71584.50207578484, 2023: 68947.86299496423, 2024: 66311.22391414456, 2025: 63674.584833323956, 2026: 61037.94575250428, 2027: 58401.30667168368, 2028: 55764.667590864, 2029: 53128.0285100434, 2030: 50491.389429223724, 2031: 47854.75034840312, 2032: 45218.111267583445, 2033: 42581.47218676284, 2034: 39944.833105943166, 2035: 37308.19402512256, 2036: 34671.55494430289, 2037: 32034.91586348228, 2038: 29398.276782662608, 2039: 26761.637701842003, 2040: 24124.99862102233, 2041: 21488.359540201724, 2042: 18851.72045938205, 2043: 16215.081378561445, 2044: 13578.44229774177, 2045: 10941.803216921166, 2046: 8305.164136101492, 2047: 5668.525055280887, 2048: 3031.8859744612128, 2049: 395.2468936415389, 2050: 0}</t>
         </is>
       </c>
-      <c r="T170" t="n">
+      <c r="S170" t="n">
         <v>1043809.96351218</v>
       </c>
     </row>
@@ -12736,15 +11886,10 @@
       </c>
       <c r="R171" t="inlineStr">
         <is>
-          <t>{2021: 28308.7374505601, 2022: 22193.59532549648, 2023: 17399.422151274845, 2024: 13640.86741053982, 2025: 10694.220882404066, 2026: 8384.097348038169, 2027: 6572.997613789583, 2028: 5153.1245210306515, 2029: 4039.9668293714176, 2030: 3167.2690841860326, 2031: 2483.0880735724895, 2032: 1946.7011539698353, 2033: 1526.1824271159342, 2034: 1196.5025017258376, 2035: 938.0387371787218, 2036: 735.4072985043141, 2037: 576.5475062575924, 2038: 452.0039815322808, 2039: 354.3638591851842, 2040: 277.8155720463468, 2041: 217.80294482882158, 2042: 170.75400931159018, 2043: 133.86839980009458, 2044: 104.95067458320334, 2045: 82.27964263349365, 2046: 64.50591783979739, 2047: 50.57160317150997, 2048: 39.64732435384114, 2049: 31.08286528089022, 2050: 24.36846697263617}</t>
-        </is>
-      </c>
-      <c r="S171" t="inlineStr">
-        <is>
           <t>{2021: 28308.7374505601, 2022: 26172.11326950183, 2023: 24595.62199503649, 2024: 23019.130720571615, 2025: 21442.639446106274, 2026: 19866.148171640933, 2027: 18289.65689717559, 2028: 16713.165622710716, 2029: 15136.674348245375, 2030: 13560.183073780034, 2031: 11983.691799314693, 2032: 10407.200524849817, 2033: 8830.709250384476, 2034: 7254.217975919135, 2035: 5677.7267014542595, 2036: 4101.235426988918, 2037: 2524.744152523577, 2038: 948.2528780582361, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T171" t="n">
+      <c r="S171" t="n">
         <v>244677.480979542</v>
       </c>
     </row>
@@ -12808,15 +11953,10 @@
       </c>
       <c r="R172" t="inlineStr">
         <is>
-          <t>{2021: 1689173.9907568, 2022: 1276705.5585121994, 2023: 964955.1153730879, 2024: 729328.9893480103, 2025: 551238.8775696883, 2026: 416635.4341899009, 2027: 314899.9319277192, 2028: 238006.56158996918, 2029: 179889.28423421297, 2030: 135963.28759224128, 2031: 102763.29494324973, 2032: 77670.19299550942, 2033: 58704.41273113298, 2034: 44369.76324117611, 2035: 33535.39876285935, 2036: 25346.607419809603, 2037: 19157.38388074467, 2038: 14479.46666295795, 2039: 10943.8196858621, 2040: 8271.519393946794, 2041: 6251.750764207548, 2042: 4725.17632569079, 2043: 3571.366190203338, 2044: 2699.297462230231, 2045: 2040.1735362756829, 2046: 1541.9968033758742, 2047: 1165.4666131793788, 2048: 880.8788860405379, 2049: 665.7827887109038, 2050: 503.2096111828805}</t>
-        </is>
-      </c>
-      <c r="S172" t="inlineStr">
-        <is>
           <t>{2021: 1689173.9907568, 2022: 1590012.2309478372, 2023: 1547612.3955596685, 2024: 1505212.5601714998, 2025: 1462812.7247833312, 2026: 1420412.8893951625, 2027: 1378013.0540069938, 2028: 1335613.218618825, 2029: 1293213.3832306564, 2030: 1250813.5478424877, 2031: 1208413.712454304, 2032: 1166013.8770661354, 2033: 1123614.0416779667, 2034: 1081214.206289798, 2035: 1038814.3709016293, 2036: 996414.5355134606, 2037: 954014.700125292, 2038: 911614.8647371233, 2039: 869215.0293489546, 2040: 826815.1939607859, 2041: 784415.3585726172, 2042: 742015.5231844485, 2043: 699615.6877962649, 2044: 657215.8524080962, 2045: 614816.0170199275, 2046: 572416.1816317588, 2047: 530016.3462435901, 2048: 487616.5108554214, 2049: 445216.67546725273, 2050: 402816.84007908404}</t>
         </is>
       </c>
-      <c r="T172" t="n">
+      <c r="S172" t="n">
         <v>29539200.10522923</v>
       </c>
     </row>
@@ -12880,15 +12020,10 @@
       </c>
       <c r="R173" t="inlineStr">
         <is>
-          <t>{2021: 61688.0519093829, 2022: 36614.27577579033, 2023: 21732.007237883252, 2024: 12898.79776618948, 2025: 7655.941855339657, 2026: 4544.101454631692, 2027: 2697.102253406516, 2028: 1600.8358611614906, 2029: 950.1588051190572, 2030: 563.9564785175693, 2031: 334.73026608650486, 2032: 198.6755278153111, 2033: 117.92170996121307, 2034: 69.99115509134595, 2035: 41.54249283386532, 2036: 24.657097151767626, 2037: 14.634953236510881, 2038: 8.686418150382556, 2039: 5.1557295102969825, 2040: 3.060127468325537, 2041: 1.8163055497186178, 2042: 1.0780485074838393, 2043: 0.6398640276511744, 2044: 0.3797843705916179, 2045: 0.22541690408060033, 2046: 0.13379376451465808, 2047: 0.07941184134355407, 2048: 0.04713403923157353, 2049: 0.027975899018287138, 2050: 0.016604792176545074}</t>
-        </is>
-      </c>
-      <c r="S173" t="inlineStr">
-        <is>
           <t>{2021: 61688.0519093829, 2022: 66762.03687416017, 2023: 72405.28307181224, 2024: 78048.52926946431, 2025: 83691.77546711825, 2026: 89335.02166477032, 2027: 94978.26786242239, 2028: 100621.51406007446, 2029: 106264.76025772654, 2030: 111908.0064553786, 2031: 117551.25265303068, 2032: 123194.49885068461, 2033: 128837.74504833668, 2034: 134480.99124598876, 2035: 140124.23744364083, 2036: 145767.4836412929, 2037: 151410.72983894497, 2038: 157053.9760365989, 2039: 162697.22223425098, 2040: 168340.46843190305, 2041: 173983.71462955512, 2042: 179626.9608272072, 2043: 185270.20702485926, 2044: 190913.45322251134, 2045: 196556.69942016527, 2046: 202199.94561781734, 2047: 207843.1918154694, 2048: 213486.4380131215, 2049: 219129.68421077356, 2050: 224772.93040842563}</t>
         </is>
       </c>
-      <c r="T173" t="n">
+      <c r="S173" t="n">
         <v>4145714.586347984</v>
       </c>
     </row>
@@ -12952,15 +12087,10 @@
       </c>
       <c r="R174" t="inlineStr">
         <is>
-          <t>{2021: 42692.4197822988, 2022: 32738.160002284, 2023: 25104.85762579178, 2024: 19251.353049997484, 2025: 14762.664651596831, 2026: 11320.568847784705, 2027: 8681.039775808451, 2028: 6656.949187135199, 2029: 5104.800072866043, 2030: 3914.5535066262937, 2031: 3001.827483448701, 2032: 2301.914694775481, 2033: 1765.1951323783833, 2034: 1353.6182997764179, 2035: 1038.0056390824193, 2036: 795.9819300203532, 2037: 610.3890085597296, 2038: 468.0693464498659, 2039: 358.93325406197204, 2040: 275.2435762962641, 2041: 211.0671703861607, 2042: 161.85427836059267, 2043: 124.11597396079897, 2044: 95.17681675313929, 2045: 72.98517796042717, 2046: 55.96779114531085, 2047: 42.91821618059945, 2048: 32.91130920893945, 2049: 25.237634977383927, 2050: 19.353171738262738}</t>
-        </is>
-      </c>
-      <c r="S174" t="inlineStr">
-        <is>
           <t>{2021: 42692.4197822988, 2022: 41329.597800705116, 2023: 40135.11978953425, 2024: 38940.641778362915, 2025: 37746.16376719205, 2026: 36551.68575602118, 2027: 35357.207744849846, 2028: 34162.72973367898, 2029: 32968.25172250811, 2030: 31773.773711336777, 2031: 30579.29570016591, 2032: 29384.81768899504, 2033: 28190.339677824173, 2034: 26995.86166665284, 2035: 25801.38365548197, 2036: 24606.905644311104, 2037: 23412.42763313977, 2038: 22217.949621968903, 2039: 21023.471610798035, 2040: 19828.9935996267, 2041: 18634.515588455833, 2042: 17440.037577284966, 2043: 16245.559566114098, 2044: 15051.081554942764, 2045: 13856.603543771897, 2046: 12662.125532601029, 2047: 11467.647521429695, 2048: 10273.169510258827, 2049: 9078.69149908796, 2050: 7884.213487916626}</t>
         </is>
       </c>
-      <c r="T174" t="n">
+      <c r="S174" t="n">
         <v>731004.3668322085</v>
       </c>
     </row>
@@ -13024,15 +12154,10 @@
       </c>
       <c r="R175" t="inlineStr">
         <is>
-          <t>{2021: 51009.6333632543, 2022: 37841.414343743105, 2023: 28072.592275607178, 2024: 20825.60736006907, 2025: 15449.443273987148, 2026: 11461.14460670189, 2027: 8502.431664764536, 2028: 6307.515234710358, 2029: 4679.220016666263, 2030: 3471.2718320331815, 2031: 2575.1574170371864, 2032: 1910.3763817417582, 2033: 1417.2096415432582, 2034: 1051.3546897245267, 2035: 779.9457830403251, 2036: 578.6015228046166, 2037: 429.2346076759445, 2038: 318.42700228934126, 2039: 236.22455872320066, 2040: 175.24280837611204, 2041: 130.00359511108945, 2042: 96.44295762217372, 2043: 71.5460527608054, 2044: 53.07632399356295, 2045: 39.37458545879329, 2046: 29.20997279766101, 2047: 21.66937126825169, 2048: 16.075388170129763, 2049: 11.925500819627466, 2050: 8.846913573334113}</t>
-        </is>
-      </c>
-      <c r="S175" t="inlineStr">
-        <is>
           <t>{2021: 51009.6333632543, 2022: 50270.947194789944, 2023: 50113.93128321064, 2024: 49956.91537163133, 2025: 49799.899460051965, 2026: 49642.88354847266, 2027: 49485.86763689335, 2028: 49328.851725314045, 2029: 49171.83581373468, 2030: 49014.819902155374, 2031: 48857.80399057607, 2032: 48700.7880789967, 2033: 48543.772167417395, 2034: 48386.75625583809, 2035: 48229.740344258724, 2036: 48072.72443267942, 2037: 47915.70852110011, 2038: 47758.692609520745, 2039: 47601.67669794144, 2040: 47444.66078636213, 2041: 47287.64487478277, 2042: 47130.62896320346, 2043: 46973.613051624154, 2044: 46816.59714004479, 2045: 46659.58122846548, 2046: 46502.565316886175, 2047: 46345.54940530681, 2048: 46188.533493727504, 2049: 46031.5175821482, 2050: 45874.50167056883}</t>
         </is>
       </c>
-      <c r="T175" t="n">
+      <c r="S175" t="n">
         <v>1396676.574394046</v>
       </c>
     </row>
@@ -13096,15 +12221,10 @@
       </c>
       <c r="R176" t="inlineStr">
         <is>
-          <t>{2021: 134037.461587914, 2022: 101250.17755920846, 2023: 76483.08416410367, 2024: 57774.33980135627, 2025: 43641.99451372499, 2026: 32966.602330456924, 2027: 24902.548137956914, 2028: 18811.06513637695, 2029: 14209.637086321394, 2030: 10733.777415639173, 2031: 8108.157647417603, 2032: 6124.798185174752, 2033: 4626.593912005107, 2034: 3494.869639691155, 2035: 2639.979654739471, 2036: 1994.206736150032, 2037: 1506.398164609577, 2038: 1137.9138327052458, 2039: 859.5654994027004, 2040: 649.3047421762022, 2041: 490.4764657323564, 2042: 370.4996249234548, 2043: 279.8706597745838, 2044: 211.4107030981296, 2045: 159.6969307909724, 2046: 120.63301114995562, 2047: 91.12462779984722, 2048: 68.8343738791249, 2049: 51.9966022548637, 2050: 39.277565752223985}</t>
-        </is>
-      </c>
-      <c r="S176" t="inlineStr">
-        <is>
           <t>{2021: 134037.461587914, 2022: 131933.9211818031, 2023: 130058.37787509896, 2024: 128182.83456839435, 2025: 126307.29126168974, 2026: 124431.74795498513, 2027: 122556.20464828052, 2028: 120680.6613415759, 2029: 118805.11803487176, 2030: 116929.57472816715, 2031: 115054.03142146254, 2032: 113178.48811475793, 2033: 111302.94480805332, 2034: 109427.40150134871, 2035: 107551.85819464456, 2036: 105676.31488793995, 2037: 103800.77158123534, 2038: 101925.22827453073, 2039: 100049.68496782612, 2040: 98174.14166112198, 2041: 96298.59835441737, 2042: 94423.05504771275, 2043: 92547.51174100814, 2044: 90671.96843430353, 2045: 88796.42512759892, 2046: 86920.88182089478, 2047: 85045.33851419017, 2048: 83169.79520748556, 2049: 81294.25190078095, 2050: 79418.70859407634}</t>
         </is>
       </c>
-      <c r="T176" t="n">
+      <c r="S176" t="n">
         <v>3091922.508247175</v>
       </c>
     </row>
@@ -13168,15 +12288,10 @@
       </c>
       <c r="R177" t="inlineStr">
         <is>
-          <t>{2021: 23761.3196384102, 2022: 18890.62181327784, 2023: 15018.34064449144, 2024: 11939.816377852032, 2025: 9492.341298644915, 2026: 7546.560221570979, 2027: 5999.633745357159, 2028: 4769.802932936127, 2029: 3792.0681469351443, 2030: 3014.7536561114152, 2031: 2396.7764435834083, 2032: 1905.4748665355085, 2033: 1514.8824066253214, 2034: 1204.3552744809513, 2035: 957.4813337500424, 2036: 761.2126786050462, 2037: 605.1760192542171, 2038: 481.1244276061282, 2039: 382.50146647348595, 2040: 304.09466545344804, 2041: 241.76002881718242, 2042: 192.2030149609196, 2043: 152.80441163416137, 2044: 121.4819040149281, 2045: 96.58001915824859, 2046: 76.78263010646789, 2047: 61.043395284553064, 2048: 48.53045672828941, 2049: 38.58247430827871, 2050: 30.673672248405758}</t>
-        </is>
-      </c>
-      <c r="S177" t="inlineStr">
-        <is>
           <t>{2021: 23761.3196384102, 2022: 20528.280543173198, 2023: 18552.81049216492, 2024: 16577.340441156644, 2025: 14601.870390148368, 2026: 12626.400339140091, 2027: 10650.930288131814, 2028: 8675.460237123538, 2029: 6699.990186115261, 2030: 4724.5201351069845, 2031: 2749.050084098708, 2032: 773.5800330904312, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T177" t="n">
+      <c r="S177" t="n">
         <v>129040.8929886551</v>
       </c>
     </row>
@@ -13240,15 +12355,10 @@
       </c>
       <c r="R178" t="inlineStr">
         <is>
-          <t>{2021: 37555.3370470512, 2022: 29269.816488625467, 2023: 22812.26117620691, 2024: 17779.382394614917, 2025: 13856.865651864471, 2026: 10799.741038922637, 2027: 8417.084313153919, 2028: 6560.09325403319, 2029: 5112.794632977418, 2030: 3984.801426859476, 2031: 3105.667947052756, 2032: 2420.4903492399326, 2033: 1886.4777660224624, 2034: 1470.279921923512, 2035: 1145.9043343878286, 2036: 893.0930253410098, 2037: 696.0573653287241, 2038: 542.4920384339246, 2039: 422.8065478844661, 2040: 329.5262681643079, 2041: 256.8256379983203, 2042: 200.16434107266866, 2043: 156.003753166254, 2044: 121.58594718487853, 2045: 94.76145447019849, 2046: 73.85502569349809, 2047: 57.56100780304792, 2048: 44.861803082335534, 2049: 34.96431790570004, 2050: 27.250432274582874}</t>
-        </is>
-      </c>
-      <c r="S178" t="inlineStr">
-        <is>
           <t>{2021: 37555.3370470512, 2022: 37915.44006904075, 2023: 36801.94996392075, 2024: 35688.459858801216, 2025: 34574.96975368122, 2026: 33461.47964856168, 2027: 32347.989543441683, 2028: 31234.49943832215, 2029: 30121.009333202615, 2030: 29007.519228082616, 2031: 27894.029122963082, 2032: 26780.539017843083, 2033: 25667.04891272355, 2034: 24553.55880760355, 2035: 23440.068702484015, 2036: 22326.578597364016, 2037: 21213.088492244482, 2038: 20099.59838712495, 2039: 18986.10828200495, 2040: 17872.618176885415, 2041: 16759.128071765415, 2042: 15645.637966645882, 2043: 14532.147861525882, 2044: 13418.657756406348, 2045: 12305.167651286349, 2046: 11191.677546166815, 2047: 10078.187441046815, 2048: 8964.697335927282, 2049: 7851.207230807748, 2050: 6737.717125687748}</t>
         </is>
       </c>
-      <c r="T178" t="n">
+      <c r="S178" t="n">
         <v>662879.5892842438</v>
       </c>
     </row>
@@ -13312,15 +12422,10 @@
       </c>
       <c r="R179" t="inlineStr">
         <is>
-          <t>{2021: 63258.8422269992, 2022: 49498.95691038136, 2023: 38732.083120074174, 2024: 30307.189412827902, 2025: 23714.854872573887, 2026: 18556.466387120698, 2027: 14520.116046527899, 2028: 11361.741271547704, 2029: 8890.367288246205, 2030: 6956.55961800928, 2031: 5443.3883494215015, 2032: 4259.357836294506, 2033: 3332.8743078805833, 2034: 2607.9168689414682, 2035: 2040.6501316980239, 2036: 1596.7736585443376, 2037: 1249.4479465225509, 2038: 977.6715458173194, 2039: 765.0111828676928, 2040: 598.6081035255792, 2041: 468.4005536536883, 2042: 366.5153835554562, 2043: 286.79198889701246, 2044: 224.4098026599183, 2045: 175.5968139959018, 2046: 137.40148923992902, 2047: 107.51430402257145, 2048: 84.12809521498825, 2049: 65.8287887257892, 2050: 51.50989587997413}</t>
-        </is>
-      </c>
-      <c r="S179" t="inlineStr">
-        <is>
           <t>{2021: 63258.8422269992, 2022: 58324.06329756882, 2023: 54860.98519458622, 2024: 51397.907091603614, 2025: 47934.82898862101, 2026: 44471.75088563748, 2027: 41008.672782654874, 2028: 37545.59467967227, 2029: 34082.51657668967, 2030: 30619.438473706134, 2031: 27156.36037072353, 2032: 23693.282267740928, 2033: 20230.204164758325, 2034: 16767.12606177479, 2035: 13304.047958792187, 2036: 9840.969855809584, 2037: 6377.891752826981, 2038: 2914.813649843447, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T179" t="n">
+      <c r="S179" t="n">
         <v>552159.8751665095</v>
       </c>
     </row>
@@ -13384,15 +12489,10 @@
       </c>
       <c r="R180" t="inlineStr">
         <is>
-          <t>{2021: 176132.127440084, 2022: 132237.51858305844, 2023: 99282.0649767789, 2024: 74539.57493812323, 2025: 55963.262178880126, 2026: 42016.428404668455, 2027: 31545.342196846846, 2028: 23683.798268907587, 2029: 17781.461901477727, 2030: 13350.07095415054, 2031: 10023.045094286794, 2032: 7525.160975333476, 2033: 5649.784788153875, 2034: 4241.778781488511, 2035: 3184.667718461088, 2036: 2391.0036330204666, 2037: 1795.13182489243, 2038: 1347.7596705575734, 2039: 1011.8789630896932, 2040: 759.7044623837726, 2041: 570.3754018203249, 2042: 428.2298118677549, 2043: 321.50890656757326, 2044: 241.38435517001878, 2045: 181.2279713893388, 2046: 136.06340639086446, 2047: 102.15448761445779, 2048: 76.69614936579362, 2049: 57.58238786083056, 2050: 43.23204514402833}</t>
-        </is>
-      </c>
-      <c r="S180" t="inlineStr">
-        <is>
           <t>{2021: 176132.127440084, 2022: 165177.95761501323, 2023: 161323.68943696935, 2024: 157469.42125892546, 2025: 153615.15308088064, 2026: 149760.88490283675, 2027: 145906.61672479287, 2028: 142052.34854674898, 2029: 138198.0803687051, 2030: 134343.8121906612, 2031: 130489.54401261639, 2032: 126635.2758345725, 2033: 122781.00765652861, 2034: 118926.73947848473, 2035: 115072.47130044084, 2036: 111218.20312239695, 2037: 107363.93494435307, 2038: 103509.66676630825, 2039: 99655.39858826436, 2040: 95801.13041022047, 2041: 91946.86223217659, 2042: 88092.5940541327, 2043: 84238.32587608881, 2044: 80384.05769804493, 2045: 76529.78952000011, 2046: 72675.52134195622, 2047: 68821.25316391233, 2048: 64966.98498586845, 2049: 61112.71680782456, 2050: 57258.44862978067}</t>
         </is>
       </c>
-      <c r="T180" t="n">
+      <c r="S180" t="n">
         <v>3284764.729954657</v>
       </c>
     </row>
@@ -13456,15 +12556,10 @@
       </c>
       <c r="R181" t="inlineStr">
         <is>
-          <t>{2021: 62672.5396044912, 2022: 48025.069336945126, 2023: 36800.92269075858, 2024: 28200.019897719067, 2025: 21609.271292305166, 2026: 16558.875046120585, 2027: 12688.828747810363, 2028: 9723.267706460487, 2029: 7450.800761087736, 2030: 5709.441893134322, 2031: 4375.063536971872, 2032: 3352.548517142866, 2033: 2569.0099046141218, 2034: 1968.5954897470056, 2035: 1508.5065243585943, 2036: 1155.946940793253, 2037: 885.7855821985445, 2038: 678.7648030733851, 2039: 520.1277455292593, 2040: 398.56644075297027, 2041: 305.4157542256217, 2042: 234.0357174903723, 2043: 179.3382178339457, 2044: 137.42430736957417, 2045: 105.30627818267804, 2046: 80.69469249617465, 2047: 61.835186936872404, 2048: 47.38341798252982, 2049: 36.309234449298984, 2050: 27.823246241548834}</t>
-        </is>
-      </c>
-      <c r="S181" t="inlineStr">
-        <is>
           <t>{2021: 62672.5396044912, 2022: 59526.92461933382, 2023: 57518.573754691985, 2024: 55510.22289005015, 2025: 53501.87202540785, 2026: 51493.52116076602, 2027: 49485.17029612372, 2028: 47476.81943148188, 2029: 45468.46856683958, 2030: 43460.11770219775, 2031: 41451.76683755545, 2032: 39443.415972913615, 2033: 37435.06510827178, 2034: 35426.71424362948, 2035: 33418.36337898765, 2036: 31410.012514345348, 2037: 29401.661649703514, 2038: 27393.310785061214, 2039: 25384.95992041938, 2040: 23376.609055777546, 2041: 21368.258191135246, 2042: 19359.907326493412, 2043: 17351.556461851113, 2044: 15343.205597209278, 2045: 13334.854732566979, 2046: 11326.503867925145, 2047: 9318.153003282845, 2048: 7309.802138641011, 2049: 5301.451273999177, 2050: 3293.100409356877}</t>
         </is>
       </c>
-      <c r="T181" t="n">
+      <c r="S181" t="n">
         <v>940580.0825135859</v>
       </c>
     </row>
@@ -13528,15 +12623,10 @@
       </c>
       <c r="R182" t="inlineStr">
         <is>
-          <t>{2021: 36625.9984524092, 2022: 28031.98920484582, 2023: 21454.498224850562, 2024: 16420.3649878884, 2025: 12567.452452612613, 2026: 9618.596253199941, 2027: 7361.6665136328975, 2028: 5634.3080041346475, 2029: 4312.260902700107, 2030: 3300.4220002367397, 2031: 2526.003325268701, 2032: 1933.296044812102, 2033: 1479.662975696411, 2034: 1132.4714223266037, 2035: 866.7457005084756, 2036: 663.3704785296285, 2037: 507.71569045738204, 2038: 388.5841029706043, 2039: 297.4058275517175, 2040: 227.62183420666835, 2041: 174.2121189558676, 2042: 133.33458319968244, 2043: 102.04864726739652, 2044: 78.10371592424423, 2045: 59.77727882262667, 2046: 45.750999439053025, 2047: 35.01587879038642, 2048: 26.799671755726195, 2049: 20.51133460091412, 2050: 15.69850746477014}</t>
-        </is>
-      </c>
-      <c r="S182" t="inlineStr">
-        <is>
           <t>{2021: 36625.9984524092, 2022: 35943.068436298054, 2023: 35088.870224009734, 2024: 34234.67201172141, 2025: 33380.47379943309, 2026: 32526.275587144773, 2027: 31672.07737485622, 2028: 30817.8791625679, 2029: 29963.68095027958, 2030: 29109.48273799126, 2031: 28255.284525702707, 2032: 27401.086313414387, 2033: 26546.888101126067, 2034: 25692.689888837747, 2035: 24838.491676549427, 2036: 23984.293464260874, 2037: 23130.095251972554, 2038: 22275.897039684234, 2039: 21421.698827395914, 2040: 20567.500615107594, 2041: 19713.30240281904, 2042: 18859.10419053072, 2043: 18004.9059782424, 2044: 17150.70776595408, 2045: 16296.50955366576, 2046: 15442.311341377208, 2047: 14588.113129088888, 2048: 13733.914916800568, 2049: 12879.716704512248, 2050: 12025.518492223928}</t>
         </is>
       </c>
-      <c r="T182" t="n">
+      <c r="S182" t="n">
         <v>707844.750443661</v>
       </c>
     </row>
@@ -13600,15 +12690,10 @@
       </c>
       <c r="R183" t="inlineStr">
         <is>
-          <t>{2021: 168389.147393076, 2022: 135031.58072751047, 2023: 108282.08394693685, 2024: 86831.61109957073, 2025: 69630.43572232967, 2026: 55836.780148208665, 2027: 44775.621249194104, 2028: 35905.656682383065, 2029: 28792.815059296663, 2030: 23089.013699772222, 2031: 18515.124434008434, 2032: 14847.313846506913, 2033: 11906.089491452109, 2034: 9547.516031784871, 2035: 7656.171444254079, 2036: 6139.498586718093, 2037: 4923.275709114669, 2038: 3947.9842475076557, 2039: 3165.8961511565335, 2040: 2538.738204498958, 2041: 2035.819042462306, 2042: 1632.5272004444828, 2043: 1309.1266977086689, 2044: 1049.791213394172, 2045: 841.8295904044417, 2046: 675.0647654872479, 2047: 541.3357320730597, 2048: 434.0981633185409, 2049: 348.10415095801983, 2050: 279.1453872733496}</t>
-        </is>
-      </c>
-      <c r="S183" t="inlineStr">
-        <is>
           <t>{2021: 168389.147393076, 2022: 173015.2177704759, 2023: 164490.63727303594, 2024: 155966.056775596, 2025: 147441.47627815604, 2026: 138916.8957807161, 2027: 130392.31528327242, 2028: 121867.73478583246, 2029: 113343.15428839251, 2030: 104818.57379095256, 2031: 96293.99329351261, 2032: 87769.41279607266, 2033: 79244.83229863271, 2034: 70720.25180119276, 2035: 62195.67130375281, 2036: 53671.090806309134, 2037: 45146.51030886918, 2038: 36621.92981142923, 2039: 28097.34931398928, 2040: 19572.76881654933, 2041: 11048.18831910938, 2042: 2523.6078216694295, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T183" t="n">
+      <c r="S183" t="n">
         <v>1927352.242414056</v>
       </c>
     </row>
@@ -13672,15 +12757,10 @@
       </c>
       <c r="R184" t="inlineStr">
         <is>
-          <t>{2021: 211306.066490469, 2022: 161761.05530932738, 2023: 123832.88113485149, 2024: 94797.73991851576, 2025: 72570.47894954747, 2026: 55554.85204070854, 2027: 42528.885435780416, 2028: 32557.122014912075, 2029: 24923.441633438655, 2030: 19079.633100582614, 2031: 14606.024505236945, 2032: 11181.344563752002, 2033: 8559.65058859925, 2034: 6552.66616471408, 2035: 5016.260117367157, 2036: 3840.095761415356, 2037: 2939.7070948904425, 2038: 2250.4328903933483, 2039: 1722.7730623118075, 2040: 1318.8338283255562, 2041: 1009.6063752017488, 2042: 772.8835968229339, 2043: 591.665295416332, 2044: 452.9373158378668, 2045: 346.736936689947, 2046: 265.43739952785086, 2047: 203.20019476641684, 2048: 155.55577031177683, 2049: 119.08255159452955, 2050: 91.16122189387012}</t>
-        </is>
-      </c>
-      <c r="S184" t="inlineStr">
-        <is>
           <t>{2021: 211306.066490469, 2022: 209882.24599868804, 2023: 205550.52451353706, 2024: 201218.8030283861, 2025: 196887.0815432351, 2026: 192555.360058086, 2027: 188223.63857293501, 2028: 183891.91708778404, 2029: 179560.19560263306, 2030: 175228.47411748394, 2031: 170896.75263233297, 2032: 166565.031147182, 2033: 162233.309662031, 2034: 157901.5881768819, 2035: 153569.86669173092, 2036: 149238.14520657994, 2037: 144906.42372142896, 2038: 140574.70223627985, 2039: 136242.98075112887, 2040: 131911.2592659779, 2041: 127579.53778082691, 2042: 123247.8162956778, 2043: 118916.09481052682, 2044: 114584.37332537584, 2045: 110252.65184022486, 2046: 105920.93035507575, 2047: 101589.20886992477, 2048: 97257.48738477379, 2049: 92925.76589962281, 2050: 88594.04441447183}</t>
         </is>
       </c>
-      <c r="T184" t="n">
+      <c r="S184" t="n">
         <v>4389262.222028823</v>
       </c>
     </row>
@@ -13744,15 +12824,10 @@
       </c>
       <c r="R185" t="inlineStr">
         <is>
-          <t>{2021: 42381.5768764867, 2022: 32482.654405697245, 2023: 24895.789987119257, 2024: 19080.963992094144, 2025: 14624.287361677018, 2026: 11208.541713380899, 2027: 8590.60029617696, 2028: 6584.122657149433, 2029: 5046.291256698404, 2030: 3867.6459679528107, 2031: 2964.292897990303, 2032: 2271.932968499395, 2033: 1741.285220787031, 2034: 1334.5790840537065, 2035: 1022.8659327784349, 2036: 783.9585746097264, 2037: 600.8520051446875, 2038: 460.51302170668606, 2039: 352.95254296497666, 2040: 270.51460374293066, 2041: 207.3314169192887, 2042: 158.90571468965754, 2043: 121.79064097584752, 2044: 93.34441028931226, 2045: 71.54227009928775, 2046: 54.8323825186293, 2047: 42.025367219920156, 2048: 32.20964344142982, 2049: 24.68654527621316, 2050: 18.920591865063784}</t>
-        </is>
-      </c>
-      <c r="S185" t="inlineStr">
-        <is>
           <t>{2021: 42381.5768764867, 2022: 40477.351177245844, 2023: 39169.29830239108, 2024: 37861.24542753631, 2025: 36553.19255268201, 2026: 35245.13967782725, 2027: 33937.08680297248, 2028: 32629.03392811818, 2029: 31320.981053263415, 2030: 30012.92817840865, 2031: 28704.87530355435, 2032: 27396.822428699583, 2033: 26088.769553844817, 2034: 24780.716678990517, 2035: 23472.66380413575, 2036: 22164.610929280985, 2037: 20856.55805442622, 2038: 19548.50517957192, 2039: 18240.452304717153, 2040: 16932.399429862387, 2041: 15624.346555008087, 2042: 14316.293680153321, 2043: 13008.240805298556, 2044: 11700.187930444255, 2045: 10392.13505558949, 2046: 9084.082180734724, 2047: 7776.029305880424, 2048: 6467.976431025658, 2049: 5159.923556170892, 2050: 3851.870681316592}</t>
         </is>
       </c>
-      <c r="T185" t="n">
+      <c r="S185" t="n">
         <v>662038.5700467359</v>
       </c>
     </row>
@@ -13816,15 +12891,10 @@
       </c>
       <c r="R186" t="inlineStr">
         <is>
-          <t>{2021: 43101.3112244717, 2022: 33128.75003931215, 2023: 25463.589111045134, 2024: 19571.95395681155, 2025: 15043.495244014677, 2026: 11562.808172146324, 2027: 8887.464692026817, 2028: 6831.128517923126, 2029: 5250.576901897166, 2030: 4035.7252436992267, 2031: 3101.9597554596803, 2032: 2384.2441552516634, 2033: 1832.589923788136, 2034: 1408.5746299817686, 2035: 1082.665828548806, 2036: 832.164140513055, 2037: 639.6222532339898, 2038: 491.6297241309783, 2039: 377.87895031332226, 2040: 290.44724938530334, 2041: 223.2450487266915, 2042: 171.59174991830596, 2043: 131.88972748987166, 2044: 101.37375617204353, 2045: 77.91841439067429, 2046: 59.89004975659717, 2047: 46.032996024069234, 2048: 35.38211658804893, 2049: 27.195583220255966, 2050: 20.903208117845736}</t>
-        </is>
-      </c>
-      <c r="S186" t="inlineStr">
-        <is>
           <t>{2021: 43101.3112244717, 2022: 41553.54124577576, 2023: 40234.05496354867, 2024: 38914.56868132157, 2025: 37595.08239909494, 2026: 36275.59611686785, 2027: 34956.10983464122, 2028: 33636.62355241412, 2029: 32317.137270187028, 2030: 30997.6509879604, 2031: 29678.164705733303, 2032: 28358.678423506673, 2033: 27039.19214127958, 2034: 25719.705859052483, 2035: 24400.219576825853, 2036: 23080.73329459876, 2037: 21761.24701237213, 2038: 20441.760730145033, 2039: 19122.27444791794, 2040: 17802.78816569131, 2041: 16483.301883464213, 2042: 15163.815601237584, 2043: 13844.329319010489, 2044: 12524.843036783393, 2045: 11205.356754556764, 2046: 9885.870472329669, 2047: 8566.38419010304, 2048: 7246.897907875944, 2049: 5927.411625648849, 2050: 4607.925343422219}</t>
         </is>
       </c>
-      <c r="T186" t="n">
+      <c r="S186" t="n">
         <v>688587.9584838916</v>
       </c>
     </row>
@@ -13888,15 +12958,10 @@
       </c>
       <c r="R187" t="inlineStr">
         <is>
-          <t>{2021: 51343.2670589828, 2022: 39637.79099656717, 2023: 30600.983635938283, 2024: 23624.429513946958, 2025: 18238.4225454763, 2026: 14080.342416351694, 2027: 10870.240672808975, 2028: 8391.992807473716, 2029: 6478.747380161912, 2030: 5001.6925155814715, 2031: 3861.383466968658, 2032: 2981.047361973929, 2033: 2301.4143636213616, 2034: 1776.7272471563767, 2035: 1371.6607320641715, 2036: 1058.9431590572242, 2037: 817.5203881695958, 2038: 631.1382998762545, 2039: 487.24846417904087, 2040: 376.1633003279672, 2041: 290.40384714611287, 2042: 224.19623169972687, 2043: 173.082935375398, 2044: 133.62268531920515, 2045: 103.15876601693704, 2046: 79.64015227441074, 2047: 61.48342113020218, 2048: 47.466145730718495, 2049: 36.644593763879854, 2050: 28.290189385458152}</t>
-        </is>
-      </c>
-      <c r="S187" t="inlineStr">
-        <is>
           <t>{2021: 51343.2670589828, 2022: 49523.17784818821, 2023: 47794.17980670743, 2024: 46065.18176522618, 2025: 44336.183723744936, 2026: 42607.18568226369, 2027: 40878.18764078291, 2028: 39149.189599301666, 2029: 37420.19155782042, 2030: 35691.193516339175, 2031: 33962.195474858396, 2032: 32233.19743337715, 2033: 30504.199391895905, 2034: 28775.20135041466, 2035: 27046.20330893388, 2036: 25317.205267452635, 2037: 23588.20722597139, 2038: 21859.209184490144, 2039: 20130.211143009365, 2040: 18401.21310152812, 2041: 16672.215060046874, 2042: 14943.217018565629, 2043: 13214.218977084849, 2044: 11485.220935603604, 2045: 9756.222894122358, 2046: 8027.224852641113, 2047: 6298.226811160333, 2048: 4569.228769679088, 2049: 2840.230728197843, 2050: 1111.2326867170632}</t>
         </is>
       </c>
-      <c r="T187" t="n">
+      <c r="S187" t="n">
         <v>759314.9699422579</v>
       </c>
     </row>
@@ -13960,15 +13025,10 @@
       </c>
       <c r="R188" t="inlineStr">
         <is>
-          <t>{2021: 497032.578523585, 2022: 374249.58817610744, 2023: 281797.93498856097, 2024: 212184.80573571104, 2025: 159768.35240800836, 2026: 120300.44442938872, 2027: 90582.37574454096, 2028: 68205.62329959874, 2029: 51356.64649386419, 2030: 38669.907428457576, 2031: 29117.199868261177, 2032: 21924.317500288507, 2033: 16508.307805291788, 2034: 12430.226235807408, 2035: 9359.561627741516, 2036: 7047.449676429904, 2037: 5306.503543349883, 2038: 3995.6269499535665, 2039: 3008.5789244789335, 2040: 2265.3634231103592, 2041: 1705.7459909100082, 2042: 1284.3720154670402, 2043: 967.0909284886002, 2044: 728.1884475074376, 2045: 548.3025426698987, 2046: 412.85422657739326, 2047: 310.8659893730145, 2048: 234.07211826314574, 2049: 176.24879665576, 2050: 132.7096903001555}</t>
-        </is>
-      </c>
-      <c r="S188" t="inlineStr">
-        <is>
           <t>{2021: 497032.578523585, 2022: 484743.9525061697, 2023: 477651.57442601956, 2024: 470559.19634586945, 2025: 463466.81826571934, 2026: 456374.44018556736, 2027: 449282.06210541725, 2028: 442189.68402526714, 2029: 435097.305945117, 2030: 428004.9278649669, 2031: 420912.54978481494, 2032: 413820.1717046648, 2033: 406727.7936245147, 2034: 399635.4155443646, 2035: 392543.0374642145, 2036: 385450.6593840625, 2037: 378358.2813039124, 2038: 371265.9032237623, 2039: 364173.5251436122, 2040: 357081.14706346206, 2041: 349988.7689833101, 2042: 342896.39090316, 2043: 335804.01282300986, 2044: 328711.63474285975, 2045: 321619.25666270964, 2046: 314526.87858255766, 2047: 307434.50050240755, 2048: 300342.12242225744, 2049: 293249.7443421073, 2050: 286157.3662619572}</t>
         </is>
       </c>
-      <c r="T188" t="n">
+      <c r="S188" t="n">
         <v>11283506.72826865</v>
       </c>
     </row>
@@ -14032,15 +13092,10 @@
       </c>
       <c r="R189" t="inlineStr">
         <is>
-          <t>{2021: 15746.9656758898, 2022: 12159.130166090206, 2023: 9388.757773333416, 2024: 7249.5952689248215, 2025: 5597.825913934223, 2026: 4322.400603111304, 2027: 3337.5719897381045, 2028: 2577.129657687475, 2029: 1989.9487690312023, 2030: 1536.5529210207123, 2031: 1186.4601319594387, 2032: 916.1335255502298, 2033: 707.3989374181402, 2034: 546.2230588709934, 2035: 421.7699720207888, 2036: 325.67264675003565, 2037: 251.4704219767114, 2038: 194.17465286141166, 2039: 149.93332224710477, 2040: 115.77206802629807, 2041: 89.39421560336044, 2042: 69.02637155557098, 2043: 53.29919769382287, 2044: 41.15534991605593, 2045: 31.778392546222246, 2046: 24.537909041755338, 2047: 18.94711884075569, 2048: 14.630150912811374, 2049: 11.296773801366982, 2050: 8.722883248422223}</t>
-        </is>
-      </c>
-      <c r="S189" t="inlineStr">
-        <is>
           <t>{2021: 15746.9656758898, 2022: 14933.135255242698, 2023: 14336.827159343753, 2024: 13740.519063444808, 2025: 13144.210967545863, 2026: 12547.902871646918, 2027: 11951.594775747973, 2028: 11355.286679849029, 2029: 10758.978583950317, 2030: 10162.670488051372, 2031: 9566.362392152427, 2032: 8970.054296253482, 2033: 8373.746200354537, 2034: 7777.438104455592, 2035: 7181.130008556647, 2036: 6584.821912657702, 2037: 5988.51381675899, 2038: 5392.205720860045, 2039: 4795.8976249611005, 2040: 4199.589529062156, 2041: 3603.2814331632107, 2042: 3006.973337264266, 2043: 2410.665241365321, 2044: 1814.357145466376, 2045: 1218.049049567664, 2046: 621.7409536687192, 2047: 25.432857769774273, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T189" t="n">
+      <c r="S189" t="n">
         <v>202334.8683071056</v>
       </c>
     </row>
@@ -14104,15 +13159,10 @@
       </c>
       <c r="R190" t="inlineStr">
         <is>
-          <t>{2021: 31112.2751602701, 2022: 23740.262210919627, 2023: 18115.038097982855, 2024: 13822.703488945943, 2025: 10547.431957352277, 2026: 8048.23173584977, 2027: 6141.213741491595, 2028: 4686.061169274114, 2029: 3575.7050978077777, 2030: 2728.4464467349385, 2031: 2081.9446260444133, 2032: 1588.6305670768013, 2033: 1212.2066298399818, 2034: 924.9758527131299, 2035: 705.8040329438909, 2036: 538.5646895090993, 2037: 410.9524899939054, 2038: 313.5778344215743, 2039: 239.27597626183643, 2040: 182.57984631363962, 2041: 139.31779028009794, 2042: 106.30662189948058, 2043: 81.11740673576794, 2044: 61.89674319402072, 2045: 47.23039076565077, 2046: 36.039211382797916, 2047: 27.499767332828966, 2048: 20.983733393253193, 2049: 16.01166518210802, 2050: 12.217722037316813}</t>
-        </is>
-      </c>
-      <c r="S190" t="inlineStr">
-        <is>
           <t>{2021: 31112.2751602701, 2022: 29856.788370328024, 2023: 29026.15760140377, 2024: 28195.52683247975, 2025: 27364.89606355573, 2026: 26534.265294631477, 2027: 25703.634525707457, 2028: 24873.003756783204, 2029: 24042.372987859184, 2030: 23211.742218935164, 2031: 22381.11145001091, 2032: 21550.48068108689, 2033: 20719.84991216287, 2034: 19889.219143238617, 2035: 19058.588374314597, 2036: 18227.957605390344, 2037: 17397.326836466324, 2038: 16566.696067542303, 2039: 15736.06529861805, 2040: 14905.43452969403, 2041: 14074.80376077001, 2042: 13244.172991845757, 2043: 12413.542222921737, 2044: 11582.911453997483, 2045: 10752.280685073463, 2046: 9921.649916149443, 2047: 9091.01914722519, 2048: 8260.38837830117, 2049: 7429.7576093771495, 2050: 6599.126840452896}</t>
         </is>
       </c>
-      <c r="T190" t="n">
+      <c r="S190" t="n">
         <v>540867.3447162316</v>
       </c>
     </row>
@@ -14176,15 +13226,10 @@
       </c>
       <c r="R191" t="inlineStr">
         <is>
-          <t>{2021: 131967.22007073794, 2022: 98629.10709729319, 2023: 73713.00813637678, 2024: 55091.318662689904, 2025: 41173.91853523165, 2026: 30772.390436426653, 2027: 22998.540019007567, 2028: 17188.552319282004, 2029: 12846.308095579878, 2030: 9601.01983117183, 2031: 7175.569907923328, 2032: 5362.847323398397, 2033: 4008.062325798562, 2034: 2995.5288000453065, 2035: 2238.7857429619853, 2036: 1673.2142928534145, 2037: 1250.519876057872, 2038: 934.6082967944114, 2039: 698.5036265001571, 2040: 522.0447088981898, 2041: 390.1635836224741, 2042: 291.59882169176257, 2043: 217.93390357594222, 2044: 162.87852623099192, 2045: 121.7314693669742, 2046: 90.97915469364662, 2047: 67.99561881421013, 2048: 50.818280225791476, 2049: 37.98035300132257, 2050: 28.385596830428845}</t>
-        </is>
-      </c>
-      <c r="S191" t="inlineStr">
-        <is>
           <t>{2021: 131967.22007073794, 2022: 120830.91176124662, 2023: 117564.64772975165, 2024: 114298.38369825762, 2025: 111032.11966676265, 2026: 107765.85563526861, 2027: 104499.59160377365, 2028: 101233.32757227961, 2029: 97967.06354078557, 2030: 94700.7995092906, 2031: 91434.53547779657, 2032: 88168.2714463016, 2033: 84902.00741480757, 2034: 81635.7433833126, 2035: 78369.47935181856, 2036: 75103.2153203236, 2037: 71836.95128882956, 2038: 68570.68725733552, 2039: 65304.423225840554, 2040: 62038.15919434652, 2041: 58771.89516285155, 2042: 55505.63113135751, 2043: 52239.367099862546, 2044: 48973.10306836851, 2045: 45706.83903687354, 2046: 42440.575005379505, 2047: 39174.31097388454, 2048: 35908.0469423905, 2049: 32641.782910896465, 2050: 29375.518879401498}</t>
         </is>
       </c>
-      <c r="T191" t="n">
+      <c r="S191" t="n">
         <v>2229289.094885064</v>
       </c>
     </row>
@@ -14248,15 +13293,10 @@
       </c>
       <c r="R192" t="inlineStr">
         <is>
-          <t>{2021: 71079.1096970575, 2022: 52883.91953055864, 2023: 39346.42621206577, 2024: 29274.328934090307, 2025: 21780.538082986506, 2026: 16205.045733157373, 2027: 12056.796127495587, 2028: 8970.436446381424, 2029: 6674.138733677249, 2030: 4965.658928929768, 2031: 3694.524429652403, 2032: 2748.781371547047, 2033: 2045.134406994555, 2034: 1521.6105529407632, 2035: 1132.1009841221942, 2036: 842.3000456808309, 2037: 626.6838178787003, 2038: 466.26212310552387, 2039: 346.90598550759154, 2040: 258.1032359640273, 2041: 192.03266359797232, 2042: 142.87517066880775, 2043: 106.30126152068073, 2044: 79.08972670333367, 2045: 58.84393826117546, 2046: 43.78076918982554, 2047: 32.573546358256415, 2048: 24.23520513659819, 2049: 18.031354693564733, 2050: 13.41559727894161}</t>
-        </is>
-      </c>
-      <c r="S192" t="inlineStr">
-        <is>
           <t>{2021: 71079.1096970575, 2022: 62901.643468535505, 2023: 60780.43267293647, 2024: 58659.221877338365, 2025: 56538.01108173933, 2026: 54416.80028614029, 2027: 52295.58949054126, 2028: 50174.37869494315, 2029: 48053.16789934412, 2030: 45931.95710374508, 2031: 43810.746308146976, 2032: 41689.53551254794, 2033: 39568.324716948904, 2034: 37447.1139213508, 2035: 35325.90312575176, 2036: 33204.69233015273, 2037: 31083.481534554623, 2038: 28962.270738955587, 2039: 26841.05994335655, 2040: 24719.849147758447, 2041: 22598.63835215941, 2042: 20477.427556560375, 2043: 18356.21676096134, 2044: 16235.005965363234, 2045: 14113.795169764198, 2046: 11992.584374165162, 2047: 9871.373578567058, 2048: 7750.162782968022, 2049: 5628.951987368986, 2050: 3507.7411917708814}</t>
         </is>
       </c>
-      <c r="T192" t="n">
+      <c r="S192" t="n">
         <v>996721.7618270798</v>
       </c>
     </row>
@@ -14320,15 +13360,10 @@
       </c>
       <c r="R193" t="inlineStr">
         <is>
-          <t>{2021: 56168.719156538, 2022: 44262.702985836666, 2023: 34880.390812407306, 2024: 27486.836120595104, 2025: 21660.484367385685, 2026: 17069.137421684518, 2027: 13451.012792633866, 2028: 10599.817710632997, 2029: 8352.987037539518, 2030: 6582.414372967228, 2031: 5187.147876887935, 2032: 4087.6343499739382, 2033: 3221.1833893410026, 2034: 2538.393001769482, 2035: 2000.3328754127513, 2036: 1576.3247100302312, 2037: 1242.193047964167, 2038: 978.8868743806692, 2039: 771.3933952578332, 2040: 607.8820605536142, 2041: 479.03002775827264, 2042: 377.49060613025335, 2043: 297.4743741711614, 2044: 234.41908712819793, 2045: 184.72955380821827, 2046: 145.57265139216813, 2047: 114.71579071395416, 2048: 90.39962186081152, 2049: 71.23772221520015, 2050: 56.13754750239692}</t>
-        </is>
-      </c>
-      <c r="S193" t="inlineStr">
-        <is>
           <t>{2021: 56168.719156538, 2022: 50797.959167866036, 2023: 47141.92553534359, 2024: 43485.89190282021, 2025: 39829.85827029683, 2026: 36173.82463777438, 2027: 32517.791005250998, 2028: 28861.75737272855, 2029: 25205.72374020517, 2030: 21549.69010768179, 2031: 17893.65647515934, 2032: 14237.62284263596, 2033: 10581.58921011258, 2034: 6925.55557759013, 2035: 3269.52194506675, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T193" t="n">
+      <c r="S193" t="n">
         <v>406556.7273688013</v>
       </c>
     </row>
@@ -14392,15 +13427,10 @@
       </c>
       <c r="R194" t="inlineStr">
         <is>
-          <t>{2021: 112633.150159207, 2022: 89662.47909713068, 2023: 71376.50102549524, 2024: 56819.808574817296, 2025: 45231.8424144339, 2026: 36007.1534825786, 2027: 28663.7694312501, 2028: 22818.012493139435, 2029: 18164.45305234093, 2030: 14459.951531269478, 2031: 11510.954812906746, 2032: 9163.38346074306, 2033: 7294.581363004759, 2034: 5806.907185479878, 2035: 4622.632798613125, 2036: 3679.8821314461793, 2037: 2929.398265291497, 2038: 2331.969853969313, 2039: 1856.3824059889423, 2040: 1477.7873870879985, 2041: 1176.4039318574441, 2042: 936.4853313687435, 2043: 745.4962977589744, 2044: 593.458019422521, 2045: 472.42678719615594, 2046: 376.07895075318, 2047: 299.3805199722671, 2048: 238.32414858466305, 2049: 189.7197579985031, 2050: 151.02786179565072}</t>
-        </is>
-      </c>
-      <c r="S194" t="inlineStr">
-        <is>
           <t>{2021: 112633.150159207, 2022: 94380.5037884675, 2023: 84145.96594263613, 2024: 73911.4280968085, 2025: 63676.89025097713, 2026: 53442.35240514949, 2027: 43207.814559318125, 2028: 32973.27671348676, 2029: 22738.73886765912, 2030: 12504.201021827757, 2031: 2269.663175996393, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T194" t="n">
+      <c r="S194" t="n">
         <v>539567.4099019304</v>
       </c>
     </row>
@@ -14464,15 +13494,10 @@
       </c>
       <c r="R195" t="inlineStr">
         <is>
-          <t>{2021: 101943.766644076, 2022: 80706.00869481255, 2023: 63892.6739109817, 2024: 50582.03032852289, 2025: 40044.36871307485, 2026: 31701.9988168497, 2027: 25097.579541949242, 2028: 19869.046822677996, 2029: 15729.764736153895, 2030: 12452.811695644392, 2031: 9858.540272427159, 2032: 7804.728657148371, 2033: 6178.783849174875, 2034: 4891.569141209994, 2035: 3872.5175127194634, 2036: 3065.7630411433547, 2037: 2427.0782491155737, 2038: 1921.449488520489, 2039: 1521.1574403425193, 2040: 1204.257500461861, 2041: 953.3767438905592, 2042: 754.7615152430192, 2043: 597.5234329371598, 2044: 473.0424719575826, 2045: 374.49440129199695, 2046: 296.47666945987675, 2047: 234.71222862284066, 2048: 185.81506047495625, 2049: 147.10454969431316, 2050: 116.45852863300716}</t>
-        </is>
-      </c>
-      <c r="S195" t="inlineStr">
-        <is>
           <t>{2021: 101943.766644076, 2022: 87200.30110003054, 2023: 78900.8152080439, 2024: 70601.32931605354, 2025: 62301.8434240669, 2026: 54002.35753208026, 2027: 45702.871640093625, 2028: 37403.385748106986, 2029: 29103.899856120348, 2030: 20804.413964129984, 2031: 12504.928072143346, 2032: 4205.442180156708, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T195" t="n">
+      <c r="S195" t="n">
         <v>553703.4713630641</v>
       </c>
     </row>
@@ -14536,15 +13561,10 @@
       </c>
       <c r="R196" t="inlineStr">
         <is>
-          <t>{2021: 15392.0842487046, 2022: 11484.252573041518, 2023: 8568.563881951883, 2024: 6393.127156697976, 2025: 4770.002932206495, 2026: 3558.9669054870405, 2027: 2655.3957333717785, 2028: 1981.22845422866, 2029: 1478.2226763846777, 2030: 1102.9229245693466, 2031: 822.9064517638665, 2032: 613.9821861251182, 2033: 458.10082552026495, 2034: 341.79552938948535, 2035: 255.01849680790548, 2036: 190.2729208609839, 2037: 141.9653274807005, 2038: 105.92234625665648, 2039: 79.03016627803194, 2040: 58.965529018772855, 2041: 43.99501831024527, 2042: 32.825307740435775, 2043: 24.49142811251865, 2044: 18.273402209471737, 2045: 13.634044808454696, 2046: 10.172554388508935, 2047: 7.589887244833038, 2048: 5.66292262387432, 2049: 4.225186963853645, 2050: 3.1524719769709804}</t>
-        </is>
-      </c>
-      <c r="S196" t="inlineStr">
-        <is>
           <t>{2021: 15392.0842487046, 2022: 15926.314491379424, 2023: 16018.618740735255, 2024: 16110.922990091087, 2025: 16203.227239446918, 2026: 16295.53148880275, 2027: 16387.83573815858, 2028: 16480.139987514412, 2029: 16572.444236870244, 2030: 16664.748486226075, 2031: 16757.052735581907, 2032: 16849.356984937738, 2033: 16941.66123429357, 2034: 17033.9654836494, 2035: 17126.269733005232, 2036: 17218.573982361064, 2037: 17310.878231716895, 2038: 17403.182481072727, 2039: 17495.486730428558, 2040: 17587.79097978436, 2041: 17680.09522914019, 2042: 17772.399478496023, 2043: 17864.703727851855, 2044: 17957.007977207686, 2045: 18049.312226563517, 2046: 18141.61647591935, 2047: 18233.92072527518, 2048: 18326.22497463101, 2049: 18418.529223986843, 2050: 18510.833473342675}</t>
         </is>
       </c>
-      <c r="T196" t="n">
+      <c r="S196" t="n">
         <v>497779.2708761515</v>
       </c>
     </row>
@@ -14608,15 +13628,10 @@
       </c>
       <c r="R197" t="inlineStr">
         <is>
-          <t>{2021: 27416.5036901078, 2022: 20945.09556356734, 2023: 16001.202528433829, 2024: 12224.26899790898, 2025: 9338.845144150851, 2026: 7134.498483414291, 2027: 5450.467142794569, 2028: 4163.935579178411, 2029: 3181.0777045906766, 2030: 2430.2141976558933, 2031: 1856.5849674043784, 2032: 1418.355527885852, 2033: 1083.5660305366378, 2034: 827.8004487936939, 2035: 632.4059297832252, 2036: 483.13245131455454, 2037: 369.09357506059524, 2038: 281.9725041866739, 2039: 215.4155436172268, 2040: 164.56872830829158, 2041: 125.723826063044, 2042: 96.04789805703416, 2043: 73.37669406074602, 2044: 56.056814778884245, 2045: 42.82513028663682, 2046: 32.7166606112314, 2047: 24.994200236782515, 2048: 19.09455408361331, 2049: 14.587463979562347, 2050: 11.14423015186545}</t>
-        </is>
-      </c>
-      <c r="S197" t="inlineStr">
-        <is>
           <t>{2021: 27416.5036901078, 2022: 28058.804164221394, 2023: 27741.993497113, 2024: 27425.182830004604, 2025: 27108.37216289621, 2026: 26791.561495787813, 2027: 26474.75082867942, 2028: 26157.940161571023, 2029: 25841.129494462744, 2030: 25524.31882735435, 2031: 25207.508160245954, 2032: 24890.69749313756, 2033: 24573.886826029164, 2034: 24257.07615892077, 2035: 23940.265491812374, 2036: 23623.45482470398, 2037: 23306.644157595583, 2038: 22989.833490487188, 2039: 22673.022823378793, 2040: 22356.212156270398, 2041: 22039.401489162003, 2042: 21722.590822053724, 2043: 21405.78015494533, 2044: 21088.969487836934, 2045: 20772.15882072854, 2046: 20455.348153620143, 2047: 20138.53748651175, 2048: 19821.726819403353, 2049: 19504.916152294958, 2050: 19188.105485186563}</t>
         </is>
       </c>
-      <c r="T197" t="n">
+      <c r="S197" t="n">
         <v>689194.3890188762</v>
       </c>
     </row>
@@ -14680,15 +13695,10 @@
       </c>
       <c r="R198" t="inlineStr">
         <is>
-          <t>{2021: 59245.4924784036, 2022: 45597.458082756486, 2023: 35093.44081098873, 2024: 27009.171996368415, 2025: 20787.228469799596, 2026: 15998.597347365818, 2027: 12313.0949108969, 2028: 9476.599916411937, 2029: 7293.531530912009, 2030: 5613.363723447003, 2031: 4320.2462563112695, 2032: 3325.016627233661, 2033: 2559.05217329439, 2034: 1969.5384293735553, 2035: 1515.827486934557, 2036: 1166.6352561991732, 2037: 897.8843784917266, 2038: 691.044054133948, 2039: 531.8523143882534, 2040: 409.3326360714363, 2041: 315.03709285521103, 2042: 242.46385733421474, 2043: 186.60888970431617, 2044: 143.62090127386443, 2045: 110.53580199421776, 2046: 85.07232174519393, 2047: 65.47471313861168, 2048: 50.39168994850759, 2049: 38.78325378059628, 2050: 29.848984531916543}</t>
-        </is>
-      </c>
-      <c r="S198" t="inlineStr">
-        <is>
           <t>{2021: 59245.4924784036, 2022: 56778.17843033979, 2023: 54823.97018944053, 2024: 52869.76194854127, 2025: 50915.553707642015, 2026: 48961.34546674229, 2027: 47007.137225843035, 2028: 45052.92898494378, 2029: 43098.72074404452, 2030: 41144.5125031448, 2031: 39190.30426224554, 2032: 37236.09602134628, 2033: 35281.887780447025, 2034: 33327.6795395473, 2035: 31373.471298648044, 2036: 29419.263057748787, 2037: 27465.05481684953, 2038: 25510.846575949807, 2039: 23556.63833505055, 2040: 21602.430094151292, 2041: 19648.221853252035, 2042: 17694.01361235231, 2043: 15739.805371453054, 2044: 13785.597130553797, 2045: 11831.38888965454, 2046: 9877.180648754817, 2047: 7922.972407855559, 2048: 5968.764166956302, 2049: 4014.5559260570444, 2050: 2060.347685157787}</t>
         </is>
       </c>
-      <c r="T198" t="n">
+      <c r="S198" t="n">
         <v>881751.2010713364</v>
       </c>
     </row>
@@ -14752,15 +13762,10 @@
       </c>
       <c r="R199" t="inlineStr">
         <is>
-          <t>{2021: 1054375.11108919, 2022: 756218.1795724293, 2023: 542374.2737298589, 2024: 389001.297178967, 2025: 278999.23823136225, 2026: 200103.6384664509, 2027: 143518.1915955892, 2028: 102934.01697601611, 2029: 73826.2636465969, 2030: 52949.62116640967, 2031: 37976.490251319075, 2032: 27237.471771062414, 2033: 19535.24044928437, 2034: 14011.051488883133, 2035: 10048.996547228346, 2036: 7207.334273686045, 2037: 5169.239245780898, 2038: 3707.4781556448524, 2039: 2659.0748891730395, 2040: 1907.1398318193956, 2041: 1367.8374960109766, 2042: 981.0394519990061, 2043: 703.6204294627605, 2044: 504.65015219169965, 2045: 361.94482911980884, 2046: 259.59381713770625, 2047: 186.18569592499452, 2048: 133.53597458249854, 2049: 95.77457827308773, 2050: 68.69137602856877}</t>
-        </is>
-      </c>
-      <c r="S199" t="inlineStr">
-        <is>
           <t>{2021: 1054375.11108919, 2022: 894905.3654717505, 2023: 873238.5421475321, 2024: 851571.7188233212, 2025: 829904.8954991028, 2026: 808238.0721748918, 2027: 786571.2488506809, 2028: 764904.4255264625, 2029: 743237.6022022516, 2030: 721570.7788780406, 2031: 699903.9555538222, 2032: 678237.1322296113, 2033: 656570.3089054003, 2034: 634903.485581182, 2035: 613236.662256971, 2036: 591569.8389327526, 2037: 569903.0156085417, 2038: 548236.1922843307, 2039: 526569.3689601123, 2040: 504902.5456359014, 2041: 483235.72231169045, 2042: 461568.89898747206, 2043: 439902.0756632611, 2044: 418235.2523390427, 2045: 396568.4290148318, 2046: 374901.60569062084, 2047: 353234.78236640245, 2048: 331567.9590421915, 2049: 309901.13571798056, 2050: 288234.3123937622}</t>
         </is>
       </c>
-      <c r="T199" t="n">
+      <c r="S199" t="n">
         <v>17538595.72839763</v>
       </c>
     </row>
@@ -14824,15 +13829,10 @@
       </c>
       <c r="R200" t="inlineStr">
         <is>
-          <t>{2021: 1052156.51907693, 2022: 874836.7550489353, 2023: 727400.6615061348, 2024: 604811.9484074098, 2025: 502883.090838765, 2026: 418132.2867669247, 2027: 347664.52167904266, 2028: 289072.6773789971, 2029: 240355.3069018803, 2030: 199848.2668085409, 2031: 166167.8714782116, 2032: 138163.62759879293, 2033: 114878.93430566664, 2034: 95518.40651961118, 2035: 79420.70527716978, 2036: 66035.94696094538, 2037: 54906.91974857505, 2038: 45653.465650450045, 2039: 37959.49464003419, 2040: 31562.187290650512, 2041: 26243.017090103276, 2042: 21820.285763130905, 2043: 18142.916614730584, 2044: 15085.293880305095, 2045: 12542.97179927537, 2046: 10429.106837806954, 2047: 8671.491188449882, 2048: 7210.086213593341, 2049: 5994.971577286659, 2050: 4984.640009535113}</t>
-        </is>
-      </c>
-      <c r="S200" t="inlineStr">
-        <is>
           <t>{2021: 1052156.51907693, 2022: 861250.791710496, 2023: 707077.3713434935, 2024: 552903.9509764314, 2025: 398730.5306094289, 2026: 244557.1102424264, 2027: 90383.68987542391, 2028: 0, 2029: 0, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T200" t="n">
+      <c r="S200" t="n">
         <v>3380981.704296165</v>
       </c>
     </row>
@@ -14896,15 +13896,10 @@
       </c>
       <c r="R201" t="inlineStr">
         <is>
-          <t>{2021: 11281.0686929347, 2022: 8514.318111831511, 2023: 6426.129906900104, 2024: 4850.0825360250665, 2025: 3660.570350592667, 2026: 2762.793249827877, 2027: 2085.2014331752025, 2028: 1573.7931230238828, 2029: 1187.8108055516377, 2030: 896.4929946283796, 2031: 676.622645341662, 2032: 510.676833987896, 2033: 385.43024027848514, 2034: 290.9011340127714, 2035: 219.55586491805465, 2036: 165.70845618566315, 2037: 125.06745133720082, 2038: 94.39389964781051, 2039: 71.24322272065541, 2040: 53.77038985106318, 2041: 40.58287531533947, 2042: 30.629678777153707, 2043: 23.117564112984574, 2044: 17.447841174115442, 2045: 13.168652205280098, 2046: 9.938960308791316, 2047: 7.501369956457745, 2048: 5.661613435952032, 2049: 4.273068370739163, 2050: 3.22507241223209}</t>
-        </is>
-      </c>
-      <c r="S201" t="inlineStr">
-        <is>
           <t>{2021: 11281.0686929347, 2022: 10932.390978483949, 2023: 10737.61353507574, 2024: 10542.836091667472, 2025: 10348.058648259263, 2026: 10153.281204850995, 2027: 9958.503761442786, 2028: 9763.726318034518, 2029: 9568.948874626309, 2030: 9374.1714312181, 2031: 9179.393987809832, 2032: 8984.616544401622, 2033: 8789.839100993355, 2034: 8595.061657585145, 2035: 8400.284214176878, 2036: 8205.506770768669, 2037: 8010.729327360401, 2038: 7815.951883952192, 2039: 7621.174440543924, 2040: 7426.396997135715, 2041: 7231.619553727447, 2042: 7036.842110319238, 2043: 6842.06466691097, 2044: 6647.287223502761, 2045: 6452.509780094493, 2046: 6257.732336686284, 2047: 6062.954893278016, 2048: 5868.177449869807, 2049: 5673.4000064615975, 2050: 5478.62256305333}</t>
         </is>
       </c>
-      <c r="T201" t="n">
+      <c r="S201" t="n">
         <v>240860.9194172315</v>
       </c>
     </row>
@@ -14968,15 +13963,10 @@
       </c>
       <c r="R202" t="inlineStr">
         <is>
-          <t>{2021: 29140.3773059041, 2022: 22295.02893157111, 2023: 17057.717195682377, 2024: 13050.699185945128, 2025: 9984.967348687209, 2026: 7639.40471953568, 2027: 5844.836786225152, 2028: 4471.829718649481, 2029: 3421.354909297954, 2030: 2617.6465008404634, 2031: 2002.7367475794372, 2032: 1532.2750718316015, 2033: 1172.3292632415298, 2034: 896.9381064260186, 2035: 686.238919375456, 2036: 525.0349506746446, 2037: 401.69930857434485, 2038: 307.3363674204239, 2039: 235.1401675905559, 2040: 179.90353331299377, 2041: 137.64250332106735, 2042: 105.30898627504432, 2043: 80.5709161247147, 2044: 61.64405104252893, 2045: 47.163284367425526, 2046: 36.08418581686045, 2047: 27.60767159305427, 2048: 21.122370188931992, 2049: 16.16052700766439, 2050: 12.364267401311713}</t>
-        </is>
-      </c>
-      <c r="S202" t="inlineStr">
-        <is>
           <t>{2021: 29140.3773059041, 2022: 29318.091447584447, 2023: 28825.722171694273, 2024: 28333.352895804215, 2025: 27840.983619914157, 2026: 27348.6143440241, 2027: 26856.245068133925, 2028: 26363.875792243867, 2029: 25871.50651635381, 2030: 25379.13724046375, 2031: 24886.767964573577, 2032: 24394.39868868352, 2033: 23902.02941279346, 2034: 23409.660136903403, 2035: 22917.29086101323, 2036: 22424.92158512317, 2037: 21932.552309233113, 2038: 21440.183033343055, 2039: 20947.81375745288, 2040: 20455.444481562823, 2041: 19963.075205672765, 2042: 19470.705929782707, 2043: 18978.336653892533, 2044: 18485.967378002475, 2045: 17993.598102112417, 2046: 17501.22882622236, 2047: 17008.859550332185, 2048: 16516.490274442127, 2049: 16024.120998552069, 2050: 15531.751722661895}</t>
         </is>
       </c>
-      <c r="T202" t="n">
+      <c r="S202" t="n">
         <v>657127.0387601934</v>
       </c>
     </row>
@@ -15040,15 +14030,10 @@
       </c>
       <c r="R203" t="inlineStr">
         <is>
-          <t>{2021: 97788.2316329065, 2022: 74453.4214745283, 2023: 56686.90267427215, 2024: 43159.936389246526, 2025: 32860.85535185265, 2026: 25019.40236233594, 2027: 19049.1235808069, 2028: 14503.508274966414, 2029: 11042.594762415258, 2030: 8407.545041870448, 2031: 6401.286577288071, 2032: 4873.773454736353, 2033: 3710.764609785061, 2034: 2825.2798611005933, 2035: 2151.09475618367, 2036: 1637.7877157551195, 2037: 1246.9690580424353, 2038: 949.4098757471264, 2039: 722.8560374875792, 2040: 550.3638252351791, 2041: 419.03273185665756, 2042: 319.04064605303915, 2043: 242.90926721390304, 2044: 184.94481135355406, 2045: 140.81217912728508, 2046: 107.2107384114164, 2047: 81.6274735747907, 2048: 62.14903974109402, 2049: 47.318665782312706, 2050: 36.02720397203031}</t>
-        </is>
-      </c>
-      <c r="S203" t="inlineStr">
-        <is>
           <t>{2021: 97788.2316329065, 2022: 95161.2417995669, 2023: 93023.73170825187, 2024: 90886.22161693685, 2025: 88748.71152562089, 2026: 86611.20143430587, 2027: 84473.69134299085, 2028: 82336.18125167489, 2029: 80198.67116035987, 2030: 78061.16106904484, 2031: 75923.65097772889, 2032: 73786.14088641386, 2033: 71648.63079509791, 2034: 69511.12070378289, 2035: 67373.61061246786, 2036: 65236.10052115191, 2037: 63098.590429836884, 2038: 60961.08033852186, 2039: 58823.570247205906, 2040: 56686.06015589088, 2041: 54548.55006457586, 2042: 52411.0399732599, 2043: 50273.52988194488, 2044: 48136.019790628925, 2045: 45998.5096993139, 2046: 43860.99960799888, 2047: 41723.48951668292, 2048: 39585.9794253679, 2049: 37448.469334052876, 2050: 35310.95924273692}</t>
         </is>
       </c>
-      <c r="T203" t="n">
+      <c r="S203" t="n">
         <v>1923085.551308499</v>
       </c>
     </row>
@@ -15112,15 +14097,10 @@
       </c>
       <c r="R204" t="inlineStr">
         <is>
-          <t>{2021: 53167.1119846155, 2022: 39187.1052152083, 2023: 28883.06620062713, 2024: 21288.418947211456, 2025: 15690.743431601168, 2026: 11564.94665230104, 2027: 8524.00599459172, 2028: 6282.664363296388, 2029: 4630.671485552492, 2030: 3413.061269416301, 2031: 2515.61512517871, 2032: 1854.1476283284417, 2033: 1366.6094599394485, 2034: 1007.2668365030335, 2035: 742.4114274489092, 2036: 547.1983268309131, 2037: 403.31546338860255, 2038: 297.26582672579514, 2039: 219.10137289684602, 2040: 161.48984272438457, 2041: 119.02695523238253, 2042: 87.72945612481143, 2043: 64.66146644622657, 2044: 47.659080856811485, 2045: 35.1273813130269, 2046: 25.890824911585295, 2047: 19.08297144694282, 2048: 14.065206515760158, 2049: 10.366835944864103, 2050: 7.640932067887089}</t>
-        </is>
-      </c>
-      <c r="S204" t="inlineStr">
-        <is>
           <t>{2021: 53167.1119846155, 2022: 54327.26358602673, 2023: 54832.04724874406, 2024: 55336.83091146138, 2025: 55841.614574178704, 2026: 56346.39823689603, 2027: 56851.18189961335, 2028: 57355.965562330675, 2029: 57860.749225048, 2030: 58365.53288776532, 2031: 58870.31655048265, 2032: 59375.10021319997, 2033: 59879.883875917294, 2034: 60384.66753863462, 2035: 60889.45120135194, 2036: 61394.234864069265, 2037: 61899.01852678659, 2038: 62403.80218950403, 2039: 62908.58585222135, 2040: 63413.36951493868, 2041: 63918.153177656, 2042: 64422.936840373324, 2043: 64927.72050309065, 2044: 65432.50416580797, 2045: 65937.2878285253, 2046: 66442.07149124262, 2047: 66946.85515395994, 2048: 67451.63881667727, 2049: 67956.42247939459, 2050: 68461.20614211191}</t>
         </is>
       </c>
-      <c r="T204" t="n">
+      <c r="S204" t="n">
         <v>1772785.763979262</v>
       </c>
     </row>
@@ -15184,15 +14164,10 @@
       </c>
       <c r="R205" t="inlineStr">
         <is>
-          <t>{2021: 45590.2016067924, 2022: 35980.52373194448, 2023: 28396.410684705992, 2024: 22410.90612748863, 2025: 17687.04922011898, 2026: 13958.905023086074, 2027: 11016.593385282998, 2028: 8694.473500316813, 2029: 6861.8189674402165, 2030: 5415.458398971097, 2031: 4273.967268758626, 2032: 3373.0840251474638, 2033: 2662.09241326494, 2034: 2100.9663453174535, 2035: 1658.116586096621, 2036: 1308.6124007727929, 2037: 1032.7780505999622, 2038: 815.0851246489533, 2039: 643.2783501140999, 2040: 507.68566768254976, 2041: 400.6737318682647, 2042: 316.2181830778518, 2043: 249.56449938159244, 2044: 196.96033525134473, 2045: 155.4442789677621, 2046: 122.67913655291389, 2047: 96.82035675619683, 2048: 76.41218992729016, 2049: 60.305734920880305, 2050: 47.594260389710726}</t>
-        </is>
-      </c>
-      <c r="S205" t="inlineStr">
-        <is>
           <t>{2021: 45590.2016067924, 2022: 34408.2051695548, 2023: 29675.338276157156, 2024: 24942.471382761374, 2025: 20209.60448936373, 2026: 15476.737595967948, 2027: 10743.870702570304, 2028: 6011.003809174523, 2029: 1278.1369157768786, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T205" t="n">
+      <c r="S205" t="n">
         <v>165540.4691447229</v>
       </c>
     </row>
@@ -15256,15 +14231,10 @@
       </c>
       <c r="R206" t="inlineStr">
         <is>
-          <t>{2021: 17518.5543303956, 2022: 13656.633240471614, 2023: 10646.062908350877, 2024: 8299.165208060485, 2025: 6469.635182848159, 2026: 5043.420434442529, 2027: 3931.611127932968, 2028: 3064.8973771299197, 2029: 2389.248485334437, 2030: 1862.5446865756246, 2031: 1451.9514109916893, 2032: 1131.872386781073, 2033: 882.3539756626303, 2034: 687.8412685565733, 2035: 536.2083968332641, 2036: 418.0026089999738, 2037: 325.8549887742931, 2038: 254.02107887106817, 2039: 198.02277311616237, 2040: 154.3691525399678, 2041: 120.33886244956787, 2042: 93.81046392611773, 2043: 73.13018390647949, 2044: 57.008819425596826, 2045: 44.441369058451784, 2046: 34.64438140781301, 2047: 27.00711495974405, 2048: 21.05346462570522, 2049: 16.41228148236171, 2050: 12.794235449845836}</t>
-        </is>
-      </c>
-      <c r="S206" t="inlineStr">
-        <is>
           <t>{2021: 17518.5543303956, 2022: 16392.596084017307, 2023: 15546.599187081447, 2024: 14700.602290145354, 2025: 13854.605393209262, 2026: 13008.608496273402, 2027: 12162.61159933731, 2028: 11316.61470240145, 2029: 10470.617805465357, 2030: 9624.620908529265, 2031: 8778.624011593405, 2032: 7932.627114657313, 2033: 7086.63021772122, 2034: 6240.63332078536, 2035: 5394.636423849268, 2036: 4548.639526913408, 2037: 3702.6426299773157, 2038: 2856.645733041223, 2039: 2010.6488361053634, 2040: 1164.651939169271, 2041: 318.6550422331784, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T206" t="n">
+      <c r="S206" t="n">
         <v>175871.7884277043</v>
       </c>
     </row>
@@ -15328,15 +14298,10 @@
       </c>
       <c r="R207" t="inlineStr">
         <is>
-          <t>{2021: 498927.295715117, 2022: 384332.81890880683, 2023: 296058.5980341548, 2024: 228059.35157659976, 2025: 175678.28864588117, 2026: 135328.19806856036, 2027: 104245.78548461899, 2028: 80302.4347209562, 2029: 61858.43381711462, 2030: 47650.68266738085, 2031: 36706.192164199565, 2032: 28275.45100665402, 2033: 21781.09693463286, 2034: 16778.377241948485, 2035: 12924.690786602014, 2036: 9956.125644357946, 2037: 7669.385634277318, 2038: 5907.867990857649, 2039: 4550.938740308797, 2040: 3505.671326795641, 2041: 2700.4827251713787, 2042: 2080.231222250616, 2043: 1602.4401480856236, 2044: 1234.3889471183588, 2045: 950.8723770983263, 2046: 732.4743790353524, 2047: 564.2384076614577, 2048: 434.6431626722762, 2049: 334.813575773288, 2050: 257.913019574219}</t>
-        </is>
-      </c>
-      <c r="S207" t="inlineStr">
-        <is>
           <t>{2021: 498927.295715117, 2022: 492790.54507369176, 2023: 479675.744625397, 2024: 466560.9441771023, 2025: 453446.14372880384, 2026: 440331.3432805091, 2027: 427216.5428322144, 2028: 414101.74238391966, 2029: 400986.9419356212, 2030: 387872.1414873265, 2031: 374757.34103903174, 2032: 361642.540590737, 2033: 348527.74014243856, 2034: 335412.93969414383, 2035: 322298.1392458491, 2036: 309183.33879755065, 2037: 296068.5383492559, 2038: 282953.7379009612, 2039: 269838.93745266646, 2040: 256724.137004368, 2041: 243609.33655607328, 2042: 230494.53610777855, 2043: 217379.7356594801, 2044: 204264.93521118537, 2045: 191150.13476289064, 2046: 178035.3343145959, 2047: 164920.53386629745, 2048: 151805.73341800272, 2049: 138690.932969708, 2050: 125576.13252140954}</t>
         </is>
       </c>
-      <c r="T207" t="n">
+      <c r="S207" t="n">
         <v>9152992.406725863</v>
       </c>
     </row>
@@ -15400,15 +14365,10 @@
       </c>
       <c r="R208" t="inlineStr">
         <is>
-          <t>{2021: 50616.0916247363, 2022: 39514.830709970694, 2023: 30848.328978339563, 2024: 24082.588325900237, 2025: 18800.72858669325, 2026: 14677.300903340163, 2027: 11458.234760096573, 2028: 8945.183087961834, 2029: 6983.300844543354, 2030: 5451.704029516003, 2031: 4256.021255143923, 2032: 3322.5789269130523, 2033: 2593.861746396137, 2034: 2024.968829158316, 2035: 1580.847076664728, 2036: 1234.1313326971886, 2037: 963.4582426266895, 2038: 752.149921723986, 2039: 587.1863249693544, 2040: 458.40299955191887, 2041: 357.86478850501766, 2042: 279.3768953888269, 2043: 218.10318361624792, 2044: 170.2681914241258, 2045: 132.92450174341707, 2046: 103.77113315148608, 2047: 81.01176182198292, 2048: 63.24403862797852, 2049: 49.373181523523776, 2050: 38.544519082568726}</t>
-        </is>
-      </c>
-      <c r="S208" t="inlineStr">
-        <is>
           <t>{2021: 50616.0916247363, 2022: 46404.61965116393, 2023: 43662.56015069876, 2024: 40920.50065023359, 2025: 38178.44114976842, 2026: 35436.38164930325, 2027: 32694.32214883808, 2028: 29952.26264837198, 2029: 27210.20314790681, 2030: 24468.14364744164, 2031: 21726.08414697647, 2032: 18984.0246465113, 2033: 16241.965146046132, 2034: 13499.905645580031, 2035: 10757.846145114861, 2036: 8015.786644649692, 2037: 5273.727144184522, 2038: 2531.667643719353, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T208" t="n">
+      <c r="S208" t="n">
         <v>441266.487818877</v>
       </c>
     </row>
@@ -15472,15 +14432,10 @@
       </c>
       <c r="R209" t="inlineStr">
         <is>
-          <t>{2021: 25547.0441284823, 2022: 20010.002511345185, 2023: 15673.053934941772, 2024: 12276.091395206935, 2025: 9615.383228376139, 2026: 7531.354374295011, 2027: 5899.015916892562, 2028: 4620.468916788843, 2029: 3619.0329559676425, 2030: 2834.6472559937474, 2031: 2220.2685534164893, 2032: 1739.049696171799, 2033: 1362.129748269202, 2034: 1066.9030650499742, 2035: 835.6635273984687, 2036: 654.5426233182123, 2037: 512.677688679359, 2038: 401.56042266147165, 2039: 314.52660532865485, 2040: 246.35641332354615, 2041: 192.96136275093238, 2042: 151.13910375775944, 2043: 118.38136069853394, 2044: 92.72349916337865, 2045: 72.6266977028213, 2046: 56.88565753890593, 2047: 44.556315184188506, 2048: 34.89922255772398, 2049: 27.335198839911264, 2050: 21.410594301394024}</t>
-        </is>
-      </c>
-      <c r="S209" t="inlineStr">
-        <is>
           <t>{2021: 25547.0441284823, 2022: 20849.415951226838, 2023: 18753.845139840618, 2024: 16658.274328453466, 2025: 14562.703517067246, 2026: 12467.132705681026, 2027: 10371.561894293875, 2028: 8275.991082907654, 2029: 6180.420271521434, 2030: 4084.849460135214, 2031: 1989.2786487480626, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T209" t="n">
+      <c r="S209" t="n">
         <v>126966.9950641166</v>
       </c>
     </row>
@@ -15544,15 +14499,10 @@
       </c>
       <c r="R210" t="inlineStr">
         <is>
-          <t>{2021: 34907.3224756623, 2022: 26928.118735164575, 2023: 20772.821493848, 2024: 16024.517607751714, 2025: 12361.59299001309, 2026: 9535.948912235639, 2027: 7356.197678586709, 2028: 5674.699475058107, 2029: 4377.562368390774, 2030: 3376.928130446031, 2031: 2605.0213882823086, 2032: 2009.5590345039295, 2033: 1550.2089661609828, 2034: 1195.8582940357028, 2035: 922.5059915344817, 2036: 711.6372472068249, 2037: 548.9694118622732, 2038: 423.4846002556452, 2039: 326.68342311698206, 2040: 252.00930299473498, 2041: 194.4043814342862, 2042: 149.96693801274876, 2043: 115.68711739412049, 2044: 89.24306456015844, 2045: 68.84365996393448, 2046: 53.10720267830997, 2047: 40.967824456059155, 2048: 31.603295899973187, 2049: 24.37933488053557, 2050: 18.806645075832193}</t>
-        </is>
-      </c>
-      <c r="S210" t="inlineStr">
-        <is>
           <t>{2021: 34907.3224756623, 2022: 32347.9938882445, 2023: 30861.803540764377, 2024: 29375.613193284255, 2025: 27889.422845804133, 2026: 26403.23249832401, 2027: 24917.04215084389, 2028: 23430.851803363767, 2029: 21944.661455883645, 2030: 20458.471108403523, 2031: 18972.2807609234, 2032: 17486.09041344328, 2033: 15999.900065963622, 2034: 14513.7097184835, 2035: 13027.519371003378, 2036: 11541.329023523256, 2037: 10055.138676043134, 2038: 8568.948328563012, 2039: 7082.75798108289, 2040: 5596.567633602768, 2041: 4110.377286122646, 2042: 2624.186938642524, 2043: 1137.9965911624022, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T210" t="n">
+      <c r="S210" t="n">
         <v>385799.5565113071</v>
       </c>
     </row>
@@ -15616,15 +14566,10 @@
       </c>
       <c r="R211" t="inlineStr">
         <is>
-          <t>{2021: 71581.5772144457, 2022: 54479.7471672017, 2023: 41463.78114176629, 2024: 31557.5096429105, 2025: 24017.98358566116, 2026: 18279.754709690253, 2027: 13912.46817430301, 2028: 10588.58686973453, 2029: 8058.826837426453, 2030: 6133.461508566071, 2031: 4668.092618934486, 2032: 3552.820649239736, 2033: 2704.002597220405, 2034: 2057.978932130814, 2035: 1566.2992666678515, 2036: 1192.0886819886593, 2037: 907.2821880001619, 2038: 690.5199093822051, 2039: 525.5451408168988, 2040: 399.9851290071599, 2041: 304.42314275457215, 2042: 231.69223834547023, 2043: 176.33775416612275, 2044: 134.20822279763624, 2045: 102.14401987637612, 2046: 77.74039905317403, 2047: 59.16714118223669, 2048: 45.031291816295365, 2049: 34.2726926149534, 2050: 26.084471746245264}</t>
-        </is>
-      </c>
-      <c r="S211" t="inlineStr">
-        <is>
           <t>{2021: 71581.5772144457, 2022: 67709.56985297613, 2023: 65675.51738003781, 2024: 63641.46490709949, 2025: 61607.412434161175, 2026: 59573.35996122286, 2027: 57539.30748828454, 2028: 55505.25501534622, 2029: 53471.202542407904, 2030: 51437.150069469586, 2031: 49403.09759653127, 2032: 47369.04512359295, 2033: 45334.99265065463, 2034: 43300.940177716315, 2035: 41266.887704778, 2036: 39232.83523183968, 2037: 37198.78275890136, 2038: 35164.73028596304, 2039: 33130.677813024726, 2040: 31096.625340086874, 2041: 29062.572867148556, 2042: 27028.520394210238, 2043: 24994.46792127192, 2044: 22960.415448333602, 2045: 20926.362975395285, 2046: 18892.310502456967, 2047: 16858.25802951865, 2048: 14824.205556580331, 2049: 12790.153083642013, 2050: 10756.100610703696}</t>
         </is>
       </c>
-      <c r="T211" t="n">
+      <c r="S211" t="n">
         <v>1168164.960025227</v>
       </c>
     </row>
@@ -15688,15 +14633,10 @@
       </c>
       <c r="R212" t="inlineStr">
         <is>
-          <t>{2021: 30903.7259124321, 2022: 23123.992733533927, 2023: 17302.736940383635, 2024: 12946.92958426488, 2025: 9687.657290141788, 2026: 7248.877284796488, 2027: 5424.038063723605, 2028: 4058.5855934445535, 2029: 3036.873418990641, 2030: 2272.3680333040884, 2031: 1700.319956206315, 2032: 1272.2798028758225, 2033: 951.9948824321928, 2034: 712.3387906720868, 2035: 533.0139500327757, 2036: 398.8325143173688, 2037: 298.4300400898195, 2038: 223.30297964910125, 2039: 167.08847643206119, 2040: 125.02546540247144, 2041: 93.55143653763784, 2042: 70.00070945612882, 2043: 52.37866467598216, 2044: 39.19281010942351, 2045: 29.32637503792047, 2046: 21.94372565946674, 2047: 16.419591415417035, 2048: 12.286107948716865, 2049: 9.193191517895636, 2050: 6.878888793544647}</t>
-        </is>
-      </c>
-      <c r="S212" t="inlineStr">
-        <is>
           <t>{2021: 30903.7259124321, 2022: 28305.437653321307, 2023: 27521.70419979212, 2024: 26737.97074626293, 2025: 25954.237292733742, 2026: 25170.503839204554, 2027: 24386.770385675365, 2028: 23603.036932146177, 2029: 22819.30347861699, 2030: 22035.5700250878, 2031: 21251.83657155861, 2032: 20468.103118029423, 2033: 19684.369664500235, 2034: 18900.636210971046, 2035: 18116.902757441858, 2036: 17333.16930391267, 2037: 16549.43585038348, 2038: 15765.702396854293, 2039: 14981.968943325104, 2040: 14198.235489795916, 2041: 13414.502036266727, 2042: 12630.768582737539, 2043: 11847.03512920835, 2044: 11063.301675679162, 2045: 10279.568222149974, 2046: 9495.834768620785, 2047: 8712.101315091597, 2048: 7928.3678615624085, 2049: 7144.63440803322, 2050: 6360.900954504032}</t>
         </is>
       </c>
-      <c r="T212" t="n">
+      <c r="S212" t="n">
         <v>514933.3222924314</v>
       </c>
     </row>
@@ -15760,15 +14700,10 @@
       </c>
       <c r="R213" t="inlineStr">
         <is>
-          <t>{2021: 62848.4238097407, 2022: 46314.5311933314, 2023: 34130.30382673837, 2024: 25151.450512214113, 2025: 18534.715251282574, 2026: 13658.682201223271, 2027: 10065.414922471156, 2028: 7417.448921421681, 2029: 5466.098409820156, 2030: 4028.100785372413, 2031: 2968.405381792551, 2032: 2187.4900803506903, 2033: 1612.0146126210866, 2034: 1187.9327520823852, 2035: 875.4165206824564, 2036: 645.1157132761919, 2037: 475.4014502621096, 2038: 350.3348845179306, 2039: 258.1702921657535, 2040: 190.25196377079365, 2041: 140.2012966519189, 2042: 103.31774344553126, 2043: 76.13735654084994, 2044: 56.10746874359104, 2045: 41.34695754933418, 2046: 30.4695780591906, 2047: 22.45377271102404, 2048: 16.546730905787964, 2049: 12.193688214102872, 2050: 8.985825243023784}</t>
-        </is>
-      </c>
-      <c r="S213" t="inlineStr">
-        <is>
           <t>{2021: 62848.4238097407, 2022: 58420.74130347464, 2023: 57573.56793453451, 2024: 56726.39456559415, 2025: 55879.22119665402, 2026: 55032.04782771389, 2027: 54184.87445877376, 2028: 53337.70108983363, 2029: 52490.5277208935, 2030: 51643.35435195337, 2031: 50796.18098301324, 2032: 49949.00761407311, 2033: 49101.83424513298, 2034: 48254.66087619262, 2035: 47407.48750725249, 2036: 46560.31413831236, 2037: 45713.14076937223, 2038: 44865.9674004321, 2039: 44018.79403149197, 2040: 43171.62066255184, 2041: 42324.44729361171, 2042: 41477.27392467158, 2043: 40630.10055573145, 2044: 39782.92718679109, 2045: 38935.75381785096, 2046: 38088.58044891083, 2047: 37241.4070799707, 2048: 36394.23371103057, 2049: 35547.06034209044, 2050: 34699.88697315031}</t>
         </is>
       </c>
-      <c r="T213" t="n">
+      <c r="S213" t="n">
         <v>1364323.378429355</v>
       </c>
     </row>
@@ -15832,15 +14767,10 @@
       </c>
       <c r="R214" t="inlineStr">
         <is>
-          <t>{2021: 30700.30201637, 2022: 23779.01452030251, 2023: 18418.109738961302, 2024: 14265.804247976279, 2025: 11049.623100630699, 2026: 8558.519978522183, 2027: 6629.028298583541, 2028: 5134.53450990358, 2029: 3976.9696923792017, 2030: 3080.374258580985, 2031: 2385.913473545176, 2032: 1848.0167101080665, 2033: 1431.3870971037868, 2034: 1108.6853330646532, 2035: 858.7356769107124, 2036: 665.1363924522095, 2037: 515.1834638522179, 2038: 399.0369560869268, 2039: 309.07531684440073, 2040: 239.39524904970648, 2041: 185.42433557197623, 2042: 143.62099648506359, 2043: 111.24209002952507, 2044: 86.16290721408508, 2045: 66.73774807370656, 2046: 51.69193057614748, 2047: 40.038145784274576, 2048: 31.01167048658324, 2049: 24.020185938434384, 2050: 18.604909811826456}</t>
-        </is>
-      </c>
-      <c r="S214" t="inlineStr">
-        <is>
           <t>{2021: 30700.30201637, 2022: 28589.991700837854, 2023: 27225.73830733914, 2024: 25861.484913840424, 2025: 24497.231520341244, 2026: 23132.97812684253, 2027: 21768.724733343814, 2028: 20404.4713398451, 2029: 19040.217946346384, 2030: 17675.96455284767, 2031: 16311.711159348954, 2032: 14947.457765849773, 2033: 13583.204372351058, 2034: 12218.950978852343, 2035: 10854.697585353628, 2036: 9490.444191854913, 2037: 8126.190798356198, 2038: 6761.937404857017, 2039: 5397.684011358302, 2040: 4033.430617859587, 2041: 2669.177224360872, 2042: 1304.923830862157, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T214" t="n">
+      <c r="S214" t="n">
         <v>329246.764091034</v>
       </c>
     </row>
@@ -15904,15 +14834,10 @@
       </c>
       <c r="R215" t="inlineStr">
         <is>
-          <t>{2021: 31268.2196793714, 2022: 24303.61094197708, 2023: 18890.282557681665, 2024: 14682.706037427344, 2025: 11412.31508439453, 2026: 8870.363218708106, 2027: 6894.5996539653115, 2028: 5358.912957273663, 2029: 4165.28145577226, 2030: 3237.516590421884, 2031: 2516.399860261933, 2032: 1955.9029521146374, 2033: 1520.2497895912895, 2034: 1181.6329743015287, 2035: 918.4388615058141, 2036: 713.867978187315, 2037: 554.8627259148471, 2038: 431.2739246147707, 2039: 335.21299839696064, 2040: 260.54845396612296, 2041: 202.51451223185143, 2042: 157.40691238120795, 2043: 122.34647182725882, 2044: 95.09531025122423, 2045: 73.91400746353024, 2046: 57.450577582488776, 2047: 44.6541728398381, 2048: 34.70800879498754, 2049: 26.977229627198707, 2050: 20.96838578834609}</t>
-        </is>
-      </c>
-      <c r="S215" t="inlineStr">
-        <is>
           <t>{2021: 31268.2196793714, 2022: 29848.16678335052, 2023: 28557.63886864623, 2024: 27267.11095394194, 2025: 25976.583039237652, 2026: 24686.055124533363, 2027: 23395.527209829073, 2028: 22104.99929512432, 2029: 20814.47138042003, 2030: 19523.94346571574, 2031: 18233.41555101145, 2032: 16942.88763630716, 2033: 15652.359721602872, 2034: 14361.831806898583, 2035: 13071.303892194293, 2036: 11780.775977489538, 2037: 10490.24806278525, 2038: 9199.72014808096, 2039: 7909.192233376671, 2040: 6618.664318672381, 2041: 5328.136403968092, 2042: 4037.6084892638028, 2043: 2747.0805745595135, 2044: 1456.5526598547585, 2045: 166.02474515046924, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T215" t="n">
+      <c r="S215" t="n">
         <v>375804.4081817004</v>
       </c>
     </row>
@@ -15976,15 +14901,10 @@
       </c>
       <c r="R216" t="inlineStr">
         <is>
-          <t>{2021: 96823.3419136609, 2022: 77237.5027619948, 2023: 61613.57080846079, 2024: 49150.11454302443, 2025: 39207.81944455479, 2026: 31276.694263879017, 2027: 24949.910959968463, 2028: 19902.936405567263, 2029: 15876.885420538412, 2030: 12665.241224726744, 2031: 10103.262134336046, 2032: 8059.5311170088535, 2033: 6429.214738998031, 2034: 5128.6857212966715, 2035: 4091.2332680820728, 2036: 3263.6411282439926, 2037: 2603.457861242648, 2038: 2076.8192852481466, 2039: 1656.71140977097, 2040: 1321.5847496992826, 2041: 1054.248941811278, 2042: 840.9909629806934, 2043: 670.8717189699613, 2044: 535.1649222466649, 2045: 426.90947599194106, 2046: 340.5524037835039, 2047: 271.6640089874979, 2048: 216.7106529251702, 2049: 172.87349644249275, 2050: 137.9039072092681}</t>
-        </is>
-      </c>
-      <c r="S216" t="inlineStr">
-        <is>
           <t>{2021: 96823.3419136609, 2022: 86880.68370117247, 2023: 79327.6189957019, 2024: 71774.55429023318, 2025: 64221.4895847626, 2026: 56668.424879292026, 2027: 49115.36017382145, 2028: 41562.295468352735, 2029: 34009.23076288216, 2030: 26456.16605741158, 2031: 18903.101351941004, 2032: 11350.03664647229, 2033: 3796.9719410017133, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T216" t="n">
+      <c r="S216" t="n">
         <v>592477.6048098756</v>
       </c>
     </row>
@@ -16048,15 +14968,10 @@
       </c>
       <c r="R217" t="inlineStr">
         <is>
-          <t>{2021: 34326.3895574425, 2022: 27010.88458850937, 2023: 21254.431230900802, 2024: 16724.770544585186, 2025: 13160.453306431256, 2026: 10355.749322183186, 2027: 8148.7728064420635, 2028: 6412.138434904752, 2029: 5045.608741954205, 2030: 3970.3084759215512, 2031: 3124.1719681715226, 2032: 2458.360740960619, 2033: 1934.444580601474, 2034: 1522.183369213817, 2035: 1197.7816437577626, 2036: 942.5151365725643, 2037: 741.6500221872286, 2038: 583.5924899949537, 2039: 459.21955665030816, 2040: 361.35249309313235, 2041: 284.34247273152295, 2042: 223.74452465238437, 2043: 176.0609726398129, 2044: 138.53955145957406, 2045: 109.01454780603547, 2046: 85.78179666491985, 2047: 67.5003179589785, 2048: 53.11491600439366, 2049: 41.795274266238295, 2050: 32.888029999813625}</t>
-        </is>
-      </c>
-      <c r="S217" t="inlineStr">
-        <is>
           <t>{2021: 34326.3895574425, 2022: 31698.749662001617, 2023: 29671.13724380359, 2024: 27643.52482560603, 2025: 25615.912407408003, 2026: 23588.29998921044, 2027: 21560.687571012415, 2028: 19533.075152814854, 2029: 17505.462734616827, 2030: 15477.850316419266, 2031: 13450.23789822124, 2032: 11422.625480023678, 2033: 9395.013061825652, 2034: 7367.400643627625, 2035: 5339.788225430064, 2036: 3312.175807232037, 2037: 1284.5633890344761, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T217" t="n">
+      <c r="S217" t="n">
         <v>281029.6991870091</v>
       </c>
     </row>
@@ -16120,15 +15035,10 @@
       </c>
       <c r="R218" t="inlineStr">
         <is>
-          <t>{2021: 263087.387205743, 2022: 209060.76947659435, 2023: 166128.85094322625, 2024: 132013.26669184837, 2025: 104903.52809704827, 2026: 83360.94154003481, 2027: 66242.2580107354, 2028: 52639.001735044534, 2029: 41829.25804269788, 2030: 33239.36189385877, 2031: 26413.453903081714, 2032: 20989.28822153841, 2033: 16679.008419849677, 2034: 13253.871161955316, 2035: 10532.10696678178, 2036: 8369.27383737815, 2037: 6650.591831809453, 2038: 5284.851777198714, 2039: 4199.574866912481, 2040: 3337.166264320724, 2041: 2651.8585877498613, 2042: 2107.283069653743, 2043: 1674.5394932303852, 2044: 1330.662479459406, 2045: 1057.4027315565045, 2046: 840.258558396713, 2047: 667.7062805764036, 2048: 530.5886773374388, 2049: 421.62901968761463, 2050: 335.0448998173437}</t>
-        </is>
-      </c>
-      <c r="S218" t="inlineStr">
-        <is>
           <t>{2021: 263087.387205743, 2022: 315639.2866946977, 2023: 315968.53649326693, 2024: 316297.7862918363, 2025: 316627.03609040554, 2026: 316956.2858889749, 2027: 317285.53568754415, 2028: 317614.7854861135, 2029: 317944.03528468276, 2030: 318273.285083252, 2031: 318602.53488182137, 2032: 318931.7846803906, 2033: 319261.03447896, 2034: 319590.2842775292, 2035: 319919.5340760986, 2036: 320248.78387466783, 2037: 320578.0336732371, 2038: 320907.28347180644, 2039: 321236.5332703757, 2040: 321565.78306894505, 2041: 321895.0328675143, 2042: 322224.28266608354, 2043: 322553.5324646529, 2044: 322882.78226322215, 2045: 323212.0320617915, 2046: 323541.28186036076, 2047: 323870.5316589301, 2048: 324199.78145749937, 2049: 324529.0312560686, 2050: 324858.281054638}</t>
         </is>
       </c>
-      <c r="T218" t="n">
+      <c r="S218" t="n">
         <v>9256329.28544092</v>
       </c>
     </row>
@@ -16192,15 +15102,10 @@
       </c>
       <c r="R219" t="inlineStr">
         <is>
-          <t>{2021: 39524.008095575, 2022: 30726.75224984108, 2023: 23887.590082970775, 2024: 18570.688998704536, 2025: 14437.224043477725, 2026: 11223.785940096854, 2027: 8725.595062440454, 2028: 6783.4516445729905, 2029: 5273.590613015458, 2030: 4099.794530994318, 2031: 3187.2620439833236, 2032: 2477.8410869661298, 2033: 1926.3230846825275, 2034: 1497.561988983004, 2035: 1164.2345610037394, 2036: 905.0991698554343, 2037: 703.6421479935476, 2038: 547.0254408829638, 2039: 425.26848885684575, 2040: 330.61220575530547, 2041: 257.02452323285723, 2042: 199.8159910404864, 2043: 155.34093701759144, 2044: 120.76514290897752, 2045: 93.88523091098773, 2046: 72.98825116990133, 2047: 56.742522302484225, 2048: 44.112768639340345, 2049: 34.29414622519829, 2050: 26.660953315599215}</t>
-        </is>
-      </c>
-      <c r="S219" t="inlineStr">
-        <is>
           <t>{2021: 39524.008095575, 2022: 37184.578495761845, 2023: 35410.99470931897, 2024: 33637.41092287609, 2025: 31863.827136432752, 2026: 30090.243349989876, 2027: 28316.659563547, 2028: 26543.075777104124, 2029: 24769.491990660783, 2030: 22995.908204217907, 2031: 21222.32441777503, 2032: 19448.74063133169, 2033: 17675.156844888814, 2034: 15901.573058445938, 2035: 14127.989272003062, 2036: 12354.40548555972, 2037: 10580.821699116845, 2038: 8807.237912673969, 2039: 7033.654126231093, 2040: 5260.070339787751, 2041: 3486.4865533448756, 2042: 1712.9027669019997, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T219" t="n">
+      <c r="S219" t="n">
         <v>428185.5573057577</v>
       </c>
     </row>
@@ -16264,15 +15169,10 @@
       </c>
       <c r="R220" t="inlineStr">
         <is>
-          <t>{2021: 75194.2350471489, 2022: 56439.34069015449, 2023: 42362.27917661498, 2024: 31796.308657987534, 2025: 23865.695234644332, 2026: 17913.129953525073, 2027: 13445.249408283551, 2028: 10091.74455385308, 2029: 7574.668572341853, 2030: 5685.399949894399, 2031: 4267.351407068324, 2032: 3202.991555896829, 2033: 2404.10360631501, 2034: 1804.4737393254002, 2035: 1354.4031410967164, 2036: 1016.5888417408851, 2037: 763.0319524475148, 2038: 572.7170479845439, 2039: 429.87035601853415, 2040: 322.6523876559862, 2041: 242.17665117531476, 2042: 181.77311750447214, 2043: 136.43539163226558, 2044: 102.40577014580668, 2045: 76.86379343140857, 2046: 57.69247897119755, 2047: 43.3028605700066, 2048: 32.502290887544945, 2049: 24.395591862360543, 2050: 18.310860129029727}</t>
-        </is>
-      </c>
-      <c r="S220" t="inlineStr">
-        <is>
           <t>{2021: 75194.2350471489, 2022: 73957.14540860173, 2023: 73183.83328762092, 2024: 72410.5211666401, 2025: 71637.20904565929, 2026: 70863.89692467847, 2027: 70090.58480369765, 2028: 69317.27268271684, 2029: 68543.96056173602, 2030: 67770.6484407552, 2031: 66997.33631977439, 2032: 66224.02419879357, 2033: 65450.71207781276, 2034: 64677.39995683194, 2035: 63904.087835851125, 2036: 63130.77571487031, 2037: 62357.463593889726, 2038: 61584.15147290891, 2039: 60810.839351928094, 2040: 60037.52723094728, 2041: 59264.21510996646, 2042: 58490.90298898565, 2043: 57717.59086800483, 2044: 56944.278747024015, 2045: 56170.9666260432, 2046: 55397.65450506238, 2047: 54624.34238408157, 2048: 53851.03026310075, 2049: 53077.718142119935, 2050: 52304.40602113912}</t>
         </is>
       </c>
-      <c r="T220" t="n">
+      <c r="S220" t="n">
         <v>1842237.410244247</v>
       </c>
     </row>
@@ -16336,15 +15236,10 @@
       </c>
       <c r="R221" t="inlineStr">
         <is>
-          <t>{2021: 18164.1222101262, 2022: 14236.469172415776, 2023: 11158.097933527204, 2024: 8745.3671262407, 2025: 6854.3444078335715, 2026: 5372.220123295743, 2027: 4210.577603914951, 2028: 3300.1186384212847, 2029: 2586.52946273438, 2030: 2027.2406524128598, 2031: 1588.8876279996803, 2032: 1245.3202787768028, 2033: 976.0429683030083, 2034: 764.991859692097, 2035: 599.5766215217448, 2036: 469.9293469869368, 2037: 368.3158802941417, 2038: 288.6744327559939, 2039: 226.2539645601055, 2040: 177.33075974357334, 2041: 138.9862865491539, 2042: 108.93309134104463, 2043: 85.37833971785192, 2044: 66.91686431770574, 2045: 52.4473390430425, 2046: 41.10657904763817, 2047: 32.21804712748116, 2048: 25.251494645313635, 2049: 19.79132935336774, 2050: 15.511823085140414}</t>
-        </is>
-      </c>
-      <c r="S221" t="inlineStr">
-        <is>
           <t>{2021: 18164.1222101262, 2022: 17046.61467460892, 2023: 16102.565454939846, 2024: 15158.516235271003, 2025: 14214.46701560216, 2026: 13270.417795933317, 2027: 12326.368576264242, 2028: 11382.319356595399, 2029: 10438.270136926556, 2030: 9494.220917257713, 2031: 8550.171697588637, 2032: 7606.122477919795, 2033: 6662.073258250952, 2034: 5718.024038582109, 2035: 4773.974818913033, 2036: 3829.9255992441904, 2037: 2885.8763795753475, 2038: 1941.8271599065047, 2039: 997.777940237429, 2040: 53.72872056858614, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T221" t="n">
+      <c r="S221" t="n">
         <v>171535.3233592488</v>
       </c>
     </row>
@@ -16408,15 +15303,10 @@
       </c>
       <c r="R222" t="inlineStr">
         <is>
-          <t>{2021: 32974.0144768152, 2022: 23423.24544421403, 2023: 16638.811981042247, 2024: 11819.457931217728, 2025: 8396.007235792742, 2026: 5964.14301854716, 2027: 4236.656894963508, 2028: 3009.529045467827, 2029: 2137.833036770494, 2030: 1518.6196989824703, 2031: 1078.758607651356, 2032: 766.3012236451475, 2033: 544.34565916329, 2034: 386.678485570487, 2035: 274.67887120274247, 2036: 195.11942117467362, 2037: 138.60399364841845, 2038: 98.4579953119726, 2039: 69.94009758075273, 2040: 49.68227551359039, 2041: 35.29203683707154, 2042: 25.069863472104966, 2043: 17.808494800441622, 2044: 12.650347594044069, 2045: 8.98623359488911, 2046: 6.3834130739563895, 2047: 4.53448734027264, 2048: 3.221094295617773, 2049: 2.2881194019691593, 2050: 1.6253763215781887}</t>
-        </is>
-      </c>
-      <c r="S222" t="inlineStr">
-        <is>
           <t>{2021: 32974.0144768152, 2022: 30624.730539163313, 2023: 30743.72678498522, 2024: 30862.72303080713, 2025: 30981.71927662904, 2026: 31100.715522450948, 2027: 31219.711768272857, 2028: 31338.708014094736, 2029: 31457.704259916645, 2030: 31576.700505738554, 2031: 31695.696751560463, 2032: 31814.69299738237, 2033: 31933.68924320428, 2034: 32052.68548902619, 2035: 32171.681734848098, 2036: 32290.677980669978, 2037: 32409.674226491887, 2038: 32528.670472313795, 2039: 32647.666718135704, 2040: 32766.662963957613, 2041: 32885.65920977952, 2042: 33004.65545560143, 2043: 33123.65170142334, 2044: 33242.64794724522, 2045: 33361.64419306713, 2046: 33480.64043888904, 2047: 33599.636684710946, 2048: 33718.632930532855, 2049: 33837.62917635476, 2050: 33956.62542217667}</t>
         </is>
       </c>
-      <c r="T222" t="n">
+      <c r="S222" t="n">
         <v>935938.355966749</v>
       </c>
     </row>
@@ -16480,15 +15370,10 @@
       </c>
       <c r="R223" t="inlineStr">
         <is>
-          <t>{2021: 95883.4634120662, 2022: 75168.09170478022, 2023: 58928.221921395554, 2024: 46196.93356664545, 2025: 36216.20679150658, 2026: 28391.789954477903, 2027: 22257.81792830489, 2028: 17449.0745290765, 2029: 13679.247575031908, 2030: 10723.88188308803, 2031: 8407.01522592009, 2032: 6590.7015555919115, 2033: 5166.797707343005, 2034: 4050.5245645594046, 2035: 3175.419317226615, 2036: 2489.3782717529934, 2037: 1951.5546013898834, 2038: 1529.9263295666499, 2039: 1199.3897440708388, 2040: 940.264724112419, 2041: 737.1229875699083, 2042: 577.8694923569452, 2043: 453.0222986231366, 2044: 355.14801484453847, 2045: 278.41921431099945, 2046: 218.26747062485018, 2047: 171.11135397341616, 2048: 134.14319309605023, 2049: 105.16190677095459, 2050: 82.44195162243065}</t>
-        </is>
-      </c>
-      <c r="S223" t="inlineStr">
-        <is>
           <t>{2021: 95883.4634120662, 2022: 91023.43355966173, 2023: 86281.14977847412, 2024: 81538.86599728651, 2025: 76796.58221609704, 2026: 72054.29843490943, 2027: 67312.01465372182, 2028: 62569.73087253235, 2029: 57827.447091344744, 2030: 53085.163310157135, 2031: 48342.879528967664, 2032: 43600.595747780055, 2033: 38858.311966592446, 2034: 34116.028185402974, 2035: 29373.744404215366, 2036: 24631.460623027757, 2037: 19889.176841840148, 2038: 15146.893060650676, 2039: 10404.609279463068, 2040: 5662.325498275459, 2041: 920.0417170859873, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T223" t="n">
+      <c r="S223" t="n">
         <v>967376.4844735196</v>
       </c>
     </row>
@@ -16552,15 +15437,10 @@
       </c>
       <c r="R224" t="inlineStr">
         <is>
-          <t>{2021: 80120.958481875, 2022: 63247.861658902395, 2023: 49928.159625406915, 2024: 39413.52416029449, 2025: 31113.221444349547, 2026: 24560.92342080733, 2027: 19388.50852721057, 2028: 15305.379869848583, 2029: 12082.138893334895, 2030: 9537.69729854343, 2031: 7529.103129978493, 2032: 5943.50944126829, 2033: 4691.834321911619, 2034: 3703.756092557065, 2035: 2923.7624886047684, 2036: 2308.0318671499117, 2037: 1821.971217067492, 2038: 1438.2726525875923, 2039: 1135.3792001779584, 2040: 896.2736834893922, 2041: 707.5226634323876, 2042: 558.5217199745933, 2043: 440.8996740401778, 2044: 348.04827747357365, 2045: 274.75094808367425, 2046: 216.88969134062006, 2047: 171.21374298407613, 2048: 135.15693440948334, 2049: 106.69352004452328, 2050: 84.22436680165151}</t>
-        </is>
-      </c>
-      <c r="S224" t="inlineStr">
-        <is>
           <t>{2021: 80120.958481875, 2022: 101012.39203483472, 2023: 102813.68436476216, 2024: 104614.9766946896, 2025: 106416.2690246175, 2026: 108217.56135454495, 2027: 110018.85368447285, 2028: 111820.14601440029, 2029: 113621.4383443282, 2030: 115422.73067425564, 2031: 117224.02300418355, 2032: 119025.31533411099, 2033: 120826.60766403843, 2034: 122627.89999396633, 2035: 124429.19232389377, 2036: 126230.48465382168, 2037: 128031.77698374912, 2038: 129833.06931367703, 2039: 131634.36164360447, 2040: 133435.6539735319, 2041: 135236.94630345982, 2042: 137038.23863338726, 2043: 138839.53096331516, 2044: 140640.8232932426, 2045: 142442.1156231705, 2046: 144243.40795309795, 2047: 146044.70028302586, 2048: 147845.9926129533, 2049: 149647.28494288074, 2050: 151448.57727280864}</t>
         </is>
       </c>
-      <c r="T224" t="n">
+      <c r="S224" t="n">
         <v>3625020.245565359</v>
       </c>
     </row>
@@ -16624,15 +15504,10 @@
       </c>
       <c r="R225" t="inlineStr">
         <is>
-          <t>{2021: 39625.5755394863, 2022: 30810.220911067587, 2023: 23955.985488282768, 2024: 18626.586364678198, 2025: 14482.798871727238, 2026: 11260.864393094475, 2027: 8755.701712271295, 2028: 6807.853269353133, 2029: 5293.335435592337, 2030: 4115.74675967713, 2031: 3200.1318631524136, 2032: 2488.2104122379737, 2033: 1934.6674825676066, 2034: 1504.2691927078495, 2035: 1169.6200119758053, 2036: 909.4189916578117, 2037: 707.1039259928627, 2038: 549.7971416267212, 2039: 427.4858133710377, 2040: 332.3846320713864, 2041: 258.4402573877693, 2042: 200.94601312467313, 2043: 156.2422998601001, 2044: 121.48365566440818, 2045: 94.45763795593827, 2046: 73.4439980375823, 2047: 57.1051845512011, 2048: 44.40120622188946, 2049: 34.523434771340554, 2050: 26.84313445123084}</t>
-        </is>
-      </c>
-      <c r="S225" t="inlineStr">
-        <is>
           <t>{2021: 39625.5755394863, 2022: 36904.67575613689, 2023: 35028.17131542647, 2024: 33151.66687471559, 2025: 31275.16243400518, 2026: 29398.6579932943, 2027: 27522.153552583884, 2028: 25645.64911187347, 2029: 23769.14467116259, 2030: 21892.640230452176, 2031: 20016.135789741296, 2032: 18139.631349030882, 2033: 16263.126908320468, 2034: 14386.622467609588, 2035: 12510.118026899174, 2036: 10633.61358618876, 2037: 8757.10914547788, 2038: 6880.604704767466, 2039: 5004.100264056586, 2040: 3127.5958233461715, 2041: 1251.0913826357573, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T225" t="n">
+      <c r="S225" t="n">
         <v>401370.4591574677</v>
       </c>
     </row>
@@ -16696,15 +15571,10 @@
       </c>
       <c r="R226" t="inlineStr">
         <is>
-          <t>{2021: 36571.9935715315, 2022: 28207.435643413133, 2023: 21755.97630523084, 2024: 16780.061504963272, 2025: 12942.212298817942, 2026: 9982.136188126029, 2027: 7699.073433326078, 2028: 5938.181028050609, 2029: 4580.030860501435, 2030: 3532.5098012432545, 2031: 2724.572361181309, 2032: 2101.422209416232, 2033: 1620.795749507323, 2034: 1250.095697023575, 2035: 964.1802504676405, 2036: 743.6579116345124, 2037: 573.5723058716236, 2038: 442.3878034724366, 2039: 341.2071445181844, 2040: 263.16800453452595, 2041: 202.9775745419457, 2042: 156.5535895588932, 2043: 120.74745921604054, 2044: 93.13072250984452, 2045: 71.8303435245572, 2046: 55.401677468039544, 2047: 42.73049126130578, 2048: 32.957393473976715, 2049: 25.419548255512606, 2050: 19.605720155768363}</t>
-        </is>
-      </c>
-      <c r="S226" t="inlineStr">
-        <is>
           <t>{2021: 36571.9935715315, 2022: 35055.708996374626, 2023: 33794.49354217108, 2024: 32533.278087968007, 2025: 31272.06263376493, 2026: 30010.847179561853, 2027: 28749.631725358777, 2028: 27488.4162711557, 2029: 26227.200816952623, 2030: 24965.985362749547, 2031: 23704.76990854647, 2032: 22443.554454343393, 2033: 21182.33900013985, 2034: 19921.123545936774, 2035: 18659.908091733698, 2036: 17398.69263753062, 2037: 16137.477183327544, 2038: 14876.261729124468, 2039: 13615.046274921391, 2040: 12353.830820718314, 2041: 11092.615366515238, 2042: 9831.399912312161, 2043: 8570.184458108619, 2044: 7308.969003905542, 2045: 6047.7535497024655, 2046: 4786.538095499389, 2047: 3525.322641296312, 2048: 2264.1071870932356, 2049: 1002.8917328901589, 2050: 0}</t>
         </is>
       </c>
-      <c r="T226" t="n">
+      <c r="S226" t="n">
         <v>523106.4069954685</v>
       </c>
     </row>
@@ -16768,15 +15638,10 @@
       </c>
       <c r="R227" t="inlineStr">
         <is>
-          <t>{2021: 35500.9478648096, 2022: 27838.926980983448, 2023: 21830.56797254573, 2024: 17118.96792320635, 2025: 13424.252778229176, 2026: 10526.95252787416, 2027: 8254.964455364963, 2028: 6473.330052443982, 2029: 5076.218340424311, 2030: 3980.6393974815987, 2031: 3121.5146690199663, 2032: 2447.811232303885, 2033: 1919.5103865631513, 2034: 1505.2304995985905, 2035: 1180.3629054482753, 2036: 925.6101234527489, 2037: 725.8395673768117, 2038: 569.1846536903739, 2039: 446.3399138840895, 2040: 350.0082397415238, 2041: 274.46742734904404, 2042: 215.23027209655024, 2043: 168.77802395052194, 2044: 132.35136995907516, 2045: 103.78652812749569, 2046: 81.38671646610223, 2047: 63.8213623351652, 2048: 50.04706501475496, 2049: 39.24561659209566, 2050: 30.77539954120554}</t>
-        </is>
-      </c>
-      <c r="S227" t="inlineStr">
-        <is>
           <t>{2021: 35500.9478648096, 2022: 34258.368213813286, 2023: 32633.41336054355, 2024: 31008.458507273812, 2025: 29383.503654004075, 2026: 27758.548800734337, 2027: 26133.5939474646, 2028: 24508.639094194863, 2029: 22883.68424092559, 2030: 21258.729387655854, 2031: 19633.774534386117, 2032: 18008.81968111638, 2033: 16383.864827846643, 2034: 14758.909974576905, 2035: 13133.955121307168, 2036: 11509.000268037431, 2037: 9884.04541476816, 2038: 8259.090561498422, 2039: 6634.135708228685, 2040: 5009.180854958948, 2041: 3384.2260016892105, 2042: 1759.2711484194733, 2043: 134.3162951497361, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T227" t="n">
+      <c r="S227" t="n">
         <v>396070.003530998</v>
       </c>
     </row>
@@ -16840,15 +15705,10 @@
       </c>
       <c r="R228" t="inlineStr">
         <is>
-          <t>{2021: 38584.8137626988, 2022: 29780.34184956487, 2023: 22984.91748933384, 2024: 17740.106364803327, 2025: 13692.081948111294, 2026: 10567.755582669168, 2027: 8156.353319988736, 2028: 6295.196644176011, 2029: 4858.727820400459, 2030: 3750.0394931385626, 2031: 2894.33710220464, 2032: 2233.89307673321, 2033: 1724.1524059085705, 2034: 1330.72685965235, 2035: 1027.075082766268, 2036: 792.7120565635255, 2037: 611.8271343207902, 2038: 472.21742017391944, 2039: 364.4645348448952, 2040: 281.29923099995426, 2041: 217.11099378939733, 2042: 167.56954313973003, 2043: 129.33270350784568, 2044: 99.82093334646342, 2045: 77.04330354120096, 2046: 59.463184940775946, 2047: 45.89458396484806, 2048: 35.42213286093456, 2049: 27.339336976640443, 2050: 21.10091307196851}</t>
-        </is>
-      </c>
-      <c r="S228" t="inlineStr">
-        <is>
           <t>{2021: 38584.8137626988, 2022: 34352.89567818493, 2023: 32344.8560235505, 2024: 30336.816368916072, 2025: 28328.77671428118, 2026: 26320.73705964675, 2027: 24312.697405012324, 2028: 22304.657750377897, 2029: 20296.618095743004, 2030: 18288.578441108577, 2031: 16280.53878647415, 2032: 14272.499131839257, 2033: 12264.45947720483, 2034: 10256.419822570402, 2035: 8248.380167935975, 2036: 6240.340513301082, 2037: 4232.300858666655, 2038: 2224.2612040322274, 2039: 216.22154939780012, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T228" t="n">
+      <c r="S228" t="n">
         <v>330414.461929593</v>
       </c>
     </row>
@@ -16912,15 +15772,10 @@
       </c>
       <c r="R229" t="inlineStr">
         <is>
-          <t>{2021: 18501.3328867235, 2022: 14126.237583709668, 2023: 10785.741194603792, 2024: 8235.18735456688, 2025: 6287.774714893807, 2026: 4800.87570118643, 2027: 3665.5905377219856, 2028: 2798.771479735751, 2029: 2136.9331121883056, 2030: 1631.602708198936, 2031: 1245.7701096109545, 2032: 951.1771206320324, 2033: 726.2478910305422, 2034: 554.5087111387236, 2035: 423.3814852011701, 2036: 323.2625176312234, 2037: 246.8191429193564, 2038: 188.45268470297142, 2039: 143.88841137561698, 2040: 109.86245677970092, 2041: 83.88277620331667, 2042: 64.04663021222183, 2043: 48.90122891973264, 2044: 37.33733034722197, 2045: 28.50800006981102, 2046: 21.766582142389655, 2047: 16.619338326125412, 2048: 12.689286934962874, 2049: 9.688592876450494, 2050: 7.397486746632696}</t>
-        </is>
-      </c>
-      <c r="S229" t="inlineStr">
-        <is>
           <t>{2021: 18501.3328867235, 2022: 17535.46835323563, 2023: 16978.963688151445, 2024: 16422.459023067495, 2025: 15865.954357983544, 2026: 15309.449692899594, 2027: 14752.945027815644, 2028: 14196.440362731693, 2029: 13639.93569764751, 2030: 13083.43103256356, 2031: 12526.92636747961, 2032: 11970.421702395659, 2033: 11413.917037311709, 2034: 10857.412372227525, 2035: 10300.907707143575, 2036: 9744.403042059625, 2037: 9187.898376975674, 2038: 8631.393711891724, 2039: 8074.889046807773, 2040: 7518.38438172359, 2041: 6961.87971663964, 2042: 6405.375051555689, 2043: 5848.870386471739, 2044: 5292.365721387789, 2045: 4735.861056303838, 2046: 4179.356391219655, 2047: 3622.8517261357047, 2048: 3066.3470610517543, 2049: 2509.842395967804, 2050: 1953.3377308838535}</t>
         </is>
       </c>
-      <c r="T229" t="n">
+      <c r="S229" t="n">
         <v>290861.6857976499</v>
       </c>
     </row>
@@ -16984,15 +15839,10 @@
       </c>
       <c r="R230" t="inlineStr">
         <is>
-          <t>{2021: 95076.8950230667, 2022: 71530.77913085358, 2023: 53815.938791707515, 2024: 40488.23881443789, 2025: 30461.18899160696, 2026: 22917.372104896753, 2027: 17241.807085698827, 2028: 12971.815015253625, 2029: 9759.300980088612, 2030: 7342.376954031544, 2031: 5524.012369849469, 2032: 4155.971949314721, 2033: 3126.731384195192, 2034: 2352.385739880468, 2035: 1769.8094237210391, 2036: 1331.5101104340793, 2037: 1001.7571103563209, 2038: 753.6685604454736, 2039: 567.0199823207759, 2040: 426.5955583459869, 2041: 320.9477197887746, 2042: 241.46392718432972, 2043: 181.66456571073758, 2044: 136.6747191586828, 2045: 102.82676087118017, 2046: 77.36136438651067, 2047: 58.20255981067151, 2048: 43.788498242999864, 2049: 32.9441279664411, 2050: 24.785402811633205}</t>
-        </is>
-      </c>
-      <c r="S230" t="inlineStr">
-        <is>
           <t>{2021: 95076.8950230667, 2022: 93354.7234351593, 2023: 92202.93441925291, 2024: 91051.14540334698, 2025: 89899.35638744058, 2026: 88747.56737153418, 2027: 87595.77835562779, 2028: 86443.98933972185, 2029: 85292.20032381546, 2030: 84140.41130790906, 2031: 82988.62229200313, 2032: 81836.83327609673, 2033: 80685.04426019033, 2034: 79533.2552442844, 2035: 78381.466228378, 2036: 77229.67721247161, 2037: 76077.88819656568, 2038: 74926.09918065928, 2039: 73774.31016475288, 2040: 72622.52114884695, 2041: 71470.73213294055, 2042: 70318.94311703416, 2043: 69167.15410112776, 2044: 68015.36508522183, 2045: 66863.57606931543, 2046: 65711.78705340903, 2047: 64559.9980375031, 2048: 63408.209021596704, 2049: 62256.42000569031, 2050: 61104.630989784375}</t>
         </is>
       </c>
-      <c r="T230" t="n">
+      <c r="S230" t="n">
         <v>2256646.771178321</v>
       </c>
     </row>
@@ -17056,15 +15906,10 @@
       </c>
       <c r="R231" t="inlineStr">
         <is>
-          <t>{2021: 29775.6551819717, 2022: 22634.021525238615, 2023: 17205.294972489715, 2024: 13078.638047608689, 2025: 9941.751853360147, 2026: 7557.2417826687715, 2027: 5744.651868615269, 2028: 4366.808161049849, 2029: 3319.4376180724225, 2030: 2523.2768864353457, 2031: 1918.073775797024, 2032: 1458.0274678446476, 2033: 1108.3223824934028, 2034: 842.4933896147529, 2035: 640.4229696667533, 2036: 486.81875149706315, 2037: 370.0562097772345, 2038: 281.2989392326617, 2039: 213.82992940735832, 2040: 162.5432318908899, 2041: 123.55755018374151, 2042: 93.92250929067113, 2043: 71.39537598744803, 2044: 54.2713323023979, 2045: 41.25445757712831, 2046: 31.359655231973775, 2047: 23.838102208219965, 2048: 18.12057921829953, 2049: 13.774393126540238, 2050: 10.470631414081463}</t>
-        </is>
-      </c>
-      <c r="S231" t="inlineStr">
-        <is>
           <t>{2021: 29775.6551819717, 2022: 30144.108102774015, 2023: 29816.78670771187, 2024: 29489.465312649845, 2025: 29162.143917587702, 2026: 28834.82252252556, 2027: 28507.501127463416, 2028: 28180.179732401273, 2029: 27852.85833733913, 2030: 27525.536942276987, 2031: 27198.215547214844, 2032: 26870.8941521527, 2033: 26543.57275709056, 2034: 26216.25136202853, 2035: 25888.92996696639, 2036: 25561.608571904246, 2037: 25234.287176842103, 2038: 24906.96578177996, 2039: 24579.644386717817, 2040: 24252.322991655674, 2041: 23925.00159659353, 2042: 23597.680201531388, 2043: 23270.358806469245, 2044: 22943.03741140722, 2045: 22615.716016345075, 2046: 22288.394621282932, 2047: 21961.07322622079, 2048: 21633.751831158646, 2049: 21306.430436096503, 2050: 20979.10904103436}</t>
         </is>
       </c>
-      <c r="T231" t="n">
+      <c r="S231" t="n">
         <v>745684.921655691</v>
       </c>
     </row>
@@ -17128,15 +15973,10 @@
       </c>
       <c r="R232" t="inlineStr">
         <is>
-          <t>{2021: 73048.6159903349, 2022: 56137.64871764695, 2023: 43141.61960252467, 2024: 33154.2090636915, 2025: 25478.913141560362, 2026: 19580.470570963338, 2027: 15047.534627957903, 2028: 11563.986552773238, 2029: 8886.889998861443, 2030: 6829.549091175963, 2031: 5248.488593282704, 2032: 4033.448203690335, 2033: 3099.693201710365, 2034: 2382.1052011870856, 2035: 1830.6409119429945, 2036: 1406.8422111707903, 2037: 1081.1541434585563, 2038: 830.8638116173929, 2039: 638.5164202830858, 2040: 490.6980100354527, 2041: 377.0999921129699, 2042: 289.80024606443305, 2043: 222.71064538724877, 2044: 171.15248258891071, 2045: 131.53018458283597, 2046: 101.080563919999, 2047: 77.68011909046095, 2048: 59.696945366114164, 2049: 45.87692871447261, 2050: 35.256286152749986}</t>
-        </is>
-      </c>
-      <c r="S232" t="inlineStr">
-        <is>
           <t>{2021: 73048.6159903349, 2022: 68007.75621171016, 2023: 65175.68559788447, 2024: 62343.614984058775, 2025: 59511.54437023308, 2026: 56679.473756406456, 2027: 53847.40314258076, 2028: 51015.33252875507, 2029: 48183.261914928444, 2030: 45351.19130110275, 2031: 42519.120687277056, 2032: 39687.05007345136, 2033: 36854.97945962474, 2034: 34022.908845799044, 2035: 31190.83823197335, 2036: 28358.767618146725, 2037: 25526.69700432103, 2038: 22694.626390495338, 2039: 19862.555776669644, 2040: 17030.48516284302, 2041: 14198.414549017325, 2042: 11366.343935191631, 2043: 8534.273321365006, 2044: 5702.2027075393125, 2045: 2870.132093713619, 2046: 38.06147988792509, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T232" t="n">
+      <c r="S232" t="n">
         <v>887097.0291401435</v>
       </c>
     </row>
@@ -17200,15 +16040,10 @@
       </c>
       <c r="R233" t="inlineStr">
         <is>
-          <t>{2021: 77221.628535876, 2022: 59891.30523625371, 2023: 46450.30817027719, 2024: 36025.78238364475, 2025: 27940.761804982096, 2026: 21670.207240167194, 2027: 16806.910459687646, 2028: 13035.05019907593, 2029: 10109.682805770552, 2030: 7840.835660190877, 2031: 6081.1704018081755, 2032: 4716.414813230193, 2033: 3657.942011268587, 2034: 2837.0150395315995, 2035: 2200.323107838766, 2036: 1706.5196029727713, 2037: 1323.5370500611693, 2038: 1026.5046588583325, 2039: 796.1332209092019, 2040: 617.4624732246187, 2041: 478.88958258173943, 2042: 371.4156604653858, 2043: 288.0613775209715, 2044: 223.41372766917266, 2045: 173.27450885845118, 2046: 134.38769288428253, 2047: 104.22797974001804, 2048: 80.83680527233882, 2049: 62.69515251986682, 2050: 48.62490713539354}</t>
-        </is>
-      </c>
-      <c r="S233" t="inlineStr">
-        <is>
           <t>{2021: 77221.628535876, 2022: 72655.6029271232, 2023: 69332.36477293819, 2024: 66009.12661875226, 2025: 62685.88846456725, 2026: 59362.65031038225, 2027: 56039.41215619631, 2028: 52716.17400201131, 2029: 49392.93584782537, 2030: 46069.697693640366, 2031: 42746.45953945536, 2032: 39423.221385269426, 2033: 36099.98323108442, 2034: 32776.745076898485, 2035: 29453.50692271348, 2036: 26130.268768528476, 2037: 22807.03061434254, 2038: 19483.792460157536, 2039: 16160.5543059716, 2040: 12837.316151786596, 2041: 9514.077997601591, 2042: 6190.839843415655, 2043: 2867.6016892306507, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T233" t="n">
+      <c r="S233" t="n">
         <v>869366.0650478303</v>
       </c>
     </row>
@@ -17272,15 +16107,10 @@
       </c>
       <c r="R234" t="inlineStr">
         <is>
-          <t>{2021: 39717.4925609034, 2022: 30638.051735965793, 2023: 23634.176118653882, 2024: 18231.39035149037, 2025: 14063.684406839711, 2026: 10848.718352356373, 2027: 8368.695320801886, 2028: 6455.606929568743, 2029: 4979.851605483315, 2030: 3841.4547668706036, 2031: 2963.2960768678727, 2032: 2285.8849503866372, 2033: 1763.3303830804168, 2034: 1360.232079645396, 2035: 1049.2822719156077, 2036: 809.4157626714714, 2037: 624.3828704596018, 2038: 481.6486000181928, 2039: 371.54346295362484, 2040: 286.60842128131884, 2041: 221.08957723641336, 2042: 170.54837727394434, 2043: 131.56092365074687, 2044: 101.48602354648105, 2045: 78.28626228422222, 2046: 60.38997931204828, 2047: 46.58479655177795, 2048: 35.935486226231944, 2049: 27.720614146728916, 2050: 21.383666380194764}</t>
-        </is>
-      </c>
-      <c r="S234" t="inlineStr">
-        <is>
           <t>{2021: 39717.4925609034, 2022: 38261.12147500599, 2023: 36934.72128996998, 2024: 35608.32110493397, 2025: 34281.92091989843, 2026: 32955.520734862424, 2027: 31629.120549826417, 2028: 30302.72036479041, 2029: 28976.320179754402, 2030: 27649.91999471886, 2031: 26323.519809682854, 2032: 24997.119624646846, 2033: 23670.71943961084, 2034: 22344.31925457483, 2035: 21017.919069538824, 2036: 19691.518884503283, 2037: 18365.118699467275, 2038: 17038.718514431268, 2039: 15712.31832939526, 2040: 14385.918144359253, 2041: 13059.517959323712, 2042: 11733.117774287704, 2043: 10406.717589251697, 2044: 9080.31740421569, 2045: 7753.917219179682, 2046: 6427.517034144141, 2047: 5101.1168491081335, 2048: 3774.716664072126, 2049: 2448.316479036119, 2050: 1121.9162940001115}</t>
         </is>
       </c>
-      <c r="T234" t="n">
+      <c r="S234" t="n">
         <v>590351.8357840423</v>
       </c>
     </row>
@@ -17344,15 +16174,10 @@
       </c>
       <c r="R235" t="inlineStr">
         <is>
-          <t>{2021: 18138.2408672054, 2022: 14351.578026233074, 2023: 11355.444739707546, 2024: 8984.80466753222, 2025: 7109.075581286996, 2026: 5624.936488945634, 2027: 4450.636393282527, 2028: 3521.4911926807986, 2029: 2786.3206796325712, 2030: 2204.6293757270337, 2031: 1744.375914749161, 2032: 1380.208104572459, 2033: 1092.066449565392, 2034: 864.0792111822807, 2035: 683.688143239387, 2036: 540.9567446560342, 2037: 428.02292607024293, 2038: 338.66594150373726, 2039: 267.9637303254878, 2040: 212.0217948433956, 2041: 167.7586792586127, 2042: 132.736233496095, 2043: 105.0253123152512, 2044: 83.09951198999894, 2045: 65.75109124406005, 2046: 52.02444510510493, 2047: 41.16346721072228, 2048: 32.569901118309915, 2049: 25.77038647949869, 2050: 20.390384879903188}</t>
-        </is>
-      </c>
-      <c r="S235" t="inlineStr">
-        <is>
           <t>{2021: 18138.2408672054, 2022: 16207.206026570406, 2023: 14912.606186018791, 2024: 13618.00634546671, 2025: 12323.40650491463, 2026: 11028.80666436255, 2027: 9734.206823810935, 2028: 8439.606983258855, 2029: 7145.007142706774, 2030: 5850.407302154694, 2031: 4555.807461603079, 2032: 3261.2076210509986, 2033: 1966.6077804989181, 2034: 672.0079399468377, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T235" t="n">
+      <c r="S235" t="n">
         <v>118784.0112159669</v>
       </c>
     </row>
@@ -17416,15 +16241,10 @@
       </c>
       <c r="R236" t="inlineStr">
         <is>
-          <t>{2021: 76539.0082403048, 2022: 59054.39348675559, 2023: 45563.97411290356, 2024: 35155.313845141056, 2025: 27124.413873292153, 2026: 20928.097277428584, 2027: 16147.27078341673, 2028: 12458.579024008612, 2029: 9612.534116717396, 2030: 7416.6413334131175, 2031: 5722.379551592809, 2032: 4415.155898797939, 2033: 3406.555163797942, 2034: 2628.359756709353, 2035: 2027.9357528404948, 2036: 1564.672951315283, 2037: 1207.2381687380996, 2038: 931.4559920224809, 2039: 718.673653253922, 2040: 554.4994334728295, 2041: 427.82926621779694, 2042: 330.09570431135097, 2043: 254.68845310207544, 2044: 196.50727742383873, 2045: 151.6170427445848, 2046: 116.98155891210034, 2047: 90.25822478650058, 2048: 69.63958437014644, 2049: 53.73107794573074, 2050: 41.4567198141955}</t>
-        </is>
-      </c>
-      <c r="S236" t="inlineStr">
-        <is>
           <t>{2021: 76539.0082403048, 2022: 74456.43899118621, 2023: 72069.75850719959, 2024: 69683.0780232139, 2025: 67296.39753922727, 2026: 64909.717055240646, 2027: 62523.03657125402, 2028: 60136.3560872674, 2029: 57749.675603280775, 2030: 55362.99511929415, 2031: 52976.31463530846, 2032: 50589.634151321836, 2033: 48202.95366733521, 2034: 45816.27318334859, 2035: 43429.592699361965, 2036: 41042.91221537534, 2037: 38656.23173138872, 2038: 36269.551247403026, 2039: 33882.8707634164, 2040: 31496.19027942978, 2041: 29109.509795443155, 2042: 26722.82931145653, 2043: 24336.148827469908, 2044: 21949.468343483284, 2045: 19562.787859497592, 2046: 17176.10737551097, 2047: 14789.426891524345, 2048: 12402.746407537721, 2049: 10016.065923551098, 2050: 7629.385439564474}</t>
         </is>
       </c>
-      <c r="T236" t="n">
+      <c r="S236" t="n">
         <v>1224699.265646263</v>
       </c>
     </row>
@@ -17488,15 +16308,10 @@
       </c>
       <c r="R237" t="inlineStr">
         <is>
-          <t>{2021: 25684.0025508181, 2022: 19875.059651257438, 2023: 15379.923567577247, 2024: 11901.451019270413, 2025: 9209.703529521867, 2026: 7126.7477355788105, 2027: 5514.893408215341, 2028: 4267.591674690712, 2029: 3302.3917878012303, 2030: 2555.4908602935598, 2031: 1977.5162841571944, 2032: 1530.2620388388527, 2033: 1184.1631476168911, 2034: 916.3413353950477, 2035: 709.092699467489, 2036: 548.7174233183762, 2037: 424.6141736888135, 2038: 328.5793175785891, 2039: 254.2646351215187, 2040: 196.75768137176215, 2041: 152.2570575349174, 2042: 117.82112600417217, 2043: 91.17355843887555, 2044: 70.55286297393464, 2045: 54.595943813643565, 2046: 42.24799611609998, 2047: 32.69277992369743, 2048: 25.298664017155755, 2049: 19.576873014368815, 2050: 15.149177709970234}</t>
-        </is>
-      </c>
-      <c r="S237" t="inlineStr">
-        <is>
           <t>{2021: 25684.0025508181, 2022: 24714.69669777667, 2023: 23790.396268501645, 2024: 22866.09583922685, 2025: 21941.795409951825, 2026: 21017.494980676798, 2027: 20093.194551402004, 2028: 19168.894122126978, 2029: 18244.59369285195, 2030: 17320.293263577158, 2031: 16395.99283430213, 2032: 15471.692405027105, 2033: 14547.39197575231, 2034: 13623.091546477284, 2035: 12698.791117202258, 2036: 11774.490687927464, 2037: 10850.190258652437, 2038: 9925.889829377411, 2039: 9001.589400102617, 2040: 8077.288970827591, 2041: 7152.988541552797, 2042: 6228.68811227777, 2043: 5304.387683002744, 2044: 4380.08725372795, 2045: 3455.7868244529236, 2046: 2531.486395177897, 2047: 1607.1859659031034, 2048: 682.8855366280768, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T237" t="n">
+      <c r="S237" t="n">
         <v>355709.3614398728</v>
       </c>
     </row>
@@ -17560,15 +16375,10 @@
       </c>
       <c r="R238" t="inlineStr">
         <is>
-          <t>{2021: 221935.89138647, 2022: 161084.15640443141, 2023: 116917.1208966033, 2024: 84860.07229929471, 2025: 61592.620613793595, 2026: 44704.7806027646, 2027: 32447.35146557074, 2028: 23550.738935181518, 2029: 17093.453836489225, 2030: 12406.666511159994, 2031: 9004.93109184031, 2032: 6535.904216966879, 2033: 4743.850174719689, 2034: 3443.152428973559, 2035: 2499.0879164616604, 2036: 1813.872764287266, 2037: 1316.5340776331998, 2038: 955.5587424295219, 2039: 693.5578240974985, 2040: 503.3939139564044, 2041: 365.3703033890434, 2042: 265.1908473612633, 2043: 192.47920499248139, 2044: 139.7040837690288, 2045: 101.39916684769247, 2046: 73.5969254442479, 2047: 53.41767199115257, 2048: 38.77128920441033, 2049: 28.140740892283755, 2050: 20.4249410895671}</t>
-        </is>
-      </c>
-      <c r="S238" t="inlineStr">
-        <is>
           <t>{2021: 221935.89138647, 2022: 217279.27749661868, 2023: 218726.26639888342, 2024: 220173.25530114863, 2025: 221620.24420341337, 2026: 223067.2331056781, 2027: 224514.22200794285, 2028: 225961.21091020806, 2029: 227408.1998124728, 2030: 228855.18871473754, 2031: 230302.17761700274, 2032: 231749.16651926748, 2033: 233196.15542153222, 2034: 234643.14432379743, 2035: 236090.13322606217, 2036: 237537.1221283269, 2037: 238984.11103059212, 2038: 240431.09993285686, 2039: 241878.0888351216, 2040: 243325.0777373868, 2041: 244772.06663965154, 2042: 246219.05554191628, 2043: 247666.04444418103, 2044: 249113.03334644623, 2045: 250560.02224871097, 2046: 252007.0111509757, 2047: 253454.00005324092, 2048: 254900.98895550566, 2049: 256347.9778577704, 2050: 257794.9667600356}</t>
         </is>
       </c>
-      <c r="T238" t="n">
+      <c r="S238" t="n">
         <v>6870647.004034702</v>
       </c>
     </row>
@@ -17632,15 +16442,10 @@
       </c>
       <c r="R239" t="inlineStr">
         <is>
-          <t>{2021: 83502.181146889, 2022: 62854.19247190052, 2023: 47311.931940377865, 2024: 35612.88143080751, 2025: 26806.711791076883, 2026: 20178.086360297253, 2027: 15188.553237594153, 2028: 11432.806130969167, 2029: 8605.7607978619, 2030: 6477.772653679962, 2031: 4875.982442271608, 2032: 3670.274652790497, 2033: 2762.7080668158887, 2034: 2079.5598652669155, 2035: 1565.3370275250106, 2036: 1178.268560893936, 2037: 886.9123883092228, 2038: 667.6012673541735, 2039: 502.5202692484072, 2040: 378.2596489163376, 2041: 284.7255538812567, 2042: 214.32008744585636, 2043: 161.32412162048396, 2044: 121.43272488723444, 2045: 91.40546699041462, 2046: 68.80319455479896, 2047: 51.789895471372006, 2048: 38.983557235839974, 2049: 29.343904267968032, 2050: 22.087894967574762}</t>
-        </is>
-      </c>
-      <c r="S239" t="inlineStr">
-        <is>
           <t>{2021: 83502.181146889, 2022: 85521.89281031396, 2023: 85367.8382081443, 2024: 85213.78360597458, 2025: 85059.72900380485, 2026: 84905.67440163519, 2027: 84751.61979946546, 2028: 84597.56519729574, 2029: 84443.51059512602, 2030: 84289.45599295635, 2031: 84135.40139078663, 2032: 83981.34678861691, 2033: 83827.29218644724, 2034: 83673.23758427752, 2035: 83519.1829821078, 2036: 83365.12837993813, 2037: 83211.07377776841, 2038: 83057.01917559869, 2039: 82902.96457342897, 2040: 82748.9099712593, 2041: 82594.85536908958, 2042: 82440.80076691986, 2043: 82286.74616475019, 2044: 82132.69156258047, 2045: 81978.63696041075, 2046: 81824.58235824102, 2047: 81670.52775607136, 2048: 81516.47315390164, 2049: 81362.41855173191, 2050: 81208.36394956225}</t>
         </is>
       </c>
-      <c r="T239" t="n">
+      <c r="S239" t="n">
         <v>2418735.631616869</v>
       </c>
     </row>
@@ -17704,15 +16509,10 @@
       </c>
       <c r="R240" t="inlineStr">
         <is>
-          <t>{2021: 291976.86744178, 2022: 225966.0971291389, 2023: 174879.18648883, 2024: 135342.11660750615, 2025: 104743.67416484853, 2026: 81062.99467274245, 2027: 62736.095117029385, 2028: 48552.58119222164, 2029: 37575.70719104868, 2030: 29080.508929433105, 2031: 22505.92371542368, 2032: 17417.735140522662, 2033: 13479.895393828614, 2034: 10432.331090269947, 2035: 8073.766805849197, 2036: 6248.431905696506, 2037: 4835.772721580302, 2038: 3742.4906228810837, 2039: 2896.380137934954, 2040: 2241.560166412917, 2041: 1734.7833296604194, 2042: 1342.5797112033965, 2043: 1039.0463466626898, 2044: 804.1364706348702, 2045: 622.3355343888476, 2046: 481.6365523842939, 2047: 372.74710469559477, 2048: 288.47562206634444, 2049: 223.2564209842081, 2050: 172.78211986735857}</t>
-        </is>
-      </c>
-      <c r="S240" t="inlineStr">
-        <is>
           <t>{2021: 291976.86744178, 2022: 277243.2629548088, 2023: 265782.4607527219, 2024: 254321.6585506387, 2025: 242860.8563485518, 2026: 231400.05414646864, 2027: 219939.25194438174, 2028: 208478.44974229857, 2029: 197017.64754021168, 2030: 185556.8453381285, 2031: 174096.0431360416, 2032: 162635.24093395844, 2033: 151174.43873187155, 2034: 139713.63652978465, 2035: 128252.83432770148, 2036: 116792.03212561458, 2037: 105331.22992353141, 2038: 93870.42772144452, 2039: 82409.62551936135, 2040: 70948.82331727445, 2041: 59488.02111519128, 2042: 48027.218913104385, 2043: 36566.416711021215, 2044: 25105.61450893432, 2045: 13644.812306851149, 2046: 2184.010104764253, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T240" t="n">
+      <c r="S240" t="n">
         <v>3638829.346965551</v>
       </c>
     </row>
@@ -17776,15 +16576,10 @@
       </c>
       <c r="R241" t="inlineStr">
         <is>
-          <t>{2021: 61795.375408763, 2022: 48124.517763517026, 2023: 37478.034475095126, 2024: 29186.849726341403, 2025: 22729.90590032465, 2026: 17701.41783309122, 2027: 13785.371337467983, 2028: 10735.663363452593, 2029: 8360.635708094573, 2030: 6511.030299387677, 2031: 5070.60910673335, 2032: 3948.8491883850024, 2033: 3075.253797793667, 2034: 2394.9220316292117, 2035: 1865.0985950161314, 2036: 1452.4868547660983, 2037: 1131.1563200496996, 2038: 880.9130466068319, 2039: 686.0305529195425, 2040: 534.261493063285, 2041: 416.0679750420479, 2042: 324.02215413845005, 2043: 252.33943170442555, 2044: 196.51492337682856, 2045: 153.04035064577474, 2046: 119.18356389081913, 2047: 92.81684106040139, 2048: 72.28317146417731, 2049: 56.292121313626005, 2050: 43.838736704551046}</t>
-        </is>
-      </c>
-      <c r="S241" t="inlineStr">
-        <is>
           <t>{2021: 61795.375408763, 2022: 60695.89867698774, 2023: 58478.62447662093, 2024: 56261.35027625412, 2025: 54044.07607588731, 2026: 51826.8018755205, 2027: 49609.52767515369, 2028: 47392.253474785946, 2029: 45174.979274419136, 2030: 42957.70507405233, 2031: 40740.43087368552, 2032: 38523.15667331871, 2033: 36305.8824729519, 2034: 34088.608272584155, 2035: 31871.334072217345, 2036: 29654.059871850535, 2037: 27436.785671483725, 2038: 25219.511471116915, 2039: 23002.237270750105, 2040: 20784.963070382364, 2041: 18567.688870015554, 2042: 16350.414669648744, 2043: 14133.140469281934, 2044: 11915.866268915124, 2045: 9698.592068548314, 2046: 7481.317868180573, 2047: 5264.043667813763, 2048: 3046.769467446953, 2049: 829.4952670801431, 2050: 0}</t>
         </is>
       </c>
-      <c r="T241" t="n">
+      <c r="S241" t="n">
         <v>892253.2029213356</v>
       </c>
     </row>
@@ -17848,15 +16643,10 @@
       </c>
       <c r="R242" t="inlineStr">
         <is>
-          <t>{2021: 175701.494107733, 2022: 85685.75830887223, 2023: 41787.06171083907, 2024: 20378.631885722247, 2025: 9938.211028272757, 2026: 4846.647164360504, 2027: 2363.603335547831, 2028: 1152.677415614999, 2029: 562.1354499235034, 2030: 274.14110815392615, 2031: 133.69259524566485, 2032: 65.19894131851747, 2033: 31.796091183990427, 2034: 15.50625507309419, 2035: 7.562059908575338, 2036: 3.6878504701052512, 2037: 1.7984836478791897, 2038: 0.877080960279966, 2039: 0.4277331138332931, 2040: 0.20859604181936117, 2041: 0.10172770649611969, 2042: 0.049610367381382296, 2043: 0.02419388617406409, 2044: 0.011798826719094921, 2045: 0.005754028556870069, 2046: 0.0028061133044435353, 2047: 0.001368479804983496, 2048: 0.000667377533787446, 2049: 0.00032546536016261245, 2050: 0.0001587223052964137}</t>
-        </is>
-      </c>
-      <c r="S242" t="inlineStr">
-        <is>
           <t>{2021: 175701.494107733, 2022: 175919.20989701152, 2023: 192962.6390188858, 2024: 210006.06814076751, 2025: 227049.49726264924, 2026: 244092.9263845235, 2027: 261136.35550640523, 2028: 278179.78462828696, 2029: 295223.21375016123, 2030: 312266.64287204295, 2031: 329310.0719939172, 2032: 346353.50111579895, 2033: 363396.9302376807, 2034: 380440.35935955495, 2035: 397483.78848143667, 2036: 414527.2176033184, 2037: 431570.64672519267, 2038: 448614.0758470744, 2039: 465657.50496894866, 2040: 482700.9340908304, 2041: 499744.3632127121, 2042: 516787.7923345864, 2043: 533831.2214564681, 2044: 550874.6505783498, 2045: 567918.0797002241, 2046: 584961.5088221058, 2047: 602004.9379439801, 2048: 619048.3670658618, 2049: 636091.7961877435, 2050: 653135.2253096178}</t>
         </is>
       </c>
-      <c r="T242" t="n">
+      <c r="S242" t="n">
         <v>11782572.44489519</v>
       </c>
     </row>
@@ -17920,15 +16710,10 @@
       </c>
       <c r="R243" t="inlineStr">
         <is>
-          <t>{2021: 466991.936441858, 2022: 379102.26470112713, 2023: 307753.7659355642, 2024: 249833.32801293192, 2025: 202813.7384323209, 2026: 164643.41576863086, 2027: 133656.89408169966, 2028: 108502.15450261749, 2029: 88081.63329392974, 2030: 71504.3324189397, 2031: 58046.943085359286, 2032: 47122.28598700209, 2033: 38253.69121291204, 2034: 31054.199955759006, 2035: 25209.680538403936, 2036: 20465.122068956207, 2037: 16613.50768246564, 2038: 13486.78188116091, 2039: 10948.517855864087, 2040: 8887.96484561049, 2041: 7215.215806995946, 2042: 5857.284546668158, 2043: 4754.921152513893, 2044: 3860.02677289855, 2045: 3133.5549443582627, 2046: 2543.807897461488, 2047: 2065.0535044352505, 2048: 1676.4025225473488, 2049: 1360.8971445859377, 2050: 1104.7710876311025}</t>
-        </is>
-      </c>
-      <c r="S243" t="inlineStr">
-        <is>
           <t>{2021: 466991.936441858, 2022: 447233.02179344, 2023: 409330.2044853866, 2024: 371427.38717733324, 2025: 333524.56986927986, 2026: 295621.7525612265, 2027: 257718.9352531731, 2028: 219816.11794511974, 2029: 181913.30063706636, 2030: 144010.483329013, 2031: 106107.66602094471, 2032: 68204.84871289134, 2033: 30302.031404837966, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T243" t="n">
+      <c r="S243" t="n">
         <v>3098706.287410642</v>
       </c>
     </row>
@@ -17992,15 +16777,10 @@
       </c>
       <c r="R244" t="inlineStr">
         <is>
-          <t>{2021: 33989.8922974653, 2022: 26307.749236753414, 2023: 20361.867105872272, 2024: 15759.829102292628, 2025: 12197.909555250964, 2026: 9441.028614735296, 2027: 7307.237432817382, 2028: 5655.709889092911, 2029: 4377.448337168702, 2030: 3388.089969313178, 2031: 2622.339033151261, 2032: 2029.6574373975977, 2033: 1570.9293348819876, 2034: 1215.8795517518322, 2035: 941.0754841364617, 2036: 728.3805912902105, 2037: 563.7574187315089, 2038: 436.3411532037694, 2039: 337.7225658645759, 2040: 261.3930193306542, 2041: 202.314910109365, 2042: 156.58919644209607, 2043: 121.19806903567576, 2044: 93.80578144424, 2045: 72.60449528923029, 2046: 56.194966398071, 2047: 43.494197375802834, 2048: 33.66396185673726, 2049: 26.05548317399989, 2050: 20.166616345387865}</t>
-        </is>
-      </c>
-      <c r="S244" t="inlineStr">
-        <is>
           <t>{2021: 33989.8922974653, 2022: 32534.943696273025, 2023: 31263.527658886276, 2024: 29992.111621499527, 2025: 28720.69558411278, 2026: 27449.279546725564, 2027: 26177.863509338815, 2028: 24906.447471952066, 2029: 23635.031434565317, 2030: 22363.615397178568, 2031: 21092.19935979182, 2032: 19820.78332240507, 2033: 18549.367285017855, 2034: 17277.951247631107, 2035: 16006.535210244358, 2036: 14735.119172857609, 2037: 13463.70313547086, 2038: 12192.28709808411, 2039: 10920.871060696896, 2040: 9649.455023310147, 2041: 8378.038985923398, 2042: 7106.622948536649, 2043: 5835.2069111499, 2044: 4563.7908737631515, 2045: 3292.374836375937, 2046: 2020.958798989188, 2047: 749.542761602439, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T244" t="n">
+      <c r="S244" t="n">
         <v>449693.2701011151</v>
       </c>
     </row>
@@ -18064,15 +16844,10 @@
       </c>
       <c r="R245" t="inlineStr">
         <is>
-          <t>{2021: 13009.6628354071, 2022: 10467.679285622567, 2023: 8422.378889669588, 2024: 6776.7137514982605, 2025: 5452.59835390132, 2026: 4387.20446210292, 2027: 3529.979973405557, 2028: 2840.2502596542954, 2029: 2285.2881881036883, 2030: 1838.761244694651, 2031: 1479.4820769614103, 2032: 1190.403170811628, 2033: 957.8079593831667, 2034: 770.6599827285884, 2035: 620.0792164660168, 2036: 498.92072160248904, 2037: 401.43562279512474, 2038: 322.9983287350912, 2039: 259.88705147601326, 2040: 209.10721052148338, 2041: 168.24934233443983, 2042: 135.3747731863279, 2043: 108.92363061260188, 2044: 87.640828690443, 2045: 70.5165151983002, 2046: 56.73815492178647, 2047: 45.651975496461304, 2048: 36.73194642304531, 2049: 29.55481933372315, 2050: 23.78004518979144}</t>
-        </is>
-      </c>
-      <c r="S245" t="inlineStr">
-        <is>
           <t>{2021: 13009.6628354071, 2022: 10185.11928575486, 2023: 8686.143603522796, 2024: 7187.167921290733, 2025: 5688.19223905867, 2026: 4189.216556826606, 2027: 2690.240874595009, 2028: 1191.2651923629455, 2029: 0, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T245" t="n">
+      <c r="S245" t="n">
         <v>46322.17709111517</v>
       </c>
     </row>
@@ -18136,15 +16911,10 @@
       </c>
       <c r="R246" t="inlineStr">
         <is>
-          <t>{2021: 89584.2704334941, 2022: 68297.89024873951, 2023: 52069.42903990934, 2024: 39697.05990430928, 2025: 30264.52554028358, 2026: 23073.283220127036, 2027: 17590.772994196675, 2028: 13410.978038159554, 2029: 10224.356371339289, 2030: 7794.917187299518, 2031: 5942.744144480401, 2032: 4530.671348798653, 2033: 3454.125294943142, 2034: 2633.3804936722354, 2035: 2007.6552621313003, 2036: 1530.6104306798197, 2037: 1166.9176151381753, 2038: 889.6429118903692, 2039: 678.2522608359602, 2040: 517.0907598775776, 2041: 394.22331393516544, 2042: 300.55076073457246, 2043: 229.13601652941858, 2044: 174.6903383064053, 2045: 133.18165672871575, 2046: 101.53597423284118, 2047: 77.40971479587624, 2048: 59.01616633960209, 2049: 44.99316266191855, 2050: 34.30220585106729}</t>
-        </is>
-      </c>
-      <c r="S246" t="inlineStr">
-        <is>
           <t>{2021: 89584.2704334941, 2022: 87254.38110717945, 2023: 85236.22292087693, 2024: 83218.06473457394, 2025: 81199.90654827096, 2026: 79181.74836196797, 2027: 77163.59017566545, 2028: 75145.43198936246, 2029: 73127.27380305948, 2030: 71109.11561675649, 2031: 69090.95743045397, 2032: 67072.79924415099, 2033: 65054.641057848, 2034: 63036.48287154501, 2035: 61018.32468524249, 2036: 59000.16649893951, 2037: 56982.00831263652, 2038: 54963.850126333535, 2039: 52945.691940031014, 2040: 50927.53375372803, 2041: 48909.37556742504, 2042: 46891.21738112206, 2043: 44873.059194819536, 2044: 42854.90100851655, 2045: 40836.742822213564, 2046: 38818.58463591058, 2047: 36800.42644960806, 2048: 34782.26826330507, 2049: 32764.110077002086, 2050: 30745.951890699565}</t>
         </is>
       </c>
-      <c r="T246" t="n">
+      <c r="S246" t="n">
         <v>1740423.987740642</v>
       </c>
     </row>
@@ -18208,15 +16978,10 @@
       </c>
       <c r="R247" t="inlineStr">
         <is>
-          <t>{2021: 29546.2176247229, 2022: 23029.83199484654, 2023: 17950.62801091216, 2024: 13991.63684990188, 2025: 10905.79681226342, 2026: 8500.535383121309, 2027: 6625.751702841464, 2028: 5164.449490425711, 2029: 4025.4358652951396, 2030: 3137.6304358567186, 2031: 2445.62951229447, 2032: 1906.2486273252166, 2033: 1485.8276001789345, 2034: 1158.129965738645, 2035: 902.7056822610309, 2036: 703.614942099034, 2037: 548.4334445585876, 2038: 427.4770547269909, 2039: 333.1974629394462, 2040: 259.7111308820707, 2041: 202.43212811107767, 2042: 157.7859460717046, 2043: 122.98643011884847, 2044: 95.86190893392155, 2045: 74.71967090658009, 2046: 58.24033010062488, 2047: 45.39548968932953, 2048: 35.383564629073305, 2049: 27.57975857134761, 2050: 21.497073311512278}</t>
-        </is>
-      </c>
-      <c r="S247" t="inlineStr">
-        <is>
           <t>{2021: 29546.2176247229, 2022: 26969.49690903211, 2023: 25376.282107915264, 2024: 23783.067306798883, 2025: 22189.852505682036, 2026: 20596.637704565655, 2027: 19003.42290344881, 2028: 17410.208102331962, 2029: 15816.993301215582, 2030: 14223.778500098735, 2031: 12630.563698982354, 2032: 11037.348897865508, 2033: 9444.134096749127, 2034: 7850.91929563228, 2035: 6257.704494515434, 2036: 4664.489693399053, 2037: 3071.2748922822066, 2038: 1478.0600911658257, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T247" t="n">
+      <c r="S247" t="n">
         <v>256577.3433140423</v>
       </c>
     </row>
@@ -18280,15 +17045,10 @@
       </c>
       <c r="R248" t="inlineStr">
         <is>
-          <t>{2021: 58851.761582854, 2022: 45271.15045754338, 2023: 34824.39622243405, 2024: 26788.33119989785, 2025: 20606.665622909768, 2026: 15851.478949014578, 2027: 12193.597424694455, 2028: 9379.807312222962, 2029: 7215.326384013036, 2030: 5550.320288562142, 2031: 4269.530394894037, 2032: 3284.2951118495503, 2033: 2526.412364839613, 2034: 1943.418365233335, 2035: 1494.9558492071346, 2036: 1149.9803804778257, 2037: 884.6113256022259, 2038: 680.4787374360052, 2039: 523.4517111650849, 2040: 402.6601844373186, 2041: 309.74246654045567, 2042: 238.26640747367, 2043: 183.2841378338867, 2044: 140.9895567642007, 2045: 108.45485785890314, 2046: 83.42785425495812, 2047: 64.17607291175072, 2048: 49.36682563820797, 2049: 37.9749548861379, 2050: 29.211868090786915}</t>
-        </is>
-      </c>
-      <c r="S248" t="inlineStr">
-        <is>
           <t>{2021: 58851.761582854, 2022: 59469.70359059004, 2023: 58317.34329282213, 2024: 57164.982995054685, 2025: 56012.62269728677, 2026: 54860.26239951886, 2027: 53707.90210175142, 2028: 52555.541803983506, 2029: 51403.181506215595, 2030: 50250.82120844815, 2031: 49098.46091068024, 2032: 47946.10061291233, 2033: 46793.740315144416, 2034: 45641.38001737697, 2035: 44489.01971960906, 2036: 43336.65942184115, 2037: 42184.2991240737, 2038: 41031.93882630579, 2039: 39879.57852853788, 2040: 38727.218230770435, 2041: 37574.857933002524, 2042: 36422.49763523461, 2043: 35270.1373374667, 2044: 34117.77703969926, 2045: 32965.416741931345, 2046: 31813.056444163434, 2047: 30660.69614639599, 2048: 29508.335848628078, 2049: 28355.975550860167, 2050: 27203.61525309272}</t>
         </is>
       </c>
-      <c r="T248" t="n">
+      <c r="S248" t="n">
         <v>1272587.196398278</v>
       </c>
     </row>
@@ -18352,15 +17112,10 @@
       </c>
       <c r="R249" t="inlineStr">
         <is>
-          <t>{2021: 24562.7675003953, 2022: 19220.026237867874, 2023: 15039.405009162116, 2024: 11768.126652396371, 2025: 9208.39653047933, 2026: 7205.443072392225, 2027: 5638.159661960448, 2028: 4411.782045098302, 2029: 3452.158502138617, 2030: 2701.266336837454, 2031: 2113.703590959348, 2032: 1653.9438594067383, 2033: 1294.1882209830942, 2034: 1012.6844038903312, 2035: 792.411555951035, 2036: 620.0510954770667, 2037: 485.18141629179814, 2038: 379.64775553504626, 2039: 297.0691239256247, 2040: 232.45248550347762, 2041: 181.8908586079537, 2042: 142.32708406399743, 2043: 111.36897705135355, 2044: 87.14468599587046, 2045: 68.18951290014166, 2046: 53.357351815794395, 2047: 41.75139067151986, 2048: 32.66988641085209, 2049: 25.563734786588473, 2050: 20.00326931109122}</t>
-        </is>
-      </c>
-      <c r="S249" t="inlineStr">
-        <is>
           <t>{2021: 24562.7675003953, 2022: 21235.194614964537, 2023: 19537.56798189925, 2024: 17839.94134883443, 2025: 16142.314715769142, 2026: 14444.688082703855, 2027: 12747.061449638568, 2028: 11049.43481657328, 2029: 9351.80818350846, 2030: 7654.1815504431725, 2031: 5956.554917377885, 2032: 4258.928284312598, 2033: 2561.3016512473114, 2034: 863.6750181820244, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T249" t="n">
+      <c r="S249" t="n">
         <v>155924.0363656522</v>
       </c>
     </row>
@@ -18424,15 +17179,10 @@
       </c>
       <c r="R250" t="inlineStr">
         <is>
-          <t>{2021: 64177.5873165772, 2022: 49516.44193209513, 2023: 38204.583938624055, 2024: 29476.880344613517, 2025: 22742.99011465575, 2026: 17547.433558376815, 2027: 13538.78372779258, 2028: 10445.895932196752, 2029: 8059.567537244019, 2030: 6218.387518794416, 2031: 4797.818636695842, 2032: 3701.7737477848177, 2033: 2856.1164807233986, 2034: 2203.6466589405395, 2035: 1700.2312861658415, 2036: 1311.8193947876252, 2037: 1012.1388416641087, 2038: 780.9192628768924, 2039: 602.5209882564417, 2040: 464.87717558933986, 2041: 358.6776105663927, 2042: 276.7389647782203, 2043: 213.51891606946262, 2044: 164.7412663988771, 2045: 127.10670021328055, 2046: 98.0696190594471, 2047: 75.66595754847695, 2048: 58.38033416095325, 2049: 45.04355098606917, 2050: 34.753509286893134}</t>
-        </is>
-      </c>
-      <c r="S250" t="inlineStr">
-        <is>
           <t>{2021: 64177.5873165772, 2022: 62247.65712211002, 2023: 60200.87116045691, 2024: 58154.085198803805, 2025: 56107.2992371507, 2026: 54060.51327549713, 2027: 52013.72731384402, 2028: 49966.941352190915, 2029: 47920.155390537344, 2030: 45873.36942888424, 2031: 43826.58346723113, 2032: 41779.797505578026, 2033: 39733.011543924455, 2034: 37686.22558227135, 2035: 35639.43962061824, 2036: 33592.65365896467, 2037: 31545.867697311565, 2038: 29499.08173565846, 2039: 27452.295774005353, 2040: 25405.509812351782, 2041: 23358.723850698676, 2042: 21311.93788904557, 2043: 19265.151927392, 2044: 17218.365965738893, 2045: 15171.580004085787, 2046: 13124.79404243268, 2047: 11078.00808077911, 2048: 9031.222119126003, 2049: 6984.436157472897, 2050: 4937.650195819326}</t>
         </is>
       </c>
-      <c r="T250" t="n">
+      <c r="S250" t="n">
         <v>1003806.92467036</v>
       </c>
     </row>
@@ -18496,15 +17246,10 @@
       </c>
       <c r="R251" t="inlineStr">
         <is>
-          <t>{2021: 191695.965846031, 2022: 146073.7987912908, 2023: 111309.35697654013, 2024: 84818.58521549962, 2025: 64632.413602705834, 2026: 49250.395741661945, 2027: 37529.17995017852, 2028: 28597.523461957742, 2029: 21791.53259524749, 2030: 16605.315263800283, 2031: 12653.3778110831, 2032: 9641.971109036804, 2033: 7347.256065180479, 2034: 5598.665571268648, 2035: 4266.226180336473, 2036: 3250.8971271995592, 2037: 2477.208587848672, 2038: 1887.6519765476153, 2039: 1438.4053091219903, 2040: 1096.0758969428277, 2041: 835.218254715949, 2042: 636.4427271473364, 2043: 484.97424793055586, 2044: 369.5541030219983, 2045: 281.60306581876364, 2046: 214.5836997345053, 2047: 163.51442786273887, 2048: 124.59925032683877, 2049: 94.94558605582237, 2050: 72.34926604965139}</t>
-        </is>
-      </c>
-      <c r="S251" t="inlineStr">
-        <is>
           <t>{2021: 191695.965846031, 2022: 194916.25888834894, 2023: 192712.79497997463, 2024: 190509.3310715994, 2025: 188305.86716322508, 2026: 186102.40325485077, 2027: 183898.93934647646, 2028: 181695.47543810215, 2029: 179492.01152972784, 2030: 177288.54762135353, 2031: 175085.08371297922, 2032: 172881.6198046049, 2033: 170678.1558962306, 2034: 168474.6919878563, 2035: 166271.22807948198, 2036: 164067.76417110767, 2037: 161864.30026273336, 2038: 159660.83635435905, 2039: 157457.37244598474, 2040: 155253.9085376095, 2041: 153050.4446292352, 2042: 150846.98072086088, 2043: 148643.51681248657, 2044: 146440.05290411226, 2045: 144236.58899573795, 2046: 142033.12508736365, 2047: 139829.66117898934, 2048: 137626.19727061503, 2049: 135422.73336224072, 2050: 133219.2694538664}</t>
         </is>
       </c>
-      <c r="T251" t="n">
+      <c r="S251" t="n">
         <v>4787203.509158196</v>
       </c>
     </row>
@@ -18568,15 +17313,10 @@
       </c>
       <c r="R252" t="inlineStr">
         <is>
-          <t>{2021: 18576.8750164496, 2022: 13697.012023079698, 2023: 10099.01494165542, 2024: 7446.157061111165, 2025: 5490.1646644803495, 2026: 4047.9817704262405, 2027: 2984.6384243657526, 2028: 2200.619229385139, 2029: 1622.549972286422, 2030: 1196.3307315560655, 2031: 882.0728136025791, 2032: 650.36567896635, 2033: 479.52449033072014, 2034: 353.56068787700326, 2035: 260.68566367871176, 2036: 192.20749811203922, 2037: 141.71750685922538, 2038: 104.49046966257042, 2039: 77.042409877773, 2040: 56.80453862387934, 2041: 41.88284885417026, 2042: 30.880860414274327, 2043: 22.768927282054786, 2044: 16.7878758111242, 2045: 12.377955744619292, 2046: 9.126454718841154, 2047: 6.729073641361593, 2048: 4.961448170820154, 2049: 3.658151071557261, 2050: 2.6972103308545514}</t>
-        </is>
-      </c>
-      <c r="S252" t="inlineStr">
-        <is>
           <t>{2021: 18576.8750164496, 2022: 17413.519918653823, 2023: 17194.253297938325, 2024: 16974.986677222827, 2025: 16755.72005650733, 2026: 16536.45343579183, 2027: 16317.186815076333, 2028: 16097.920194360835, 2029: 15878.653573645337, 2030: 15659.386952929839, 2031: 15440.120332214341, 2032: 15220.853711498901, 2033: 15001.587090783403, 2034: 14782.320470067905, 2035: 14563.053849352407, 2036: 14343.78722863691, 2037: 14124.520607921411, 2038: 13905.253987205913, 2039: 13685.987366490415, 2040: 13466.720745774917, 2041: 13247.45412505942, 2042: 13028.187504343921, 2043: 12808.920883628482, 2044: 12589.654262912984, 2045: 12370.387642197486, 2046: 12151.121021481988, 2047: 11931.85440076649, 2048: 11712.587780050992, 2049: 11493.321159335494, 2050: 11274.054538619996}</t>
         </is>
       </c>
-      <c r="T252" t="n">
+      <c r="S252" t="n">
         <v>419621.239869385</v>
       </c>
     </row>
@@ -18640,15 +17380,10 @@
       </c>
       <c r="R253" t="inlineStr">
         <is>
-          <t>{2021: 58096.946436543, 2022: 44295.95777115461, 2023: 33773.40798809576, 2024: 25750.50059924776, 2025: 19633.443013674558, 2026: 14969.498673841974, 2027: 11413.479051538867, 2028: 8702.195504218775, 2029: 6634.980118830209, 2030: 5058.833848990182, 2031: 3857.102727264966, 2032: 2940.8440547310247, 2033: 2242.243560979622, 2034: 1709.5963244519662, 2035: 1303.4799802492266, 2036: 993.8369863161582, 2037: 757.7500002578736, 2038: 577.745717654493, 2039: 440.5016353078338, 2040: 335.8600241930621, 2041: 256.0761341376979, 2042: 195.2449882431197, 2043: 148.86434287373945, 2044: 113.50146694488156, 2045: 86.53907812945188, 2046: 65.98163217689672, 2047: 50.307628401297194, 2048: 38.357000150856805, 2049: 29.245255785798328, 2050: 22.29801555421337}</t>
-        </is>
-      </c>
-      <c r="S253" t="inlineStr">
-        <is>
           <t>{2021: 58096.946436543, 2022: 57339.76715920167, 2023: 56216.254389686044, 2024: 55092.74162017042, 2025: 53969.22885065479, 2026: 52845.716081139166, 2027: 51722.20331162354, 2028: 50598.690542107914, 2029: 49475.17777259229, 2030: 48351.66500307666, 2031: 47228.152233561035, 2032: 46104.63946404541, 2033: 44981.12669452978, 2034: 43857.61392501416, 2035: 42734.10115549853, 2036: 41610.588385982905, 2037: 40487.07561646728, 2038: 39363.56284695119, 2039: 38240.05007743556, 2040: 37116.537307919934, 2041: 35993.02453840431, 2042: 34869.51176888868, 2043: 33745.998999373056, 2044: 32622.48622985743, 2045: 31498.973460341804, 2046: 30375.460690826178, 2047: 29251.94792131055, 2048: 28128.435151794925, 2049: 27004.9223822793, 2050: 25881.409612763673}</t>
         </is>
       </c>
-      <c r="T253" t="n">
+      <c r="S253" t="n">
         <v>1222814.831605388</v>
       </c>
     </row>
@@ -18712,15 +17447,10 @@
       </c>
       <c r="R254" t="inlineStr">
         <is>
-          <t>{2021: 85979.9412789594, 2022: 66733.88067599245, 2023: 51795.92779237471, 2024: 40201.74023594644, 2025: 31202.837498673893, 2026: 24218.28165284469, 2027: 18797.174014749162, 2028: 14589.546690619909, 2029: 11323.76986406373, 2030: 8789.016317876392, 2031: 6821.651160630012, 2032: 5294.668126019428, 2033: 4109.4904891174565, 2034: 3189.6072951494493, 2035: 2475.6340778039953, 2036: 1921.4792041969154, 2037: 1491.3683590251203, 2038: 1157.5350789346053, 2039: 898.4282460169691, 2040: 697.3208224359374, 2041: 541.2300109201469, 2042: 420.0791304314356, 2043: 326.0471006107364, 2044: 253.063539975164, 2045: 196.41688315829964, 2046: 152.4502186028354, 2047: 118.32521104268562, 2048: 91.83886842938037, 2049: 71.28132441146757, 2050: 55.3254552973935}</t>
-        </is>
-      </c>
-      <c r="S254" t="inlineStr">
-        <is>
           <t>{2021: 85979.9412789594, 2022: 76254.63231541775, 2023: 71345.11011238582, 2024: 66435.5879093539, 2025: 61526.06570632197, 2026: 56616.54350328818, 2027: 51707.02130025625, 2028: 46797.499097224325, 2029: 41887.976894190535, 2030: 36978.45469115861, 2031: 32068.93248812668, 2032: 27159.410285094753, 2033: 22249.888082060963, 2034: 17340.365879029036, 2035: 12430.843675997108, 2036: 7521.321472963318, 2037: 2611.799269931391, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T254" t="n">
+      <c r="S254" t="n">
         <v>673921.4233222803</v>
       </c>
     </row>
@@ -18784,15 +17514,10 @@
       </c>
       <c r="R255" t="inlineStr">
         <is>
-          <t>{2021: 27988.1283048806, 2022: 21398.41105754103, 2023: 16360.222119878112, 2024: 12508.25900540049, 2025: 9563.228555196909, 2026: 7311.596310841292, 2027: 5590.10383409238, 2028: 4273.931375231888, 2029: 3267.6476041088285, 2030: 2498.2901986953043, 2031: 1910.0755874191727, 2032: 1460.354266113686, 2033: 1116.5184229373795, 2034: 853.6376533319391, 2035: 652.6513384964799, 2036: 498.98662269483293, 2037: 381.5017834821134, 2038: 291.6783821057343, 2039: 223.0036195671088, 2040: 170.49811501630003, 2041: 130.35486724628484, 2042: 99.6632215738691, 2043: 76.19782785491059, 2044: 58.25728767460296, 2045: 44.54079155200912, 2046: 34.053801528841035, 2047: 26.035940497635522, 2048: 19.905859762009587, 2049: 15.219087357369604, 2050: 11.635800852636187}</t>
-        </is>
-      </c>
-      <c r="S255" t="inlineStr">
-        <is>
           <t>{2021: 27988.1283048806, 2022: 27363.24114322639, 2023: 26704.895302629564, 2024: 26046.549462032504, 2025: 25388.203621435678, 2026: 24729.857780838618, 2027: 24071.51194024179, 2028: 23413.16609964473, 2029: 22754.820259047905, 2030: 22096.474418450845, 2031: 21438.12857785402, 2032: 20779.782737257192, 2033: 20121.436896660132, 2034: 19463.091056063306, 2035: 18804.745215466246, 2036: 18146.39937486942, 2037: 17488.05353427236, 2038: 16829.707693675533, 2039: 16171.361853078473, 2040: 15513.016012481647, 2041: 14854.670171884587, 2042: 14196.32433128776, 2043: 13537.9784906907, 2044: 12879.632650093874, 2045: 12221.286809496814, 2046: 11562.940968899988, 2047: 10904.595128302928, 2048: 10246.249287706101, 2049: 9587.903447109275, 2050: 8929.557606512215}</t>
         </is>
       </c>
-      <c r="T255" t="n">
+      <c r="S255" t="n">
         <v>535774.8672203948</v>
       </c>
     </row>
@@ -18856,15 +17581,10 @@
       </c>
       <c r="R256" t="inlineStr">
         <is>
-          <t>{2021: 48351.5039526337, 2022: 37469.197527830016, 2023: 29036.134320762332, 2024: 22501.07159800119, 2025: 17436.832929111588, 2026: 13512.385011243592, 2027: 10471.19906661761, 2028: 8114.482365733185, 2029: 6288.183773882156, 2030: 4872.9239145425245, 2031: 3776.1917162068985, 2032: 2926.2972555335514, 2033: 2267.685613257147, 2034: 1757.3054244059806, 2035: 1361.79474641157, 2036: 1055.3002941882007, 2037: 817.7874924604288, 2038: 633.7308787914044, 2039: 491.09925309007946, 2040: 380.56923602269165, 2041: 294.91582912330233, 2042: 228.54013944074796, 2043: 177.10339757232637, 2044: 137.24334599784152, 2045: 106.35445891426792, 2046: 82.41762723509088, 2047: 63.86817580011334, 2048: 49.493585497173896, 2049: 38.354234713585136, 2050: 29.72197923605224}</t>
-        </is>
-      </c>
-      <c r="S256" t="inlineStr">
-        <is>
           <t>{2021: 48351.5039526337, 2022: 46298.34538530558, 2023: 44449.421592939645, 2024: 42600.49780057371, 2025: 40751.5740082073, 2026: 38902.650215841364, 2027: 37053.726423475426, 2028: 35204.80263110902, 2029: 33355.87883874308, 2030: 31506.955046377145, 2031: 29658.031254011206, 2032: 27809.107461644802, 2033: 25960.183669278864, 2034: 24111.259876912925, 2035: 22262.336084546987, 2036: 20413.412292180583, 2037: 18564.488499814644, 2038: 16715.564707448706, 2039: 14866.640915082302, 2040: 13017.717122716364, 2041: 11168.793330350425, 2042: 9319.869537984487, 2043: 7470.945745618083, 2044: 5622.021953252144, 2045: 3773.0981608862057, 2046: 1924.1743685202673, 2047: 75.25057615386322, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T256" t="n">
+      <c r="S256" t="n">
         <v>627032.4994752919</v>
       </c>
     </row>
@@ -18928,15 +17648,10 @@
       </c>
       <c r="R257" t="inlineStr">
         <is>
-          <t>{2021: 27235.1355432164, 2022: 20923.274645279067, 2023: 16074.214912097948, 2024: 12348.9458232873, 2025: 9487.024018305949, 2026: 7288.365016079964, 2027: 5599.254782650347, 2028: 4301.603178746283, 2029: 3304.6879675372734, 2030: 2538.812184430407, 2031: 1950.431438952366, 2032: 1498.4104855740961, 2033: 1151.1473504981952, 2034: 884.3639545483458, 2035: 679.4087687956805, 2036: 521.9528371124135, 2037: 400.9880011596189, 2038: 308.05729108309606, 2039: 236.66367650656787, 2040: 181.8158420489948, 2041: 139.6792313376728, 2042: 107.30796308621767, 2043: 82.43887678530872, 2044: 63.33330919871123, 2045: 48.65553984324027, 2046: 37.37940725644753, 2047: 28.71656734967821, 2048: 22.06137819925872, 2049: 16.948558026597915, 2050: 13.020656125219261}</t>
-        </is>
-      </c>
-      <c r="S257" t="inlineStr">
-        <is>
           <t>{2021: 27235.1355432164, 2022: 27006.980903149582, 2023: 26370.20771686104, 2024: 25733.4345305725, 2025: 25096.66134428419, 2026: 24459.88815799565, 2027: 23823.11497170711, 2028: 23186.3417854188, 2029: 22549.56859913026, 2030: 21912.79541284172, 2031: 21276.02222655341, 2032: 20639.24904026487, 2033: 20002.475853976328, 2034: 19365.70266768802, 2035: 18728.92948139948, 2036: 18092.156295110937, 2037: 17455.383108822396, 2038: 16818.609922534088, 2039: 16181.836736245546, 2040: 15545.063549957005, 2041: 14908.290363668697, 2042: 14271.517177380156, 2043: 13634.743991091615, 2044: 12997.970804803306, 2045: 12361.197618514765, 2046: 11724.424432226224, 2047: 11087.651245937916, 2048: 10450.878059649374, 2049: 9814.104873360833, 2050: 9177.331687072525}</t>
         </is>
       </c>
-      <c r="T257" t="n">
+      <c r="S257" t="n">
         <v>533701.4344862902</v>
       </c>
     </row>
@@ -19000,15 +17715,10 @@
       </c>
       <c r="R258" t="inlineStr">
         <is>
-          <t>{2021: 24994.5544836964, 2022: 19374.800882635343, 2023: 15018.587728243943, 2024: 11641.82170011955, 2025: 9024.284769632039, 2026: 6995.272535618415, 2027: 5422.4616240221485, 2028: 4203.28013158583, 2029: 3258.2183313782793, 2030: 2525.6433933952944, 2031: 1957.779958810474, 2032: 1517.5944383689343, 2033: 1176.3798423841536, 2034: 911.8836354297059, 2035: 706.856522532078, 2036: 547.9275249968648, 2037: 424.73198319474415, 2038: 329.2356184325156, 2039: 255.21057215731327, 2040: 197.82925204434886, 2041: 153.34949737232125, 2042: 118.87053153833786, 2043: 92.14378599428915, 2044: 71.42625836263738, 2045: 55.3668413842081, 2046: 42.91820956517579, 2047: 33.26851715268194, 2048: 25.788453077417152, 2049: 19.990200016249712, 2050: 15.49562106304101}</t>
-        </is>
-      </c>
-      <c r="S258" t="inlineStr">
-        <is>
           <t>{2021: 24994.5544836964, 2022: 23910.60524038179, 2023: 22943.631478241645, 2024: 21976.6577161015, 2025: 21009.683953961125, 2026: 20042.71019182098, 2027: 19075.736429680837, 2028: 18108.762667540694, 2029: 17141.78890540055, 2030: 16174.815143260173, 2031: 15207.84138112003, 2032: 14240.867618979886, 2033: 13273.893856839743, 2034: 12306.920094699599, 2035: 11339.946332559455, 2036: 10372.972570419079, 2037: 9405.998808278935, 2038: 8439.025046138791, 2039: 7472.051283998648, 2040: 6505.077521858504, 2041: 5538.103759718128, 2042: 4571.129997577984, 2043: 3604.15623543784, 2044: 2637.1824732976966, 2045: 1670.208711157553, 2046: 703.2349490171764, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T258" t="n">
+      <c r="S258" t="n">
         <v>320170.2796093365</v>
       </c>
     </row>
@@ -19072,15 +17782,10 @@
       </c>
       <c r="R259" t="inlineStr">
         <is>
-          <t>{2021: 244532.808764144, 2022: 181047.1123653148, 2023: 134043.59546466384, 2024: 99243.14864983573, 2025: 73477.6064443139, 2026: 54401.3236403339, 2027: 40277.632288733534, 2028: 29820.738802458913, 2029: 22078.667791334567, 2030: 16346.5960608568, 2031: 12102.686869616928, 2032: 8960.582920057832, 2033: 6634.233136180734, 2034: 4911.851125966076, 2035: 3636.634557214777, 2036: 2692.490176018427, 2037: 1993.4649011057038, 2038: 1475.9208213033708, 2039: 1092.7417229912437, 2040: 809.0437209981145, 2041: 598.9994970583912, 2042: 443.48703063111975, 2043: 328.3487670755672, 2044: 243.10274121571976, 2045: 179.98831947188643, 2046: 133.25968676579873, 2047: 98.66275861135843, 2048: 73.04789747788543, 2049: 54.083175871441284, 2050: 40.04208215885696}</t>
-        </is>
-      </c>
-      <c r="S259" t="inlineStr">
-        <is>
           <t>{2021: 244532.808764144, 2022: 257760.53108856548, 2023: 261465.39970888477, 2024: 265170.268329205, 2025: 268875.1369495252, 2026: 272580.0055698445, 2027: 276284.87419016473, 2028: 279989.74281048495, 2029: 283694.61143080425, 2030: 287399.48005112447, 2031: 291104.3486714447, 2032: 294809.2172917649, 2033: 298514.0859120842, 2034: 302218.95453240443, 2035: 305923.82315272465, 2036: 309628.69177304395, 2037: 313333.56039336417, 2038: 317038.4290136844, 2039: 320743.2976340046, 2040: 324448.1662543239, 2041: 328153.03487464413, 2042: 331857.90349496435, 2043: 335562.77211528365, 2044: 339267.64073560387, 2045: 342972.5093559241, 2046: 346677.3779762443, 2047: 350382.2465965636, 2048: 354087.11521688383, 2049: 357791.98383720405, 2050: 361496.85245752335}</t>
         </is>
       </c>
-      <c r="T259" t="n">
+      <c r="S259" t="n">
         <v>8920750.039571594</v>
       </c>
     </row>
@@ -19144,15 +17849,10 @@
       </c>
       <c r="R260" t="inlineStr">
         <is>
-          <t>{2021: 17672.8918327639, 2022: 13565.24351044005, 2023: 10412.321494345797, 2024: 7992.222094515025, 2025: 6134.617918082964, 2026: 4708.770171275903, 2027: 3614.327220044128, 2028: 2774.2618090048395, 2029: 2129.4498578379507, 2030: 1634.5092890395476, 2031: 1254.606022359731, 2032: 963.002340761382, 2033: 739.175081088521, 2034: 567.3712070837078, 2035: 435.49910550768806, 2036: 334.277574417016, 2037: 256.5826091143398, 2038: 196.94601235137722, 2039: 151.1705408055308, 2040: 116.03450171240203, 2041: 89.06500906790981, 2042: 68.36394109683164, 2043: 52.4743498170818, 2044: 40.27792056085965, 2045: 30.916264619991853, 2046: 23.730505565924854, 2047: 18.214907309670288, 2048: 13.981280229288256, 2049: 10.731660256437792, 2050: 8.237338067106979}</t>
-        </is>
-      </c>
-      <c r="S260" t="inlineStr">
-        <is>
           <t>{2021: 17672.8918327639, 2022: 17428.940660738386, 2023: 17002.664837648044, 2024: 16576.38901455782, 2025: 16150.113191467477, 2026: 15723.837368377252, 2027: 15297.56154528691, 2028: 14871.285722196684, 2029: 14445.009899106342, 2030: 14018.734076016, 2031: 13592.458252925775, 2032: 13166.182429835433, 2033: 12739.906606745208, 2034: 12313.630783654866, 2035: 11887.35496056464, 2036: 11461.079137474298, 2037: 11034.803314384073, 2038: 10608.527491293731, 2039: 10182.251668203506, 2040: 9755.975845113164, 2041: 9329.700022022938, 2042: 8903.424198932596, 2043: 8477.148375842371, 2044: 8050.872552752029, 2045: 7624.596729661804, 2046: 7198.320906571462, 2047: 6772.045083481236, 2048: 6345.7692603908945, 2049: 5919.493437300553, 2050: 5493.217614210327}</t>
         </is>
       </c>
-      <c r="T260" t="n">
+      <c r="S260" t="n">
         <v>338461.1320960326</v>
       </c>
     </row>
@@ -19216,15 +17916,10 @@
       </c>
       <c r="R261" t="inlineStr">
         <is>
-          <t>{2021: 89825.1859719511, 2022: 66713.83776093464, 2023: 49548.8665081317, 2024: 36800.31391745646, 2025: 27331.868514107882, 2026: 20299.58326301458, 2027: 15076.6523861829, 2028: 11197.542542064906, 2029: 8316.498634422536, 2030: 6176.725766080238, 2031: 4587.500445373262, 2032: 3407.170907905659, 2033: 2530.53132831557, 2034: 1879.4445528776719, 2035: 1395.8775328392444, 2036: 1036.7286886447432, 2037: 769.9861546398489, 2038: 571.8744786662535, 2039: 424.73545450017633, 2040: 315.45420024724183, 2041: 234.29019498909204, 2042: 174.00908095376283, 2043: 129.2378464911128, 2044: 95.98591564367008, 2045: 71.28945778733099, 2046: 52.947213739964965, 2047: 39.32429183552768, 2048: 29.206445800159557, 2049: 21.691845840361612, 2050: 16.110696220333757}</t>
-        </is>
-      </c>
-      <c r="S261" t="inlineStr">
-        <is>
           <t>{2021: 89825.1859719511, 2022: 87837.65480462764, 2023: 87331.94558334316, 2024: 86826.23636205879, 2025: 86320.5271407743, 2026: 85814.81791948981, 2027: 85309.10869820544, 2028: 84803.39947692095, 2029: 84297.69025563658, 2030: 83791.9810343521, 2031: 83286.27181306761, 2032: 82780.56259178324, 2033: 82274.85337049875, 2034: 81769.14414921426, 2035: 81263.43492792989, 2036: 80757.7257066454, 2037: 80252.01648536103, 2038: 79746.30726407655, 2039: 79240.59804279206, 2040: 78734.88882150769, 2041: 78229.1796002232, 2042: 77723.47037893883, 2043: 77217.76115765434, 2044: 76712.05193636985, 2045: 76206.34271508548, 2046: 75700.633493801, 2047: 75194.92427251663, 2048: 74689.21505123214, 2049: 74183.50582994765, 2050: 73677.79660866328}</t>
         </is>
       </c>
-      <c r="T261" t="n">
+      <c r="S261" t="n">
         <v>2350047.740174362</v>
       </c>
     </row>
@@ -19288,15 +17983,10 @@
       </c>
       <c r="R262" t="inlineStr">
         <is>
-          <t>{2021: 113560.106743427, 2022: 86871.66434812936, 2023: 66455.4330127984, 2024: 50837.34276369525, 2025: 38889.75366055791, 2026: 29750.0391947894, 2027: 22758.303891987387, 2028: 17409.73827458901, 2029: 13318.171170761227, 2030: 10188.187813976929, 2031: 7793.800635386725, 2032: 5962.1327613162175, 2033: 4560.936149965599, 2034: 3489.0431657329727, 2035: 2669.062186375879, 2036: 2041.7898593825532, 2037: 1561.9365675170263, 2038: 1194.8564783667946, 2039: 914.0460845760524, 2040: 699.2306271551543, 2041: 534.9002399354508, 2042: 409.19012350343684, 2043: 313.023896181021, 2044: 239.45827123445633, 2045: 183.18174542634506, 2046: 140.13110378044803, 2047: 107.19805186386529, 2048: 82.00479417768847, 2049: 62.73235521728609, 2050: 47.98924783081124}</t>
-        </is>
-      </c>
-      <c r="S262" t="inlineStr">
-        <is>
           <t>{2021: 113560.106743427, 2022: 112241.21947505511, 2023: 109830.43820479978, 2024: 107419.65693454538, 2025: 105008.87566429097, 2026: 102598.09439403564, 2027: 100187.31312378123, 2028: 97776.5318535259, 2029: 95365.7505832715, 2030: 92954.96931301709, 2031: 90544.18804276176, 2032: 88133.40677250735, 2033: 85722.62550225202, 2034: 83311.84423199762, 2035: 80901.06296174228, 2036: 78490.28169148788, 2037: 76079.50042123348, 2038: 73668.71915097814, 2039: 71257.93788072374, 2040: 68847.1566104684, 2041: 66436.375340214, 2042: 64025.594069959596, 2043: 61614.81279970426, 2044: 59204.03152944986, 2045: 56793.25025919452, 2046: 54382.46898894012, 2047: 51971.687718684785, 2048: 49560.90644843038, 2049: 47150.12517817598, 2050: 44739.343907920644}</t>
         </is>
       </c>
-      <c r="T262" t="n">
+      <c r="S262" t="n">
         <v>2310628.550470903</v>
       </c>
     </row>
@@ -19360,15 +18050,10 @@
       </c>
       <c r="R263" t="inlineStr">
         <is>
-          <t>{2021: 113249.74480656, 2022: 86711.45525683156, 2023: 66391.99483937352, 2024: 50834.07913862828, 2025: 38921.91533217541, 2026: 29801.179027827868, 2027: 22817.74326543682, 2028: 17470.765409691114, 2029: 13376.767388859313, 2030: 10242.133162431011, 2031: 7842.050972967875, 2032: 6004.390148744137, 2033: 4597.356123112682, 2034: 3520.038305162824, 2035: 2695.172907645962, 2036: 2063.6016919062426, 2037: 1580.0292184436341, 2038: 1209.774318817057, 2039: 926.2828088147063, 2040: 709.2230580201377, 2041: 543.0278325807242, 2042: 415.77783409989786, 2043: 318.34686356173836, 2044: 243.7473025924854, 2045: 186.628970853958, 2046: 142.89541829408256, 2047: 109.41013324999419, 2048: 83.77159604337857, 2049: 64.14104521397581, 2050: 49.11060401679515}</t>
-        </is>
-      </c>
-      <c r="S263" t="inlineStr">
-        <is>
           <t>{2021: 113249.74480656, 2022: 104685.99533880316, 2023: 100400.3654416278, 2024: 96114.73554445244, 2025: 91829.10564727709, 2026: 87543.47575010173, 2027: 83257.84585292451, 2028: 78972.21595574915, 2029: 74686.5860585738, 2030: 70400.95616139844, 2031: 66115.32626422308, 2032: 61829.696367045864, 2033: 57544.06646987051, 2034: 53258.43657269515, 2035: 48972.806675519794, 2036: 44687.17677834444, 2037: 40401.54688116722, 2038: 36115.91698399186, 2039: 31830.287086816505, 2040: 27544.657189641148, 2041: 23259.02729246393, 2042: 18973.39739528857, 2043: 14687.767498113215, 2044: 10402.137600937858, 2045: 6116.5077037625015, 2046: 1830.877806585282, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T263" t="n">
+      <c r="S263" t="n">
         <v>1388085.786720655</v>
       </c>
     </row>
@@ -19432,15 +18117,10 @@
       </c>
       <c r="R264" t="inlineStr">
         <is>
-          <t>{2021: 432745.081804335, 2022: 328810.9010953789, 2023: 249839.02353866567, 2024: 189834.1492779395, 2025: 144240.89448341055, 2026: 109597.9607489524, 2027: 83275.3640591878, 2028: 63274.77456515134, 2029: 48077.809583937735, 2030: 36530.762697690014, 2031: 27757.017942863615, 2032: 21090.49984683652, 2033: 16025.107045181441, 2034: 12176.290636755264, 2035: 9251.860424565122, 2036: 7029.802742819895, 2037: 5341.425868438882, 2038: 4058.5534689673777, 2039: 3083.7938532097073, 2040: 2343.1462962870733, 2041: 1780.383134264739, 2042: 1352.7811344076595, 2043: 1027.878079942064, 2044: 781.0083393039096, 2045: 593.4303279398965, 2046: 450.90370537236885, 2047: 342.60829274489686, 2048: 260.3226384237335, 2049: 197.7998709049149, 2050: 150.2934557167351}</t>
-        </is>
-      </c>
-      <c r="S264" t="inlineStr">
-        <is>
           <t>{2021: 432745.081804335, 2022: 414557.803280022, 2023: 404036.27183391526, 2024: 393514.74038781226, 2025: 382993.2089417055, 2026: 372471.6774956025, 2027: 361950.1460494958, 2028: 351428.6146033928, 2029: 340907.08315728605, 2030: 330385.55171118304, 2031: 319864.0202650763, 2032: 309342.4888189696, 2033: 298820.9573728666, 2034: 288299.42592675984, 2035: 277777.89448065683, 2036: 267256.3630345501, 2037: 256734.8315884471, 2038: 246213.30014234036, 2039: 235691.76869623736, 2040: 225170.23725013062, 2041: 214648.70580402762, 2042: 204127.17435792089, 2043: 193605.64291181788, 2044: 183084.11146571115, 2045: 172562.58001960814, 2046: 162041.0485735014, 2047: 151519.5171273984, 2048: 140997.98568129167, 2049: 130476.45423518494, 2050: 119954.92278908193}</t>
         </is>
       </c>
-      <c r="T264" t="n">
+      <c r="S264" t="n">
         <v>7906829.60750962</v>
       </c>
     </row>
@@ -19504,15 +18184,10 @@
       </c>
       <c r="R265" t="inlineStr">
         <is>
-          <t>{2021: 130580.639700426, 2022: 104617.76273886455, 2023: 83816.99083106613, 2024: 67151.96127363936, 2025: 53800.37935249986, 2026: 43103.4442416074, 2027: 34533.34210371193, 2028: 27667.20242047023, 2029: 22166.232491380957, 2030: 17759.00054493483, 2031: 14228.042608396694, 2032: 11399.132285295771, 2033: 9132.683984302099, 2034: 7316.865413055778, 2035: 5862.0794899718685, 2036: 4696.54339759097, 2037: 3762.746636784549, 2038: 3014.6133132498535, 2039: 2415.2286363318112, 2040: 1935.0174498727663, 2041: 1550.2849191945825, 2042: 1242.04736801737, 2043: 995.0955758508856, 2044: 797.2443165824229, 2045: 638.7311085967667, 2046: 511.73450923820576, 2047: 409.9881850448405, 2048: 328.47171500431, 2049: 263.162870281426, 2050: 210.839147272848}</t>
-        </is>
-      </c>
-      <c r="S265" t="inlineStr">
-        <is>
           <t>{2021: 130580.639700426, 2022: 127023.2412871588, 2023: 118745.65563288704, 2024: 110468.06997861527, 2025: 102190.4843243435, 2026: 93912.89867007174, 2027: 85635.31301579997, 2028: 77357.72736152634, 2029: 69080.14170725644, 2030: 60802.55605298281, 2031: 52524.9703987129, 2032: 44247.384744439274, 2033: 35969.79909016937, 2034: 27692.21343589574, 2035: 19414.627781625837, 2036: 11137.042127352208, 2037: 2859.456473082304, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T265" t="n">
+      <c r="S265" t="n">
         <v>1104351.901932132</v>
       </c>
     </row>
@@ -19576,15 +18251,10 @@
       </c>
       <c r="R266" t="inlineStr">
         <is>
-          <t>{2021: 44254.4045734121, 2022: 33904.08525793532, 2023: 25974.521818963873, 2024: 19899.542447201726, 2025: 15245.39286489854, 2026: 11679.766216824877, 2027: 8948.076319749962, 2028: 6855.280177503107, 2029: 5251.951886948168, 2030: 4023.6136100370077, 2031: 3082.561842028319, 2032: 2361.6053704126975, 2033: 1809.267814037535, 2034: 1386.1122031324464, 2035: 1061.9251747949488, 2036: 813.5597351461522, 2037: 623.2825611078314, 2038: 477.5078389435643, 2039: 365.82723547932716, 2040: 280.2667418288483, 2041: 214.7173281738809, 2042: 164.49875828036804, 2043: 126.02542005305489, 2044: 96.55031238885893, 2045: 73.96890895869917, 2046: 56.66889476757077, 2047: 43.41504666468837, 2048: 33.26103825789979, 2049: 25.481872092360987, 2050: 19.522114742681723}</t>
-        </is>
-      </c>
-      <c r="S266" t="inlineStr">
-        <is>
           <t>{2021: 44254.4045734121, 2022: 42546.69280240452, 2023: 41263.643444984686, 2024: 39980.59408756439, 2025: 38697.54473014409, 2026: 37414.49537272379, 2027: 36131.44601530349, 2028: 34848.396657883655, 2029: 33565.347300463356, 2030: 32282.297943043057, 2031: 30999.248585622758, 2032: 29716.19922820246, 2033: 28433.14987078216, 2034: 27150.100513362326, 2035: 25867.051155942027, 2036: 24584.001798521727, 2037: 23300.952441101428, 2038: 22017.90308368113, 2039: 20734.85372626083, 2040: 19451.804368840996, 2041: 18168.755011420697, 2042: 16885.705654000398, 2043: 15602.656296580099, 2044: 14319.6069391598, 2045: 13036.5575817395, 2046: 11753.508224319667, 2047: 10470.458866899367, 2048: 9187.409509479068, 2049: 7904.360152058769, 2050: 6621.31079463847}</t>
         </is>
       </c>
-      <c r="T266" t="n">
+      <c r="S266" t="n">
         <v>731752.5990465155</v>
       </c>
     </row>
@@ -19648,15 +18318,10 @@
       </c>
       <c r="R267" t="inlineStr">
         <is>
-          <t>{2021: 11651.4229570806, 2022: 9187.971228378816, 2023: 7245.365274652173, 2024: 5713.483059349781, 2025: 4505.4855665705645, 2026: 3552.89408924682, 2027: 2801.7083226421846, 2028: 2209.3452064670246, 2029: 1742.22498533878, 2030: 1373.867646691824, 2031: 1083.3918274105674, 2032: 854.3310955216731, 2033: 673.7005045716138, 2034: 531.2605057210317, 2035: 418.93649035996054, 2036: 330.3610583981214, 2037: 260.5130644316816, 2038: 205.4329801117124, 2039: 161.99843723632782, 2040: 127.74722760065836, 2041: 100.7377258574864, 2042: 79.43882306911046, 2043: 62.64313152684163, 2044: 49.39854061124778, 2045: 38.95424374618789, 2046: 30.718176833991475, 2047: 24.223455450773912, 2048: 19.101908200695252, 2049: 15.063205893531208, 2050: 11.878403424776947}</t>
-        </is>
-      </c>
-      <c r="S267" t="inlineStr">
-        <is>
           <t>{2021: 11651.4229570806, 2022: 10765.957601174014, 2023: 10057.793333124602, 2024: 9349.629065075424, 2025: 8641.464797026245, 2026: 7933.300528977066, 2027: 7225.136260927655, 2028: 6516.971992878476, 2029: 5808.8077248292975, 2030: 5100.643456780119, 2031: 4392.479188730707, 2032: 3684.3149206815287, 2033: 2976.15065263235, 2034: 2267.9863845831715, 2035: 1559.82211653376, 2036: 851.6578484845813, 2037: 143.4935804354027, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T267" t="n">
+      <c r="S267" t="n">
         <v>93101.3209314147</v>
       </c>
     </row>
@@ -19720,15 +18385,10 @@
       </c>
       <c r="R268" t="inlineStr">
         <is>
-          <t>{2021: 63515.5467990261, 2022: 49358.778866301895, 2023: 38357.36562075613, 2024: 29808.020602568806, 2025: 23164.210520296176, 2026: 18001.21706110061, 2027: 13988.985957321398, 2028: 10871.027633848802, 2029: 8448.020619682795, 2030: 6565.0695402857755, 2031: 5101.80313343108, 2032: 3964.6792852028484, 2033: 3081.0051708023066, 2034: 2394.290226182789, 2035: 1860.6348803048693, 2036: 1445.9241907888968, 2037: 1123.646980737006, 2038: 873.2010608595763, 2039: 678.5761949773366, 2040: 527.3306149406633, 2041: 409.79565671764453, 2042: 318.4576724860588, 2043: 247.47770627328654, 2044: 192.31822748741666, 2045: 149.45306056400196, 2046: 116.14196742432368, 2047: 90.2554724961028, 2048: 70.13873189984153, 2049: 54.5057443772207, 2050: 42.35714119207844}</t>
-        </is>
-      </c>
-      <c r="S268" t="inlineStr">
-        <is>
           <t>{2021: 63515.5467990261, 2022: 58916.75698980875, 2023: 55876.157814805396, 2024: 52835.55863980111, 2025: 49794.95946479775, 2026: 46754.36028979346, 2027: 43713.761114790104, 2028: 40673.161939785816, 2029: 37632.56276478246, 2030: 34591.96358977817, 2031: 31551.364414774813, 2032: 28510.765239771456, 2033: 25470.166064767167, 2034: 22429.56688976381, 2035: 19388.96771475952, 2036: 16348.368539756164, 2037: 13307.769364751875, 2038: 10267.170189748518, 2039: 7226.57101474423, 2040: 4185.971839740872, 2041: 1145.3726647365838, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T268" t="n">
+      <c r="S268" t="n">
         <v>632379.069944971</v>
       </c>
     </row>
@@ -19792,15 +18452,10 @@
       </c>
       <c r="R269" t="inlineStr">
         <is>
-          <t>{2021: 49230.8804101019, 2022: 37972.37472720515, 2023: 29288.552843499798, 2024: 22590.615778683416, 2025: 17424.415743141177, 2026: 13439.6630425769, 2027: 10366.174990349798, 2028: 7995.556405702113, 2029: 6167.0695600139425, 2030: 4756.735495096641, 2031: 3668.927737902981, 2032: 2829.888430800883, 2033: 2182.7272442705284, 2034: 1683.5639776556416, 2035: 1298.5533003721425, 2036: 1001.5898987429447, 2037: 772.5384279385435, 2038: 595.8682524562155, 2039: 459.6004049049963, 2040: 354.49536255391985, 2041: 273.4265695397103, 2042: 210.8972269528139, 2043: 162.66758717435874, 2044: 125.46748148114773, 2045: 96.77458910328991, 2046: 74.64341346102333, 2047: 57.57336946340868, 2048: 44.40703764306011, 2049: 34.25168633712626, 2050: 26.418740794348476}</t>
-        </is>
-      </c>
-      <c r="S269" t="inlineStr">
-        <is>
           <t>{2021: 49230.8804101019, 2022: 46871.820241840556, 2023: 45093.31434197351, 2024: 43314.808442106936, 2025: 41536.30254223989, 2026: 39757.79664237285, 2027: 37979.29074250581, 2028: 36200.784842638765, 2029: 34422.27894277172, 2030: 32643.77304290468, 2031: 30865.2671430381, 2032: 29086.76124317106, 2033: 27308.255343304016, 2034: 25529.749443436973, 2035: 23751.24354356993, 2036: 21972.737643702887, 2037: 20194.231743835844, 2038: 18415.725843969267, 2039: 16637.219944102224, 2040: 14858.714044235181, 2041: 13080.208144368138, 2042: 11301.702244501095, 2043: 9523.196344634052, 2044: 7744.6904447670095, 2045: 5966.184544900432, 2046: 4187.678645033389, 2047: 2409.1727451663464, 2048: 630.6668452993035, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T269" t="n">
+      <c r="S269" t="n">
         <v>665899.015881441</v>
       </c>
     </row>
@@ -19864,15 +18519,10 @@
       </c>
       <c r="R270" t="inlineStr">
         <is>
-          <t>{2021: 33344.2790431293, 2022: 25946.670650746575, 2023: 20190.261633413087, 2024: 15710.943045941163, 2025: 12225.385479122227, 2026: 9513.1176833936, 2027: 7402.581146635043, 2028: 5760.278539197941, 2029: 4482.329635012136, 2030: 3487.9005972002055, 2031: 2714.09101216551, 2032: 2111.9552627820426, 2033: 1643.406581429984, 2034: 1278.8079555859952, 2035: 995.0975040194005, 2036: 774.3297484037681, 2037: 602.5405116997995, 2038: 468.86364496246085, 2039: 364.84371307635996, 2040: 283.90116487279084, 2041: 220.9161581448393, 2042: 171.90471533057462, 2043: 133.7667258069518, 2044: 104.0898552358076, 2045: 80.99695868049945, 2046: 63.02734594671311, 2047: 49.044388848677244, 2048: 38.16362630236527, 2049: 29.696819692062846, 2050: 23.10841985600917}</t>
-        </is>
-      </c>
-      <c r="S270" t="inlineStr">
-        <is>
           <t>{2021: 33344.2790431293, 2022: 30453.012721930165, 2023: 28703.154857493937, 2024: 26953.296993057244, 2025: 25203.439128621016, 2026: 23453.581264184322, 2027: 21703.723399748094, 2028: 19953.8655353114, 2029: 18204.007670875173, 2030: 16454.14980643848, 2031: 14704.291942002252, 2032: 12954.434077565558, 2033: 11204.57621312933, 2034: 9454.718348693103, 2035: 7704.860484256409, 2036: 5955.002619820181, 2037: 4205.144755383488, 2038: 2455.28689094726, 2039: 705.4290265105665, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T270" t="n">
+      <c r="S270" t="n">
         <v>297098.1152575326</v>
       </c>
     </row>
@@ -19936,15 +18586,10 @@
       </c>
       <c r="R271" t="inlineStr">
         <is>
-          <t>{2021: 21794.3737869597, 2022: 17106.368193202565, 2023: 13426.760301619743, 2024: 10538.64211041521, 2025: 8271.762885200133, 2026: 6492.493104149892, 2027: 5095.947175039708, 2028: 3999.800568782496, 2029: 3139.436897696671, 2030: 2464.1388652083224, 2031: 1934.0985485279296, 2032: 1518.0707744332403, 2033: 1191.5312577750274, 2034: 935.2309274150867, 2035: 734.0612190291587, 2036: 576.1634452914287, 2037: 452.22974199499663, 2038: 354.9543818098653, 2039: 278.6031113526752, 2040: 218.67512456000296, 2041: 171.63774614419302, 2042: 134.71818507356085, 2043: 105.74008222100056, 2044: 82.99521688180968, 2045: 65.14280943022189, 2046: 51.13048413989122, 2047: 40.1322330314909, 2048: 31.499723798572965, 2049: 24.724081478541216, 2050: 19.40589094896247}</t>
-        </is>
-      </c>
-      <c r="S271" t="inlineStr">
-        <is>
           <t>{2021: 21794.3737869597, 2022: 18147.294181198813, 2023: 16411.8653651271, 2024: 14676.436549054924, 2025: 12941.007732983213, 2026: 11205.578916911036, 2027: 9470.150100839324, 2028: 7734.721284767147, 2029: 5999.292468695436, 2030: 4263.8636526232585, 2031: 2528.4348365510814, 2032: 793.0060204793699, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T271" t="n">
+      <c r="S271" t="n">
         <v>115068.8380027105</v>
       </c>
     </row>
@@ -20008,15 +18653,10 @@
       </c>
       <c r="R272" t="inlineStr">
         <is>
-          <t>{2021: 23006.9546629168, 2022: 17625.686966959685, 2023: 13503.083985208614, 2024: 10344.747268766947, 2025: 7925.137410971076, 2026: 6071.468093996245, 2027: 4651.367276658687, 2028: 3563.4243987488258, 2029: 2729.948570029938, 2030: 2091.4206002589062, 2031: 1602.2426851577488, 2032: 1227.4822299367765, 2033: 940.3772841454524, 2034: 720.4254489145025, 2035: 551.9197838932323, 2036: 422.8271617996419, 2037: 323.9289729648933, 2038: 248.16281688122024, 2039: 190.11817040859887, 2040: 145.65001789455565, 2041: 111.5828522181322, 2042: 85.48390923060056, 2043: 65.48944207896926, 2044: 50.17162951971534, 2045: 38.436614036629955, 2046: 29.446388581425545, 2047: 22.55895380539958, 2048: 17.282472361149406, 2049: 13.240146395547916, 2050: 10.14331010704313}</t>
-        </is>
-      </c>
-      <c r="S272" t="inlineStr">
-        <is>
           <t>{2021: 23006.9546629168, 2022: 23032.539706559386, 2023: 22594.17199874553, 2024: 22155.804290931672, 2025: 21717.43658311793, 2026: 21279.068875304074, 2027: 20840.701167490217, 2028: 20402.333459676476, 2029: 19963.96575186262, 2030: 19525.598044048762, 2031: 19087.230336234905, 2032: 18648.862628421164, 2033: 18210.494920607307, 2034: 17772.12721279345, 2035: 17333.759504979593, 2036: 16895.391797165852, 2037: 16457.024089351995, 2038: 16018.656381538138, 2039: 15580.288673724397, 2040: 15141.92096591054, 2041: 14703.553258096683, 2042: 14265.185550282826, 2043: 13826.817842469085, 2044: 13388.450134655228, 2045: 12950.08242684137, 2046: 12511.714719027514, 2047: 12073.347011213773, 2048: 11634.979303399916, 2049: 11196.611595586059, 2050: 10758.243887772318}</t>
         </is>
       </c>
-      <c r="T272" t="n">
+      <c r="S272" t="n">
         <v>496090.717505381</v>
       </c>
     </row>
@@ -20080,15 +18720,10 @@
       </c>
       <c r="R273" t="inlineStr">
         <is>
-          <t>{2021: 120399.758867021, 2022: 95164.24197777791, 2023: 75218.0322986152, 2024: 59452.50301259878, 2025: 46991.39297383801, 2026: 37142.103388880474, 2027: 29357.202603428454, 2028: 23203.999398611435, 2029: 18340.493655477934, 2030: 14496.367705765218, 2031: 11457.961852514627, 2032: 9056.39898755247, 2033: 7158.198262262606, 2034: 5657.856111715672, 2035: 4471.982279345257, 2036: 3534.6649175766465, 2037: 2793.807152870996, 2038: 2208.2314984427057, 2039: 1745.3911755160002, 2040: 1379.5611364648628, 2041: 1090.4082454075497, 2042: 861.8611457115773, 2043: 681.2170007111805, 2044: 538.4354595481834, 2045: 425.58060617424223, 2046: 336.37987457887215, 2047: 265.87541438711884, 2048: 210.1485294386933, 2049: 166.10187341708934, 2050: 131.2872967817533}</t>
-        </is>
-      </c>
-      <c r="S273" t="inlineStr">
-        <is>
           <t>{2021: 120399.758867021, 2022: 118408.94764437713, 2023: 112635.21552699618, 2024: 106861.4834096171, 2025: 101087.75129223615, 2026: 95314.01917485707, 2027: 89540.28705747612, 2028: 83766.55494009703, 2029: 77992.82282271609, 2030: 72219.09070533514, 2031: 66445.35858795606, 2032: 60671.62647057511, 2033: 54897.894353196025, 2034: 49124.16223581508, 2035: 43350.43011843413, 2036: 37576.69800105505, 2037: 31802.9658836741, 2038: 26029.233766295016, 2039: 20255.50164891407, 2040: 14481.769531534985, 2041: 8708.037414154038, 2042: 2934.305296773091, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T273" t="n">
+      <c r="S273" t="n">
         <v>1334304.035315595</v>
       </c>
     </row>
@@ -20152,15 +18787,10 @@
       </c>
       <c r="R274" t="inlineStr">
         <is>
-          <t>{2021: 29559.2865580057, 2022: 22629.160198415193, 2023: 17323.79062264103, 2024: 13262.25626164083, 2025: 10152.941984853958, 2026: 7772.60135184997, 2027: 5950.3276848133155, 2028: 4555.283096852596, 2029: 3487.304429541177, 2030: 2669.7116130279974, 2031: 2043.8020943512222, 2032: 1564.6360380238702, 2033: 1197.809679444597, 2034: 916.985160320895, 2035: 701.9994901348853, 2036: 537.4168584987619, 2037: 411.42035550935196, 2038: 314.9635264518437, 2039: 241.12084311474055, 2040: 184.5904560420666, 2041: 141.31352570629375, 2042: 108.18280086480996, 2043: 82.81952024379987, 2044: 63.40261925723829, 2045: 48.5379789311115, 2046: 37.158329203380084, 2047: 28.446619731456355, 2048: 21.777356288465, 2049: 16.671690745396912, 2050: 12.763040133451586}</t>
-        </is>
-      </c>
-      <c r="S274" t="inlineStr">
-        <is>
           <t>{2021: 29559.2865580057, 2022: 28920.31515496457, 2023: 28203.82332932297, 2024: 27487.331503681373, 2025: 26770.839678040007, 2026: 26054.34785239841, 2027: 25337.856026757043, 2028: 24621.364201115444, 2029: 23904.87237547408, 2030: 23188.38054983248, 2031: 22471.888724191114, 2032: 21755.396898549516, 2033: 21038.905072907917, 2034: 20322.41324726655, 2035: 19605.921421624953, 2036: 18889.429595983587, 2037: 18172.93777034199, 2038: 17456.445944700623, 2039: 16739.954119059024, 2040: 16023.462293417426, 2041: 15306.97046777606, 2042: 14590.478642134462, 2043: 13873.986816493096, 2044: 13157.494990851497, 2045: 12441.003165210132, 2046: 11724.511339568533, 2047: 11008.019513927167, 2048: 10291.527688285569, 2049: 9575.03586264397, 2050: 8858.544037002604}</t>
         </is>
       </c>
-      <c r="T274" t="n">
+      <c r="S274" t="n">
         <v>558143.8295440237</v>
       </c>
     </row>
@@ -20224,15 +18854,10 @@
       </c>
       <c r="R275" t="inlineStr">
         <is>
-          <t>{2021: 64215.5717053796, 2022: 48247.66522152665, 2023: 36250.35388625995, 2024: 27236.305650139017, 2025: 20463.699410917114, 2026: 15375.176022752259, 2027: 11551.96980681322, 2028: 8679.445765046677, 2029: 6521.20634387014, 2030: 4899.636835175667, 2031: 3681.2883768316915, 2032: 2765.8956304891585, 2033: 2078.12533430026, 2034: 1561.3766685392993, 2035: 1173.123228334908, 2036: 881.4132659907094, 2037: 662.2401864526197, 2038: 497.56689792937954, 2039: 373.84142940829906, 2040: 280.88165616249705, 2041: 211.03735049766462, 2042: 158.56059777470307, 2043: 119.13276539618712, 2044: 89.50909614448531, 2045: 67.25167728591258, 2046: 50.52880983702324, 2047: 37.96426686417943, 2048: 28.524035360883957, 2049: 21.43122099999345, 2050: 16.10211275296662}</t>
-        </is>
-      </c>
-      <c r="S275" t="inlineStr">
-        <is>
           <t>{2021: 64215.5717053796, 2022: 60027.22272345144, 2023: 58544.99198178435, 2024: 57062.76124011772, 2025: 55580.53049845109, 2026: 54098.29975678399, 2027: 52616.06901511736, 2028: 51133.83827345027, 2029: 49651.60753178364, 2030: 48169.37679011701, 2031: 46687.14604844991, 2032: 45204.91530678328, 2033: 43722.68456511665, 2034: 42240.453823449556, 2035: 40758.223081782926, 2036: 39275.99234011583, 2037: 37793.7615984492, 2038: 36311.53085678257, 2039: 34829.300115115475, 2040: 33347.069373448845, 2041: 31864.838631782215, 2042: 30382.60789011512, 2043: 28900.37714844849, 2044: 27418.146406781394, 2045: 25935.915665114764, 2046: 24453.684923448134, 2047: 22971.45418178104, 2048: 21489.22344011441, 2049: 20006.99269844778, 2050: 18524.761956780683}</t>
         </is>
       </c>
-      <c r="T275" t="n">
+      <c r="S275" t="n">
         <v>1161849.182737665</v>
       </c>
     </row>
@@ -20296,15 +18921,10 @@
       </c>
       <c r="R276" t="inlineStr">
         <is>
-          <t>{2021: 27256.1945967649, 2022: 22459.415416651227, 2023: 18506.814627658336, 2024: 15249.826467370125, 2025: 12566.031052007562, 2026: 10354.553000185677, 2027: 8532.269846374857, 2028: 7030.6877303203855, 2029: 5793.3669294671245, 2030: 4773.800468295563, 2031: 3933.666068203813, 2032: 3241.3857342602314, 2033: 2670.938838248475, 2034: 2200.884085550606, 2035: 1813.553604696697, 2036: 1494.3888679560164, 2037: 1231.3934823251889, 2038: 1014.6822830572536, 2039: 836.109781583517, 2040: 688.9640023607184, 2041: 567.7142009389182, 2042: 467.80298077020507, 2043: 385.4749950865404, 2044: 317.6357952921198, 2045: 261.7355204277435, 2046: 215.67305596203133, 2047: 177.71705954157153, 2048: 146.4408853077254, 2049: 120.66896079098144, 2050: 99.4326008599133}</t>
-        </is>
-      </c>
-      <c r="S276" t="inlineStr">
-        <is>
           <t>{2021: 27256.1945967649, 2022: 19301.244344605133, 2023: 14892.884435448796, 2024: 10484.524526292458, 2025: 6076.164617137983, 2026: 1667.804707981646, 2027: 0, 2028: 0, 2029: 0, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T276" t="n">
+      <c r="S276" t="n">
         <v>66050.71992984846</v>
       </c>
     </row>
@@ -20368,15 +18988,10 @@
       </c>
       <c r="R277" t="inlineStr">
         <is>
-          <t>{2021: 38379.083489963, 2022: 29362.520103354756, 2023: 22464.25678834634, 2024: 17186.632185399772, 2025: 13148.902661647462, 2026: 10059.774325789944, 2027: 7696.388215040831, 2028: 5888.242582615588, 2029: 4504.892391468789, 2030: 3446.538618947092, 2031: 2636.8284566328525, 2032: 2017.3469902486893, 2033: 1543.4029729269203, 2034: 1180.8046649158762, 2035: 903.3931391507784, 2036: 691.155097971128, 2037: 528.7790539349576, 2038: 404.5507132930515, 2039: 309.5078717812596, 2040: 236.7938543842634, 2041: 181.16285428043435, 2042: 138.60148463893168, 2043: 106.03924088311702, 2044: 81.12698530149302, 2045: 62.067473223080675, 2046: 47.485694408355336, 2047: 36.329675695662075, 2048: 27.794588509160473, 2049: 21.264686116804523, 2050: 16.268881818386625}</t>
-        </is>
-      </c>
-      <c r="S277" t="inlineStr">
-        <is>
           <t>{2021: 38379.083489963, 2022: 36534.16298870416, 2023: 35366.80453846371, 2024: 34199.44608822325, 2025: 33032.08763798233, 2026: 31864.729187741876, 2027: 30697.37073750142, 2028: 29530.012287260965, 2029: 28362.65383702051, 2030: 27195.295386779588, 2031: 26027.936936539132, 2032: 24860.578486298677, 2033: 23693.22003605822, 2034: 22525.861585817765, 2035: 21358.503135576844, 2036: 20191.14468533639, 2037: 19023.786235095933, 2038: 17856.427784855478, 2039: 16689.069334615022, 2040: 15521.710884374566, 2041: 14354.352434133645, 2042: 13186.99398389319, 2043: 12019.635533652734, 2044: 10852.277083412278, 2045: 9684.918633171823, 2046: 8517.560182930902, 2047: 7350.201732690446, 2048: 6182.8432824499905, 2049: 5015.484832209535, 2050: 3848.1263819690794}</t>
         </is>
       </c>
-      <c r="T277" t="n">
+      <c r="S277" t="n">
         <v>602808.6744287563</v>
       </c>
     </row>
@@ -20440,15 +19055,10 @@
       </c>
       <c r="R278" t="inlineStr">
         <is>
-          <t>{2021: 21601.5547051383, 2022: 16464.66198981175, 2023: 12549.332589208017, 2024: 9565.076315080732, 2025: 7290.482124284217, 2026: 5556.790960539147, 2027: 4235.37500713112, 2028: 3228.1943982450025, 2029: 2460.523343343653, 2030: 1875.405993650928, 2031: 1429.4307146228107, 2032: 1089.5092448378919, 2033: 830.421777316055, 2034: 632.9458253870636, 2035: 482.43004798083086, 2036: 367.70722210303035, 2037: 280.26571262016336, 2038: 213.61796817925665, 2039: 162.8191900551126, 2040: 124.10046250396421, 2041: 94.58912544943125, 2042: 72.09564310046335, 2043: 54.95115563625973, 2044: 41.88366142393187, 2045: 31.923643351314997, 2046: 24.332137405724648, 2047: 18.545906687893012, 2048: 14.135653154544222, 2049: 10.774166691781023, 2050: 8.212048402232224}</t>
-        </is>
-      </c>
-      <c r="S278" t="inlineStr">
-        <is>
           <t>{2021: 21601.5547051383, 2022: 21001.33928079193, 2023: 20508.67131592054, 2024: 20016.00335104915, 2025: 19523.335386177758, 2026: 19030.667421306483, 2027: 18537.999456435093, 2028: 18045.331491563702, 2029: 17552.66352669231, 2030: 17059.99556182092, 2031: 16567.327596949646, 2032: 16074.659632078256, 2033: 15581.991667206865, 2034: 15089.323702335474, 2035: 14596.655737464083, 2036: 14103.987772592809, 2037: 13611.319807721418, 2038: 13118.651842850028, 2039: 12625.983877978637, 2040: 12133.315913107246, 2041: 11640.647948235972, 2042: 11147.979983364581, 2043: 10655.31201849319, 2044: 10162.6440536218, 2045: 9669.976088750409, 2046: 9177.308123879135, 2047: 8684.640159007744, 2048: 8191.972194136353, 2049: 7699.3042292649625, 2050: 7206.636264393572}</t>
         </is>
       </c>
-      <c r="T278" t="n">
+      <c r="S278" t="n">
         <v>416213.1046255624</v>
       </c>
     </row>
@@ -20512,15 +19122,10 @@
       </c>
       <c r="R279" t="inlineStr">
         <is>
-          <t>{2021: 45865.6598646384, 2022: 35757.25257454426, 2023: 27876.653589050737, 2024: 21732.872616649565, 2025: 16943.129513832013, 2026: 13209.005674774957, 2027: 10297.851454998145, 2028: 8028.291243126757, 2029: 6258.923093436423, 2030: 4879.50886474003, 2031: 3804.105978877593, 2032: 2965.712882110574, 2033: 2312.094601978392, 2034: 1802.5283164610485, 2035: 1405.2661724410996, 2036: 1095.5572777266445, 2037: 854.1056294658111, 2038: 665.8679022231895, 2039: 519.1161934951973, 2040: 404.7073322639551, 2041: 315.5132258260455, 2042: 245.97675340912872, 2043: 191.76553711587923, 2044: 149.5020188520664, 2045: 116.5530260389673, 2046: 90.8657152802885, 2047: 70.83967267085818, 2048: 55.227202126069024, 2049: 43.05558932838493, 2050: 33.56649804896577}</t>
-        </is>
-      </c>
-      <c r="S279" t="inlineStr">
-        <is>
           <t>{2021: 45865.6598646384, 2022: 42575.54111571144, 2023: 40272.4591843579, 2024: 37969.37725300435, 2025: 35666.2953216508, 2026: 33363.21339029726, 2027: 31060.13145894371, 2028: 28757.049527590163, 2029: 26453.967596236616, 2030: 24150.88566488307, 2031: 21847.803733529523, 2032: 19544.721802175976, 2033: 17241.63987082243, 2034: 14938.557939468883, 2035: 12635.476008115336, 2036: 10332.39407676179, 2037: 8029.312145408243, 2038: 5726.230214054696, 2039: 3423.1482827011496, 2040: 1120.066351347603, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T279" t="n">
+      <c r="S279" t="n">
         <v>438041.1008693802</v>
       </c>
     </row>
@@ -20584,15 +19189,10 @@
       </c>
       <c r="R280" t="inlineStr">
         <is>
-          <t>{2021: 22521.1005462786, 2022: 17812.57640077716, 2023: 14088.471270821283, 2024: 11142.971026925487, 2025: 8813.291443768025, 2026: 6970.681866183237, 2027: 5513.309753746384, 2028: 4360.632865518868, 2029: 3448.948061538209, 2030: 2727.870723822737, 2031: 2157.550230713077, 2032: 1706.4675966486695, 2033: 1349.6935630784596, 2034: 1067.510873217288, 2035: 844.3245901224557, 2036: 667.8002363919225, 2037: 528.1821244367982, 2038: 417.7542045834829, 2039: 330.41363456453223, 2040: 261.33350354904036, 2041: 206.6960710239026, 2042: 163.48177786818266, 2043: 129.3023692349294, 2044: 102.26890671110043, 2045: 80.88737539589033, 2046: 63.97611658173252, 2047: 50.60052292273263, 2048: 40.02138699342502, 2049: 31.654048700708376, 2050: 25.036083814672104}</t>
-        </is>
-      </c>
-      <c r="S280" t="inlineStr">
-        <is>
           <t>{2021: 22521.1005462786, 2022: 20393.716080020647, 2023: 18861.625023625325, 2024: 17329.53396723047, 2025: 15797.442910835147, 2026: 14265.351854439825, 2027: 12733.260798044968, 2028: 11201.169741649646, 2029: 9669.07868525479, 2030: 8136.987628859468, 2031: 6604.896572464146, 2032: 5072.805516069289, 2033: 3540.714459673967, 2034: 2008.6234032791108, 2035: 476.5323468837887, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T280" t="n">
+      <c r="S280" t="n">
         <v>157352.2892614699</v>
       </c>
     </row>
@@ -20656,15 +19256,10 @@
       </c>
       <c r="R281" t="inlineStr">
         <is>
-          <t>{2021: 25201.3309250789, 2022: 19780.115978096477, 2023: 15525.092276677946, 2024: 12185.393172935297, 2025: 9564.11750299694, 2026: 7506.72073629102, 2027: 5891.903376867121, 2028: 4624.459417347422, 2029: 3629.6632064025034, 2030: 2848.863792055707, 2031: 2236.0269931848916, 2032: 1755.021327517965, 2033: 1377.4877805279841, 2034: 1081.167821582777, 2035: 848.5910909336745, 2036: 666.0453865134483, 2037: 522.7682232767178, 2038: 410.3123012359133, 2039: 322.04747161228005, 2040: 252.76983814392284, 2041: 198.3949470413065, 2042: 155.7169767585625, 2043: 122.21972994996797, 2044: 95.92828412154303, 2045: 75.29255463312285, 2046: 59.095905186827835, 2047: 46.38341768143691, 2048: 36.40559238426176, 2049: 28.574159109009422, 2050: 22.42739412585284}</t>
-        </is>
-      </c>
-      <c r="S281" t="inlineStr">
-        <is>
           <t>{2021: 25201.3309250789, 2022: 25420.580852974905, 2023: 24523.36979712732, 2024: 23626.158741279505, 2025: 22728.94768543169, 2026: 21831.736629583873, 2027: 20934.525573736057, 2028: 20037.31451788824, 2029: 19140.103462040424, 2030: 18242.89240619284, 2031: 17345.681350345025, 2032: 16448.47029449721, 2033: 15551.259238649393, 2034: 14654.048182801576, 2035: 13756.83712695376, 2036: 12859.626071105944, 2037: 11962.41501525836, 2038: 11065.203959410544, 2039: 10167.992903562728, 2040: 9270.781847714912, 2041: 8373.570791867096, 2042: 7476.35973601928, 2043: 6579.148680171464, 2044: 5681.9376243236475, 2045: 4784.726568476064, 2046: 3887.515512628248, 2047: 2990.304456780432, 2048: 2093.0934009326156, 2049: 1195.8823450847995, 2050: 298.6712892369833}</t>
         </is>
       </c>
-      <c r="T281" t="n">
+      <c r="S281" t="n">
         <v>385380.4858799959</v>
       </c>
     </row>
@@ -20728,15 +19323,10 @@
       </c>
       <c r="R282" t="inlineStr">
         <is>
-          <t>{2021: 51341.8145557251, 2022: 39812.972967429705, 2023: 30872.941095311133, 2024: 23940.399845404576, 2025: 18564.565746698307, 2026: 14395.879082597667, 2027: 11163.274023666869, 2028: 8656.552768501628, 2029: 6712.717584015602, 2030: 5205.371995965071, 2031: 4036.501949806206, 2032: 3130.1025178256305, 2033: 2427.235733793895, 2034: 1882.1981944216263, 2035: 1459.5492286802537, 2036: 1131.8063938509576, 2037: 877.6584496024127, 2038: 680.5796100317366, 2039: 527.7549664117965, 2040: 409.2472070377312, 2041: 317.3504507345551, 2042: 246.08917751792978, 2043: 190.82967473742767, 2044: 147.97873326932148, 2045: 114.75000169718453, 2046: 88.9828058302058, 2047: 69.00165242969562, 2048: 53.50728147540936, 2049: 41.49218272425817, 2050: 32.17508308685866}</t>
-        </is>
-      </c>
-      <c r="S282" t="inlineStr">
-        <is>
           <t>{2021: 51341.8145557251, 2022: 48598.024286033586, 2023: 46467.94479240291, 2024: 44337.86529877316, 2025: 42207.785805142485, 2026: 40077.70631151181, 2027: 37947.62681788206, 2028: 35817.54732425138, 2029: 33687.46783062164, 2030: 31557.38833699096, 2031: 29427.308843360282, 2032: 27297.229349730536, 2033: 25167.14985609986, 2034: 23037.070362470113, 2035: 20906.990868839435, 2036: 18776.911375208758, 2037: 16646.83188157901, 2038: 14516.752387948334, 2039: 12386.672894317657, 2040: 10256.59340068791, 2041: 8126.513907057233, 2042: 5996.434413427487, 2043: 3866.3549197968096, 2044: 1736.275426166132, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T282" t="n">
+      <c r="S282" t="n">
         <v>604515.3539681621</v>
       </c>
     </row>
@@ -20800,15 +19390,10 @@
       </c>
       <c r="R283" t="inlineStr">
         <is>
-          <t>{2021: 321310.710146619, 2022: 243087.91866489025, 2023: 183908.39251472143, 2024: 139136.06658492435, 2025: 105263.52147401252, 2026: 79637.21574913689, 2027: 60249.61015426707, 2028: 45581.898985217915, 2029: 34485.02836414552, 2030: 26089.680503692503, 2031: 19738.172217728395, 2032: 14932.932675874094, 2033: 11297.524200437421, 2034: 8547.152513831195, 2035: 6466.356238640533, 2036: 4892.127868005323, 2037: 3701.143919956054, 2038: 2800.1038987177926, 2039: 2118.4212268372626, 2040: 1602.6935630387427, 2041: 1212.519316019459, 2042: 917.332624043712, 2043: 694.0088557908117, 2044: 525.0530497791613, 2045: 397.22937651604525, 2046: 300.52425680356225, 2047: 227.36190792194677, 2048: 172.01086435993497, 2049: 130.13498051753422, 2050: 98.45374138032396}</t>
-        </is>
-      </c>
-      <c r="S283" t="inlineStr">
-        <is>
           <t>{2021: 321310.710146619, 2022: 283814.66819117963, 2023: 270894.65672452375, 2024: 257974.64525786787, 2025: 245054.63379121572, 2026: 232134.62232455984, 2027: 219214.61085790396, 2028: 206294.59939124808, 2029: 193374.5879245922, 2030: 180454.57645793632, 2031: 167534.56499128044, 2032: 154614.55352462456, 2033: 141694.54205796868, 2034: 128774.5305913128, 2035: 115854.51912466064, 2036: 102934.50765800476, 2037: 90014.49619134888, 2038: 77094.484724693, 2039: 64174.47325803712, 2040: 51254.46179138124, 2041: 38334.45032472536, 2042: 25414.43885806948, 2043: 12494.4273914136, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T283" t="n">
+      <c r="S283" t="n">
         <v>3420055.406481857</v>
       </c>
     </row>
@@ -20872,15 +19457,10 @@
       </c>
       <c r="R284" t="inlineStr">
         <is>
-          <t>{2021: 58028.5562909162, 2022: 43926.0027802864, 2023: 33250.76210031045, 2024: 25169.901886625372, 2025: 19052.915511263796, 2026: 14422.52699730437, 2027: 10917.451707850249, 2028: 8264.207223569043, 2029: 6255.774961201006, 2030: 4735.44761239523, 2031: 3584.6021042666403, 2032: 2713.4440706891296, 2033: 2054.001674549681, 2034: 1554.8221261039005, 2035: 1176.9570949119407, 2036: 890.9237783582885, 2037: 674.4045150631396, 2038: 510.5054562306678, 2039: 386.4384283027564, 2040: 292.52313965794116, 2041: 221.43187884073325, 2042: 167.61777213341946, 2043: 126.88199044356655, 2044: 96.04613695800045, 2045: 72.70425371091518, 2046: 55.03509745501345, 2047: 41.660037718372195, 2048: 31.535489586710863, 2049: 23.871488312046782, 2050: 18.070052556670014}</t>
-        </is>
-      </c>
-      <c r="S284" t="inlineStr">
-        <is>
           <t>{2021: 58028.5562909162, 2022: 56737.3606419689, 2023: 55753.71763164108, 2024: 54770.074621313484, 2025: 53786.43161098589, 2026: 52802.78860065807, 2027: 51819.145590330474, 2028: 50835.50258000288, 2029: 49851.859569675056, 2030: 48868.216559347464, 2031: 47884.57354901987, 2032: 46900.93053869228, 2033: 45917.28752836445, 2034: 44933.64451803686, 2035: 43950.00150770927, 2036: 42966.35849738144, 2037: 41982.71548705385, 2038: 40999.07247672626, 2039: 40015.429466398666, 2040: 39031.78645607084, 2041: 38048.14344574325, 2042: 37064.500435415655, 2043: 36080.85742508783, 2044: 35097.21441476024, 2045: 34113.571404432645, 2046: 33129.92839410505, 2047: 32146.285383777227, 2048: 31162.642373449635, 2049: 30178.999363122042, 2050: 29195.356352794217}</t>
         </is>
       </c>
-      <c r="T284" t="n">
+      <c r="S284" t="n">
         <v>1260440.996393126</v>
       </c>
     </row>
@@ -20944,15 +19524,10 @@
       </c>
       <c r="R285" t="inlineStr">
         <is>
-          <t>{2021: 287664.06180264, 2022: 204117.34554762265, 2023: 144835.2306934756, 2024: 102770.5117061602, 2025: 72922.71380226957, 2026: 51743.657786701144, 2027: 36715.66760950562, 2028: 26052.2797512426, 2029: 18485.876042229047, 2030: 13116.99460897884, 2031: 9307.405674415277, 2032: 6604.241518010476, 2033: 4686.161488384187, 2034: 3325.1523941587434, 2035: 2359.4232660966213, 2036: 1674.1723351920093, 2037: 1187.9398869195888, 2038: 842.9246770301436, 2039: 598.1127656120752, 2040: 424.40195445284445, 2041: 301.142241562212, 2042: 213.6810368133915, 2043: 151.62132438405638, 2044: 107.58570976071995, 2045: 76.33942647407048, 2046: 54.16804933807056, 2047: 38.435939390876506, 2048: 27.27293035122896, 2049: 19.352011209580162, 2050: 13.7315768064813}</t>
-        </is>
-      </c>
-      <c r="S285" t="inlineStr">
-        <is>
           <t>{2021: 287664.06180264, 2022: 251449.83134938218, 2023: 248691.59666488506, 2024: 245933.36198038887, 2025: 243175.1272958927, 2026: 240416.8926113965, 2027: 237658.6579269003, 2028: 234900.42324240413, 2029: 232142.188557907, 2030: 229383.95387341082, 2031: 226625.71918891463, 2032: 223867.48450441845, 2033: 221109.24981992226, 2034: 218351.01513542607, 2035: 215592.78045092896, 2036: 212834.54576643277, 2037: 210076.31108193658, 2038: 207318.0763974404, 2039: 204559.8417129442, 2040: 201801.6070284471, 2041: 199043.3723439509, 2042: 196285.13765945472, 2043: 193526.90297495853, 2044: 190768.66829046234, 2045: 188010.43360596616, 2046: 185252.19892146904, 2047: 182493.96423697285, 2048: 179735.72955247667, 2049: 176977.49486798048, 2050: 174219.2601834843}</t>
         </is>
       </c>
-      <c r="T285" t="n">
+      <c r="S285" t="n">
         <v>6228924.228036132</v>
       </c>
     </row>
@@ -21016,15 +19591,10 @@
       </c>
       <c r="R286" t="inlineStr">
         <is>
-          <t>{2021: 95248.2864179093, 2022: 76958.83236554031, 2023: 62181.29587215032, 2024: 50241.3230228685, 2025: 40594.04847847096, 2026: 32799.23124481379, 2027: 26501.16483999652, 2028: 21412.44508551454, 2029: 17300.854785379157, 2030: 13978.766792367202, 2031: 11294.581883926585, 2032: 9125.810726192107, 2033: 7373.484230416704, 2034: 5957.637225606792, 2035: 4813.659350557791, 2036: 3889.3466429306504, 2037: 3142.519278420284, 2038: 2539.0967485998985, 2039: 2051.542640652129, 2040: 1657.608048505727, 2041: 1339.3162725574914, 2042: 1082.1424760541606, 2043: 874.3508628059045, 2044: 706.4591291869469, 2045: 570.8057513776026, 2046: 461.2003615562731, 2047: 372.6412584075848, 2048: 301.0871609012069, 2049: 243.2727896179307, 2050: 196.55985991348425}</t>
-        </is>
-      </c>
-      <c r="S286" t="inlineStr">
-        <is>
           <t>{2021: 95248.2864179093, 2022: 84372.56920722872, 2023: 75426.45974573866, 2024: 66480.35028424859, 2025: 57534.240822758526, 2026: 48588.13136126846, 2027: 39642.021899778396, 2028: 30695.912438292056, 2029: 21749.80297680199, 2030: 12803.693515311927, 2031: 3857.5840538218617, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T286" t="n">
+      <c r="S286" t="n">
         <v>488774.9095142038</v>
       </c>
     </row>
@@ -21088,15 +19658,10 @@
       </c>
       <c r="R287" t="inlineStr">
         <is>
-          <t>{2021: 66972.2779992721, 2022: 50965.42923940103, 2023: 38784.330698511185, 2024: 29514.600979139224, 2025: 22460.402313742794, 2026: 17092.207089356867, 2027: 13007.048542790706, 2028: 9898.271821189343, 2029: 7532.514753353104, 2030: 5732.1903797409195, 2031: 4362.1562818669, 2032: 3319.570036383002, 2033: 2526.1692874826895, 2034: 1922.396936674999, 2035: 1462.9304538097965, 2036: 1113.2797144307742, 2037: 847.1979780962333, 2038: 644.711661217444, 2039: 490.62100814237596, 2040: 373.359112469127, 2041: 284.1236403461992, 2042: 216.21607805340923, 2043: 164.53890409060912, 2044: 125.21294069838386, 2045: 95.28616107533563, 2046: 72.51209373275262, 2047: 55.181189777919556, 2048: 41.99249461102527, 2049: 31.955990995369717, 2050: 24.318282825427445}</t>
-        </is>
-      </c>
-      <c r="S287" t="inlineStr">
-        <is>
           <t>{2021: 66972.2779992721, 2022: 65777.96392579889, 2023: 64487.388164676726, 2024: 63196.81240355503, 2025: 61906.236642432865, 2026: 60615.66088131117, 2027: 59325.08512018947, 2028: 58034.509359067306, 2029: 56743.93359794561, 2030: 55453.357836823445, 2031: 54162.78207570175, 2032: 52872.20631458005, 2033: 51581.630553457886, 2034: 50291.05479233619, 2035: 49000.479031214025, 2036: 47709.90327009233, 2037: 46419.32750897063, 2038: 45128.751747848466, 2039: 43838.17598672677, 2040: 42547.600225604605, 2041: 41257.02446448291, 2042: 39966.448703360744, 2043: 38675.872942239046, 2044: 37385.29718111735, 2045: 36094.721419995185, 2046: 34804.14565887349, 2047: 33513.569897751324, 2048: 32222.994136629626, 2049: 30932.41837550793, 2050: 29641.842614385765}</t>
         </is>
       </c>
-      <c r="T287" t="n">
+      <c r="S287" t="n">
         <v>1402252.41252512</v>
       </c>
     </row>
@@ -21160,15 +19725,10 @@
       </c>
       <c r="R288" t="inlineStr">
         <is>
-          <t>{2021: 66856.4788173378, 2022: 52846.96754108693, 2023: 41773.09406196908, 2024: 33019.707065565075, 2025: 26100.557767597984, 2026: 20631.28889747651, 2027: 16308.083733733549, 2028: 12890.789149823524, 2029: 10189.575159065282, 2030: 8054.389899291902, 2031: 6366.624283849574, 2032: 5032.52329208282, 2033: 3977.977897895146, 2034: 3144.408329125297, 2035: 2485.509973673855, 2036: 1964.6811681581833, 2037: 1552.989983303081, 2038: 1227.567061428424, 2039: 970.3352284983326, 2040: 767.0053109516494, 2041: 606.2823751524211, 2042: 479.23829623082304, 2043: 378.8158026472114, 2044: 299.4364462604096, 2045: 236.69072072097504, 2046: 187.0931143321603, 2047: 147.8884906171349, 2048: 116.8990410741957, 2049: 92.40330837809746, 2050: 73.04055979209008}</t>
-        </is>
-      </c>
-      <c r="S288" t="inlineStr">
-        <is>
           <t>{2021: 66856.4788173378, 2022: 64090.72265093215, 2023: 60465.68601022381, 2024: 56840.64936951548, 2025: 53215.612728807144, 2026: 49590.57608809881, 2027: 45965.539447390474, 2028: 42340.50280668214, 2029: 38715.466165973805, 2030: 35090.42952526547, 2031: 31465.392884557135, 2032: 27840.3562438488, 2033: 24215.319603140466, 2034: 20590.28296243213, 2035: 16965.246321723796, 2036: 13340.20968101453, 2037: 9715.173040306196, 2038: 6090.136399597861, 2039: 2465.099758889526, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T288" t="n">
+      <c r="S288" t="n">
         <v>632430.6410970686</v>
       </c>
     </row>
@@ -21232,15 +19792,10 @@
       </c>
       <c r="R289" t="inlineStr">
         <is>
-          <t>{2021: 30157.3238665339, 2022: 23350.628933289696, 2023: 18080.24723922076, 2024: 13999.423363081813, 2025: 10839.66673163965, 2026: 8393.08675833556, 2027: 6498.715050651013, 2028: 5031.914780055645, 2029: 3896.1804228061947, 2030: 3016.7883500782164, 2031: 2335.8805192632, 2032: 1808.6578066147226, 2033: 1400.4325283127998, 2034: 1084.3462257945819, 2035: 839.602561082705, 2036: 650.0990585918078, 2037: 503.36767129075434, 2038: 389.75446764917064, 2039: 301.7844683250292, 2040: 233.66984314904323, 2041: 180.92911109822666, 2042: 140.0922891958918, 2043: 108.47259113261484, 2044: 83.98965492362358, 2045: 65.0326691796738, 2046: 50.35439262702993, 2047: 38.98909407872783, 2048: 30.189013862990834, 2049: 23.375166301109136, 2050: 18.099246371023273}</t>
-        </is>
-      </c>
-      <c r="S289" t="inlineStr">
-        <is>
           <t>{2021: 30157.3238665339, 2022: 29415.63985156198, 2023: 28415.935537898447, 2024: 27416.23122423468, 2025: 26416.52691057115, 2026: 25416.822596907616, 2027: 24417.118283244083, 2028: 23417.413969580317, 2029: 22417.709655916784, 2030: 21418.00534225325, 2031: 20418.301028589718, 2032: 19418.596714925952, 2033: 18418.89240126242, 2034: 17419.188087598886, 2035: 16419.483773935353, 2036: 15419.779460271588, 2037: 14420.075146608055, 2038: 13420.370832944522, 2039: 12420.666519280756, 2040: 11420.962205617223, 2041: 10421.25789195369, 2042: 9421.553578290157, 2043: 8421.849264626391, 2044: 7422.144950962858, 2045: 6422.440637299325, 2046: 5422.736323635792, 2047: 4423.032009972027, 2048: 3423.3276963084936, 2049: 2423.6233826449607, 2050: 1423.9190689811949}</t>
         </is>
       </c>
-      <c r="T289" t="n">
+      <c r="S289" t="n">
         <v>461540.306746654</v>
       </c>
     </row>
@@ -21304,15 +19859,10 @@
       </c>
       <c r="R290" t="inlineStr">
         <is>
-          <t>{2021: 25041.7369677682, 2022: 19047.74741414692, 2023: 14488.479054792826, 2024: 11020.517059422154, 2025: 8382.646363203887, 2026: 6376.176332893383, 2027: 4849.974920403412, 2028: 3689.085041013623, 2029: 2806.065735015901, 2030: 2134.405908698392, 2031: 1623.5145621279587, 2032: 1234.9101558891891, 2033: 939.3220909083952, 2034: 714.4859779966795, 2035: 543.4666316217358, 2036: 413.3824718497809, 2037: 314.43525340774653, 2038: 239.1720387736274, 2039: 181.92382537003488, 2040: 138.37854293909353, 2041: 105.25625825533335, 2042: 80.06212283063083, 2043: 60.89845505050741, 2044: 46.32180232572844, 2045: 35.234216843830836, 2046: 26.800555554129524, 2047: 20.385575226308596, 2048: 15.50608443426293, 2049: 11.794548439927912, 2050: 8.97140561123344}</t>
-        </is>
-      </c>
-      <c r="S290" t="inlineStr">
-        <is>
           <t>{2021: 25041.7369677682, 2022: 23382.21895939717, 2023: 22604.059352454497, 2024: 21825.899745511822, 2025: 21047.74013856938, 2026: 20269.580531626707, 2027: 19491.420924684033, 2028: 18713.26131774136, 2029: 17935.101710798917, 2030: 17156.942103856243, 2031: 16378.782496913569, 2032: 15600.622889971128, 2033: 14822.463283028454, 2034: 14044.30367608578, 2035: 13266.144069143105, 2036: 12487.984462200664, 2037: 11709.82485525799, 2038: 10931.665248315316, 2039: 10153.505641372642, 2040: 9375.3460344302, 2041: 8597.186427487526, 2042: 7819.026820544852, 2043: 7040.867213602411, 2044: 6262.7076066597365, 2045: 5484.547999717062, 2046: 4706.388392774388, 2047: 3928.228785831947, 2048: 3150.0691788892727, 2049: 2371.9095719465986, 2050: 1593.7499650041573}</t>
         </is>
       </c>
-      <c r="T290" t="n">
+      <c r="S290" t="n">
         <v>373875.5429051989</v>
       </c>
     </row>
@@ -21376,15 +19926,10 @@
       </c>
       <c r="R291" t="inlineStr">
         <is>
-          <t>{2021: 15397.0438344427, 2022: 11904.74278927076, 2023: 9204.55266625042, 2024: 7116.809769475715, 2025: 5502.601063994718, 2026: 4254.5212602621505, 2027: 3289.5263428168473, 2028: 2543.408035389445, 2029: 1966.5215475806788, 2030: 1520.4823383783023, 2031: 1175.6121076651987, 2032: 908.9640785719853, 2033: 702.7961780481384, 2034: 543.3905250194706, 2035: 420.14067791460184, 2036: 324.8459093618096, 2037: 251.16555091233076, 2038: 194.1971012934389, 2039: 150.15002660113095, 2040: 116.09354793743262, 2041: 89.76163493133517, 2042: 69.40222991452207, 2043: 53.66067051689492, 2044: 41.489553921670776, 2045: 32.07904537974891, 2046: 24.802993891397062, 2047: 19.177269731506446, 2048: 14.827551704655855, 2049: 11.46442077690755, 2050: 8.864102878745623}</t>
-        </is>
-      </c>
-      <c r="S291" t="inlineStr">
-        <is>
           <t>{2021: 15397.0438344427, 2022: 14216.414564732928, 2023: 13522.019320736174, 2024: 12827.624076739652, 2025: 12133.22883274313, 2026: 11438.833588746376, 2027: 10744.438344749855, 2028: 10050.043100753333, 2029: 9355.64785675658, 2030: 8661.252612760058, 2031: 7966.857368763536, 2032: 7272.462124766782, 2033: 6578.0668807702605, 2034: 5883.671636773739, 2035: 5189.276392776985, 2036: 4494.881148780463, 2037: 3800.485904783942, 2038: 3106.0906607871875, 2039: 2411.695416790666, 2040: 1717.3001727941446, 2041: 1022.9049287973903, 2042: 328.50968480086885, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="T291" t="n">
+      <c r="S291" t="n">
         <v>160420.2265373254</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Store trend coefficients in df to use later and reuse trend emission values, both instead of recalculating them
</commit_message>
<xml_diff>
--- a/data/tests/reference_dataframes/df_trend.xlsx
+++ b/data/tests/reference_dataframes/df_trend.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S291"/>
+  <dimension ref="A1:T291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,10 +494,15 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
+          <t>trendCoefficients</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>trend</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>trendEmission</t>
         </is>
@@ -563,10 +568,15 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
+          <t>[ 7.82334178e+02 -1.43894275e+06]</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
           <t>{2021: 140535.25077554, 2022: 142936.95388118387, 2023: 143719.28805910517, 2024: 144501.62223702623, 2025: 145283.9564149473, 2026: 146066.29059286858, 2027: 146848.62477078964, 2028: 147630.95894871093, 2029: 148413.293126632, 2030: 149195.6273045533, 2031: 149977.96148247435, 2032: 150760.2956603954, 2033: 151542.6298383167, 2034: 152324.96401623776, 2035: 153107.29819415906, 2036: 153889.63237208012, 2037: 154671.96655000118, 2038: 155454.30072792247, 2039: 156236.63490584353, 2040: 157018.96908376482, 2041: 157801.30326168588, 2042: 158583.63743960718, 2043: 159365.97161752824, 2044: 160148.3057954493, 2045: 160930.6399733706, 2046: 161712.97415129165, 2047: 162495.30832921294, 2048: 163277.642507134, 2049: 164059.97668505507, 2050: 164842.31086297636}</t>
         </is>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>4450645.808746605</v>
       </c>
     </row>
@@ -630,10 +640,15 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
+          <t>[-1.97662497e+03  4.06091905e+06]</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
           <t>{2021: 63674.7692719455, 2022: 64183.36643868731, 2023: 62206.74147178279, 2024: 60230.11650487827, 2025: 58253.49153797375, 2026: 56276.86657106923, 2027: 54300.24160416471, 2028: 52323.61663726065, 2029: 50346.99167035613, 2030: 48370.36670345161, 2031: 46393.74173654709, 2032: 44417.11676964257, 2033: 42440.49180273805, 2034: 40463.86683583353, 2035: 38487.241868929006, 2036: 36510.616902024485, 2037: 34533.991935119964, 2038: 32557.366968215443, 2039: 30580.742001310922, 2040: 28604.1170344064, 2041: 26627.49206750188, 2042: 24650.86710059736, 2043: 22674.24213369284, 2044: 20697.617166788317, 2045: 18720.992199883796, 2046: 16744.367232979275, 2047: 14767.742266074754, 2048: 12791.117299170233, 2049: 10814.492332265712, 2050: 8837.867365361191}</t>
         </is>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>1086226.341111999</v>
       </c>
     </row>
@@ -697,10 +712,15 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
+          <t>[-2.03302222e+03  4.16139769e+06]</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
           <t>{2021: 52912.9774987249, 2022: 50626.769764077384, 2023: 48593.747548584826, 2024: 46560.7253330918, 2025: 44527.70311759878, 2026: 42494.68090210622, 2027: 40461.6586866132, 2028: 38428.63647112064, 2029: 36395.61425562762, 2030: 34362.592040134594, 2031: 32329.569824642036, 2032: 30296.547609149013, 2033: 28263.52539365599, 2034: 26230.50317816343, 2035: 24197.48096267041, 2036: 22164.45874717785, 2037: 20131.436531684827, 2038: 18098.414316191804, 2039: 16065.392100699246, 2040: 14032.369885206223, 2041: 11999.3476697132, 2042: 9966.325454220641, 2043: 7933.303238727618, 2044: 5900.28102323506, 2045: 3867.258807742037, 2046: 1834.2365922490135, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>682219.0682034459</v>
       </c>
     </row>
@@ -764,10 +784,15 @@
       </c>
       <c r="R5" t="inlineStr">
         <is>
+          <t>[-3.70447730e+02  7.65127013e+05]</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
           <t>{2021: 16087.2823225698, 2022: 16081.702993880841, 2023: 15711.255263767787, 2024: 15340.807533654734, 2025: 14970.359803541796, 2026: 14599.912073428743, 2027: 14229.464343315689, 2028: 13859.016613202752, 2029: 13488.568883089698, 2030: 13118.121152976644, 2031: 12747.673422863707, 2032: 12377.225692750653, 2033: 12006.777962637716, 2034: 11636.330232524662, 2035: 11265.882502411609, 2036: 10895.434772298671, 2037: 10524.987042185618, 2038: 10154.539312072564, 2039: 9784.091581959627, 2040: 9413.643851846573, 2041: 9043.19612173352, 2042: 8672.748391620582, 2043: 8302.300661507528, 2044: 7931.852931394591, 2045: 7561.405201281537, 2046: 7190.957471168484, 2047: 6820.509741055546, 2048: 6450.062010942493, 2049: 6079.614280829439, 2050: 5709.166550716502}</t>
         </is>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>321156.666282587</v>
       </c>
     </row>
@@ -831,10 +856,15 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
+          <t>[-7.49654314e+02  1.56196192e+06]</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
           <t>{2021: 46192.2589353511, 2022: 46160.89896231075, 2023: 45411.244647955056, 2024: 44661.590333599364, 2025: 43911.936019243905, 2026: 43162.28170488821, 2027: 42412.62739053252, 2028: 41662.97307617706, 2029: 40913.31876182137, 2030: 40163.66444746568, 2031: 39414.01013311022, 2032: 38664.35581875453, 2033: 37914.701504398836, 2034: 37165.04719004338, 2035: 36415.392875687685, 2036: 35665.73856133199, 2037: 34916.084246976534, 2038: 34166.42993262084, 2039: 33416.77561826515, 2040: 32667.12130390969, 2041: 31917.466989554, 2042: 31167.812675198307, 2043: 30418.158360842615, 2044: 29668.504046487156, 2045: 28918.849732131464, 2046: 28169.195417775773, 2047: 27419.541103420313, 2048: 26669.88678906462, 2049: 25920.23247470893, 2050: 25170.57816035347}</t>
         </is>
       </c>
-      <c r="S6" t="n">
+      <c r="T6" t="n">
         <v>1044817.258666128</v>
       </c>
     </row>
@@ -898,10 +928,15 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
+          <t>[-9.25516465e+02  1.88084374e+06]</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
           <t>{2021: 11742.698661745, 2022: 9449.445710867876, 2023: 8523.929245739244, 2024: 7598.4127806108445, 2025: 6672.896315482212, 2026: 5747.379850353813, 2027: 4821.8633852251805, 2028: 3896.346920096781, 2029: 2970.830454968149, 2030: 2045.3139898397494, 2031: 1119.7975247111171, 2032: 194.28105958271772, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S7" t="n">
+      <c r="T7" t="n">
         <v>58911.84656835019</v>
       </c>
     </row>
@@ -965,10 +1000,15 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
+          <t>[-6.81424027e+02  1.41330127e+06]</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
           <t>{2021: 36324.1026555328, 2022: 35461.88679012493, 2023: 34780.46276358259, 2024: 34099.03873704001, 2025: 33417.61471049767, 2026: 32736.190683955327, 2027: 32054.766657412983, 2028: 31373.342630870407, 2029: 30691.918604328064, 2030: 30010.49457778572, 2031: 29329.070551243378, 2032: 28647.646524701035, 2033: 27966.22249815846, 2034: 27284.798471616115, 2035: 26603.374445073772, 2036: 25921.95041853143, 2037: 25240.526391988853, 2038: 24559.10236544651, 2039: 23877.678338904167, 2040: 23196.254312361823, 2041: 22514.83028581948, 2042: 21833.406259276904, 2043: 21151.98223273456, 2044: 20470.558206192218, 2045: 19789.134179649875, 2046: 19107.7101531073, 2047: 18426.286126564955, 2048: 17744.862100022612, 2049: 17063.43807348027, 2050: 16382.014046937926}</t>
         </is>
       </c>
-      <c r="S8" t="n">
+      <c r="T8" t="n">
         <v>761707.6064417068</v>
       </c>
     </row>
@@ -1032,10 +1072,15 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
+          <t>[-1.49086232e+03  3.07417898e+06]</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
           <t>{2021: 62127.6159510355, 2022: 59655.35764219379, 2023: 58164.495317440946, 2024: 56673.63299268857, 2025: 55182.77066793572, 2026: 53691.90834318288, 2027: 52201.0460184305, 2028: 50710.18369367765, 2029: 49219.32136892481, 2030: 47728.45904417243, 2031: 46237.596719419584, 2032: 44746.73439466674, 2033: 43255.87206991436, 2034: 41765.009745161515, 2035: 40274.14742040867, 2036: 38783.28509565629, 2037: 37292.422770903446, 2038: 35801.56044615107, 2039: 34310.69812139822, 2040: 32819.83579664538, 2041: 31328.973471892998, 2042: 29838.111147140153, 2043: 28347.248822387308, 2044: 26856.38649763493, 2045: 25365.524172882084, 2046: 23874.66184812924, 2047: 22383.79952337686, 2048: 20892.937198624015, 2049: 19402.07487387117, 2050: 17911.21254911879}</t>
         </is>
       </c>
-      <c r="S9" t="n">
+      <c r="T9" t="n">
         <v>1146823.469474989</v>
       </c>
     </row>
@@ -1099,10 +1144,15 @@
       </c>
       <c r="R10" t="inlineStr">
         <is>
+          <t>[ 7.10153688e+02 -1.35531898e+06]</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
           <t>{2021: 83063.063221357, 2022: 80611.78063574666, 2023: 81321.93432401074, 2024: 82032.08801227505, 2025: 82742.24170053913, 2026: 83452.39538880321, 2027: 84162.54907706729, 2028: 84872.70276533137, 2029: 85582.85645359545, 2030: 86293.01014185953, 2031: 87003.16383012361, 2032: 87713.31751838769, 2033: 88423.47120665177, 2034: 89133.62489491585, 2035: 89843.77858317993, 2036: 90553.932271444, 2037: 91264.08595970809, 2038: 91974.23964797216, 2039: 92684.39333623624, 2040: 93394.54702450056, 2041: 94104.70071276464, 2042: 94814.85440102872, 2043: 95525.0080892928, 2044: 96235.16177755687, 2045: 96945.31546582095, 2046: 97655.46915408503, 2047: 98365.62284234911, 2048: 99075.77653061319, 2049: 99785.93021887727, 2050: 100496.08390714135}</t>
         </is>
       </c>
-      <c r="S10" t="n">
+      <c r="T10" t="n">
         <v>2617347.525528986</v>
       </c>
     </row>
@@ -1166,10 +1216,15 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
+          <t>[-1.34025379e+03  2.91789445e+06]</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
           <t>{2021: 207670.893624396, 2022: 207901.28197011352, 2023: 206561.02817861876, 2024: 205220.774387124, 2025: 203880.5205956297, 2026: 202540.26680413494, 2027: 201200.01301264018, 2028: 199859.75922114542, 2029: 198519.50542965112, 2030: 197179.25163815636, 2031: 195838.9978466616, 2032: 194498.74405516684, 2033: 193158.49026367208, 2034: 191818.23647217778, 2035: 190477.98268068302, 2036: 189137.72888918826, 2037: 187797.4750976935, 2038: 186457.2213061992, 2039: 185116.96751470445, 2040: 183776.7137232097, 2041: 182436.45993171493, 2042: 181096.20614022063, 2043: 179755.95234872587, 2044: 178415.6985572311, 2045: 177075.44476573635, 2046: 175735.19097424205, 2047: 174394.9371827473, 2048: 173054.68339125253, 2049: 171714.42959975777, 2050: 170374.175808263}</t>
         </is>
       </c>
-      <c r="S11" t="n">
+      <c r="T11" t="n">
         <v>5503642.496694528</v>
       </c>
     </row>
@@ -1233,10 +1288,15 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
+          <t>[-1.43039005e+03  2.94775270e+06]</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
           <t>{2021: 54901.5850984739, 2022: 55504.01357598929, 2023: 54073.623524431605, 2024: 52643.23347287392, 2025: 51212.84342131624, 2026: 49782.45336975856, 2027: 48352.063318200875, 2028: 46921.67326664319, 2029: 45491.28321508551, 2030: 44060.89316352783, 2031: 42630.503111970145, 2032: 41200.11306041246, 2033: 39769.72300885478, 2034: 38339.33295729663, 2035: 36908.94290573895, 2036: 35478.55285418127, 2037: 34048.162802623585, 2038: 32617.772751065902, 2039: 31187.38269950822, 2040: 29756.992647950538, 2041: 28326.602596392855, 2042: 26896.212544835173, 2043: 25465.82249327749, 2044: 24035.432441719808, 2045: 22605.042390162125, 2046: 21174.652338604443, 2047: 19744.26228704676, 2048: 18313.872235489078, 2049: 16883.482183931395, 2050: 15453.092132373713}</t>
         </is>
       </c>
-      <c r="S12" t="n">
+      <c r="T12" t="n">
         <v>1048602.279254312</v>
       </c>
     </row>
@@ -1300,10 +1360,15 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
+          <t>[-4.27946398e+03  8.67340974e+06]</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
           <t>{2021: 28585.8132476701, 2022: 20333.569486629218, 2023: 16054.105502955616, 2024: 11774.64151928015, 2025: 7495.177535606548, 2026: 3215.713551931083, 2027: 0, 2028: 0, 2029: 0, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S13" t="n">
+      <c r="T13" t="n">
         <v>73166.11422023766</v>
       </c>
     </row>
@@ -1367,10 +1432,15 @@
       </c>
       <c r="R14" t="inlineStr">
         <is>
+          <t>[-1.30334742e+02  2.75514016e+05]</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
           <t>{2021: 11516.2724727444, 2022: 11977.16764754086, 2023: 11846.832905431918, 2024: 11716.498163323035, 2025: 11586.16342121415, 2026: 11455.828679105209, 2027: 11325.493936996325, 2028: 11195.159194887383, 2029: 11064.8244527785, 2030: 10934.489710669615, 2031: 10804.154968560673, 2032: 10673.82022645179, 2033: 10543.485484342847, 2034: 10413.150742233964, 2035: 10282.816000125022, 2036: 10152.481258016138, 2037: 10022.146515907254, 2038: 9891.811773798312, 2039: 9761.477031689428, 2040: 9631.142289580486, 2041: 9500.807547471602, 2042: 9370.472805362719, 2043: 9240.138063253777, 2044: 9109.803321144893, 2045: 8979.46857903595, 2046: 8849.133836927067, 2047: 8718.799094818125, 2048: 8588.464352709241, 2049: 8458.129610600357, 2050: 8327.794868491415}</t>
         </is>
       </c>
-      <c r="S14" t="n">
+      <c r="T14" t="n">
         <v>296016.1952845945</v>
       </c>
     </row>
@@ -1434,10 +1504,15 @@
       </c>
       <c r="R15" t="inlineStr">
         <is>
+          <t>[-3.46625532e+03  7.05233467e+06]</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
           <t>{2021: 50848.2087199788, 2022: 43566.39934455324, 2023: 40100.144019882195, 2024: 36633.88869521022, 2025: 33167.63337053824, 2026: 29701.378045867197, 2027: 26235.12272119522, 2028: 22768.867396523245, 2029: 19302.6120718522, 2030: 15836.356747180223, 2031: 12370.101422508247, 2032: 8903.846097837202, 2033: 5437.590773165226, 2034: 1971.3354484932497, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S15" t="n">
+      <c r="T15" t="n">
         <v>321419.3805147953</v>
       </c>
     </row>
@@ -1501,10 +1576,15 @@
       </c>
       <c r="R16" t="inlineStr">
         <is>
+          <t>[ 2.97889749e+03 -5.90337105e+06]</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
           <t>{2021: 117644.889726228, 2022: 119959.68802870438, 2023: 122938.58552350104, 2024: 125917.4830182977, 2025: 128896.38051309437, 2026: 131875.27800789196, 2027: 134854.17550268862, 2028: 137833.0729974853, 2029: 140811.97049228195, 2030: 143790.86798707955, 2031: 146769.7654818762, 2032: 149748.66297667287, 2033: 152727.56047146954, 2034: 155706.45796626713, 2035: 158685.3554610638, 2036: 161664.25295586046, 2037: 164643.15045065712, 2038: 167622.04794545472, 2039: 170600.94544025138, 2040: 173579.84293504804, 2041: 176558.7404298447, 2042: 179537.6379246423, 2043: 182516.53541943897, 2044: 185495.43291423563, 2045: 188474.3304090323, 2046: 191453.2279038299, 2047: 194432.12539862655, 2048: 197411.02289342321, 2049: 200389.92038821988, 2050: 203368.81788301654}</t>
         </is>
       </c>
-      <c r="S16" t="n">
+      <c r="T16" t="n">
         <v>4645401.371641561</v>
       </c>
     </row>
@@ -1568,10 +1648,15 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
+          <t>[ 8.44335003e+01 -1.28592103e+05]</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
           <t>{2021: 40428.9261016411, 2022: 42132.43465925561, 2023: 42216.868159533944, 2024: 42301.30165981231, 2025: 42385.73516009064, 2026: 42470.168660369, 2027: 42554.60216064734, 2028: 42639.0356609257, 2029: 42723.46916120403, 2030: 42807.902661482396, 2031: 42892.33616176073, 2032: 42976.76966203909, 2033: 43061.203162317426, 2034: 43145.63666259579, 2035: 43230.07016287412, 2036: 43314.503663152485, 2037: 43398.93716343082, 2038: 43483.37066370918, 2039: 43567.804163987515, 2040: 43652.23766426588, 2041: 43736.67116454421, 2042: 43821.104664822575, 2043: 43905.53816510091, 2044: 43989.97166537927, 2045: 44074.405165657605, 2046: 44158.83866593597, 2047: 44243.2721662143, 2048: 44327.705666492664, 2049: 44412.13916677103, 2050: 44496.57266704936}</t>
         </is>
       </c>
-      <c r="S17" t="n">
+      <c r="T17" t="n">
         <v>1254086.782948718</v>
       </c>
     </row>
@@ -1635,10 +1720,15 @@
       </c>
       <c r="R18" t="inlineStr">
         <is>
+          <t>[-2.58073148e+03  5.29470099e+06]</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
           <t>{2021: 83466.9995600362, 2022: 76461.93214879185, 2023: 73881.20066807512, 2024: 71300.46918735933, 2025: 68719.7377066426, 2026: 66139.0062259268, 2027: 63558.274745210074, 2028: 60977.54326449428, 2029: 58396.81178377755, 2030: 55816.08030306175, 2031: 53235.34882234596, 2032: 50654.61734162923, 2033: 48073.88586091343, 2034: 45493.154380196705, 2035: 42912.42289948091, 2036: 40331.69141876418, 2037: 37750.959938048385, 2038: 35170.22845733166, 2039: 32589.49697661586, 2040: 30008.765495900065, 2041: 27428.034015183337, 2042: 24847.30253446754, 2043: 22266.571053750813, 2044: 19685.839573035017, 2045: 17105.10809231829, 2046: 14524.376611602493, 2047: 11943.645130885765, 2048: 9362.913650169969, 2049: 6782.182169454172, 2050: 4201.450688737445}</t>
         </is>
       </c>
-      <c r="S18" t="n">
+      <c r="T18" t="n">
         <v>1209251.82557982</v>
       </c>
     </row>
@@ -1702,10 +1792,15 @@
       </c>
       <c r="R19" t="inlineStr">
         <is>
+          <t>[-1.49114673e+03  3.05939939e+06]</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
           <t>{2021: 44760.6499832772, 2022: 44300.70058780536, 2023: 42809.55385685153, 2024: 41318.407125897706, 2025: 39827.26039494388, 2026: 38336.11366399005, 2027: 36844.96693303622, 2028: 35353.820202082396, 2029: 33862.67347112857, 2030: 32371.52674017474, 2031: 30880.380009220913, 2032: 29389.233278267086, 2033: 27898.086547313258, 2034: 26406.93981635943, 2035: 24915.793085405603, 2036: 23424.646354451776, 2037: 21933.499623498414, 2038: 20442.352892544586, 2039: 18951.20616159076, 2040: 17460.05943063693, 2041: 15968.912699683104, 2042: 14477.765968729276, 2043: 12986.619237775449, 2044: 11495.472506821621, 2045: 10004.325775867794, 2046: 8513.179044913966, 2047: 7022.032313960139, 2048: 5530.885583006311, 2049: 4039.7388520524837, 2050: 2548.592121098656}</t>
         </is>
       </c>
-      <c r="S19" t="n">
+      <c r="T19" t="n">
         <v>700420.7732101972</v>
       </c>
     </row>
@@ -1769,10 +1864,15 @@
       </c>
       <c r="R20" t="inlineStr">
         <is>
+          <t>[-9.94240159e+03  2.04566616e+07]</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
           <t>{2021: 374800.097747541, 2022: 353125.6057465039, 2023: 343183.20415410027, 2024: 333240.80256170034, 2025: 323298.4009692967, 2026: 313355.99937689677, 2027: 303413.5977844931, 2028: 293471.1961920932, 2029: 283528.79459968954, 2030: 273586.3930072896, 2031: 263643.99141488597, 2032: 253701.58982248604, 2033: 243759.1882300824, 2034: 233816.78663768247, 2035: 223874.38504527882, 2036: 213931.9834528789, 2037: 203989.58186047524, 2038: 194047.18026807532, 2039: 184104.77867567167, 2040: 174162.37708327174, 2041: 164219.9754908681, 2042: 154277.57389846817, 2043: 144335.17230606452, 2044: 134392.7707136646, 2045: 124450.36912126094, 2046: 114507.96752886102, 2047: 104565.56593645737, 2048: 94623.16434405744, 2049: 84680.76275165752, 2050: 74738.36115925387}</t>
         </is>
       </c>
-      <c r="S20" t="n">
+      <c r="T20" t="n">
         <v>6354058.38842761</v>
       </c>
     </row>
@@ -1836,10 +1936,15 @@
       </c>
       <c r="R21" t="inlineStr">
         <is>
+          <t>[-5.83888263e+03  1.20117642e+07]</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
           <t>{2021: 211464.938310871, 2022: 205543.5100499764, 2023: 199704.62742255442, 2024: 193865.74479513243, 2025: 188026.86216771044, 2026: 182187.97954028845, 2027: 176349.09691286646, 2028: 170510.21428544447, 2029: 164671.33165802248, 2030: 158832.4490306005, 2031: 152993.5664031785, 2032: 147154.6837757565, 2033: 141315.80114833452, 2034: 135476.91852091253, 2035: 129638.03589349054, 2036: 123799.15326606855, 2037: 117960.27063864656, 2038: 112121.38801122457, 2039: 106282.50538380258, 2040: 100443.62275638059, 2041: 94604.7401289586, 2042: 88765.85750153661, 2043: 82926.97487411462, 2044: 77088.09224669263, 2045: 71249.20961927064, 2046: 65410.32699184865, 2047: 59571.44436442666, 2048: 53732.56173700467, 2049: 47893.67910958268, 2050: 42054.79648216069}</t>
         </is>
       </c>
-      <c r="S21" t="n">
+      <c r="T21" t="n">
         <v>3674880.515630343</v>
       </c>
     </row>
@@ -1903,10 +2008,15 @@
       </c>
       <c r="R22" t="inlineStr">
         <is>
+          <t>[-4.71668918e+03  9.61876688e+06]</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
           <t>{2021: 87998.058069537, 2022: 81621.35252710804, 2023: 76904.6633452028, 2024: 72187.97416329756, 2025: 67471.28498139232, 2026: 62754.595799487084, 2027: 58037.906617581844, 2028: 53321.217435676605, 2029: 48604.528253771365, 2030: 43887.839071866125, 2031: 39171.149889960885, 2032: 34454.460708055645, 2033: 29737.771526150405, 2034: 25021.082344245166, 2035: 20304.393162339926, 2036: 15587.703980434686, 2037: 10871.014798529446, 2038: 6154.325616624206, 2039: 1437.6364347189665, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S22" t="n">
+      <c r="T22" t="n">
         <v>791529.9296912116</v>
       </c>
     </row>
@@ -1970,10 +2080,15 @@
       </c>
       <c r="R23" t="inlineStr">
         <is>
+          <t>[-1.73273706e+03  3.54131698e+06]</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
           <t>{2021: 42576.6794264777, 2022: 37722.64099948527, 2023: 35989.90393816214, 2024: 34257.16687683854, 2025: 32524.429815514944, 2026: 30791.692754191812, 2027: 29058.955692868214, 2028: 27326.21863154508, 2029: 25593.481570221484, 2030: 23860.744508897886, 2031: 22128.007447574753, 2032: 20395.270386251155, 2033: 18662.533324927557, 2034: 16929.796263604425, 2035: 15197.059202280827, 2036: 13464.322140957695, 2037: 11731.585079634096, 2038: 9998.848018310498, 2039: 8266.110956987366, 2040: 6533.373895663768, 2041: 4800.63683434017, 2042: 3067.8997730170377, 2043: 1335.1627116934396, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S23" t="n">
+      <c r="T23" t="n">
         <v>450924.180536207</v>
       </c>
     </row>
@@ -2037,10 +2152,15 @@
       </c>
       <c r="R24" t="inlineStr">
         <is>
+          <t>[-1.62665755e+03  3.35886220e+06]</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
           <t>{2021: 69760.3160810483, 2022: 69760.62110681739, 2023: 68133.9635529453, 2024: 66507.3059990732, 2025: 64880.64844520064, 2026: 63253.99089132855, 2027: 61627.33333745645, 2028: 60000.67578358436, 2029: 58374.0182297118, 2030: 56747.36067583971, 2031: 55120.703121967614, 2032: 53494.045568095054, 2033: 51867.38801422296, 2034: 50240.73046035087, 2035: 48614.072906478774, 2036: 46987.415352606215, 2037: 45360.75779873412, 2038: 43734.10024486203, 2039: 42107.44269098947, 2040: 40480.785137117375, 2041: 38854.12758324528, 2042: 37227.47002937319, 2043: 35600.81247550063, 2044: 33974.154921628535, 2045: 32347.49736775644, 2046: 30720.839813884348, 2047: 29094.18226001179, 2048: 27467.524706139695, 2049: 25840.8671522676, 2050: 24214.209598395042}</t>
         </is>
       </c>
-      <c r="S24" t="n">
+      <c r="T24" t="n">
         <v>1385408.098466911</v>
       </c>
     </row>
@@ -2104,10 +2224,15 @@
       </c>
       <c r="R25" t="inlineStr">
         <is>
+          <t>[-2.00557054e+03  4.08099956e+06]</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
           <t>{2021: 27906.4222363986, 2022: 25735.92634930974, 2023: 23730.355808773078, 2024: 21724.785268236417, 2025: 19719.214727699757, 2026: 17713.644187163096, 2027: 15708.073646626435, 2028: 13702.503106089775, 2029: 11696.932565553114, 2030: 9691.362025016919, 2031: 7685.791484480258, 2032: 5680.220943943597, 2033: 3674.6504034069367, 2034: 1669.079862870276, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S25" t="n">
+      <c r="T25" t="n">
         <v>192085.7514973687</v>
       </c>
     </row>
@@ -2171,10 +2296,15 @@
       </c>
       <c r="R26" t="inlineStr">
         <is>
+          <t>[-4.37592516e+03  8.89837716e+06]</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
           <t>{2021: 51015.1708721754, 2022: 50256.47665881179, 2023: 45880.55149605684, 2024: 41504.62633330189, 2025: 37128.701170546934, 2026: 32752.77600779198, 2027: 28376.85084503703, 2028: 24000.925682282075, 2029: 19625.000519527122, 2030: 15249.07535677217, 2031: 10873.150194017217, 2032: 6497.225031262264, 2033: 2121.2998685091734, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S26" t="n">
+      <c r="T26" t="n">
         <v>339774.2446000042</v>
       </c>
     </row>
@@ -2238,10 +2368,15 @@
       </c>
       <c r="R27" t="inlineStr">
         <is>
+          <t>[-1.59397702e+03  3.26160822e+06]</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
           <t>{2021: 40976.4441285849, 2022: 38586.685532626696, 2023: 36992.708514933474, 2024: 35398.73149724072, 2025: 33804.75447954796, 2026: 32210.77746185474, 2027: 30616.800444161985, 2028: 29022.82342646923, 2029: 27428.846408776008, 2030: 25834.86939108325, 2031: 24240.89237339003, 2032: 22646.915355697274, 2033: 21052.93833800452, 2034: 19458.961320311297, 2035: 17864.98430261854, 2036: 16271.007284925785, 2037: 14677.030267232563, 2038: 13083.053249539807, 2039: 11489.076231846586, 2040: 9895.09921415383, 2041: 8301.122196461074, 2042: 6707.1451787678525, 2043: 5113.168161075097, 2044: 3519.1911433823407, 2045: 1925.214125689119, 2046: 331.2371079963632, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S27" t="n">
+      <c r="T27" t="n">
         <v>506962.2550720786</v>
       </c>
     </row>
@@ -2305,10 +2440,15 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
+          <t>[-4.36267675e+02  8.94073259e+05]</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
           <t>{2021: 12572.1630489804, 2022: 11940.020779401646, 2023: 11503.75310466357, 2024: 11067.485429925495, 2025: 10631.217755187536, 2026: 10194.95008044946, 2027: 9758.682405711384, 2028: 9322.414730973309, 2029: 8886.147056235233, 2030: 8449.879381497158, 2031: 8013.611706759082, 2032: 7577.344032021123, 2033: 7141.076357283047, 2034: 6704.808682544972, 2035: 6268.541007806896, 2036: 5832.273333068821, 2037: 5396.005658330745, 2038: 4959.7379835926695, 2039: 4523.47030885471, 2040: 4087.2026341166347, 2041: 3650.934959378559, 2042: 3214.6672846404836, 2043: 2778.399609902408, 2044: 2342.1319351643324, 2045: 1905.8642604263732, 2046: 1469.5965856882976, 2047: 1033.328910950222, 2048: 597.0612362121465, 2049: 160.79356147407088, 2050: 0}</t>
         </is>
       </c>
-      <c r="S28" t="n">
+      <c r="T28" t="n">
         <v>175697.4822967506</v>
       </c>
     </row>
@@ -2372,10 +2512,15 @@
       </c>
       <c r="R29" t="inlineStr">
         <is>
+          <t>[-3.91068473e+03  7.93211653e+06]</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
           <t>{2021: 32705.8422088023, 2022: 24712.003630937077, 2023: 20801.318899401464, 2024: 16890.63416786585, 2025: 12979.949436329305, 2026: 9069.264704793692, 2027: 5158.579973257147, 2028: 1247.8952417215332, 2029: 0, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S29" t="n">
+      <c r="T29" t="n">
         <v>107212.5671587072</v>
       </c>
     </row>
@@ -2439,10 +2584,15 @@
       </c>
       <c r="R30" t="inlineStr">
         <is>
+          <t>[-8.76889043e+02  1.82460620e+06]</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
           <t>{2021: 52284.4338444058, 2022: 51536.55996318464, 2023: 50659.67092035944, 2024: 49782.781877534, 2025: 48905.89283470879, 2026: 48029.003791883355, 2027: 47152.11474905815, 2028: 46275.22570623271, 2029: 45398.33666340751, 2030: 44521.44762058207, 2031: 43644.55857775686, 2032: 42767.66953493166, 2033: 41890.78049210622, 2034: 41013.891449281015, 2035: 40137.00240645558, 2036: 39260.11336363037, 2037: 38383.22432080493, 2038: 37506.33527797973, 2039: 36629.44623515429, 2040: 35752.557192329085, 2041: 34875.66814950365, 2042: 33998.77910667844, 2043: 33121.890063853, 2044: 32245.001021027798, 2045: 31368.11197820236, 2046: 30491.222935377154, 2047: 29614.333892551716, 2048: 28737.44484972651, 2049: 27860.555806901306, 2050: 26983.666764075868}</t>
         </is>
       </c>
-      <c r="S30" t="n">
+      <c r="T30" t="n">
         <v>1151193.671085443</v>
       </c>
     </row>
@@ -2506,10 +2656,15 @@
       </c>
       <c r="R31" t="inlineStr">
         <is>
+          <t>[ 6.07171391e+01 -1.10652426e+05]</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
           <t>{2021: 11311.794475375, 2022: 12117.62980881147, 2023: 12178.346947960541, 2024: 12239.064087109626, 2025: 12299.781226258696, 2026: 12360.498365407766, 2027: 12421.21550455685, 2028: 12481.93264370592, 2029: 12542.649782855005, 2030: 12603.366922004076, 2031: 12664.08406115316, 2032: 12724.80120030223, 2033: 12785.5183394513, 2034: 12846.235478600385, 2035: 12906.952617749455, 2036: 12967.66975689854, 2037: 13028.38689604761, 2038: 13089.104035196695, 2039: 13149.821174345765, 2040: 13210.53831349485, 2041: 13271.25545264392, 2042: 13331.97259179299, 2043: 13392.689730942075, 2044: 13453.406870091145, 2045: 13514.12400924023, 2046: 13574.8411483893, 2047: 13635.558287538384, 2048: 13696.275426687454, 2049: 13756.992565836525, 2050: 13817.70970498561}</t>
         </is>
       </c>
-      <c r="S31" t="n">
+      <c r="T31" t="n">
         <v>374809.4653352522</v>
       </c>
     </row>
@@ -2573,10 +2728,15 @@
       </c>
       <c r="R32" t="inlineStr">
         <is>
+          <t>[-3.89811287e+02  8.40213862e+05]</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
           <t>{2021: 54733.137085012, 2022: 52015.440560412826, 2023: 51625.62927374488, 2024: 51235.81798707682, 2025: 50846.00670040888, 2026: 50456.19541374082, 2027: 50066.38412707287, 2028: 49676.57284040481, 2029: 49286.76155373675, 2030: 48896.95026706881, 2031: 48507.13898040075, 2032: 48117.327693732805, 2033: 47727.516407064744, 2034: 47337.7051203968, 2035: 46947.89383372874, 2036: 46558.082547060796, 2037: 46168.271260392736, 2038: 45778.45997372479, 2039: 45388.64868705673, 2040: 44998.83740038867, 2041: 44609.02611372073, 2042: 44219.21482705267, 2043: 43829.40354038472, 2044: 43439.59225371666, 2045: 43049.78096704872, 2046: 42659.96968038066, 2047: 42270.158393712714, 2048: 41880.347107044654, 2049: 41490.53582037659, 2050: 41100.72453370865}</t>
         </is>
       </c>
-      <c r="S32" t="n">
+      <c r="T32" t="n">
         <v>1357000.600140414</v>
       </c>
     </row>
@@ -2640,10 +2800,15 @@
       </c>
       <c r="R33" t="inlineStr">
         <is>
+          <t>[-1.39151452e+03  2.85227545e+06]</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
           <t>{2021: 41621.0163834535, 2022: 38633.08863250399, 2023: 37241.57411222113, 2024: 35850.059591938276, 2025: 34458.54507165542, 2026: 33067.03055137256, 2027: 31675.516031089704, 2028: 30284.001510806847, 2029: 28892.48699052399, 2030: 27500.972470240667, 2031: 26109.45794995781, 2032: 24717.943429674953, 2033: 23326.428909392096, 2034: 21934.91438910924, 2035: 20543.399868826382, 2036: 19151.885348543525, 2037: 17760.370828260668, 2038: 16368.85630797781, 2039: 14977.341787694953, 2040: 13585.827267412096, 2041: 12194.31274712924, 2042: 10802.798226845916, 2043: 9411.28370656306, 2044: 8019.769186280202, 2045: 6628.254665997345, 2046: 5236.740145714488, 2047: 3845.2256254316308, 2048: 2453.7111051487736, 2049: 1062.1965848659165, 2050: 0}</t>
         </is>
       </c>
-      <c r="S33" t="n">
+      <c r="T33" t="n">
         <v>576544.5012349054</v>
       </c>
     </row>
@@ -2707,10 +2872,15 @@
       </c>
       <c r="R34" t="inlineStr">
         <is>
+          <t>[-1.60301145e+03  3.30524483e+06]</t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
           <t>{2021: 66296.8699431275, 2022: 63955.68469541287, 2023: 62352.67324674642, 2024: 60749.66179808043, 2025: 59146.65034941444, 2026: 57543.638900748454, 2027: 55940.627452082, 2028: 54337.61600341601, 2029: 52734.604554750025, 2030: 51131.59310608357, 2031: 49528.581657417584, 2032: 47925.5702087516, 2033: 46322.55876008514, 2034: 44719.547311419155, 2035: 43116.53586275317, 2036: 41513.52441408718, 2037: 39910.51296542073, 2038: 38307.50151675474, 2039: 36704.49006808875, 2040: 35101.4786194223, 2041: 33498.46717075631, 2042: 31895.455722090323, 2043: 30292.44427342387, 2044: 28689.43282475788, 2045: 27086.421376091894, 2046: 25483.409927425906, 2047: 23880.398478759453, 2048: 22277.387030093465, 2049: 20674.375581427477, 2050: 19071.364132761024}</t>
         </is>
       </c>
-      <c r="S34" t="n">
+      <c r="T34" t="n">
         <v>1227504.960913705</v>
       </c>
     </row>
@@ -2774,10 +2944,15 @@
       </c>
       <c r="R35" t="inlineStr">
         <is>
+          <t>[-9.47361738e+02  1.93935861e+06]</t>
+        </is>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
           <t>{2021: 24807.5654940032, 2022: 23793.173673806945, 2023: 22845.8119354886, 2024: 21898.450197170256, 2025: 20951.08845885168, 2026: 20003.726720533334, 2027: 19056.36498221499, 2028: 18109.00324389641, 2029: 17161.641505578067, 2030: 16214.27976725949, 2031: 15266.918028941145, 2032: 14319.5562906228, 2033: 13372.194552304223, 2034: 12424.832813985879, 2035: 11477.471075667534, 2036: 10530.109337348957, 2037: 9582.747599030612, 2038: 8635.385860712267, 2039: 7688.02412239369, 2040: 6740.6623840753455, 2041: 5793.300645757001, 2042: 4845.9389074384235, 2043: 3898.577169120079, 2044: 2951.2154308015015, 2045: 2003.853692483157, 2046: 1056.4919541648123, 2047: 109.13021584623493, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S35" t="n">
+      <c r="T35" t="n">
         <v>323133.7333124951</v>
       </c>
     </row>
@@ -2841,10 +3016,15 @@
       </c>
       <c r="R36" t="inlineStr">
         <is>
+          <t>[-4.79172995e+03  9.83448133e+06]</t>
+        </is>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
           <t>{2021: 148655.679597746, 2022: 145603.3699548114, 2023: 140811.64000288025, 2024: 136019.91005094722, 2025: 131228.18009901606, 2026: 126436.45014708303, 2027: 121644.72019515187, 2028: 116852.9902432207, 2029: 112061.26029128768, 2030: 107269.53033935651, 2031: 102477.80038742349, 2032: 97686.07043549232, 2033: 92894.3404835593, 2034: 88102.61053162813, 2035: 83310.88057969697, 2036: 78519.15062776394, 2037: 73727.42067583278, 2038: 68935.69072389975, 2039: 64143.96077196859, 2040: 59352.23082003556, 2041: 54560.5008681044, 2042: 49768.770916173235, 2043: 44977.04096424021, 2044: 40185.311012309045, 2045: 35393.58106037602, 2046: 30601.851108444855, 2047: 25810.12115651183, 2048: 21018.391204580665, 2049: 16226.661252649501, 2050: 11434.931300716475}</t>
         </is>
       </c>
-      <c r="S36" t="n">
+      <c r="T36" t="n">
         <v>2345665.742353677</v>
       </c>
     </row>
@@ -2908,10 +3088,15 @@
       </c>
       <c r="R37" t="inlineStr">
         <is>
+          <t>[-5.36851692e+03  1.10125420e+07]</t>
+        </is>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
           <t>{2021: 164615.166399523, 2022: 157400.80845420994, 2023: 152032.29153708182, 2024: 146663.77461995557, 2025: 141295.25770282745, 2026: 135926.74078569934, 2027: 130558.22386857122, 2028: 125189.7069514431, 2029: 119821.19003431499, 2030: 114452.67311718687, 2031: 109084.15620005876, 2032: 103715.63928293064, 2033: 98347.12236580253, 2034: 92978.60544867627, 2035: 87610.08853154816, 2036: 82241.57161442004, 2037: 76873.05469729193, 2038: 71504.53778016381, 2039: 66136.0208630357, 2040: 60767.50394590758, 2041: 55398.98702877946, 2042: 50030.470111651346, 2043: 44661.95319452323, 2044: 39293.43627739698, 2045: 33924.91936026886, 2046: 28556.402443140745, 2047: 23187.88552601263, 2048: 17819.368608884513, 2049: 12450.851691756397, 2050: 7082.334774628282}</t>
         </is>
       </c>
-      <c r="S37" t="n">
+      <c r="T37" t="n">
         <v>2463771.992630616</v>
       </c>
     </row>
@@ -2975,10 +3160,15 @@
       </c>
       <c r="R38" t="inlineStr">
         <is>
+          <t>[ 6.14411976e+02 -1.04742191e+06]</t>
+        </is>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
           <t>{2021: 206371.803466873, 2022: 194919.10329792276, 2023: 195533.51527403155, 2024: 196147.92725014058, 2025: 196762.3392262496, 2026: 197376.75120235863, 2027: 197991.16317846766, 2028: 198605.57515457645, 2029: 199219.98713068548, 2030: 199834.3991067945, 2031: 200448.81108290353, 2032: 201063.22305901255, 2033: 201677.63503512158, 2034: 202292.04701123037, 2035: 202906.4589873394, 2036: 203520.87096344843, 2037: 204135.28293955745, 2038: 204749.69491566648, 2039: 205364.1068917755, 2040: 205978.5188678843, 2041: 206592.93084399332, 2042: 207207.34282010235, 2043: 207821.75479621137, 2044: 208436.1667723204, 2045: 209050.57874842943, 2046: 209664.99072453822, 2047: 210279.40270064725, 2048: 210893.81467675627, 2049: 211508.2266528653, 2050: 212122.63862897432}</t>
         </is>
       </c>
-      <c r="S38" t="n">
+      <c r="T38" t="n">
         <v>5899229.840358955</v>
       </c>
     </row>
@@ -3042,10 +3232,15 @@
       </c>
       <c r="R39" t="inlineStr">
         <is>
+          <t>[-8.20391364e+02  1.67300407e+06]</t>
+        </is>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
           <t>{2021: 14794.4064289437, 2022: 14172.733631623443, 2023: 13352.342267934931, 2024: 12531.95090424642, 2025: 11711.559540557675, 2026: 10891.168176869163, 2027: 10070.776813180419, 2028: 9250.385449491907, 2029: 8429.994085803395, 2030: 7609.6027221146505, 2031: 6789.211358426139, 2032: 5968.819994737394, 2033: 5148.428631048882, 2034: 4328.037267360371, 2035: 3507.645903671626, 2036: 2687.2545399831142, 2037: 1866.8631762943696, 2038: 1046.4718126058578, 2039: 226.08044891734608, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S39" t="n">
+      <c r="T39" t="n">
         <v>136986.529939339</v>
       </c>
     </row>
@@ -3109,10 +3304,15 @@
       </c>
       <c r="R40" t="inlineStr">
         <is>
+          <t>[-2.20914867e+03  4.49497764e+06]</t>
+        </is>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
           <t>{2021: 31616.9086770801, 2022: 28079.02995773405, 2023: 25869.88128668256, 2024: 23660.732615631074, 2025: 21451.583944579586, 2026: 19242.4352735281, 2027: 17033.28660247568, 2028: 14824.137931424193, 2029: 12614.989260372706, 2030: 10405.840589321218, 2031: 8196.691918269731, 2032: 5987.543247218244, 2033: 3778.394576165825, 2034: 1569.2459051143378, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S40" t="n">
+      <c r="T40" t="n">
         <v>208522.2474470573</v>
       </c>
     </row>
@@ -3176,10 +3376,15 @@
       </c>
       <c r="R41" t="inlineStr">
         <is>
+          <t>[-2.58100361e+03  5.36723256e+06]</t>
+        </is>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
           <t>{2021: 151025.992624885, 2022: 148443.25598497968, 2023: 145862.25237088464, 2024: 143281.2487567896, 2025: 140700.24514269456, 2026: 138119.24152859952, 2027: 135538.23791450355, 2028: 132957.2343004085, 2029: 130376.23068631347, 2030: 127795.22707221843, 2031: 125214.2234581234, 2032: 122633.21984402742, 2033: 120052.21622993238, 2034: 117471.21261583734, 2035: 114890.2090017423, 2036: 112309.20538764726, 2037: 109728.20177355129, 2038: 107147.19815945625, 2039: 104566.19454536121, 2040: 101985.19093126617, 2041: 99404.1873171702, 2042: 96823.18370307516, 2043: 94242.18008898012, 2044: 91661.17647488508, 2045: 89080.17286079004, 2046: 86499.16924669407, 2047: 83918.16563259903, 2048: 81337.162018504, 2049: 78756.15840440895, 2050: 76175.15479031391}</t>
         </is>
       </c>
-      <c r="S41" t="n">
+      <c r="T41" t="n">
         <v>3294392.375159043</v>
       </c>
     </row>
@@ -3243,10 +3448,15 @@
       </c>
       <c r="R42" t="inlineStr">
         <is>
+          <t>[-2.79000291e+03  5.71704173e+06]</t>
+        </is>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
           <t>{2021: 78304.915550821, 2022: 75655.85794758704, 2023: 72865.85504138656, 2024: 70075.85213518515, 2025: 67285.84922898468, 2026: 64495.8463227842, 2027: 61705.84341658279, 2028: 58915.84051038232, 2029: 56125.83760418184, 2030: 53335.834697980434, 2031: 50545.83179177996, 2032: 47755.82888557948, 2033: 44965.825979378074, 2034: 42175.8230731776, 2035: 39385.82016697712, 2036: 36595.817260775715, 2037: 33805.81435457524, 2038: 31015.811448374763, 2039: 28225.808542173356, 2040: 25435.80563597288, 2041: 22645.802729771473, 2042: 19855.799823570997, 2043: 17065.79691737052, 2044: 14275.794011169113, 2045: 11485.791104968637, 2046: 8695.788198768161, 2047: 5905.785292566754, 2048: 3115.782386366278, 2049: 325.77948016580194, 2050: 0}</t>
         </is>
       </c>
-      <c r="S42" t="n">
+      <c r="T42" t="n">
         <v>1102895.381763947</v>
       </c>
     </row>
@@ -3310,10 +3520,15 @@
       </c>
       <c r="R43" t="inlineStr">
         <is>
+          <t>[-6.08157191e+03  1.23802466e+07]</t>
+        </is>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
           <t>{2021: 94224.9197475128, 2022: 83308.24585822597, 2023: 77226.67395072244, 2024: 71145.10204321891, 2025: 65063.53013571352, 2026: 58981.95822820999, 2027: 52900.38632070646, 2028: 46818.81441320293, 2029: 40737.242505699396, 2030: 34655.670598195866, 2031: 28574.098690692335, 2032: 22492.526783188805, 2033: 16410.954875685275, 2034: 10329.382968181744, 2035: 4247.811060678214, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S43" t="n">
+      <c r="T43" t="n">
         <v>660004.8583060782</v>
       </c>
     </row>
@@ -3377,10 +3592,15 @@
       </c>
       <c r="R44" t="inlineStr">
         <is>
+          <t>[-1.24178045e+03  2.54931633e+06]</t>
+        </is>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
           <t>{2021: 39073.6294879557, 2022: 38436.26228732243, 2023: 37194.481840590015, 2024: 35952.701393858064, 2025: 34710.92094712611, 2026: 33469.14050039416, 2027: 32227.36005366221, 2028: 30985.579606929794, 2029: 29743.799160197843, 2030: 28502.01871346589, 2031: 27260.23826673394, 2032: 26018.457820001524, 2033: 24776.677373269573, 2034: 23534.89692653762, 2035: 22293.11647980567, 2036: 21051.33603307372, 2037: 19809.555586341303, 2038: 18567.77513960935, 2039: 17325.9946928774, 2040: 16084.21424614545, 2041: 14842.433799413498, 2042: 13600.653352681082, 2043: 12358.87290594913, 2044: 11117.09245921718, 2045: 9875.312012485228, 2046: 8633.531565752812, 2047: 7391.751119020861, 2048: 6149.97067228891, 2049: 4908.1902255569585, 2050: 3666.4097788250074}</t>
         </is>
       </c>
-      <c r="S44" t="n">
+      <c r="T44" t="n">
         <v>628192.3548136981</v>
       </c>
     </row>
@@ -3444,10 +3664,15 @@
       </c>
       <c r="R45" t="inlineStr">
         <is>
+          <t>[-1.73095109e+03  3.57136333e+06]</t>
+        </is>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
           <t>{2021: 73237.1079251592, 2022: 71380.21577896085, 2023: 69649.26468487224, 2024: 67918.31359078363, 2025: 66187.36249669502, 2026: 64456.411402606405, 2027: 62725.460308517795, 2028: 60994.509214429185, 2029: 59263.558120340575, 2030: 57532.607026251964, 2031: 55801.655932163354, 2032: 54070.704838074744, 2033: 52339.75374398613, 2034: 50608.80264989752, 2035: 48877.85155580891, 2036: 47146.90046172077, 2037: 45415.94936763216, 2038: 43684.99827354355, 2039: 41954.04717945494, 2040: 40223.09608536633, 2041: 38492.14499127772, 2042: 36761.19389718911, 2043: 35030.2428031005, 2044: 33299.291709011886, 2045: 31568.340614923276, 2046: 29837.389520834666, 2047: 28106.438426746055, 2048: 26375.487332657445, 2049: 24644.536238568835, 2050: 22913.585144480225}</t>
         </is>
       </c>
-      <c r="S45" t="n">
+      <c r="T45" t="n">
         <v>1392421.874780235</v>
       </c>
     </row>
@@ -3511,10 +3736,15 @@
       </c>
       <c r="R46" t="inlineStr">
         <is>
+          <t>[-1.98098082e+03  4.04260569e+06]</t>
+        </is>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
           <t>{2021: 40493.1623118517, 2022: 37062.474532493856, 2023: 35081.49371446064, 2024: 33100.51289642742, 2025: 31119.5320783942, 2026: 29138.551260360982, 2027: 27157.570442327764, 2028: 25176.589624294546, 2029: 23195.608806261327, 2030: 21214.627988227643, 2031: 19233.647170194425, 2032: 17252.666352161206, 2033: 15271.685534127988, 2034: 13290.70471609477, 2035: 11309.723898061551, 2036: 9328.743080028333, 2037: 7347.762261994649, 2038: 5366.78144396143, 2039: 3385.800625928212, 2040: 1404.8198078949936, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S46" t="n">
+      <c r="T46" t="n">
         <v>385685.8773896218</v>
       </c>
     </row>
@@ -3578,10 +3808,15 @@
       </c>
       <c r="R47" t="inlineStr">
         <is>
+          <t>[-7.16338995e+02  1.46589703e+06]</t>
+        </is>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
           <t>{2021: 18740.6365816607, 2022: 17459.580516267102, 2023: 16743.24152156408, 2024: 16026.902526861057, 2025: 15310.563532158034, 2026: 14594.224537455011, 2027: 13877.885542751988, 2028: 13161.546548048966, 2029: 12445.207553345943, 2030: 11728.86855864292, 2031: 11012.529563939897, 2032: 10296.190569236875, 2033: 9579.851574533852, 2034: 8863.512579830829, 2035: 8147.173585127806, 2036: 7430.8345904247835, 2037: 6714.495595721761, 2038: 5998.156601018738, 2039: 5281.817606315715, 2040: 4565.4786116126925, 2041: 3849.1396169096697, 2042: 3132.800622206647, 2043: 2416.461627503624, 2044: 1700.1226328006014, 2045: 983.7836380975787, 2046: 267.4446433945559, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S47" t="n">
+      <c r="T47" t="n">
         <v>230958.1327866011</v>
       </c>
     </row>
@@ -3645,10 +3880,15 @@
       </c>
       <c r="R48" t="inlineStr">
         <is>
+          <t>[-1.81084818e+02  3.87404771e+05]</t>
+        </is>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
           <t>{2021: 20970.6401639379, 2022: 21251.269496103225, 2023: 21070.1846784777, 2024: 20889.099860852235, 2025: 20708.01504322671, 2026: 20526.930225601245, 2027: 20345.84540797572, 2028: 20164.760590350255, 2029: 19983.67577272473, 2030: 19802.590955099266, 2031: 19621.50613747374, 2032: 19440.421319848276, 2033: 19259.33650222275, 2034: 19078.251684597286, 2035: 18897.166866971762, 2036: 18716.082049346296, 2037: 18534.997231720772, 2038: 18353.912414095306, 2039: 18172.827596469782, 2040: 17991.742778844316, 2041: 17810.657961218792, 2042: 17629.573143593327, 2043: 17448.488325967803, 2044: 17267.403508342337, 2045: 17086.318690716813, 2046: 16905.233873091347, 2047: 16724.149055465823, 2048: 16543.064237840357, 2049: 16361.979420214891, 2050: 16180.894602589367}</t>
         </is>
       </c>
-      <c r="S48" t="n">
+      <c r="T48" t="n">
         <v>545161.2522117165</v>
       </c>
     </row>
@@ -3712,10 +3952,15 @@
       </c>
       <c r="R49" t="inlineStr">
         <is>
+          <t>[-1.34320390e+03  2.73759994e+06]</t>
+        </is>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
           <t>{2021: 23598.9801315176, 2022: 21641.651221164968, 2023: 20298.447318035644, 2024: 18955.243414906785, 2025: 17612.039511777926, 2026: 16268.835608648602, 2027: 14925.631705519743, 2028: 13582.427802390885, 2029: 12239.22389926156, 2030: 10896.019996132702, 2031: 9552.816093003843, 2032: 8209.612189874984, 2033: 6866.40828674566, 2034: 5523.204383616801, 2035: 4180.000480487943, 2036: 2836.7965773586184, 2037: 1493.5926742297597, 2038: 150.38877110090107, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S49" t="n">
+      <c r="T49" t="n">
         <v>197031.8300000161</v>
       </c>
     </row>
@@ -3779,10 +4024,15 @@
       </c>
       <c r="R50" t="inlineStr">
         <is>
+          <t>[-2.99933730e+03  6.12684672e+06]</t>
+        </is>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
           <t>{2021: 66254.0238426647, 2022: 62186.69878190849, 2023: 59187.361482637934, 2024: 56188.02418336831, 2025: 53188.686884097755, 2026: 50189.34958482813, 2027: 47190.01228555851, 2028: 44190.67498628795, 2029: 41191.33768701833, 2030: 38192.0003877487, 2031: 35192.66308847815, 2032: 32193.325789208524, 2033: 29193.9884899389, 2034: 26194.651190668344, 2035: 23195.31389139872, 2036: 20195.976592128165, 2037: 17196.63929285854, 2038: 14197.301993588917, 2039: 11197.964694318362, 2040: 8198.627395048738, 2041: 5199.2900957791135, 2042: 2199.952796508558, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S50" t="n">
+      <c r="T50" t="n">
         <v>709186.8534947095</v>
       </c>
     </row>
@@ -3846,10 +4096,15 @@
       </c>
       <c r="R51" t="inlineStr">
         <is>
+          <t>[-1.60647131e+03  3.26309933e+06]</t>
+        </is>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
           <t>{2021: 17725.0476255144, 2022: 14814.346514039673, 2023: 13207.875206804369, 2024: 11601.403899569064, 2025: 9994.93259233376, 2026: 8388.46128509799, 2027: 6781.989977862686, 2028: 5175.518670627382, 2029: 3569.0473633920774, 2030: 1962.5760561563075, 2031: 356.1047489210032, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S51" t="n">
+      <c r="T51" t="n">
         <v>84714.78012756151</v>
       </c>
     </row>
@@ -3913,10 +4168,15 @@
       </c>
       <c r="R52" t="inlineStr">
         <is>
+          <t>[-1.51761783e+03  3.09036385e+06]</t>
+        </is>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
           <t>{2021: 21233.9116098986, 2022: 21740.60284140939, 2023: 20222.985016007908, 2024: 18705.367190606426, 2025: 17187.74936520448, 2026: 15670.131539802998, 2027: 14152.513714401517, 2028: 12634.895889000036, 2029: 11117.278063598089, 2030: 9599.660238196608, 2031: 8082.042412795126, 2032: 6564.4245873931795, 2033: 5046.806761991698, 2034: 3529.188936590217, 2035: 2011.5711111887358, 2036: 493.9532857867889, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S52" t="n">
+      <c r="T52" t="n">
         <v>177376.1267589225</v>
       </c>
     </row>
@@ -3980,10 +4240,15 @@
       </c>
       <c r="R53" t="inlineStr">
         <is>
+          <t>[-1.20273679e+04  2.45434225e+07]</t>
+        </is>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
           <t>{2021: 119802.94296870008, 2022: 224084.6072674282, 2023: 212057.23936547711, 2024: 200029.87146352604, 2025: 188002.50356157497, 2026: 175975.13565962762, 2027: 163947.76775767654, 2028: 151920.39985572547, 2029: 139893.0319537744, 2030: 127865.66405182332, 2031: 115838.29614987224, 2032: 103810.92824792117, 2033: 91783.5603459701, 2034: 79756.19244401902, 2035: 67728.82454206795, 2036: 55701.45664011687, 2037: 43674.088738165796, 2038: 31646.72083621472, 2039: 19619.352934263647, 2040: 7591.985032312572, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S53" t="n">
+      <c r="T53" t="n">
         <v>2260829.098331908</v>
       </c>
     </row>
@@ -4047,10 +4312,15 @@
       </c>
       <c r="R54" t="inlineStr">
         <is>
+          <t>[ 3.14647428e+02 -5.77344835e+05]</t>
+        </is>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
           <t>{2021: 52270.3371590495, 2022: 58872.26422920241, 2023: 59186.91165715468, 2024: 59501.55908510694, 2025: 59816.20651305921, 2026: 60130.853941011475, 2027: 60445.50136896374, 2028: 60760.148796916124, 2029: 61074.79622486839, 2030: 61389.44365282066, 2031: 61704.09108077292, 2032: 62018.73850872519, 2033: 62333.385936677456, 2034: 62648.03336462972, 2035: 62962.68079258199, 2036: 63277.328220534255, 2037: 63591.97564848652, 2038: 63906.62307643879, 2039: 64221.270504391054, 2040: 64535.91793234332, 2041: 64850.565360295586, 2042: 65165.21278824797, 2043: 65479.860216200235, 2044: 65794.5076441525, 2045: 66109.15507210477, 2046: 66423.80250005703, 2047: 66738.4499280093, 2048: 67053.09735596157, 2049: 67367.74478391383, 2050: 67682.3922118661}</t>
         </is>
       </c>
-      <c r="S54" t="n">
+      <c r="T54" t="n">
         <v>1827336.490869086</v>
       </c>
     </row>
@@ -4114,10 +4384,15 @@
       </c>
       <c r="R55" t="inlineStr">
         <is>
+          <t>[-6.09353877e+02  1.25362411e+06]</t>
+        </is>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
           <t>{2021: 22395.1016488455, 2022: 21510.56886509573, 2023: 20901.21498796367, 2024: 20291.86111083161, 2025: 19682.50723369955, 2026: 19073.15335656749, 2027: 18463.79947943543, 2028: 17854.44560230337, 2029: 17245.09172517131, 2030: 16635.73784803925, 2031: 16026.38397090719, 2032: 15417.03009377513, 2033: 14807.67621664307, 2034: 14198.32233951101, 2035: 13588.968462379184, 2036: 12979.614585247124, 2037: 12370.260708115064, 2038: 11760.906830983004, 2039: 11151.552953850944, 2040: 10542.199076718884, 2041: 9932.845199586824, 2042: 9323.491322454764, 2043: 8714.137445322704, 2044: 8104.783568190644, 2045: 7495.429691058584, 2046: 6886.075813926524, 2047: 6276.7219367944635, 2048: 5667.3680596624035, 2049: 5058.0141825303435, 2050: 4448.6603053982835}</t>
         </is>
       </c>
-      <c r="S55" t="n">
+      <c r="T55" t="n">
         <v>385382.0436438872</v>
       </c>
     </row>
@@ -4181,10 +4456,15 @@
       </c>
       <c r="R56" t="inlineStr">
         <is>
+          <t>[-8.14941738e+02  1.66927470e+06]</t>
+        </is>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
           <t>{2021: 22545.4803600213, 2022: 21462.501178817358, 2023: 20647.559440587414, 2024: 19832.61770235747, 2025: 19017.675964127295, 2026: 18202.73422589735, 2027: 17387.792487667408, 2028: 16572.85074943723, 2029: 15757.909011207288, 2030: 14942.967272977345, 2031: 14128.025534747401, 2032: 13313.083796517225, 2033: 12498.142058287282, 2034: 11683.200320057338, 2035: 10868.258581827395, 2036: 10053.316843597218, 2037: 9238.375105367275, 2038: 8423.433367137332, 2039: 7608.491628907155, 2040: 6793.549890677212, 2041: 5978.608152447268, 2042: 5163.666414217325, 2043: 4348.724675987149, 2044: 3533.782937757205, 2045: 2718.841199527262, 2046: 1903.8994612973183, 2047: 1088.957723067142, 2048: 274.01598483719863, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S56" t="n">
+      <c r="T56" t="n">
         <v>304715.7218893475</v>
       </c>
     </row>
@@ -4248,10 +4528,15 @@
       </c>
       <c r="R57" t="inlineStr">
         <is>
+          <t>[ 8.01959775e+03 -1.57866255e+07]</t>
+        </is>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
           <t>{2021: 379312.20194903, 2022: 429001.1505482327, 2023: 437020.7483017165, 2024: 445040.3460552003, 2025: 453059.943808686, 2026: 461079.5415621698, 2027: 469099.1393156536, 2028: 477118.7370691374, 2029: 485138.3348226212, 2030: 493157.93257610686, 2031: 501177.53032959066, 2032: 509197.12808307447, 2033: 517216.72583655827, 2034: 525236.3235900421, 2035: 533255.9213435277, 2036: 541275.5190970115, 2037: 549295.1168504953, 2038: 557314.7146039791, 2039: 565334.312357463, 2040: 573353.9101109467, 2041: 581373.5078644324, 2042: 589393.1056179162, 2043: 597412.7033714, 2044: 605432.3011248838, 2045: 613451.8988783676, 2046: 621471.4966318533, 2047: 629491.0943853371, 2048: 637510.6921388209, 2049: 645530.2898923047, 2050: 653549.8876457885}</t>
         </is>
       </c>
-      <c r="S57" t="n">
+      <c r="T57" t="n">
         <v>15559871.21096494</v>
       </c>
     </row>
@@ -4315,10 +4600,15 @@
       </c>
       <c r="R58" t="inlineStr">
         <is>
+          <t>[-9.40268875e+03  1.92262890e+07]</t>
+        </is>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
           <t>{2021: 235613.396453782, 2022: 214052.3302645944, 2023: 204649.64151547477, 2024: 195246.95276635513, 2025: 185844.2640172355, 2026: 176441.57526811212, 2027: 167038.88651899248, 2028: 157636.19776987284, 2029: 148233.5090207532, 2030: 138830.82027162984, 2031: 129428.1315225102, 2032: 120025.44277339056, 2033: 110622.75402427092, 2034: 101220.06527514756, 2035: 91817.37652602792, 2036: 82414.68777690828, 2037: 73011.99902778864, 2038: 63609.310278665274, 2039: 54206.621529545635, 2040: 44803.932780425996, 2041: 35401.244031306356, 2042: 25998.55528218299, 2043: 16595.866533063352, 2044: 7193.177783943713, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S58" t="n">
+      <c r="T58" t="n">
         <v>2662130.040785089</v>
       </c>
     </row>
@@ -4382,10 +4672,15 @@
       </c>
       <c r="R59" t="inlineStr">
         <is>
+          <t>[-4.08976507e+04  8.47261316e+07]</t>
+        </is>
+      </c>
+      <c r="S59" t="inlineStr">
+        <is>
           <t>{2021: 2043704.69976698, 2022: 2031081.8973403573, 2023: 1990184.2466693372, 2024: 1949286.595998302, 2025: 1908388.945327267, 2026: 1867491.294656232, 2027: 1826593.643985197, 2028: 1785695.993314162, 2029: 1744798.3426431417, 2030: 1703900.6919721067, 2031: 1663003.0413010716, 2032: 1622105.3906300366, 2033: 1581207.7399590015, 2034: 1540310.0892879814, 2035: 1499412.4386169463, 2036: 1458514.7879459113, 2037: 1417617.1372748762, 2038: 1376719.4866038412, 2039: 1335821.8359328061, 2040: 1294924.185261786, 2041: 1254026.534590751, 2042: 1213128.8839197159, 2043: 1172231.2332486808, 2044: 1131333.5825776458, 2045: 1090435.9319066107, 2046: 1049538.2812355906, 2047: 1008640.6305645555, 2048: 967742.9798935205, 2049: 926845.3292224854, 2050: 885947.6785514504}</t>
         </is>
       </c>
-      <c r="S59" t="n">
+      <c r="T59" t="n">
         <v>42875807.36103913</v>
       </c>
     </row>
@@ -4449,10 +4744,15 @@
       </c>
       <c r="R60" t="inlineStr">
         <is>
+          <t>[-6.39574640e+02  1.39791755e+06]</t>
+        </is>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
           <t>{2021: 101111.400908884, 2022: 104697.62903068285, 2023: 104058.05439084605, 2024: 103418.47975100903, 2025: 102778.90511117224, 2026: 102139.33047133544, 2027: 101499.75583149865, 2028: 100860.18119166186, 2029: 100220.60655182484, 2030: 99581.03191198804, 2031: 98941.45727215125, 2032: 98301.88263231446, 2033: 97662.30799247767, 2034: 97022.73335264088, 2035: 96383.15871280385, 2036: 95743.58407296706, 2037: 95104.00943313027, 2038: 94464.43479329348, 2039: 93824.86015345668, 2040: 93185.28551361966, 2041: 92545.71087378287, 2042: 91906.13623394608, 2043: 91266.56159410928, 2044: 90626.98695427249, 2045: 89987.4123144357, 2046: 89347.83767459868, 2047: 88708.26303476188, 2048: 88068.68839492509, 2049: 87429.1137550883, 2050: 86789.53911525151}</t>
         </is>
       </c>
-      <c r="S60" t="n">
+      <c r="T60" t="n">
         <v>2783724.869012862</v>
       </c>
     </row>
@@ -4516,10 +4816,15 @@
       </c>
       <c r="R61" t="inlineStr">
         <is>
+          <t>[-2.05457259e+02  4.49386827e+05]</t>
+        </is>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
           <t>{2021: 33448.1706049408, 2022: 33952.249976868276, 2023: 33746.792717992095, 2024: 33541.335459115915, 2025: 33335.87820023979, 2026: 33130.42094136361, 2027: 32924.96368248743, 2028: 32719.506423611252, 2029: 32514.049164735072, 2030: 32308.59190585895, 2031: 32103.13464698277, 2032: 31897.67738810659, 2033: 31692.22012923041, 2034: 31486.76287035423, 2035: 31281.30561147805, 2036: 31075.848352601926, 2037: 30870.391093725746, 2038: 30664.933834849566, 2039: 30459.476575973385, 2040: 30254.019317097205, 2041: 30048.562058221083, 2042: 29843.104799344903, 2043: 29637.647540468723, 2044: 29432.190281592542, 2045: 29226.733022716362, 2046: 29021.27576384024, 2047: 28815.81850496406, 2048: 28610.36124608788, 2049: 28404.9039872117, 2050: 28199.44672833552}</t>
         </is>
       </c>
-      <c r="S61" t="n">
+      <c r="T61" t="n">
         <v>903823.9641637581</v>
       </c>
     </row>
@@ -4583,10 +4888,15 @@
       </c>
       <c r="R62" t="inlineStr">
         <is>
+          <t>[-1.47356144e+03  3.05169292e+06]</t>
+        </is>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
           <t>{2021: 79688.3208022694, 2022: 72151.6844737134, 2023: 70678.12303419923, 2024: 69204.56159468507, 2025: 67731.00015517091, 2026: 66257.43871565675, 2027: 64783.87727614213, 2028: 63310.31583662797, 2029: 61836.75439711381, 2030: 60363.19295759965, 2031: 58889.63151808549, 2032: 57416.07007857133, 2033: 55942.50863905717, 2034: 54468.94719954301, 2035: 52995.38576002885, 2036: 51521.82432051469, 2037: 50048.262881000526, 2038: 48574.701441486366, 2039: 47101.140001972206, 2040: 45627.578562458046, 2041: 44154.017122943886, 2042: 42680.455683429725, 2043: 41206.894243915565, 2044: 39733.332804401405, 2045: 38259.771364887245, 2046: 36786.209925373085, 2047: 35312.648485858925, 2048: 33839.087046344765, 2049: 32365.525606830604, 2050: 30891.964167316444}</t>
         </is>
       </c>
-      <c r="S62" t="n">
+      <c r="T62" t="n">
         <v>1518531.083612405</v>
       </c>
     </row>
@@ -4650,10 +4960,15 @@
       </c>
       <c r="R63" t="inlineStr">
         <is>
+          <t>[-1.93893657e+03  3.96249491e+06]</t>
+        </is>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
           <t>{2021: 45571.0255636995, 2022: 41965.16419702163, 2023: 40026.22762812255, 2024: 38087.29105922347, 2025: 36148.35449032439, 2026: 34209.41792142531, 2027: 32270.48135252623, 2028: 30331.54478362715, 2029: 28392.60821472807, 2030: 26453.67164582899, 2031: 24514.73507692991, 2032: 22575.798508030828, 2033: 20636.861939131748, 2034: 18697.925370232668, 2035: 16758.988801333588, 2036: 14820.052232434507, 2037: 12881.115663535427, 2038: 10942.179094635881, 2039: 9003.242525736801, 2040: 7064.305956837721, 2041: 5125.369387938641, 2042: 3186.432819039561, 2043: 1247.4962501404807, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S63" t="n">
+      <c r="T63" t="n">
         <v>498124.7777006353</v>
       </c>
     </row>
@@ -4717,10 +5032,15 @@
       </c>
       <c r="R64" t="inlineStr">
         <is>
+          <t>[-4.18611550e+02  8.81869147e+05]</t>
+        </is>
+      </c>
+      <c r="S64" t="inlineStr">
+        <is>
           <t>{2021: 35566.2660676553, 2022: 35436.592202680185, 2023: 35017.980652291095, 2024: 34599.369101902004, 2025: 34180.757551512914, 2026: 33762.14600112382, 2027: 33343.53445073473, 2028: 32924.92290034576, 2029: 32506.311349956668, 2030: 32087.699799567577, 2031: 31669.088249178487, 2032: 31250.476698789396, 2033: 30831.865148400306, 2034: 30413.253598011215, 2035: 29994.642047622125, 2036: 29576.030497233034, 2037: 29157.418946843944, 2038: 28738.807396454853, 2039: 28320.195846065762, 2040: 27901.584295676672, 2041: 27482.97274528758, 2042: 27064.361194898607, 2043: 26645.749644509517, 2044: 26227.138094120426, 2045: 25808.526543731336, 2046: 25389.914993342245, 2047: 24971.303442953154, 2048: 24552.691892564064, 2049: 24134.080342174973, 2050: 23715.468791785883}</t>
         </is>
       </c>
-      <c r="S64" t="n">
+      <c r="T64" t="n">
         <v>863630.283057693</v>
       </c>
     </row>
@@ -4784,10 +5104,15 @@
       </c>
       <c r="R65" t="inlineStr">
         <is>
+          <t>[-8.49830159e+03  1.74883889e+07]</t>
+        </is>
+      </c>
+      <c r="S65" t="inlineStr">
+        <is>
           <t>{2021: 323846.285250688, 2022: 304823.0623716749, 2023: 296324.7607831955, 2024: 287826.45919471607, 2025: 279328.1576062329, 2026: 270829.8560177535, 2027: 262331.55442927405, 2028: 253833.2528407909, 2029: 245334.95125231147, 2030: 236836.64966383204, 2031: 228338.34807534888, 2032: 219840.04648686945, 2033: 211341.74489839002, 2034: 202843.44330990687, 2035: 194345.14172142744, 2036: 185846.840132948, 2037: 177348.53854446858, 2038: 168850.23695598543, 2039: 160351.935367506, 2040: 151853.63377902657, 2041: 143355.3321905434, 2042: 134857.03060206398, 2043: 126358.72901358455, 2044: 117860.4274251014, 2045: 109362.12583662197, 2046: 100863.82424814254, 2047: 92365.52265965939, 2048: 83867.22107117996, 2049: 75368.91948270053, 2050: 66870.61789421737}</t>
         </is>
       </c>
-      <c r="S65" t="n">
+      <c r="T65" t="n">
         <v>5518046.197533709</v>
       </c>
     </row>
@@ -4851,10 +5176,15 @@
       </c>
       <c r="R66" t="inlineStr">
         <is>
+          <t>[-2.25814119e+03  4.62447717e+06]</t>
+        </is>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
           <t>{2021: 60909.6622028492, 2022: 58515.67462476529, 2023: 56257.53343027085, 2024: 53999.39223577641, 2025: 51741.25104128197, 2026: 49483.10984678753, 2027: 47224.968652293086, 2028: 44966.82745779771, 2029: 42708.68626330327, 2030: 40450.54506880883, 2031: 38192.40387431439, 2032: 35934.26267981995, 2033: 33676.12148532551, 2034: 31417.980290831067, 2035: 29159.839096336626, 2036: 26901.697901841253, 2037: 24643.556707346812, 2038: 22385.41551285237, 2039: 20127.27431835793, 2040: 17869.13312386349, 2041: 15610.991929369047, 2042: 13352.850734874606, 2043: 11094.709540380165, 2044: 8836.568345884793, 2045: 6578.427151390351, 2046: 4320.28595689591, 2047: 2062.144762401469, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S66" t="n">
+      <c r="T66" t="n">
         <v>817966.4831345952</v>
       </c>
     </row>
@@ -4918,10 +5248,15 @@
       </c>
       <c r="R67" t="inlineStr">
         <is>
+          <t>[-5.17541851e+03  1.05663638e+07]</t>
+        </is>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
           <t>{2021: 107898.699030336, 2022: 101667.53271860257, 2023: 96492.11420881748, 2024: 91316.6956990324, 2025: 86141.27718924917, 2026: 80965.85867946409, 2027: 75790.44016968086, 2028: 70615.02165989578, 2029: 65439.603150112554, 2030: 60264.18464032747, 2031: 55088.766130544245, 2032: 49913.34762075916, 2033: 44737.92911097407, 2034: 39562.51060119085, 2035: 34387.092091405764, 2036: 29211.67358162254, 2037: 24036.255071837455, 2038: 18860.83656205423, 2039: 13685.418052269146, 2040: 8509.99954248406, 2041: 3334.5810327008367, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S67" t="n">
+      <c r="T67" t="n">
         <v>1103970.487028193</v>
       </c>
     </row>
@@ -4985,10 +5320,15 @@
       </c>
       <c r="R68" t="inlineStr">
         <is>
+          <t>[-5.39024451e+02  1.11665677e+06]</t>
+        </is>
+      </c>
+      <c r="S68" t="inlineStr">
+        <is>
           <t>{2021: 26695.9585691294, 2022: 26749.33097979799, 2023: 26210.306528806454, 2024: 25671.282077814918, 2025: 25132.257626823615, 2026: 24593.23317583208, 2027: 24054.208724840544, 2028: 23515.18427384901, 2029: 22976.159822857706, 2030: 22437.13537186617, 2031: 21898.110920874635, 2032: 21359.086469883332, 2033: 20820.062018891796, 2034: 20281.03756790026, 2035: 19742.013116908725, 2036: 19202.988665917423, 2037: 18663.964214925887, 2038: 18124.93976393435, 2039: 17585.915312942816, 2040: 17046.890861951513, 2041: 16507.866410959978, 2042: 15968.841959968442, 2043: 15429.81750897714, 2044: 14890.793057985604, 2045: 14351.768606994068, 2046: 13812.744156002533, 2047: 13273.71970501123, 2048: 12734.695254019694, 2049: 12195.670803028159, 2050: 11656.646352036856}</t>
         </is>
       </c>
-      <c r="S68" t="n">
+      <c r="T68" t="n">
         <v>564406.3274201492</v>
       </c>
     </row>
@@ -5052,10 +5392,15 @@
       </c>
       <c r="R69" t="inlineStr">
         <is>
+          <t>[-2.30040820e+03  4.69254439e+06]</t>
+        </is>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
           <t>{2021: 46040.8639867489, 2022: 41119.0098768007, 2023: 38818.60167533811, 2024: 36518.19347387552, 2025: 34217.78527241293, 2026: 31917.377070950344, 2027: 29616.968869487755, 2028: 27316.560668025166, 2029: 25016.152466562577, 2030: 22715.744265099987, 2031: 20415.3360636374, 2032: 18114.92786217481, 2033: 15814.51966071222, 2034: 13514.11145924963, 2035: 11213.703257787041, 2036: 8913.295056324452, 2037: 6612.886854861863, 2038: 4312.478653399274, 2039: 2012.0704519366845, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S69" t="n">
+      <c r="T69" t="n">
         <v>411200.154952011</v>
       </c>
     </row>
@@ -5119,10 +5464,15 @@
       </c>
       <c r="R70" t="inlineStr">
         <is>
+          <t>[ 8.13724232e+02 -1.58453372e+06]</t>
+        </is>
+      </c>
+      <c r="S70" t="inlineStr">
+        <is>
           <t>{2021: 58791.6820261748, 2022: 60816.67669059592, 2023: 61630.40092231287, 2024: 62444.12515403004, 2025: 63257.84938574722, 2026: 64071.5736174644, 2027: 64885.297849181574, 2028: 65699.02208089852, 2029: 66512.7463126157, 2030: 67326.47054433287, 2031: 68140.19477605005, 2032: 68953.91900776722, 2033: 69767.64323948417, 2034: 70581.36747120135, 2035: 71395.09170291852, 2036: 72208.8159346357, 2037: 73022.54016635264, 2038: 73836.26439806982, 2039: 74649.988629787, 2040: 75463.71286150417, 2041: 76277.43709322135, 2042: 77091.1613249383, 2043: 77904.88555665547, 2044: 78718.60978837265, 2045: 79532.33402008982, 2046: 80346.05825180677, 2047: 81159.78248352394, 2048: 81973.50671524112, 2049: 82787.2309469583, 2050: 83600.95517867547}</t>
         </is>
       </c>
-      <c r="S70" t="n">
+      <c r="T70" t="n">
         <v>2081651.025528183</v>
       </c>
     </row>
@@ -5186,10 +5536,15 @@
       </c>
       <c r="R71" t="inlineStr">
         <is>
+          <t>[-6.65571706e+03  1.38778695e+07]</t>
+        </is>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
           <t>{2021: 433330.272411755, 2022: 420009.65124240704, 2023: 413353.93418391794, 2024: 406698.2171254307, 2025: 400042.5000669416, 2026: 393386.7830084525, 2027: 386731.06594996527, 2028: 380075.34889147617, 2029: 373419.63183298707, 2030: 366763.91477449983, 2031: 360108.19771601073, 2032: 353452.48065752164, 2033: 346796.7635990344, 2034: 340141.0465405453, 2035: 333485.3294820562, 2036: 326829.61242356896, 2037: 320173.89536507986, 2038: 313518.17830659077, 2039: 306862.46124810353, 2040: 300206.74418961443, 2041: 293551.0271311272, 2042: 286895.3100726381, 2043: 280239.593014149, 2044: 273583.87595566176, 2045: 266928.15889717266, 2046: 260272.44183868356, 2047: 253616.72478019632, 2048: 246961.00772170722, 2049: 240305.29066321813, 2050: 233649.5736047309}</t>
         </is>
       </c>
-      <c r="S71" t="n">
+      <c r="T71" t="n">
         <v>9577899.109687002</v>
       </c>
     </row>
@@ -5253,10 +5608,15 @@
       </c>
       <c r="R72" t="inlineStr">
         <is>
+          <t>[-8.89007020e+02  1.81766405e+06]</t>
+        </is>
+      </c>
+      <c r="S72" t="inlineStr">
+        <is>
           <t>{2021: 21156.8159179098, 2022: 20091.85724540893, 2023: 19202.850225555012, 2024: 18313.843205701327, 2025: 17424.836185847642, 2026: 16535.829165993724, 2027: 15646.822146140039, 2028: 14757.815126286354, 2029: 13868.808106432436, 2030: 12979.801086578751, 2031: 12090.794066724833, 2032: 11201.787046871148, 2033: 10312.780027017463, 2034: 9423.773007163545, 2035: 8534.76598730986, 2036: 7645.758967456175, 2037: 6756.751947602257, 2038: 5867.744927748572, 2039: 4978.737907894654, 2040: 4089.730888040969, 2041: 3200.723868187284, 2042: 2311.716848333366, 2043: 1422.7098284796812, 2044: 533.7028086259961, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S72" t="n">
+      <c r="T72" t="n">
         <v>247772.3485803549</v>
       </c>
     </row>
@@ -5320,10 +5680,15 @@
       </c>
       <c r="R73" t="inlineStr">
         <is>
+          <t>[-7.66188476e+02  1.56698101e+06]</t>
+        </is>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
           <t>{2021: 18812.6023604529, 2022: 17747.910900079412, 2023: 16981.722424515523, 2024: 16215.533948951634, 2025: 15449.345473387511, 2026: 14683.156997823622, 2027: 13916.968522259733, 2028: 13150.780046695843, 2029: 12384.591571131954, 2030: 11618.403095567832, 2031: 10852.214620003942, 2032: 10086.026144440053, 2033: 9319.837668876164, 2034: 8553.649193312274, 2035: 7787.460717748385, 2036: 7021.272242184263, 2037: 6255.083766620373, 2038: 5488.895291056484, 2039: 4722.706815492595, 2040: 3956.5183399287052, 2041: 3190.329864364583, 2042: 2424.1413888006937, 2043: 1657.9529132368043, 2044: 891.7644376729149, 2045: 125.57596210902557, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S73" t="n">
+      <c r="T73" t="n">
         <v>223888.1435264868</v>
       </c>
     </row>
@@ -5387,10 +5752,15 @@
       </c>
       <c r="R74" t="inlineStr">
         <is>
+          <t>[-4.77469594e+03  9.73343685e+06]</t>
+        </is>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
           <t>{2021: 88139.5693861936, 2022: 79001.64650530554, 2023: 74226.95056099631, 2024: 69452.25461668707, 2025: 64677.55867237784, 2026: 59902.862728068605, 2027: 55128.16678375937, 2028: 50353.470839450136, 2029: 45578.7748951409, 2030: 40804.07895083167, 2031: 36029.38300652243, 2032: 31254.687062213197, 2033: 26479.991117903963, 2034: 21705.295173594728, 2035: 16930.599229285493, 2036: 12155.903284976259, 2037: 7381.207340667024, 2038: 2606.5113963577896, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S74" t="n">
+      <c r="T74" t="n">
         <v>737739.1268572351</v>
       </c>
     </row>
@@ -5454,10 +5824,15 @@
       </c>
       <c r="R75" t="inlineStr">
         <is>
+          <t>[-5.21424350e+03  1.06405746e+07]</t>
+        </is>
+      </c>
+      <c r="S75" t="inlineStr">
+        <is>
           <t>{2021: 104930.608832851, 2022: 97374.26597972587, 2023: 92160.02247765288, 2024: 86945.77897557989, 2025: 81731.5354735069, 2026: 76517.29197143577, 2027: 71303.04846936278, 2028: 66088.80496728979, 2029: 60874.5614652168, 2030: 55660.31796314567, 2031: 50446.07446107268, 2032: 45231.83095899969, 2033: 40017.5874569267, 2034: 34803.343954855576, 2035: 29589.100452782586, 2036: 24374.856950709596, 2037: 19160.613448636606, 2038: 13946.369946565479, 2039: 8732.12644449249, 2040: 3517.882942419499, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S75" t="n">
+      <c r="T75" t="n">
         <v>1010940.719176803</v>
       </c>
     </row>
@@ -5521,10 +5896,15 @@
       </c>
       <c r="R76" t="inlineStr">
         <is>
+          <t>[-6.21473540e+03  1.26754478e+07]</t>
+        </is>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
           <t>{2021: 118289.914595419, 2022: 109252.78523007222, 2023: 103038.04982997291, 2024: 96823.3144298736, 2025: 90608.57902977243, 2026: 84393.84362967312, 2027: 78179.10822957382, 2028: 71964.37282947451, 2029: 65749.63742937334, 2030: 59534.90202927403, 2031: 53320.166629174724, 2032: 47105.43122907542, 2033: 40890.69582897425, 2034: 34675.96042887494, 2035: 28461.225028775632, 2036: 22246.489628676325, 2037: 16031.754228577018, 2038: 9817.018828475848, 2039: 3602.2834283765405, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S76" t="n">
+      <c r="T76" t="n">
         <v>1074840.57522375</v>
       </c>
     </row>
@@ -5588,10 +5968,15 @@
       </c>
       <c r="R77" t="inlineStr">
         <is>
+          <t>[-1.55687104e+03  3.18596024e+06]</t>
+        </is>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
           <t>{2021: 40751.1227109742, 2022: 37966.99699595617, 2023: 36410.12595556304, 2024: 34853.25491517037, 2025: 33296.38387477724, 2026: 31739.51283438457, 2027: 30182.64179399144, 2028: 28625.770753598772, 2029: 27068.89971320564, 2030: 25512.028672812972, 2031: 23955.15763241984, 2032: 22398.286592027172, 2033: 20841.41555163404, 2034: 19284.544511241373, 2035: 17727.67347084824, 2036: 16170.802430455573, 2037: 14613.93139006244, 2038: 13057.060349669773, 2039: 11500.18930927664, 2040: 9943.318268883973, 2041: 8386.44722849084, 2042: 6829.576188098174, 2043: 5272.705147705041, 2044: 3715.834107312374, 2045: 2158.963066919241, 2046: 602.092026526574, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S77" t="n">
+      <c r="T77" t="n">
         <v>502489.1741365186</v>
       </c>
     </row>
@@ -5655,10 +6040,15 @@
       </c>
       <c r="R78" t="inlineStr">
         <is>
+          <t>[-1.54548393e+03  3.16244847e+06]</t>
+        </is>
+      </c>
+      <c r="S78" t="inlineStr">
+        <is>
           <t>{2021: 43088.441163385, 2022: 37479.95586147439, 2023: 35934.471928820945, 2024: 34388.98799616704, 2025: 32843.504063513596, 2026: 31298.020130859688, 2027: 29752.536198206246, 2028: 28207.05226555234, 2029: 26661.568332898896, 2030: 25116.08440024499, 2031: 23570.600467591546, 2032: 22025.11653493764, 2033: 20479.632602284197, 2034: 18934.14866963029, 2035: 17388.664736976847, 2036: 15843.18080432294, 2037: 14297.696871669497, 2038: 12752.21293901559, 2039: 11206.729006362148, 2040: 9661.24507370824, 2041: 8115.761141054798, 2042: 6570.27720840089, 2043: 5024.793275747448, 2044: 3479.3093430935405, 2045: 1933.8254104400985, 2046: 388.3414777861908, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S78" t="n">
+      <c r="T78" t="n">
         <v>494897.9373224525</v>
       </c>
     </row>
@@ -5722,10 +6112,15 @@
       </c>
       <c r="R79" t="inlineStr">
         <is>
+          <t>[-1.45459440e+03  2.97072551e+06]</t>
+        </is>
+      </c>
+      <c r="S79" t="inlineStr">
+        <is>
           <t>{2021: 31849.0491117575, 2022: 29535.626407840755, 2023: 28081.032003912143, 2024: 26626.437599983998, 2025: 25171.843196055386, 2026: 23717.24879212724, 2027: 22262.65438819863, 2028: 20808.059984270018, 2029: 19353.465580341872, 2030: 17898.87117641326, 2031: 16444.276772485115, 2032: 14989.682368556503, 2033: 13535.087964628357, 2034: 12080.493560699746, 2035: 10625.899156771135, 2036: 9171.304752842989, 2037: 7716.710348914377, 2038: 6262.115944986232, 2039: 4807.52154105762, 2040: 3352.9271371294744, 2041: 1898.332733200863, 2042: 443.7383292722516, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S79" t="n">
+      <c r="T79" t="n">
         <v>330707.8542955667</v>
       </c>
     </row>
@@ -5789,10 +6184,15 @@
       </c>
       <c r="R80" t="inlineStr">
         <is>
+          <t>[-8.47801727e+03  1.71684978e+07]</t>
+        </is>
+      </c>
+      <c r="S80" t="inlineStr">
+        <is>
           <t>{2021: 41363.3668840834, 2022: 25946.91946527362, 2023: 17468.90219083801, 2024: 8990.8849164024, 2025: 512.8676419630647, 2026: 0, 2027: 0, 2028: 0, 2029: 0, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S80" t="n">
+      <c r="T80" t="n">
         <v>73601.25765651879</v>
       </c>
     </row>
@@ -5856,10 +6256,15 @@
       </c>
       <c r="R81" t="inlineStr">
         <is>
+          <t>[-3.07369546e+03  6.27027318e+06]</t>
+        </is>
+      </c>
+      <c r="S81" t="inlineStr">
+        <is>
           <t>{2021: 59782.1249581941, 2022: 55260.955024997704, 2023: 52187.259563962, 2024: 49113.56410292629, 2025: 46039.86864189152, 2026: 42966.17318085581, 2027: 39892.477719820105, 2028: 36818.78225878533, 2029: 33745.086797749624, 2030: 30671.391336713918, 2031: 27597.695875679143, 2032: 24524.000414643437, 2033: 21450.304953608662, 2034: 18376.609492572956, 2035: 15302.91403153725, 2036: 12229.218570502475, 2037: 9155.523109466769, 2038: 6081.827648431063, 2039: 3008.132187396288, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S81" t="n">
+      <c r="T81" t="n">
         <v>554312.8473906374</v>
       </c>
     </row>
@@ -5923,10 +6328,15 @@
       </c>
       <c r="R82" t="inlineStr">
         <is>
+          <t>[-1.67410255e+03  3.51637953e+06]</t>
+        </is>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
           <t>{2021: 131690.249963079, 2022: 131344.1780527183, 2023: 129670.07550462475, 2024: 127995.97295653075, 2025: 126321.87040843721, 2026: 124647.76786034368, 2027: 122973.66531224968, 2028: 121299.56276415614, 2029: 119625.46021606261, 2030: 117951.35766796861, 2031: 116277.25511987507, 2032: 114603.15257178154, 2033: 112929.05002368754, 2034: 111254.947475594, 2035: 109580.84492750047, 2036: 107906.74237940647, 2037: 106232.63983131293, 2038: 104558.53728321893, 2039: 102884.4347351254, 2040: 101210.33218703186, 2041: 99536.22963893786, 2042: 97862.12709084433, 2043: 96188.02454275079, 2044: 94513.92199465679, 2045: 92839.81944656326, 2046: 91165.71689846972, 2047: 89491.61435037572, 2048: 87817.51180228218, 2049: 86143.40925418865, 2050: 84469.30670609465}</t>
         </is>
       </c>
-      <c r="S82" t="n">
+      <c r="T82" t="n">
         <v>3152906.000631282</v>
       </c>
     </row>
@@ -5990,10 +6400,15 @@
       </c>
       <c r="R83" t="inlineStr">
         <is>
+          <t>[-1.05976138e+03  2.32642197e+06]</t>
+        </is>
+      </c>
+      <c r="S83" t="inlineStr">
+        <is>
           <t>{2021: 174606.772585002, 2022: 183584.46941203158, 2023: 182524.70803548768, 2024: 181464.94665894425, 2025: 180405.18528240034, 2026: 179345.4239058569, 2027: 178285.66252931347, 2028: 177225.90115276957, 2029: 176166.13977622613, 2030: 175106.37839968223, 2031: 174046.6170231388, 2032: 172986.8556465949, 2033: 171927.09427005146, 2034: 170867.33289350756, 2035: 169807.57151696412, 2036: 168747.81014042022, 2037: 167688.04876387678, 2038: 166628.28738733334, 2039: 165568.52601078944, 2040: 164508.764634246, 2041: 163449.0032577021, 2042: 162389.24188115867, 2043: 161329.48050461477, 2044: 160269.71912807133, 2045: 159209.95775152743, 2046: 158150.196374984, 2047: 157090.4349984401, 2048: 156030.67362189665, 2049: 154970.91224535322, 2050: 153911.15086880932}</t>
         </is>
       </c>
-      <c r="S83" t="n">
+      <c r="T83" t="n">
         <v>4904034.304930289</v>
       </c>
     </row>
@@ -6057,10 +6472,15 @@
       </c>
       <c r="R84" t="inlineStr">
         <is>
+          <t>[-1.30069938e+03  2.69706413e+06]</t>
+        </is>
+      </c>
+      <c r="S84" t="inlineStr">
+        <is>
           <t>{2021: 70300.7397701479, 2022: 67049.97637300054, 2023: 65749.27698854217, 2024: 64448.57760408381, 2025: 63147.87821962545, 2026: 61847.178835167084, 2027: 60546.47945070872, 2028: 59245.78006625036, 2029: 57945.080681791995, 2030: 56644.38129733363, 2031: 55343.68191287527, 2032: 54042.982528416906, 2033: 52742.28314395854, 2034: 51441.58375950018, 2035: 50140.88437504182, 2036: 48840.18499058299, 2037: 47539.485606124625, 2038: 46238.78622166626, 2039: 44938.0868372079, 2040: 43637.387452749535, 2041: 42336.68806829117, 2042: 41035.98868383281, 2043: 39735.289299374446, 2044: 38434.58991491608, 2045: 37133.89053045772, 2046: 35833.19114599936, 2047: 34532.491761540994, 2048: 33231.79237708263, 2049: 31931.092992624268, 2050: 30630.393608165905}</t>
         </is>
       </c>
-      <c r="S84" t="n">
+      <c r="T84" t="n">
         <v>1436200.537807904</v>
       </c>
     </row>
@@ -6124,10 +6544,15 @@
       </c>
       <c r="R85" t="inlineStr">
         <is>
+          <t>[-2.82179165e+03  5.92404133e+06]</t>
+        </is>
+      </c>
+      <c r="S85" t="inlineStr">
+        <is>
           <t>{2021: 241295.112733841, 2022: 218378.61377188656, 2023: 215556.82212197874, 2024: 212735.03047206998, 2025: 209913.23882216215, 2026: 207091.4471722534, 2027: 204269.65552234557, 2028: 201447.8638724368, 2029: 198626.07222252898, 2030: 195804.28057262022, 2031: 192982.4889227124, 2032: 190160.69727280363, 2033: 187338.9056228958, 2034: 184517.11397298705, 2035: 181695.32232307922, 2036: 178873.53067317046, 2037: 176051.73902326263, 2038: 173229.94737335388, 2039: 170408.15572344605, 2040: 167586.3640735373, 2041: 164764.57242362946, 2042: 161942.7807737207, 2043: 159120.98912381288, 2044: 156299.19747390412, 2045: 153477.4058239963, 2046: 150655.61417408753, 2047: 147833.8225241797, 2048: 145012.03087427095, 2049: 142190.2392243622, 2050: 139368.44757445436}</t>
         </is>
       </c>
-      <c r="S85" t="n">
+      <c r="T85" t="n">
         <v>5238295.722101643</v>
       </c>
     </row>
@@ -6191,10 +6616,15 @@
       </c>
       <c r="R86" t="inlineStr">
         <is>
+          <t>[-1.17173470e+03  2.38482469e+06]</t>
+        </is>
+      </c>
+      <c r="S86" t="inlineStr">
+        <is>
           <t>{2021: 17959.3007233107, 2022: 15577.125830624718, 2023: 14405.391130300704, 2024: 13233.65642997669, 2025: 12061.921729652677, 2026: 10890.187029328663, 2027: 9718.452329005115, 2028: 8546.7176286811, 2029: 7374.982928357087, 2030: 6203.248228033073, 2031: 5031.513527709059, 2032: 3859.7788273850456, 2033: 2688.0441270614974, 2034: 1516.3094267374836, 2035: 344.57472641346976, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S86" t="n">
+      <c r="T86" t="n">
         <v>120431.5542609217</v>
       </c>
     </row>
@@ -6258,10 +6688,15 @@
       </c>
       <c r="R87" t="inlineStr">
         <is>
+          <t>[-8.93680181e+02  1.84836892e+06]</t>
+        </is>
+      </c>
+      <c r="S87" t="inlineStr">
+        <is>
           <t>{2021: 41796.3025070363, 2022: 41347.59122243873, 2023: 40453.91104177572, 2024: 39560.23086111271, 2025: 38666.5506804497, 2026: 37772.87049978669, 2027: 36879.19031912368, 2028: 35985.51013846067, 2029: 35091.82995779766, 2030: 34198.14977713465, 2031: 33304.46959647164, 2032: 32410.789415808627, 2033: 31517.109235145617, 2034: 30623.429054482607, 2035: 29729.748873819597, 2036: 28836.068693156587, 2037: 27942.388512493577, 2038: 27048.708331830567, 2039: 26155.028151167324, 2040: 25261.347970504314, 2041: 24367.667789841304, 2042: 23473.987609178293, 2043: 22580.307428515283, 2044: 21686.627247852273, 2045: 20792.947067189263, 2046: 19899.266886526253, 2047: 19005.586705863243, 2048: 18111.906525200233, 2049: 17218.226344537223, 2050: 16324.546163874213}</t>
         </is>
       </c>
-      <c r="S87" t="n">
+      <c r="T87" t="n">
         <v>848981.8702731193</v>
       </c>
     </row>
@@ -6325,10 +6760,15 @@
       </c>
       <c r="R88" t="inlineStr">
         <is>
+          <t>[-1.64427514e+03  3.36582016e+06]</t>
+        </is>
+      </c>
+      <c r="S88" t="inlineStr">
+        <is>
           <t>{2021: 43181.7418189813, 2022: 41095.81622094149, 2023: 39451.54107758403, 2024: 37807.26593422657, 2025: 36162.990790868644, 2026: 34518.715647511184, 2027: 32874.44050415326, 2028: 31230.1653607958, 2029: 29585.89021743834, 2030: 27941.615074080415, 2031: 26297.339930722956, 2032: 24653.064787365496, 2033: 23008.78964400757, 2034: 21364.51450065011, 2035: 19720.239357292652, 2036: 18075.964213934727, 2037: 16431.689070577268, 2038: 14787.413927219808, 2039: 13143.138783861883, 2040: 11498.863640504424, 2041: 9854.588497146498, 2042: 8210.313353789039, 2043: 6566.0382104315795, 2044: 4921.763067073654, 2045: 3277.487923716195, 2046: 1633.2127803587355, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S88" t="n">
+      <c r="T88" t="n">
         <v>555703.7334257429</v>
       </c>
     </row>
@@ -6392,10 +6832,15 @@
       </c>
       <c r="R89" t="inlineStr">
         <is>
+          <t>[-2.23255540e+03  4.54087991e+06]</t>
+        </is>
+      </c>
+      <c r="S89" t="inlineStr">
+        <is>
           <t>{2021: 31891.2540988899, 2022: 26652.894434583373, 2023: 24420.339035529643, 2024: 22187.783636475913, 2025: 19955.228237422183, 2026: 17722.672838368453, 2027: 15490.117439314723, 2028: 13257.562040260993, 2029: 11025.006641207263, 2030: 8792.451242153533, 2031: 6559.895843099803, 2032: 4327.340444046073, 2033: 2094.7850449923426, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S89" t="n">
+      <c r="T89" t="n">
         <v>188431.7039268992</v>
       </c>
     </row>
@@ -6459,10 +6904,15 @@
       </c>
       <c r="R90" t="inlineStr">
         <is>
+          <t>[-7.42259790e+02  1.57578228e+06]</t>
+        </is>
+      </c>
+      <c r="S90" t="inlineStr">
+        <is>
           <t>{2021: 72857.259205152, 2022: 74932.9882925069, 2023: 74190.72850280395, 2024: 73448.46871310077, 2025: 72706.20892339782, 2026: 71963.94913369487, 2027: 71221.68934399169, 2028: 70479.42955428874, 2029: 69737.1697645858, 2030: 68994.90997488284, 2031: 68252.65018517966, 2032: 67510.39039547672, 2033: 66768.13060577377, 2034: 66025.87081607082, 2035: 65283.61102636764, 2036: 64541.35123666469, 2037: 63799.09144696174, 2038: 63056.831657258794, 2039: 62314.57186755561, 2040: 61572.312077852665, 2041: 60830.052288149716, 2042: 60087.79249844677, 2043: 59345.53270874359, 2044: 58603.27291904064, 2045: 57861.01312933769, 2046: 57118.75333963474, 2047: 56376.49354993156, 2048: 55634.23376022861, 2049: 54891.973970525665, 2050: 54149.714180822484}</t>
         </is>
       </c>
-      <c r="S90" t="n">
+      <c r="T90" t="n">
         <v>1881052.958375442</v>
       </c>
     </row>
@@ -6526,10 +6976,15 @@
       </c>
       <c r="R91" t="inlineStr">
         <is>
+          <t>[-8.44138407e+03  1.74391738e+07]</t>
+        </is>
+      </c>
+      <c r="S91" t="inlineStr">
+        <is>
           <t>{2021: 385811.84637716, 2022: 370695.2034085393, 2023: 362253.81933544204, 2024: 353812.4352623485, 2025: 345371.05118925497, 2026: 336929.6671161577, 2027: 328488.2830430642, 2028: 320046.8989699669, 2029: 311605.5148968734, 2030: 303164.1308237761, 2031: 294722.7467506826, 2032: 286281.36267758533, 2033: 277839.9786044918, 2034: 269398.59453139454, 2035: 260957.210458301, 2036: 252515.82638520375, 2037: 244074.44231211022, 2038: 235633.05823901668, 2039: 227191.67416591942, 2040: 218750.2900928259, 2041: 210308.90601972863, 2042: 201867.5219466351, 2043: 193426.13787353784, 2044: 184984.7538004443, 2045: 176543.36972734705, 2046: 168101.9856542535, 2047: 159660.60158115625, 2048: 151219.21750806272, 2049: 142777.8334349692, 2050: 134336.44936187193}</t>
         </is>
       </c>
-      <c r="S91" t="n">
+      <c r="T91" t="n">
         <v>7448696.663678605</v>
       </c>
     </row>
@@ -6593,10 +7048,15 @@
       </c>
       <c r="R92" t="inlineStr">
         <is>
+          <t>[-1.15638179e+03  2.39868465e+06]</t>
+        </is>
+      </c>
+      <c r="S92" t="inlineStr">
+        <is>
           <t>{2021: 64815.2841043127, 2022: 60480.66651944583, 2023: 59324.284727805294, 2024: 58167.902936164755, 2025: 57011.52114452422, 2026: 55855.13935288321, 2027: 54698.75756124267, 2028: 53542.375769602135, 2029: 52385.99397796113, 2030: 51229.61218632059, 2031: 50073.23039468005, 2032: 48916.848603039514, 2033: 47760.46681139851, 2034: 46604.08501975797, 2035: 45447.70322811743, 2036: 44291.32143647643, 2037: 43134.93964483589, 2038: 41978.55785319535, 2039: 40822.17606155481, 2040: 39665.79426991381, 2041: 38509.41247827327, 2042: 37353.03068663273, 2043: 36196.648894991726, 2044: 35040.26710335119, 2045: 33883.88531171065, 2046: 32727.50352007011, 2047: 31571.121728429105, 2048: 30414.739936788566, 2049: 29258.358145148028, 2050: 28101.976353507023}</t>
         </is>
       </c>
-      <c r="S92" t="n">
+      <c r="T92" t="n">
         <v>1302804.975533225</v>
       </c>
     </row>
@@ -6660,10 +7120,15 @@
       </c>
       <c r="R93" t="inlineStr">
         <is>
+          <t>[-6.08447065e+03  1.24099946e+07]</t>
+        </is>
+      </c>
+      <c r="S93" t="inlineStr">
+        <is>
           <t>{2021: 116813.181802889, 2022: 107194.90756044537, 2023: 101110.43690934218, 2024: 95025.96625823714, 2025: 88941.49560713395, 2026: 82857.02495603077, 2027: 76772.55430492572, 2028: 70688.08365382254, 2029: 64603.61300271936, 2030: 58519.14235161431, 2031: 52434.67170051113, 2032: 46350.201049407944, 2033: 40265.7303983029, 2034: 34181.259747199714, 2035: 28096.78909609653, 2036: 22012.318444991484, 2037: 15927.8477938883, 2038: 9843.377142783254, 2039: 3758.9064916800708, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S93" t="n">
+      <c r="T93" t="n">
         <v>1056990.917370577</v>
       </c>
     </row>
@@ -6727,10 +7192,15 @@
       </c>
       <c r="R94" t="inlineStr">
         <is>
+          <t>[-1.03094104e+03  2.10108099e+06]</t>
+        </is>
+      </c>
+      <c r="S94" t="inlineStr">
+        <is>
           <t>{2021: 17780.8039766664, 2022: 16518.201988180168, 2023: 15487.26094591245, 2024: 14456.3199036445, 2025: 13425.378861376783, 2026: 12394.437819109065, 2027: 11363.496776841348, 2028: 10332.555734573398, 2029: 9301.61469230568, 2030: 8270.673650037963, 2031: 7239.732607770013, 2032: 6208.791565502295, 2033: 5177.850523234578, 2034: 4146.909480966628, 2035: 3115.96843869891, 2036: 2085.0273964311928, 2037: 1054.0863541634753, 2038: 23.145311895757914, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S94" t="n">
+      <c r="T94" t="n">
         <v>149491.8540389774</v>
       </c>
     </row>
@@ -6794,10 +7264,15 @@
       </c>
       <c r="R95" t="inlineStr">
         <is>
+          <t>[ 4.00737271e+03 -7.97963742e+06]</t>
+        </is>
+      </c>
+      <c r="S95" t="inlineStr">
+        <is>
           <t>{2021: 161074.659994972, 2022: 123270.19169470947, 2023: 127277.5643997658, 2024: 131284.9371048212, 2025: 135292.30980987754, 2026: 139299.68251493294, 2027: 143307.05521998927, 2028: 147314.42792504467, 2029: 151321.800630101, 2030: 155329.1733351564, 2031: 159336.5460402118, 2032: 163343.91874526814, 2033: 167351.29145032354, 2034: 171358.66415537987, 2035: 175366.03686043527, 2036: 179373.4095654916, 2037: 183380.782270547, 2038: 187388.15497560333, 2039: 191395.52768065874, 2040: 195402.90038571414, 2041: 199410.27309077047, 2042: 203417.64579582587, 2043: 207425.0185008822, 2044: 211432.3912059376, 2045: 215439.76391099393, 2046: 219447.13661604933, 2047: 223454.50932110567, 2048: 227461.88202616107, 2049: 231469.25473121647, 2050: 235476.6274362728}</t>
         </is>
       </c>
-      <c r="S95" t="n">
+      <c r="T95" t="n">
         <v>5164627.893678596</v>
       </c>
     </row>
@@ -6861,10 +7336,15 @@
       </c>
       <c r="R96" t="inlineStr">
         <is>
+          <t>[-3.51507449e+03  7.18494203e+06]</t>
+        </is>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
           <t>{2021: 81092.8269941256, 2022: 77461.40557587333, 2023: 73946.3310853364, 2024: 70431.25659479853, 2025: 66916.18210426159, 2026: 63401.10761372466, 2027: 59886.03312318772, 2028: 56370.958632650785, 2029: 52855.88414211385, 2030: 49340.809651576914, 2031: 45825.73516103905, 2032: 42310.66067050211, 2033: 38795.586179965176, 2034: 35280.51168942824, 2035: 31765.437198891304, 2036: 28250.36270835437, 2037: 24735.288217817433, 2038: 21220.213727279566, 2039: 17705.13923674263, 2040: 14190.064746205695, 2041: 10674.99025566876, 2042: 7159.915765131824, 2043: 3644.841274594888, 2044: 129.76678405795246, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S96" t="n">
+      <c r="T96" t="n">
         <v>932844.8956362656</v>
       </c>
     </row>
@@ -6928,10 +7408,15 @@
       </c>
       <c r="R97" t="inlineStr">
         <is>
+          <t>[-2.76121247e+03  5.68691603e+06]</t>
+        </is>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
           <t>{2021: 104241.611582051, 2022: 103744.41315040365, 2023: 100983.2006800687, 2024: 98221.98820973467, 2025: 95460.77573939972, 2026: 92699.5632690657, 2027: 89938.35079873167, 2028: 87177.13832839672, 2029: 84415.92585806269, 2030: 81654.71338772774, 2031: 78893.50091739371, 2032: 76132.28844705876, 2033: 73371.07597672474, 2034: 70609.86350638978, 2035: 67848.65103605576, 2036: 65087.438565720804, 2037: 62326.22609538678, 2038: 59565.01362505276, 2039: 56803.8011547178, 2040: 54042.58868438378, 2041: 51281.376214048825, 2042: 48520.1637437148, 2043: 45758.95127337985, 2044: 42997.738803045824, 2045: 40236.52633271087, 2046: 37475.31386237685, 2047: 34714.10139204189, 2048: 31952.88892170787, 2049: 29191.676451373845, 2050: 26430.46398103889}</t>
         </is>
       </c>
-      <c r="S97" t="n">
+      <c r="T97" t="n">
         <v>1926441.292206421</v>
       </c>
     </row>
@@ -6995,10 +7480,15 @@
       </c>
       <c r="R98" t="inlineStr">
         <is>
+          <t>[-4.86873682e+03  1.00334123e+07]</t>
+        </is>
+      </c>
+      <c r="S98" t="inlineStr">
+        <is>
           <t>{2021: 196040.384620013, 2022: 188826.4148816131, 2023: 183957.67806071043, 2024: 179088.94123980775, 2025: 174220.20441890694, 2026: 169351.46759800427, 2027: 164482.7307771016, 2028: 159613.99395620078, 2029: 154745.2571352981, 2030: 149876.52031439543, 2031: 145007.78349349461, 2032: 140139.04667259194, 2033: 135270.30985169113, 2034: 130401.57303078845, 2035: 125532.83620988578, 2036: 120664.09938898496, 2037: 115795.36256808229, 2038: 110926.62574717961, 2039: 106057.8889262788, 2040: 101189.15210537612, 2041: 96320.41528447345, 2042: 91451.67846357264, 2043: 86582.94164266996, 2044: 81714.20482176915, 2045: 76845.46800086647, 2046: 71976.7311799638, 2047: 67107.99435906298, 2048: 62239.25753816031, 2049: 57370.520717257634, 2050: 52501.78389635682}</t>
         </is>
       </c>
-      <c r="S98" t="n">
+      <c r="T98" t="n">
         <v>3571028.182642373</v>
       </c>
     </row>
@@ -7062,10 +7552,15 @@
       </c>
       <c r="R99" t="inlineStr">
         <is>
+          <t>[-2.76030861e+03  5.64596541e+06]</t>
+        </is>
+      </c>
+      <c r="S99" t="inlineStr">
+        <is>
           <t>{2021: 70156.4487205661, 2022: 64621.3902753545, 2023: 61861.08166215848, 2024: 59100.77304896247, 2025: 56340.46443576738, 2026: 53580.15582257137, 2027: 50819.84720937535, 2028: 48059.53859618027, 2029: 45299.22998298425, 2030: 42538.92136978824, 2031: 39778.61275659315, 2032: 37018.30414339714, 2033: 34257.99553020112, 2034: 31497.686917006038, 2035: 28737.378303810023, 2036: 25977.069690614007, 2037: 23216.761077418923, 2038: 20456.452464222908, 2039: 17696.143851026893, 2040: 14935.835237830877, 2041: 12175.526624635793, 2042: 9415.218011439778, 2043: 6654.909398243763, 2044: 3894.6007850486785, 2045: 1134.2921718526632, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S99" t="n">
+      <c r="T99" t="n">
         <v>824146.4137267671</v>
       </c>
     </row>
@@ -7129,10 +7624,15 @@
       </c>
       <c r="R100" t="inlineStr">
         <is>
+          <t>[-4.45389017e+02  9.34941939e+05]</t>
+        </is>
+      </c>
+      <c r="S100" t="inlineStr">
+        <is>
           <t>{2021: 35690.6495938968, 2022: 34365.34639013617, 2023: 33919.957372837, 2024: 33474.56835553795, 2025: 33029.179338238784, 2026: 32583.790320939734, 2027: 32138.401303640567, 2028: 31693.012286341516, 2029: 31247.62326904235, 2030: 30802.2342517433, 2031: 30356.845234444132, 2032: 29911.456217144965, 2033: 29466.067199845915, 2034: 29020.678182546748, 2035: 28575.289165247697, 2036: 28129.90014794853, 2037: 27684.51113064948, 2038: 27239.122113350313, 2039: 26793.733096051263, 2040: 26348.344078752096, 2041: 25902.955061453045, 2042: 25457.56604415388, 2043: 25012.177026854828, 2044: 24566.78800955566, 2045: 24121.39899225661, 2046: 23676.009974957444, 2047: 23230.620957658393, 2048: 22785.231940359226, 2049: 22339.84292306006, 2050: 21894.45390576101}</t>
         </is>
       </c>
-      <c r="S100" t="n">
+      <c r="T100" t="n">
         <v>822665.2021345767</v>
       </c>
     </row>
@@ -7196,10 +7696,15 @@
       </c>
       <c r="R101" t="inlineStr">
         <is>
+          <t>[-1.81287146e+03  3.70205654e+06]</t>
+        </is>
+      </c>
+      <c r="S101" t="inlineStr">
+        <is>
           <t>{2021: 38712.3814730806, 2022: 36430.448973326944, 2023: 34617.57751195319, 2024: 32804.70605057897, 2025: 30991.83458920475, 2026: 29178.96312783053, 2027: 27366.091666456312, 2028: 25553.220205082092, 2029: 23740.348743707873, 2030: 21927.477282333653, 2031: 20114.605820959434, 2032: 18301.734359585214, 2033: 16488.86289821146, 2034: 14675.991436837241, 2035: 12863.119975463022, 2036: 11050.248514088802, 2037: 9237.377052714583, 2038: 7424.505591340363, 2039: 5611.6341299661435, 2040: 3798.762668591924, 2041: 1985.8912072177045, 2042: 173.019745843485, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S101" t="n">
+      <c r="T101" t="n">
         <v>403692.612287834</v>
       </c>
     </row>
@@ -7263,10 +7768,15 @@
       </c>
       <c r="R102" t="inlineStr">
         <is>
+          <t>[ 2.28368894e+03 -3.91316511e+06]</t>
+        </is>
+      </c>
+      <c r="S102" t="inlineStr">
+        <is>
           <t>{2021: 685614.104946655, 2022: 704453.9260673192, 2023: 706737.6150065442, 2024: 709021.3039457691, 2025: 711304.992884994, 2026: 713588.681824219, 2027: 715872.3707634439, 2028: 718156.0597026697, 2029: 720439.7486418947, 2030: 722723.4375811196, 2031: 725007.1265203445, 2032: 727290.8154595695, 2033: 729574.5043987944, 2034: 731858.1933380202, 2035: 734141.8822772452, 2036: 736425.5712164701, 2037: 738709.260155695, 2038: 740992.94909492, 2039: 743276.6380341449, 2040: 745560.3269733707, 2041: 747844.0159125957, 2042: 750127.7048518206, 2043: 752411.3937910455, 2044: 754695.0827302705, 2045: 756978.7716694954, 2046: 759262.4606087212, 2047: 761546.1495479462, 2048: 763829.8384871711, 2049: 766113.527426396, 2050: 768397.216365621}</t>
         </is>
       </c>
-      <c r="S102" t="n">
+      <c r="T102" t="n">
         <v>21314950.00956815</v>
       </c>
     </row>
@@ -7330,10 +7840,15 @@
       </c>
       <c r="R103" t="inlineStr">
         <is>
+          <t>[-1.85002009e+03  3.80453736e+06]</t>
+        </is>
+      </c>
+      <c r="S103" t="inlineStr">
+        <is>
           <t>{2021: 67082.1645574866, 2022: 63796.74409774132, 2023: 61946.72401086707, 2024: 60096.70392399235, 2025: 58246.68383711809, 2026: 56396.66375024337, 2027: 54546.64366336912, 2028: 52696.623576494865, 2029: 50846.603489620145, 2030: 48996.58340274589, 2031: 47146.56331587117, 2032: 45296.54322899692, 2033: 43446.5231421222, 2034: 41596.503055247944, 2035: 39746.48296837369, 2036: 37896.46288149897, 2037: 36046.442794624716, 2038: 34196.422707749996, 2039: 32346.402620875742, 2040: 30496.382534001023, 2041: 28646.36244712677, 2042: 26796.342360252514, 2043: 24946.322273377795, 2044: 23096.30218650354, 2045: 21246.28209962882, 2046: 19396.262012754567, 2047: 17546.241925879847, 2048: 15696.221839005593, 2049: 13846.20175213134, 2050: 11996.18166525662}</t>
         </is>
       </c>
-      <c r="S103" t="n">
+      <c r="T103" t="n">
         <v>1126540.415009587</v>
       </c>
     </row>
@@ -7397,10 +7912,15 @@
       </c>
       <c r="R104" t="inlineStr">
         <is>
+          <t>[-2.16311534e+03  4.43097487e+06]</t>
+        </is>
+      </c>
+      <c r="S104" t="inlineStr">
+        <is>
           <t>{2021: 58815.7302393248, 2022: 57155.65197950788, 2023: 54992.5366402138, 2024: 52829.42130092066, 2025: 50666.30596162658, 2026: 48503.19062233344, 2027: 46340.07528304029, 2028: 44176.95994374622, 2029: 42013.84460445307, 2030: 39850.729265158996, 2031: 37687.61392586585, 2032: 35524.498586571775, 2033: 33361.38324727863, 2034: 31198.267907985486, 2035: 29035.15256869141, 2036: 26872.037229398265, 2037: 24708.92189010419, 2038: 22545.806550811045, 2039: 20382.6912115179, 2040: 18219.575872223824, 2041: 16056.46053293068, 2042: 13893.345193636604, 2043: 11730.229854343459, 2044: 9567.114515050314, 2045: 7403.999175756238, 2046: 5240.883836463094, 2047: 3077.768497169018, 2048: 914.6531578758731, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S104" t="n">
+      <c r="T104" t="n">
         <v>813356.984474337</v>
       </c>
     </row>
@@ -7464,10 +7984,15 @@
       </c>
       <c r="R105" t="inlineStr">
         <is>
+          <t>[-2.51896435e+03  5.17186588e+06]</t>
+        </is>
+      </c>
+      <c r="S105" t="inlineStr">
+        <is>
           <t>{2021: 82433.5722273519, 2022: 78519.97336343955, 2023: 76001.00901693944, 2024: 73482.04467044026, 2025: 70963.08032394014, 2026: 68444.11597744003, 2027: 65925.15163094085, 2028: 63406.18728444073, 2029: 60887.22293794155, 2030: 58368.25859144144, 2031: 55849.294244941324, 2032: 53330.32989844214, 2033: 50811.36555194203, 2034: 48292.401205441914, 2035: 45773.43685894273, 2036: 43254.47251244262, 2037: 40735.508165943436, 2038: 38216.54381944332, 2039: 35697.57947294321, 2040: 33178.61512644403, 2041: 30659.650779943913, 2042: 28140.68643344473, 2043: 25621.722086944617, 2044: 23102.757740444504, 2045: 20583.79339394532, 2046: 18064.829047445208, 2047: 15545.864700946026, 2048: 13026.900354445912, 2049: 10507.936007945798, 2050: 7988.971661446616}</t>
         </is>
       </c>
-      <c r="S105" t="n">
+      <c r="T105" t="n">
         <v>1291602.003143796</v>
       </c>
     </row>
@@ -7531,10 +8056,15 @@
       </c>
       <c r="R106" t="inlineStr">
         <is>
+          <t>[-7.55792010e+03  1.54720545e+07]</t>
+        </is>
+      </c>
+      <c r="S106" t="inlineStr">
+        <is>
           <t>{2021: 196241.92700692, 2022: 189940.06575100496, 2023: 182382.14565159753, 2024: 174824.2255521901, 2025: 167266.30545278266, 2026: 159708.38535337523, 2027: 152150.46525396965, 2028: 144592.54515456222, 2029: 137034.6250551548, 2030: 129476.70495574735, 2031: 121918.78485633992, 2032: 114360.86475693434, 2033: 106802.94465752691, 2034: 99245.02455811948, 2035: 91687.10445871204, 2036: 84129.1843593046, 2037: 76571.26425989904, 2038: 69013.3441604916, 2039: 61455.424061084166, 2040: 53897.50396167673, 2041: 46339.58386227116, 2042: 38781.663762863725, 2043: 31223.74366345629, 2044: 23665.823564048856, 2045: 16107.903464641422, 2046: 8549.98336523585, 2047: 992.0632658284158, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S106" t="n">
+      <c r="T106" t="n">
         <v>2580238.640722279</v>
       </c>
     </row>
@@ -7598,10 +8128,15 @@
       </c>
       <c r="R107" t="inlineStr">
         <is>
+          <t>[-3.28475292e+03  6.71747422e+06]</t>
+        </is>
+      </c>
+      <c r="S107" t="inlineStr">
+        <is>
           <t>{2021: 80865.1948404024, 2022: 75703.8092484381, 2023: 72419.05632735603, 2024: 69134.30340627395, 2025: 65849.55048519094, 2026: 62564.797564108856, 2027: 59280.04464302678, 2028: 55995.2917219447, 2029: 52710.53880086262, 2030: 49425.78587977961, 2031: 46141.03295869753, 2032: 42856.28003761545, 2033: 39571.52711653337, 2034: 36286.77419545129, 2035: 33002.02127436828, 2036: 29717.2683532862, 2037: 26432.51543220412, 2038: 23147.76251112204, 2039: 19863.00959003996, 2040: 16578.25666895788, 2041: 13293.50374787487, 2042: 10008.750826792791, 2043: 6723.997905710712, 2044: 3439.2449846286327, 2045: 154.49206354655325, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S107" t="n">
+      <c r="T107" t="n">
         <v>950732.2131640124</v>
       </c>
     </row>
@@ -7665,10 +8200,15 @@
       </c>
       <c r="R108" t="inlineStr">
         <is>
+          <t>[-3.98033692e+03  8.08052691e+06]</t>
+        </is>
+      </c>
+      <c r="S108" t="inlineStr">
+        <is>
           <t>{2021: 39702.8662282482, 2022: 32285.66622049734, 2023: 28305.32930536568, 2024: 24324.992390234023, 2025: 20344.655475102365, 2026: 16364.318559970707, 2027: 12383.981644839048, 2028: 8403.64472970739, 2029: 4423.3078145748, 2030: 442.9708994431421, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S108" t="n">
+      <c r="T108" t="n">
         <v>167130.3001538586</v>
       </c>
     </row>
@@ -7732,10 +8272,15 @@
       </c>
       <c r="R109" t="inlineStr">
         <is>
+          <t>[-1.65940370e+03  3.54025972e+06]</t>
+        </is>
+      </c>
+      <c r="S109" t="inlineStr">
+        <is>
           <t>{2021: 191950.953151967, 2022: 184945.44318343047, 2023: 183286.03948637284, 2024: 181626.63578931475, 2025: 179967.23209225712, 2026: 178307.82839519903, 2027: 176648.4246981414, 2028: 174989.02100108378, 2029: 173329.61730402568, 2030: 171670.21360696806, 2031: 170010.80990990996, 2032: 168351.40621285234, 2033: 166692.00251579424, 2034: 165032.59881873662, 2035: 163373.195121679, 2036: 161713.7914246209, 2037: 160054.38772756327, 2038: 158394.98403050518, 2039: 156735.58033344755, 2040: 155076.17663638946, 2041: 153416.77293933183, 2042: 151757.3692422742, 2043: 150097.9655452161, 2044: 148438.56184815848, 2045: 146779.1581511004, 2046: 145119.75445404276, 2047: 143460.35075698467, 2048: 141800.94705992704, 2049: 140141.54336286942, 2050: 138482.13966581132}</t>
         </is>
       </c>
-      <c r="S109" t="n">
+      <c r="T109" t="n">
         <v>4716434.358057086</v>
       </c>
     </row>
@@ -7799,10 +8344,15 @@
       </c>
       <c r="R110" t="inlineStr">
         <is>
+          <t>[-4.81118013e+03  9.89413728e+06]</t>
+        </is>
+      </c>
+      <c r="S110" t="inlineStr">
+        <is>
           <t>{2021: 170972.7920826, 2022: 165931.0548950415, 2023: 161119.87476525642, 2024: 156308.6946354732, 2025: 151497.5145056881, 2026: 146686.334375903, 2027: 141875.15424611978, 2028: 137063.9741163347, 2029: 132252.7939865496, 2030: 127441.61385676451, 2031: 122630.43372698128, 2032: 117819.25359719619, 2033: 113008.0734674111, 2034: 108196.89333762787, 2035: 103385.71320784278, 2036: 98574.53307805769, 2037: 93763.35294827446, 2038: 88952.17281848937, 2039: 84140.99268870428, 2040: 79329.81255892105, 2041: 74518.63242913596, 2042: 69707.45229935087, 2043: 64896.27216956578, 2044: 60085.092039782554, 2045: 55273.91190999746, 2046: 50462.73178021237, 2047: 45651.551650429145, 2048: 40840.371520644054, 2049: 36029.19139085896, 2050: 31218.011261075735}</t>
         </is>
       </c>
-      <c r="S110" t="n">
+      <c r="T110" t="n">
         <v>2928538.849674452</v>
       </c>
     </row>
@@ -7866,10 +8416,15 @@
       </c>
       <c r="R111" t="inlineStr">
         <is>
+          <t>[-7.07885891e+02  1.46418783e+06]</t>
+        </is>
+      </c>
+      <c r="S111" t="inlineStr">
+        <is>
           <t>{2021: 33670.3774418063, 2022: 32842.559767727274, 2023: 32134.673877174966, 2024: 31426.787986622658, 2025: 30718.90209607035, 2026: 30011.01620551804, 2027: 29303.130314965732, 2028: 28595.244424413657, 2029: 27887.35853386135, 2030: 27179.47264330904, 2031: 26471.58675275673, 2032: 25763.700862204423, 2033: 25055.814971652115, 2034: 24347.929081099806, 2035: 23640.043190547498, 2036: 22932.15729999519, 2037: 22224.27140944288, 2038: 21516.385518890573, 2039: 20808.499628338264, 2040: 20100.613737785956, 2041: 19392.727847233647, 2042: 18684.841956681572, 2043: 17976.956066129263, 2044: 17269.070175576955, 2045: 16561.184285024647, 2046: 15853.298394472338, 2047: 15145.41250392003, 2048: 14437.526613367721, 2049: 13729.640722815413, 2050: 13021.754832263105}</t>
         </is>
       </c>
-      <c r="S111" t="n">
+      <c r="T111" t="n">
         <v>675356.8730046328</v>
       </c>
     </row>
@@ -7933,10 +8488,15 @@
       </c>
       <c r="R112" t="inlineStr">
         <is>
+          <t>[-1.73676002e+03  3.60550236e+06]</t>
+        </is>
+      </c>
+      <c r="S112" t="inlineStr">
+        <is>
           <t>{2021: 94700.2499214517, 2022: 93773.6012194599, 2023: 92036.84119936451, 2024: 90300.08117926866, 2025: 88563.32115917327, 2026: 86826.56113907741, 2027: 85089.80111898202, 2028: 83353.04109888617, 2029: 81616.28107879078, 2030: 79879.52105869493, 2031: 78142.76103859907, 2032: 76406.00101850368, 2033: 74669.24099840783, 2034: 72932.48097831244, 2035: 71195.72095821658, 2036: 69458.96093812119, 2037: 67722.20091802534, 2038: 65985.44089792995, 2039: 64248.68087783409, 2040: 62511.92085773824, 2041: 60775.16083764285, 2042: 59038.40081754699, 2043: 57301.640797451604, 2044: 55564.88077735575, 2045: 53828.12075726036, 2046: 52091.360737164505, 2047: 50354.600717069115, 2048: 48617.84069697326, 2049: 46881.080676877405, 2050: 45144.320656782016}</t>
         </is>
       </c>
-      <c r="S112" t="n">
+      <c r="T112" t="n">
         <v>2039087.831837845</v>
       </c>
     </row>
@@ -8000,10 +8560,15 @@
       </c>
       <c r="R113" t="inlineStr">
         <is>
+          <t>[-2.02687182e+03  4.16071648e+06]</t>
+        </is>
+      </c>
+      <c r="S113" t="inlineStr">
+        <is>
           <t>{2021: 64984.7393355088, 2022: 62381.65052912757, 2023: 60354.77870488493, 2024: 58327.90688064229, 2025: 56301.03505639965, 2026: 54274.16323215701, 2027: 52247.29140791437, 2028: 50220.419583671726, 2029: 48193.547759429086, 2030: 46166.675935186446, 2031: 44139.804110943805, 2032: 42112.932286701165, 2033: 40086.060462458525, 2034: 38059.188638215885, 2035: 36032.316813973244, 2036: 34005.444989730604, 2037: 31978.573165487964, 2038: 29951.701341245323, 2039: 27924.829517002683, 2040: 25897.957692759577, 2041: 23871.085868516937, 2042: 21844.214044274297, 2043: 19817.342220031656, 2044: 17790.470395789016, 2045: 15763.598571546376, 2046: 13736.726747303735, 2047: 11709.854923061095, 2048: 9682.983098818455, 2049: 7656.111274575815, 2050: 5629.239450333174}</t>
         </is>
       </c>
-      <c r="S113" t="n">
+      <c r="T113" t="n">
         <v>1015835.65464477</v>
       </c>
     </row>
@@ -8067,10 +8632,15 @@
       </c>
       <c r="R114" t="inlineStr">
         <is>
+          <t>[-9.67400997e+03  1.98076993e+07]</t>
+        </is>
+      </c>
+      <c r="S114" t="inlineStr">
+        <is>
           <t>{2021: 270481.333456314, 2022: 246851.15575986728, 2023: 237177.1457912475, 2024: 227503.1358226277, 2025: 217829.12585401163, 2026: 208155.11588539183, 2027: 198481.10591677204, 2028: 188807.09594815224, 2029: 179133.08597953618, 2030: 169459.07601091638, 2031: 159785.0660422966, 2032: 150111.05607368052, 2033: 140437.04610506073, 2034: 130763.03613644093, 2035: 121089.02616782486, 2036: 111415.01619920507, 2037: 101741.00623058528, 2038: 92066.99626196921, 2039: 82392.98629334942, 2040: 72718.97632472962, 2041: 63044.96635611355, 2042: 53370.95638749376, 2043: 43696.946418873966, 2044: 34022.9364502579, 2045: 24348.926481638104, 2046: 14674.91651301831, 2047: 5000.906544402242, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S114" t="n">
+      <c r="T114" t="n">
         <v>3409317.47668362</v>
       </c>
     </row>
@@ -8134,10 +8704,15 @@
       </c>
       <c r="R115" t="inlineStr">
         <is>
+          <t>[-4.42120483e+03  9.01196352e+06]</t>
+        </is>
+      </c>
+      <c r="S115" t="inlineStr">
+        <is>
           <t>{2021: 77361.1891192005, 2022: 72287.36137899384, 2023: 67866.15655204095, 2024: 63444.95172508806, 2025: 59023.74689813517, 2026: 54602.54207118228, 2027: 50181.33724422939, 2028: 45760.1324172765, 2029: 41338.92759032361, 2030: 36917.72276337072, 2031: 32496.517936417833, 2032: 28075.313109464943, 2033: 23654.108282512054, 2034: 19232.903455559164, 2035: 14811.698628606275, 2036: 10390.493801653385, 2037: 5969.288974700496, 2038: 1548.084147747606, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S115" t="n">
+      <c r="T115" t="n">
         <v>666281.8815369025</v>
       </c>
     </row>
@@ -8201,10 +8776,15 @@
       </c>
       <c r="R116" t="inlineStr">
         <is>
+          <t>[-1.94076850e+03  4.12266356e+06]</t>
+        </is>
+      </c>
+      <c r="S116" t="inlineStr">
+        <is>
           <t>{2021: 200544.976214399, 2022: 198429.64659976307, 2023: 196488.87809868297, 2024: 194548.10959760332, 2025: 192607.34109652322, 2026: 190666.5725954431, 2027: 188725.804094363, 2028: 186785.03559328336, 2029: 184844.26709220326, 2030: 182903.49859112315, 2031: 180962.7300900435, 2032: 179021.9615889634, 2033: 177081.1930878833, 2034: 175140.42458680365, 2035: 173199.65608572355, 2036: 171258.88758464344, 2037: 169318.1190835638, 2038: 167377.3505824837, 2039: 165436.58208140358, 2040: 163495.81358032394, 2041: 161555.04507924384, 2042: 159614.27657816373, 2043: 157673.50807708362, 2044: 155732.73957600398, 2045: 153791.97107492387, 2046: 151851.20257384377, 2047: 149910.43407276412, 2048: 147969.66557168402, 2049: 146028.8970706039, 2050: 144088.12856952427}</t>
         </is>
       </c>
-      <c r="S116" t="n">
+      <c r="T116" t="n">
         <v>4994736.1637771</v>
       </c>
     </row>
@@ -8268,10 +8848,15 @@
       </c>
       <c r="R117" t="inlineStr">
         <is>
+          <t>[-1.0297076e+03  2.1124729e+06]</t>
+        </is>
+      </c>
+      <c r="S117" t="inlineStr">
+        <is>
           <t>{2021: 31187.2362827871, 2022: 30404.135164321866, 2023: 29374.42756361491, 2024: 28344.719962908188, 2025: 27315.012362201232, 2026: 26285.304761494277, 2027: 25255.59716078732, 2028: 24225.8895600806, 2029: 23196.181959373644, 2030: 22166.47435866669, 2031: 21136.766757959733, 2032: 20107.059157252777, 2033: 19077.351556546055, 2034: 18047.6439558391, 2035: 17017.936355132144, 2036: 15988.228754425189, 2037: 14958.521153718233, 2038: 13928.81355301151, 2039: 12899.105952304322, 2040: 11869.3983515976, 2041: 10839.690750890877, 2042: 9809.983150183689, 2043: 8780.275549476966, 2044: 7750.567948770244, 2045: 6720.860348063055, 2046: 5691.152747356333, 2047: 4661.445146649145, 2048: 3631.737545942422, 2049: 2602.0299452356994, 2050: 1572.3223445285112}</t>
         </is>
       </c>
-      <c r="S117" t="n">
+      <c r="T117" t="n">
         <v>478466.0908474616</v>
       </c>
     </row>
@@ -8335,10 +8920,15 @@
       </c>
       <c r="R118" t="inlineStr">
         <is>
+          <t>[-5.68579397e+02  1.17440375e+06]</t>
+        </is>
+      </c>
+      <c r="S118" t="inlineStr">
+        <is>
           <t>{2021: 25252.8960235231, 2022: 24736.205273374682, 2023: 24167.625875891652, 2024: 23599.04647840862, 2025: 23030.46708092559, 2026: 22461.887683442328, 2027: 21893.308285959298, 2028: 21324.728888476267, 2029: 20756.149490993237, 2030: 20187.570093510207, 2031: 19618.990696027176, 2032: 19050.411298543913, 2033: 18481.831901060883, 2034: 17913.252503577853, 2035: 17344.673106094822, 2036: 16776.093708611792, 2037: 16207.514311128762, 2038: 15638.934913645731, 2039: 15070.355516162468, 2040: 14501.776118679438, 2041: 13933.196721196407, 2042: 13364.617323713377, 2043: 12796.037926230347, 2044: 12227.458528747316, 2045: 11658.879131264053, 2046: 11090.299733781023, 2047: 10521.720336297993, 2048: 9953.140938814962, 2049: 9384.561541331932, 2050: 8815.982143848902}</t>
         </is>
       </c>
-      <c r="S118" t="n">
+      <c r="T118" t="n">
         <v>494725.1744895781</v>
       </c>
     </row>
@@ -8402,10 +8992,15 @@
       </c>
       <c r="R119" t="inlineStr">
         <is>
+          <t>[-1.70252598e+03  3.47383292e+06]</t>
+        </is>
+      </c>
+      <c r="S119" t="inlineStr">
+        <is>
           <t>{2021: 35064.8140512671, 2022: 31325.386217971798, 2023: 29622.860235315282, 2024: 27920.334252658766, 2025: 26217.80827000225, 2026: 24515.282287345733, 2027: 22812.756304689217, 2028: 21110.2303220327, 2029: 19407.704339376185, 2030: 17705.17835671967, 2031: 16002.652374063153, 2032: 14300.126391406637, 2033: 12597.60040875012, 2034: 10895.074426093604, 2035: 9192.548443437088, 2036: 7490.022460780572, 2037: 5787.496478124056, 2038: 4084.97049546754, 2039: 2382.4445128110237, 2040: 679.9185301545076, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S119" t="n">
+      <c r="T119" t="n">
         <v>321582.8021328335</v>
       </c>
     </row>
@@ -8469,10 +9064,15 @@
       </c>
       <c r="R120" t="inlineStr">
         <is>
+          <t>[-3.74943073e+03  7.63634432e+06]</t>
+        </is>
+      </c>
+      <c r="S120" t="inlineStr">
+        <is>
           <t>{2021: 61848.1688683312, 2022: 54995.39154841006, 2023: 51245.96082262695, 2024: 47496.53009684384, 2025: 43747.09937106073, 2026: 39997.66864527762, 2027: 36248.23791949451, 2028: 32498.80719371047, 2029: 28749.37646792736, 2030: 24999.94574214425, 2031: 21250.51501636114, 2032: 17501.08429057803, 2033: 13751.65356479492, 2034: 10002.22283901181, 2035: 6252.792113228701, 2036: 2503.3613874455914, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S120" t="n">
+      <c r="T120" t="n">
         <v>462164.7314530816</v>
       </c>
     </row>
@@ -8536,10 +9136,15 @@
       </c>
       <c r="R121" t="inlineStr">
         <is>
+          <t>[-7.21728620e+02  1.47583467e+06]</t>
+        </is>
+      </c>
+      <c r="S121" t="inlineStr">
+        <is>
           <t>{2021: 18018.7501951159, 2022: 16499.39944294491, 2023: 15777.670823313296, 2024: 15055.94220368145, 2025: 14334.213584049838, 2026: 13612.484964418225, 2027: 12890.756344786612, 2028: 12169.027725155, 2029: 11447.299105523387, 2030: 10725.570485891774, 2031: 10003.841866260162, 2032: 9282.113246628549, 2033: 8560.384626996936, 2034: 7838.656007365091, 2035: 7116.927387733478, 2036: 6395.198768101865, 2037: 5673.470148470253, 2038: 4951.74152883864, 2039: 4230.012909207027, 2040: 3508.2842895754147, 2041: 2786.555669943802, 2042: 2064.8270503121894, 2043: 1343.0984306805767, 2044: 621.3698110487312, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S121" t="n">
+      <c r="T121" t="n">
         <v>205898.2215184852</v>
       </c>
     </row>
@@ -8603,10 +9208,15 @@
       </c>
       <c r="R122" t="inlineStr">
         <is>
+          <t>[ 4.96360208e+02 -9.75601962e+05]</t>
+        </is>
+      </c>
+      <c r="S122" t="inlineStr">
+        <is>
           <t>{2021: 28583.0430247821, 2022: 28038.377532879123, 2023: 28534.737740429933, 2024: 29031.097947980743, 2025: 29527.458155531553, 2026: 30023.818363082362, 2027: 30520.178570633172, 2028: 31016.53877818398, 2029: 31512.89898573479, 2030: 32009.2591932856, 2031: 32505.61940083641, 2032: 33001.97960838722, 2033: 33498.33981593803, 2034: 33994.70002348884, 2035: 34491.06023103965, 2036: 34987.42043859046, 2037: 35483.78064614127, 2038: 35980.14085369208, 2039: 36476.50106124277, 2040: 36972.86126879358, 2041: 37469.22147634439, 2042: 37965.5816838952, 2043: 38461.94189144601, 2044: 38958.30209899682, 2045: 39454.66230654763, 2046: 39951.02251409844, 2047: 40447.38272164925, 2048: 40943.74292920006, 2049: 41440.10313675087, 2050: 41936.46334430168}</t>
         </is>
       </c>
-      <c r="S122" t="n">
+      <c r="T122" t="n">
         <v>1007958.482559362</v>
       </c>
     </row>
@@ -8670,10 +9280,15 @@
       </c>
       <c r="R123" t="inlineStr">
         <is>
+          <t>[-3.37243734e+03  6.93442687e+06]</t>
+        </is>
+      </c>
+      <c r="S123" t="inlineStr">
+        <is>
           <t>{2021: 116793.301802271, 2022: 115358.56333628204, 2023: 111986.12599193677, 2024: 108613.68864759244, 2025: 105241.25130324718, 2026: 101868.81395890191, 2027: 98496.37661455758, 2028: 95123.93927021232, 2029: 91751.50192586705, 2030: 88379.06458152179, 2031: 85006.62723717745, 2032: 81634.18989283219, 2033: 78261.75254848693, 2034: 74889.31520414166, 2035: 71516.87785979733, 2036: 68144.44051545206, 2037: 64772.0031711068, 2038: 61399.565826761536, 2039: 58027.1284824172, 2040: 54654.69113807194, 2041: 51282.253793726675, 2042: 47909.81644938141, 2043: 44537.37910503708, 2044: 41164.941760691814, 2045: 37792.50441634655, 2046: 34420.067072001286, 2047: 31047.629727656953, 2048: 27675.19238331169, 2049: 24302.755038966425, 2050: 20930.317694622092}</t>
         </is>
       </c>
-      <c r="S123" t="n">
+      <c r="T123" t="n">
         <v>2024120.267001931</v>
       </c>
     </row>
@@ -8737,10 +9352,15 @@
       </c>
       <c r="R124" t="inlineStr">
         <is>
+          <t>[-1.88078459e+01  8.44701937e+04]</t>
+        </is>
+      </c>
+      <c r="S124" t="inlineStr">
+        <is>
           <t>{2021: 45044.8635477766, 2022: 46440.72932252592, 2023: 46421.9214766393, 2024: 46403.113630752676, 2025: 46384.30578486605, 2026: 46365.497938979424, 2027: 46346.6900930928, 2028: 46327.88224720618, 2029: 46309.07440131955, 2030: 46290.26655543293, 2031: 46271.45870954631, 2032: 46252.650863659685, 2033: 46233.84301777306, 2034: 46215.03517188643, 2035: 46196.22732599981, 2036: 46177.41948011319, 2037: 46158.61163422657, 2038: 46139.80378833994, 2039: 46120.995942453315, 2040: 46102.18809656669, 2041: 46083.38025068007, 2042: 46064.57240479344, 2043: 46045.76455890682, 2044: 46026.9567130202, 2045: 46008.148867133576, 2046: 45989.341021246946, 2047: 45970.533175360324, 2048: 45951.7253294737, 2049: 45932.91748358708, 2050: 45914.10963770046}</t>
         </is>
       </c>
-      <c r="S124" t="n">
+      <c r="T124" t="n">
         <v>1338710.541878321</v>
       </c>
     </row>
@@ -8804,10 +9424,15 @@
       </c>
       <c r="R125" t="inlineStr">
         <is>
+          <t>[-1.99143991e+03  4.09832407e+06]</t>
+        </is>
+      </c>
+      <c r="S125" t="inlineStr">
+        <is>
           <t>{2021: 75179.0501123718, 2022: 71632.5786566753, 2023: 69641.13874990027, 2024: 67649.69884312479, 2025: 65658.25893634977, 2026: 63666.81902957475, 2027: 61675.37912279926, 2028: 59683.93921602424, 2029: 57692.49930924922, 2030: 55701.0594024742, 2031: 53709.61949569872, 2032: 51718.1795889237, 2033: 49726.73968214868, 2034: 47735.299775373656, 2035: 45743.85986859817, 2036: 43752.41996182315, 2037: 41760.98005504813, 2038: 39769.54014827311, 2039: 37778.100241497625, 2040: 35786.660334722605, 2041: 33795.220427947585, 2042: 31803.780521172564, 2043: 29812.34061439708, 2044: 27820.90070762206, 2045: 25829.46080084704, 2046: 23838.02089407202, 2047: 21846.580987296533, 2048: 19855.141080521513, 2049: 17863.701173746493, 2050: 15872.261266971007}</t>
         </is>
       </c>
-      <c r="S125" t="n">
+      <c r="T125" t="n">
         <v>1298473.573315574</v>
       </c>
     </row>
@@ -8871,10 +9496,15 @@
       </c>
       <c r="R126" t="inlineStr">
         <is>
+          <t>[-9.10336037e+03  1.89220976e+07]</t>
+        </is>
+      </c>
+      <c r="S126" t="inlineStr">
+        <is>
           <t>{2021: 534930.625645295, 2022: 515102.9410064779, 2023: 505999.5806408264, 2024: 496896.22027517855, 2025: 487792.8599095307, 2026: 478689.4995438792, 2027: 469586.13917823136, 2028: 460482.77881258354, 2029: 451379.418446932, 2030: 442276.05808128417, 2031: 433172.69771563634, 2032: 424069.3373499848, 2033: 414965.976984337, 2034: 405862.61661868915, 2035: 396759.2562530376, 2036: 387655.8958873898, 2037: 378552.53552174196, 2038: 369449.1751560904, 2039: 360345.8147904426, 2040: 351242.45442479476, 2041: 342139.0940591432, 2042: 333035.7336934954, 2043: 323932.37332784757, 2044: 314829.012962196, 2045: 305725.6525965482, 2046: 296622.2922309004, 2047: 287518.93186524883, 2048: 278415.571499601, 2049: 269312.2111339532, 2050: 260208.85076830164}</t>
         </is>
       </c>
-      <c r="S126" t="n">
+      <c r="T126" t="n">
         <v>11379381.8681728</v>
       </c>
     </row>
@@ -8938,10 +9568,15 @@
       </c>
       <c r="R127" t="inlineStr">
         <is>
+          <t>[-6.18391142e+03  1.26339183e+07]</t>
+        </is>
+      </c>
+      <c r="S127" t="inlineStr">
+        <is>
           <t>{2021: 138928.587827763, 2022: 130049.44578203, 2023: 123865.53436541744, 2024: 117681.62294880673, 2025: 111497.71153219417, 2026: 105313.80011558346, 2027: 99129.88869897276, 2028: 92945.9772823602, 2029: 86762.0658657495, 2030: 80578.15444913879, 2031: 74394.24303252622, 2032: 68210.33161591552, 2033: 62026.42019930482, 2034: 55842.50878269225, 2035: 49658.59736608155, 2036: 43474.685949468985, 2037: 37290.77453285828, 2038: 31106.86311624758, 2039: 24922.951699635014, 2040: 18739.04028302431, 2041: 12555.128866413608, 2042: 6371.217449801043, 2043: 187.3060331903398, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S127" t="n">
+      <c r="T127" t="n">
         <v>1502068.563881294</v>
       </c>
     </row>
@@ -9005,10 +9640,15 @@
       </c>
       <c r="R128" t="inlineStr">
         <is>
+          <t>[-4.11156976e+03  8.37067937e+06]</t>
+        </is>
+      </c>
+      <c r="S128" t="inlineStr">
+        <is>
           <t>{2021: 61431.3880270318, 2022: 57085.317437249236, 2023: 52973.74767869618, 2024: 48862.17792014405, 2025: 44750.60816159099, 2026: 40639.038403037935, 2027: 36527.46864448488, 2028: 32415.89888593182, 2029: 28304.32912737876, 2030: 24192.759368826635, 2031: 20081.189610273577, 2032: 15969.61985172052, 2033: 11858.050093167461, 2034: 7746.480334614404, 2035: 3634.910576062277, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S128" t="n">
+      <c r="T128" t="n">
         <v>455757.2901066946</v>
       </c>
     </row>
@@ -9072,10 +9712,15 @@
       </c>
       <c r="R129" t="inlineStr">
         <is>
+          <t>[-1.87035738e+03  3.80384275e+06]</t>
+        </is>
+      </c>
+      <c r="S129" t="inlineStr">
+        <is>
           <t>{2021: 25568.9786086761, 2022: 21980.12846724037, 2023: 20109.771087557077, 2024: 18239.41370787332, 2025: 16369.056328190025, 2026: 14498.698948506732, 2027: 12628.341568823438, 2028: 10757.984189140145, 2029: 8887.626809456851, 2030: 7017.269429773092, 2031: 5146.912050089799, 2032: 3276.5546704065055, 2033: 1406.197290723212, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S129" t="n">
+      <c r="T129" t="n">
         <v>153102.4438521186</v>
       </c>
     </row>
@@ -9139,10 +9784,15 @@
       </c>
       <c r="R130" t="inlineStr">
         <is>
+          <t>[-2.60370568e+03  5.32947983e+06]</t>
+        </is>
+      </c>
+      <c r="S130" t="inlineStr">
+        <is>
           <t>{2021: 68352.2524712745, 2022: 64786.94272489473, 2023: 62183.237042020075, 2024: 59579.53135914635, 2025: 56975.82567627169, 2026: 54372.119993397035, 2027: 51768.41431052331, 2028: 49164.70862764865, 2029: 46561.002944773994, 2030: 43957.29726189934, 2031: 41353.59157902561, 2032: 38749.885896150954, 2033: 36146.1802132763, 2034: 33542.47453040257, 2035: 30938.768847527914, 2036: 28335.063164653257, 2037: 25731.35748177953, 2038: 23127.651798904873, 2039: 20523.946116030216, 2040: 17920.24043315649, 2041: 15316.534750281833, 2042: 12712.829067407176, 2043: 10109.123384532519, 2044: 7505.417701658793, 2045: 4901.712018784136, 2046: 2298.0063359094784, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S130" t="n">
+      <c r="T130" t="n">
         <v>872737.9894956941</v>
       </c>
     </row>
@@ -9206,10 +9856,15 @@
       </c>
       <c r="R131" t="inlineStr">
         <is>
+          <t>[-4.75598489e+03  9.65712875e+06]</t>
+        </is>
+      </c>
+      <c r="S131" t="inlineStr">
+        <is>
           <t>{2021: 45248.6761688049, 2022: 40527.30157988705, 2023: 35771.316687176004, 2024: 31015.33179446496, 2025: 26259.346901753917, 2026: 21503.362009042874, 2027: 16747.37711633183, 2028: 11991.392223620787, 2029: 7235.407330909744, 2030: 2479.422438200563, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S131" t="n">
+      <c r="T131" t="n">
         <v>216154.5961657902</v>
       </c>
     </row>
@@ -9273,10 +9928,15 @@
       </c>
       <c r="R132" t="inlineStr">
         <is>
+          <t>[ 3.37079064e+04 -6.46038815e+07]</t>
+        </is>
+      </c>
+      <c r="S132" t="inlineStr">
+        <is>
           <t>{2021: 3410027.6165376, 2022: 3553505.1782942116, 2023: 3587213.084647909, 2024: 3620920.991001621, 2025: 3654628.897355318, 2026: 3688336.8037090153, 2027: 3722044.7100627273, 2028: 3755752.6164164245, 2029: 3789460.5227701217, 2030: 3823168.429123834, 2031: 3856876.335477531, 2032: 3890584.241831228, 2033: 3924292.14818494, 2034: 3958000.0545386374, 2035: 3991707.9608923346, 2036: 4025415.8672460467, 2037: 4059123.773599744, 2038: 4092831.679953441, 2039: 4126539.586307153, 2040: 4160247.4926608503, 2041: 4193955.3990145624, 2042: 4227663.30536826, 2043: 4261371.211721957, 2044: 4295079.118075669, 2045: 4328787.024429366, 2046: 4362494.930783063, 2047: 4396202.837136775, 2048: 4429910.743490472, 2049: 4463618.64984417, 2050: 4497326.556197882}</t>
         </is>
       </c>
-      <c r="S132" t="n">
+      <c r="T132" t="n">
         <v>116193410.6803051</v>
       </c>
     </row>
@@ -9340,10 +10000,15 @@
       </c>
       <c r="R133" t="inlineStr">
         <is>
+          <t>[-7.25730549e+03  1.48067093e+07]</t>
+        </is>
+      </c>
+      <c r="S133" t="inlineStr">
+        <is>
           <t>{2021: 138840.37075476, 2022: 132437.60999295302, 2023: 125180.30450269766, 2024: 117922.99901244417, 2025: 110665.69352219068, 2026: 103408.38803193532, 2027: 96151.08254168183, 2028: 88893.77705142833, 2029: 81636.47156117484, 2030: 74379.16607091948, 2031: 67121.86058066599, 2032: 59864.5550904125, 2033: 52607.24960015714, 2034: 45349.94410990365, 2035: 38092.638619650155, 2036: 30835.333129396662, 2037: 23578.027639141306, 2038: 16320.722148887813, 2039: 9063.41665863432, 2040: 1806.111168378964, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S133" t="n">
+      <c r="T133" t="n">
         <v>1344735.536410034</v>
       </c>
     </row>
@@ -9407,10 +10072,15 @@
       </c>
       <c r="R134" t="inlineStr">
         <is>
+          <t>[-2.08758971e+03  4.27372678e+06]</t>
+        </is>
+      </c>
+      <c r="S134" t="inlineStr">
+        <is>
           <t>{2021: 53014.7113861568, 2022: 52620.389775073156, 2023: 50532.800064861774, 2024: 48445.210354651324, 2025: 46357.620644440874, 2026: 44270.03093422949, 2027: 42182.44122401904, 2028: 40094.85151380859, 2029: 38007.26180359721, 2030: 35919.67209338676, 2031: 33832.08238317631, 2032: 31744.49267296493, 2033: 29656.90296275448, 2034: 27569.31325254403, 2035: 25481.72354233265, 2036: 23394.1338321222, 2037: 21306.54412191175, 2038: 19218.954411700368, 2039: 17131.364701489918, 2040: 15043.774991279468, 2041: 12956.185281068087, 2042: 10868.595570857637, 2043: 8781.005860647187, 2044: 6693.416150435805, 2045: 4605.826440225355, 2046: 2518.2367300149053, 2047: 430.647019803524, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S134" t="n">
+      <c r="T134" t="n">
         <v>716170.8340264752</v>
       </c>
     </row>
@@ -9474,10 +10144,15 @@
       </c>
       <c r="R135" t="inlineStr">
         <is>
+          <t>[-4.92676132e+04  1.01025429e+08]</t>
+        </is>
+      </c>
+      <c r="S135" t="inlineStr">
+        <is>
           <t>{2021: 1743973.00699289, 2022: 1406315.31029962, 2023: 1357047.6970992386, 2024: 1307780.0838988721, 2025: 1258512.4706985056, 2026: 1209244.8574981242, 2027: 1159977.2442977577, 2028: 1110709.6310973763, 2029: 1061442.0178970098, 2030: 1012174.4046966434, 2031: 962906.791496262, 2032: 913639.1782958955, 2033: 864371.5650955141, 2034: 815103.9518951476, 2035: 765836.3386947662, 2036: 716568.7254943997, 2037: 667301.1122940332, 2038: 618033.4990936518, 2039: 568765.8858932853, 2040: 519498.2726929039, 2041: 470230.6594925374, 2042: 420963.0462921709, 2043: 371695.4330917895, 2044: 322427.819891423, 2045: 273160.2066910416, 2046: 223892.5934906751, 2047: 174624.9802902937, 2048: 125357.3670899272, 2049: 76089.7538895607, 2050: 26822.1406891793}</t>
         </is>
       </c>
-      <c r="S135" t="n">
+      <c r="T135" t="n">
         <v>21639068.47248946</v>
       </c>
     </row>
@@ -9541,10 +10216,15 @@
       </c>
       <c r="R136" t="inlineStr">
         <is>
+          <t>[-6.78173466e+04  1.37666273e+08]</t>
+        </is>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
           <t>{2021: 670375.543352161, 2022: 539598.1808344126, 2023: 471780.83422094584, 2024: 403963.4876074791, 2025: 336146.14099398255, 2026: 268328.7943805158, 2027: 200511.44776704907, 2028: 132694.10115358233, 2029: 64876.754540115595, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S136" t="n">
+      <c r="T136" t="n">
         <v>2753087.513174163</v>
       </c>
     </row>
@@ -9608,10 +10288,15 @@
       </c>
       <c r="R137" t="inlineStr">
         <is>
+          <t>[-2.40899720e+03  4.90471283e+06]</t>
+        </is>
+      </c>
+      <c r="S137" t="inlineStr">
+        <is>
           <t>{2021: 38990.1000466931, 2022: 33720.49754332006, 2023: 31311.50034698751, 2024: 28902.503150655888, 2025: 26493.505954324268, 2026: 24084.508757992648, 2027: 21675.511561660096, 2028: 19266.514365328476, 2029: 16857.517168996856, 2030: 14448.519972665235, 2031: 12039.522776332684, 2032: 9630.525580001064, 2033: 7221.528383669443, 2034: 4812.531187337823, 2035: 2403.5339910052717, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S137" t="n">
+      <c r="T137" t="n">
         <v>272363.2707636239</v>
       </c>
     </row>
@@ -9675,10 +10360,15 @@
       </c>
       <c r="R138" t="inlineStr">
         <is>
+          <t>[-2.08383080e+02  4.31007342e+05]</t>
+        </is>
+      </c>
+      <c r="S138" t="inlineStr">
+        <is>
           <t>{2021: 9691.38713817754, 2022: 9656.753873407608, 2023: 9448.37079324678, 2024: 9239.987713085953, 2025: 9031.604632925068, 2026: 8823.22155276424, 2027: 8614.838472603413, 2028: 8406.455392442585, 2029: 8198.072312281758, 2030: 7989.6892321208725, 2031: 7781.306151960045, 2032: 7572.923071799218, 2033: 7364.53999163839, 2034: 7156.156911477505, 2035: 6947.773831316677, 2036: 6739.39075115585, 2037: 6531.007670995023, 2038: 6322.624590834137, 2039: 6114.24151067331, 2040: 5905.858430512482, 2041: 5697.475350351655, 2042: 5489.092270190769, 2043: 5280.709190029942, 2044: 5072.326109869115, 2045: 4863.943029708287, 2046: 4655.559949547402, 2047: 4447.176869386574, 2048: 4238.793789225747, 2049: 4030.4107090649195, 2050: 3822.027628904092}</t>
         </is>
       </c>
-      <c r="S138" t="n">
+      <c r="T138" t="n">
         <v>198377.0115381561</v>
       </c>
     </row>
@@ -9742,10 +10432,15 @@
       </c>
       <c r="R139" t="inlineStr">
         <is>
+          <t>[-2.30997711e+03  4.75246506e+06]</t>
+        </is>
+      </c>
+      <c r="S139" t="inlineStr">
+        <is>
           <t>{2021: 84355.9376558259, 2022: 81691.34000113048, 2023: 79381.36288961861, 2024: 77071.38577810768, 2025: 74761.40866659582, 2026: 72451.43155508395, 2027: 70141.45444357302, 2028: 67831.47733206116, 2029: 65521.50022054929, 2030: 63211.52310903743, 2031: 60901.5459975265, 2032: 58591.56888601463, 2033: 56281.59177450277, 2034: 53971.61466299184, 2035: 51661.63755147997, 2036: 49351.66043996811, 2037: 47041.68332845718, 2038: 44731.70621694531, 2039: 42421.72910543345, 2040: 40111.75199392252, 2041: 37801.77488241065, 2042: 35491.79777089879, 2043: 33181.820659386925, 2044: 30871.843547875993, 2045: 28561.86643636413, 2046: 26251.889324852265, 2047: 23941.912213341333, 2048: 21631.93510182947, 2049: 19321.957990317605, 2050: 17011.980878806673}</t>
         </is>
       </c>
-      <c r="S139" t="n">
+      <c r="T139" t="n">
         <v>1464870.131147593</v>
       </c>
     </row>
@@ -9809,10 +10504,15 @@
       </c>
       <c r="R140" t="inlineStr">
         <is>
+          <t>[-2.18230613e+03  4.47693502e+06]</t>
+        </is>
+      </c>
+      <c r="S140" t="inlineStr">
+        <is>
           <t>{2021: 67266.4918853514, 2022: 64312.02968478203, 2023: 62129.723555357195, 2024: 59947.41742593236, 2025: 57765.11129650753, 2026: 55582.8051670827, 2027: 53400.499037657864, 2028: 51218.19290823396, 2029: 49035.88677880913, 2030: 46853.5806493843, 2031: 44671.274519959465, 2032: 42488.96839053463, 2033: 40306.6622611098, 2034: 38124.3561316859, 2035: 35942.050002261065, 2036: 33759.74387283623, 2037: 31577.4377434114, 2038: 29395.131613986567, 2039: 27212.825484561734, 2040: 25030.519355137832, 2041: 22848.213225713, 2042: 20665.907096288167, 2043: 18483.600966863334, 2044: 16301.294837438501, 2045: 14118.988708013669, 2046: 11936.682578589767, 2047: 9754.376449164934, 2048: 7572.070319740102, 2049: 5389.764190315269, 2050: 3207.458060890436}</t>
         </is>
       </c>
-      <c r="S140" t="n">
+      <c r="T140" t="n">
         <v>1011062.089224479</v>
       </c>
     </row>
@@ -9876,10 +10576,15 @@
       </c>
       <c r="R141" t="inlineStr">
         <is>
+          <t>[-1.52791144e+03  3.14180357e+06]</t>
+        </is>
+      </c>
+      <c r="S141" t="inlineStr">
+        <is>
           <t>{2021: 53982.9166032395, 2022: 52366.64851130545, 2023: 50838.737074654084, 2024: 49310.825638002716, 2025: 47782.914201351814, 2026: 46255.002764700446, 2027: 44727.09132804908, 2028: 43199.17989139771, 2029: 41671.26845474634, 2030: 40143.357018094976, 2031: 38615.44558144361, 2032: 37087.534144792706, 2033: 35559.62270814134, 2034: 34031.71127148997, 2035: 32503.799834838603, 2036: 30975.888398187235, 2037: 29447.976961535867, 2038: 27920.065524884965, 2039: 26392.154088233598, 2040: 24864.24265158223, 2041: 23336.331214930862, 2042: 21808.419778279494, 2043: 20280.508341628127, 2044: 18752.59690497676, 2045: 17224.685468325857, 2046: 15696.77403167449, 2047: 14168.862595023122, 2048: 12640.951158371754, 2049: 11113.039721720386, 2050: 9585.128285069019}</t>
         </is>
       </c>
-      <c r="S141" t="n">
+      <c r="T141" t="n">
         <v>920499.6577065178</v>
       </c>
     </row>
@@ -9943,10 +10648,15 @@
       </c>
       <c r="R142" t="inlineStr">
         <is>
+          <t>[-9.68883095e+02  1.98505840e+06]</t>
+        </is>
+      </c>
+      <c r="S142" t="inlineStr">
+        <is>
           <t>{2021: 27478.4286960322, 2022: 25976.78196628089, 2023: 25007.89887116989, 2024: 24039.01577605889, 2025: 23070.132680947892, 2026: 22101.249585836893, 2027: 21132.366490725894, 2028: 20163.483395614894, 2029: 19194.600300503895, 2030: 18225.717205393128, 2031: 17256.83411028213, 2032: 16287.95101517113, 2033: 15319.06792006013, 2034: 14350.18482494913, 2035: 13381.301729838131, 2036: 12412.418634727132, 2037: 11443.535539616132, 2038: 10474.652444505133, 2039: 9505.769349394133, 2040: 8536.886254283134, 2041: 7568.0031591721345, 2042: 6599.120064061368, 2043: 5630.2369689503685, 2044: 4661.353873839369, 2045: 3692.4707787283696, 2046: 2723.58768361737, 2047: 1754.7045885063708, 2048: 785.8214933953714, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S142" t="n">
+      <c r="T142" t="n">
         <v>375034.3610536454</v>
       </c>
     </row>
@@ -10010,10 +10720,15 @@
       </c>
       <c r="R143" t="inlineStr">
         <is>
+          <t>[-2.99801617e+03  6.15433294e+06]</t>
+        </is>
+      </c>
+      <c r="S143" t="inlineStr">
+        <is>
           <t>{2021: 96057.566686439, 2022: 92344.25144417211, 2023: 89346.23527793027, 2024: 86348.21911168844, 2025: 83350.2029454466, 2026: 80352.18677920476, 2027: 77354.17061296292, 2028: 74356.15444672108, 2029: 71358.1382804783, 2030: 68360.12211423647, 2031: 65362.10594799463, 2032: 62364.08978175279, 2033: 59366.07361551095, 2034: 56368.05744926911, 2035: 53370.04128302727, 2036: 50372.02511678543, 2037: 47374.00895054359, 2038: 44375.99278430175, 2039: 41377.97661805991, 2040: 38379.96045181807, 2041: 35381.94428557623, 2042: 32383.928119334392, 2043: 29385.911953092553, 2044: 26387.895786850713, 2045: 23389.879620608874, 2046: 20391.863454367034, 2047: 17393.847288125195, 2048: 14395.831121883355, 2049: 11397.814955641516, 2050: 8399.798789399676}</t>
         </is>
       </c>
-      <c r="S143" t="n">
+      <c r="T143" t="n">
         <v>1504617.612335304</v>
       </c>
     </row>
@@ -10077,10 +10792,15 @@
       </c>
       <c r="R144" t="inlineStr">
         <is>
+          <t>[-2.65989835e+03  5.43318833e+06]</t>
+        </is>
+      </c>
+      <c r="S144" t="inlineStr">
+        <is>
           <t>{2021: 58397.5072941933, 2022: 54873.87793009728, 2023: 52213.979584635235, 2024: 49554.08123917319, 2025: 46894.18289371114, 2026: 44234.284548249096, 2027: 41574.38620278705, 2028: 38914.487857325, 2029: 36254.589511862956, 2030: 33594.69116640091, 2031: 30934.792820938863, 2032: 28274.894475476816, 2033: 25614.99613001477, 2034: 22955.097784552723, 2035: 20295.199439090677, 2036: 17635.30109362863, 2037: 14975.402748166583, 2038: 12315.504402704537, 2039: 9655.60605724249, 2040: 6995.707711780444, 2041: 4335.809366318397, 2042: 1675.9110208563507, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S144" t="n">
+      <c r="T144" t="n">
         <v>622971.5376321098</v>
       </c>
     </row>
@@ -10144,10 +10864,15 @@
       </c>
       <c r="R145" t="inlineStr">
         <is>
+          <t>[-3.5362948e+03  7.2186395e+06]</t>
+        </is>
+      </c>
+      <c r="S145" t="inlineStr">
+        <is>
           <t>{2021: 74871.3006511838, 2022: 68251.4099735422, 2023: 64715.11517315172, 2024: 61178.82037276216, 2025: 57642.5255723726, 2026: 54106.23077198211, 2027: 50569.93597159255, 2028: 47033.641171202995, 2029: 43497.346370812505, 2030: 39961.05157042295, 2031: 36424.75677003339, 2032: 32888.4619696429, 2033: 29352.167169253342, 2034: 25815.872368863784, 2035: 22279.577568473294, 2036: 18743.282768083736, 2037: 15206.987967694178, 2038: 11670.693167303689, 2039: 8134.398366914131, 2040: 4598.103566524573, 2041: 1061.8087661340833, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S145" t="n">
+      <c r="T145" t="n">
         <v>730567.8377223548</v>
       </c>
     </row>
@@ -10211,10 +10936,15 @@
       </c>
       <c r="R146" t="inlineStr">
         <is>
+          <t>[-3.77841228e+02  7.79359205e+05]</t>
+        </is>
+      </c>
+      <c r="S146" t="inlineStr">
+        <is>
           <t>{2021: 15721.0330251436, 2022: 15364.241592120961, 2023: 14986.400364014204, 2024: 14608.559135907446, 2025: 14230.717907800688, 2026: 13852.87667969393, 2027: 13475.035451587173, 2028: 13097.194223480416, 2029: 12719.352995373658, 2030: 12341.5117672669, 2031: 11963.670539160143, 2032: 11585.829311053385, 2033: 11207.988082946744, 2034: 10830.146854839986, 2035: 10452.305626733229, 2036: 10074.464398626471, 2037: 9696.623170519713, 2038: 9318.781942412956, 2039: 8940.940714306198, 2040: 8563.09948619944, 2041: 8185.258258092683, 2042: 7807.417029985925, 2043: 7429.575801879168, 2044: 7051.73457377241, 2045: 6673.893345665652, 2046: 6296.052117558895, 2047: 5918.210889452137, 2048: 5540.369661345379, 2049: 5162.528433238622, 2050: 4784.687205131864}</t>
         </is>
       </c>
-      <c r="S146" t="n">
+      <c r="T146" t="n">
         <v>297627.6404701723</v>
       </c>
     </row>
@@ -10278,10 +11008,15 @@
       </c>
       <c r="R147" t="inlineStr">
         <is>
+          <t>[ 3.53607129e+02 -6.28032736e+05]</t>
+        </is>
+      </c>
+      <c r="S147" t="inlineStr">
+        <is>
           <t>{2021: 77022.5277997303, 2022: 86960.87805970327, 2023: 87314.48518824019, 2024: 87668.09231677698, 2025: 88021.69944531389, 2026: 88375.30657385068, 2027: 88728.9137023876, 2028: 89082.52083092439, 2029: 89436.1279594613, 2030: 89789.7350879981, 2031: 90143.342216535, 2032: 90496.9493450718, 2033: 90850.55647360871, 2034: 91204.1636021455, 2035: 91557.77073068242, 2036: 91911.37785921921, 2037: 92264.98498775612, 2038: 92618.59211629292, 2039: 92972.19924482983, 2040: 93325.80637336662, 2041: 93679.41350190353, 2042: 94033.02063044033, 2043: 94386.62775897724, 2044: 94740.23488751403, 2045: 95093.84201605094, 2046: 95447.44914458774, 2047: 95801.05627312465, 2048: 96154.66340166144, 2049: 96508.27053019824, 2050: 96861.87765873515}</t>
         </is>
       </c>
-      <c r="S147" t="n">
+      <c r="T147" t="n">
         <v>2655510.282987855</v>
       </c>
     </row>
@@ -10345,10 +11080,15 @@
       </c>
       <c r="R148" t="inlineStr">
         <is>
+          <t>[-3.76458140e+02  7.67115221e+05]</t>
+        </is>
+      </c>
+      <c r="S148" t="inlineStr">
+        <is>
           <t>{2021: 6579.59905935159, 2022: 5916.860855815234, 2023: 5540.402715367847, 2024: 5163.944574920577, 2025: 4787.486434473307, 2026: 4411.02829402592, 2027: 4034.57015357865, 2028: 3658.11201313138, 2029: 3281.6538726839935, 2030: 2905.1957322367234, 2031: 2528.7375917894533, 2032: 2152.2794513420667, 2033: 1775.8213108947966, 2034: 1399.3631704475265, 2035: 1022.90503000014, 2036: 646.4468895528698, 2037: 269.9887491055997, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S148" t="n">
+      <c r="T148" t="n">
         <v>52784.59636904188</v>
       </c>
     </row>
@@ -10412,10 +11152,15 @@
       </c>
       <c r="R149" t="inlineStr">
         <is>
+          <t>[-6.30622287e+03  1.28760521e+07]</t>
+        </is>
+      </c>
+      <c r="S149" t="inlineStr">
+        <is>
           <t>{2021: 135435.135194512, 2022: 124869.41999418102, 2023: 118563.19712628424, 2024: 112256.97425838746, 2025: 105950.75139049068, 2026: 99644.52852259576, 2027: 93338.30565469898, 2028: 87032.0827868022, 2029: 80725.85991890728, 2030: 74419.6370510105, 2031: 68113.41418311372, 2032: 61807.19131521694, 2033: 55500.968447322026, 2034: 49194.745579425246, 2035: 42888.522711528465, 2036: 36582.29984363355, 2037: 30276.076975736767, 2038: 23969.854107839987, 2039: 17663.631239943206, 2040: 11357.408372048289, 2041: 5051.185504151508, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S149" t="n">
+      <c r="T149" t="n">
         <v>1366923.622580574</v>
       </c>
     </row>
@@ -10479,10 +11224,15 @@
       </c>
       <c r="R150" t="inlineStr">
         <is>
+          <t>[-3.07417660e+03  6.26135702e+06]</t>
+        </is>
+      </c>
+      <c r="S150" t="inlineStr">
+        <is>
           <t>{2021: 49623.5862728977, 2022: 45371.93333962001, 2023: 42297.75673761405, 2024: 39223.58013560809, 2025: 36149.40353360213, 2026: 33075.226931596175, 2027: 30001.050329591148, 2028: 26926.87372758519, 2029: 23852.69712557923, 2030: 20778.520523573272, 2031: 17704.343921567313, 2032: 14630.167319561355, 2033: 11555.990717555396, 2034: 8481.814115549438, 2035: 5407.6375135444105, 2036: 2333.460911538452, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S150" t="n">
+      <c r="T150" t="n">
         <v>382602.2500201345</v>
       </c>
     </row>
@@ -10546,10 +11296,15 @@
       </c>
       <c r="R151" t="inlineStr">
         <is>
+          <t>[-3.90951064e+02  8.31146522e+05]</t>
+        </is>
+      </c>
+      <c r="S151" t="inlineStr">
+        <is>
           <t>{2021: 41166.6984468059, 2022: 40643.47096043837, 2023: 40252.51989679551, 2024: 39861.56883315253, 2025: 39470.61776950967, 2026: 39079.66670586669, 2027: 38688.71564222383, 2028: 38297.764578580856, 2029: 37906.813514937996, 2030: 37515.86245129502, 2031: 37124.91138765216, 2032: 36733.96032400918, 2033: 36343.00926036632, 2034: 35952.058196723345, 2035: 35561.107133080484, 2036: 35170.15606943751, 2037: 34779.20500579465, 2038: 34388.25394215167, 2039: 33997.30287850881, 2040: 33606.35181486583, 2041: 33215.40075122297, 2042: 32824.449687579996, 2043: 32433.498623937136, 2044: 32042.54756029416, 2045: 31651.5964966513, 2046: 31260.64543300832, 2047: 30869.69436936546, 2048: 30478.743305722484, 2049: 30087.792242079508, 2050: 29696.841178436647}</t>
         </is>
       </c>
-      <c r="S151" t="n">
+      <c r="T151" t="n">
         <v>1025669.454647873</v>
       </c>
     </row>
@@ -10613,10 +11368,15 @@
       </c>
       <c r="R152" t="inlineStr">
         <is>
+          <t>[-2.06103910e+03  4.25547667e+06]</t>
+        </is>
+      </c>
+      <c r="S152" t="inlineStr">
+        <is>
           <t>{2021: 89603.7420854587, 2022: 88055.60655205604, 2023: 85994.56744903699, 2024: 83933.5283460184, 2025: 81872.48924299935, 2026: 79811.45013998076, 2027: 77750.41103696171, 2028: 75689.37193394313, 2029: 73628.33283092408, 2030: 71567.29372790502, 2031: 69506.25462488644, 2032: 67445.21552186739, 2033: 65384.1764188488, 2034: 63323.13731582975, 2035: 61262.098212811165, 2036: 59201.05910979211, 2037: 57140.02000677306, 2038: 55078.98090375494, 2039: 53017.94180073589, 2040: 50956.90269771684, 2041: 48895.86359469779, 2042: 46834.82449167967, 2043: 44773.78538866062, 2044: 42712.746285641566, 2045: 40651.707182622515, 2046: 38590.668079604395, 2047: 36529.62897658534, 2048: 34468.58987356629, 2049: 32407.55077054724, 2050: 30346.51166752819}</t>
         </is>
       </c>
-      <c r="S152" t="n">
+      <c r="T152" t="n">
         <v>1746459.329392941</v>
       </c>
     </row>
@@ -10680,10 +11440,15 @@
       </c>
       <c r="R153" t="inlineStr">
         <is>
+          <t>[-1.12658769e+03  2.29654750e+06]</t>
+        </is>
+      </c>
+      <c r="S153" t="inlineStr">
+        <is>
           <t>{2021: 20293.7181386378, 2022: 18587.19970992254, 2023: 17460.61202347465, 2024: 16334.02433702629, 2025: 15207.436650578398, 2026: 14080.848964130506, 2027: 12954.261277682614, 2028: 11827.673591234256, 2029: 10701.085904786363, 2030: 9574.49821833847, 2031: 8447.910531890579, 2032: 7321.322845442221, 2033: 6194.735158994328, 2034: 5068.147472546436, 2035: 3941.559786098078, 2036: 2814.9720996501856, 2037: 1688.3844132022932, 2038: 561.7967267544009, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S153" t="n">
+      <c r="T153" t="n">
         <v>172913.3287810715</v>
       </c>
     </row>
@@ -10747,10 +11512,15 @@
       </c>
       <c r="R154" t="inlineStr">
         <is>
+          <t>[-7.86904811e+02  1.60535983e+06]</t>
+        </is>
+      </c>
+      <c r="S154" t="inlineStr">
+        <is>
           <t>{2021: 15596.1794677321, 2022: 14238.2978310443, 2023: 13451.393019699259, 2024: 12664.488208354218, 2025: 11877.58339700941, 2026: 11090.67858566437, 2027: 10303.773774319561, 2028: 9516.86896297452, 2029: 8729.964151629712, 2030: 7943.059340284672, 2031: 7156.154528939864, 2032: 6369.249717594823, 2033: 5582.344906249782, 2034: 4795.440094904974, 2035: 4008.5352835599333, 2036: 3221.6304722151253, 2037: 2434.7256608700845, 2038: 1647.8208495252766, 2039: 860.9160381802358, 2040: 74.01122683519498, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S154" t="n">
+      <c r="T154" t="n">
         <v>143765.0257837214</v>
       </c>
     </row>
@@ -10814,10 +11584,15 @@
       </c>
       <c r="R155" t="inlineStr">
         <is>
+          <t>[-1.99667659e+03  4.07366455e+06]</t>
+        </is>
+      </c>
+      <c r="S155" t="inlineStr">
+        <is>
           <t>{2021: 39224.6787840837, 2022: 36384.49622808257, 2023: 34387.81964153238, 2024: 32391.14305498218, 2025: 30394.466468431987, 2026: 28397.789881881792, 2027: 26401.113295332063, 2028: 24404.43670878187, 2029: 22407.760122231673, 2030: 20411.08353568148, 2031: 18414.40694913175, 2032: 16417.730362581555, 2033: 14421.05377603136, 2034: 12424.377189481165, 2035: 10427.70060293097, 2036: 8431.024016381241, 2037: 6434.347429831047, 2038: 4437.670843280852, 2039: 2440.994256730657, 2040: 444.3176701804623, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S155" t="n">
+      <c r="T155" t="n">
         <v>369486.0714255409</v>
       </c>
     </row>
@@ -10881,10 +11656,15 @@
       </c>
       <c r="R156" t="inlineStr">
         <is>
+          <t>[-5.03128941e+02  1.05202482e+06]</t>
+        </is>
+      </c>
+      <c r="S156" t="inlineStr">
+        <is>
           <t>{2021: 33896.0681128131, 2022: 34698.09880006558, 2023: 34194.96985922323, 2024: 33691.84091838088, 2025: 33188.711977538536, 2026: 32685.583036696073, 2027: 32182.454095853725, 2028: 31679.32515501138, 2029: 31176.19621416903, 2030: 30673.067273326684, 2031: 30169.93833248422, 2032: 29666.809391641873, 2033: 29163.680450799526, 2034: 28660.55150995718, 2035: 28157.42256911483, 2036: 27654.293628272368, 2037: 27151.16468743002, 2038: 26648.035746587673, 2039: 26144.906805745326, 2040: 25641.77786490298, 2041: 25138.648924060515, 2042: 24635.519983218168, 2043: 24132.39104237582, 2044: 23629.262101533473, 2045: 23126.133160691126, 2046: 22623.004219848663, 2047: 22119.875279006315, 2048: 21616.746338163968, 2049: 21113.61739732162, 2050: 20610.488456479274}</t>
         </is>
       </c>
-      <c r="S156" t="n">
+      <c r="T156" t="n">
         <v>808617.3050480669</v>
       </c>
     </row>
@@ -10948,10 +11728,15 @@
       </c>
       <c r="R157" t="inlineStr">
         <is>
+          <t>[-8.89777111e+03  1.85140662e+07]</t>
+        </is>
+      </c>
+      <c r="S157" t="inlineStr">
+        <is>
           <t>{2021: 543303.129520453, 2022: 522772.98167590424, 2023: 513875.21056812257, 2024: 504977.43946033716, 2025: 496079.66835255176, 2026: 487181.8972447701, 2027: 478284.1261369847, 2028: 469386.355029203, 2029: 460488.5839214176, 2030: 451590.8128136322, 2031: 442693.0417058505, 2032: 433795.2705980651, 2033: 424897.4994902797, 2034: 415999.728382498, 2035: 407101.9572747126, 2036: 398204.18616693094, 2037: 389306.41505914554, 2038: 380408.64395136014, 2039: 371510.87284357846, 2040: 362613.10173579305, 2041: 353715.33062800765, 2042: 344817.559520226, 2043: 335919.78841244057, 2044: 327022.0173046589, 2045: 318124.2461968735, 2046: 309226.4750890881, 2047: 300328.7039813064, 2048: 291430.932873521, 2049: 282533.1617657356, 2050: 273635.3906579539}</t>
         </is>
       </c>
-      <c r="S157" t="n">
+      <c r="T157" t="n">
         <v>11682755.2682722</v>
       </c>
     </row>
@@ -11015,10 +11800,15 @@
       </c>
       <c r="R158" t="inlineStr">
         <is>
+          <t>[-4.58006464e+03  9.40657474e+06]</t>
+        </is>
+      </c>
+      <c r="S158" t="inlineStr">
+        <is>
           <t>{2021: 152121.872219682, 2022: 145684.03787789308, 2023: 141103.97323600948, 2024: 136523.90859412774, 2025: 131943.84395224415, 2026: 127363.77931036055, 2027: 122783.71466847695, 2028: 118203.65002659336, 2029: 113623.58538470976, 2030: 109043.52074282616, 2031: 104463.45610094257, 2032: 99883.39145905897, 2033: 95303.32681717537, 2034: 90723.26217529178, 2035: 86143.19753340818, 2036: 81563.13289152458, 2037: 76983.06824964099, 2038: 72403.00360775739, 2039: 67822.9389658738, 2040: 63242.87432399206, 2041: 58662.80968210846, 2042: 54082.745040224865, 2043: 49502.68039834127, 2044: 44922.61575645767, 2045: 40342.551114574075, 2046: 35762.48647269048, 2047: 31182.42183080688, 2048: 26602.357188923284, 2049: 22022.292547039688, 2050: 17442.22790515609}</t>
         </is>
       </c>
-      <c r="S158" t="n">
+      <c r="T158" t="n">
         <v>2432670.676011492</v>
       </c>
     </row>
@@ -11082,10 +11872,15 @@
       </c>
       <c r="R159" t="inlineStr">
         <is>
+          <t>[-9.89011407e+02  2.01372271e+06]</t>
+        </is>
+      </c>
+      <c r="S159" t="inlineStr">
+        <is>
           <t>{2021: 15373.6263462622, 2022: 13941.64697230095, 2023: 12952.635565133998, 2024: 11963.624157967279, 2025: 10974.61275080056, 2026: 9985.60134363384, 2027: 8996.589936466888, 2028: 8007.578529300168, 2029: 7018.567122133449, 2030: 6029.555714966729, 2031: 5040.544307799777, 2032: 4051.5329006330576, 2033: 3062.521493466338, 2034: 2073.5100862996187, 2035: 1084.4986791326664, 2036: 95.487271965947, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S159" t="n">
+      <c r="T159" t="n">
         <v>112965.3200051324</v>
       </c>
     </row>
@@ -11149,10 +11944,15 @@
       </c>
       <c r="R160" t="inlineStr">
         <is>
+          <t>[ 5.50765188e+02 -1.04534055e+06]</t>
+        </is>
+      </c>
+      <c r="S160" t="inlineStr">
+        <is>
           <t>{2021: 69235.9040374478, 2022: 68306.6654896239, 2023: 68857.43067811907, 2024: 69408.19586661423, 2025: 69958.9610551094, 2026: 70509.72624360432, 2027: 71060.49143209949, 2028: 71611.25662059465, 2029: 72162.02180908981, 2030: 72712.78699758498, 2031: 73263.55218608014, 2032: 73814.3173745753, 2033: 74365.08256307046, 2034: 74915.84775156563, 2035: 75466.61294006079, 2036: 76017.37812855595, 2037: 76568.14331705112, 2038: 77118.90850554628, 2039: 77669.67369404144, 2040: 78220.4388825366, 2041: 78771.20407103177, 2042: 79321.96925952693, 2043: 79872.73444802209, 2044: 80423.49963651726, 2045: 80974.26482501242, 2046: 81525.03001350758, 2047: 82075.79520200274, 2048: 82626.5603904979, 2049: 83177.32557899307, 2050: 83728.09076748823}</t>
         </is>
       </c>
-      <c r="S160" t="n">
+      <c r="T160" t="n">
         <v>2197257.872363103</v>
       </c>
     </row>
@@ -11216,10 +12016,15 @@
       </c>
       <c r="R161" t="inlineStr">
         <is>
+          <t>[-1.14590069e+03  2.35443865e+06]</t>
+        </is>
+      </c>
+      <c r="S161" t="inlineStr">
+        <is>
           <t>{2021: 38141.8121612654, 2022: 37427.45519132633, 2023: 36281.55449908879, 2024: 35135.653806851245, 2025: 33989.75311461417, 2026: 32843.85242237663, 2027: 31697.951730139088, 2028: 30552.051037901547, 2029: 29406.150345664006, 2030: 28260.24965342693, 2031: 27114.34896118939, 2032: 25968.448268951848, 2033: 24822.547576714307, 2034: 23676.646884476766, 2035: 22530.746192239225, 2036: 21384.84550000215, 2037: 20238.94480776461, 2038: 19093.044115527067, 2039: 17947.143423289526, 2040: 16801.242731051985, 2041: 15655.34203881491, 2042: 14509.441346577369, 2043: 13363.540654339828, 2044: 12217.639962102287, 2045: 11071.739269864745, 2046: 9925.83857762767, 2047: 8779.937885390129, 2048: 7634.037193152588, 2049: 6488.136500915047, 2050: 5342.235808677506}</t>
         </is>
       </c>
-      <c r="S161" t="n">
+      <c r="T161" t="n">
         <v>636560.3076763516</v>
       </c>
     </row>
@@ -11283,10 +12088,15 @@
       </c>
       <c r="R162" t="inlineStr">
         <is>
+          <t>[-4.01605845e+03  8.33007224e+06]</t>
+        </is>
+      </c>
+      <c r="S162" t="inlineStr">
+        <is>
           <t>{2021: 213705.500467378, 2022: 209602.0461340025, 2023: 205585.987681441, 2024: 201569.92922887858, 2025: 197553.87077631708, 2026: 193537.81232375465, 2027: 189521.75387119316, 2028: 185505.69541863073, 2029: 181489.63696606923, 2030: 177473.57851350773, 2031: 173457.5200609453, 2032: 169441.4616083838, 2033: 165425.40315582138, 2034: 161409.34470325988, 2035: 157393.28625069745, 2036: 153377.22779813595, 2037: 149361.16934557352, 2038: 145345.11089301202, 2039: 141329.0524404496, 2040: 137312.9939878881, 2041: 133296.93553532567, 2042: 129280.87708276417, 2043: 125264.81863020174, 2044: 121248.76017764024, 2045: 117232.70172507782, 2046: 113216.64327251632, 2047: 109200.58481995389, 2048: 105184.52636739239, 2049: 101168.4679148309, 2050: 97152.40946226846}</t>
         </is>
       </c>
-      <c r="S162" t="n">
+      <c r="T162" t="n">
         <v>4506216.151648488</v>
       </c>
     </row>
@@ -11350,10 +12160,15 @@
       </c>
       <c r="R163" t="inlineStr">
         <is>
+          <t>[-9.55747973e+03  1.95077426e+07]</t>
+        </is>
+      </c>
+      <c r="S163" t="inlineStr">
+        <is>
           <t>{2021: 186079.663676732, 2022: 182518.53520077094, 2023: 172961.05546812713, 2024: 163403.5757354796, 2025: 153846.09600283578, 2026: 144288.61627018824, 2027: 134731.13653754443, 2028: 125173.65680489689, 2029: 115616.17707225308, 2030: 106058.69733960554, 2031: 96501.21760696173, 2032: 86943.73787431419, 2033: 77386.25814167038, 2034: 67828.77840902284, 2035: 58271.298676379025, 2036: 48713.81894373521, 2037: 39156.339211087674, 2038: 29598.85947844386, 2039: 20041.379745796323, 2040: 10483.90001315251, 2041: 926.4202805049717, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S163" t="n">
+      <c r="T163" t="n">
         <v>1927489.386651136</v>
       </c>
     </row>
@@ -11417,10 +12232,15 @@
       </c>
       <c r="R164" t="inlineStr">
         <is>
+          <t>[-2.04866765e+03  4.20284828e+06]</t>
+        </is>
+      </c>
+      <c r="S164" t="inlineStr">
+        <is>
           <t>{2021: 63097.8564675558, 2022: 60442.29463734198, 2023: 58393.62699066289, 2024: 56344.959343983326, 2025: 54296.29169730423, 2026: 52247.624050625134, 2027: 50198.95640394604, 2028: 48150.28875726648, 2029: 46101.62111058738, 2030: 44052.953463908285, 2031: 42004.28581722919, 2032: 39955.61817055009, 2033: 37906.95052387053, 2034: 35858.282877191436, 2035: 33809.61523051234, 2036: 31760.947583833244, 2037: 29712.279937153682, 2038: 27663.612290474586, 2039: 25614.94464379549, 2040: 23566.276997116394, 2041: 21517.6093504373, 2042: 19468.941703757737, 2043: 17420.27405707864, 2044: 15371.606410399545, 2045: 13322.938763720449, 2046: 11274.271117040887, 2047: 9225.603470361792, 2048: 7176.935823682696, 2049: 5128.2681770036, 2050: 3079.600530324504}</t>
         </is>
       </c>
-      <c r="S164" t="n">
+      <c r="T164" t="n">
         <v>951076.6078997755</v>
       </c>
     </row>
@@ -11484,10 +12304,15 @@
       </c>
       <c r="R165" t="inlineStr">
         <is>
+          <t>[-1.26402611e+03  2.56828470e+06]</t>
+        </is>
+      </c>
+      <c r="S165" t="inlineStr">
+        <is>
           <t>{2021: 14328.4594416561, 2022: 12423.919117198791, 2023: 11159.893011445645, 2024: 9895.866905692033, 2025: 8631.840799938422, 2026: 7367.81469418481, 2027: 6103.788588431198, 2028: 4839.762482677586, 2029: 3575.7363769239746, 2030: 2311.710271170363, 2031: 1047.684165416751, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S165" t="n">
+      <c r="T165" t="n">
         <v>74522.24613390763</v>
       </c>
     </row>
@@ -11551,10 +12376,15 @@
       </c>
       <c r="R166" t="inlineStr">
         <is>
+          <t>[-1.12345484e+03  2.29912106e+06]</t>
+        </is>
+      </c>
+      <c r="S166" t="inlineStr">
+        <is>
           <t>{2021: 29250.7309323134, 2022: 27495.367590732872, 2023: 26371.912746458314, 2024: 25248.457902183756, 2025: 24125.003057909198, 2026: 23001.548213634174, 2027: 21878.093369359616, 2028: 20754.638525085058, 2029: 19631.1836808105, 2030: 18507.72883653594, 2031: 17384.273992261384, 2032: 16260.819147986826, 2033: 15137.364303712267, 2034: 14013.90945943771, 2035: 12890.454615162686, 2036: 11766.999770888127, 2037: 10643.54492661357, 2038: 9520.090082339011, 2039: 8396.635238064453, 2040: 7273.180393789895, 2041: 6149.725549515337, 2042: 5026.270705240779, 2043: 3902.8158609662205, 2044: 2779.3610166911967, 2045: 1655.9061724166386, 2046: 532.4513281420805, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S166" t="n">
+      <c r="T166" t="n">
         <v>364973.1019520943</v>
       </c>
     </row>
@@ -11618,10 +12448,15 @@
       </c>
       <c r="R167" t="inlineStr">
         <is>
+          <t>[-7.93914387e+02  1.62228874e+06]</t>
+        </is>
+      </c>
+      <c r="S167" t="inlineStr">
+        <is>
           <t>{2021: 18256.261785925, 2022: 16993.85341228661, 2023: 16199.939025656553, 2024: 15406.024639026495, 2025: 14612.110252396436, 2026: 13818.195865766378, 2027: 13024.28147913632, 2028: 12230.367092506262, 2029: 11436.452705876203, 2030: 10642.538319246145, 2031: 9848.623932616087, 2032: 9054.709545985796, 2033: 8260.795159355737, 2034: 7466.880772725679, 2035: 6672.966386095621, 2036: 5879.051999465562, 2037: 5085.137612835504, 2038: 4291.223226205446, 2039: 3497.3088395753875, 2040: 2703.3944529453292, 2041: 1909.480066315271, 2042: 1115.5656796852127, 2043: 321.65129305492155, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S167" t="n">
+      <c r="T167" t="n">
         <v>199598.6826517215</v>
       </c>
     </row>
@@ -11685,10 +12520,15 @@
       </c>
       <c r="R168" t="inlineStr">
         <is>
+          <t>[-5.95021756e+02  1.24024753e+06]</t>
+        </is>
+      </c>
+      <c r="S168" t="inlineStr">
+        <is>
           <t>{2021: 38514.0563417962, 2022: 37113.541805813555, 2023: 36518.52005013684, 2024: 35923.49829445989, 2025: 35328.47653878294, 2026: 34733.45478310622, 2027: 34138.43302742927, 2028: 33543.411271752324, 2029: 32948.38951607561, 2030: 32353.367760398658, 2031: 31758.34600472171, 2032: 31163.324249044992, 2033: 30568.302493368043, 2034: 29973.280737691093, 2035: 29378.258982014377, 2036: 28783.237226337427, 2037: 28188.215470660478, 2038: 27593.19371498376, 2039: 26998.171959306812, 2040: 26403.150203629863, 2041: 25808.128447953146, 2042: 25213.106692276197, 2043: 24618.084936599247, 2044: 24023.06318092253, 2045: 23428.04142524558, 2046: 22833.01966956863, 2047: 22237.997913891915, 2048: 21642.976158214966, 2049: 21047.954402538016, 2050: 20452.9326468613}</t>
         </is>
       </c>
-      <c r="S168" t="n">
+      <c r="T168" t="n">
         <v>843744.4414112528</v>
       </c>
     </row>
@@ -11752,10 +12592,15 @@
       </c>
       <c r="R169" t="inlineStr">
         <is>
+          <t>[-5.83765711e+02  1.21278391e+06]</t>
+        </is>
+      </c>
+      <c r="S169" t="inlineStr">
+        <is>
           <t>{2021: 31969.8315052147, 2022: 32409.64653846342, 2023: 31825.880827790592, 2024: 31242.11511711753, 2025: 30658.3494064447, 2026: 30074.58369577187, 2027: 29490.81798509881, 2028: 28907.05227442598, 2029: 28323.286563752918, 2030: 27739.52085308009, 2031: 27155.75514240726, 2032: 26571.989431734197, 2033: 25988.223721061368, 2034: 25404.45801038854, 2035: 24820.692299715476, 2036: 24236.926589042647, 2037: 23653.160878369818, 2038: 23069.395167696755, 2039: 22485.629457023926, 2040: 21901.863746351097, 2041: 21318.098035678035, 2042: 20734.332325005205, 2043: 20150.566614332376, 2044: 19566.800903659314, 2045: 18983.035192986485, 2046: 18399.269482313655, 2047: 17815.503771640593, 2048: 17231.738060967764, 2049: 16647.972350294935, 2050: 16064.206639621872}</t>
         </is>
       </c>
-      <c r="S169" t="n">
+      <c r="T169" t="n">
         <v>710823.6835150337</v>
       </c>
     </row>
@@ -11819,10 +12664,15 @@
       </c>
       <c r="R170" t="inlineStr">
         <is>
+          <t>[-2.63663908e+03  5.40286872e+06]</t>
+        </is>
+      </c>
+      <c r="S170" t="inlineStr">
+        <is>
           <t>{2021: 72186.9558804449, 2022: 71584.50207578484, 2023: 68947.86299496423, 2024: 66311.22391414456, 2025: 63674.584833323956, 2026: 61037.94575250428, 2027: 58401.30667168368, 2028: 55764.667590864, 2029: 53128.0285100434, 2030: 50491.389429223724, 2031: 47854.75034840312, 2032: 45218.111267583445, 2033: 42581.47218676284, 2034: 39944.833105943166, 2035: 37308.19402512256, 2036: 34671.55494430289, 2037: 32034.91586348228, 2038: 29398.276782662608, 2039: 26761.637701842003, 2040: 24124.99862102233, 2041: 21488.359540201724, 2042: 18851.72045938205, 2043: 16215.081378561445, 2044: 13578.44229774177, 2045: 10941.803216921166, 2046: 8305.164136101492, 2047: 5668.525055280887, 2048: 3031.8859744612128, 2049: 395.2468936415389, 2050: 0}</t>
         </is>
       </c>
-      <c r="S170" t="n">
+      <c r="T170" t="n">
         <v>1043809.96351218</v>
       </c>
     </row>
@@ -11886,10 +12736,15 @@
       </c>
       <c r="R171" t="inlineStr">
         <is>
+          <t>[-1.57649127e+03  3.21383747e+06]</t>
+        </is>
+      </c>
+      <c r="S171" t="inlineStr">
+        <is>
           <t>{2021: 28308.7374505601, 2022: 26172.11326950183, 2023: 24595.62199503649, 2024: 23019.130720571615, 2025: 21442.639446106274, 2026: 19866.148171640933, 2027: 18289.65689717559, 2028: 16713.165622710716, 2029: 15136.674348245375, 2030: 13560.183073780034, 2031: 11983.691799314693, 2032: 10407.200524849817, 2033: 8830.709250384476, 2034: 7254.217975919135, 2035: 5677.7267014542595, 2036: 4101.235426988918, 2037: 2524.744152523577, 2038: 948.2528780582361, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S171" t="n">
+      <c r="T171" t="n">
         <v>244677.480979542</v>
       </c>
     </row>
@@ -11953,10 +12808,15 @@
       </c>
       <c r="R172" t="inlineStr">
         <is>
+          <t>[-4.23998354e+04  8.73224794e+07]</t>
+        </is>
+      </c>
+      <c r="S172" t="inlineStr">
+        <is>
           <t>{2021: 1689173.9907568, 2022: 1590012.2309478372, 2023: 1547612.3955596685, 2024: 1505212.5601714998, 2025: 1462812.7247833312, 2026: 1420412.8893951625, 2027: 1378013.0540069938, 2028: 1335613.218618825, 2029: 1293213.3832306564, 2030: 1250813.5478424877, 2031: 1208413.712454304, 2032: 1166013.8770661354, 2033: 1123614.0416779667, 2034: 1081214.206289798, 2035: 1038814.3709016293, 2036: 996414.5355134606, 2037: 954014.700125292, 2038: 911614.8647371233, 2039: 869215.0293489546, 2040: 826815.1939607859, 2041: 784415.3585726172, 2042: 742015.5231844485, 2043: 699615.6877962649, 2044: 657215.8524080962, 2045: 614816.0170199275, 2046: 572416.1816317588, 2047: 530016.3462435901, 2048: 487616.5108554214, 2049: 445216.67546725273, 2050: 402816.84007908404}</t>
         </is>
       </c>
-      <c r="S172" t="n">
+      <c r="T172" t="n">
         <v>29539200.10522923</v>
       </c>
     </row>
@@ -12020,10 +12880,15 @@
       </c>
       <c r="R173" t="inlineStr">
         <is>
+          <t>[ 5.64324620e+03 -1.13438818e+07]</t>
+        </is>
+      </c>
+      <c r="S173" t="inlineStr">
+        <is>
           <t>{2021: 61688.0519093829, 2022: 66762.03687416017, 2023: 72405.28307181224, 2024: 78048.52926946431, 2025: 83691.77546711825, 2026: 89335.02166477032, 2027: 94978.26786242239, 2028: 100621.51406007446, 2029: 106264.76025772654, 2030: 111908.0064553786, 2031: 117551.25265303068, 2032: 123194.49885068461, 2033: 128837.74504833668, 2034: 134480.99124598876, 2035: 140124.23744364083, 2036: 145767.4836412929, 2037: 151410.72983894497, 2038: 157053.9760365989, 2039: 162697.22223425098, 2040: 168340.46843190305, 2041: 173983.71462955512, 2042: 179626.9608272072, 2043: 185270.20702485926, 2044: 190913.45322251134, 2045: 196556.69942016527, 2046: 202199.94561781734, 2047: 207843.1918154694, 2048: 213486.4380131215, 2049: 219129.68421077356, 2050: 224772.93040842563}</t>
         </is>
       </c>
-      <c r="S173" t="n">
+      <c r="T173" t="n">
         <v>4145714.586347984</v>
       </c>
     </row>
@@ -12087,10 +12952,15 @@
       </c>
       <c r="R174" t="inlineStr">
         <is>
+          <t>[-1.19447801e+03  2.45656414e+06]</t>
+        </is>
+      </c>
+      <c r="S174" t="inlineStr">
+        <is>
           <t>{2021: 42692.4197822988, 2022: 41329.597800705116, 2023: 40135.11978953425, 2024: 38940.641778362915, 2025: 37746.16376719205, 2026: 36551.68575602118, 2027: 35357.207744849846, 2028: 34162.72973367898, 2029: 32968.25172250811, 2030: 31773.773711336777, 2031: 30579.29570016591, 2032: 29384.81768899504, 2033: 28190.339677824173, 2034: 26995.86166665284, 2035: 25801.38365548197, 2036: 24606.905644311104, 2037: 23412.42763313977, 2038: 22217.949621968903, 2039: 21023.471610798035, 2040: 19828.9935996267, 2041: 18634.515588455833, 2042: 17440.037577284966, 2043: 16245.559566114098, 2044: 15051.081554942764, 2045: 13856.603543771897, 2046: 12662.125532601029, 2047: 11467.647521429695, 2048: 10273.169510258827, 2049: 9078.69149908796, 2050: 7884.213487916626}</t>
         </is>
       </c>
-      <c r="S174" t="n">
+      <c r="T174" t="n">
         <v>731004.3668322085</v>
       </c>
     </row>
@@ -12154,10 +13024,15 @@
       </c>
       <c r="R175" t="inlineStr">
         <is>
+          <t>[-1.57015912e+02  3.67757120e+05]</t>
+        </is>
+      </c>
+      <c r="S175" t="inlineStr">
+        <is>
           <t>{2021: 51009.6333632543, 2022: 50270.947194789944, 2023: 50113.93128321064, 2024: 49956.91537163133, 2025: 49799.899460051965, 2026: 49642.88354847266, 2027: 49485.86763689335, 2028: 49328.851725314045, 2029: 49171.83581373468, 2030: 49014.819902155374, 2031: 48857.80399057607, 2032: 48700.7880789967, 2033: 48543.772167417395, 2034: 48386.75625583809, 2035: 48229.740344258724, 2036: 48072.72443267942, 2037: 47915.70852110011, 2038: 47758.692609520745, 2039: 47601.67669794144, 2040: 47444.66078636213, 2041: 47287.64487478277, 2042: 47130.62896320346, 2043: 46973.613051624154, 2044: 46816.59714004479, 2045: 46659.58122846548, 2046: 46502.565316886175, 2047: 46345.54940530681, 2048: 46188.533493727504, 2049: 46031.5175821482, 2050: 45874.50167056883}</t>
         </is>
       </c>
-      <c r="S175" t="n">
+      <c r="T175" t="n">
         <v>1396676.574394046</v>
       </c>
     </row>
@@ -12221,10 +13096,15 @@
       </c>
       <c r="R176" t="inlineStr">
         <is>
+          <t>[-1.87554331e+03  3.92428249e+06]</t>
+        </is>
+      </c>
+      <c r="S176" t="inlineStr">
+        <is>
           <t>{2021: 134037.461587914, 2022: 131933.9211818031, 2023: 130058.37787509896, 2024: 128182.83456839435, 2025: 126307.29126168974, 2026: 124431.74795498513, 2027: 122556.20464828052, 2028: 120680.6613415759, 2029: 118805.11803487176, 2030: 116929.57472816715, 2031: 115054.03142146254, 2032: 113178.48811475793, 2033: 111302.94480805332, 2034: 109427.40150134871, 2035: 107551.85819464456, 2036: 105676.31488793995, 2037: 103800.77158123534, 2038: 101925.22827453073, 2039: 100049.68496782612, 2040: 98174.14166112198, 2041: 96298.59835441737, 2042: 94423.05504771275, 2043: 92547.51174100814, 2044: 90671.96843430353, 2045: 88796.42512759892, 2046: 86920.88182089478, 2047: 85045.33851419017, 2048: 83169.79520748556, 2049: 81294.25190078095, 2050: 79418.70859407634}</t>
         </is>
       </c>
-      <c r="S176" t="n">
+      <c r="T176" t="n">
         <v>3091922.508247175</v>
       </c>
     </row>
@@ -12288,10 +13168,15 @@
       </c>
       <c r="R177" t="inlineStr">
         <is>
+          <t>[-1.97547005e+03  4.01492872e+06]</t>
+        </is>
+      </c>
+      <c r="S177" t="inlineStr">
+        <is>
           <t>{2021: 23761.3196384102, 2022: 20528.280543173198, 2023: 18552.81049216492, 2024: 16577.340441156644, 2025: 14601.870390148368, 2026: 12626.400339140091, 2027: 10650.930288131814, 2028: 8675.460237123538, 2029: 6699.990186115261, 2030: 4724.5201351069845, 2031: 2749.050084098708, 2032: 773.5800330904312, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S177" t="n">
+      <c r="T177" t="n">
         <v>129040.8929886551</v>
       </c>
     </row>
@@ -12355,10 +13240,15 @@
       </c>
       <c r="R178" t="inlineStr">
         <is>
+          <t>[-1.11349011e+03  2.28939243e+06]</t>
+        </is>
+      </c>
+      <c r="S178" t="inlineStr">
+        <is>
           <t>{2021: 37555.3370470512, 2022: 37915.44006904075, 2023: 36801.94996392075, 2024: 35688.459858801216, 2025: 34574.96975368122, 2026: 33461.47964856168, 2027: 32347.989543441683, 2028: 31234.49943832215, 2029: 30121.009333202615, 2030: 29007.519228082616, 2031: 27894.029122963082, 2032: 26780.539017843083, 2033: 25667.04891272355, 2034: 24553.55880760355, 2035: 23440.068702484015, 2036: 22326.578597364016, 2037: 21213.088492244482, 2038: 20099.59838712495, 2039: 18986.10828200495, 2040: 17872.618176885415, 2041: 16759.128071765415, 2042: 15645.637966645882, 2043: 14532.147861525882, 2044: 13418.657756406348, 2045: 12305.167651286349, 2046: 11191.677546166815, 2047: 10078.187441046815, 2048: 8964.697335927282, 2049: 7851.207230807748, 2050: 6737.717125687748}</t>
         </is>
       </c>
-      <c r="S178" t="n">
+      <c r="T178" t="n">
         <v>662879.5892842438</v>
       </c>
     </row>
@@ -12422,10 +13312,15 @@
       </c>
       <c r="R179" t="inlineStr">
         <is>
+          <t>[-3.46307810e+03  7.06066799e+06]</t>
+        </is>
+      </c>
+      <c r="S179" t="inlineStr">
+        <is>
           <t>{2021: 63258.8422269992, 2022: 58324.06329756882, 2023: 54860.98519458622, 2024: 51397.907091603614, 2025: 47934.82898862101, 2026: 44471.75088563748, 2027: 41008.672782654874, 2028: 37545.59467967227, 2029: 34082.51657668967, 2030: 30619.438473706134, 2031: 27156.36037072353, 2032: 23693.282267740928, 2033: 20230.204164758325, 2034: 16767.12606177479, 2035: 13304.047958792187, 2036: 9840.969855809584, 2037: 6377.891752826981, 2038: 2914.813649843447, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S179" t="n">
+      <c r="T179" t="n">
         <v>552159.8751665095</v>
       </c>
     </row>
@@ -12489,10 +13384,15 @@
       </c>
       <c r="R180" t="inlineStr">
         <is>
+          <t>[-3.85426818e+03  7.95850821e+06]</t>
+        </is>
+      </c>
+      <c r="S180" t="inlineStr">
+        <is>
           <t>{2021: 176132.127440084, 2022: 165177.95761501323, 2023: 161323.68943696935, 2024: 157469.42125892546, 2025: 153615.15308088064, 2026: 149760.88490283675, 2027: 145906.61672479287, 2028: 142052.34854674898, 2029: 138198.0803687051, 2030: 134343.8121906612, 2031: 130489.54401261639, 2032: 126635.2758345725, 2033: 122781.00765652861, 2034: 118926.73947848473, 2035: 115072.47130044084, 2036: 111218.20312239695, 2037: 107363.93494435307, 2038: 103509.66676630825, 2039: 99655.39858826436, 2040: 95801.13041022047, 2041: 91946.86223217659, 2042: 88092.5940541327, 2043: 84238.32587608881, 2044: 80384.05769804493, 2045: 76529.78952000011, 2046: 72675.52134195622, 2047: 68821.25316391233, 2048: 64966.98498586845, 2049: 61112.71680782456, 2050: 57258.44862978067}</t>
         </is>
       </c>
-      <c r="S180" t="n">
+      <c r="T180" t="n">
         <v>3284764.729954657</v>
       </c>
     </row>
@@ -12556,10 +13456,15 @@
       </c>
       <c r="R181" t="inlineStr">
         <is>
+          <t>[-2.00835086e+03  4.12041237e+06]</t>
+        </is>
+      </c>
+      <c r="S181" t="inlineStr">
+        <is>
           <t>{2021: 62672.5396044912, 2022: 59526.92461933382, 2023: 57518.573754691985, 2024: 55510.22289005015, 2025: 53501.87202540785, 2026: 51493.52116076602, 2027: 49485.17029612372, 2028: 47476.81943148188, 2029: 45468.46856683958, 2030: 43460.11770219775, 2031: 41451.76683755545, 2032: 39443.415972913615, 2033: 37435.06510827178, 2034: 35426.71424362948, 2035: 33418.36337898765, 2036: 31410.012514345348, 2037: 29401.661649703514, 2038: 27393.310785061214, 2039: 25384.95992041938, 2040: 23376.609055777546, 2041: 21368.258191135246, 2042: 19359.907326493412, 2043: 17351.556461851113, 2044: 15343.205597209278, 2045: 13334.854732566979, 2046: 11326.503867925145, 2047: 9318.153003282845, 2048: 7309.802138641011, 2049: 5301.451273999177, 2050: 3293.100409356877}</t>
         </is>
       </c>
-      <c r="S181" t="n">
+      <c r="T181" t="n">
         <v>940580.0825135859</v>
       </c>
     </row>
@@ -12623,10 +13528,15 @@
       </c>
       <c r="R182" t="inlineStr">
         <is>
+          <t>[-8.54198212e+02  1.76313185e+06]</t>
+        </is>
+      </c>
+      <c r="S182" t="inlineStr">
+        <is>
           <t>{2021: 36625.9984524092, 2022: 35943.068436298054, 2023: 35088.870224009734, 2024: 34234.67201172141, 2025: 33380.47379943309, 2026: 32526.275587144773, 2027: 31672.07737485622, 2028: 30817.8791625679, 2029: 29963.68095027958, 2030: 29109.48273799126, 2031: 28255.284525702707, 2032: 27401.086313414387, 2033: 26546.888101126067, 2034: 25692.689888837747, 2035: 24838.491676549427, 2036: 23984.293464260874, 2037: 23130.095251972554, 2038: 22275.897039684234, 2039: 21421.698827395914, 2040: 20567.500615107594, 2041: 19713.30240281904, 2042: 18859.10419053072, 2043: 18004.9059782424, 2044: 17150.70776595408, 2045: 16296.50955366576, 2046: 15442.311341377208, 2047: 14588.113129088888, 2048: 13733.914916800568, 2049: 12879.716704512248, 2050: 12025.518492223928}</t>
         </is>
       </c>
-      <c r="S182" t="n">
+      <c r="T182" t="n">
         <v>707844.750443661</v>
       </c>
     </row>
@@ -12690,10 +13600,15 @@
       </c>
       <c r="R183" t="inlineStr">
         <is>
+          <t>[-8.5245805e+03  1.7409717e+07]</t>
+        </is>
+      </c>
+      <c r="S183" t="inlineStr">
+        <is>
           <t>{2021: 168389.147393076, 2022: 173015.2177704759, 2023: 164490.63727303594, 2024: 155966.056775596, 2025: 147441.47627815604, 2026: 138916.8957807161, 2027: 130392.31528327242, 2028: 121867.73478583246, 2029: 113343.15428839251, 2030: 104818.57379095256, 2031: 96293.99329351261, 2032: 87769.41279607266, 2033: 79244.83229863271, 2034: 70720.25180119276, 2035: 62195.67130375281, 2036: 53671.090806309134, 2037: 45146.51030886918, 2038: 36621.92981142923, 2039: 28097.34931398928, 2040: 19572.76881654933, 2041: 11048.18831910938, 2042: 2523.6078216694295, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S183" t="n">
+      <c r="T183" t="n">
         <v>1927352.242414056</v>
       </c>
     </row>
@@ -12757,10 +13672,15 @@
       </c>
       <c r="R184" t="inlineStr">
         <is>
+          <t>[-4.33172149e+03  8.96862309e+06]</t>
+        </is>
+      </c>
+      <c r="S184" t="inlineStr">
+        <is>
           <t>{2021: 211306.066490469, 2022: 209882.24599868804, 2023: 205550.52451353706, 2024: 201218.8030283861, 2025: 196887.0815432351, 2026: 192555.360058086, 2027: 188223.63857293501, 2028: 183891.91708778404, 2029: 179560.19560263306, 2030: 175228.47411748394, 2031: 170896.75263233297, 2032: 166565.031147182, 2033: 162233.309662031, 2034: 157901.5881768819, 2035: 153569.86669173092, 2036: 149238.14520657994, 2037: 144906.42372142896, 2038: 140574.70223627985, 2039: 136242.98075112887, 2040: 131911.2592659779, 2041: 127579.53778082691, 2042: 123247.8162956778, 2043: 118916.09481052682, 2044: 114584.37332537584, 2045: 110252.65184022486, 2046: 105920.93035507575, 2047: 101589.20886992477, 2048: 97257.48738477379, 2049: 92925.76589962281, 2050: 88594.04441447183}</t>
         </is>
       </c>
-      <c r="S184" t="n">
+      <c r="T184" t="n">
         <v>4389262.222028823</v>
       </c>
     </row>
@@ -12824,10 +13744,15 @@
       </c>
       <c r="R185" t="inlineStr">
         <is>
+          <t>[-1.30805287e+03  2.68536026e+06]</t>
+        </is>
+      </c>
+      <c r="S185" t="inlineStr">
+        <is>
           <t>{2021: 42381.5768764867, 2022: 40477.351177245844, 2023: 39169.29830239108, 2024: 37861.24542753631, 2025: 36553.19255268201, 2026: 35245.13967782725, 2027: 33937.08680297248, 2028: 32629.03392811818, 2029: 31320.981053263415, 2030: 30012.92817840865, 2031: 28704.87530355435, 2032: 27396.822428699583, 2033: 26088.769553844817, 2034: 24780.716678990517, 2035: 23472.66380413575, 2036: 22164.610929280985, 2037: 20856.55805442622, 2038: 19548.50517957192, 2039: 18240.452304717153, 2040: 16932.399429862387, 2041: 15624.346555008087, 2042: 14316.293680153321, 2043: 13008.240805298556, 2044: 11700.187930444255, 2045: 10392.13505558949, 2046: 9084.082180734724, 2047: 7776.029305880424, 2048: 6467.976431025658, 2049: 5159.923556170892, 2050: 3851.870681316592}</t>
         </is>
       </c>
-      <c r="S185" t="n">
+      <c r="T185" t="n">
         <v>662038.5700467359</v>
       </c>
     </row>
@@ -12891,10 +13816,15 @@
       </c>
       <c r="R186" t="inlineStr">
         <is>
+          <t>[-1.31948628e+03  2.70955480e+06]</t>
+        </is>
+      </c>
+      <c r="S186" t="inlineStr">
+        <is>
           <t>{2021: 43101.3112244717, 2022: 41553.54124577576, 2023: 40234.05496354867, 2024: 38914.56868132157, 2025: 37595.08239909494, 2026: 36275.59611686785, 2027: 34956.10983464122, 2028: 33636.62355241412, 2029: 32317.137270187028, 2030: 30997.6509879604, 2031: 29678.164705733303, 2032: 28358.678423506673, 2033: 27039.19214127958, 2034: 25719.705859052483, 2035: 24400.219576825853, 2036: 23080.73329459876, 2037: 21761.24701237213, 2038: 20441.760730145033, 2039: 19122.27444791794, 2040: 17802.78816569131, 2041: 16483.301883464213, 2042: 15163.815601237584, 2043: 13844.329319010489, 2044: 12524.843036783393, 2045: 11205.356754556764, 2046: 9885.870472329669, 2047: 8566.38419010304, 2048: 7246.897907875944, 2049: 5927.411625648849, 2050: 4607.925343422219}</t>
         </is>
       </c>
-      <c r="S186" t="n">
+      <c r="T186" t="n">
         <v>688587.9584838916</v>
       </c>
     </row>
@@ -12958,10 +13888,15 @@
       </c>
       <c r="R187" t="inlineStr">
         <is>
+          <t>[-1.72899804e+03  3.54555722e+06]</t>
+        </is>
+      </c>
+      <c r="S187" t="inlineStr">
+        <is>
           <t>{2021: 51343.2670589828, 2022: 49523.17784818821, 2023: 47794.17980670743, 2024: 46065.18176522618, 2025: 44336.183723744936, 2026: 42607.18568226369, 2027: 40878.18764078291, 2028: 39149.189599301666, 2029: 37420.19155782042, 2030: 35691.193516339175, 2031: 33962.195474858396, 2032: 32233.19743337715, 2033: 30504.199391895905, 2034: 28775.20135041466, 2035: 27046.20330893388, 2036: 25317.205267452635, 2037: 23588.20722597139, 2038: 21859.209184490144, 2039: 20130.211143009365, 2040: 18401.21310152812, 2041: 16672.215060046874, 2042: 14943.217018565629, 2043: 13214.218977084849, 2044: 11485.220935603604, 2045: 9756.222894122358, 2046: 8027.224852641113, 2047: 6298.226811160333, 2048: 4569.228769679088, 2049: 2840.230728197843, 2050: 1111.2326867170632}</t>
         </is>
       </c>
-      <c r="S187" t="n">
+      <c r="T187" t="n">
         <v>759314.9699422579</v>
       </c>
     </row>
@@ -13025,10 +13960,15 @@
       </c>
       <c r="R188" t="inlineStr">
         <is>
+          <t>[-7.09237808e+03  1.48255324e+07]</t>
+        </is>
+      </c>
+      <c r="S188" t="inlineStr">
+        <is>
           <t>{2021: 497032.578523585, 2022: 484743.9525061697, 2023: 477651.57442601956, 2024: 470559.19634586945, 2025: 463466.81826571934, 2026: 456374.44018556736, 2027: 449282.06210541725, 2028: 442189.68402526714, 2029: 435097.305945117, 2030: 428004.9278649669, 2031: 420912.54978481494, 2032: 413820.1717046648, 2033: 406727.7936245147, 2034: 399635.4155443646, 2035: 392543.0374642145, 2036: 385450.6593840625, 2037: 378358.2813039124, 2038: 371265.9032237623, 2039: 364173.5251436122, 2040: 357081.14706346206, 2041: 349988.7689833101, 2042: 342896.39090316, 2043: 335804.01282300986, 2044: 328711.63474285975, 2045: 321619.25666270964, 2046: 314526.87858255766, 2047: 307434.50050240755, 2048: 300342.12242225744, 2049: 293249.7443421073, 2050: 286157.3662619572}</t>
         </is>
       </c>
-      <c r="S188" t="n">
+      <c r="T188" t="n">
         <v>11283506.72826865</v>
       </c>
     </row>
@@ -13092,10 +14032,15 @@
       </c>
       <c r="R189" t="inlineStr">
         <is>
+          <t>[-5.96308096e+02  1.22066811e+06]</t>
+        </is>
+      </c>
+      <c r="S189" t="inlineStr">
+        <is>
           <t>{2021: 15746.9656758898, 2022: 14933.135255242698, 2023: 14336.827159343753, 2024: 13740.519063444808, 2025: 13144.210967545863, 2026: 12547.902871646918, 2027: 11951.594775747973, 2028: 11355.286679849029, 2029: 10758.978583950317, 2030: 10162.670488051372, 2031: 9566.362392152427, 2032: 8970.054296253482, 2033: 8373.746200354537, 2034: 7777.438104455592, 2035: 7181.130008556647, 2036: 6584.821912657702, 2037: 5988.51381675899, 2038: 5392.205720860045, 2039: 4795.8976249611005, 2040: 4199.589529062156, 2041: 3603.2814331632107, 2042: 3006.973337264266, 2043: 2410.665241365321, 2044: 1814.357145466376, 2045: 1218.049049567664, 2046: 621.7409536687192, 2047: 25.432857769774273, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S189" t="n">
+      <c r="T189" t="n">
         <v>202334.8683071056</v>
       </c>
     </row>
@@ -13159,10 +14104,15 @@
       </c>
       <c r="R190" t="inlineStr">
         <is>
+          <t>[-8.30630769e+02  1.70939220e+06]</t>
+        </is>
+      </c>
+      <c r="S190" t="inlineStr">
+        <is>
           <t>{2021: 31112.2751602701, 2022: 29856.788370328024, 2023: 29026.15760140377, 2024: 28195.52683247975, 2025: 27364.89606355573, 2026: 26534.265294631477, 2027: 25703.634525707457, 2028: 24873.003756783204, 2029: 24042.372987859184, 2030: 23211.742218935164, 2031: 22381.11145001091, 2032: 21550.48068108689, 2033: 20719.84991216287, 2034: 19889.219143238617, 2035: 19058.588374314597, 2036: 18227.957605390344, 2037: 17397.326836466324, 2038: 16566.696067542303, 2039: 15736.06529861805, 2040: 14905.43452969403, 2041: 14074.80376077001, 2042: 13244.172991845757, 2043: 12413.542222921737, 2044: 11582.911453997483, 2045: 10752.280685073463, 2046: 9921.649916149443, 2047: 9091.01914722519, 2048: 8260.38837830117, 2049: 7429.7576093771495, 2050: 6599.126840452896}</t>
         </is>
       </c>
-      <c r="S190" t="n">
+      <c r="T190" t="n">
         <v>540867.3447162316</v>
       </c>
     </row>
@@ -13226,10 +14176,15 @@
       </c>
       <c r="R191" t="inlineStr">
         <is>
+          <t>[-3.26626403e+03  6.72521678e+06]</t>
+        </is>
+      </c>
+      <c r="S191" t="inlineStr">
+        <is>
           <t>{2021: 131967.22007073794, 2022: 120830.91176124662, 2023: 117564.64772975165, 2024: 114298.38369825762, 2025: 111032.11966676265, 2026: 107765.85563526861, 2027: 104499.59160377365, 2028: 101233.32757227961, 2029: 97967.06354078557, 2030: 94700.7995092906, 2031: 91434.53547779657, 2032: 88168.2714463016, 2033: 84902.00741480757, 2034: 81635.7433833126, 2035: 78369.47935181856, 2036: 75103.2153203236, 2037: 71836.95128882956, 2038: 68570.68725733552, 2039: 65304.423225840554, 2040: 62038.15919434652, 2041: 58771.89516285155, 2042: 55505.63113135751, 2043: 52239.367099862546, 2044: 48973.10306836851, 2045: 45706.83903687354, 2046: 42440.575005379505, 2047: 39174.31097388454, 2048: 35908.0469423905, 2049: 32641.782910896465, 2050: 29375.518879401498}</t>
         </is>
       </c>
-      <c r="S191" t="n">
+      <c r="T191" t="n">
         <v>2229289.094885064</v>
       </c>
     </row>
@@ -13293,10 +14248,15 @@
       </c>
       <c r="R192" t="inlineStr">
         <is>
+          <t>[-2.12121080e+03  4.35198987e+06]</t>
+        </is>
+      </c>
+      <c r="S192" t="inlineStr">
+        <is>
           <t>{2021: 71079.1096970575, 2022: 62901.643468535505, 2023: 60780.43267293647, 2024: 58659.221877338365, 2025: 56538.01108173933, 2026: 54416.80028614029, 2027: 52295.58949054126, 2028: 50174.37869494315, 2029: 48053.16789934412, 2030: 45931.95710374508, 2031: 43810.746308146976, 2032: 41689.53551254794, 2033: 39568.324716948904, 2034: 37447.1139213508, 2035: 35325.90312575176, 2036: 33204.69233015273, 2037: 31083.481534554623, 2038: 28962.270738955587, 2039: 26841.05994335655, 2040: 24719.849147758447, 2041: 22598.63835215941, 2042: 20477.427556560375, 2043: 18356.21676096134, 2044: 16235.005965363234, 2045: 14113.795169764198, 2046: 11992.584374165162, 2047: 9871.373578567058, 2048: 7750.162782968022, 2049: 5628.951987368986, 2050: 3507.7411917708814}</t>
         </is>
       </c>
-      <c r="S192" t="n">
+      <c r="T192" t="n">
         <v>996721.7618270798</v>
       </c>
     </row>
@@ -13360,10 +14320,15 @@
       </c>
       <c r="R193" t="inlineStr">
         <is>
+          <t>[-3.65603363e+03  7.44329796e+06]</t>
+        </is>
+      </c>
+      <c r="S193" t="inlineStr">
+        <is>
           <t>{2021: 56168.719156538, 2022: 50797.959167866036, 2023: 47141.92553534359, 2024: 43485.89190282021, 2025: 39829.85827029683, 2026: 36173.82463777438, 2027: 32517.791005250998, 2028: 28861.75737272855, 2029: 25205.72374020517, 2030: 21549.69010768179, 2031: 17893.65647515934, 2032: 14237.62284263596, 2033: 10581.58921011258, 2034: 6925.55557759013, 2035: 3269.52194506675, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S193" t="n">
+      <c r="T193" t="n">
         <v>406556.7273688013</v>
       </c>
     </row>
@@ -13427,10 +14392,15 @@
       </c>
       <c r="R194" t="inlineStr">
         <is>
+          <t>[-1.02345378e+04  2.07886160e+07]</t>
+        </is>
+      </c>
+      <c r="S194" t="inlineStr">
+        <is>
           <t>{2021: 112633.150159207, 2022: 94380.5037884675, 2023: 84145.96594263613, 2024: 73911.4280968085, 2025: 63676.89025097713, 2026: 53442.35240514949, 2027: 43207.814559318125, 2028: 32973.27671348676, 2029: 22738.73886765912, 2030: 12504.201021827757, 2031: 2269.663175996393, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S194" t="n">
+      <c r="T194" t="n">
         <v>539567.4099019304</v>
       </c>
     </row>
@@ -13494,10 +14464,15 @@
       </c>
       <c r="R195" t="inlineStr">
         <is>
+          <t>[-8.29948589e+03  1.68687608e+07]</t>
+        </is>
+      </c>
+      <c r="S195" t="inlineStr">
+        <is>
           <t>{2021: 101943.766644076, 2022: 87200.30110003054, 2023: 78900.8152080439, 2024: 70601.32931605354, 2025: 62301.8434240669, 2026: 54002.35753208026, 2027: 45702.871640093625, 2028: 37403.385748106986, 2029: 29103.899856120348, 2030: 20804.413964129984, 2031: 12504.928072143346, 2032: 4205.442180156708, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S195" t="n">
+      <c r="T195" t="n">
         <v>553703.4713630641</v>
       </c>
     </row>
@@ -13561,10 +14536,15 @@
       </c>
       <c r="R196" t="inlineStr">
         <is>
+          <t>[ 9.23042494e+01 -1.70712878e+05]</t>
+        </is>
+      </c>
+      <c r="S196" t="inlineStr">
+        <is>
           <t>{2021: 15392.0842487046, 2022: 15926.314491379424, 2023: 16018.618740735255, 2024: 16110.922990091087, 2025: 16203.227239446918, 2026: 16295.53148880275, 2027: 16387.83573815858, 2028: 16480.139987514412, 2029: 16572.444236870244, 2030: 16664.748486226075, 2031: 16757.052735581907, 2032: 16849.356984937738, 2033: 16941.66123429357, 2034: 17033.9654836494, 2035: 17126.269733005232, 2036: 17218.573982361064, 2037: 17310.878231716895, 2038: 17403.182481072727, 2039: 17495.486730428558, 2040: 17587.79097978436, 2041: 17680.09522914019, 2042: 17772.399478496023, 2043: 17864.703727851855, 2044: 17957.007977207686, 2045: 18049.312226563517, 2046: 18141.61647591935, 2047: 18233.92072527518, 2048: 18326.22497463101, 2049: 18418.529223986843, 2050: 18510.833473342675}</t>
         </is>
       </c>
-      <c r="S196" t="n">
+      <c r="T196" t="n">
         <v>497779.2708761515</v>
       </c>
     </row>
@@ -13628,10 +14608,15 @@
       </c>
       <c r="R197" t="inlineStr">
         <is>
+          <t>[-3.16810667e+02  6.68649973e+05]</t>
+        </is>
+      </c>
+      <c r="S197" t="inlineStr">
+        <is>
           <t>{2021: 27416.5036901078, 2022: 28058.804164221394, 2023: 27741.993497113, 2024: 27425.182830004604, 2025: 27108.37216289621, 2026: 26791.561495787813, 2027: 26474.75082867942, 2028: 26157.940161571023, 2029: 25841.129494462744, 2030: 25524.31882735435, 2031: 25207.508160245954, 2032: 24890.69749313756, 2033: 24573.886826029164, 2034: 24257.07615892077, 2035: 23940.265491812374, 2036: 23623.45482470398, 2037: 23306.644157595583, 2038: 22989.833490487188, 2039: 22673.022823378793, 2040: 22356.212156270398, 2041: 22039.401489162003, 2042: 21722.590822053724, 2043: 21405.78015494533, 2044: 21088.969487836934, 2045: 20772.15882072854, 2046: 20455.348153620143, 2047: 20138.53748651175, 2048: 19821.726819403353, 2049: 19504.916152294958, 2050: 19188.105485186563}</t>
         </is>
       </c>
-      <c r="S197" t="n">
+      <c r="T197" t="n">
         <v>689194.3890188762</v>
       </c>
     </row>
@@ -13695,10 +14680,15 @@
       </c>
       <c r="R198" t="inlineStr">
         <is>
+          <t>[-1.95420824e+03  4.00818724e+06]</t>
+        </is>
+      </c>
+      <c r="S198" t="inlineStr">
+        <is>
           <t>{2021: 59245.4924784036, 2022: 56778.17843033979, 2023: 54823.97018944053, 2024: 52869.76194854127, 2025: 50915.553707642015, 2026: 48961.34546674229, 2027: 47007.137225843035, 2028: 45052.92898494378, 2029: 43098.72074404452, 2030: 41144.5125031448, 2031: 39190.30426224554, 2032: 37236.09602134628, 2033: 35281.887780447025, 2034: 33327.6795395473, 2035: 31373.471298648044, 2036: 29419.263057748787, 2037: 27465.05481684953, 2038: 25510.846575949807, 2039: 23556.63833505055, 2040: 21602.430094151292, 2041: 19648.221853252035, 2042: 17694.01361235231, 2043: 15739.805371453054, 2044: 13785.597130553797, 2045: 11831.38888965454, 2046: 9877.180648754817, 2047: 7922.972407855559, 2048: 5968.764166956302, 2049: 4014.5559260570444, 2050: 2060.347685157787}</t>
         </is>
       </c>
-      <c r="S198" t="n">
+      <c r="T198" t="n">
         <v>881751.2010713364</v>
       </c>
     </row>
@@ -13762,10 +14752,15 @@
       </c>
       <c r="R199" t="inlineStr">
         <is>
+          <t>[-2.16668233e+04  4.47052221e+07]</t>
+        </is>
+      </c>
+      <c r="S199" t="inlineStr">
+        <is>
           <t>{2021: 1054375.11108919, 2022: 894905.3654717505, 2023: 873238.5421475321, 2024: 851571.7188233212, 2025: 829904.8954991028, 2026: 808238.0721748918, 2027: 786571.2488506809, 2028: 764904.4255264625, 2029: 743237.6022022516, 2030: 721570.7788780406, 2031: 699903.9555538222, 2032: 678237.1322296113, 2033: 656570.3089054003, 2034: 634903.485581182, 2035: 613236.662256971, 2036: 591569.8389327526, 2037: 569903.0156085417, 2038: 548236.1922843307, 2039: 526569.3689601123, 2040: 504902.5456359014, 2041: 483235.72231169045, 2042: 461568.89898747206, 2043: 439902.0756632611, 2044: 418235.2523390427, 2045: 396568.4290148318, 2046: 374901.60569062084, 2047: 353234.78236640245, 2048: 331567.9590421915, 2049: 309901.13571798056, 2050: 288234.3123937622}</t>
         </is>
       </c>
-      <c r="S199" t="n">
+      <c r="T199" t="n">
         <v>17538595.72839763</v>
       </c>
     </row>
@@ -13829,10 +14824,15 @@
       </c>
       <c r="R200" t="inlineStr">
         <is>
+          <t>[-1.54173420e+05  3.12599907e+08]</t>
+        </is>
+      </c>
+      <c r="S200" t="inlineStr">
+        <is>
           <t>{2021: 1052156.51907693, 2022: 861250.791710496, 2023: 707077.3713434935, 2024: 552903.9509764314, 2025: 398730.5306094289, 2026: 244557.1102424264, 2027: 90383.68987542391, 2028: 0, 2029: 0, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S200" t="n">
+      <c r="T200" t="n">
         <v>3380981.704296165</v>
       </c>
     </row>
@@ -13896,10 +14896,15 @@
       </c>
       <c r="R201" t="inlineStr">
         <is>
+          <t>[-1.94777443e+02  4.04772382e+05]</t>
+        </is>
+      </c>
+      <c r="S201" t="inlineStr">
+        <is>
           <t>{2021: 11281.0686929347, 2022: 10932.390978483949, 2023: 10737.61353507574, 2024: 10542.836091667472, 2025: 10348.058648259263, 2026: 10153.281204850995, 2027: 9958.503761442786, 2028: 9763.726318034518, 2029: 9568.948874626309, 2030: 9374.1714312181, 2031: 9179.393987809832, 2032: 8984.616544401622, 2033: 8789.839100993355, 2034: 8595.061657585145, 2035: 8400.284214176878, 2036: 8205.506770768669, 2037: 8010.729327360401, 2038: 7815.951883952192, 2039: 7621.174440543924, 2040: 7426.396997135715, 2041: 7231.619553727447, 2042: 7036.842110319238, 2043: 6842.06466691097, 2044: 6647.287223502761, 2045: 6452.509780094493, 2046: 6257.732336686284, 2047: 6062.954893278016, 2048: 5868.177449869807, 2049: 5673.4000064615975, 2050: 5478.62256305333}</t>
         </is>
       </c>
-      <c r="S201" t="n">
+      <c r="T201" t="n">
         <v>240860.9194172315</v>
       </c>
     </row>
@@ -13963,10 +14968,15 @@
       </c>
       <c r="R202" t="inlineStr">
         <is>
+          <t>[-4.92369276e+02  1.02488877e+06]</t>
+        </is>
+      </c>
+      <c r="S202" t="inlineStr">
+        <is>
           <t>{2021: 29140.3773059041, 2022: 29318.091447584447, 2023: 28825.722171694273, 2024: 28333.352895804215, 2025: 27840.983619914157, 2026: 27348.6143440241, 2027: 26856.245068133925, 2028: 26363.875792243867, 2029: 25871.50651635381, 2030: 25379.13724046375, 2031: 24886.767964573577, 2032: 24394.39868868352, 2033: 23902.02941279346, 2034: 23409.660136903403, 2035: 22917.29086101323, 2036: 22424.92158512317, 2037: 21932.552309233113, 2038: 21440.183033343055, 2039: 20947.81375745288, 2040: 20455.444481562823, 2041: 19963.075205672765, 2042: 19470.705929782707, 2043: 18978.336653892533, 2044: 18485.967378002475, 2045: 17993.598102112417, 2046: 17501.22882622236, 2047: 17008.859550332185, 2048: 16516.490274442127, 2049: 16024.120998552069, 2050: 15531.751722661895}</t>
         </is>
       </c>
-      <c r="S202" t="n">
+      <c r="T202" t="n">
         <v>657127.0387601934</v>
       </c>
     </row>
@@ -14030,10 +15040,15 @@
       </c>
       <c r="R203" t="inlineStr">
         <is>
+          <t>[-2.13751009e+03  4.41720665e+06]</t>
+        </is>
+      </c>
+      <c r="S203" t="inlineStr">
+        <is>
           <t>{2021: 97788.2316329065, 2022: 95161.2417995669, 2023: 93023.73170825187, 2024: 90886.22161693685, 2025: 88748.71152562089, 2026: 86611.20143430587, 2027: 84473.69134299085, 2028: 82336.18125167489, 2029: 80198.67116035987, 2030: 78061.16106904484, 2031: 75923.65097772889, 2032: 73786.14088641386, 2033: 71648.63079509791, 2034: 69511.12070378289, 2035: 67373.61061246786, 2036: 65236.10052115191, 2037: 63098.590429836884, 2038: 60961.08033852186, 2039: 58823.570247205906, 2040: 56686.06015589088, 2041: 54548.55006457586, 2042: 52411.0399732599, 2043: 50273.52988194488, 2044: 48136.019790628925, 2045: 45998.5096993139, 2046: 43860.99960799888, 2047: 41723.48951668292, 2048: 39585.9794253679, 2049: 37448.469334052876, 2050: 35310.95924273692}</t>
         </is>
       </c>
-      <c r="S203" t="n">
+      <c r="T203" t="n">
         <v>1923085.551308499</v>
       </c>
     </row>
@@ -14097,10 +15112,15 @@
       </c>
       <c r="R204" t="inlineStr">
         <is>
+          <t>[ 5.04783663e+02 -9.66345302e+05]</t>
+        </is>
+      </c>
+      <c r="S204" t="inlineStr">
+        <is>
           <t>{2021: 53167.1119846155, 2022: 54327.26358602673, 2023: 54832.04724874406, 2024: 55336.83091146138, 2025: 55841.614574178704, 2026: 56346.39823689603, 2027: 56851.18189961335, 2028: 57355.965562330675, 2029: 57860.749225048, 2030: 58365.53288776532, 2031: 58870.31655048265, 2032: 59375.10021319997, 2033: 59879.883875917294, 2034: 60384.66753863462, 2035: 60889.45120135194, 2036: 61394.234864069265, 2037: 61899.01852678659, 2038: 62403.80218950403, 2039: 62908.58585222135, 2040: 63413.36951493868, 2041: 63918.153177656, 2042: 64422.936840373324, 2043: 64927.72050309065, 2044: 65432.50416580797, 2045: 65937.2878285253, 2046: 66442.07149124262, 2047: 66946.85515395994, 2048: 67451.63881667727, 2049: 67956.42247939459, 2050: 68461.20614211191}</t>
         </is>
       </c>
-      <c r="S204" t="n">
+      <c r="T204" t="n">
         <v>1772785.763979262</v>
       </c>
     </row>
@@ -14164,10 +15184,15 @@
       </c>
       <c r="R205" t="inlineStr">
         <is>
+          <t>[-4.73286689e+03  9.60426506e+06]</t>
+        </is>
+      </c>
+      <c r="S205" t="inlineStr">
+        <is>
           <t>{2021: 45590.2016067924, 2022: 34408.2051695548, 2023: 29675.338276157156, 2024: 24942.471382761374, 2025: 20209.60448936373, 2026: 15476.737595967948, 2027: 10743.870702570304, 2028: 6011.003809174523, 2029: 1278.1369157768786, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S205" t="n">
+      <c r="T205" t="n">
         <v>165540.4691447229</v>
       </c>
     </row>
@@ -14231,10 +15256,15 @@
       </c>
       <c r="R206" t="inlineStr">
         <is>
+          <t>[-8.45996897e+02  1.72699832e+06]</t>
+        </is>
+      </c>
+      <c r="S206" t="inlineStr">
+        <is>
           <t>{2021: 17518.5543303956, 2022: 16392.596084017307, 2023: 15546.599187081447, 2024: 14700.602290145354, 2025: 13854.605393209262, 2026: 13008.608496273402, 2027: 12162.61159933731, 2028: 11316.61470240145, 2029: 10470.617805465357, 2030: 9624.620908529265, 2031: 8778.624011593405, 2032: 7932.627114657313, 2033: 7086.63021772122, 2034: 6240.63332078536, 2035: 5394.636423849268, 2036: 4548.639526913408, 2037: 3702.6426299773157, 2038: 2856.645733041223, 2039: 2010.6488361053634, 2040: 1164.651939169271, 2041: 318.6550422331784, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S206" t="n">
+      <c r="T206" t="n">
         <v>175871.7884277043</v>
       </c>
     </row>
@@ -14298,10 +15328,15 @@
       </c>
       <c r="R207" t="inlineStr">
         <is>
+          <t>[-1.31148004e+04  2.70109171e+07]</t>
+        </is>
+      </c>
+      <c r="S207" t="inlineStr">
+        <is>
           <t>{2021: 498927.295715117, 2022: 492790.54507369176, 2023: 479675.744625397, 2024: 466560.9441771023, 2025: 453446.14372880384, 2026: 440331.3432805091, 2027: 427216.5428322144, 2028: 414101.74238391966, 2029: 400986.9419356212, 2030: 387872.1414873265, 2031: 374757.34103903174, 2032: 361642.540590737, 2033: 348527.74014243856, 2034: 335412.93969414383, 2035: 322298.1392458491, 2036: 309183.33879755065, 2037: 296068.5383492559, 2038: 282953.7379009612, 2039: 269838.93745266646, 2040: 256724.137004368, 2041: 243609.33655607328, 2042: 230494.53610777855, 2043: 217379.7356594801, 2044: 204264.93521118537, 2045: 191150.13476289064, 2046: 178035.3343145959, 2047: 164920.53386629745, 2048: 151805.73341800272, 2049: 138690.932969708, 2050: 125576.13252140954}</t>
         </is>
       </c>
-      <c r="S207" t="n">
+      <c r="T207" t="n">
         <v>9152992.406725863</v>
       </c>
     </row>
@@ -14365,10 +15400,15 @@
       </c>
       <c r="R208" t="inlineStr">
         <is>
+          <t>[-2.74205950e+03  5.59084893e+06]</t>
+        </is>
+      </c>
+      <c r="S208" t="inlineStr">
+        <is>
           <t>{2021: 50616.0916247363, 2022: 46404.61965116393, 2023: 43662.56015069876, 2024: 40920.50065023359, 2025: 38178.44114976842, 2026: 35436.38164930325, 2027: 32694.32214883808, 2028: 29952.26264837198, 2029: 27210.20314790681, 2030: 24468.14364744164, 2031: 21726.08414697647, 2032: 18984.0246465113, 2033: 16241.965146046132, 2034: 13499.905645580031, 2035: 10757.846145114861, 2036: 8015.786644649692, 2037: 5273.727144184522, 2038: 2531.667643719353, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S208" t="n">
+      <c r="T208" t="n">
         <v>441266.487818877</v>
       </c>
     </row>
@@ -14432,10 +15472,15 @@
       </c>
       <c r="R209" t="inlineStr">
         <is>
+          <t>[-2.09557081e+03  4.25809360e+06]</t>
+        </is>
+      </c>
+      <c r="S209" t="inlineStr">
+        <is>
           <t>{2021: 25547.0441284823, 2022: 20849.415951226838, 2023: 18753.845139840618, 2024: 16658.274328453466, 2025: 14562.703517067246, 2026: 12467.132705681026, 2027: 10371.561894293875, 2028: 8275.991082907654, 2029: 6180.420271521434, 2030: 4084.849460135214, 2031: 1989.2786487480626, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S209" t="n">
+      <c r="T209" t="n">
         <v>126966.9950641166</v>
       </c>
     </row>
@@ -14499,10 +15544,15 @@
       </c>
       <c r="R210" t="inlineStr">
         <is>
+          <t>[-1.48619035e+03  3.03742488e+06]</t>
+        </is>
+      </c>
+      <c r="S210" t="inlineStr">
+        <is>
           <t>{2021: 34907.3224756623, 2022: 32347.9938882445, 2023: 30861.803540764377, 2024: 29375.613193284255, 2025: 27889.422845804133, 2026: 26403.23249832401, 2027: 24917.04215084389, 2028: 23430.851803363767, 2029: 21944.661455883645, 2030: 20458.471108403523, 2031: 18972.2807609234, 2032: 17486.09041344328, 2033: 15999.900065963622, 2034: 14513.7097184835, 2035: 13027.519371003378, 2036: 11541.329023523256, 2037: 10055.138676043134, 2038: 8568.948328563012, 2039: 7082.75798108289, 2040: 5596.567633602768, 2041: 4110.377286122646, 2042: 2624.186938642524, 2043: 1137.9965911624022, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S210" t="n">
+      <c r="T210" t="n">
         <v>385799.5565113071</v>
       </c>
     </row>
@@ -14566,10 +15616,15 @@
       </c>
       <c r="R211" t="inlineStr">
         <is>
+          <t>[-2.03405247e+03  4.18056367e+06]</t>
+        </is>
+      </c>
+      <c r="S211" t="inlineStr">
+        <is>
           <t>{2021: 71581.5772144457, 2022: 67709.56985297613, 2023: 65675.51738003781, 2024: 63641.46490709949, 2025: 61607.412434161175, 2026: 59573.35996122286, 2027: 57539.30748828454, 2028: 55505.25501534622, 2029: 53471.202542407904, 2030: 51437.150069469586, 2031: 49403.09759653127, 2032: 47369.04512359295, 2033: 45334.99265065463, 2034: 43300.940177716315, 2035: 41266.887704778, 2036: 39232.83523183968, 2037: 37198.78275890136, 2038: 35164.73028596304, 2039: 33130.677813024726, 2040: 31096.625340086874, 2041: 29062.572867148556, 2042: 27028.520394210238, 2043: 24994.46792127192, 2044: 22960.415448333602, 2045: 20926.362975395285, 2046: 18892.310502456967, 2047: 16858.25802951865, 2048: 14824.205556580331, 2049: 12790.153083642013, 2050: 10756.100610703696}</t>
         </is>
       </c>
-      <c r="S211" t="n">
+      <c r="T211" t="n">
         <v>1168164.960025227</v>
       </c>
     </row>
@@ -14633,10 +15688,15 @@
       </c>
       <c r="R212" t="inlineStr">
         <is>
+          <t>[-7.83733454e+02  1.61301448e+06]</t>
+        </is>
+      </c>
+      <c r="S212" t="inlineStr">
+        <is>
           <t>{2021: 30903.7259124321, 2022: 28305.437653321307, 2023: 27521.70419979212, 2024: 26737.97074626293, 2025: 25954.237292733742, 2026: 25170.503839204554, 2027: 24386.770385675365, 2028: 23603.036932146177, 2029: 22819.30347861699, 2030: 22035.5700250878, 2031: 21251.83657155861, 2032: 20468.103118029423, 2033: 19684.369664500235, 2034: 18900.636210971046, 2035: 18116.902757441858, 2036: 17333.16930391267, 2037: 16549.43585038348, 2038: 15765.702396854293, 2039: 14981.968943325104, 2040: 14198.235489795916, 2041: 13414.502036266727, 2042: 12630.768582737539, 2043: 11847.03512920835, 2044: 11063.301675679162, 2045: 10279.568222149974, 2046: 9495.834768620785, 2047: 8712.101315091597, 2048: 7928.3678615624085, 2049: 7144.63440803322, 2050: 6360.900954504032}</t>
         </is>
       </c>
-      <c r="S212" t="n">
+      <c r="T212" t="n">
         <v>514933.3222924314</v>
       </c>
     </row>
@@ -14700,10 +15760,15 @@
       </c>
       <c r="R213" t="inlineStr">
         <is>
+          <t>[-8.47173369e+02  1.77140529e+06]</t>
+        </is>
+      </c>
+      <c r="S213" t="inlineStr">
+        <is>
           <t>{2021: 62848.4238097407, 2022: 58420.74130347464, 2023: 57573.56793453451, 2024: 56726.39456559415, 2025: 55879.22119665402, 2026: 55032.04782771389, 2027: 54184.87445877376, 2028: 53337.70108983363, 2029: 52490.5277208935, 2030: 51643.35435195337, 2031: 50796.18098301324, 2032: 49949.00761407311, 2033: 49101.83424513298, 2034: 48254.66087619262, 2035: 47407.48750725249, 2036: 46560.31413831236, 2037: 45713.14076937223, 2038: 44865.9674004321, 2039: 44018.79403149197, 2040: 43171.62066255184, 2041: 42324.44729361171, 2042: 41477.27392467158, 2043: 40630.10055573145, 2044: 39782.92718679109, 2045: 38935.75381785096, 2046: 38088.58044891083, 2047: 37241.4070799707, 2048: 36394.23371103057, 2049: 35547.06034209044, 2050: 34699.88697315031}</t>
         </is>
       </c>
-      <c r="S213" t="n">
+      <c r="T213" t="n">
         <v>1364323.378429355</v>
       </c>
     </row>
@@ -14767,10 +15832,15 @@
       </c>
       <c r="R214" t="inlineStr">
         <is>
+          <t>[-1.36425339e+03  2.78711035e+06]</t>
+        </is>
+      </c>
+      <c r="S214" t="inlineStr">
+        <is>
           <t>{2021: 30700.30201637, 2022: 28589.991700837854, 2023: 27225.73830733914, 2024: 25861.484913840424, 2025: 24497.231520341244, 2026: 23132.97812684253, 2027: 21768.724733343814, 2028: 20404.4713398451, 2029: 19040.217946346384, 2030: 17675.96455284767, 2031: 16311.711159348954, 2032: 14947.457765849773, 2033: 13583.204372351058, 2034: 12218.950978852343, 2035: 10854.697585353628, 2036: 9490.444191854913, 2037: 8126.190798356198, 2038: 6761.937404857017, 2039: 5397.684011358302, 2040: 4033.430617859587, 2041: 2669.177224360872, 2042: 1304.923830862157, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S214" t="n">
+      <c r="T214" t="n">
         <v>329246.764091034</v>
       </c>
     </row>
@@ -14834,10 +15904,15 @@
       </c>
       <c r="R215" t="inlineStr">
         <is>
+          <t>[-1.29052791e+03  2.63929561e+06]</t>
+        </is>
+      </c>
+      <c r="S215" t="inlineStr">
+        <is>
           <t>{2021: 31268.2196793714, 2022: 29848.16678335052, 2023: 28557.63886864623, 2024: 27267.11095394194, 2025: 25976.583039237652, 2026: 24686.055124533363, 2027: 23395.527209829073, 2028: 22104.99929512432, 2029: 20814.47138042003, 2030: 19523.94346571574, 2031: 18233.41555101145, 2032: 16942.88763630716, 2033: 15652.359721602872, 2034: 14361.831806898583, 2035: 13071.303892194293, 2036: 11780.775977489538, 2037: 10490.24806278525, 2038: 9199.72014808096, 2039: 7909.192233376671, 2040: 6618.664318672381, 2041: 5328.136403968092, 2042: 4037.6084892638028, 2043: 2747.0805745595135, 2044: 1456.5526598547585, 2045: 166.02474515046924, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S215" t="n">
+      <c r="T215" t="n">
         <v>375804.4081817004</v>
       </c>
     </row>
@@ -14901,10 +15976,15 @@
       </c>
       <c r="R216" t="inlineStr">
         <is>
+          <t>[-7.55306471e+03  1.53591775e+07]</t>
+        </is>
+      </c>
+      <c r="S216" t="inlineStr">
+        <is>
           <t>{2021: 96823.3419136609, 2022: 86880.68370117247, 2023: 79327.6189957019, 2024: 71774.55429023318, 2025: 64221.4895847626, 2026: 56668.424879292026, 2027: 49115.36017382145, 2028: 41562.295468352735, 2029: 34009.23076288216, 2030: 26456.16605741158, 2031: 18903.101351941004, 2032: 11350.03664647229, 2033: 3796.9719410017133, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S216" t="n">
+      <c r="T216" t="n">
         <v>592477.6048098756</v>
       </c>
     </row>
@@ -14968,10 +16048,15 @@
       </c>
       <c r="R217" t="inlineStr">
         <is>
+          <t>[-2.02761242e+03  4.13153106e+06]</t>
+        </is>
+      </c>
+      <c r="S217" t="inlineStr">
+        <is>
           <t>{2021: 34326.3895574425, 2022: 31698.749662001617, 2023: 29671.13724380359, 2024: 27643.52482560603, 2025: 25615.912407408003, 2026: 23588.29998921044, 2027: 21560.687571012415, 2028: 19533.075152814854, 2029: 17505.462734616827, 2030: 15477.850316419266, 2031: 13450.23789822124, 2032: 11422.625480023678, 2033: 9395.013061825652, 2034: 7367.400643627625, 2035: 5339.788225430064, 2036: 3312.175807232037, 2037: 1284.5633890344761, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S217" t="n">
+      <c r="T217" t="n">
         <v>281029.6991870091</v>
       </c>
     </row>
@@ -15035,10 +16120,15 @@
       </c>
       <c r="R218" t="inlineStr">
         <is>
+          <t>[ 3.29249799e+02 -3.50103806e+05]</t>
+        </is>
+      </c>
+      <c r="S218" t="inlineStr">
+        <is>
           <t>{2021: 263087.387205743, 2022: 315639.2866946977, 2023: 315968.53649326693, 2024: 316297.7862918363, 2025: 316627.03609040554, 2026: 316956.2858889749, 2027: 317285.53568754415, 2028: 317614.7854861135, 2029: 317944.03528468276, 2030: 318273.285083252, 2031: 318602.53488182137, 2032: 318931.7846803906, 2033: 319261.03447896, 2034: 319590.2842775292, 2035: 319919.5340760986, 2036: 320248.78387466783, 2037: 320578.0336732371, 2038: 320907.28347180644, 2039: 321236.5332703757, 2040: 321565.78306894505, 2041: 321895.0328675143, 2042: 322224.28266608354, 2043: 322553.5324646529, 2044: 322882.78226322215, 2045: 323212.0320617915, 2046: 323541.28186036076, 2047: 323870.5316589301, 2048: 324199.78145749937, 2049: 324529.0312560686, 2050: 324858.281054638}</t>
         </is>
       </c>
-      <c r="S218" t="n">
+      <c r="T218" t="n">
         <v>9256329.28544092</v>
       </c>
     </row>
@@ -15102,10 +16192,15 @@
       </c>
       <c r="R219" t="inlineStr">
         <is>
+          <t>[-1.77358379e+03  3.62337099e+06]</t>
+        </is>
+      </c>
+      <c r="S219" t="inlineStr">
+        <is>
           <t>{2021: 39524.008095575, 2022: 37184.578495761845, 2023: 35410.99470931897, 2024: 33637.41092287609, 2025: 31863.827136432752, 2026: 30090.243349989876, 2027: 28316.659563547, 2028: 26543.075777104124, 2029: 24769.491990660783, 2030: 22995.908204217907, 2031: 21222.32441777503, 2032: 19448.74063133169, 2033: 17675.156844888814, 2034: 15901.573058445938, 2035: 14127.989272003062, 2036: 12354.40548555972, 2037: 10580.821699116845, 2038: 8807.237912673969, 2039: 7033.654126231093, 2040: 5260.070339787751, 2041: 3486.4865533448756, 2042: 1712.9027669019997, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S219" t="n">
+      <c r="T219" t="n">
         <v>428185.5573057577</v>
       </c>
     </row>
@@ -15169,10 +16264,15 @@
       </c>
       <c r="R220" t="inlineStr">
         <is>
+          <t>[-7.73312121e+02  1.63759425e+06]</t>
+        </is>
+      </c>
+      <c r="S220" t="inlineStr">
+        <is>
           <t>{2021: 75194.2350471489, 2022: 73957.14540860173, 2023: 73183.83328762092, 2024: 72410.5211666401, 2025: 71637.20904565929, 2026: 70863.89692467847, 2027: 70090.58480369765, 2028: 69317.27268271684, 2029: 68543.96056173602, 2030: 67770.6484407552, 2031: 66997.33631977439, 2032: 66224.02419879357, 2033: 65450.71207781276, 2034: 64677.39995683194, 2035: 63904.087835851125, 2036: 63130.77571487031, 2037: 62357.463593889726, 2038: 61584.15147290891, 2039: 60810.839351928094, 2040: 60037.52723094728, 2041: 59264.21510996646, 2042: 58490.90298898565, 2043: 57717.59086800483, 2044: 56944.278747024015, 2045: 56170.9666260432, 2046: 55397.65450506238, 2047: 54624.34238408157, 2048: 53851.03026310075, 2049: 53077.718142119935, 2050: 52304.40602113912}</t>
         </is>
       </c>
-      <c r="S220" t="n">
+      <c r="T220" t="n">
         <v>1842237.410244247</v>
       </c>
     </row>
@@ -15236,10 +16336,15 @@
       </c>
       <c r="R221" t="inlineStr">
         <is>
+          <t>[-9.44049220e+02  1.92591414e+06]</t>
+        </is>
+      </c>
+      <c r="S221" t="inlineStr">
+        <is>
           <t>{2021: 18164.1222101262, 2022: 17046.61467460892, 2023: 16102.565454939846, 2024: 15158.516235271003, 2025: 14214.46701560216, 2026: 13270.417795933317, 2027: 12326.368576264242, 2028: 11382.319356595399, 2029: 10438.270136926556, 2030: 9494.220917257713, 2031: 8550.171697588637, 2032: 7606.122477919795, 2033: 6662.073258250952, 2034: 5718.024038582109, 2035: 4773.974818913033, 2036: 3829.9255992441904, 2037: 2885.8763795753475, 2038: 1941.8271599065047, 2039: 997.777940237429, 2040: 53.72872056858614, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S221" t="n">
+      <c r="T221" t="n">
         <v>171535.3233592488</v>
       </c>
     </row>
@@ -15303,10 +16408,15 @@
       </c>
       <c r="R222" t="inlineStr">
         <is>
+          <t>[ 1.18996246e+02 -2.09985679e+05]</t>
+        </is>
+      </c>
+      <c r="S222" t="inlineStr">
+        <is>
           <t>{2021: 32974.0144768152, 2022: 30624.730539163313, 2023: 30743.72678498522, 2024: 30862.72303080713, 2025: 30981.71927662904, 2026: 31100.715522450948, 2027: 31219.711768272857, 2028: 31338.708014094736, 2029: 31457.704259916645, 2030: 31576.700505738554, 2031: 31695.696751560463, 2032: 31814.69299738237, 2033: 31933.68924320428, 2034: 32052.68548902619, 2035: 32171.681734848098, 2036: 32290.677980669978, 2037: 32409.674226491887, 2038: 32528.670472313795, 2039: 32647.666718135704, 2040: 32766.662963957613, 2041: 32885.65920977952, 2042: 33004.65545560143, 2043: 33123.65170142334, 2044: 33242.64794724522, 2045: 33361.64419306713, 2046: 33480.64043888904, 2047: 33599.636684710946, 2048: 33718.632930532855, 2049: 33837.62917635476, 2050: 33956.62542217667}</t>
         </is>
       </c>
-      <c r="S222" t="n">
+      <c r="T222" t="n">
         <v>935938.355966749</v>
       </c>
     </row>
@@ -15370,10 +16480,15 @@
       </c>
       <c r="R223" t="inlineStr">
         <is>
+          <t>[-4.74228378e+03  9.67992124e+06]</t>
+        </is>
+      </c>
+      <c r="S223" t="inlineStr">
+        <is>
           <t>{2021: 95883.4634120662, 2022: 91023.43355966173, 2023: 86281.14977847412, 2024: 81538.86599728651, 2025: 76796.58221609704, 2026: 72054.29843490943, 2027: 67312.01465372182, 2028: 62569.73087253235, 2029: 57827.447091344744, 2030: 53085.163310157135, 2031: 48342.879528967664, 2032: 43600.595747780055, 2033: 38858.311966592446, 2034: 34116.028185402974, 2035: 29373.744404215366, 2036: 24631.460623027757, 2037: 19889.176841840148, 2038: 15146.893060650676, 2039: 10404.609279463068, 2040: 5662.325498275459, 2041: 920.0417170859873, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S223" t="n">
+      <c r="T223" t="n">
         <v>967376.4844735196</v>
       </c>
     </row>
@@ -15437,10 +16552,15 @@
       </c>
       <c r="R224" t="inlineStr">
         <is>
+          <t>[ 1.80129233e+03 -3.54120070e+06]</t>
+        </is>
+      </c>
+      <c r="S224" t="inlineStr">
+        <is>
           <t>{2021: 80120.958481875, 2022: 101012.39203483472, 2023: 102813.68436476216, 2024: 104614.9766946896, 2025: 106416.2690246175, 2026: 108217.56135454495, 2027: 110018.85368447285, 2028: 111820.14601440029, 2029: 113621.4383443282, 2030: 115422.73067425564, 2031: 117224.02300418355, 2032: 119025.31533411099, 2033: 120826.60766403843, 2034: 122627.89999396633, 2035: 124429.19232389377, 2036: 126230.48465382168, 2037: 128031.77698374912, 2038: 129833.06931367703, 2039: 131634.36164360447, 2040: 133435.6539735319, 2041: 135236.94630345982, 2042: 137038.23863338726, 2043: 138839.53096331516, 2044: 140640.8232932426, 2045: 142442.1156231705, 2046: 144243.40795309795, 2047: 146044.70028302586, 2048: 147845.9926129533, 2049: 149647.28494288074, 2050: 151448.57727280864}</t>
         </is>
       </c>
-      <c r="S224" t="n">
+      <c r="T224" t="n">
         <v>3625020.245565359</v>
       </c>
     </row>
@@ -15504,10 +16624,15 @@
       </c>
       <c r="R225" t="inlineStr">
         <is>
+          <t>[-1.87650444e+03  3.83119665e+06]</t>
+        </is>
+      </c>
+      <c r="S225" t="inlineStr">
+        <is>
           <t>{2021: 39625.5755394863, 2022: 36904.67575613689, 2023: 35028.17131542647, 2024: 33151.66687471559, 2025: 31275.16243400518, 2026: 29398.6579932943, 2027: 27522.153552583884, 2028: 25645.64911187347, 2029: 23769.14467116259, 2030: 21892.640230452176, 2031: 20016.135789741296, 2032: 18139.631349030882, 2033: 16263.126908320468, 2034: 14386.622467609588, 2035: 12510.118026899174, 2036: 10633.61358618876, 2037: 8757.10914547788, 2038: 6880.604704767466, 2039: 5004.100264056586, 2040: 3127.5958233461715, 2041: 1251.0913826357573, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S225" t="n">
+      <c r="T225" t="n">
         <v>401370.4591574677</v>
       </c>
     </row>
@@ -15571,10 +16696,15 @@
       </c>
       <c r="R226" t="inlineStr">
         <is>
+          <t>[-1.26121545e+03  2.58523336e+06]</t>
+        </is>
+      </c>
+      <c r="S226" t="inlineStr">
+        <is>
           <t>{2021: 36571.9935715315, 2022: 35055.708996374626, 2023: 33794.49354217108, 2024: 32533.278087968007, 2025: 31272.06263376493, 2026: 30010.847179561853, 2027: 28749.631725358777, 2028: 27488.4162711557, 2029: 26227.200816952623, 2030: 24965.985362749547, 2031: 23704.76990854647, 2032: 22443.554454343393, 2033: 21182.33900013985, 2034: 19921.123545936774, 2035: 18659.908091733698, 2036: 17398.69263753062, 2037: 16137.477183327544, 2038: 14876.261729124468, 2039: 13615.046274921391, 2040: 12353.830820718314, 2041: 11092.615366515238, 2042: 9831.399912312161, 2043: 8570.184458108619, 2044: 7308.969003905542, 2045: 6047.7535497024655, 2046: 4786.538095499389, 2047: 3525.322641296312, 2048: 2264.1071870932356, 2049: 1002.8917328901589, 2050: 0}</t>
         </is>
       </c>
-      <c r="S226" t="n">
+      <c r="T226" t="n">
         <v>523106.4069954685</v>
       </c>
     </row>
@@ -15638,10 +16768,15 @@
       </c>
       <c r="R227" t="inlineStr">
         <is>
+          <t>[-1.62495485e+03  3.31991708e+06]</t>
+        </is>
+      </c>
+      <c r="S227" t="inlineStr">
+        <is>
           <t>{2021: 35500.9478648096, 2022: 34258.368213813286, 2023: 32633.41336054355, 2024: 31008.458507273812, 2025: 29383.503654004075, 2026: 27758.548800734337, 2027: 26133.5939474646, 2028: 24508.639094194863, 2029: 22883.68424092559, 2030: 21258.729387655854, 2031: 19633.774534386117, 2032: 18008.81968111638, 2033: 16383.864827846643, 2034: 14758.909974576905, 2035: 13133.955121307168, 2036: 11509.000268037431, 2037: 9884.04541476816, 2038: 8259.090561498422, 2039: 6634.135708228685, 2040: 5009.180854958948, 2041: 3384.2260016892105, 2042: 1759.2711484194733, 2043: 134.3162951497361, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S227" t="n">
+      <c r="T227" t="n">
         <v>396070.003530998</v>
       </c>
     </row>
@@ -15705,10 +16840,15 @@
       </c>
       <c r="R228" t="inlineStr">
         <is>
+          <t>[-2.00803965e+03  4.09460908e+06]</t>
+        </is>
+      </c>
+      <c r="S228" t="inlineStr">
+        <is>
           <t>{2021: 38584.8137626988, 2022: 34352.89567818493, 2023: 32344.8560235505, 2024: 30336.816368916072, 2025: 28328.77671428118, 2026: 26320.73705964675, 2027: 24312.697405012324, 2028: 22304.657750377897, 2029: 20296.618095743004, 2030: 18288.578441108577, 2031: 16280.53878647415, 2032: 14272.499131839257, 2033: 12264.45947720483, 2034: 10256.419822570402, 2035: 8248.380167935975, 2036: 6240.340513301082, 2037: 4232.300858666655, 2038: 2224.2612040322274, 2039: 216.22154939780012, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S228" t="n">
+      <c r="T228" t="n">
         <v>330414.461929593</v>
       </c>
     </row>
@@ -15772,10 +16912,15 @@
       </c>
       <c r="R229" t="inlineStr">
         <is>
+          <t>[-5.56504665e+02  1.14278790e+06]</t>
+        </is>
+      </c>
+      <c r="S229" t="inlineStr">
+        <is>
           <t>{2021: 18501.3328867235, 2022: 17535.46835323563, 2023: 16978.963688151445, 2024: 16422.459023067495, 2025: 15865.954357983544, 2026: 15309.449692899594, 2027: 14752.945027815644, 2028: 14196.440362731693, 2029: 13639.93569764751, 2030: 13083.43103256356, 2031: 12526.92636747961, 2032: 11970.421702395659, 2033: 11413.917037311709, 2034: 10857.412372227525, 2035: 10300.907707143575, 2036: 9744.403042059625, 2037: 9187.898376975674, 2038: 8631.393711891724, 2039: 8074.889046807773, 2040: 7518.38438172359, 2041: 6961.87971663964, 2042: 6405.375051555689, 2043: 5848.870386471739, 2044: 5292.365721387789, 2045: 4735.861056303838, 2046: 4179.356391219655, 2047: 3622.8517261357047, 2048: 3066.3470610517543, 2049: 2509.842395967804, 2050: 1953.3377308838535}</t>
         </is>
       </c>
-      <c r="S229" t="n">
+      <c r="T229" t="n">
         <v>290861.6857976499</v>
       </c>
     </row>
@@ -15839,10 +16984,15 @@
       </c>
       <c r="R230" t="inlineStr">
         <is>
+          <t>[-1.15178902e+03  2.42227211e+06]</t>
+        </is>
+      </c>
+      <c r="S230" t="inlineStr">
+        <is>
           <t>{2021: 95076.8950230667, 2022: 93354.7234351593, 2023: 92202.93441925291, 2024: 91051.14540334698, 2025: 89899.35638744058, 2026: 88747.56737153418, 2027: 87595.77835562779, 2028: 86443.98933972185, 2029: 85292.20032381546, 2030: 84140.41130790906, 2031: 82988.62229200313, 2032: 81836.83327609673, 2033: 80685.04426019033, 2034: 79533.2552442844, 2035: 78381.466228378, 2036: 77229.67721247161, 2037: 76077.88819656568, 2038: 74926.09918065928, 2039: 73774.31016475288, 2040: 72622.52114884695, 2041: 71470.73213294055, 2042: 70318.94311703416, 2043: 69167.15410112776, 2044: 68015.36508522183, 2045: 66863.57606931543, 2046: 65711.78705340903, 2047: 64559.9980375031, 2048: 63408.209021596704, 2049: 62256.42000569031, 2050: 61104.630989784375}</t>
         </is>
       </c>
-      <c r="S230" t="n">
+      <c r="T230" t="n">
         <v>2256646.771178321</v>
       </c>
     </row>
@@ -15906,10 +17056,15 @@
       </c>
       <c r="R231" t="inlineStr">
         <is>
+          <t>[-3.27321395e+02  6.91987969e+05]</t>
+        </is>
+      </c>
+      <c r="S231" t="inlineStr">
+        <is>
           <t>{2021: 29775.6551819717, 2022: 30144.108102774015, 2023: 29816.78670771187, 2024: 29489.465312649845, 2025: 29162.143917587702, 2026: 28834.82252252556, 2027: 28507.501127463416, 2028: 28180.179732401273, 2029: 27852.85833733913, 2030: 27525.536942276987, 2031: 27198.215547214844, 2032: 26870.8941521527, 2033: 26543.57275709056, 2034: 26216.25136202853, 2035: 25888.92996696639, 2036: 25561.608571904246, 2037: 25234.287176842103, 2038: 24906.96578177996, 2039: 24579.644386717817, 2040: 24252.322991655674, 2041: 23925.00159659353, 2042: 23597.680201531388, 2043: 23270.358806469245, 2044: 22943.03741140722, 2045: 22615.716016345075, 2046: 22288.394621282932, 2047: 21961.07322622079, 2048: 21633.751831158646, 2049: 21306.430436096503, 2050: 20979.10904103436}</t>
         </is>
       </c>
-      <c r="S231" t="n">
+      <c r="T231" t="n">
         <v>745684.921655691</v>
       </c>
     </row>
@@ -15973,10 +17128,15 @@
       </c>
       <c r="R232" t="inlineStr">
         <is>
+          <t>[-2.83207061e+03  5.79445454e+06]</t>
+        </is>
+      </c>
+      <c r="S232" t="inlineStr">
+        <is>
           <t>{2021: 73048.6159903349, 2022: 68007.75621171016, 2023: 65175.68559788447, 2024: 62343.614984058775, 2025: 59511.54437023308, 2026: 56679.473756406456, 2027: 53847.40314258076, 2028: 51015.33252875507, 2029: 48183.261914928444, 2030: 45351.19130110275, 2031: 42519.120687277056, 2032: 39687.05007345136, 2033: 36854.97945962474, 2034: 34022.908845799044, 2035: 31190.83823197335, 2036: 28358.767618146725, 2037: 25526.69700432103, 2038: 22694.626390495338, 2039: 19862.555776669644, 2040: 17030.48516284302, 2041: 14198.414549017325, 2042: 11366.343935191631, 2043: 8534.273321365006, 2044: 5702.2027075393125, 2045: 2870.132093713619, 2046: 38.06147988792509, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S232" t="n">
+      <c r="T232" t="n">
         <v>887097.0291401435</v>
       </c>
     </row>
@@ -16040,10 +17200,15 @@
       </c>
       <c r="R233" t="inlineStr">
         <is>
+          <t>[-3.32323815e+03  6.79224315e+06]</t>
+        </is>
+      </c>
+      <c r="S233" t="inlineStr">
+        <is>
           <t>{2021: 77221.628535876, 2022: 72655.6029271232, 2023: 69332.36477293819, 2024: 66009.12661875226, 2025: 62685.88846456725, 2026: 59362.65031038225, 2027: 56039.41215619631, 2028: 52716.17400201131, 2029: 49392.93584782537, 2030: 46069.697693640366, 2031: 42746.45953945536, 2032: 39423.221385269426, 2033: 36099.98323108442, 2034: 32776.745076898485, 2035: 29453.50692271348, 2036: 26130.268768528476, 2037: 22807.03061434254, 2038: 19483.792460157536, 2039: 16160.5543059716, 2040: 12837.316151786596, 2041: 9514.077997601591, 2042: 6190.839843415655, 2043: 2867.6016892306507, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S233" t="n">
+      <c r="T233" t="n">
         <v>869366.0650478303</v>
       </c>
     </row>
@@ -16107,10 +17272,15 @@
       </c>
       <c r="R234" t="inlineStr">
         <is>
+          <t>[-1.32640019e+03  2.72024230e+06]</t>
+        </is>
+      </c>
+      <c r="S234" t="inlineStr">
+        <is>
           <t>{2021: 39717.4925609034, 2022: 38261.12147500599, 2023: 36934.72128996998, 2024: 35608.32110493397, 2025: 34281.92091989843, 2026: 32955.520734862424, 2027: 31629.120549826417, 2028: 30302.72036479041, 2029: 28976.320179754402, 2030: 27649.91999471886, 2031: 26323.519809682854, 2032: 24997.119624646846, 2033: 23670.71943961084, 2034: 22344.31925457483, 2035: 21017.919069538824, 2036: 19691.518884503283, 2037: 18365.118699467275, 2038: 17038.718514431268, 2039: 15712.31832939526, 2040: 14385.918144359253, 2041: 13059.517959323712, 2042: 11733.117774287704, 2043: 10406.717589251697, 2044: 9080.31740421569, 2045: 7753.917219179682, 2046: 6427.517034144141, 2047: 5101.1168491081335, 2048: 3774.716664072126, 2049: 2448.316479036119, 2050: 1121.9162940001115}</t>
         </is>
       </c>
-      <c r="S234" t="n">
+      <c r="T234" t="n">
         <v>590351.8357840423</v>
       </c>
     </row>
@@ -16174,10 +17344,15 @@
       </c>
       <c r="R235" t="inlineStr">
         <is>
+          <t>[-1.29459984e+03  2.63388808e+06]</t>
+        </is>
+      </c>
+      <c r="S235" t="inlineStr">
+        <is>
           <t>{2021: 18138.2408672054, 2022: 16207.206026570406, 2023: 14912.606186018791, 2024: 13618.00634546671, 2025: 12323.40650491463, 2026: 11028.80666436255, 2027: 9734.206823810935, 2028: 8439.606983258855, 2029: 7145.007142706774, 2030: 5850.407302154694, 2031: 4555.807461603079, 2032: 3261.2076210509986, 2033: 1966.6077804989181, 2034: 672.0079399468377, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S235" t="n">
+      <c r="T235" t="n">
         <v>118784.0112159669</v>
       </c>
     </row>
@@ -16241,10 +17416,15 @@
       </c>
       <c r="R236" t="inlineStr">
         <is>
+          <t>[-2.38668048e+03  4.90032438e+06]</t>
+        </is>
+      </c>
+      <c r="S236" t="inlineStr">
+        <is>
           <t>{2021: 76539.0082403048, 2022: 74456.43899118621, 2023: 72069.75850719959, 2024: 69683.0780232139, 2025: 67296.39753922727, 2026: 64909.717055240646, 2027: 62523.03657125402, 2028: 60136.3560872674, 2029: 57749.675603280775, 2030: 55362.99511929415, 2031: 52976.31463530846, 2032: 50589.634151321836, 2033: 48202.95366733521, 2034: 45816.27318334859, 2035: 43429.592699361965, 2036: 41042.91221537534, 2037: 38656.23173138872, 2038: 36269.551247403026, 2039: 33882.8707634164, 2040: 31496.19027942978, 2041: 29109.509795443155, 2042: 26722.82931145653, 2043: 24336.148827469908, 2044: 21949.468343483284, 2045: 19562.787859497592, 2046: 17176.10737551097, 2047: 14789.426891524345, 2048: 12402.746407537721, 2049: 10016.065923551098, 2050: 7629.385439564474}</t>
         </is>
       </c>
-      <c r="S236" t="n">
+      <c r="T236" t="n">
         <v>1224699.265646263</v>
       </c>
     </row>
@@ -16308,10 +17488,15 @@
       </c>
       <c r="R237" t="inlineStr">
         <is>
+          <t>[-9.24300429e+02  1.89365016e+06]</t>
+        </is>
+      </c>
+      <c r="S237" t="inlineStr">
+        <is>
           <t>{2021: 25684.0025508181, 2022: 24714.69669777667, 2023: 23790.396268501645, 2024: 22866.09583922685, 2025: 21941.795409951825, 2026: 21017.494980676798, 2027: 20093.194551402004, 2028: 19168.894122126978, 2029: 18244.59369285195, 2030: 17320.293263577158, 2031: 16395.99283430213, 2032: 15471.692405027105, 2033: 14547.39197575231, 2034: 13623.091546477284, 2035: 12698.791117202258, 2036: 11774.490687927464, 2037: 10850.190258652437, 2038: 9925.889829377411, 2039: 9001.589400102617, 2040: 8077.288970827591, 2041: 7152.988541552797, 2042: 6228.68811227777, 2043: 5304.387683002744, 2044: 4380.08725372795, 2045: 3455.7868244529236, 2046: 2531.486395177897, 2047: 1607.1859659031034, 2048: 682.8855366280768, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S237" t="n">
+      <c r="T237" t="n">
         <v>355709.3614398728</v>
       </c>
     </row>
@@ -16375,10 +17560,15 @@
       </c>
       <c r="R238" t="inlineStr">
         <is>
+          <t>[ 1.44698890e+03 -2.70853228e+06]</t>
+        </is>
+      </c>
+      <c r="S238" t="inlineStr">
+        <is>
           <t>{2021: 221935.89138647, 2022: 217279.27749661868, 2023: 218726.26639888342, 2024: 220173.25530114863, 2025: 221620.24420341337, 2026: 223067.2331056781, 2027: 224514.22200794285, 2028: 225961.21091020806, 2029: 227408.1998124728, 2030: 228855.18871473754, 2031: 230302.17761700274, 2032: 231749.16651926748, 2033: 233196.15542153222, 2034: 234643.14432379743, 2035: 236090.13322606217, 2036: 237537.1221283269, 2037: 238984.11103059212, 2038: 240431.09993285686, 2039: 241878.0888351216, 2040: 243325.0777373868, 2041: 244772.06663965154, 2042: 246219.05554191628, 2043: 247666.04444418103, 2044: 249113.03334644623, 2045: 250560.02224871097, 2046: 252007.0111509757, 2047: 253454.00005324092, 2048: 254900.98895550566, 2049: 256347.9778577704, 2050: 257794.9667600356}</t>
         </is>
       </c>
-      <c r="S238" t="n">
+      <c r="T238" t="n">
         <v>6870647.004034702</v>
       </c>
     </row>
@@ -16442,10 +17632,15 @@
       </c>
       <c r="R239" t="inlineStr">
         <is>
+          <t>[-1.54054602e+02  3.97020298e+05]</t>
+        </is>
+      </c>
+      <c r="S239" t="inlineStr">
+        <is>
           <t>{2021: 83502.181146889, 2022: 85521.89281031396, 2023: 85367.8382081443, 2024: 85213.78360597458, 2025: 85059.72900380485, 2026: 84905.67440163519, 2027: 84751.61979946546, 2028: 84597.56519729574, 2029: 84443.51059512602, 2030: 84289.45599295635, 2031: 84135.40139078663, 2032: 83981.34678861691, 2033: 83827.29218644724, 2034: 83673.23758427752, 2035: 83519.1829821078, 2036: 83365.12837993813, 2037: 83211.07377776841, 2038: 83057.01917559869, 2039: 82902.96457342897, 2040: 82748.9099712593, 2041: 82594.85536908958, 2042: 82440.80076691986, 2043: 82286.74616475019, 2044: 82132.69156258047, 2045: 81978.63696041075, 2046: 81824.58235824102, 2047: 81670.52775607136, 2048: 81516.47315390164, 2049: 81362.41855173191, 2050: 81208.36394956225}</t>
         </is>
       </c>
-      <c r="S239" t="n">
+      <c r="T239" t="n">
         <v>2418735.631616869</v>
       </c>
     </row>
@@ -16509,10 +17704,15 @@
       </c>
       <c r="R240" t="inlineStr">
         <is>
+          <t>[-1.14608022e+04  2.34509853e+07]</t>
+        </is>
+      </c>
+      <c r="S240" t="inlineStr">
+        <is>
           <t>{2021: 291976.86744178, 2022: 277243.2629548088, 2023: 265782.4607527219, 2024: 254321.6585506387, 2025: 242860.8563485518, 2026: 231400.05414646864, 2027: 219939.25194438174, 2028: 208478.44974229857, 2029: 197017.64754021168, 2030: 185556.8453381285, 2031: 174096.0431360416, 2032: 162635.24093395844, 2033: 151174.43873187155, 2034: 139713.63652978465, 2035: 128252.83432770148, 2036: 116792.03212561458, 2037: 105331.22992353141, 2038: 93870.42772144452, 2039: 82409.62551936135, 2040: 70948.82331727445, 2041: 59488.02111519128, 2042: 48027.218913104385, 2043: 36566.416711021215, 2044: 25105.61450893432, 2045: 13644.812306851149, 2046: 2184.010104764253, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S240" t="n">
+      <c r="T240" t="n">
         <v>3638829.346965551</v>
       </c>
     </row>
@@ -16576,10 +17776,15 @@
       </c>
       <c r="R241" t="inlineStr">
         <is>
+          <t>[-2.21727420e+03  4.54402433e+06]</t>
+        </is>
+      </c>
+      <c r="S241" t="inlineStr">
+        <is>
           <t>{2021: 61795.375408763, 2022: 60695.89867698774, 2023: 58478.62447662093, 2024: 56261.35027625412, 2025: 54044.07607588731, 2026: 51826.8018755205, 2027: 49609.52767515369, 2028: 47392.253474785946, 2029: 45174.979274419136, 2030: 42957.70507405233, 2031: 40740.43087368552, 2032: 38523.15667331871, 2033: 36305.8824729519, 2034: 34088.608272584155, 2035: 31871.334072217345, 2036: 29654.059871850535, 2037: 27436.785671483725, 2038: 25219.511471116915, 2039: 23002.237270750105, 2040: 20784.963070382364, 2041: 18567.688870015554, 2042: 16350.414669648744, 2043: 14133.140469281934, 2044: 11915.866268915124, 2045: 9698.592068548314, 2046: 7481.317868180573, 2047: 5264.043667813763, 2048: 3046.769467446953, 2049: 829.4952670801431, 2050: 0}</t>
         </is>
       </c>
-      <c r="S241" t="n">
+      <c r="T241" t="n">
         <v>892253.2029213356</v>
       </c>
     </row>
@@ -16643,10 +17848,15 @@
       </c>
       <c r="R242" t="inlineStr">
         <is>
+          <t>[ 1.70434291e+04 -3.42858945e+07]</t>
+        </is>
+      </c>
+      <c r="S242" t="inlineStr">
+        <is>
           <t>{2021: 175701.494107733, 2022: 175919.20989701152, 2023: 192962.6390188858, 2024: 210006.06814076751, 2025: 227049.49726264924, 2026: 244092.9263845235, 2027: 261136.35550640523, 2028: 278179.78462828696, 2029: 295223.21375016123, 2030: 312266.64287204295, 2031: 329310.0719939172, 2032: 346353.50111579895, 2033: 363396.9302376807, 2034: 380440.35935955495, 2035: 397483.78848143667, 2036: 414527.2176033184, 2037: 431570.64672519267, 2038: 448614.0758470744, 2039: 465657.50496894866, 2040: 482700.9340908304, 2041: 499744.3632127121, 2042: 516787.7923345864, 2043: 533831.2214564681, 2044: 550874.6505783498, 2045: 567918.0797002241, 2046: 584961.5088221058, 2047: 602004.9379439801, 2048: 619048.3670658618, 2049: 636091.7961877435, 2050: 653135.2253096178}</t>
         </is>
       </c>
-      <c r="S242" t="n">
+      <c r="T242" t="n">
         <v>11782572.44489519</v>
       </c>
     </row>
@@ -16710,10 +17920,15 @@
       </c>
       <c r="R243" t="inlineStr">
         <is>
+          <t>[-3.79028173e+04  7.70867296e+07]</t>
+        </is>
+      </c>
+      <c r="S243" t="inlineStr">
+        <is>
           <t>{2021: 466991.936441858, 2022: 447233.02179344, 2023: 409330.2044853866, 2024: 371427.38717733324, 2025: 333524.56986927986, 2026: 295621.7525612265, 2027: 257718.9352531731, 2028: 219816.11794511974, 2029: 181913.30063706636, 2030: 144010.483329013, 2031: 106107.66602094471, 2032: 68204.84871289134, 2033: 30302.031404837966, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S243" t="n">
+      <c r="T243" t="n">
         <v>3098706.287410642</v>
       </c>
     </row>
@@ -16777,10 +17992,15 @@
       </c>
       <c r="R244" t="inlineStr">
         <is>
+          <t>[-1.27141604e+03  2.60333817e+06]</t>
+        </is>
+      </c>
+      <c r="S244" t="inlineStr">
+        <is>
           <t>{2021: 33989.8922974653, 2022: 32534.943696273025, 2023: 31263.527658886276, 2024: 29992.111621499527, 2025: 28720.69558411278, 2026: 27449.279546725564, 2027: 26177.863509338815, 2028: 24906.447471952066, 2029: 23635.031434565317, 2030: 22363.615397178568, 2031: 21092.19935979182, 2032: 19820.78332240507, 2033: 18549.367285017855, 2034: 17277.951247631107, 2035: 16006.535210244358, 2036: 14735.119172857609, 2037: 13463.70313547086, 2038: 12192.28709808411, 2039: 10920.871060696896, 2040: 9649.455023310147, 2041: 8378.038985923398, 2042: 7106.622948536649, 2043: 5835.2069111499, 2044: 4563.7908737631515, 2045: 3292.374836375937, 2046: 2020.958798989188, 2047: 749.542761602439, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S244" t="n">
+      <c r="T244" t="n">
         <v>449693.2701011151</v>
       </c>
     </row>
@@ -16844,10 +18064,15 @@
       </c>
       <c r="R245" t="inlineStr">
         <is>
+          <t>[-1.49897568e+03  3.04111395e+06]</t>
+        </is>
+      </c>
+      <c r="S245" t="inlineStr">
+        <is>
           <t>{2021: 13009.6628354071, 2022: 10185.11928575486, 2023: 8686.143603522796, 2024: 7187.167921290733, 2025: 5688.19223905867, 2026: 4189.216556826606, 2027: 2690.240874595009, 2028: 1191.2651923629455, 2029: 0, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S245" t="n">
+      <c r="T245" t="n">
         <v>46322.17709111517</v>
       </c>
     </row>
@@ -16911,10 +18136,15 @@
       </c>
       <c r="R246" t="inlineStr">
         <is>
+          <t>[-2.01815819e+03  4.16797023e+06]</t>
+        </is>
+      </c>
+      <c r="S246" t="inlineStr">
+        <is>
           <t>{2021: 89584.2704334941, 2022: 87254.38110717945, 2023: 85236.22292087693, 2024: 83218.06473457394, 2025: 81199.90654827096, 2026: 79181.74836196797, 2027: 77163.59017566545, 2028: 75145.43198936246, 2029: 73127.27380305948, 2030: 71109.11561675649, 2031: 69090.95743045397, 2032: 67072.79924415099, 2033: 65054.641057848, 2034: 63036.48287154501, 2035: 61018.32468524249, 2036: 59000.16649893951, 2037: 56982.00831263652, 2038: 54963.850126333535, 2039: 52945.691940031014, 2040: 50927.53375372803, 2041: 48909.37556742504, 2042: 46891.21738112206, 2043: 44873.059194819536, 2044: 42854.90100851655, 2045: 40836.742822213564, 2046: 38818.58463591058, 2047: 36800.42644960806, 2048: 34782.26826330507, 2049: 32764.110077002086, 2050: 30745.951890699565}</t>
         </is>
       </c>
-      <c r="S246" t="n">
+      <c r="T246" t="n">
         <v>1740423.987740642</v>
       </c>
     </row>
@@ -16978,10 +18208,15 @@
       </c>
       <c r="R247" t="inlineStr">
         <is>
+          <t>[-1.59321480e+03  3.24844982e+06]</t>
+        </is>
+      </c>
+      <c r="S247" t="inlineStr">
+        <is>
           <t>{2021: 29546.2176247229, 2022: 26969.49690903211, 2023: 25376.282107915264, 2024: 23783.067306798883, 2025: 22189.852505682036, 2026: 20596.637704565655, 2027: 19003.42290344881, 2028: 17410.208102331962, 2029: 15816.993301215582, 2030: 14223.778500098735, 2031: 12630.563698982354, 2032: 11037.348897865508, 2033: 9444.134096749127, 2034: 7850.91929563228, 2035: 6257.704494515434, 2036: 4664.489693399053, 2037: 3071.2748922822066, 2038: 1478.0600911658257, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S247" t="n">
+      <c r="T247" t="n">
         <v>256577.3433140423</v>
       </c>
     </row>
@@ -17045,10 +18280,15 @@
       </c>
       <c r="R248" t="inlineStr">
         <is>
+          <t>[-1.15236030e+03  2.38954223e+06]</t>
+        </is>
+      </c>
+      <c r="S248" t="inlineStr">
+        <is>
           <t>{2021: 58851.761582854, 2022: 59469.70359059004, 2023: 58317.34329282213, 2024: 57164.982995054685, 2025: 56012.62269728677, 2026: 54860.26239951886, 2027: 53707.90210175142, 2028: 52555.541803983506, 2029: 51403.181506215595, 2030: 50250.82120844815, 2031: 49098.46091068024, 2032: 47946.10061291233, 2033: 46793.740315144416, 2034: 45641.38001737697, 2035: 44489.01971960906, 2036: 43336.65942184115, 2037: 42184.2991240737, 2038: 41031.93882630579, 2039: 39879.57852853788, 2040: 38727.218230770435, 2041: 37574.857933002524, 2042: 36422.49763523461, 2043: 35270.1373374667, 2044: 34117.77703969926, 2045: 32965.416741931345, 2046: 31813.056444163434, 2047: 30660.69614639599, 2048: 29508.335848628078, 2049: 28355.975550860167, 2050: 27203.61525309272}</t>
         </is>
       </c>
-      <c r="S248" t="n">
+      <c r="T248" t="n">
         <v>1272587.196398278</v>
       </c>
     </row>
@@ -17112,10 +18352,15 @@
       </c>
       <c r="R249" t="inlineStr">
         <is>
+          <t>[-1.69762663e+03  3.45383625e+06]</t>
+        </is>
+      </c>
+      <c r="S249" t="inlineStr">
+        <is>
           <t>{2021: 24562.7675003953, 2022: 21235.194614964537, 2023: 19537.56798189925, 2024: 17839.94134883443, 2025: 16142.314715769142, 2026: 14444.688082703855, 2027: 12747.061449638568, 2028: 11049.43481657328, 2029: 9351.80818350846, 2030: 7654.1815504431725, 2031: 5956.554917377885, 2032: 4258.928284312598, 2033: 2561.3016512473114, 2034: 863.6750181820244, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S249" t="n">
+      <c r="T249" t="n">
         <v>155924.0363656522</v>
       </c>
     </row>
@@ -17179,10 +18424,15 @@
       </c>
       <c r="R250" t="inlineStr">
         <is>
+          <t>[-2.04678596e+03  4.20084887e+06]</t>
+        </is>
+      </c>
+      <c r="S250" t="inlineStr">
+        <is>
           <t>{2021: 64177.5873165772, 2022: 62247.65712211002, 2023: 60200.87116045691, 2024: 58154.085198803805, 2025: 56107.2992371507, 2026: 54060.51327549713, 2027: 52013.72731384402, 2028: 49966.941352190915, 2029: 47920.155390537344, 2030: 45873.36942888424, 2031: 43826.58346723113, 2032: 41779.797505578026, 2033: 39733.011543924455, 2034: 37686.22558227135, 2035: 35639.43962061824, 2036: 33592.65365896467, 2037: 31545.867697311565, 2038: 29499.08173565846, 2039: 27452.295774005353, 2040: 25405.509812351782, 2041: 23358.723850698676, 2042: 21311.93788904557, 2043: 19265.151927392, 2044: 17218.365965738893, 2045: 15171.580004085787, 2046: 13124.79404243268, 2047: 11078.00808077911, 2048: 9031.222119126003, 2049: 6984.436157472897, 2050: 4937.650195819326}</t>
         </is>
       </c>
-      <c r="S250" t="n">
+      <c r="T250" t="n">
         <v>1003806.92467036</v>
       </c>
     </row>
@@ -17246,10 +18496,15 @@
       </c>
       <c r="R251" t="inlineStr">
         <is>
+          <t>[-2.20346391e+03  4.65032028e+06]</t>
+        </is>
+      </c>
+      <c r="S251" t="inlineStr">
+        <is>
           <t>{2021: 191695.965846031, 2022: 194916.25888834894, 2023: 192712.79497997463, 2024: 190509.3310715994, 2025: 188305.86716322508, 2026: 186102.40325485077, 2027: 183898.93934647646, 2028: 181695.47543810215, 2029: 179492.01152972784, 2030: 177288.54762135353, 2031: 175085.08371297922, 2032: 172881.6198046049, 2033: 170678.1558962306, 2034: 168474.6919878563, 2035: 166271.22807948198, 2036: 164067.76417110767, 2037: 161864.30026273336, 2038: 159660.83635435905, 2039: 157457.37244598474, 2040: 155253.9085376095, 2041: 153050.4446292352, 2042: 150846.98072086088, 2043: 148643.51681248657, 2044: 146440.05290411226, 2045: 144236.58899573795, 2046: 142033.12508736365, 2047: 139829.66117898934, 2048: 137626.19727061503, 2049: 135422.73336224072, 2050: 133219.2694538664}</t>
         </is>
       </c>
-      <c r="S251" t="n">
+      <c r="T251" t="n">
         <v>4787203.509158196</v>
       </c>
     </row>
@@ -17313,10 +18568,15 @@
       </c>
       <c r="R252" t="inlineStr">
         <is>
+          <t>[-2.19266621e+02  4.60770627e+05]</t>
+        </is>
+      </c>
+      <c r="S252" t="inlineStr">
+        <is>
           <t>{2021: 18576.8750164496, 2022: 17413.519918653823, 2023: 17194.253297938325, 2024: 16974.986677222827, 2025: 16755.72005650733, 2026: 16536.45343579183, 2027: 16317.186815076333, 2028: 16097.920194360835, 2029: 15878.653573645337, 2030: 15659.386952929839, 2031: 15440.120332214341, 2032: 15220.853711498901, 2033: 15001.587090783403, 2034: 14782.320470067905, 2035: 14563.053849352407, 2036: 14343.78722863691, 2037: 14124.520607921411, 2038: 13905.253987205913, 2039: 13685.987366490415, 2040: 13466.720745774917, 2041: 13247.45412505942, 2042: 13028.187504343921, 2043: 12808.920883628482, 2044: 12589.654262912984, 2045: 12370.387642197486, 2046: 12151.121021481988, 2047: 11931.85440076649, 2048: 11712.587780050992, 2049: 11493.321159335494, 2050: 11274.054538619996}</t>
         </is>
       </c>
-      <c r="S252" t="n">
+      <c r="T252" t="n">
         <v>419621.239869385</v>
       </c>
     </row>
@@ -17380,10 +18640,15 @@
       </c>
       <c r="R253" t="inlineStr">
         <is>
+          <t>[-1.12351277e+03  2.32908259e+06]</t>
+        </is>
+      </c>
+      <c r="S253" t="inlineStr">
+        <is>
           <t>{2021: 58096.946436543, 2022: 57339.76715920167, 2023: 56216.254389686044, 2024: 55092.74162017042, 2025: 53969.22885065479, 2026: 52845.716081139166, 2027: 51722.20331162354, 2028: 50598.690542107914, 2029: 49475.17777259229, 2030: 48351.66500307666, 2031: 47228.152233561035, 2032: 46104.63946404541, 2033: 44981.12669452978, 2034: 43857.61392501416, 2035: 42734.10115549853, 2036: 41610.588385982905, 2037: 40487.07561646728, 2038: 39363.56284695119, 2039: 38240.05007743556, 2040: 37116.537307919934, 2041: 35993.02453840431, 2042: 34869.51176888868, 2043: 33745.998999373056, 2044: 32622.48622985743, 2045: 31498.973460341804, 2046: 30375.460690826178, 2047: 29251.94792131055, 2048: 28128.435151794925, 2049: 27004.9223822793, 2050: 25881.409612763673}</t>
         </is>
       </c>
-      <c r="S253" t="n">
+      <c r="T253" t="n">
         <v>1222814.831605388</v>
       </c>
     </row>
@@ -17447,10 +18712,15 @@
       </c>
       <c r="R254" t="inlineStr">
         <is>
+          <t>[-4.90952220e+03  1.00033085e+07]</t>
+        </is>
+      </c>
+      <c r="S254" t="inlineStr">
+        <is>
           <t>{2021: 85979.9412789594, 2022: 76254.63231541775, 2023: 71345.11011238582, 2024: 66435.5879093539, 2025: 61526.06570632197, 2026: 56616.54350328818, 2027: 51707.02130025625, 2028: 46797.499097224325, 2029: 41887.976894190535, 2030: 36978.45469115861, 2031: 32068.93248812668, 2032: 27159.410285094753, 2033: 22249.888082060963, 2034: 17340.365879029036, 2035: 12430.843675997108, 2036: 7521.321472963318, 2037: 2611.799269931391, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S254" t="n">
+      <c r="T254" t="n">
         <v>673921.4233222803</v>
       </c>
     </row>
@@ -17514,10 +18784,15 @@
       </c>
       <c r="R255" t="inlineStr">
         <is>
+          <t>[-6.58345841e+02  1.35853853e+06]</t>
+        </is>
+      </c>
+      <c r="S255" t="inlineStr">
+        <is>
           <t>{2021: 27988.1283048806, 2022: 27363.24114322639, 2023: 26704.895302629564, 2024: 26046.549462032504, 2025: 25388.203621435678, 2026: 24729.857780838618, 2027: 24071.51194024179, 2028: 23413.16609964473, 2029: 22754.820259047905, 2030: 22096.474418450845, 2031: 21438.12857785402, 2032: 20779.782737257192, 2033: 20121.436896660132, 2034: 19463.091056063306, 2035: 18804.745215466246, 2036: 18146.39937486942, 2037: 17488.05353427236, 2038: 16829.707693675533, 2039: 16171.361853078473, 2040: 15513.016012481647, 2041: 14854.670171884587, 2042: 14196.32433128776, 2043: 13537.9784906907, 2044: 12879.632650093874, 2045: 12221.286809496814, 2046: 11562.940968899988, 2047: 10904.595128302928, 2048: 10246.249287706101, 2049: 9587.903447109275, 2050: 8929.557606512215}</t>
         </is>
       </c>
-      <c r="S255" t="n">
+      <c r="T255" t="n">
         <v>535774.8672203948</v>
       </c>
     </row>
@@ -17581,10 +18856,15 @@
       </c>
       <c r="R256" t="inlineStr">
         <is>
+          <t>[-1.84892379e+03  3.78482225e+06]</t>
+        </is>
+      </c>
+      <c r="S256" t="inlineStr">
+        <is>
           <t>{2021: 48351.5039526337, 2022: 46298.34538530558, 2023: 44449.421592939645, 2024: 42600.49780057371, 2025: 40751.5740082073, 2026: 38902.650215841364, 2027: 37053.726423475426, 2028: 35204.80263110902, 2029: 33355.87883874308, 2030: 31506.955046377145, 2031: 29658.031254011206, 2032: 27809.107461644802, 2033: 25960.183669278864, 2034: 24111.259876912925, 2035: 22262.336084546987, 2036: 20413.412292180583, 2037: 18564.488499814644, 2038: 16715.564707448706, 2039: 14866.640915082302, 2040: 13017.717122716364, 2041: 11168.793330350425, 2042: 9319.869537984487, 2043: 7470.945745618083, 2044: 5622.021953252144, 2045: 3773.0981608862057, 2046: 1924.1743685202673, 2047: 75.25057615386322, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S256" t="n">
+      <c r="T256" t="n">
         <v>627032.4994752919</v>
       </c>
     </row>
@@ -17648,10 +18928,15 @@
       </c>
       <c r="R257" t="inlineStr">
         <is>
+          <t>[-6.36773186e+02  1.31456236e+06]</t>
+        </is>
+      </c>
+      <c r="S257" t="inlineStr">
+        <is>
           <t>{2021: 27235.1355432164, 2022: 27006.980903149582, 2023: 26370.20771686104, 2024: 25733.4345305725, 2025: 25096.66134428419, 2026: 24459.88815799565, 2027: 23823.11497170711, 2028: 23186.3417854188, 2029: 22549.56859913026, 2030: 21912.79541284172, 2031: 21276.02222655341, 2032: 20639.24904026487, 2033: 20002.475853976328, 2034: 19365.70266768802, 2035: 18728.92948139948, 2036: 18092.156295110937, 2037: 17455.383108822396, 2038: 16818.609922534088, 2039: 16181.836736245546, 2040: 15545.063549957005, 2041: 14908.290363668697, 2042: 14271.517177380156, 2043: 13634.743991091615, 2044: 12997.970804803306, 2045: 12361.197618514765, 2046: 11724.424432226224, 2047: 11087.651245937916, 2048: 10450.878059649374, 2049: 9814.104873360833, 2050: 9177.331687072525}</t>
         </is>
       </c>
-      <c r="S257" t="n">
+      <c r="T257" t="n">
         <v>533701.4344862902</v>
       </c>
     </row>
@@ -17715,10 +19000,15 @@
       </c>
       <c r="R258" t="inlineStr">
         <is>
+          <t>[-9.66973762e+02  1.97913155e+06]</t>
+        </is>
+      </c>
+      <c r="S258" t="inlineStr">
+        <is>
           <t>{2021: 24994.5544836964, 2022: 23910.60524038179, 2023: 22943.631478241645, 2024: 21976.6577161015, 2025: 21009.683953961125, 2026: 20042.71019182098, 2027: 19075.736429680837, 2028: 18108.762667540694, 2029: 17141.78890540055, 2030: 16174.815143260173, 2031: 15207.84138112003, 2032: 14240.867618979886, 2033: 13273.893856839743, 2034: 12306.920094699599, 2035: 11339.946332559455, 2036: 10372.972570419079, 2037: 9405.998808278935, 2038: 8439.025046138791, 2039: 7472.051283998648, 2040: 6505.077521858504, 2041: 5538.103759718128, 2042: 4571.129997577984, 2043: 3604.15623543784, 2044: 2637.1824732976966, 2045: 1670.208711157553, 2046: 703.2349490171764, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S258" t="n">
+      <c r="T258" t="n">
         <v>320170.2796093365</v>
       </c>
     </row>
@@ -17782,10 +19072,15 @@
       </c>
       <c r="R259" t="inlineStr">
         <is>
+          <t>[ 3.70486862e+03 -7.23348382e+06]</t>
+        </is>
+      </c>
+      <c r="S259" t="inlineStr">
+        <is>
           <t>{2021: 244532.808764144, 2022: 257760.53108856548, 2023: 261465.39970888477, 2024: 265170.268329205, 2025: 268875.1369495252, 2026: 272580.0055698445, 2027: 276284.87419016473, 2028: 279989.74281048495, 2029: 283694.61143080425, 2030: 287399.48005112447, 2031: 291104.3486714447, 2032: 294809.2172917649, 2033: 298514.0859120842, 2034: 302218.95453240443, 2035: 305923.82315272465, 2036: 309628.69177304395, 2037: 313333.56039336417, 2038: 317038.4290136844, 2039: 320743.2976340046, 2040: 324448.1662543239, 2041: 328153.03487464413, 2042: 331857.90349496435, 2043: 335562.77211528365, 2044: 339267.64073560387, 2045: 342972.5093559241, 2046: 346677.3779762443, 2047: 350382.2465965636, 2048: 354087.11521688383, 2049: 357791.98383720405, 2050: 361496.85245752335}</t>
         </is>
       </c>
-      <c r="S259" t="n">
+      <c r="T259" t="n">
         <v>8920750.039571594</v>
       </c>
     </row>
@@ -17849,10 +19144,15 @@
       </c>
       <c r="R260" t="inlineStr">
         <is>
+          <t>[-4.26275823e+02  8.79358655e+05]</t>
+        </is>
+      </c>
+      <c r="S260" t="inlineStr">
+        <is>
           <t>{2021: 17672.8918327639, 2022: 17428.940660738386, 2023: 17002.664837648044, 2024: 16576.38901455782, 2025: 16150.113191467477, 2026: 15723.837368377252, 2027: 15297.56154528691, 2028: 14871.285722196684, 2029: 14445.009899106342, 2030: 14018.734076016, 2031: 13592.458252925775, 2032: 13166.182429835433, 2033: 12739.906606745208, 2034: 12313.630783654866, 2035: 11887.35496056464, 2036: 11461.079137474298, 2037: 11034.803314384073, 2038: 10608.527491293731, 2039: 10182.251668203506, 2040: 9755.975845113164, 2041: 9329.700022022938, 2042: 8903.424198932596, 2043: 8477.148375842371, 2044: 8050.872552752029, 2045: 7624.596729661804, 2046: 7198.320906571462, 2047: 6772.045083481236, 2048: 6345.7692603908945, 2049: 5919.493437300553, 2050: 5493.217614210327}</t>
         </is>
       </c>
-      <c r="S260" t="n">
+      <c r="T260" t="n">
         <v>338461.1320960326</v>
       </c>
     </row>
@@ -17916,10 +19216,15 @@
       </c>
       <c r="R261" t="inlineStr">
         <is>
+          <t>[-5.05709221e+02  1.11038170e+06]</t>
+        </is>
+      </c>
+      <c r="S261" t="inlineStr">
+        <is>
           <t>{2021: 89825.1859719511, 2022: 87837.65480462764, 2023: 87331.94558334316, 2024: 86826.23636205879, 2025: 86320.5271407743, 2026: 85814.81791948981, 2027: 85309.10869820544, 2028: 84803.39947692095, 2029: 84297.69025563658, 2030: 83791.9810343521, 2031: 83286.27181306761, 2032: 82780.56259178324, 2033: 82274.85337049875, 2034: 81769.14414921426, 2035: 81263.43492792989, 2036: 80757.7257066454, 2037: 80252.01648536103, 2038: 79746.30726407655, 2039: 79240.59804279206, 2040: 78734.88882150769, 2041: 78229.1796002232, 2042: 77723.47037893883, 2043: 77217.76115765434, 2044: 76712.05193636985, 2045: 76206.34271508548, 2046: 75700.633493801, 2047: 75194.92427251663, 2048: 74689.21505123214, 2049: 74183.50582994765, 2050: 73677.79660866328}</t>
         </is>
       </c>
-      <c r="S261" t="n">
+      <c r="T261" t="n">
         <v>2350047.740174362</v>
       </c>
     </row>
@@ -17983,10 +19288,15 @@
       </c>
       <c r="R262" t="inlineStr">
         <is>
+          <t>[-2.41078127e+03  4.98684095e+06]</t>
+        </is>
+      </c>
+      <c r="S262" t="inlineStr">
+        <is>
           <t>{2021: 113560.106743427, 2022: 112241.21947505511, 2023: 109830.43820479978, 2024: 107419.65693454538, 2025: 105008.87566429097, 2026: 102598.09439403564, 2027: 100187.31312378123, 2028: 97776.5318535259, 2029: 95365.7505832715, 2030: 92954.96931301709, 2031: 90544.18804276176, 2032: 88133.40677250735, 2033: 85722.62550225202, 2034: 83311.84423199762, 2035: 80901.06296174228, 2036: 78490.28169148788, 2037: 76079.50042123348, 2038: 73668.71915097814, 2039: 71257.93788072374, 2040: 68847.1566104684, 2041: 66436.375340214, 2042: 64025.594069959596, 2043: 61614.81279970426, 2044: 59204.03152944986, 2045: 56793.25025919452, 2046: 54382.46898894012, 2047: 51971.687718684785, 2048: 49560.90644843038, 2049: 47150.12517817598, 2050: 44739.343907920644}</t>
         </is>
       </c>
-      <c r="S262" t="n">
+      <c r="T262" t="n">
         <v>2310628.550470903</v>
       </c>
     </row>
@@ -18050,10 +19360,15 @@
       </c>
       <c r="R263" t="inlineStr">
         <is>
+          <t>[-4.28562990e+03  8.77022965e+06]</t>
+        </is>
+      </c>
+      <c r="S263" t="inlineStr">
+        <is>
           <t>{2021: 113249.74480656, 2022: 104685.99533880316, 2023: 100400.3654416278, 2024: 96114.73554445244, 2025: 91829.10564727709, 2026: 87543.47575010173, 2027: 83257.84585292451, 2028: 78972.21595574915, 2029: 74686.5860585738, 2030: 70400.95616139844, 2031: 66115.32626422308, 2032: 61829.696367045864, 2033: 57544.06646987051, 2034: 53258.43657269515, 2035: 48972.806675519794, 2036: 44687.17677834444, 2037: 40401.54688116722, 2038: 36115.91698399186, 2039: 31830.287086816505, 2040: 27544.657189641148, 2041: 23259.02729246393, 2042: 18973.39739528857, 2043: 14687.767498113215, 2044: 10402.137600937858, 2045: 6116.5077037625015, 2046: 1830.877806585282, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S263" t="n">
+      <c r="T263" t="n">
         <v>1388085.786720655</v>
       </c>
     </row>
@@ -18117,10 +19432,15 @@
       </c>
       <c r="R264" t="inlineStr">
         <is>
+          <t>[-1.05215314e+04  2.16890944e+07]</t>
+        </is>
+      </c>
+      <c r="S264" t="inlineStr">
+        <is>
           <t>{2021: 432745.081804335, 2022: 414557.803280022, 2023: 404036.27183391526, 2024: 393514.74038781226, 2025: 382993.2089417055, 2026: 372471.6774956025, 2027: 361950.1460494958, 2028: 351428.6146033928, 2029: 340907.08315728605, 2030: 330385.55171118304, 2031: 319864.0202650763, 2032: 309342.4888189696, 2033: 298820.9573728666, 2034: 288299.42592675984, 2035: 277777.89448065683, 2036: 267256.3630345501, 2037: 256734.8315884471, 2038: 246213.30014234036, 2039: 235691.76869623736, 2040: 225170.23725013062, 2041: 214648.70580402762, 2042: 204127.17435792089, 2043: 193605.64291181788, 2044: 183084.11146571115, 2045: 172562.58001960814, 2046: 162041.0485735014, 2047: 151519.5171273984, 2048: 140997.98568129167, 2049: 130476.45423518494, 2050: 119954.92278908193}</t>
         </is>
       </c>
-      <c r="S264" t="n">
+      <c r="T264" t="n">
         <v>7906829.60750962</v>
       </c>
     </row>
@@ -18184,10 +19504,15 @@
       </c>
       <c r="R265" t="inlineStr">
         <is>
+          <t>[-8.27758565e+03  1.68643014e+07]</t>
+        </is>
+      </c>
+      <c r="S265" t="inlineStr">
+        <is>
           <t>{2021: 130580.639700426, 2022: 127023.2412871588, 2023: 118745.65563288704, 2024: 110468.06997861527, 2025: 102190.4843243435, 2026: 93912.89867007174, 2027: 85635.31301579997, 2028: 77357.72736152634, 2029: 69080.14170725644, 2030: 60802.55605298281, 2031: 52524.9703987129, 2032: 44247.384744439274, 2033: 35969.79909016937, 2034: 27692.21343589574, 2035: 19414.627781625837, 2036: 11137.042127352208, 2037: 2859.456473082304, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S265" t="n">
+      <c r="T265" t="n">
         <v>1104351.901932132</v>
       </c>
     </row>
@@ -18251,10 +19576,15 @@
       </c>
       <c r="R266" t="inlineStr">
         <is>
+          <t>[-1.28304936e+03  2.63687249e+06]</t>
+        </is>
+      </c>
+      <c r="S266" t="inlineStr">
+        <is>
           <t>{2021: 44254.4045734121, 2022: 42546.69280240452, 2023: 41263.643444984686, 2024: 39980.59408756439, 2025: 38697.54473014409, 2026: 37414.49537272379, 2027: 36131.44601530349, 2028: 34848.396657883655, 2029: 33565.347300463356, 2030: 32282.297943043057, 2031: 30999.248585622758, 2032: 29716.19922820246, 2033: 28433.14987078216, 2034: 27150.100513362326, 2035: 25867.051155942027, 2036: 24584.001798521727, 2037: 23300.952441101428, 2038: 22017.90308368113, 2039: 20734.85372626083, 2040: 19451.804368840996, 2041: 18168.755011420697, 2042: 16885.705654000398, 2043: 15602.656296580099, 2044: 14319.6069391598, 2045: 13036.5575817395, 2046: 11753.508224319667, 2047: 10470.458866899367, 2048: 9187.409509479068, 2049: 7904.360152058769, 2050: 6621.31079463847}</t>
         </is>
       </c>
-      <c r="S266" t="n">
+      <c r="T266" t="n">
         <v>731752.5990465155</v>
       </c>
     </row>
@@ -18318,10 +19648,15 @@
       </c>
       <c r="R267" t="inlineStr">
         <is>
+          <t>[-7.08164268e+02  1.44267411e+06]</t>
+        </is>
+      </c>
+      <c r="S267" t="inlineStr">
+        <is>
           <t>{2021: 11651.4229570806, 2022: 10765.957601174014, 2023: 10057.793333124602, 2024: 9349.629065075424, 2025: 8641.464797026245, 2026: 7933.300528977066, 2027: 7225.136260927655, 2028: 6516.971992878476, 2029: 5808.8077248292975, 2030: 5100.643456780119, 2031: 4392.479188730707, 2032: 3684.3149206815287, 2033: 2976.15065263235, 2034: 2267.9863845831715, 2035: 1559.82211653376, 2036: 851.6578484845813, 2037: 143.4935804354027, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S267" t="n">
+      <c r="T267" t="n">
         <v>93101.3209314147</v>
       </c>
     </row>
@@ -18385,10 +19720,15 @@
       </c>
       <c r="R268" t="inlineStr">
         <is>
+          <t>[-3.04059918e+03  6.20700829e+06]</t>
+        </is>
+      </c>
+      <c r="S268" t="inlineStr">
+        <is>
           <t>{2021: 63515.5467990261, 2022: 58916.75698980875, 2023: 55876.157814805396, 2024: 52835.55863980111, 2025: 49794.95946479775, 2026: 46754.36028979346, 2027: 43713.761114790104, 2028: 40673.161939785816, 2029: 37632.56276478246, 2030: 34591.96358977817, 2031: 31551.364414774813, 2032: 28510.765239771456, 2033: 25470.166064767167, 2034: 22429.56688976381, 2035: 19388.96771475952, 2036: 16348.368539756164, 2037: 13307.769364751875, 2038: 10267.170189748518, 2039: 7226.57101474423, 2040: 4185.971839740872, 2041: 1145.3726647365838, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S268" t="n">
+      <c r="T268" t="n">
         <v>632379.069944971</v>
       </c>
     </row>
@@ -18452,10 +19792,15 @@
       </c>
       <c r="R269" t="inlineStr">
         <is>
+          <t>[-1.77850590e+03  3.64301075e+06]</t>
+        </is>
+      </c>
+      <c r="S269" t="inlineStr">
+        <is>
           <t>{2021: 49230.8804101019, 2022: 46871.820241840556, 2023: 45093.31434197351, 2024: 43314.808442106936, 2025: 41536.30254223989, 2026: 39757.79664237285, 2027: 37979.29074250581, 2028: 36200.784842638765, 2029: 34422.27894277172, 2030: 32643.77304290468, 2031: 30865.2671430381, 2032: 29086.76124317106, 2033: 27308.255343304016, 2034: 25529.749443436973, 2035: 23751.24354356993, 2036: 21972.737643702887, 2037: 20194.231743835844, 2038: 18415.725843969267, 2039: 16637.219944102224, 2040: 14858.714044235181, 2041: 13080.208144368138, 2042: 11301.702244501095, 2043: 9523.196344634052, 2044: 7744.6904447670095, 2045: 5966.184544900432, 2046: 4187.678645033389, 2047: 2409.1727451663464, 2048: 630.6668452993035, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S269" t="n">
+      <c r="T269" t="n">
         <v>665899.015881441</v>
       </c>
     </row>
@@ -18519,10 +19864,15 @@
       </c>
       <c r="R270" t="inlineStr">
         <is>
+          <t>[-1.74985786e+03  3.56866561e+06]</t>
+        </is>
+      </c>
+      <c r="S270" t="inlineStr">
+        <is>
           <t>{2021: 33344.2790431293, 2022: 30453.012721930165, 2023: 28703.154857493937, 2024: 26953.296993057244, 2025: 25203.439128621016, 2026: 23453.581264184322, 2027: 21703.723399748094, 2028: 19953.8655353114, 2029: 18204.007670875173, 2030: 16454.14980643848, 2031: 14704.291942002252, 2032: 12954.434077565558, 2033: 11204.57621312933, 2034: 9454.718348693103, 2035: 7704.860484256409, 2036: 5955.002619820181, 2037: 4205.144755383488, 2038: 2455.28689094726, 2039: 705.4290265105665, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S270" t="n">
+      <c r="T270" t="n">
         <v>297098.1152575326</v>
       </c>
     </row>
@@ -18586,10 +19936,15 @@
       </c>
       <c r="R271" t="inlineStr">
         <is>
+          <t>[-1.73542882e+03  3.52718436e+06]</t>
+        </is>
+      </c>
+      <c r="S271" t="inlineStr">
+        <is>
           <t>{2021: 21794.3737869597, 2022: 18147.294181198813, 2023: 16411.8653651271, 2024: 14676.436549054924, 2025: 12941.007732983213, 2026: 11205.578916911036, 2027: 9470.150100839324, 2028: 7734.721284767147, 2029: 5999.292468695436, 2030: 4263.8636526232585, 2031: 2528.4348365510814, 2032: 793.0060204793699, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S271" t="n">
+      <c r="T271" t="n">
         <v>115068.8380027105</v>
       </c>
     </row>
@@ -18653,10 +20008,15 @@
       </c>
       <c r="R272" t="inlineStr">
         <is>
+          <t>[-4.38367708e+02  9.09412045e+05]</t>
+        </is>
+      </c>
+      <c r="S272" t="inlineStr">
+        <is>
           <t>{2021: 23006.9546629168, 2022: 23032.539706559386, 2023: 22594.17199874553, 2024: 22155.804290931672, 2025: 21717.43658311793, 2026: 21279.068875304074, 2027: 20840.701167490217, 2028: 20402.333459676476, 2029: 19963.96575186262, 2030: 19525.598044048762, 2031: 19087.230336234905, 2032: 18648.862628421164, 2033: 18210.494920607307, 2034: 17772.12721279345, 2035: 17333.759504979593, 2036: 16895.391797165852, 2037: 16457.024089351995, 2038: 16018.656381538138, 2039: 15580.288673724397, 2040: 15141.92096591054, 2041: 14703.553258096683, 2042: 14265.185550282826, 2043: 13826.817842469085, 2044: 13388.450134655228, 2045: 12950.08242684137, 2046: 12511.714719027514, 2047: 12073.347011213773, 2048: 11634.979303399916, 2049: 11196.611595586059, 2050: 10758.243887772318}</t>
         </is>
       </c>
-      <c r="S272" t="n">
+      <c r="T272" t="n">
         <v>496090.717505381</v>
       </c>
     </row>
@@ -18720,10 +20080,15 @@
       </c>
       <c r="R273" t="inlineStr">
         <is>
+          <t>[-5.77373212e+03  1.17928953e+07]</t>
+        </is>
+      </c>
+      <c r="S273" t="inlineStr">
+        <is>
           <t>{2021: 120399.758867021, 2022: 118408.94764437713, 2023: 112635.21552699618, 2024: 106861.4834096171, 2025: 101087.75129223615, 2026: 95314.01917485707, 2027: 89540.28705747612, 2028: 83766.55494009703, 2029: 77992.82282271609, 2030: 72219.09070533514, 2031: 66445.35858795606, 2032: 60671.62647057511, 2033: 54897.894353196025, 2034: 49124.16223581508, 2035: 43350.43011843413, 2036: 37576.69800105505, 2037: 31802.9658836741, 2038: 26029.233766295016, 2039: 20255.50164891407, 2040: 14481.769531534985, 2041: 8708.037414154038, 2042: 2934.305296773091, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S273" t="n">
+      <c r="T273" t="n">
         <v>1334304.035315595</v>
       </c>
     </row>
@@ -18787,10 +20152,15 @@
       </c>
       <c r="R274" t="inlineStr">
         <is>
+          <t>[-7.16491826e+02  1.47766679e+06]</t>
+        </is>
+      </c>
+      <c r="S274" t="inlineStr">
+        <is>
           <t>{2021: 29559.2865580057, 2022: 28920.31515496457, 2023: 28203.82332932297, 2024: 27487.331503681373, 2025: 26770.839678040007, 2026: 26054.34785239841, 2027: 25337.856026757043, 2028: 24621.364201115444, 2029: 23904.87237547408, 2030: 23188.38054983248, 2031: 22471.888724191114, 2032: 21755.396898549516, 2033: 21038.905072907917, 2034: 20322.41324726655, 2035: 19605.921421624953, 2036: 18889.429595983587, 2037: 18172.93777034199, 2038: 17456.445944700623, 2039: 16739.954119059024, 2040: 16023.462293417426, 2041: 15306.97046777606, 2042: 14590.478642134462, 2043: 13873.986816493096, 2044: 13157.494990851497, 2045: 12441.003165210132, 2046: 11724.511339568533, 2047: 11008.019513927167, 2048: 10291.527688285569, 2049: 9575.03586264397, 2050: 8858.544037002604}</t>
         </is>
       </c>
-      <c r="S274" t="n">
+      <c r="T274" t="n">
         <v>558143.8295440237</v>
       </c>
     </row>
@@ -18854,10 +20224,15 @@
       </c>
       <c r="R275" t="inlineStr">
         <is>
+          <t>[-1.48223074e+03  3.05709778e+06]</t>
+        </is>
+      </c>
+      <c r="S275" t="inlineStr">
+        <is>
           <t>{2021: 64215.5717053796, 2022: 60027.22272345144, 2023: 58544.99198178435, 2024: 57062.76124011772, 2025: 55580.53049845109, 2026: 54098.29975678399, 2027: 52616.06901511736, 2028: 51133.83827345027, 2029: 49651.60753178364, 2030: 48169.37679011701, 2031: 46687.14604844991, 2032: 45204.91530678328, 2033: 43722.68456511665, 2034: 42240.453823449556, 2035: 40758.223081782926, 2036: 39275.99234011583, 2037: 37793.7615984492, 2038: 36311.53085678257, 2039: 34829.300115115475, 2040: 33347.069373448845, 2041: 31864.838631782215, 2042: 30382.60789011512, 2043: 28900.37714844849, 2044: 27418.146406781394, 2045: 25935.915665114764, 2046: 24453.684923448134, 2047: 22971.45418178104, 2048: 21489.22344011441, 2049: 20006.99269844778, 2050: 18524.761956780683}</t>
         </is>
       </c>
-      <c r="S275" t="n">
+      <c r="T275" t="n">
         <v>1161849.182737665</v>
       </c>
     </row>
@@ -18921,10 +20296,15 @@
       </c>
       <c r="R276" t="inlineStr">
         <is>
+          <t>[-4.40835991e+03  8.93300498e+06]</t>
+        </is>
+      </c>
+      <c r="S276" t="inlineStr">
+        <is>
           <t>{2021: 27256.1945967649, 2022: 19301.244344605133, 2023: 14892.884435448796, 2024: 10484.524526292458, 2025: 6076.164617137983, 2026: 1667.804707981646, 2027: 0, 2028: 0, 2029: 0, 2030: 0, 2031: 0, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S276" t="n">
+      <c r="T276" t="n">
         <v>66050.71992984846</v>
       </c>
     </row>
@@ -18988,10 +20368,15 @@
       </c>
       <c r="R277" t="inlineStr">
         <is>
+          <t>[-1.16735845e+03  2.39693295e+06]</t>
+        </is>
+      </c>
+      <c r="S277" t="inlineStr">
+        <is>
           <t>{2021: 38379.083489963, 2022: 36534.16298870416, 2023: 35366.80453846371, 2024: 34199.44608822325, 2025: 33032.08763798233, 2026: 31864.729187741876, 2027: 30697.37073750142, 2028: 29530.012287260965, 2029: 28362.65383702051, 2030: 27195.295386779588, 2031: 26027.936936539132, 2032: 24860.578486298677, 2033: 23693.22003605822, 2034: 22525.861585817765, 2035: 21358.503135576844, 2036: 20191.14468533639, 2037: 19023.786235095933, 2038: 17856.427784855478, 2039: 16689.069334615022, 2040: 15521.710884374566, 2041: 14354.352434133645, 2042: 13186.99398389319, 2043: 12019.635533652734, 2044: 10852.277083412278, 2045: 9684.918633171823, 2046: 8517.560182930902, 2047: 7350.201732690446, 2048: 6182.8432824499905, 2049: 5015.484832209535, 2050: 3848.1263819690794}</t>
         </is>
       </c>
-      <c r="S277" t="n">
+      <c r="T277" t="n">
         <v>602808.6744287563</v>
       </c>
     </row>
@@ -19055,10 +20440,15 @@
       </c>
       <c r="R278" t="inlineStr">
         <is>
+          <t>[-4.92667965e+02  1.01717596e+06]</t>
+        </is>
+      </c>
+      <c r="S278" t="inlineStr">
+        <is>
           <t>{2021: 21601.5547051383, 2022: 21001.33928079193, 2023: 20508.67131592054, 2024: 20016.00335104915, 2025: 19523.335386177758, 2026: 19030.667421306483, 2027: 18537.999456435093, 2028: 18045.331491563702, 2029: 17552.66352669231, 2030: 17059.99556182092, 2031: 16567.327596949646, 2032: 16074.659632078256, 2033: 15581.991667206865, 2034: 15089.323702335474, 2035: 14596.655737464083, 2036: 14103.987772592809, 2037: 13611.319807721418, 2038: 13118.651842850028, 2039: 12625.983877978637, 2040: 12133.315913107246, 2041: 11640.647948235972, 2042: 11147.979983364581, 2043: 10655.31201849319, 2044: 10162.6440536218, 2045: 9669.976088750409, 2046: 9177.308123879135, 2047: 8684.640159007744, 2048: 8191.972194136353, 2049: 7699.3042292649625, 2050: 7206.636264393572}</t>
         </is>
       </c>
-      <c r="S278" t="n">
+      <c r="T278" t="n">
         <v>416213.1046255624</v>
       </c>
     </row>
@@ -19122,10 +20512,15 @@
       </c>
       <c r="R279" t="inlineStr">
         <is>
+          <t>[-2.30308193e+03  4.69940721e+06]</t>
+        </is>
+      </c>
+      <c r="S279" t="inlineStr">
+        <is>
           <t>{2021: 45865.6598646384, 2022: 42575.54111571144, 2023: 40272.4591843579, 2024: 37969.37725300435, 2025: 35666.2953216508, 2026: 33363.21339029726, 2027: 31060.13145894371, 2028: 28757.049527590163, 2029: 26453.967596236616, 2030: 24150.88566488307, 2031: 21847.803733529523, 2032: 19544.721802175976, 2033: 17241.63987082243, 2034: 14938.557939468883, 2035: 12635.476008115336, 2036: 10332.39407676179, 2037: 8029.312145408243, 2038: 5726.230214054696, 2039: 3423.1482827011496, 2040: 1120.066351347603, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S279" t="n">
+      <c r="T279" t="n">
         <v>438041.1008693802</v>
       </c>
     </row>
@@ -19189,10 +20584,15 @@
       </c>
       <c r="R280" t="inlineStr">
         <is>
+          <t>[-1.53209106e+03  3.11828183e+06]</t>
+        </is>
+      </c>
+      <c r="S280" t="inlineStr">
+        <is>
           <t>{2021: 22521.1005462786, 2022: 20393.716080020647, 2023: 18861.625023625325, 2024: 17329.53396723047, 2025: 15797.442910835147, 2026: 14265.351854439825, 2027: 12733.260798044968, 2028: 11201.169741649646, 2029: 9669.07868525479, 2030: 8136.987628859468, 2031: 6604.896572464146, 2032: 5072.805516069289, 2033: 3540.714459673967, 2034: 2008.6234032791108, 2035: 476.5323468837887, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S280" t="n">
+      <c r="T280" t="n">
         <v>157352.2892614699</v>
       </c>
     </row>
@@ -19256,10 +20656,15 @@
       </c>
       <c r="R281" t="inlineStr">
         <is>
+          <t>[-8.97211056e+02  1.83958134e+06]</t>
+        </is>
+      </c>
+      <c r="S281" t="inlineStr">
+        <is>
           <t>{2021: 25201.3309250789, 2022: 25420.580852974905, 2023: 24523.36979712732, 2024: 23626.158741279505, 2025: 22728.94768543169, 2026: 21831.736629583873, 2027: 20934.525573736057, 2028: 20037.31451788824, 2029: 19140.103462040424, 2030: 18242.89240619284, 2031: 17345.681350345025, 2032: 16448.47029449721, 2033: 15551.259238649393, 2034: 14654.048182801576, 2035: 13756.83712695376, 2036: 12859.626071105944, 2037: 11962.41501525836, 2038: 11065.203959410544, 2039: 10167.992903562728, 2040: 9270.781847714912, 2041: 8373.570791867096, 2042: 7476.35973601928, 2043: 6579.148680171464, 2044: 5681.9376243236475, 2045: 4784.726568476064, 2046: 3887.515512628248, 2047: 2990.304456780432, 2048: 2093.0934009326156, 2049: 1195.8823450847995, 2050: 298.6712892369833}</t>
         </is>
       </c>
-      <c r="S281" t="n">
+      <c r="T281" t="n">
         <v>385380.4858799959</v>
       </c>
     </row>
@@ -19323,10 +20728,15 @@
       </c>
       <c r="R282" t="inlineStr">
         <is>
+          <t>[-2.13007949e+03  4.35561876e+06]</t>
+        </is>
+      </c>
+      <c r="S282" t="inlineStr">
+        <is>
           <t>{2021: 51341.8145557251, 2022: 48598.024286033586, 2023: 46467.94479240291, 2024: 44337.86529877316, 2025: 42207.785805142485, 2026: 40077.70631151181, 2027: 37947.62681788206, 2028: 35817.54732425138, 2029: 33687.46783062164, 2030: 31557.38833699096, 2031: 29427.308843360282, 2032: 27297.229349730536, 2033: 25167.14985609986, 2034: 23037.070362470113, 2035: 20906.990868839435, 2036: 18776.911375208758, 2037: 16646.83188157901, 2038: 14516.752387948334, 2039: 12386.672894317657, 2040: 10256.59340068791, 2041: 8126.513907057233, 2042: 5996.434413427487, 2043: 3866.3549197968096, 2044: 1736.275426166132, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S282" t="n">
+      <c r="T282" t="n">
         <v>604515.3539681621</v>
       </c>
     </row>
@@ -19390,10 +20800,15 @@
       </c>
       <c r="R283" t="inlineStr">
         <is>
+          <t>[-1.29200115e+04  2.64080779e+07]</t>
+        </is>
+      </c>
+      <c r="S283" t="inlineStr">
+        <is>
           <t>{2021: 321310.710146619, 2022: 283814.66819117963, 2023: 270894.65672452375, 2024: 257974.64525786787, 2025: 245054.63379121572, 2026: 232134.62232455984, 2027: 219214.61085790396, 2028: 206294.59939124808, 2029: 193374.5879245922, 2030: 180454.57645793632, 2031: 167534.56499128044, 2032: 154614.55352462456, 2033: 141694.54205796868, 2034: 128774.5305913128, 2035: 115854.51912466064, 2036: 102934.50765800476, 2037: 90014.49619134888, 2038: 77094.484724693, 2039: 64174.47325803712, 2040: 51254.46179138124, 2041: 38334.45032472536, 2042: 25414.43885806948, 2043: 12494.4273914136, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S283" t="n">
+      <c r="T283" t="n">
         <v>3420055.406481857</v>
       </c>
     </row>
@@ -19457,10 +20872,15 @@
       </c>
       <c r="R284" t="inlineStr">
         <is>
+          <t>[-9.83643010e+02  2.04566353e+06]</t>
+        </is>
+      </c>
+      <c r="S284" t="inlineStr">
+        <is>
           <t>{2021: 58028.5562909162, 2022: 56737.3606419689, 2023: 55753.71763164108, 2024: 54770.074621313484, 2025: 53786.43161098589, 2026: 52802.78860065807, 2027: 51819.145590330474, 2028: 50835.50258000288, 2029: 49851.859569675056, 2030: 48868.216559347464, 2031: 47884.57354901987, 2032: 46900.93053869228, 2033: 45917.28752836445, 2034: 44933.64451803686, 2035: 43950.00150770927, 2036: 42966.35849738144, 2037: 41982.71548705385, 2038: 40999.07247672626, 2039: 40015.429466398666, 2040: 39031.78645607084, 2041: 38048.14344574325, 2042: 37064.500435415655, 2043: 36080.85742508783, 2044: 35097.21441476024, 2045: 34113.571404432645, 2046: 33129.92839410505, 2047: 32146.285383777227, 2048: 31162.642373449635, 2049: 30178.999363122042, 2050: 29195.356352794217}</t>
         </is>
       </c>
-      <c r="S284" t="n">
+      <c r="T284" t="n">
         <v>1260440.996393126</v>
       </c>
     </row>
@@ -19524,10 +20944,15 @@
       </c>
       <c r="R285" t="inlineStr">
         <is>
+          <t>[-2.75823468e+03  5.82860036e+06]</t>
+        </is>
+      </c>
+      <c r="S285" t="inlineStr">
+        <is>
           <t>{2021: 287664.06180264, 2022: 251449.83134938218, 2023: 248691.59666488506, 2024: 245933.36198038887, 2025: 243175.1272958927, 2026: 240416.8926113965, 2027: 237658.6579269003, 2028: 234900.42324240413, 2029: 232142.188557907, 2030: 229383.95387341082, 2031: 226625.71918891463, 2032: 223867.48450441845, 2033: 221109.24981992226, 2034: 218351.01513542607, 2035: 215592.78045092896, 2036: 212834.54576643277, 2037: 210076.31108193658, 2038: 207318.0763974404, 2039: 204559.8417129442, 2040: 201801.6070284471, 2041: 199043.3723439509, 2042: 196285.13765945472, 2043: 193526.90297495853, 2044: 190768.66829046234, 2045: 188010.43360596616, 2046: 185252.19892146904, 2047: 182493.96423697285, 2048: 179735.72955247667, 2049: 176977.49486798048, 2050: 174219.2601834843}</t>
         </is>
       </c>
-      <c r="S285" t="n">
+      <c r="T285" t="n">
         <v>6228924.228036132</v>
       </c>
     </row>
@@ -19591,10 +21016,15 @@
       </c>
       <c r="R286" t="inlineStr">
         <is>
+          <t>[-8.94610946e+03  1.81734059e+07]</t>
+        </is>
+      </c>
+      <c r="S286" t="inlineStr">
+        <is>
           <t>{2021: 95248.2864179093, 2022: 84372.56920722872, 2023: 75426.45974573866, 2024: 66480.35028424859, 2025: 57534.240822758526, 2026: 48588.13136126846, 2027: 39642.021899778396, 2028: 30695.912438292056, 2029: 21749.80297680199, 2030: 12803.693515311927, 2031: 3857.5840538218617, 2032: 0, 2033: 0, 2034: 0, 2035: 0, 2036: 0, 2037: 0, 2038: 0, 2039: 0, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S286" t="n">
+      <c r="T286" t="n">
         <v>488774.9095142038</v>
       </c>
     </row>
@@ -19658,10 +21088,15 @@
       </c>
       <c r="R287" t="inlineStr">
         <is>
+          <t>[-1.29057576e+03  2.67532215e+06]</t>
+        </is>
+      </c>
+      <c r="S287" t="inlineStr">
+        <is>
           <t>{2021: 66972.2779992721, 2022: 65777.96392579889, 2023: 64487.388164676726, 2024: 63196.81240355503, 2025: 61906.236642432865, 2026: 60615.66088131117, 2027: 59325.08512018947, 2028: 58034.509359067306, 2029: 56743.93359794561, 2030: 55453.357836823445, 2031: 54162.78207570175, 2032: 52872.20631458005, 2033: 51581.630553457886, 2034: 50291.05479233619, 2035: 49000.479031214025, 2036: 47709.90327009233, 2037: 46419.32750897063, 2038: 45128.751747848466, 2039: 43838.17598672677, 2040: 42547.600225604605, 2041: 41257.02446448291, 2042: 39966.448703360744, 2043: 38675.872942239046, 2044: 37385.29718111735, 2045: 36094.721419995185, 2046: 34804.14565887349, 2047: 33513.569897751324, 2048: 32222.994136629626, 2049: 30932.41837550793, 2050: 29641.842614385765}</t>
         </is>
       </c>
-      <c r="S287" t="n">
+      <c r="T287" t="n">
         <v>1402252.41252512</v>
       </c>
     </row>
@@ -19725,10 +21160,15 @@
       </c>
       <c r="R288" t="inlineStr">
         <is>
+          <t>[-3.62503664e+03  7.39391481e+06]</t>
+        </is>
+      </c>
+      <c r="S288" t="inlineStr">
+        <is>
           <t>{2021: 66856.4788173378, 2022: 64090.72265093215, 2023: 60465.68601022381, 2024: 56840.64936951548, 2025: 53215.612728807144, 2026: 49590.57608809881, 2027: 45965.539447390474, 2028: 42340.50280668214, 2029: 38715.466165973805, 2030: 35090.42952526547, 2031: 31465.392884557135, 2032: 27840.3562438488, 2033: 24215.319603140466, 2034: 20590.28296243213, 2035: 16965.246321723796, 2036: 13340.20968101453, 2037: 9715.173040306196, 2038: 6090.136399597861, 2039: 2465.099758889526, 2040: 0, 2041: 0, 2042: 0, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S288" t="n">
+      <c r="T288" t="n">
         <v>632430.6410970686</v>
       </c>
     </row>
@@ -19792,10 +21232,15 @@
       </c>
       <c r="R289" t="inlineStr">
         <is>
+          <t>[-9.99704314e+02  2.05081776e+06]</t>
+        </is>
+      </c>
+      <c r="S289" t="inlineStr">
+        <is>
           <t>{2021: 30157.3238665339, 2022: 29415.63985156198, 2023: 28415.935537898447, 2024: 27416.23122423468, 2025: 26416.52691057115, 2026: 25416.822596907616, 2027: 24417.118283244083, 2028: 23417.413969580317, 2029: 22417.709655916784, 2030: 21418.00534225325, 2031: 20418.301028589718, 2032: 19418.596714925952, 2033: 18418.89240126242, 2034: 17419.188087598886, 2035: 16419.483773935353, 2036: 15419.779460271588, 2037: 14420.075146608055, 2038: 13420.370832944522, 2039: 12420.666519280756, 2040: 11420.962205617223, 2041: 10421.25789195369, 2042: 9421.553578290157, 2043: 8421.849264626391, 2044: 7422.144950962858, 2045: 6422.440637299325, 2046: 5422.736323635792, 2047: 4423.032009972027, 2048: 3423.3276963084936, 2049: 2423.6233826449607, 2050: 1423.9190689811949}</t>
         </is>
       </c>
-      <c r="S289" t="n">
+      <c r="T289" t="n">
         <v>461540.306746654</v>
       </c>
     </row>
@@ -19859,10 +21304,15 @@
       </c>
       <c r="R290" t="inlineStr">
         <is>
+          <t>[-7.78159607e+02  1.59682094e+06]</t>
+        </is>
+      </c>
+      <c r="S290" t="inlineStr">
+        <is>
           <t>{2021: 25041.7369677682, 2022: 23382.21895939717, 2023: 22604.059352454497, 2024: 21825.899745511822, 2025: 21047.74013856938, 2026: 20269.580531626707, 2027: 19491.420924684033, 2028: 18713.26131774136, 2029: 17935.101710798917, 2030: 17156.942103856243, 2031: 16378.782496913569, 2032: 15600.622889971128, 2033: 14822.463283028454, 2034: 14044.30367608578, 2035: 13266.144069143105, 2036: 12487.984462200664, 2037: 11709.82485525799, 2038: 10931.665248315316, 2039: 10153.505641372642, 2040: 9375.3460344302, 2041: 8597.186427487526, 2042: 7819.026820544852, 2043: 7040.867213602411, 2044: 6262.7076066597365, 2045: 5484.547999717062, 2046: 4706.388392774388, 2047: 3928.228785831947, 2048: 3150.0691788892727, 2049: 2371.9095719465986, 2050: 1593.7499650041573}</t>
         </is>
       </c>
-      <c r="S290" t="n">
+      <c r="T290" t="n">
         <v>373875.5429051989</v>
       </c>
     </row>
@@ -19926,10 +21376,15 @@
       </c>
       <c r="R291" t="inlineStr">
         <is>
+          <t>[-6.94395244e+02  1.41828360e+06]</t>
+        </is>
+      </c>
+      <c r="S291" t="inlineStr">
+        <is>
           <t>{2021: 15397.0438344427, 2022: 14216.414564732928, 2023: 13522.019320736174, 2024: 12827.624076739652, 2025: 12133.22883274313, 2026: 11438.833588746376, 2027: 10744.438344749855, 2028: 10050.043100753333, 2029: 9355.64785675658, 2030: 8661.252612760058, 2031: 7966.857368763536, 2032: 7272.462124766782, 2033: 6578.0668807702605, 2034: 5883.671636773739, 2035: 5189.276392776985, 2036: 4494.881148780463, 2037: 3800.485904783942, 2038: 3106.0906607871875, 2039: 2411.695416790666, 2040: 1717.3001727941446, 2041: 1022.9049287973903, 2042: 328.50968480086885, 2043: 0, 2044: 0, 2045: 0, 2046: 0, 2047: 0, 2048: 0, 2049: 0, 2050: 0}</t>
         </is>
       </c>
-      <c r="S291" t="n">
+      <c r="T291" t="n">
         <v>160420.2265373254</v>
       </c>
     </row>

</xml_diff>